<commit_message>
v0.6.1s: LoadProfileForm, MainMenu button sounds
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E2F83C-23A0-4D7E-80F4-13CA5BDDAD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDE4D36-78D4-4975-88E9-4BD9206497B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
     <sheet name="Items" sheetId="2" r:id="rId2"/>
     <sheet name="Abilities" sheetId="10" r:id="rId3"/>
-    <sheet name="Projectiles" sheetId="9" r:id="rId4"/>
-    <sheet name="Features" sheetId="8" r:id="rId5"/>
-    <sheet name="Conditions" sheetId="5" r:id="rId6"/>
-    <sheet name="Effects" sheetId="6" r:id="rId7"/>
-    <sheet name="XP Chart" sheetId="7" r:id="rId8"/>
-    <sheet name="Keys-Locks" sheetId="4" r:id="rId9"/>
-    <sheet name="Statuses" sheetId="3" r:id="rId10"/>
+    <sheet name="HeroTree" sheetId="11" r:id="rId4"/>
+    <sheet name="Projectiles" sheetId="9" r:id="rId5"/>
+    <sheet name="Features" sheetId="8" r:id="rId6"/>
+    <sheet name="Conditions" sheetId="5" r:id="rId7"/>
+    <sheet name="Effects" sheetId="6" r:id="rId8"/>
+    <sheet name="XP Chart" sheetId="7" r:id="rId9"/>
+    <sheet name="Keys-Locks" sheetId="4" r:id="rId10"/>
+    <sheet name="Statuses" sheetId="3" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="739">
   <si>
     <t>ID</t>
   </si>
@@ -2083,6 +2084,183 @@
   </si>
   <si>
     <t>Star Piece</t>
+  </si>
+  <si>
+    <t>Hero Tree</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>PII</t>
+  </si>
+  <si>
+    <t>AII</t>
+  </si>
+  <si>
+    <t>SII</t>
+  </si>
+  <si>
+    <t>DII</t>
+  </si>
+  <si>
+    <t>FII</t>
+  </si>
+  <si>
+    <t>Passive I</t>
+  </si>
+  <si>
+    <t>A Ability I</t>
+  </si>
+  <si>
+    <t>S Ability I</t>
+  </si>
+  <si>
+    <t>D Ability I</t>
+  </si>
+  <si>
+    <t>F Ability I</t>
+  </si>
+  <si>
+    <t>Passive II</t>
+  </si>
+  <si>
+    <t>A Ability II</t>
+  </si>
+  <si>
+    <t>S Ability II</t>
+  </si>
+  <si>
+    <t>D Ability II</t>
+  </si>
+  <si>
+    <t>F Ability II</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Unlocks passive ability</t>
+  </si>
+  <si>
+    <t>Unlocks A ability</t>
+  </si>
+  <si>
+    <t>Unlocks S ability</t>
+  </si>
+  <si>
+    <t>Unlocks D ability</t>
+  </si>
+  <si>
+    <t>Unlocks F ability</t>
+  </si>
+  <si>
+    <t>Upgrades passive ability</t>
+  </si>
+  <si>
+    <t>Upgrades A ability</t>
+  </si>
+  <si>
+    <t>Upgrades S ability</t>
+  </si>
+  <si>
+    <t>Upgrades D ability</t>
+  </si>
+  <si>
+    <t>Upgrades F ability</t>
+  </si>
+  <si>
+    <t>Right Branch</t>
+  </si>
+  <si>
+    <t>Dependencies</t>
+  </si>
+  <si>
+    <t>PI, AI, SI, DI</t>
+  </si>
+  <si>
+    <t>PII, AII, SII, DII</t>
+  </si>
+  <si>
+    <t>Agility I</t>
+  </si>
+  <si>
+    <t>Can play without lock screen</t>
+  </si>
+  <si>
+    <t>Agility +1 (can jump)</t>
+  </si>
+  <si>
+    <t>Speed I</t>
+  </si>
+  <si>
+    <t>AGII</t>
+  </si>
+  <si>
+    <t>SPI</t>
+  </si>
+  <si>
+    <t>AGI</t>
+  </si>
+  <si>
+    <t>SPII</t>
+  </si>
+  <si>
+    <t>Speed II</t>
+  </si>
+  <si>
+    <t>Agility II</t>
+  </si>
+  <si>
+    <t>Agility +1 (can jump higher/farther)</t>
+  </si>
+  <si>
+    <t>Speed +0.4</t>
+  </si>
+  <si>
+    <t>Speed +0.6</t>
+  </si>
+  <si>
+    <t>Left Branch</t>
+  </si>
+  <si>
+    <t>Unlock Screen</t>
+  </si>
+  <si>
+    <t>FOI</t>
+  </si>
+  <si>
+    <t>Follower I</t>
+  </si>
+  <si>
+    <t>Unlock follower</t>
+  </si>
+  <si>
+    <t>Follower II</t>
+  </si>
+  <si>
+    <t>FOII</t>
+  </si>
+  <si>
+    <t>Upgrade follower</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -2976,6 +3154,26 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A228F-2BB3-44AC-82E9-D9BE084DFD89}">
   <dimension ref="B2:F34"/>
   <sheetViews>
@@ -3396,7 +3594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="J129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -7137,6 +7335,326 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
+  <dimension ref="A1:G24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="C4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D4" t="s">
+        <v>691</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" t="s">
+        <v>682</v>
+      </c>
+      <c r="D5" t="s">
+        <v>692</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G5" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" t="s">
+        <v>693</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G6" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" t="s">
+        <v>684</v>
+      </c>
+      <c r="D7" t="s">
+        <v>694</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G7" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" t="s">
+        <v>685</v>
+      </c>
+      <c r="D8" t="s">
+        <v>695</v>
+      </c>
+      <c r="F8" t="s">
+        <v>714</v>
+      </c>
+      <c r="G8" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" t="s">
+        <v>686</v>
+      </c>
+      <c r="D9" t="s">
+        <v>696</v>
+      </c>
+      <c r="F9" t="s">
+        <v>685</v>
+      </c>
+      <c r="G9" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" t="s">
+        <v>687</v>
+      </c>
+      <c r="D10" t="s">
+        <v>697</v>
+      </c>
+      <c r="F10" t="s">
+        <v>685</v>
+      </c>
+      <c r="G10" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" t="s">
+        <v>688</v>
+      </c>
+      <c r="D11" t="s">
+        <v>698</v>
+      </c>
+      <c r="F11" t="s">
+        <v>685</v>
+      </c>
+      <c r="G11" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" t="s">
+        <v>689</v>
+      </c>
+      <c r="D12" t="s">
+        <v>699</v>
+      </c>
+      <c r="F12" t="s">
+        <v>685</v>
+      </c>
+      <c r="G12" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" t="s">
+        <v>690</v>
+      </c>
+      <c r="D13" t="s">
+        <v>700</v>
+      </c>
+      <c r="F13" t="s">
+        <v>715</v>
+      </c>
+      <c r="G13" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="C15" t="s">
+        <v>722</v>
+      </c>
+      <c r="D15" t="s">
+        <v>716</v>
+      </c>
+      <c r="G15" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" t="s">
+        <v>721</v>
+      </c>
+      <c r="D16" t="s">
+        <v>719</v>
+      </c>
+      <c r="G16" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" t="s">
+        <v>737</v>
+      </c>
+      <c r="D17" t="s">
+        <v>730</v>
+      </c>
+      <c r="F17" t="s">
+        <v>722</v>
+      </c>
+      <c r="G17" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" t="s">
+        <v>738</v>
+      </c>
+      <c r="F18" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" t="s">
+        <v>732</v>
+      </c>
+      <c r="G19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" t="s">
+        <v>720</v>
+      </c>
+      <c r="D20" t="s">
+        <v>725</v>
+      </c>
+      <c r="F20" t="s">
+        <v>722</v>
+      </c>
+      <c r="G20" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" t="s">
+        <v>723</v>
+      </c>
+      <c r="D21" t="s">
+        <v>724</v>
+      </c>
+      <c r="F21" t="s">
+        <v>721</v>
+      </c>
+      <c r="G21" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" t="s">
+        <v>738</v>
+      </c>
+      <c r="F22" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" t="s">
+        <v>738</v>
+      </c>
+      <c r="F23" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" t="s">
+        <v>735</v>
+      </c>
+      <c r="D24" t="s">
+        <v>734</v>
+      </c>
+      <c r="G24" t="s">
+        <v>736</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B15:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAF6DD-D8FA-4653-B50E-0B687056C45B}">
   <dimension ref="A1:J41"/>
   <sheetViews>
@@ -7859,7 +8377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:G91"/>
   <sheetViews>
@@ -8829,7 +9347,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1FC8B3-9A49-47BD-9EE8-A4129AACB06F}">
   <dimension ref="B2:F6"/>
   <sheetViews>
@@ -8890,7 +9408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385FB665-C74B-44E6-93F0-B362228155AD}">
   <dimension ref="B2:D6"/>
   <sheetViews>
@@ -8934,7 +9452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A114E18-4580-4CF1-BE70-B14A03AAF800}">
   <dimension ref="A1:S110"/>
   <sheetViews>
@@ -14771,24 +15289,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
v0.6.2a: Outlined Profile class
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDE4D36-78D4-4975-88E9-4BD9206497B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D159D-3DA2-4562-926F-CA63998316F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="742">
   <si>
     <t>ID</t>
   </si>
@@ -2261,6 +2261,15 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Unlock Offhand gear slot</t>
+  </si>
+  <si>
+    <t>Unlock accessory gearslots</t>
+  </si>
+  <si>
+    <t>PlayerTree</t>
   </si>
 </sst>
 </file>
@@ -7336,15 +7345,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -7549,7 +7558,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" t="s">
         <v>737</v>
@@ -7564,7 +7573,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" t="s">
         <v>738</v>
@@ -7573,7 +7582,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" t="s">
         <v>731</v>
@@ -7585,7 +7594,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" t="s">
         <v>720</v>
@@ -7600,7 +7609,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" t="s">
         <v>723</v>
@@ -7615,7 +7624,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" t="s">
         <v>738</v>
@@ -7624,7 +7633,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" t="s">
         <v>738</v>
@@ -7633,7 +7642,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" t="s">
         <v>735</v>
@@ -7643,6 +7652,21 @@
       </c>
       <c r="G24" t="s">
         <v>736</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.6.2h: ListBox1 view maps/levels
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC2D159D-3DA2-4562-926F-CA63998316F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E321BA00-1574-4DEB-A134-B3D45DB49DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Units" sheetId="1" r:id="rId1"/>
-    <sheet name="Items" sheetId="2" r:id="rId2"/>
-    <sheet name="Abilities" sheetId="10" r:id="rId3"/>
-    <sheet name="HeroTree" sheetId="11" r:id="rId4"/>
-    <sheet name="Projectiles" sheetId="9" r:id="rId5"/>
-    <sheet name="Features" sheetId="8" r:id="rId6"/>
-    <sheet name="Conditions" sheetId="5" r:id="rId7"/>
-    <sheet name="Effects" sheetId="6" r:id="rId8"/>
+    <sheet name="Terrains" sheetId="13" r:id="rId1"/>
+    <sheet name="Features" sheetId="8" r:id="rId2"/>
+    <sheet name="Units" sheetId="1" r:id="rId3"/>
+    <sheet name="Statuses" sheetId="3" r:id="rId4"/>
+    <sheet name="Items" sheetId="2" r:id="rId5"/>
+    <sheet name="Projectiles" sheetId="9" r:id="rId6"/>
+    <sheet name="Keys-Locks" sheetId="4" r:id="rId7"/>
+    <sheet name="Abilities" sheetId="10" r:id="rId8"/>
     <sheet name="XP Chart" sheetId="7" r:id="rId9"/>
-    <sheet name="Keys-Locks" sheetId="4" r:id="rId10"/>
-    <sheet name="Statuses" sheetId="3" r:id="rId11"/>
+    <sheet name="HeroTree" sheetId="11" r:id="rId10"/>
+    <sheet name="Conditions" sheetId="5" r:id="rId11"/>
+    <sheet name="Effects" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="800">
   <si>
     <t>ID</t>
   </si>
@@ -2270,6 +2271,180 @@
   </si>
   <si>
     <t>PlayerTree</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Terrains</t>
+  </si>
+  <si>
+    <t>Carpet, light</t>
+  </si>
+  <si>
+    <t>Carpet, gray</t>
+  </si>
+  <si>
+    <t>Carpet, dark</t>
+  </si>
+  <si>
+    <t>Wood Floor, light</t>
+  </si>
+  <si>
+    <t>Wood Floor, brown</t>
+  </si>
+  <si>
+    <t>Wood Floor, dark</t>
+  </si>
+  <si>
+    <t>Tile, red</t>
+  </si>
+  <si>
+    <t>Tile, green</t>
+  </si>
+  <si>
+    <t>Tile, gray</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>fog layer</t>
+  </si>
+  <si>
+    <t>Base Height</t>
+  </si>
+  <si>
+    <t>Grass, light</t>
+  </si>
+  <si>
+    <t>Grass, green</t>
+  </si>
+  <si>
+    <t>Grass, dark</t>
+  </si>
+  <si>
+    <t>Grass, dead</t>
+  </si>
+  <si>
+    <t>Dirt, light</t>
+  </si>
+  <si>
+    <t>Dirt, gray</t>
+  </si>
+  <si>
+    <t>Dirt, dark</t>
+  </si>
+  <si>
+    <t>Grass, line left</t>
+  </si>
+  <si>
+    <t>Grass, line up</t>
+  </si>
+  <si>
+    <t>Road1</t>
+  </si>
+  <si>
+    <t>Road2</t>
+  </si>
+  <si>
+    <t>Road3</t>
+  </si>
+  <si>
+    <t>Road, white up</t>
+  </si>
+  <si>
+    <t>Road, white left</t>
+  </si>
+  <si>
+    <t>Road, yellow up</t>
+  </si>
+  <si>
+    <t>Road, yellow left</t>
+  </si>
+  <si>
+    <t>Road, double up</t>
+  </si>
+  <si>
+    <t>Road, double left</t>
+  </si>
+  <si>
+    <t>Brick, blue</t>
+  </si>
+  <si>
+    <t>Brick, white</t>
+  </si>
+  <si>
+    <t>Brick, yellow</t>
+  </si>
+  <si>
+    <t>Brick, pink</t>
+  </si>
+  <si>
+    <t>Brick, red</t>
+  </si>
+  <si>
+    <t>Brick, gray</t>
+  </si>
+  <si>
+    <t>Brick, green</t>
+  </si>
+  <si>
+    <t>Stair, green, up</t>
+  </si>
+  <si>
+    <t>Stair, green, down</t>
+  </si>
+  <si>
+    <t>Stair, green, left</t>
+  </si>
+  <si>
+    <t>Stair, green, right</t>
+  </si>
+  <si>
+    <t>Stair, gray, up</t>
+  </si>
+  <si>
+    <t>Stair, gray, down</t>
+  </si>
+  <si>
+    <t>Stair, gray, left</t>
+  </si>
+  <si>
+    <t>Stair, gray, right</t>
+  </si>
+  <si>
+    <t>Stair, white, right</t>
+  </si>
+  <si>
+    <t>Stair, white, left</t>
+  </si>
+  <si>
+    <t>Stair, white, down</t>
+  </si>
+  <si>
+    <t>Stair, white, up</t>
+  </si>
+  <si>
+    <t>Stair, red, up</t>
+  </si>
+  <si>
+    <t>Stair, red, down</t>
+  </si>
+  <si>
+    <t>Stair, red, left</t>
+  </si>
+  <si>
+    <t>Stair, red, right</t>
+  </si>
+  <si>
+    <t>1-3 in grid</t>
+  </si>
+  <si>
+    <t>Stairs</t>
+  </si>
+  <si>
+    <t>Table, wooden</t>
   </si>
 </sst>
 </file>
@@ -2669,6 +2844,1989 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
+  <dimension ref="A1:E71"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="4"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="7" max="7" width="78.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>744</v>
+      </c>
+      <c r="D7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>102</v>
+      </c>
+      <c r="C8" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>103</v>
+      </c>
+      <c r="C9" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>111</v>
+      </c>
+      <c r="C10" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="3">
+        <v>112</v>
+      </c>
+      <c r="C11" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
+        <v>113</v>
+      </c>
+      <c r="C12" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
+        <v>123</v>
+      </c>
+      <c r="C15" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>131</v>
+      </c>
+      <c r="C16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3">
+        <v>152</v>
+      </c>
+      <c r="C18" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="4">
+        <v>153</v>
+      </c>
+      <c r="C19" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="4">
+        <v>154</v>
+      </c>
+      <c r="C20" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>155</v>
+      </c>
+      <c r="C21" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3">
+        <v>161</v>
+      </c>
+      <c r="C23" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>162</v>
+      </c>
+      <c r="C24" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="4">
+        <v>163</v>
+      </c>
+      <c r="C25" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>171</v>
+      </c>
+      <c r="C26" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="6">
+        <v>172</v>
+      </c>
+      <c r="C27" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="4">
+        <v>173</v>
+      </c>
+      <c r="C28" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>174</v>
+      </c>
+      <c r="C29" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="4">
+        <v>175</v>
+      </c>
+      <c r="C30" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="6">
+        <v>176</v>
+      </c>
+      <c r="C31" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>177</v>
+      </c>
+      <c r="C32" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>178</v>
+      </c>
+      <c r="C33" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <v>179</v>
+      </c>
+      <c r="C34" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="4">
+        <v>201</v>
+      </c>
+      <c r="C36" t="s">
+        <v>774</v>
+      </c>
+      <c r="D36" t="s">
+        <v>247</v>
+      </c>
+      <c r="E36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>202</v>
+      </c>
+      <c r="C37" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>203</v>
+      </c>
+      <c r="C38" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>204</v>
+      </c>
+      <c r="C39" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>205</v>
+      </c>
+      <c r="C40" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <v>206</v>
+      </c>
+      <c r="C41" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>207</v>
+      </c>
+      <c r="C42" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>301</v>
+      </c>
+      <c r="C45" t="s">
+        <v>785</v>
+      </c>
+      <c r="D45" t="s">
+        <v>798</v>
+      </c>
+      <c r="E45" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>302</v>
+      </c>
+      <c r="C46" t="s">
+        <v>786</v>
+      </c>
+      <c r="E46" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <v>303</v>
+      </c>
+      <c r="C47" t="s">
+        <v>787</v>
+      </c>
+      <c r="E47" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>304</v>
+      </c>
+      <c r="C48" t="s">
+        <v>788</v>
+      </c>
+      <c r="E48" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>305</v>
+      </c>
+      <c r="C49" t="s">
+        <v>781</v>
+      </c>
+      <c r="E49" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>306</v>
+      </c>
+      <c r="C50" t="s">
+        <v>782</v>
+      </c>
+      <c r="E50" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>307</v>
+      </c>
+      <c r="C51" t="s">
+        <v>783</v>
+      </c>
+      <c r="E51" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="4">
+        <v>308</v>
+      </c>
+      <c r="C52" t="s">
+        <v>784</v>
+      </c>
+      <c r="E52" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="4">
+        <v>309</v>
+      </c>
+      <c r="C53" t="s">
+        <v>793</v>
+      </c>
+      <c r="E53" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B54" s="4">
+        <v>310</v>
+      </c>
+      <c r="C54" t="s">
+        <v>794</v>
+      </c>
+      <c r="E54" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="4">
+        <v>311</v>
+      </c>
+      <c r="C55" t="s">
+        <v>795</v>
+      </c>
+      <c r="E55" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="4">
+        <v>312</v>
+      </c>
+      <c r="C56" t="s">
+        <v>796</v>
+      </c>
+      <c r="E56" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>313</v>
+      </c>
+      <c r="C57" t="s">
+        <v>792</v>
+      </c>
+      <c r="E57" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
+        <v>314</v>
+      </c>
+      <c r="C58" t="s">
+        <v>791</v>
+      </c>
+      <c r="E58" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
+        <v>315</v>
+      </c>
+      <c r="C59" t="s">
+        <v>790</v>
+      </c>
+      <c r="E59" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
+        <v>316</v>
+      </c>
+      <c r="C60" t="s">
+        <v>789</v>
+      </c>
+      <c r="E60" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="4">
+        <v>321</v>
+      </c>
+      <c r="C61" t="s">
+        <v>799</v>
+      </c>
+      <c r="D61" t="s">
+        <v>283</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
+  <dimension ref="A1:G31"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="59.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="C4" t="s">
+        <v>681</v>
+      </c>
+      <c r="D4" t="s">
+        <v>691</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G4" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
+      <c r="C5" t="s">
+        <v>682</v>
+      </c>
+      <c r="D5" t="s">
+        <v>692</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G5" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" t="s">
+        <v>683</v>
+      </c>
+      <c r="D6" t="s">
+        <v>693</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G6" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7" t="s">
+        <v>684</v>
+      </c>
+      <c r="D7" t="s">
+        <v>694</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G7" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8" t="s">
+        <v>685</v>
+      </c>
+      <c r="D8" t="s">
+        <v>695</v>
+      </c>
+      <c r="F8" t="s">
+        <v>714</v>
+      </c>
+      <c r="G8" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9" t="s">
+        <v>686</v>
+      </c>
+      <c r="D9" t="s">
+        <v>696</v>
+      </c>
+      <c r="F9" t="s">
+        <v>685</v>
+      </c>
+      <c r="G9" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10" t="s">
+        <v>687</v>
+      </c>
+      <c r="D10" t="s">
+        <v>697</v>
+      </c>
+      <c r="F10" t="s">
+        <v>685</v>
+      </c>
+      <c r="G10" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11" t="s">
+        <v>688</v>
+      </c>
+      <c r="D11" t="s">
+        <v>698</v>
+      </c>
+      <c r="F11" t="s">
+        <v>685</v>
+      </c>
+      <c r="G11" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" t="s">
+        <v>689</v>
+      </c>
+      <c r="D12" t="s">
+        <v>699</v>
+      </c>
+      <c r="F12" t="s">
+        <v>685</v>
+      </c>
+      <c r="G12" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13" t="s">
+        <v>690</v>
+      </c>
+      <c r="D13" t="s">
+        <v>700</v>
+      </c>
+      <c r="F13" t="s">
+        <v>715</v>
+      </c>
+      <c r="G13" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="C15" t="s">
+        <v>722</v>
+      </c>
+      <c r="D15" t="s">
+        <v>716</v>
+      </c>
+      <c r="G15" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16" t="s">
+        <v>721</v>
+      </c>
+      <c r="D16" t="s">
+        <v>719</v>
+      </c>
+      <c r="G16" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17" t="s">
+        <v>737</v>
+      </c>
+      <c r="D17" t="s">
+        <v>730</v>
+      </c>
+      <c r="F17" t="s">
+        <v>722</v>
+      </c>
+      <c r="G17" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18" t="s">
+        <v>738</v>
+      </c>
+      <c r="F18" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19" t="s">
+        <v>731</v>
+      </c>
+      <c r="D19" t="s">
+        <v>732</v>
+      </c>
+      <c r="G19" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20" t="s">
+        <v>720</v>
+      </c>
+      <c r="D20" t="s">
+        <v>725</v>
+      </c>
+      <c r="F20" t="s">
+        <v>722</v>
+      </c>
+      <c r="G20" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21" t="s">
+        <v>723</v>
+      </c>
+      <c r="D21" t="s">
+        <v>724</v>
+      </c>
+      <c r="F21" t="s">
+        <v>721</v>
+      </c>
+      <c r="G21" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22" t="s">
+        <v>738</v>
+      </c>
+      <c r="F22" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23" t="s">
+        <v>738</v>
+      </c>
+      <c r="F23" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24" t="s">
+        <v>735</v>
+      </c>
+      <c r="D24" t="s">
+        <v>734</v>
+      </c>
+      <c r="G24" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B15:B24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1FC8B3-9A49-47BD-9EE8-A4129AACB06F}">
+  <dimension ref="B2:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385FB665-C74B-44E6-93F0-B362228155AD}">
+  <dimension ref="B2:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
+  <dimension ref="A1:G91"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41" customWidth="1"/>
+    <col min="7" max="7" width="78.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" t="s">
+        <v>211</v>
+      </c>
+      <c r="D4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>214</v>
+      </c>
+      <c r="D7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="C12" t="s">
+        <v>219</v>
+      </c>
+      <c r="D12" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="C13" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="C15" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="4">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C18" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C19" t="s">
+        <v>234</v>
+      </c>
+      <c r="E19" t="s">
+        <v>223</v>
+      </c>
+      <c r="F19" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="4">
+        <v>155</v>
+      </c>
+      <c r="C21" t="s">
+        <v>237</v>
+      </c>
+      <c r="E21" t="s">
+        <v>223</v>
+      </c>
+      <c r="F21" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="4">
+        <v>156</v>
+      </c>
+      <c r="C22" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="4">
+        <v>157</v>
+      </c>
+      <c r="C23" t="s">
+        <v>239</v>
+      </c>
+      <c r="E23" t="s">
+        <v>223</v>
+      </c>
+      <c r="F23" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="4">
+        <v>158</v>
+      </c>
+      <c r="C24" t="s">
+        <v>240</v>
+      </c>
+      <c r="E24" t="s">
+        <v>223</v>
+      </c>
+      <c r="F24" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="4">
+        <v>161</v>
+      </c>
+      <c r="C26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="4">
+        <v>162</v>
+      </c>
+      <c r="C27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C29" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C31" t="s">
+        <v>246</v>
+      </c>
+      <c r="D31" t="s">
+        <v>247</v>
+      </c>
+      <c r="E31" t="s">
+        <v>223</v>
+      </c>
+      <c r="F31" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="4">
+        <v>217</v>
+      </c>
+      <c r="C32" t="s">
+        <v>251</v>
+      </c>
+      <c r="E32" t="s">
+        <v>223</v>
+      </c>
+      <c r="F32" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4">
+        <v>218</v>
+      </c>
+      <c r="C33" t="s">
+        <v>250</v>
+      </c>
+      <c r="E33" t="s">
+        <v>223</v>
+      </c>
+      <c r="F33" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4">
+        <v>219</v>
+      </c>
+      <c r="C34" t="s">
+        <v>252</v>
+      </c>
+      <c r="E34" t="s">
+        <v>223</v>
+      </c>
+      <c r="F34" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="C35" t="s">
+        <v>254</v>
+      </c>
+      <c r="E35" t="s">
+        <v>223</v>
+      </c>
+      <c r="F35" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C36" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" t="s">
+        <v>223</v>
+      </c>
+      <c r="F36" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C37" t="s">
+        <v>260</v>
+      </c>
+      <c r="E37" t="s">
+        <v>223</v>
+      </c>
+      <c r="F37" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C38" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>235</v>
+      </c>
+      <c r="C39" t="s">
+        <v>263</v>
+      </c>
+      <c r="E39" t="s">
+        <v>223</v>
+      </c>
+      <c r="F39" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C40" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>238</v>
+      </c>
+      <c r="C41" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C42" t="s">
+        <v>263</v>
+      </c>
+      <c r="E42" t="s">
+        <v>223</v>
+      </c>
+      <c r="F42" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C43" t="s">
+        <v>254</v>
+      </c>
+      <c r="E43" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C44" t="s">
+        <v>270</v>
+      </c>
+      <c r="E44" t="s">
+        <v>223</v>
+      </c>
+      <c r="F44" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C45" t="s">
+        <v>254</v>
+      </c>
+      <c r="E45" t="s">
+        <v>223</v>
+      </c>
+      <c r="F45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C46" t="s">
+        <v>260</v>
+      </c>
+      <c r="E46" t="s">
+        <v>223</v>
+      </c>
+      <c r="F46" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>301</v>
+      </c>
+      <c r="C48" t="s">
+        <v>277</v>
+      </c>
+      <c r="D48" t="s">
+        <v>283</v>
+      </c>
+      <c r="E48" t="s">
+        <v>223</v>
+      </c>
+      <c r="F48" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="4">
+        <v>302</v>
+      </c>
+      <c r="C49" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="4">
+        <v>303</v>
+      </c>
+      <c r="C50" t="s">
+        <v>274</v>
+      </c>
+      <c r="E50" t="s">
+        <v>223</v>
+      </c>
+      <c r="F50" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="4">
+        <v>304</v>
+      </c>
+      <c r="C51" t="s">
+        <v>278</v>
+      </c>
+      <c r="E51" t="s">
+        <v>223</v>
+      </c>
+      <c r="F51" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C52" t="s">
+        <v>279</v>
+      </c>
+      <c r="E52" t="s">
+        <v>223</v>
+      </c>
+      <c r="F52" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C53" t="s">
+        <v>282</v>
+      </c>
+      <c r="E53" t="s">
+        <v>223</v>
+      </c>
+      <c r="F53" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C54" t="s">
+        <v>285</v>
+      </c>
+      <c r="E54" t="s">
+        <v>223</v>
+      </c>
+      <c r="F54" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C56" t="s">
+        <v>288</v>
+      </c>
+      <c r="E56" t="s">
+        <v>223</v>
+      </c>
+      <c r="F56" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="4">
+        <v>325</v>
+      </c>
+      <c r="C57" t="s">
+        <v>289</v>
+      </c>
+      <c r="E57" t="s">
+        <v>223</v>
+      </c>
+      <c r="F57" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="4">
+        <v>326</v>
+      </c>
+      <c r="C58" t="s">
+        <v>290</v>
+      </c>
+      <c r="E58" t="s">
+        <v>223</v>
+      </c>
+      <c r="F58" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="4">
+        <v>327</v>
+      </c>
+      <c r="C59" t="s">
+        <v>291</v>
+      </c>
+      <c r="E59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F59" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="4">
+        <v>328</v>
+      </c>
+      <c r="C60" t="s">
+        <v>293</v>
+      </c>
+      <c r="E60" t="s">
+        <v>223</v>
+      </c>
+      <c r="F60" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="4">
+        <v>329</v>
+      </c>
+      <c r="C61" t="s">
+        <v>294</v>
+      </c>
+      <c r="E61" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C62" t="s">
+        <v>297</v>
+      </c>
+      <c r="E62" t="s">
+        <v>223</v>
+      </c>
+      <c r="F62" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="4">
+        <v>401</v>
+      </c>
+      <c r="C64" t="s">
+        <v>298</v>
+      </c>
+      <c r="E64" t="s">
+        <v>223</v>
+      </c>
+      <c r="F64" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
+        <v>402</v>
+      </c>
+      <c r="C65" t="s">
+        <v>299</v>
+      </c>
+      <c r="E65" t="s">
+        <v>223</v>
+      </c>
+      <c r="F65" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
+        <v>403</v>
+      </c>
+      <c r="C66" t="s">
+        <v>300</v>
+      </c>
+      <c r="E66" t="s">
+        <v>223</v>
+      </c>
+      <c r="F66" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="4">
+        <v>404</v>
+      </c>
+      <c r="C67" t="s">
+        <v>301</v>
+      </c>
+      <c r="E67" t="s">
+        <v>223</v>
+      </c>
+      <c r="F67" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C68" t="s">
+        <v>303</v>
+      </c>
+      <c r="E68" t="s">
+        <v>223</v>
+      </c>
+      <c r="F68" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="4">
+        <v>407</v>
+      </c>
+      <c r="C69" t="s">
+        <v>304</v>
+      </c>
+      <c r="E69" t="s">
+        <v>223</v>
+      </c>
+      <c r="F69" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="4">
+        <v>408</v>
+      </c>
+      <c r="C70" t="s">
+        <v>305</v>
+      </c>
+      <c r="E70" t="s">
+        <v>223</v>
+      </c>
+      <c r="F70" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="4">
+        <v>409</v>
+      </c>
+      <c r="C71" t="s">
+        <v>306</v>
+      </c>
+      <c r="E71" t="s">
+        <v>223</v>
+      </c>
+      <c r="F71" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C73" t="s">
+        <v>307</v>
+      </c>
+      <c r="D73" t="s">
+        <v>314</v>
+      </c>
+      <c r="E73" t="s">
+        <v>223</v>
+      </c>
+      <c r="F73" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="C74" t="s">
+        <v>312</v>
+      </c>
+      <c r="E74" t="s">
+        <v>223</v>
+      </c>
+      <c r="F74" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C75" t="s">
+        <v>310</v>
+      </c>
+      <c r="E75" t="s">
+        <v>223</v>
+      </c>
+      <c r="F75" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C76" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="4">
+        <v>548</v>
+      </c>
+      <c r="C77" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="C78" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C79" t="s">
+        <v>320</v>
+      </c>
+      <c r="E79" t="s">
+        <v>223</v>
+      </c>
+      <c r="F79" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>555</v>
+      </c>
+      <c r="C80" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C81" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C82" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B84" s="4">
+        <v>601</v>
+      </c>
+      <c r="C84" t="s">
+        <v>326</v>
+      </c>
+      <c r="D84" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B85" s="4">
+        <v>602</v>
+      </c>
+      <c r="C85" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B86" s="4">
+        <v>603</v>
+      </c>
+      <c r="C86" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B87" s="4">
+        <v>604</v>
+      </c>
+      <c r="C87" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B88" s="4">
+        <v>605</v>
+      </c>
+      <c r="C88" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B89" s="4">
+        <v>606</v>
+      </c>
+      <c r="C89" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B90" s="4">
+        <v>607</v>
+      </c>
+      <c r="C90" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B91" s="4">
+        <v>608</v>
+      </c>
+      <c r="C91" t="s">
+        <v>333</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:M26"/>
   <sheetViews>
@@ -3162,27 +5320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A228F-2BB3-44AC-82E9-D9BE084DFD89}">
   <dimension ref="B2:F34"/>
   <sheetViews>
@@ -3599,12 +5737,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y199"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="J129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="J75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S150" sqref="S150"/>
@@ -6813,872 +8951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E132C5F-9A98-41A1-A3AA-2A3458C20EAF}">
-  <dimension ref="A1:I36"/>
-  <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="149.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>582</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4">
-        <v>101</v>
-      </c>
-      <c r="D4" t="s">
-        <v>617</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="I4" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5">
-        <v>102</v>
-      </c>
-      <c r="D5" t="s">
-        <v>619</v>
-      </c>
-      <c r="E5" t="s">
-        <v>624</v>
-      </c>
-      <c r="F5" t="s">
-        <v>584</v>
-      </c>
-      <c r="I5" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6">
-        <v>103</v>
-      </c>
-      <c r="D6" t="s">
-        <v>581</v>
-      </c>
-      <c r="E6" t="s">
-        <v>583</v>
-      </c>
-      <c r="F6" t="s">
-        <v>585</v>
-      </c>
-      <c r="I6" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7">
-        <v>104</v>
-      </c>
-      <c r="D7" t="s">
-        <v>621</v>
-      </c>
-      <c r="E7" t="s">
-        <v>623</v>
-      </c>
-      <c r="F7" t="s">
-        <v>586</v>
-      </c>
-      <c r="I7" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8">
-        <v>105</v>
-      </c>
-      <c r="D8" t="s">
-        <v>625</v>
-      </c>
-      <c r="E8" t="s">
-        <v>620</v>
-      </c>
-      <c r="F8" t="s">
-        <v>587</v>
-      </c>
-      <c r="I8" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9">
-        <v>106</v>
-      </c>
-      <c r="D9" t="s">
-        <v>647</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="I9" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10">
-        <v>107</v>
-      </c>
-      <c r="D10" t="s">
-        <v>646</v>
-      </c>
-      <c r="E10" t="s">
-        <v>656</v>
-      </c>
-      <c r="F10" t="s">
-        <v>584</v>
-      </c>
-      <c r="I10" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11">
-        <v>108</v>
-      </c>
-      <c r="D11" t="s">
-        <v>648</v>
-      </c>
-      <c r="E11" t="s">
-        <v>655</v>
-      </c>
-      <c r="F11" t="s">
-        <v>585</v>
-      </c>
-      <c r="I11" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12">
-        <v>109</v>
-      </c>
-      <c r="D12" t="s">
-        <v>649</v>
-      </c>
-      <c r="E12" t="s">
-        <v>654</v>
-      </c>
-      <c r="F12" t="s">
-        <v>586</v>
-      </c>
-      <c r="I12" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13">
-        <v>110</v>
-      </c>
-      <c r="D13" t="s">
-        <v>650</v>
-      </c>
-      <c r="E13" t="s">
-        <v>651</v>
-      </c>
-      <c r="F13" t="s">
-        <v>587</v>
-      </c>
-      <c r="I13" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>561</v>
-      </c>
-      <c r="C15">
-        <v>111</v>
-      </c>
-      <c r="D15" t="s">
-        <v>671</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>666</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="I15" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16">
-        <v>112</v>
-      </c>
-      <c r="D16" t="s">
-        <v>630</v>
-      </c>
-      <c r="E16" t="s">
-        <v>624</v>
-      </c>
-      <c r="F16" t="s">
-        <v>584</v>
-      </c>
-      <c r="G16">
-        <v>5</v>
-      </c>
-      <c r="I16" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17">
-        <v>113</v>
-      </c>
-      <c r="D17" t="s">
-        <v>629</v>
-      </c>
-      <c r="E17" t="s">
-        <v>583</v>
-      </c>
-      <c r="F17" t="s">
-        <v>585</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18">
-        <v>114</v>
-      </c>
-      <c r="D18" t="s">
-        <v>631</v>
-      </c>
-      <c r="E18" t="s">
-        <v>667</v>
-      </c>
-      <c r="F18" t="s">
-        <v>586</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="I18" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19">
-        <v>115</v>
-      </c>
-      <c r="D19" t="s">
-        <v>632</v>
-      </c>
-      <c r="E19" t="s">
-        <v>620</v>
-      </c>
-      <c r="F19" t="s">
-        <v>587</v>
-      </c>
-      <c r="G19">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20">
-        <v>116</v>
-      </c>
-      <c r="D20" t="s">
-        <v>672</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>667</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="I20" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>660</v>
-      </c>
-      <c r="E21" t="s">
-        <v>656</v>
-      </c>
-      <c r="F21" t="s">
-        <v>584</v>
-      </c>
-      <c r="G21">
-        <v>20</v>
-      </c>
-      <c r="I21" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22">
-        <v>118</v>
-      </c>
-      <c r="D22" t="s">
-        <v>661</v>
-      </c>
-      <c r="E22" t="s">
-        <v>623</v>
-      </c>
-      <c r="F22" t="s">
-        <v>585</v>
-      </c>
-      <c r="G22">
-        <v>35</v>
-      </c>
-      <c r="I22" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23">
-        <v>119</v>
-      </c>
-      <c r="D23" t="s">
-        <v>662</v>
-      </c>
-      <c r="E23" t="s">
-        <v>676</v>
-      </c>
-      <c r="F23" t="s">
-        <v>586</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
-      </c>
-      <c r="I23" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24">
-        <v>120</v>
-      </c>
-      <c r="D24" t="s">
-        <v>663</v>
-      </c>
-      <c r="E24" t="s">
-        <v>651</v>
-      </c>
-      <c r="F24" t="s">
-        <v>587</v>
-      </c>
-      <c r="G24">
-        <v>100</v>
-      </c>
-      <c r="I24" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
-        <v>627</v>
-      </c>
-      <c r="C26">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
-      <c r="C30">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
-        <v>628</v>
-      </c>
-      <c r="C32">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
-      <c r="C33">
-        <v>132</v>
-      </c>
-      <c r="D33" t="s">
-        <v>634</v>
-      </c>
-      <c r="I33" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
-      <c r="C34">
-        <v>133</v>
-      </c>
-      <c r="D34" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35">
-        <v>134</v>
-      </c>
-      <c r="D35" t="s">
-        <v>637</v>
-      </c>
-      <c r="I35" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
-      <c r="C36">
-        <v>135</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="B15:B24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
-  <dimension ref="A1:G31"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="59.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>712</v>
-      </c>
-      <c r="C4" t="s">
-        <v>681</v>
-      </c>
-      <c r="D4" t="s">
-        <v>691</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G4" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" t="s">
-        <v>682</v>
-      </c>
-      <c r="D5" t="s">
-        <v>692</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G5" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" t="s">
-        <v>683</v>
-      </c>
-      <c r="D6" t="s">
-        <v>693</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G6" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" t="s">
-        <v>684</v>
-      </c>
-      <c r="D7" t="s">
-        <v>694</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>588</v>
-      </c>
-      <c r="G7" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" t="s">
-        <v>685</v>
-      </c>
-      <c r="D8" t="s">
-        <v>695</v>
-      </c>
-      <c r="F8" t="s">
-        <v>714</v>
-      </c>
-      <c r="G8" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" t="s">
-        <v>686</v>
-      </c>
-      <c r="D9" t="s">
-        <v>696</v>
-      </c>
-      <c r="F9" t="s">
-        <v>685</v>
-      </c>
-      <c r="G9" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" t="s">
-        <v>687</v>
-      </c>
-      <c r="D10" t="s">
-        <v>697</v>
-      </c>
-      <c r="F10" t="s">
-        <v>685</v>
-      </c>
-      <c r="G10" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" t="s">
-        <v>688</v>
-      </c>
-      <c r="D11" t="s">
-        <v>698</v>
-      </c>
-      <c r="F11" t="s">
-        <v>685</v>
-      </c>
-      <c r="G11" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" t="s">
-        <v>689</v>
-      </c>
-      <c r="D12" t="s">
-        <v>699</v>
-      </c>
-      <c r="F12" t="s">
-        <v>685</v>
-      </c>
-      <c r="G12" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13" t="s">
-        <v>690</v>
-      </c>
-      <c r="D13" t="s">
-        <v>700</v>
-      </c>
-      <c r="F13" t="s">
-        <v>715</v>
-      </c>
-      <c r="G13" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>729</v>
-      </c>
-      <c r="C15" t="s">
-        <v>722</v>
-      </c>
-      <c r="D15" t="s">
-        <v>716</v>
-      </c>
-      <c r="G15" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" t="s">
-        <v>721</v>
-      </c>
-      <c r="D16" t="s">
-        <v>719</v>
-      </c>
-      <c r="G16" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" t="s">
-        <v>737</v>
-      </c>
-      <c r="D17" t="s">
-        <v>730</v>
-      </c>
-      <c r="F17" t="s">
-        <v>722</v>
-      </c>
-      <c r="G17" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" t="s">
-        <v>738</v>
-      </c>
-      <c r="F18" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" t="s">
-        <v>731</v>
-      </c>
-      <c r="D19" t="s">
-        <v>732</v>
-      </c>
-      <c r="G19" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" t="s">
-        <v>720</v>
-      </c>
-      <c r="D20" t="s">
-        <v>725</v>
-      </c>
-      <c r="F20" t="s">
-        <v>722</v>
-      </c>
-      <c r="G20" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" t="s">
-        <v>723</v>
-      </c>
-      <c r="D21" t="s">
-        <v>724</v>
-      </c>
-      <c r="F21" t="s">
-        <v>721</v>
-      </c>
-      <c r="G21" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" t="s">
-        <v>738</v>
-      </c>
-      <c r="F22" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" t="s">
-        <v>738</v>
-      </c>
-      <c r="F23" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" t="s">
-        <v>735</v>
-      </c>
-      <c r="D24" t="s">
-        <v>734</v>
-      </c>
-      <c r="G24" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G28" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G29" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>741</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="B15:B24"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAF6DD-D8FA-4653-B50E-0B687056C45B}">
   <dimension ref="A1:J41"/>
   <sheetViews>
@@ -8401,1030 +9674,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:G91"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="78.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C4" t="s">
-        <v>211</v>
-      </c>
-      <c r="D4" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>214</v>
-      </c>
-      <c r="D7" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="3" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D12" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="C13" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="C14" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C15" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C16" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
-        <v>142</v>
-      </c>
-      <c r="C17" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="3" t="s">
-        <v>231</v>
-      </c>
-      <c r="C18" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C19" t="s">
-        <v>234</v>
-      </c>
-      <c r="E19" t="s">
-        <v>223</v>
-      </c>
-      <c r="F19" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C20" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="4">
-        <v>155</v>
-      </c>
-      <c r="C21" t="s">
-        <v>237</v>
-      </c>
-      <c r="E21" t="s">
-        <v>223</v>
-      </c>
-      <c r="F21" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="4">
-        <v>156</v>
-      </c>
-      <c r="C22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="4">
-        <v>157</v>
-      </c>
-      <c r="C23" t="s">
-        <v>239</v>
-      </c>
-      <c r="E23" t="s">
-        <v>223</v>
-      </c>
-      <c r="F23" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="4">
-        <v>158</v>
-      </c>
-      <c r="C24" t="s">
-        <v>240</v>
-      </c>
-      <c r="E24" t="s">
-        <v>223</v>
-      </c>
-      <c r="F24" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="C25" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="4">
-        <v>161</v>
-      </c>
-      <c r="C26" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="4">
-        <v>162</v>
-      </c>
-      <c r="C27" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C28" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>244</v>
-      </c>
-      <c r="C29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C31" t="s">
-        <v>246</v>
-      </c>
-      <c r="D31" t="s">
-        <v>247</v>
-      </c>
-      <c r="E31" t="s">
-        <v>223</v>
-      </c>
-      <c r="F31" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4">
-        <v>217</v>
-      </c>
-      <c r="C32" t="s">
-        <v>251</v>
-      </c>
-      <c r="E32" t="s">
-        <v>223</v>
-      </c>
-      <c r="F32" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
-        <v>218</v>
-      </c>
-      <c r="C33" t="s">
-        <v>250</v>
-      </c>
-      <c r="E33" t="s">
-        <v>223</v>
-      </c>
-      <c r="F33" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="4">
-        <v>219</v>
-      </c>
-      <c r="C34" t="s">
-        <v>252</v>
-      </c>
-      <c r="E34" t="s">
-        <v>223</v>
-      </c>
-      <c r="F34" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" t="s">
-        <v>254</v>
-      </c>
-      <c r="E35" t="s">
-        <v>223</v>
-      </c>
-      <c r="F35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="C36" t="s">
-        <v>270</v>
-      </c>
-      <c r="E36" t="s">
-        <v>223</v>
-      </c>
-      <c r="F36" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C37" t="s">
-        <v>260</v>
-      </c>
-      <c r="E37" t="s">
-        <v>223</v>
-      </c>
-      <c r="F37" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="C38" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="4">
-        <v>235</v>
-      </c>
-      <c r="C39" t="s">
-        <v>263</v>
-      </c>
-      <c r="E39" t="s">
-        <v>223</v>
-      </c>
-      <c r="F39" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="C40" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="4">
-        <v>238</v>
-      </c>
-      <c r="C41" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="C42" t="s">
-        <v>263</v>
-      </c>
-      <c r="E42" t="s">
-        <v>223</v>
-      </c>
-      <c r="F42" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C43" t="s">
-        <v>254</v>
-      </c>
-      <c r="E43" t="s">
-        <v>223</v>
-      </c>
-      <c r="F43" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C44" t="s">
-        <v>270</v>
-      </c>
-      <c r="E44" t="s">
-        <v>223</v>
-      </c>
-      <c r="F44" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C45" t="s">
-        <v>254</v>
-      </c>
-      <c r="E45" t="s">
-        <v>223</v>
-      </c>
-      <c r="F45" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="C46" t="s">
-        <v>260</v>
-      </c>
-      <c r="E46" t="s">
-        <v>223</v>
-      </c>
-      <c r="F46" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="4">
-        <v>301</v>
-      </c>
-      <c r="C48" t="s">
-        <v>277</v>
-      </c>
-      <c r="D48" t="s">
-        <v>283</v>
-      </c>
-      <c r="E48" t="s">
-        <v>223</v>
-      </c>
-      <c r="F48" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="4">
-        <v>302</v>
-      </c>
-      <c r="C49" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="4">
-        <v>303</v>
-      </c>
-      <c r="C50" t="s">
-        <v>274</v>
-      </c>
-      <c r="E50" t="s">
-        <v>223</v>
-      </c>
-      <c r="F50" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
-        <v>304</v>
-      </c>
-      <c r="C51" t="s">
-        <v>278</v>
-      </c>
-      <c r="E51" t="s">
-        <v>223</v>
-      </c>
-      <c r="F51" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C52" t="s">
-        <v>279</v>
-      </c>
-      <c r="E52" t="s">
-        <v>223</v>
-      </c>
-      <c r="F52" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="C53" t="s">
-        <v>282</v>
-      </c>
-      <c r="E53" t="s">
-        <v>223</v>
-      </c>
-      <c r="F53" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C54" t="s">
-        <v>285</v>
-      </c>
-      <c r="E54" t="s">
-        <v>223</v>
-      </c>
-      <c r="F54" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="C55" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C56" t="s">
-        <v>288</v>
-      </c>
-      <c r="E56" t="s">
-        <v>223</v>
-      </c>
-      <c r="F56" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="4">
-        <v>325</v>
-      </c>
-      <c r="C57" t="s">
-        <v>289</v>
-      </c>
-      <c r="E57" t="s">
-        <v>223</v>
-      </c>
-      <c r="F57" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="4">
-        <v>326</v>
-      </c>
-      <c r="C58" t="s">
-        <v>290</v>
-      </c>
-      <c r="E58" t="s">
-        <v>223</v>
-      </c>
-      <c r="F58" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="4">
-        <v>327</v>
-      </c>
-      <c r="C59" t="s">
-        <v>291</v>
-      </c>
-      <c r="E59" t="s">
-        <v>223</v>
-      </c>
-      <c r="F59" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="4">
-        <v>328</v>
-      </c>
-      <c r="C60" t="s">
-        <v>293</v>
-      </c>
-      <c r="E60" t="s">
-        <v>223</v>
-      </c>
-      <c r="F60" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="4">
-        <v>329</v>
-      </c>
-      <c r="C61" t="s">
-        <v>294</v>
-      </c>
-      <c r="E61" t="s">
-        <v>223</v>
-      </c>
-      <c r="F61" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="4" t="s">
-        <v>296</v>
-      </c>
-      <c r="C62" t="s">
-        <v>297</v>
-      </c>
-      <c r="E62" t="s">
-        <v>223</v>
-      </c>
-      <c r="F62" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="4">
-        <v>401</v>
-      </c>
-      <c r="C64" t="s">
-        <v>298</v>
-      </c>
-      <c r="E64" t="s">
-        <v>223</v>
-      </c>
-      <c r="F64" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="4">
-        <v>402</v>
-      </c>
-      <c r="C65" t="s">
-        <v>299</v>
-      </c>
-      <c r="E65" t="s">
-        <v>223</v>
-      </c>
-      <c r="F65" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="4">
-        <v>403</v>
-      </c>
-      <c r="C66" t="s">
-        <v>300</v>
-      </c>
-      <c r="E66" t="s">
-        <v>223</v>
-      </c>
-      <c r="F66" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="4">
-        <v>404</v>
-      </c>
-      <c r="C67" t="s">
-        <v>301</v>
-      </c>
-      <c r="E67" t="s">
-        <v>223</v>
-      </c>
-      <c r="F67" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="C68" t="s">
-        <v>303</v>
-      </c>
-      <c r="E68" t="s">
-        <v>223</v>
-      </c>
-      <c r="F68" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="4">
-        <v>407</v>
-      </c>
-      <c r="C69" t="s">
-        <v>304</v>
-      </c>
-      <c r="E69" t="s">
-        <v>223</v>
-      </c>
-      <c r="F69" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="4">
-        <v>408</v>
-      </c>
-      <c r="C70" t="s">
-        <v>305</v>
-      </c>
-      <c r="E70" t="s">
-        <v>223</v>
-      </c>
-      <c r="F70" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="4">
-        <v>409</v>
-      </c>
-      <c r="C71" t="s">
-        <v>306</v>
-      </c>
-      <c r="E71" t="s">
-        <v>223</v>
-      </c>
-      <c r="F71" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="C73" t="s">
-        <v>307</v>
-      </c>
-      <c r="D73" t="s">
-        <v>314</v>
-      </c>
-      <c r="E73" t="s">
-        <v>223</v>
-      </c>
-      <c r="F73" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C74" t="s">
-        <v>312</v>
-      </c>
-      <c r="E74" t="s">
-        <v>223</v>
-      </c>
-      <c r="F74" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="C75" t="s">
-        <v>310</v>
-      </c>
-      <c r="E75" t="s">
-        <v>223</v>
-      </c>
-      <c r="F75" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C76" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="4">
-        <v>548</v>
-      </c>
-      <c r="C77" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="C78" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="C79" t="s">
-        <v>320</v>
-      </c>
-      <c r="E79" t="s">
-        <v>223</v>
-      </c>
-      <c r="F79" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="4">
-        <v>555</v>
-      </c>
-      <c r="C80" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B81" s="4" t="s">
-        <v>323</v>
-      </c>
-      <c r="C81" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B82" s="4" t="s">
-        <v>324</v>
-      </c>
-      <c r="C82" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B84" s="4">
-        <v>601</v>
-      </c>
-      <c r="C84" t="s">
-        <v>326</v>
-      </c>
-      <c r="D84" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B85" s="4">
-        <v>602</v>
-      </c>
-      <c r="C85" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B86" s="4">
-        <v>603</v>
-      </c>
-      <c r="C86" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B87" s="4">
-        <v>604</v>
-      </c>
-      <c r="C87" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B88" s="4">
-        <v>605</v>
-      </c>
-      <c r="C88" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B89" s="4">
-        <v>606</v>
-      </c>
-      <c r="C89" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B90" s="4">
-        <v>607</v>
-      </c>
-      <c r="C90" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B91" s="4">
-        <v>608</v>
-      </c>
-      <c r="C91" t="s">
-        <v>333</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1FC8B3-9A49-47BD-9EE8-A4129AACB06F}">
-  <dimension ref="B2:F6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -9433,45 +9695,531 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385FB665-C74B-44E6-93F0-B362228155AD}">
-  <dimension ref="B2:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E132C5F-9A98-41A1-A3AA-2A3458C20EAF}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="149.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>617</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="I4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="15"/>
       <c r="C5">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+        <v>619</v>
+      </c>
+      <c r="E5" t="s">
+        <v>624</v>
+      </c>
+      <c r="F5" t="s">
+        <v>584</v>
+      </c>
+      <c r="I5" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
       <c r="C6">
+        <v>103</v>
+      </c>
+      <c r="D6" t="s">
+        <v>581</v>
+      </c>
+      <c r="E6" t="s">
+        <v>583</v>
+      </c>
+      <c r="F6" t="s">
+        <v>585</v>
+      </c>
+      <c r="I6" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="15"/>
+      <c r="C7">
+        <v>104</v>
+      </c>
+      <c r="D7" t="s">
+        <v>621</v>
+      </c>
+      <c r="E7" t="s">
+        <v>623</v>
+      </c>
+      <c r="F7" t="s">
+        <v>586</v>
+      </c>
+      <c r="I7" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="15"/>
+      <c r="C8">
+        <v>105</v>
+      </c>
+      <c r="D8" t="s">
+        <v>625</v>
+      </c>
+      <c r="E8" t="s">
+        <v>620</v>
+      </c>
+      <c r="F8" t="s">
+        <v>587</v>
+      </c>
+      <c r="I8" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="15"/>
+      <c r="C9">
+        <v>106</v>
+      </c>
+      <c r="D9" t="s">
+        <v>647</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="I9" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="15"/>
+      <c r="C10">
+        <v>107</v>
+      </c>
+      <c r="D10" t="s">
+        <v>646</v>
+      </c>
+      <c r="E10" t="s">
+        <v>656</v>
+      </c>
+      <c r="F10" t="s">
+        <v>584</v>
+      </c>
+      <c r="I10" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="15"/>
+      <c r="C11">
+        <v>108</v>
+      </c>
+      <c r="D11" t="s">
+        <v>648</v>
+      </c>
+      <c r="E11" t="s">
+        <v>655</v>
+      </c>
+      <c r="F11" t="s">
+        <v>585</v>
+      </c>
+      <c r="I11" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12">
+        <v>109</v>
+      </c>
+      <c r="D12" t="s">
+        <v>649</v>
+      </c>
+      <c r="E12" t="s">
+        <v>654</v>
+      </c>
+      <c r="F12" t="s">
+        <v>586</v>
+      </c>
+      <c r="I12" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="15"/>
+      <c r="C13">
+        <v>110</v>
+      </c>
+      <c r="D13" t="s">
+        <v>650</v>
+      </c>
+      <c r="E13" t="s">
+        <v>651</v>
+      </c>
+      <c r="F13" t="s">
+        <v>587</v>
+      </c>
+      <c r="I13" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>561</v>
+      </c>
+      <c r="C15">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
+        <v>671</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>666</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="I15" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
+      <c r="C16">
+        <v>112</v>
+      </c>
+      <c r="D16" t="s">
+        <v>630</v>
+      </c>
+      <c r="E16" t="s">
+        <v>624</v>
+      </c>
+      <c r="F16" t="s">
+        <v>584</v>
+      </c>
+      <c r="G16">
+        <v>5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="15"/>
+      <c r="C17">
+        <v>113</v>
+      </c>
+      <c r="D17" t="s">
+        <v>629</v>
+      </c>
+      <c r="E17" t="s">
+        <v>583</v>
+      </c>
+      <c r="F17" t="s">
+        <v>585</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="15"/>
+      <c r="C18">
+        <v>114</v>
+      </c>
+      <c r="D18" t="s">
+        <v>631</v>
+      </c>
+      <c r="E18" t="s">
+        <v>667</v>
+      </c>
+      <c r="F18" t="s">
+        <v>586</v>
+      </c>
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>49</v>
+      <c r="I18" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="15"/>
+      <c r="C19">
+        <v>115</v>
+      </c>
+      <c r="D19" t="s">
+        <v>632</v>
+      </c>
+      <c r="E19" t="s">
+        <v>620</v>
+      </c>
+      <c r="F19" t="s">
+        <v>587</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="I19" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="15"/>
+      <c r="C20">
+        <v>116</v>
+      </c>
+      <c r="D20" t="s">
+        <v>672</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>667</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>588</v>
+      </c>
+      <c r="I20" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="15"/>
+      <c r="C21">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>660</v>
+      </c>
+      <c r="E21" t="s">
+        <v>656</v>
+      </c>
+      <c r="F21" t="s">
+        <v>584</v>
+      </c>
+      <c r="G21">
+        <v>20</v>
+      </c>
+      <c r="I21" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="15"/>
+      <c r="C22">
+        <v>118</v>
+      </c>
+      <c r="D22" t="s">
+        <v>661</v>
+      </c>
+      <c r="E22" t="s">
+        <v>623</v>
+      </c>
+      <c r="F22" t="s">
+        <v>585</v>
+      </c>
+      <c r="G22">
+        <v>35</v>
+      </c>
+      <c r="I22" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="15"/>
+      <c r="C23">
+        <v>119</v>
+      </c>
+      <c r="D23" t="s">
+        <v>662</v>
+      </c>
+      <c r="E23" t="s">
+        <v>676</v>
+      </c>
+      <c r="F23" t="s">
+        <v>586</v>
+      </c>
+      <c r="G23">
+        <v>2</v>
+      </c>
+      <c r="I23" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="15"/>
+      <c r="C24">
+        <v>120</v>
+      </c>
+      <c r="D24" t="s">
+        <v>663</v>
+      </c>
+      <c r="E24" t="s">
+        <v>651</v>
+      </c>
+      <c r="F24" t="s">
+        <v>587</v>
+      </c>
+      <c r="G24">
+        <v>100</v>
+      </c>
+      <c r="I24" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>627</v>
+      </c>
+      <c r="C26">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="15"/>
+      <c r="C27">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="15"/>
+      <c r="C28">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="15"/>
+      <c r="C29">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="15"/>
+      <c r="C30">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>628</v>
+      </c>
+      <c r="C32">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="15"/>
+      <c r="C33">
+        <v>132</v>
+      </c>
+      <c r="D33" t="s">
+        <v>634</v>
+      </c>
+      <c r="I33" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="15"/>
+      <c r="C34">
+        <v>133</v>
+      </c>
+      <c r="D34" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="15"/>
+      <c r="C35">
+        <v>134</v>
+      </c>
+      <c r="D35" t="s">
+        <v>637</v>
+      </c>
+      <c r="I35" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="15"/>
+      <c r="C36">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B15:B24"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
v0.6.2n: Terrain DImg and display
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E321BA00-1574-4DEB-A134-B3D45DB49DCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFA1D1A-E9D8-427F-A071-704BF4FFFA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="801">
   <si>
     <t>ID</t>
   </si>
@@ -2445,6 +2445,9 @@
   </si>
   <si>
     <t>Table, wooden</t>
+  </si>
+  <si>
+    <t>Carpet, green</t>
   </si>
 </sst>
 </file>
@@ -2519,6 +2522,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2527,9 +2533,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2847,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2882,52 +2885,55 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>210</v>
+      <c r="B4" s="3">
+        <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>212</v>
+      <c r="E4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>744</v>
+      </c>
+      <c r="D6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>744</v>
-      </c>
-      <c r="D7" t="s">
-        <v>220</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
+        <v>745</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>102</v>
+      <c r="B8" s="4">
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>746</v>
+        <v>800</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3141,7 +3147,7 @@
         <v>247</v>
       </c>
       <c r="E36">
-        <v>1000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
@@ -3454,7 +3460,7 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>712</v>
       </c>
       <c r="C4" t="s">
@@ -3471,7 +3477,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5" t="s">
         <v>682</v>
       </c>
@@ -3486,7 +3492,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6" t="s">
         <v>683</v>
       </c>
@@ -3501,7 +3507,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="16"/>
       <c r="C7" t="s">
         <v>684</v>
       </c>
@@ -3516,7 +3522,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8" t="s">
         <v>685</v>
       </c>
@@ -3531,7 +3537,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9" t="s">
         <v>686</v>
       </c>
@@ -3546,7 +3552,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10" t="s">
         <v>687</v>
       </c>
@@ -3561,7 +3567,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11" t="s">
         <v>688</v>
       </c>
@@ -3576,7 +3582,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12" t="s">
         <v>689</v>
       </c>
@@ -3591,7 +3597,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13" t="s">
         <v>690</v>
       </c>
@@ -3606,7 +3612,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>729</v>
       </c>
       <c r="C15" t="s">
@@ -3620,7 +3626,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16" t="s">
         <v>721</v>
       </c>
@@ -3632,7 +3638,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17" t="s">
         <v>737</v>
       </c>
@@ -3647,7 +3653,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="C18" t="s">
         <v>738</v>
       </c>
@@ -3656,7 +3662,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19" t="s">
         <v>731</v>
       </c>
@@ -3668,7 +3674,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20" t="s">
         <v>720</v>
       </c>
@@ -3683,7 +3689,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
+      <c r="B21" s="16"/>
       <c r="C21" t="s">
         <v>723</v>
       </c>
@@ -3698,7 +3704,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+      <c r="B22" s="16"/>
       <c r="C22" t="s">
         <v>738</v>
       </c>
@@ -3707,7 +3713,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="B23" s="16"/>
       <c r="C23" t="s">
         <v>738</v>
       </c>
@@ -3716,7 +3722,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
+      <c r="B24" s="16"/>
       <c r="C24" t="s">
         <v>735</v>
       </c>
@@ -5525,7 +5531,7 @@
       <c r="E16" t="s">
         <v>543</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="14" t="s">
         <v>559</v>
       </c>
     </row>
@@ -5542,7 +5548,7 @@
       <c r="E17" t="s">
         <v>544</v>
       </c>
-      <c r="F17" s="17"/>
+      <c r="F17" s="14"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
@@ -5557,7 +5563,7 @@
       <c r="E18" t="s">
         <v>555</v>
       </c>
-      <c r="F18" s="17"/>
+      <c r="F18" s="14"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -5572,7 +5578,7 @@
       <c r="E19" t="s">
         <v>556</v>
       </c>
-      <c r="F19" s="17"/>
+      <c r="F19" s="14"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -5767,23 +5773,23 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="K1" s="14" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
       <c r="T1" s="9"/>
       <c r="U1" s="9"/>
     </row>
@@ -9735,7 +9741,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C4">
@@ -9758,7 +9764,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
+      <c r="B5" s="16"/>
       <c r="C5">
         <v>102</v>
       </c>
@@ -9776,7 +9782,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
+      <c r="B6" s="16"/>
       <c r="C6">
         <v>103</v>
       </c>
@@ -9794,7 +9800,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
+      <c r="B7" s="16"/>
       <c r="C7">
         <v>104</v>
       </c>
@@ -9812,7 +9818,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
+      <c r="B8" s="16"/>
       <c r="C8">
         <v>105</v>
       </c>
@@ -9830,7 +9836,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
+      <c r="B9" s="16"/>
       <c r="C9">
         <v>106</v>
       </c>
@@ -9851,7 +9857,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="16"/>
       <c r="C10">
         <v>107</v>
       </c>
@@ -9869,7 +9875,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="16"/>
       <c r="C11">
         <v>108</v>
       </c>
@@ -9887,7 +9893,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="16"/>
       <c r="C12">
         <v>109</v>
       </c>
@@ -9905,7 +9911,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
+      <c r="B13" s="16"/>
       <c r="C13">
         <v>110</v>
       </c>
@@ -9923,7 +9929,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="16" t="s">
         <v>561</v>
       </c>
       <c r="C15">
@@ -9946,7 +9952,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
+      <c r="B16" s="16"/>
       <c r="C16">
         <v>112</v>
       </c>
@@ -9967,7 +9973,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
+      <c r="B17" s="16"/>
       <c r="C17">
         <v>113</v>
       </c>
@@ -9988,7 +9994,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
+      <c r="B18" s="16"/>
       <c r="C18">
         <v>114</v>
       </c>
@@ -10009,7 +10015,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
+      <c r="B19" s="16"/>
       <c r="C19">
         <v>115</v>
       </c>
@@ -10030,7 +10036,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="16"/>
       <c r="C20">
         <v>116</v>
       </c>
@@ -10051,7 +10057,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
+      <c r="B21" s="16"/>
       <c r="C21">
         <v>117</v>
       </c>
@@ -10072,7 +10078,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
+      <c r="B22" s="16"/>
       <c r="C22">
         <v>118</v>
       </c>
@@ -10093,7 +10099,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
+      <c r="B23" s="16"/>
       <c r="C23">
         <v>119</v>
       </c>
@@ -10114,7 +10120,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
+      <c r="B24" s="16"/>
       <c r="C24">
         <v>120</v>
       </c>
@@ -10135,7 +10141,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>627</v>
       </c>
       <c r="C26">
@@ -10143,31 +10149,31 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
+      <c r="B27" s="16"/>
       <c r="C27">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
+      <c r="B28" s="16"/>
       <c r="C28">
         <v>123</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
+      <c r="B29" s="16"/>
       <c r="C29">
         <v>124</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
+      <c r="B30" s="16"/>
       <c r="C30">
         <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="16" t="s">
         <v>628</v>
       </c>
       <c r="C32">
@@ -10175,7 +10181,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
+      <c r="B33" s="16"/>
       <c r="C33">
         <v>132</v>
       </c>
@@ -10187,7 +10193,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="15"/>
+      <c r="B34" s="16"/>
       <c r="C34">
         <v>133</v>
       </c>
@@ -10196,7 +10202,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
+      <c r="B35" s="16"/>
       <c r="C35">
         <v>134</v>
       </c>
@@ -10208,7 +10214,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
+      <c r="B36" s="16"/>
       <c r="C36">
         <v>135</v>
       </c>
@@ -10244,26 +10250,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="H1" s="16" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="H1" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
@@ -10272,13 +10278,13 @@
       <c r="H3" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
v0.6.2o: Added terrain IDs and some images
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFA1D1A-E9D8-427F-A071-704BF4FFFA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA3FEA6-964E-4F5F-B94E-1BE46FD11BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="800">
   <si>
     <t>ID</t>
   </si>
@@ -2342,15 +2342,6 @@
     <t>Grass, line up</t>
   </si>
   <si>
-    <t>Road1</t>
-  </si>
-  <si>
-    <t>Road2</t>
-  </si>
-  <si>
-    <t>Road3</t>
-  </si>
-  <si>
     <t>Road, white up</t>
   </si>
   <si>
@@ -2444,10 +2435,16 @@
     <t>Stairs</t>
   </si>
   <si>
-    <t>Table, wooden</t>
-  </si>
-  <si>
     <t>Carpet, green</t>
+  </si>
+  <si>
+    <t>Road, light</t>
+  </si>
+  <si>
+    <t>Road, asphalt</t>
+  </si>
+  <si>
+    <t>Road, dark</t>
   </si>
 </sst>
 </file>
@@ -2850,8 +2847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,7 +2930,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>800</v>
+        <v>796</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3069,7 +3066,7 @@
         <v>171</v>
       </c>
       <c r="C26" t="s">
-        <v>765</v>
+        <v>797</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3077,7 +3074,7 @@
         <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>766</v>
+        <v>798</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3085,7 +3082,7 @@
         <v>173</v>
       </c>
       <c r="C28" t="s">
-        <v>767</v>
+        <v>799</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3093,7 +3090,7 @@
         <v>174</v>
       </c>
       <c r="C29" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3101,7 +3098,7 @@
         <v>175</v>
       </c>
       <c r="C30" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3109,7 +3106,7 @@
         <v>176</v>
       </c>
       <c r="C31" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3117,7 +3114,7 @@
         <v>177</v>
       </c>
       <c r="C32" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
@@ -3125,7 +3122,7 @@
         <v>178</v>
       </c>
       <c r="C33" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
@@ -3133,7 +3130,7 @@
         <v>179</v>
       </c>
       <c r="C34" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
@@ -3141,7 +3138,7 @@
         <v>201</v>
       </c>
       <c r="C36" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D36" t="s">
         <v>247</v>
@@ -3155,7 +3152,7 @@
         <v>202</v>
       </c>
       <c r="C37" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
@@ -3163,7 +3160,7 @@
         <v>203</v>
       </c>
       <c r="C38" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
@@ -3171,7 +3168,7 @@
         <v>204</v>
       </c>
       <c r="C39" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -3179,7 +3176,7 @@
         <v>205</v>
       </c>
       <c r="C40" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -3187,7 +3184,7 @@
         <v>206</v>
       </c>
       <c r="C41" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
@@ -3195,7 +3192,7 @@
         <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
@@ -3211,13 +3208,13 @@
         <v>301</v>
       </c>
       <c r="C45" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D45" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="E45" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -3225,10 +3222,10 @@
         <v>302</v>
       </c>
       <c r="C46" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="E46" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
@@ -3236,10 +3233,10 @@
         <v>303</v>
       </c>
       <c r="C47" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E47" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
@@ -3247,10 +3244,10 @@
         <v>304</v>
       </c>
       <c r="C48" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E48" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3258,10 +3255,10 @@
         <v>305</v>
       </c>
       <c r="C49" t="s">
-        <v>781</v>
+        <v>778</v>
       </c>
       <c r="E49" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
@@ -3269,10 +3266,10 @@
         <v>306</v>
       </c>
       <c r="C50" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="E50" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -3280,10 +3277,10 @@
         <v>307</v>
       </c>
       <c r="C51" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="E51" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -3291,10 +3288,10 @@
         <v>308</v>
       </c>
       <c r="C52" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="E52" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -3302,10 +3299,10 @@
         <v>309</v>
       </c>
       <c r="C53" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="E53" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -3313,10 +3310,10 @@
         <v>310</v>
       </c>
       <c r="C54" t="s">
+        <v>791</v>
+      </c>
+      <c r="E54" t="s">
         <v>794</v>
-      </c>
-      <c r="E54" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -3324,10 +3321,10 @@
         <v>311</v>
       </c>
       <c r="C55" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="E55" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -3335,10 +3332,10 @@
         <v>312</v>
       </c>
       <c r="C56" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="E56" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -3346,10 +3343,10 @@
         <v>313</v>
       </c>
       <c r="C57" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="E57" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3357,10 +3354,10 @@
         <v>314</v>
       </c>
       <c r="C58" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="E58" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -3368,10 +3365,10 @@
         <v>315</v>
       </c>
       <c r="C59" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="E59" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
@@ -3379,24 +3376,10 @@
         <v>316</v>
       </c>
       <c r="C60" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="E60" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="4">
-        <v>321</v>
-      </c>
-      <c r="C61" t="s">
-        <v>799</v>
-      </c>
-      <c r="D61" t="s">
-        <v>283</v>
-      </c>
-      <c r="E61">
-        <v>3</v>
+        <v>794</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.2p: Can add/change terrain in GameMapEditor
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA3FEA6-964E-4F5F-B94E-1BE46FD11BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5581265E-EF39-4B24-802F-8B4FE6560828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="812">
   <si>
     <t>ID</t>
   </si>
@@ -2445,6 +2445,42 @@
   </si>
   <si>
     <t>Road, dark</t>
+  </si>
+  <si>
+    <t>Sand, light</t>
+  </si>
+  <si>
+    <t>Sand, tan</t>
+  </si>
+  <si>
+    <t>Sand, dark</t>
+  </si>
+  <si>
+    <t>Sand, line left</t>
+  </si>
+  <si>
+    <t>Sand, line up</t>
+  </si>
+  <si>
+    <t>Sidewalk, smooth</t>
+  </si>
+  <si>
+    <t>Sidewalk, cracked</t>
+  </si>
+  <si>
+    <t>Water, rocks</t>
+  </si>
+  <si>
+    <t>Water, dirt</t>
+  </si>
+  <si>
+    <t>Water, shallow</t>
+  </si>
+  <si>
+    <t>Water, medium</t>
+  </si>
+  <si>
+    <t>Water, deep</t>
   </si>
 </sst>
 </file>
@@ -2845,10 +2881,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2991,359 +3027,323 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="4">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>756</v>
+        <v>805</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
-        <v>152</v>
+      <c r="B18" s="4">
+        <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>757</v>
+        <v>806</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>758</v>
+        <v>800</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>759</v>
+        <v>801</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C21" t="s">
-        <v>763</v>
+        <v>802</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="4">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C22" t="s">
-        <v>764</v>
+        <v>803</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="3">
-        <v>161</v>
+      <c r="B23" s="4">
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>760</v>
+        <v>804</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C24" t="s">
-        <v>761</v>
+        <v>756</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="4">
-        <v>163</v>
+      <c r="B25" s="3">
+        <v>152</v>
       </c>
       <c r="C25" t="s">
-        <v>762</v>
+        <v>757</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C26" t="s">
-        <v>797</v>
+        <v>758</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="6">
-        <v>172</v>
+      <c r="B27" s="4">
+        <v>154</v>
       </c>
       <c r="C27" t="s">
-        <v>798</v>
+        <v>759</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="C28" t="s">
-        <v>799</v>
+        <v>763</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="6">
-        <v>174</v>
+      <c r="B29" s="4">
+        <v>156</v>
       </c>
       <c r="C29" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4">
-        <v>175</v>
+      <c r="B30" s="3">
+        <v>161</v>
       </c>
       <c r="C30" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="6">
-        <v>176</v>
+      <c r="B31" s="4">
+        <v>162</v>
       </c>
       <c r="C31" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="4">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="C32" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C33" t="s">
-        <v>769</v>
+        <v>797</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="3">
-        <v>179</v>
+      <c r="B34" s="6">
+        <v>172</v>
       </c>
       <c r="C34" t="s">
-        <v>770</v>
+        <v>798</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="4">
+        <v>173</v>
+      </c>
+      <c r="C35" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="4">
-        <v>201</v>
+      <c r="B36" s="6">
+        <v>174</v>
       </c>
       <c r="C36" t="s">
-        <v>771</v>
-      </c>
-      <c r="D36" t="s">
-        <v>247</v>
-      </c>
-      <c r="E36">
-        <v>100</v>
+        <v>765</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="3">
-        <v>202</v>
+      <c r="B37" s="4">
+        <v>175</v>
       </c>
       <c r="C37" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="4">
-        <v>203</v>
+      <c r="B38" s="6">
+        <v>176</v>
       </c>
       <c r="C38" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
-        <v>204</v>
+      <c r="B39" s="4">
+        <v>177</v>
       </c>
       <c r="C39" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
-        <v>205</v>
+        <v>178</v>
       </c>
       <c r="C40" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="3">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="4">
-        <v>207</v>
+      <c r="B42" s="3">
+        <v>181</v>
       </c>
       <c r="C42" t="s">
-        <v>772</v>
+        <v>807</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="3">
-        <v>211</v>
+        <v>182</v>
+      </c>
+      <c r="C43" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
+      <c r="B44" s="3">
+        <v>183</v>
+      </c>
+      <c r="C44" t="s">
+        <v>809</v>
+      </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="4">
-        <v>301</v>
+      <c r="B45" s="3">
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>782</v>
-      </c>
-      <c r="D45" t="s">
-        <v>795</v>
-      </c>
-      <c r="E45" t="s">
-        <v>794</v>
+        <v>810</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="4">
-        <v>302</v>
+      <c r="B46" s="3">
+        <v>185</v>
       </c>
       <c r="C46" t="s">
-        <v>783</v>
-      </c>
-      <c r="E46" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="4">
-        <v>303</v>
-      </c>
-      <c r="C47" t="s">
-        <v>784</v>
-      </c>
-      <c r="E47" t="s">
-        <v>794</v>
+        <v>811</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="4">
-        <v>304</v>
+        <v>201</v>
       </c>
       <c r="C48" t="s">
-        <v>785</v>
-      </c>
-      <c r="E48" t="s">
-        <v>794</v>
+        <v>771</v>
+      </c>
+      <c r="D48" t="s">
+        <v>247</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="4">
-        <v>305</v>
+      <c r="B49" s="3">
+        <v>202</v>
       </c>
       <c r="C49" t="s">
-        <v>778</v>
-      </c>
-      <c r="E49" t="s">
-        <v>794</v>
+        <v>776</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="4">
-        <v>306</v>
+        <v>203</v>
       </c>
       <c r="C50" t="s">
-        <v>779</v>
-      </c>
-      <c r="E50" t="s">
-        <v>794</v>
+        <v>777</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="4">
-        <v>307</v>
+      <c r="B51" s="3">
+        <v>204</v>
       </c>
       <c r="C51" t="s">
-        <v>780</v>
-      </c>
-      <c r="E51" t="s">
-        <v>794</v>
+        <v>774</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="4">
-        <v>308</v>
+        <v>205</v>
       </c>
       <c r="C52" t="s">
-        <v>781</v>
-      </c>
-      <c r="E52" t="s">
-        <v>794</v>
+        <v>775</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="4">
-        <v>309</v>
+      <c r="B53" s="3">
+        <v>206</v>
       </c>
       <c r="C53" t="s">
-        <v>790</v>
-      </c>
-      <c r="E53" t="s">
-        <v>794</v>
+        <v>773</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
-        <v>310</v>
+        <v>207</v>
       </c>
       <c r="C54" t="s">
-        <v>791</v>
-      </c>
-      <c r="E54" t="s">
-        <v>794</v>
+        <v>772</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="4">
-        <v>311</v>
-      </c>
-      <c r="C55" t="s">
-        <v>792</v>
-      </c>
-      <c r="E55" t="s">
-        <v>794</v>
+      <c r="B55" s="3">
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="4">
-        <v>312</v>
-      </c>
-      <c r="C56" t="s">
-        <v>793</v>
-      </c>
-      <c r="E56" t="s">
-        <v>794</v>
-      </c>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
-        <v>313</v>
+        <v>301</v>
       </c>
       <c r="C57" t="s">
-        <v>789</v>
+        <v>782</v>
+      </c>
+      <c r="D57" t="s">
+        <v>795</v>
       </c>
       <c r="E57" t="s">
         <v>794</v>
@@ -3351,10 +3351,10 @@
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="4">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C58" t="s">
-        <v>788</v>
+        <v>783</v>
       </c>
       <c r="E58" t="s">
         <v>794</v>
@@ -3362,10 +3362,10 @@
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
-        <v>315</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="E59" t="s">
         <v>794</v>
@@ -3373,32 +3373,164 @@
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="4">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="C60" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E60" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="4">
+        <v>305</v>
+      </c>
+      <c r="C61" t="s">
+        <v>778</v>
+      </c>
+      <c r="E61" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="4">
+        <v>306</v>
+      </c>
+      <c r="C62" t="s">
+        <v>779</v>
+      </c>
+      <c r="E62" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B63" s="4">
+        <v>307</v>
+      </c>
+      <c r="C63" t="s">
+        <v>780</v>
+      </c>
+      <c r="E63" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B64" s="4">
+        <v>308</v>
+      </c>
+      <c r="C64" t="s">
+        <v>781</v>
+      </c>
+      <c r="E64" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B65" s="4">
+        <v>309</v>
+      </c>
+      <c r="C65" t="s">
+        <v>790</v>
+      </c>
+      <c r="E65" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="4">
+        <v>310</v>
+      </c>
+      <c r="C66" t="s">
+        <v>791</v>
+      </c>
+      <c r="E66" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="4">
+        <v>311</v>
+      </c>
+      <c r="C67" t="s">
+        <v>792</v>
+      </c>
+      <c r="E67" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="4">
+        <v>312</v>
+      </c>
+      <c r="C68" t="s">
+        <v>793</v>
+      </c>
+      <c r="E68" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="4">
+        <v>313</v>
+      </c>
+      <c r="C69" t="s">
+        <v>789</v>
+      </c>
+      <c r="E69" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="4">
+        <v>314</v>
+      </c>
+      <c r="C70" t="s">
+        <v>788</v>
+      </c>
+      <c r="E70" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="4">
+        <v>315</v>
+      </c>
+      <c r="C71" t="s">
+        <v>787</v>
+      </c>
+      <c r="E71" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="4">
+        <v>316</v>
+      </c>
+      <c r="C72" t="s">
+        <v>786</v>
+      </c>
+      <c r="E72" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
v0.6.2x: Fog features, can toggle fog and grid on/off in MapEditor
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C3FADA-D972-4263-B273-2C304D939693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787DDDF1-8976-4AB1-B714-23AD75460246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="795">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="796">
   <si>
     <t>ID</t>
   </si>
@@ -2414,9 +2414,6 @@
     <t>Gravel</t>
   </si>
   <si>
-    <t>id 1-10 has 10-100% opacity</t>
-  </si>
-  <si>
     <t>covers map</t>
   </si>
   <si>
@@ -2430,6 +2427,12 @@
   </si>
   <si>
     <t>inventory (furniture)</t>
+  </si>
+  <si>
+    <t>id 1-10 has 100-10% opacity</t>
+  </si>
+  <si>
+    <t>height</t>
   </si>
 </sst>
 </file>
@@ -3936,29 +3939,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" style="4"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="41" customWidth="1"/>
-    <col min="7" max="7" width="78.7109375" customWidth="1"/>
+    <col min="4" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" customWidth="1"/>
+    <col min="8" max="8" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>718</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
@@ -3968,14 +3971,17 @@
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>210</v>
       </c>
@@ -3985,14 +3991,17 @@
       <c r="D4" t="s">
         <v>211</v>
       </c>
-      <c r="F4" t="s">
-        <v>790</v>
+      <c r="E4">
+        <v>0</v>
       </c>
       <c r="G4" t="s">
         <v>789</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="4">
         <v>11</v>
       </c>
@@ -4000,18 +4009,24 @@
         <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>791</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>790</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="4">
         <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4">
         <v>21</v>
       </c>
@@ -4021,41 +4036,50 @@
       <c r="D8" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="4">
         <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
         <v>101</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="G11" t="s">
-        <v>793</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <v>111</v>
       </c>
       <c r="C12" t="s">
         <v>252</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="4">
         <v>101</v>
       </c>
@@ -4065,70 +4089,70 @@
       <c r="D19" t="s">
         <v>260</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>218</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4">
         <v>304</v>
       </c>
       <c r="C20" t="s">
         <v>255</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>218</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>257</v>
       </c>
       <c r="C21" t="s">
         <v>256</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>218</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C22" t="s">
         <v>259</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>218</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C23" t="s">
         <v>262</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>218</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>263</v>
       </c>
@@ -4136,147 +4160,147 @@
         <v>255</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>264</v>
       </c>
       <c r="C25" t="s">
         <v>265</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>218</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="4">
         <v>325</v>
       </c>
       <c r="C26" t="s">
         <v>266</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>218</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <v>326</v>
       </c>
       <c r="C27" t="s">
         <v>267</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>218</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <v>327</v>
       </c>
       <c r="C28" t="s">
         <v>268</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>218</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <v>328</v>
       </c>
       <c r="C29" t="s">
         <v>270</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>218</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <v>329</v>
       </c>
       <c r="C30" t="s">
         <v>271</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>218</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>273</v>
       </c>
       <c r="C31" t="s">
         <v>274</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>218</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="4">
         <v>155</v>
       </c>
       <c r="C33" t="s">
         <v>219</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>218</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4">
         <v>157</v>
       </c>
       <c r="C34" t="s">
         <v>220</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>218</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4">
         <v>158</v>
       </c>
       <c r="C35" t="s">
         <v>221</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>218</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>223</v>
       </c>
@@ -4286,98 +4310,98 @@
       <c r="D37" t="s">
         <v>225</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>218</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="4">
         <v>217</v>
       </c>
       <c r="C38" t="s">
         <v>229</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>218</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="4">
         <v>218</v>
       </c>
       <c r="C39" t="s">
         <v>228</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>218</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="4">
         <v>219</v>
       </c>
       <c r="C40" t="s">
         <v>230</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>218</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>235</v>
       </c>
       <c r="C41" t="s">
         <v>232</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>218</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
         <v>234</v>
       </c>
       <c r="C42" t="s">
         <v>248</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>218</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="4" t="s">
         <v>237</v>
       </c>
       <c r="C43" t="s">
         <v>238</v>
       </c>
-      <c r="E43" t="s">
+      <c r="F43" t="s">
         <v>218</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>239</v>
       </c>
@@ -4385,21 +4409,21 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="4">
         <v>235</v>
       </c>
       <c r="C45" t="s">
         <v>241</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>218</v>
       </c>
-      <c r="F45" t="s">
+      <c r="G45" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
         <v>242</v>
       </c>
@@ -4407,7 +4431,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="4">
         <v>238</v>
       </c>
@@ -4415,189 +4439,189 @@
         <v>244</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>245</v>
       </c>
       <c r="C48" t="s">
         <v>241</v>
       </c>
-      <c r="E48" t="s">
+      <c r="F48" t="s">
         <v>218</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>246</v>
       </c>
       <c r="C49" t="s">
         <v>232</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>218</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>247</v>
       </c>
       <c r="C50" t="s">
         <v>248</v>
       </c>
-      <c r="E50" t="s">
+      <c r="F50" t="s">
         <v>218</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>249</v>
       </c>
       <c r="C51" t="s">
         <v>232</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>218</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="4" t="s">
         <v>250</v>
       </c>
       <c r="C52" t="s">
         <v>238</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>218</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B54" s="4">
         <v>401</v>
       </c>
       <c r="C54" t="s">
         <v>275</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>218</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="4">
         <v>402</v>
       </c>
       <c r="C55" t="s">
         <v>276</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>218</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="4">
         <v>403</v>
       </c>
       <c r="C56" t="s">
         <v>277</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>218</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B57" s="4">
         <v>404</v>
       </c>
       <c r="C57" t="s">
         <v>278</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>218</v>
       </c>
-      <c r="F57" t="s">
-        <v>794</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
         <v>279</v>
       </c>
       <c r="C58" t="s">
         <v>280</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>218</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
         <v>407</v>
       </c>
       <c r="C59" t="s">
         <v>281</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>218</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B60" s="4">
         <v>408</v>
       </c>
       <c r="C60" t="s">
         <v>282</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>218</v>
       </c>
-      <c r="F60" t="s">
+      <c r="G60" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B61" s="4">
         <v>409</v>
       </c>
       <c r="C61" t="s">
         <v>283</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>218</v>
       </c>
-      <c r="F61" t="s">
+      <c r="G61" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>285</v>
       </c>
@@ -4607,42 +4631,42 @@
       <c r="D63" t="s">
         <v>291</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>218</v>
       </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>286</v>
       </c>
       <c r="C64" t="s">
         <v>289</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>218</v>
       </c>
-      <c r="F64" t="s">
+      <c r="G64" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>288</v>
       </c>
       <c r="C65" t="s">
         <v>287</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>218</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>292</v>
       </c>
@@ -4650,7 +4674,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" s="4">
         <v>548</v>
       </c>
@@ -4658,7 +4682,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>294</v>
       </c>
@@ -4666,21 +4690,21 @@
         <v>295</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>296</v>
       </c>
       <c r="C69" t="s">
         <v>297</v>
       </c>
-      <c r="E69" t="s">
+      <c r="F69" t="s">
         <v>218</v>
       </c>
-      <c r="F69" t="s">
+      <c r="G69" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" s="4">
         <v>555</v>
       </c>
@@ -4688,7 +4712,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" s="4" t="s">
         <v>300</v>
       </c>
@@ -4696,7 +4720,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" s="4" t="s">
         <v>301</v>
       </c>
@@ -4704,7 +4728,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" s="4">
         <v>601</v>
       </c>
@@ -4715,7 +4739,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" s="4">
         <v>602</v>
       </c>
@@ -4723,7 +4747,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" s="4">
         <v>603</v>
       </c>
@@ -4731,7 +4755,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" s="4">
         <v>604</v>
       </c>
@@ -4739,7 +4763,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" s="4">
         <v>605</v>
       </c>
@@ -4747,7 +4771,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" s="4">
         <v>606</v>
       </c>
@@ -4755,7 +4779,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" s="4">
         <v>607</v>
       </c>
@@ -5692,7 +5716,7 @@
   <dimension ref="A1:Y199"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="J75" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S150" sqref="S150"/>

</xml_diff>

<commit_message>
v0.6.3a: Added stairway terrains
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787DDDF1-8976-4AB1-B714-23AD75460246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4656F7A4-3EF0-4B5B-9962-86D2E7EB1D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="804">
   <si>
     <t>ID</t>
   </si>
@@ -2357,9 +2357,6 @@
     <t>Stair, red, right</t>
   </si>
   <si>
-    <t>1-3 in grid</t>
-  </si>
-  <si>
     <t>Stairs</t>
   </si>
   <si>
@@ -2433,6 +2430,33 @@
   </si>
   <si>
     <t>height</t>
+  </si>
+  <si>
+    <t>0, allows movement up 3</t>
+  </si>
+  <si>
+    <t>Stairway, green, up</t>
+  </si>
+  <si>
+    <t>Stairway, green, down</t>
+  </si>
+  <si>
+    <t>Stairway, green, left</t>
+  </si>
+  <si>
+    <t>Stairway, green, right</t>
+  </si>
+  <si>
+    <t>Stairway, red, up</t>
+  </si>
+  <si>
+    <t>Stairway, red, down</t>
+  </si>
+  <si>
+    <t>Stairway, red, left</t>
+  </si>
+  <si>
+    <t>Stairway, red, right</t>
   </si>
 </sst>
 </file>
@@ -2833,10 +2857,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
-  <dimension ref="A1:E84"/>
+  <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,7 +2868,7 @@
     <col min="2" max="2" width="9.140625" style="4"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="41" customWidth="1"/>
     <col min="7" max="7" width="78.7109375" customWidth="1"/>
   </cols>
@@ -2918,7 +2942,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2982,7 +3006,7 @@
         <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -2990,7 +3014,7 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -2998,7 +3022,7 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3006,7 +3030,7 @@
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3014,7 +3038,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3022,7 +3046,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3030,7 +3054,7 @@
         <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3038,7 +3062,7 @@
         <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3118,7 +3142,7 @@
         <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -3126,7 +3150,7 @@
         <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -3134,7 +3158,7 @@
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -3190,7 +3214,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -3198,7 +3222,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -3206,7 +3230,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -3214,7 +3238,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -3222,7 +3246,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3288,209 +3312,211 @@
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="3">
-        <v>211</v>
-      </c>
+      <c r="B56" s="3"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
+      <c r="B57" s="4">
+        <v>301</v>
+      </c>
+      <c r="C57" t="s">
+        <v>758</v>
+      </c>
+      <c r="D57" t="s">
+        <v>770</v>
+      </c>
+      <c r="E57" t="s">
+        <v>795</v>
+      </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="4">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C58" t="s">
-        <v>758</v>
-      </c>
-      <c r="D58" t="s">
-        <v>771</v>
-      </c>
-      <c r="E58" t="s">
-        <v>770</v>
+        <v>759</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="4">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C59" t="s">
-        <v>759</v>
-      </c>
-      <c r="E59" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="4">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C60" t="s">
-        <v>760</v>
-      </c>
-      <c r="E60" t="s">
-        <v>770</v>
+        <v>761</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="4">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C61" t="s">
-        <v>761</v>
-      </c>
-      <c r="E61" t="s">
-        <v>770</v>
+        <v>754</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="4">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C62" t="s">
-        <v>754</v>
-      </c>
-      <c r="E62" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" s="4">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C63" t="s">
-        <v>755</v>
-      </c>
-      <c r="E63" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" s="4">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C64" t="s">
-        <v>756</v>
-      </c>
-      <c r="E64" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="4">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C65" t="s">
-        <v>757</v>
-      </c>
-      <c r="E65" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="4">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C66" t="s">
-        <v>766</v>
-      </c>
-      <c r="E66" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="4">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C67" t="s">
-        <v>767</v>
-      </c>
-      <c r="E67" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="4">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C68" t="s">
-        <v>768</v>
-      </c>
-      <c r="E68" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="4">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C69" t="s">
-        <v>769</v>
-      </c>
-      <c r="E69" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="4">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C70" t="s">
-        <v>765</v>
-      </c>
-      <c r="E70" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="4">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C71" t="s">
-        <v>764</v>
-      </c>
-      <c r="E71" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="4">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C72" t="s">
-        <v>763</v>
-      </c>
-      <c r="E72" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C73" t="s">
-        <v>762</v>
-      </c>
-      <c r="E73" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
+        <v>796</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="4">
+        <v>318</v>
+      </c>
+      <c r="C74" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="4">
+        <v>319</v>
+      </c>
+      <c r="C75" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="4">
+        <v>320</v>
+      </c>
+      <c r="C76" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="4">
+        <v>321</v>
+      </c>
+      <c r="C77" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="4">
+        <v>322</v>
+      </c>
+      <c r="C78" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="4">
+        <v>323</v>
+      </c>
+      <c r="C79" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>324</v>
+      </c>
+      <c r="C80" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3941,7 +3967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -3972,7 +3998,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>226</v>
@@ -3995,10 +4021,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H4" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4009,7 +4035,7 @@
         <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E6">
         <v>6</v>
@@ -4056,7 +4082,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>260</v>
@@ -4065,7 +4091,7 @@
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4562,7 +4588,7 @@
         <v>218</v>
       </c>
       <c r="G57" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.3c: Updated feature constructor
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4719FC0-A524-48EB-AF7D-98E97A0E72BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5026B144-02A4-48DE-864D-EAA739B0F46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -2327,9 +2327,6 @@
     <t>Sign, gray</t>
   </si>
   <si>
-    <t>Fridge</t>
-  </si>
-  <si>
     <t>food</t>
   </si>
   <si>
@@ -2502,6 +2499,9 @@
   </si>
   <si>
     <t>Appliance</t>
+  </si>
+  <si>
+    <t>Refridgerator</t>
   </si>
 </sst>
 </file>
@@ -3358,7 +3358,7 @@
         <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -3366,7 +3366,7 @@
         <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3374,7 +3374,7 @@
         <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -4033,8 +4033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4118,7 +4118,7 @@
         <v>214</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" t="s">
         <v>755</v>
@@ -4302,7 +4302,7 @@
         <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E23">
         <v>2</v>
@@ -4311,7 +4311,7 @@
         <v>753</v>
       </c>
       <c r="H23" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4319,7 +4319,7 @@
         <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -4341,7 +4341,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4352,7 +4352,7 @@
         <v>229</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
         <v>341</v>
@@ -4567,7 +4567,7 @@
         <v>238</v>
       </c>
       <c r="D46" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -4590,7 +4590,7 @@
         <v>344</v>
       </c>
       <c r="H47" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -4604,7 +4604,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>760</v>
+        <v>818</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -4733,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4741,7 +4741,7 @@
         <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E58">
         <v>5</v>
@@ -4766,7 +4766,7 @@
         <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="H60" t="s">
         <v>747</v>
@@ -4788,7 +4788,7 @@
         <v>224</v>
       </c>
       <c r="D62" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E62">
         <v>100</v>
@@ -4811,27 +4811,27 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C64" t="s">
         <v>250</v>
       </c>
       <c r="D64" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="G64" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="H64" t="s">
         <v>805</v>
-      </c>
-      <c r="H64" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C65" t="s">
         <v>249</v>
@@ -4843,7 +4843,7 @@
         <v>508</v>
       </c>
       <c r="H65" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4854,7 +4854,7 @@
         <v>254</v>
       </c>
       <c r="D66" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E66">
         <v>1</v>
@@ -4877,7 +4877,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C69" t="s">
         <v>219</v>
@@ -4889,10 +4889,10 @@
         <v>100</v>
       </c>
       <c r="G69" t="s">
+        <v>763</v>
+      </c>
+      <c r="H69" t="s">
         <v>764</v>
-      </c>
-      <c r="H69" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4906,7 +4906,7 @@
         <v>508</v>
       </c>
       <c r="H70" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4914,7 +4914,7 @@
         <v>312</v>
       </c>
       <c r="H71" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4922,27 +4922,33 @@
         <v>321</v>
       </c>
       <c r="C72" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D72" t="s">
-        <v>766</v>
+        <v>765</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H72" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B73" s="4">
         <v>322</v>
       </c>
+      <c r="E73">
+        <v>100</v>
+      </c>
       <c r="G73" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H73" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4950,10 +4956,10 @@
         <v>323</v>
       </c>
       <c r="G74" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H74" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4962,16 +4968,19 @@
         <v>331</v>
       </c>
       <c r="C75" t="s">
+        <v>784</v>
+      </c>
+      <c r="D75" t="s">
+        <v>783</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>770</v>
+      </c>
+      <c r="H75" t="s">
         <v>785</v>
-      </c>
-      <c r="D75" t="s">
-        <v>784</v>
-      </c>
-      <c r="G75" t="s">
-        <v>771</v>
-      </c>
-      <c r="H75" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4980,7 +4989,7 @@
         <v>332</v>
       </c>
       <c r="H76" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4989,7 +4998,7 @@
         <v>333</v>
       </c>
       <c r="H77" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -4998,7 +5007,7 @@
         <v>334</v>
       </c>
       <c r="H78" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -5007,7 +5016,7 @@
         <v>335</v>
       </c>
       <c r="H79" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -5016,7 +5025,7 @@
         <v>336</v>
       </c>
       <c r="H80" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -5025,7 +5034,7 @@
         <v>337</v>
       </c>
       <c r="H81" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -5034,7 +5043,7 @@
         <v>338</v>
       </c>
       <c r="H82" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -5043,10 +5052,13 @@
         <v>339</v>
       </c>
       <c r="C83" t="s">
-        <v>794</v>
+        <v>793</v>
+      </c>
+      <c r="E83">
+        <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H83" t="s">
         <v>747</v>
@@ -5067,7 +5079,7 @@
         <v>341</v>
       </c>
       <c r="H85" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -5076,7 +5088,7 @@
         <v>342</v>
       </c>
       <c r="H86" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -5085,10 +5097,10 @@
         <v>343</v>
       </c>
       <c r="C87" t="s">
+        <v>794</v>
+      </c>
+      <c r="G87" t="s">
         <v>795</v>
-      </c>
-      <c r="G87" t="s">
-        <v>796</v>
       </c>
       <c r="H87" t="s">
         <v>747</v>
@@ -5109,7 +5121,7 @@
         <v>345</v>
       </c>
       <c r="H89" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -5118,7 +5130,7 @@
         <v>346</v>
       </c>
       <c r="H90" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -5152,7 +5164,7 @@
         <v>304</v>
       </c>
       <c r="H93" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,7 +5175,7 @@
         <v>305</v>
       </c>
       <c r="H94" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -5171,7 +5183,7 @@
         <v>421</v>
       </c>
       <c r="C95" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E95">
         <v>20</v>
@@ -5185,7 +5197,7 @@
         <v>422</v>
       </c>
       <c r="C96" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -5193,7 +5205,7 @@
         <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -5201,7 +5213,7 @@
         <v>424</v>
       </c>
       <c r="C98" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -5209,7 +5221,7 @@
         <v>425</v>
       </c>
       <c r="C99" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E99">
         <v>35</v>
@@ -5228,19 +5240,19 @@
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="3">
-        <v>431</v>
+        <v>441</v>
       </c>
       <c r="C101" t="s">
         <v>252</v>
       </c>
       <c r="E101">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G101" t="s">
         <v>343</v>
       </c>
       <c r="H101" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -5248,7 +5260,7 @@
         <v>442</v>
       </c>
       <c r="H102" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -5256,7 +5268,7 @@
         <v>443</v>
       </c>
       <c r="H103" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
@@ -5269,6 +5281,9 @@
       <c r="D105" t="s">
         <v>255</v>
       </c>
+      <c r="E105">
+        <v>5</v>
+      </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="4">
@@ -5308,6 +5323,9 @@
       </c>
       <c r="C110" t="s">
         <v>261</v>
+      </c>
+      <c r="E110">
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.3e: Added initial units
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A588387-542D-43BE-A82D-7430E5C752A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{475EA508-45DB-46D2-BFEE-BD4491B16876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="823">
   <si>
     <t>ID</t>
   </si>
@@ -1505,9 +1505,6 @@
     <t>Mark Spinny</t>
   </si>
   <si>
-    <t>Michael Mattus</t>
-  </si>
-  <si>
     <t>Jeremiah</t>
   </si>
   <si>
@@ -2502,6 +2499,21 @@
   </si>
   <si>
     <t>unlocks with key</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Gaia</t>
+  </si>
+  <si>
+    <t>Mad Dog Mattus</t>
+  </si>
+  <si>
+    <t>Confederacy</t>
+  </si>
+  <si>
+    <t>Hero</t>
   </si>
 </sst>
 </file>
@@ -2917,7 +2929,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -2929,10 +2941,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2943,7 +2955,7 @@
         <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -2954,7 +2966,7 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D6" t="s">
         <v>217</v>
@@ -2968,7 +2980,7 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2976,7 +2988,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2984,7 +2996,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2992,7 +3004,7 @@
         <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3000,7 +3012,7 @@
         <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3008,7 +3020,7 @@
         <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3016,7 +3028,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3024,7 +3036,7 @@
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3032,7 +3044,7 @@
         <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3048,7 +3060,7 @@
         <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3056,7 +3068,7 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3064,7 +3076,7 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3072,7 +3084,7 @@
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3080,7 +3092,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3088,7 +3100,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3096,7 +3108,7 @@
         <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3104,7 +3116,7 @@
         <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3112,7 +3124,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3120,7 +3132,7 @@
         <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3128,7 +3140,7 @@
         <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3136,7 +3148,7 @@
         <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3144,7 +3156,7 @@
         <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3152,7 +3164,7 @@
         <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3160,7 +3172,7 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3168,7 +3180,7 @@
         <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -3176,7 +3188,7 @@
         <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -3184,7 +3196,7 @@
         <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -3192,7 +3204,7 @@
         <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -3200,7 +3212,7 @@
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -3208,7 +3220,7 @@
         <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -3216,7 +3228,7 @@
         <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -3224,7 +3236,7 @@
         <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -3232,7 +3244,7 @@
         <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -3240,7 +3252,7 @@
         <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -3248,7 +3260,7 @@
         <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -3256,7 +3268,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -3264,7 +3276,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -3272,7 +3284,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -3280,7 +3292,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -3288,7 +3300,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3296,7 +3308,7 @@
         <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D49" t="s">
         <v>220</v>
@@ -3310,7 +3322,7 @@
         <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -3318,7 +3330,7 @@
         <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -3326,7 +3338,7 @@
         <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -3334,7 +3346,7 @@
         <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -3342,7 +3354,7 @@
         <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -3350,7 +3362,7 @@
         <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -3358,7 +3370,7 @@
         <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -3366,7 +3378,7 @@
         <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3374,7 +3386,7 @@
         <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -3385,13 +3397,13 @@
         <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D60" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E60" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -3399,7 +3411,7 @@
         <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -3407,7 +3419,7 @@
         <v>303</v>
       </c>
       <c r="C62" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -3415,7 +3427,7 @@
         <v>304</v>
       </c>
       <c r="C63" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -3423,7 +3435,7 @@
         <v>305</v>
       </c>
       <c r="C64" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -3431,7 +3443,7 @@
         <v>306</v>
       </c>
       <c r="C65" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -3439,7 +3451,7 @@
         <v>307</v>
       </c>
       <c r="C66" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -3447,7 +3459,7 @@
         <v>308</v>
       </c>
       <c r="C67" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -3455,7 +3467,7 @@
         <v>309</v>
       </c>
       <c r="C68" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -3463,7 +3475,7 @@
         <v>310</v>
       </c>
       <c r="C69" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -3471,7 +3483,7 @@
         <v>311</v>
       </c>
       <c r="C70" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -3479,7 +3491,7 @@
         <v>312</v>
       </c>
       <c r="C71" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -3487,7 +3499,7 @@
         <v>313</v>
       </c>
       <c r="C72" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -3495,7 +3507,7 @@
         <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -3503,7 +3515,7 @@
         <v>315</v>
       </c>
       <c r="C74" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -3511,7 +3523,7 @@
         <v>316</v>
       </c>
       <c r="C75" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
@@ -3519,7 +3531,7 @@
         <v>317</v>
       </c>
       <c r="C76" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -3527,7 +3539,7 @@
         <v>318</v>
       </c>
       <c r="C77" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -3535,7 +3547,7 @@
         <v>319</v>
       </c>
       <c r="C78" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
@@ -3543,7 +3555,7 @@
         <v>320</v>
       </c>
       <c r="C79" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -3551,7 +3563,7 @@
         <v>321</v>
       </c>
       <c r="C80" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -3559,7 +3571,7 @@
         <v>322</v>
       </c>
       <c r="C81" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
@@ -3567,7 +3579,7 @@
         <v>323</v>
       </c>
       <c r="C82" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -3575,7 +3587,7 @@
         <v>324</v>
       </c>
       <c r="C83" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
@@ -3608,7 +3620,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3619,300 +3631,300 @@
         <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C4" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D4" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
       <c r="C5" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D5" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G6" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D7" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G7" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D8" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F8" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G8" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D9" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G9" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F10" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G10" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G11" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D12" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="G12" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D13" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F13" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="G13" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C15" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D15" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G15" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D16" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G16" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D17" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F17" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G17" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F18" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" t="s">
+        <v>651</v>
+      </c>
+      <c r="D19" t="s">
         <v>652</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
         <v>653</v>
-      </c>
-      <c r="G19" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D20" t="s">
+        <v>645</v>
+      </c>
+      <c r="F20" t="s">
+        <v>642</v>
+      </c>
+      <c r="G20" t="s">
         <v>646</v>
-      </c>
-      <c r="F20" t="s">
-        <v>643</v>
-      </c>
-      <c r="G20" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" t="s">
+        <v>643</v>
+      </c>
+      <c r="D21" t="s">
         <v>644</v>
       </c>
-      <c r="D21" t="s">
-        <v>645</v>
-      </c>
       <c r="F21" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G21" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F22" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F23" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" t="s">
+        <v>655</v>
+      </c>
+      <c r="D24" t="s">
+        <v>654</v>
+      </c>
+      <c r="G24" t="s">
         <v>656</v>
-      </c>
-      <c r="D24" t="s">
-        <v>655</v>
-      </c>
-      <c r="G24" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
   </sheetData>
@@ -4033,8 +4045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+    <sheetView topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4049,7 +4061,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -4064,7 +4076,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>221</v>
@@ -4087,10 +4099,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="H4" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4101,13 +4113,13 @@
         <v>213</v>
       </c>
       <c r="D6" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4121,7 +4133,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4138,7 +4150,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4160,7 +4172,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>231</v>
@@ -4169,10 +4181,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4190,7 +4202,7 @@
         <v>240</v>
       </c>
       <c r="H12" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4201,7 +4213,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4209,16 +4221,16 @@
         <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H14" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4226,7 +4238,7 @@
         <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4234,7 +4246,7 @@
         <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4242,7 +4254,7 @@
         <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4250,7 +4262,7 @@
         <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G18" t="s">
         <v>342</v>
@@ -4270,7 +4282,7 @@
         <v>342</v>
       </c>
       <c r="H19" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -4278,7 +4290,7 @@
         <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -4286,7 +4298,7 @@
         <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -4294,7 +4306,7 @@
         <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -4302,16 +4314,16 @@
         <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="H23" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4319,7 +4331,7 @@
         <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -4330,7 +4342,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -4341,7 +4353,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4358,7 +4370,7 @@
         <v>342</v>
       </c>
       <c r="H27" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -4366,7 +4378,7 @@
         <v>132</v>
       </c>
       <c r="H28" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -4374,7 +4386,7 @@
         <v>133</v>
       </c>
       <c r="H29" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -4382,7 +4394,7 @@
         <v>134</v>
       </c>
       <c r="H30" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -4399,7 +4411,7 @@
         <v>342</v>
       </c>
       <c r="H31" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -4407,7 +4419,7 @@
         <v>142</v>
       </c>
       <c r="H32" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -4415,7 +4427,7 @@
         <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D33" t="s">
         <v>233</v>
@@ -4424,10 +4436,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="H33" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -4435,7 +4447,7 @@
         <v>152</v>
       </c>
       <c r="H34" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -4443,7 +4455,7 @@
         <v>153</v>
       </c>
       <c r="H35" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -4451,7 +4463,7 @@
         <v>154</v>
       </c>
       <c r="H36" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -4459,10 +4471,10 @@
         <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="H37" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -4470,7 +4482,7 @@
         <v>156</v>
       </c>
       <c r="H38" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -4478,7 +4490,7 @@
         <v>157</v>
       </c>
       <c r="H39" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -4486,7 +4498,7 @@
         <v>158</v>
       </c>
       <c r="H40" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -4567,7 +4579,7 @@
         <v>239</v>
       </c>
       <c r="D46" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -4590,7 +4602,7 @@
         <v>345</v>
       </c>
       <c r="H47" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -4604,7 +4616,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -4626,7 +4638,7 @@
         <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -4733,7 +4745,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4741,16 +4753,16 @@
         <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H58" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -4758,7 +4770,7 @@
         <v>192</v>
       </c>
       <c r="H59" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -4766,10 +4778,10 @@
         <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="H60" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -4777,7 +4789,7 @@
         <v>194</v>
       </c>
       <c r="H61" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -4788,13 +4800,13 @@
         <v>225</v>
       </c>
       <c r="D62" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E62">
         <v>100</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -4811,27 +4823,27 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C64" t="s">
         <v>251</v>
       </c>
       <c r="D64" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="G64" s="9" t="s">
+        <v>802</v>
+      </c>
+      <c r="H64" t="s">
         <v>803</v>
-      </c>
-      <c r="H64" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C65" t="s">
         <v>250</v>
@@ -4840,10 +4852,10 @@
         <v>9</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H65" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4854,16 +4866,16 @@
         <v>255</v>
       </c>
       <c r="D66" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H66" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -4872,12 +4884,12 @@
       </c>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C69" t="s">
         <v>219</v>
@@ -4889,10 +4901,10 @@
         <v>100</v>
       </c>
       <c r="G69" t="s">
+        <v>763</v>
+      </c>
+      <c r="H69" t="s">
         <v>764</v>
-      </c>
-      <c r="H69" t="s">
-        <v>765</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -4903,10 +4915,10 @@
         <v>224</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H70" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -4914,7 +4926,7 @@
         <v>312</v>
       </c>
       <c r="H71" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -4922,19 +4934,19 @@
         <v>321</v>
       </c>
       <c r="C72" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D72" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H72" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -4945,10 +4957,10 @@
         <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H73" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -4956,10 +4968,10 @@
         <v>323</v>
       </c>
       <c r="G74" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="H74" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -4971,16 +4983,16 @@
         <v>223</v>
       </c>
       <c r="D75" t="s">
+        <v>783</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>770</v>
+      </c>
+      <c r="H75" t="s">
         <v>784</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75" t="s">
-        <v>771</v>
-      </c>
-      <c r="H75" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -4989,7 +5001,7 @@
         <v>332</v>
       </c>
       <c r="H76" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -4998,7 +5010,7 @@
         <v>333</v>
       </c>
       <c r="H77" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -5007,7 +5019,7 @@
         <v>334</v>
       </c>
       <c r="H78" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -5016,7 +5028,7 @@
         <v>335</v>
       </c>
       <c r="H79" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -5025,7 +5037,7 @@
         <v>336</v>
       </c>
       <c r="H80" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -5034,7 +5046,7 @@
         <v>337</v>
       </c>
       <c r="H81" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -5043,7 +5055,7 @@
         <v>338</v>
       </c>
       <c r="H82" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -5052,16 +5064,16 @@
         <v>339</v>
       </c>
       <c r="C83" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E83">
         <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="H83" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -5070,7 +5082,7 @@
         <v>340</v>
       </c>
       <c r="H84" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -5079,7 +5091,7 @@
         <v>341</v>
       </c>
       <c r="H85" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -5088,7 +5100,7 @@
         <v>342</v>
       </c>
       <c r="H86" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -5097,13 +5109,13 @@
         <v>343</v>
       </c>
       <c r="C87" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G87" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="H87" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -5112,7 +5124,7 @@
         <v>344</v>
       </c>
       <c r="H88" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -5121,7 +5133,7 @@
         <v>345</v>
       </c>
       <c r="H89" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -5130,7 +5142,7 @@
         <v>346</v>
       </c>
       <c r="H90" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -5155,7 +5167,7 @@
         <v>411</v>
       </c>
       <c r="C93" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -5164,7 +5176,7 @@
         <v>305</v>
       </c>
       <c r="H93" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -5175,7 +5187,7 @@
         <v>306</v>
       </c>
       <c r="H94" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -5183,7 +5195,7 @@
         <v>421</v>
       </c>
       <c r="C95" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E95">
         <v>20</v>
@@ -5197,7 +5209,7 @@
         <v>422</v>
       </c>
       <c r="C96" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -5205,7 +5217,7 @@
         <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -5213,7 +5225,7 @@
         <v>424</v>
       </c>
       <c r="C98" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -5221,7 +5233,7 @@
         <v>425</v>
       </c>
       <c r="C99" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E99">
         <v>35</v>
@@ -5252,7 +5264,7 @@
         <v>344</v>
       </c>
       <c r="H101" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -5260,7 +5272,7 @@
         <v>442</v>
       </c>
       <c r="H102" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -5268,7 +5280,7 @@
         <v>443</v>
       </c>
       <c r="H103" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
@@ -5351,25 +5363,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -5377,36 +5390,39 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>193</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C3" t="s">
         <v>416</v>
@@ -5414,427 +5430,459 @@
       <c r="D3" t="s">
         <v>417</v>
       </c>
-      <c r="G3">
+      <c r="E3" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1002</v>
+      </c>
+      <c r="C4" t="s">
+        <v>818</v>
+      </c>
+      <c r="D4" t="s">
+        <v>819</v>
+      </c>
+      <c r="E4" t="s">
+        <v>417</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>1101</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>39</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
+        <v>822</v>
+      </c>
+      <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>4</v>
       </c>
-      <c r="H5">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>1111</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>1102</v>
+      </c>
+      <c r="C7" t="s">
         <v>482</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E7" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>1112</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>1103</v>
+      </c>
+      <c r="C8" t="s">
         <v>484</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E8" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1104</v>
+      </c>
+      <c r="C9" t="s">
+        <v>485</v>
+      </c>
+      <c r="E9" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>1113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>485</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>1105</v>
+      </c>
+      <c r="C10" t="s">
+        <v>820</v>
+      </c>
+      <c r="E10" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>1106</v>
+      </c>
+      <c r="C11" t="s">
+        <v>486</v>
+      </c>
+      <c r="E11" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E12" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>1117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>488</v>
+      </c>
+      <c r="E13" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1118</v>
+      </c>
+      <c r="C14" t="s">
+        <v>489</v>
+      </c>
+      <c r="E14" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1119</v>
+      </c>
+      <c r="C15" t="s">
+        <v>497</v>
+      </c>
+      <c r="E15" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1120</v>
+      </c>
+      <c r="C16" t="s">
+        <v>490</v>
+      </c>
+      <c r="E16" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>1114</v>
-      </c>
-      <c r="C9" t="s">
-        <v>486</v>
-      </c>
-      <c r="D9" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>1115</v>
-      </c>
-      <c r="C10" t="s">
-        <v>487</v>
-      </c>
-      <c r="D10" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>1116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>488</v>
-      </c>
-      <c r="D11" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>1117</v>
-      </c>
-      <c r="C12" t="s">
-        <v>489</v>
-      </c>
-      <c r="D12" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>1118</v>
-      </c>
-      <c r="C13" t="s">
-        <v>490</v>
-      </c>
-      <c r="D13" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>1119</v>
-      </c>
-      <c r="C14" t="s">
-        <v>498</v>
-      </c>
-      <c r="D14" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>1120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>491</v>
-      </c>
-      <c r="D15" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>1401</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1201</v>
+      </c>
+      <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>12</v>
       </c>
-      <c r="E17">
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18">
         <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="M17" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>1402</v>
-      </c>
-      <c r="C18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>2</v>
       </c>
       <c r="H18">
         <v>1</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="N18" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>1403</v>
+        <v>1202</v>
       </c>
       <c r="C19" t="s">
-        <v>195</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="G19">
+        <v>194</v>
+      </c>
+      <c r="F19">
         <v>2</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
         <v>1</v>
       </c>
-      <c r="M19" t="s">
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>1203</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>1404</v>
-      </c>
-      <c r="C20" t="s">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>1204</v>
+      </c>
+      <c r="C21" t="s">
         <v>203</v>
       </c>
-      <c r="E20">
+      <c r="F21">
         <v>4</v>
-      </c>
-      <c r="G20">
-        <v>3</v>
-      </c>
-      <c r="H20">
-        <v>3</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="M20" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21">
-        <v>1405</v>
-      </c>
-      <c r="C21" t="s">
-        <v>204</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="G21">
-        <v>3</v>
       </c>
       <c r="H21">
         <v>3</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>2</v>
-      </c>
-      <c r="M21" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>1406</v>
+        <v>1205</v>
       </c>
       <c r="C22" t="s">
-        <v>196</v>
-      </c>
-      <c r="E22">
-        <v>6</v>
-      </c>
-      <c r="G22">
-        <v>3</v>
+        <v>204</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
       </c>
       <c r="H22">
         <v>3</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
+      </c>
+      <c r="N22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>1407</v>
+        <v>1206</v>
       </c>
       <c r="C23" t="s">
-        <v>197</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="G23">
-        <v>5</v>
+        <v>196</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
       </c>
       <c r="H23">
         <v>3</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
       <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>1207</v>
+      </c>
+      <c r="C24" t="s">
+        <v>197</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="H24">
+        <v>5</v>
+      </c>
+      <c r="I24">
         <v>3</v>
       </c>
-      <c r="M23" t="s">
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>3</v>
+      </c>
+      <c r="N24" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>1408</v>
-      </c>
-      <c r="C24" t="s">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>1208</v>
+      </c>
+      <c r="C25" t="s">
         <v>198</v>
       </c>
-      <c r="E24">
+      <c r="F25">
         <v>8</v>
       </c>
-      <c r="G24">
+      <c r="H25">
         <v>5</v>
       </c>
-      <c r="H24">
+      <c r="I25">
         <v>3</v>
       </c>
-      <c r="I24">
-        <v>0</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24">
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
         <v>3</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N25" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>1409</v>
-      </c>
-      <c r="C25" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>1209</v>
+      </c>
+      <c r="C26" t="s">
         <v>199</v>
       </c>
-      <c r="E25">
+      <c r="F26">
         <v>9</v>
       </c>
-      <c r="G25">
+      <c r="H26">
         <v>5</v>
       </c>
-      <c r="H25">
+      <c r="I26">
         <v>3</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
+      <c r="L26">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>1410</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>1210</v>
+      </c>
+      <c r="C27" t="s">
         <v>200</v>
       </c>
-      <c r="E26">
+      <c r="F27">
         <v>10</v>
       </c>
-      <c r="G26">
+      <c r="H27">
         <v>5</v>
       </c>
-      <c r="H26">
+      <c r="I27">
         <v>3</v>
       </c>
-      <c r="I26">
+      <c r="J27">
         <v>1</v>
       </c>
-      <c r="J26">
-        <v>0</v>
-      </c>
-      <c r="K26">
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
         <v>3</v>
       </c>
     </row>
@@ -5882,7 +5930,7 @@
         <v>450</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>454</v>
@@ -5893,7 +5941,7 @@
         <v>451</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>452</v>
@@ -5928,7 +5976,7 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
@@ -5956,7 +6004,7 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D9" t="s">
         <v>432</v>
@@ -5970,7 +6018,7 @@
         <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D10" t="s">
         <v>71</v>
@@ -5984,7 +6032,7 @@
         <v>439</v>
       </c>
       <c r="C12" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D12" t="s">
         <v>430</v>
@@ -5998,7 +6046,7 @@
         <v>438</v>
       </c>
       <c r="C13" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D13" t="s">
         <v>427</v>
@@ -6012,7 +6060,7 @@
         <v>440</v>
       </c>
       <c r="C14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D14" t="s">
         <v>462</v>
@@ -6026,7 +6074,7 @@
         <v>441</v>
       </c>
       <c r="C15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D15" t="s">
         <v>463</v>
@@ -6040,7 +6088,7 @@
         <v>434</v>
       </c>
       <c r="C16" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D16" t="s">
         <v>466</v>
@@ -6057,7 +6105,7 @@
         <v>435</v>
       </c>
       <c r="C17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D17" t="s">
         <v>426</v>
@@ -6072,7 +6120,7 @@
         <v>442</v>
       </c>
       <c r="C18" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D18" t="s">
         <v>466</v>
@@ -6087,7 +6135,7 @@
         <v>443</v>
       </c>
       <c r="C19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D19" t="s">
         <v>467</v>
@@ -6102,7 +6150,7 @@
         <v>444</v>
       </c>
       <c r="C20" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D20" t="s">
         <v>468</v>
@@ -6116,7 +6164,7 @@
         <v>445</v>
       </c>
       <c r="C21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D21" t="s">
         <v>473</v>
@@ -6130,7 +6178,7 @@
         <v>206</v>
       </c>
       <c r="C22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D22" t="s">
         <v>208</v>
@@ -6144,7 +6192,7 @@
         <v>446</v>
       </c>
       <c r="C23" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D23" t="s">
         <v>469</v>
@@ -6158,7 +6206,7 @@
         <v>447</v>
       </c>
       <c r="C24" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D24" t="s">
         <v>479</v>
@@ -6172,7 +6220,7 @@
         <v>448</v>
       </c>
       <c r="C25" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D25" t="s">
         <v>474</v>
@@ -6186,7 +6234,7 @@
         <v>449</v>
       </c>
       <c r="C26" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -6194,7 +6242,7 @@
         <v>455</v>
       </c>
       <c r="C27" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -6202,7 +6250,7 @@
         <v>456</v>
       </c>
       <c r="C28" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -6210,7 +6258,7 @@
         <v>457</v>
       </c>
       <c r="C29" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -6218,7 +6266,7 @@
         <v>458</v>
       </c>
       <c r="C30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -6226,29 +6274,29 @@
         <v>459</v>
       </c>
       <c r="C31" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C33" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="E33" t="s">
+        <v>535</v>
+      </c>
+      <c r="F33" t="s">
         <v>536</v>
-      </c>
-      <c r="F33" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>560</v>
+      </c>
+      <c r="C34" t="s">
         <v>561</v>
-      </c>
-      <c r="C34" t="s">
-        <v>562</v>
       </c>
     </row>
   </sheetData>
@@ -8683,7 +8731,7 @@
         <v>2821</v>
       </c>
       <c r="C151" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E151">
         <v>3</v>
@@ -9567,7 +9615,7 @@
         <v>3103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D5" t="s">
         <v>294</v>
@@ -10019,7 +10067,7 @@
         <v>397</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G31">
         <v>40</v>
@@ -10039,7 +10087,7 @@
         <v>397</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G32">
         <v>60</v>
@@ -10157,13 +10205,13 @@
         <v>3201</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D40" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F40" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -10177,13 +10225,13 @@
         <v>3202</v>
       </c>
       <c r="C41" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D41" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F41" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -10234,7 +10282,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10245,13 +10293,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -10265,19 +10313,19 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>537</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="I4" t="s">
         <v>538</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="I4" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -10286,16 +10334,16 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E5" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I5" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -10304,16 +10352,16 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I6" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -10322,16 +10370,16 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
+        <v>541</v>
+      </c>
+      <c r="E7" t="s">
+        <v>543</v>
+      </c>
+      <c r="F7" t="s">
+        <v>506</v>
+      </c>
+      <c r="I7" t="s">
         <v>542</v>
-      </c>
-      <c r="E7" t="s">
-        <v>544</v>
-      </c>
-      <c r="F7" t="s">
-        <v>507</v>
-      </c>
-      <c r="I7" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -10340,16 +10388,16 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
+        <v>545</v>
+      </c>
+      <c r="E8" t="s">
+        <v>540</v>
+      </c>
+      <c r="F8" t="s">
+        <v>507</v>
+      </c>
+      <c r="I8" t="s">
         <v>546</v>
-      </c>
-      <c r="E8" t="s">
-        <v>541</v>
-      </c>
-      <c r="F8" t="s">
-        <v>508</v>
-      </c>
-      <c r="I8" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -10358,19 +10406,19 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -10379,16 +10427,16 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E10" t="s">
+        <v>576</v>
+      </c>
+      <c r="F10" t="s">
+        <v>504</v>
+      </c>
+      <c r="I10" t="s">
         <v>577</v>
-      </c>
-      <c r="F10" t="s">
-        <v>505</v>
-      </c>
-      <c r="I10" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -10397,16 +10445,16 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E11" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I11" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -10415,16 +10463,16 @@
         <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E12" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F12" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I12" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -10433,16 +10481,16 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
+        <v>570</v>
+      </c>
+      <c r="E13" t="s">
         <v>571</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>507</v>
+      </c>
+      <c r="I13" t="s">
         <v>572</v>
-      </c>
-      <c r="F13" t="s">
-        <v>508</v>
-      </c>
-      <c r="I13" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -10453,19 +10501,19 @@
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I15" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -10474,19 +10522,19 @@
         <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="E16" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F16" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -10495,19 +10543,19 @@
         <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E17" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F17" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -10516,19 +10564,19 @@
         <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E18" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F18" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -10537,19 +10585,19 @@
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F19" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -10558,19 +10606,19 @@
         <v>116</v>
       </c>
       <c r="D20" t="s">
+        <v>592</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>508</v>
+      </c>
+      <c r="I20" t="s">
         <v>593</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>588</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>509</v>
-      </c>
-      <c r="I20" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -10579,19 +10627,19 @@
         <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E21" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F21" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -10600,19 +10648,19 @@
         <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E22" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F22" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G22">
         <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -10621,19 +10669,19 @@
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F23" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -10642,24 +10690,24 @@
         <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E24" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G24">
         <v>100</v>
       </c>
       <c r="I24" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C26">
         <v>121</v>
@@ -10691,7 +10739,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C32">
         <v>131</v>
@@ -10703,10 +10751,10 @@
         <v>132</v>
       </c>
       <c r="D33" t="s">
+        <v>554</v>
+      </c>
+      <c r="I33" t="s">
         <v>555</v>
-      </c>
-      <c r="I33" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -10715,7 +10763,7 @@
         <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -10724,10 +10772,10 @@
         <v>134</v>
       </c>
       <c r="D35" t="s">
+        <v>557</v>
+      </c>
+      <c r="I35" t="s">
         <v>558</v>
-      </c>
-      <c r="I35" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.3h: Item constructor finished, item tier
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8927AB0F-89F6-4F16-B011-10D43029872B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544B0B7-BF7B-43A3-A87D-9C7197D16D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -6413,13 +6413,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y200"/>
+  <dimension ref="A1:Y199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D129" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A155" sqref="A152:XFD155"/>
+      <selection pane="bottomRight" activeCell="E187" sqref="E187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6920,365 +6920,394 @@
         <v>10000</v>
       </c>
     </row>
+    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>2201</v>
+      </c>
+      <c r="C34" t="s">
+        <v>287</v>
+      </c>
+      <c r="D34" t="s">
+        <v>28</v>
+      </c>
+      <c r="L34" s="4">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>0.15</v>
+      </c>
+    </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>2201</v>
+        <v>2202</v>
       </c>
       <c r="C35" t="s">
-        <v>287</v>
-      </c>
-      <c r="D35" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="N35">
-        <v>0.15</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>2202</v>
+        <v>2203</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>284</v>
       </c>
       <c r="L36" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N36">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>2203</v>
+        <v>2204</v>
       </c>
       <c r="C37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L37" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N37">
-        <v>0.01</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q37">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>2204</v>
+        <v>2211</v>
       </c>
       <c r="C38" t="s">
-        <v>283</v>
+        <v>21</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
       </c>
       <c r="L38" s="4">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N38">
-        <v>0.08</v>
-      </c>
-      <c r="Q38">
-        <v>4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>2211</v>
+        <v>2212</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>285</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="L39" s="4">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N39">
-        <v>0.15</v>
+        <v>0.05</v>
+      </c>
+      <c r="Q39">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>2212</v>
+        <v>2213</v>
       </c>
       <c r="C40" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
       <c r="L40" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N40">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="Q40">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>2213</v>
-      </c>
-      <c r="C41" t="s">
-        <v>286</v>
-      </c>
-      <c r="E41">
-        <v>2</v>
-      </c>
-      <c r="L41" s="4">
-        <v>5</v>
-      </c>
-      <c r="N41">
-        <v>0.3</v>
-      </c>
-      <c r="Q41">
         <v>18</v>
       </c>
-      <c r="S41">
+      <c r="S40">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>2301</v>
+      </c>
+      <c r="C42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D42" t="s">
+        <v>30</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="N42">
+        <v>3</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="W42" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>2301</v>
+        <v>2311</v>
       </c>
       <c r="C43" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" t="s">
-        <v>30</v>
+        <v>288</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N43">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="Q43">
+        <v>15</v>
       </c>
       <c r="U43">
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>2311</v>
+        <v>2312</v>
       </c>
       <c r="C44" t="s">
-        <v>288</v>
+        <v>174</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
-      <c r="L44" s="10" t="s">
-        <v>419</v>
+      <c r="L44" s="4">
+        <v>20</v>
       </c>
       <c r="N44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q44">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="U44">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="W44" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>2312</v>
+        <v>2321</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E45">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" s="4">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="N45">
+        <v>10</v>
+      </c>
+      <c r="Q45">
+        <v>10</v>
+      </c>
+      <c r="U45">
         <v>6</v>
       </c>
-      <c r="Q45">
-        <v>12</v>
-      </c>
-      <c r="U45">
-        <v>8</v>
-      </c>
       <c r="W45" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>2321</v>
+        <v>2322</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
-      <c r="L46" s="4">
-        <v>200</v>
+      <c r="L46" s="4" t="s">
+        <v>359</v>
       </c>
       <c r="N46">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q46">
         <v>10</v>
       </c>
       <c r="U46">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W46" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>2322</v>
+        <v>2323</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="N47">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q47">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="U47">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="W47" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>2323</v>
+        <v>2331</v>
       </c>
       <c r="C48" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="E48">
-        <v>3</v>
-      </c>
-      <c r="L48" s="4" t="s">
-        <v>361</v>
+        <v>4</v>
+      </c>
+      <c r="L48" s="4">
+        <v>1000</v>
       </c>
       <c r="N48">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="Q48">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="U48">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="W48" t="s">
-        <v>391</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>2331</v>
+        <v>2332</v>
       </c>
       <c r="C49" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
       <c r="E49">
         <v>4</v>
       </c>
-      <c r="L49" s="4">
-        <v>1000</v>
+      <c r="L49" s="4" t="s">
+        <v>356</v>
       </c>
       <c r="N49">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q49">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U49">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W49" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>2332</v>
+        <v>2333</v>
       </c>
       <c r="C50" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="N50">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q50">
         <v>15</v>
       </c>
       <c r="U50">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W50" t="s">
-        <v>377</v>
+        <v>383</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>2333</v>
+        <v>2341</v>
       </c>
       <c r="C51" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E51">
-        <v>4</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>349</v>
+        <v>5</v>
+      </c>
+      <c r="L51" s="4">
+        <v>600</v>
       </c>
       <c r="N51">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q51">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="S51">
+        <v>-1</v>
       </c>
       <c r="U51">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W51" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>2341</v>
+        <v>2342</v>
       </c>
       <c r="C52" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="E52">
         <v>5</v>
@@ -7287,244 +7316,241 @@
         <v>600</v>
       </c>
       <c r="N52">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q52">
+        <v>15</v>
+      </c>
+      <c r="U52">
         <v>6</v>
       </c>
-      <c r="S52">
-        <v>-1</v>
-      </c>
-      <c r="U52">
-        <v>1</v>
-      </c>
       <c r="W52" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>2342</v>
+        <v>2343</v>
       </c>
       <c r="C53" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E53">
         <v>5</v>
       </c>
-      <c r="L53" s="4">
-        <v>600</v>
+      <c r="L53" s="4" t="s">
+        <v>360</v>
       </c>
       <c r="N53">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Q53">
         <v>15</v>
       </c>
       <c r="U53">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W53" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>2343</v>
+        <v>2344</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E54">
         <v>5</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="N54">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q54">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="U54">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="W54" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>2344</v>
+        <v>2345</v>
       </c>
       <c r="C55" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E55">
         <v>5</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="N55">
+        <v>4</v>
+      </c>
+      <c r="Q55">
         <v>10</v>
       </c>
-      <c r="Q55">
-        <v>24</v>
-      </c>
       <c r="U55">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="W55" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2345</v>
+        <v>2351</v>
       </c>
       <c r="C56" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E56">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="N56">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q56">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="U56">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="W56" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>2351</v>
+        <v>2352</v>
       </c>
       <c r="C57" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E57">
         <v>6</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="N57">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q57">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="U57">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W57" t="s">
-        <v>376</v>
+        <v>382</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>2352</v>
+        <v>2353</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="E58">
         <v>6</v>
       </c>
-      <c r="L58" s="4" t="s">
-        <v>357</v>
+      <c r="L58" s="4">
+        <v>500</v>
       </c>
       <c r="N58">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q58">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="S58">
+        <v>1</v>
+      </c>
+      <c r="T58">
+        <v>0.1</v>
       </c>
       <c r="U58">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W58" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>2353</v>
+        <v>2354</v>
       </c>
       <c r="C59" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E59">
         <v>6</v>
       </c>
-      <c r="L59" s="4">
-        <v>500</v>
+      <c r="L59" s="4" t="s">
+        <v>348</v>
       </c>
       <c r="N59">
         <v>7</v>
       </c>
       <c r="Q59">
-        <v>25</v>
-      </c>
-      <c r="S59">
-        <v>1</v>
-      </c>
-      <c r="T59">
-        <v>0.1</v>
+        <v>15</v>
       </c>
       <c r="U59">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="W59" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>2354</v>
+        <v>2355</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="E60">
         <v>6</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="N60">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q60">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U60">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="W60" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2355</v>
+        <v>2361</v>
       </c>
       <c r="C61" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E61">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L61" s="4" t="s">
         <v>350</v>
@@ -7533,247 +7559,247 @@
         <v>11</v>
       </c>
       <c r="Q61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U61">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="W61" t="s">
-        <v>393</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2361</v>
+        <v>2362</v>
       </c>
       <c r="C62" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
       <c r="E62">
         <v>7</v>
       </c>
-      <c r="L62" s="4" t="s">
-        <v>350</v>
+      <c r="L62" s="4">
+        <v>1200</v>
       </c>
       <c r="N62">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q62">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="U62">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="W62" t="s">
-        <v>368</v>
+        <v>379</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2362</v>
+        <v>2363</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="E63">
         <v>7</v>
       </c>
-      <c r="L63" s="4">
-        <v>1200</v>
+      <c r="L63" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="N63">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q63">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="S63">
+        <v>-1</v>
       </c>
       <c r="U63">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="W63" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>2363</v>
+        <v>2364</v>
       </c>
       <c r="C64" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="N64">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="Q64">
-        <v>30</v>
-      </c>
-      <c r="S64">
-        <v>-1</v>
+        <v>12</v>
       </c>
       <c r="U64">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W64" t="s">
-        <v>386</v>
+        <v>392</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2364</v>
+        <v>2371</v>
       </c>
       <c r="C65" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="E65">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="N65">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="Q65">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="U65">
-        <v>5</v>
+        <v>125</v>
       </c>
       <c r="W65" t="s">
-        <v>392</v>
+        <v>369</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>2371</v>
+        <v>2372</v>
       </c>
       <c r="C66" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E66">
         <v>8</v>
       </c>
-      <c r="L66" s="4" t="s">
-        <v>352</v>
+      <c r="L66" s="4">
+        <v>500</v>
+      </c>
+      <c r="M66">
+        <v>500</v>
       </c>
       <c r="N66">
-        <v>10</v>
-      </c>
-      <c r="Q66">
+        <v>9</v>
+      </c>
+      <c r="R66">
+        <v>4</v>
+      </c>
+      <c r="U66">
         <v>20</v>
       </c>
-      <c r="U66">
-        <v>125</v>
-      </c>
       <c r="W66" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>2372</v>
+        <v>2373</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="E67">
         <v>8</v>
       </c>
-      <c r="L67" s="4">
-        <v>500</v>
-      </c>
-      <c r="M67">
-        <v>500</v>
+      <c r="L67" s="4" t="s">
+        <v>355</v>
       </c>
       <c r="N67">
-        <v>9</v>
-      </c>
-      <c r="R67">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="Q67">
+        <v>22</v>
       </c>
       <c r="U67">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="W67" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>2373</v>
+        <v>2374</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="E68">
         <v>8</v>
       </c>
-      <c r="L68" s="4" t="s">
-        <v>355</v>
+      <c r="L68" s="4">
+        <v>1000</v>
       </c>
       <c r="N68">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q68">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="S68">
+        <v>2</v>
+      </c>
+      <c r="T68">
+        <v>0.15</v>
       </c>
       <c r="U68">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="W68" t="s">
-        <v>376</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>2374</v>
+        <v>2375</v>
       </c>
       <c r="C69" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E69">
         <v>8</v>
       </c>
-      <c r="L69" s="4">
-        <v>1000</v>
+      <c r="L69" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="N69">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q69">
-        <v>35</v>
-      </c>
-      <c r="S69">
-        <v>2</v>
-      </c>
-      <c r="T69">
-        <v>0.15</v>
+        <v>20</v>
       </c>
       <c r="U69">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="W69" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>2375</v>
+        <v>2381</v>
       </c>
       <c r="C70" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E70">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="N70">
         <v>12</v>
@@ -7782,717 +7808,705 @@
         <v>20</v>
       </c>
       <c r="U70">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="W70" t="s">
-        <v>394</v>
+        <v>367</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>2381</v>
+        <v>2382</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E71">
         <v>9</v>
       </c>
-      <c r="L71" s="4" t="s">
-        <v>351</v>
+      <c r="L71" s="4">
+        <v>1000</v>
       </c>
       <c r="N71">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="Q71">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="U71">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="W71" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>2382</v>
+        <v>2391</v>
       </c>
       <c r="C72" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="E72">
-        <v>9</v>
-      </c>
-      <c r="L72" s="4">
-        <v>1000</v>
+        <v>10</v>
+      </c>
+      <c r="L72" s="4" t="s">
+        <v>353</v>
       </c>
       <c r="N72">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="Q72">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="U72">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="W72" t="s">
-        <v>385</v>
+        <v>370</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>2391</v>
+        <v>2392</v>
       </c>
       <c r="C73" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="E73">
         <v>10</v>
       </c>
-      <c r="L73" s="4" t="s">
-        <v>353</v>
+      <c r="L73" s="4">
+        <v>500</v>
+      </c>
+      <c r="M73">
+        <v>500</v>
       </c>
       <c r="N73">
-        <v>11</v>
-      </c>
-      <c r="Q73">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="R73">
+        <v>8</v>
       </c>
       <c r="U73">
-        <v>125</v>
+        <v>40</v>
       </c>
       <c r="W73" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <v>2392</v>
-      </c>
-      <c r="C74" t="s">
-        <v>153</v>
-      </c>
-      <c r="E74">
-        <v>10</v>
-      </c>
-      <c r="L74" s="4">
-        <v>500</v>
-      </c>
-      <c r="M74">
-        <v>500</v>
-      </c>
-      <c r="N74">
-        <v>9</v>
-      </c>
-      <c r="R74">
-        <v>8</v>
-      </c>
-      <c r="U74">
-        <v>40</v>
-      </c>
-      <c r="W74" t="s">
         <v>375</v>
+      </c>
+    </row>
+    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>2401</v>
+      </c>
+      <c r="C75" t="s">
+        <v>99</v>
+      </c>
+      <c r="D75" t="s">
+        <v>23</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>2401</v>
+        <v>2402</v>
       </c>
       <c r="C76" t="s">
-        <v>99</v>
-      </c>
-      <c r="D76" t="s">
-        <v>23</v>
-      </c>
-      <c r="O76">
-        <v>1</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>2402</v>
+        <v>2403</v>
       </c>
       <c r="C77" t="s">
-        <v>178</v>
+        <v>180</v>
+      </c>
+      <c r="O77">
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>2403</v>
+        <v>2404</v>
       </c>
       <c r="C78" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O78">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="S78">
+        <v>-1</v>
       </c>
     </row>
     <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>2404</v>
+        <v>2411</v>
       </c>
       <c r="C79" t="s">
-        <v>179</v>
+        <v>100</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
       </c>
       <c r="O79">
         <v>2</v>
       </c>
-      <c r="S79">
-        <v>-1</v>
-      </c>
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>2411</v>
+        <v>2421</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E80">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O80">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>2421</v>
+        <v>2431</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E81">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O81">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>2431</v>
+        <v>2441</v>
       </c>
       <c r="C82" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E82">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O82">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83">
-        <v>2441</v>
+        <v>2451</v>
       </c>
       <c r="C83" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E83">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O83">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>2451</v>
+        <v>2461</v>
       </c>
       <c r="C84" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E84">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O84">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85">
-        <v>2461</v>
+        <v>2471</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E85">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O85">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>2471</v>
+        <v>2481</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E86">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O86">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>2481</v>
+        <v>2491</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E87">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O87">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B88">
-        <v>2491</v>
-      </c>
-      <c r="C88" t="s">
-        <v>108</v>
-      </c>
-      <c r="E88">
-        <v>10</v>
-      </c>
-      <c r="O88">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B89">
+        <v>2501</v>
+      </c>
+      <c r="C89" t="s">
+        <v>109</v>
+      </c>
+      <c r="D89" t="s">
+        <v>24</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>2501</v>
+        <v>2502</v>
       </c>
       <c r="C90" t="s">
-        <v>109</v>
-      </c>
-      <c r="D90" t="s">
-        <v>24</v>
-      </c>
-      <c r="O90">
-        <v>1</v>
+        <v>181</v>
+      </c>
+      <c r="N90">
+        <v>0.04</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2502</v>
+        <v>2503</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="N91">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2503</v>
+        <v>2504</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="N92">
-        <v>0.02</v>
+        <v>0.04</v>
+      </c>
+      <c r="O92">
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2504</v>
+        <v>2511</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
-      </c>
-      <c r="N93">
-        <v>0.04</v>
+        <v>110</v>
+      </c>
+      <c r="E93">
+        <v>2</v>
       </c>
       <c r="O93">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2511</v>
+        <v>2512</v>
       </c>
       <c r="C94" t="s">
-        <v>110</v>
+        <v>191</v>
       </c>
       <c r="E94">
         <v>2</v>
       </c>
+      <c r="K94">
+        <v>3</v>
+      </c>
+      <c r="N94">
+        <v>0.06</v>
+      </c>
       <c r="O94">
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2512</v>
+        <v>2513</v>
       </c>
       <c r="C95" t="s">
-        <v>191</v>
-      </c>
-      <c r="E95">
-        <v>2</v>
-      </c>
-      <c r="K95">
-        <v>3</v>
+        <v>318</v>
       </c>
       <c r="N95">
-        <v>0.06</v>
-      </c>
-      <c r="O95">
-        <v>2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2513</v>
+        <v>2521</v>
       </c>
       <c r="C96" t="s">
-        <v>318</v>
-      </c>
-      <c r="N96">
-        <v>0.04</v>
+        <v>111</v>
+      </c>
+      <c r="E96">
+        <v>3</v>
+      </c>
+      <c r="O96">
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>2521</v>
+        <v>2531</v>
       </c>
       <c r="C97" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E97">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O97">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2531</v>
+        <v>2541</v>
       </c>
       <c r="C98" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E98">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O98">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>2541</v>
+        <v>2551</v>
       </c>
       <c r="C99" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O99">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2551</v>
+        <v>2561</v>
       </c>
       <c r="C100" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E100">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O100">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2561</v>
+        <v>2571</v>
       </c>
       <c r="C101" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E101">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O101">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2571</v>
+        <v>2581</v>
       </c>
       <c r="C102" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E102">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O102">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2581</v>
+        <v>2591</v>
       </c>
       <c r="C103" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="E103">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O103">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104">
-        <v>2591</v>
-      </c>
-      <c r="C104" t="s">
-        <v>118</v>
-      </c>
-      <c r="E104">
-        <v>10</v>
-      </c>
-      <c r="O104">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B105">
+        <v>2601</v>
+      </c>
+      <c r="C105" t="s">
+        <v>119</v>
+      </c>
+      <c r="D105" t="s">
+        <v>25</v>
+      </c>
+      <c r="O105">
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2601</v>
+        <v>2602</v>
       </c>
       <c r="C106" t="s">
-        <v>119</v>
-      </c>
-      <c r="D106" t="s">
-        <v>25</v>
-      </c>
-      <c r="O106">
-        <v>1</v>
+        <v>184</v>
+      </c>
+      <c r="N106">
+        <v>0.02</v>
       </c>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2602</v>
+        <v>2603</v>
       </c>
       <c r="C107" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="N107">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2603</v>
+        <v>2604</v>
       </c>
       <c r="C108" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="N108">
-        <v>0.06</v>
+        <v>0.08</v>
+      </c>
+      <c r="O108">
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2604</v>
+        <v>2611</v>
       </c>
       <c r="C109" t="s">
-        <v>185</v>
-      </c>
-      <c r="N109">
-        <v>0.08</v>
+        <v>120</v>
+      </c>
+      <c r="E109">
+        <v>2</v>
       </c>
       <c r="O109">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2611</v>
+        <v>2621</v>
       </c>
       <c r="C110" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E110">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O110">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2621</v>
+        <v>2631</v>
       </c>
       <c r="C111" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E111">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O111">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>2631</v>
+        <v>2641</v>
       </c>
       <c r="C112" t="s">
-        <v>122</v>
+        <v>825</v>
       </c>
       <c r="E112">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O112">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="113" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B113">
-        <v>2641</v>
+        <v>2651</v>
       </c>
       <c r="C113" t="s">
-        <v>825</v>
+        <v>123</v>
       </c>
       <c r="E113">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O113">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="114" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2651</v>
+        <v>2661</v>
       </c>
       <c r="C114" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E114">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O114">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>2661</v>
+        <v>2671</v>
       </c>
       <c r="C115" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E115">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O115">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="116" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>2671</v>
+        <v>2681</v>
       </c>
       <c r="C116" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E116">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O116">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>2681</v>
+        <v>2691</v>
       </c>
       <c r="C117" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E117">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O117">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B118">
-        <v>2691</v>
-      </c>
-      <c r="C118" t="s">
-        <v>127</v>
-      </c>
-      <c r="E118">
-        <v>10</v>
-      </c>
-      <c r="O118">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B119">
+        <v>2701</v>
+      </c>
+      <c r="C119" t="s">
+        <v>128</v>
+      </c>
+      <c r="D119" t="s">
+        <v>26</v>
+      </c>
+      <c r="O119">
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>2701</v>
+        <v>2702</v>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
-      </c>
-      <c r="D120" t="s">
-        <v>26</v>
-      </c>
-      <c r="O120">
-        <v>1</v>
+        <v>187</v>
       </c>
     </row>
     <row r="121" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2702</v>
+        <v>2703</v>
       </c>
       <c r="C121" t="s">
-        <v>187</v>
+        <v>188</v>
+      </c>
+      <c r="S121">
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2703</v>
+        <v>2704</v>
       </c>
       <c r="C122" t="s">
-        <v>188</v>
+        <v>189</v>
+      </c>
+      <c r="O122">
+        <v>1</v>
       </c>
       <c r="S122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2704</v>
+        <v>2705</v>
       </c>
       <c r="C123" t="s">
-        <v>189</v>
+        <v>319</v>
       </c>
       <c r="O123">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S123">
         <v>2</v>
@@ -8500,231 +8514,228 @@
     </row>
     <row r="124" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2705</v>
+        <v>2711</v>
       </c>
       <c r="C124" t="s">
-        <v>319</v>
+        <v>129</v>
+      </c>
+      <c r="E124">
+        <v>2</v>
       </c>
       <c r="O124">
         <v>2</v>
       </c>
-      <c r="S124">
-        <v>2</v>
-      </c>
     </row>
     <row r="125" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>2711</v>
+        <v>2712</v>
       </c>
       <c r="C125" t="s">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="E125">
         <v>2</v>
       </c>
       <c r="O125">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="S125">
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2712</v>
+        <v>2713</v>
       </c>
       <c r="C126" t="s">
-        <v>190</v>
+        <v>320</v>
       </c>
       <c r="E126">
         <v>2</v>
       </c>
+      <c r="L126" s="4">
+        <v>1</v>
+      </c>
       <c r="O126">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S126">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B127">
-        <v>2713</v>
+        <v>2714</v>
       </c>
       <c r="C127" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E127">
         <v>2</v>
       </c>
-      <c r="L127" s="4">
-        <v>1</v>
-      </c>
       <c r="O127">
+        <v>2</v>
+      </c>
+      <c r="S127">
         <v>3</v>
-      </c>
-      <c r="S127">
-        <v>2</v>
       </c>
     </row>
     <row r="128" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2714</v>
+        <v>2721</v>
       </c>
       <c r="C128" t="s">
-        <v>321</v>
+        <v>130</v>
       </c>
       <c r="E128">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O128">
-        <v>2</v>
-      </c>
-      <c r="S128">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>2721</v>
+        <v>2731</v>
       </c>
       <c r="C129" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E129">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O129">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="130" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2731</v>
+        <v>2741</v>
       </c>
       <c r="C130" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E130">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O130">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="131" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2741</v>
+        <v>2751</v>
       </c>
       <c r="C131" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E131">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O131">
-        <v>48</v>
+        <v>72</v>
       </c>
     </row>
     <row r="132" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2751</v>
+        <v>2761</v>
       </c>
       <c r="C132" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E132">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="O132">
-        <v>72</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2761</v>
+        <v>2771</v>
       </c>
       <c r="C133" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E133">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O133">
-        <v>100</v>
+        <v>200</v>
       </c>
     </row>
     <row r="134" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2771</v>
+        <v>2781</v>
       </c>
       <c r="C134" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E134">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="O134">
-        <v>200</v>
+        <v>400</v>
       </c>
     </row>
     <row r="135" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2781</v>
+        <v>2791</v>
       </c>
       <c r="C135" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E135">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O135">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="136" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B136">
-        <v>2791</v>
-      </c>
-      <c r="C136" t="s">
-        <v>137</v>
-      </c>
-      <c r="E136">
-        <v>10</v>
-      </c>
-      <c r="O136">
         <v>1500</v>
+      </c>
+    </row>
+    <row r="137" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B137">
+        <v>2801</v>
+      </c>
+      <c r="C137" t="s">
+        <v>138</v>
+      </c>
+      <c r="D137" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="138" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2801</v>
+        <v>2802</v>
       </c>
       <c r="C138" t="s">
-        <v>138</v>
-      </c>
-      <c r="D138" t="s">
-        <v>27</v>
+        <v>315</v>
       </c>
     </row>
     <row r="139" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2802</v>
+        <v>2803</v>
       </c>
       <c r="C139" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="140" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2803</v>
+        <v>2811</v>
       </c>
       <c r="C140" t="s">
-        <v>316</v>
+        <v>139</v>
+      </c>
+      <c r="E140">
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>2811</v>
+        <v>2812</v>
       </c>
       <c r="C141" t="s">
-        <v>139</v>
+        <v>317</v>
       </c>
       <c r="E141">
         <v>2</v>
@@ -8732,200 +8743,200 @@
     </row>
     <row r="142" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2812</v>
+        <v>2821</v>
       </c>
       <c r="C142" t="s">
-        <v>317</v>
+        <v>140</v>
       </c>
       <c r="E142">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="143" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>2821</v>
+        <v>2822</v>
       </c>
       <c r="C143" t="s">
-        <v>140</v>
+        <v>598</v>
       </c>
       <c r="E143">
         <v>3</v>
       </c>
+      <c r="Y143" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="144" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2822</v>
+        <v>2831</v>
       </c>
       <c r="C144" t="s">
-        <v>598</v>
+        <v>141</v>
       </c>
       <c r="E144">
-        <v>3</v>
-      </c>
-      <c r="Y144" t="s">
-        <v>213</v>
+        <v>4</v>
       </c>
     </row>
     <row r="145" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>2831</v>
+        <v>2841</v>
       </c>
       <c r="C145" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E145">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="146" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>2841</v>
+        <v>2851</v>
       </c>
       <c r="C146" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E146">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B147">
-        <v>2851</v>
+        <v>2861</v>
       </c>
       <c r="C147" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E147">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="148" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2861</v>
+        <v>2871</v>
       </c>
       <c r="C148" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E148">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="149" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2871</v>
+        <v>2881</v>
       </c>
       <c r="C149" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E149">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2881</v>
+        <v>2891</v>
       </c>
       <c r="C150" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E150">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="151" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B151">
-        <v>2891</v>
-      </c>
-      <c r="C151" t="s">
-        <v>147</v>
-      </c>
-      <c r="E151">
         <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B152">
+        <v>2901</v>
+      </c>
+      <c r="C152" t="s">
+        <v>264</v>
+      </c>
+      <c r="D152" t="s">
+        <v>264</v>
+      </c>
+      <c r="W152" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="153" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2901</v>
+        <v>2902</v>
       </c>
       <c r="C153" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D153" t="s">
         <v>264</v>
       </c>
+      <c r="E153">
+        <v>2</v>
+      </c>
       <c r="W153" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="154" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2902</v>
+        <v>2903</v>
       </c>
       <c r="C154" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D154" t="s">
         <v>264</v>
       </c>
       <c r="E154">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W154" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="155" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>2903</v>
+        <v>2911</v>
       </c>
       <c r="C155" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="D155" t="s">
-        <v>264</v>
-      </c>
-      <c r="E155">
-        <v>3</v>
-      </c>
-      <c r="W155" t="s">
-        <v>269</v>
+        <v>270</v>
+      </c>
+      <c r="H155" s="7"/>
+      <c r="L155" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>2911</v>
+        <v>2912</v>
       </c>
       <c r="C156" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D156" t="s">
         <v>270</v>
       </c>
-      <c r="H156" s="7"/>
       <c r="L156" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="157" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>2912</v>
+        <v>2913</v>
       </c>
       <c r="C157" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D157" t="s">
         <v>270</v>
       </c>
-      <c r="L157" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="158" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2913</v>
+        <v>2914</v>
       </c>
       <c r="C158" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D158" t="s">
         <v>270</v>
@@ -8933,35 +8944,35 @@
     </row>
     <row r="159" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2914</v>
+        <v>2915</v>
       </c>
       <c r="C159" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D159" t="s">
         <v>270</v>
       </c>
+      <c r="L159" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>2915</v>
+        <v>2916</v>
       </c>
       <c r="C160" t="s">
-        <v>275</v>
+        <v>306</v>
       </c>
       <c r="D160" t="s">
         <v>270</v>
       </c>
-      <c r="L160" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="161" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2916</v>
+        <v>2917</v>
       </c>
       <c r="C161" t="s">
-        <v>306</v>
+        <v>822</v>
       </c>
       <c r="D161" t="s">
         <v>270</v>
@@ -8969,175 +8980,184 @@
     </row>
     <row r="162" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2917</v>
+        <v>2921</v>
       </c>
       <c r="C162" t="s">
-        <v>822</v>
+        <v>277</v>
       </c>
       <c r="D162" t="s">
-        <v>270</v>
+        <v>276</v>
+      </c>
+      <c r="N162">
+        <v>0.04</v>
+      </c>
+      <c r="W162" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="163" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2921</v>
+        <v>2922</v>
       </c>
       <c r="C163" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D163" t="s">
         <v>276</v>
       </c>
+      <c r="E163">
+        <v>2</v>
+      </c>
       <c r="N163">
         <v>0.04</v>
       </c>
       <c r="W163" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="164" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2922</v>
+        <v>2923</v>
       </c>
       <c r="C164" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D164" t="s">
         <v>276</v>
       </c>
-      <c r="E164">
-        <v>2</v>
-      </c>
       <c r="N164">
         <v>0.04</v>
       </c>
       <c r="W164" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="165" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2923</v>
+        <v>2924</v>
       </c>
       <c r="C165" t="s">
-        <v>279</v>
+        <v>307</v>
       </c>
       <c r="D165" t="s">
         <v>276</v>
       </c>
+      <c r="L165" s="4">
+        <v>1</v>
+      </c>
       <c r="N165">
-        <v>0.04</v>
+        <v>2.5</v>
+      </c>
+      <c r="Q165">
+        <v>6</v>
       </c>
       <c r="W165" t="s">
-        <v>280</v>
+        <v>314</v>
       </c>
     </row>
     <row r="166" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2924</v>
+        <v>2925</v>
       </c>
       <c r="C166" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D166" t="s">
         <v>276</v>
       </c>
-      <c r="L166" s="4">
-        <v>1</v>
-      </c>
-      <c r="N166">
-        <v>2.5</v>
-      </c>
-      <c r="Q166">
-        <v>6</v>
-      </c>
       <c r="W166" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="167" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2925</v>
+        <v>2926</v>
       </c>
       <c r="C167" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D167" t="s">
         <v>276</v>
       </c>
+      <c r="E167">
+        <v>2</v>
+      </c>
+      <c r="L167" s="4">
+        <v>1</v>
+      </c>
+      <c r="N167">
+        <v>0.02</v>
+      </c>
       <c r="W167" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="168" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2926</v>
+        <v>2927</v>
       </c>
       <c r="C168" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D168" t="s">
         <v>276</v>
       </c>
       <c r="E168">
+        <v>3</v>
+      </c>
+      <c r="L168" s="4">
         <v>2</v>
-      </c>
-      <c r="L168" s="4">
-        <v>1</v>
       </c>
       <c r="N168">
         <v>0.02</v>
       </c>
       <c r="W168" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="169" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2927</v>
+        <v>2931</v>
       </c>
       <c r="C169" t="s">
-        <v>310</v>
+        <v>251</v>
       </c>
       <c r="D169" t="s">
-        <v>276</v>
-      </c>
-      <c r="E169">
-        <v>3</v>
+        <v>294</v>
       </c>
       <c r="L169" s="4">
         <v>2</v>
       </c>
       <c r="N169">
-        <v>0.02</v>
-      </c>
-      <c r="W169" t="s">
-        <v>313</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="170" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2931</v>
+        <v>2932</v>
       </c>
       <c r="C170" t="s">
-        <v>251</v>
+        <v>295</v>
       </c>
       <c r="D170" t="s">
         <v>294</v>
       </c>
       <c r="L170" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N170">
         <v>2.5</v>
       </c>
+      <c r="Q170">
+        <v>4</v>
+      </c>
     </row>
     <row r="171" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2932</v>
+        <v>2933</v>
       </c>
       <c r="C171" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D171" t="s">
         <v>294</v>
@@ -9146,49 +9166,40 @@
         <v>1</v>
       </c>
       <c r="N171">
-        <v>2.5</v>
-      </c>
-      <c r="Q171">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="172" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2933</v>
+        <v>2941</v>
       </c>
       <c r="C172" t="s">
-        <v>299</v>
+        <v>400</v>
       </c>
       <c r="D172" t="s">
         <v>294</v>
       </c>
-      <c r="L172" s="4">
-        <v>1</v>
-      </c>
-      <c r="N172">
-        <v>2</v>
-      </c>
     </row>
     <row r="173" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2941</v>
+        <v>2942</v>
       </c>
       <c r="C173" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D173" t="s">
         <v>294</v>
       </c>
       <c r="E173">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2942</v>
+        <v>2943</v>
       </c>
       <c r="C174" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D174" t="s">
         <v>294</v>
@@ -9199,10 +9210,10 @@
     </row>
     <row r="175" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B175">
-        <v>2943</v>
+        <v>2944</v>
       </c>
       <c r="C175" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D175" t="s">
         <v>294</v>
@@ -9210,13 +9221,19 @@
       <c r="E175">
         <v>2</v>
       </c>
+      <c r="L175" s="4">
+        <v>3</v>
+      </c>
+      <c r="N175">
+        <v>3</v>
+      </c>
     </row>
     <row r="176" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B176">
-        <v>2944</v>
+        <v>2945</v>
       </c>
       <c r="C176" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D176" t="s">
         <v>294</v>
@@ -9224,19 +9241,13 @@
       <c r="E176">
         <v>2</v>
       </c>
-      <c r="L176" s="4">
-        <v>3</v>
-      </c>
-      <c r="N176">
-        <v>3</v>
-      </c>
     </row>
     <row r="177" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B177">
-        <v>2945</v>
+        <v>2946</v>
       </c>
       <c r="C177" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="D177" t="s">
         <v>294</v>
@@ -9247,10 +9258,10 @@
     </row>
     <row r="178" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B178">
-        <v>2946</v>
+        <v>2947</v>
       </c>
       <c r="C178" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D178" t="s">
         <v>294</v>
@@ -9261,10 +9272,10 @@
     </row>
     <row r="179" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2947</v>
+        <v>2948</v>
       </c>
       <c r="C179" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="D179" t="s">
         <v>294</v>
@@ -9275,24 +9286,21 @@
     </row>
     <row r="180" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2948</v>
+        <v>2961</v>
       </c>
       <c r="C180" t="s">
-        <v>407</v>
+        <v>300</v>
       </c>
       <c r="D180" t="s">
-        <v>294</v>
-      </c>
-      <c r="E180">
-        <v>2</v>
+        <v>302</v>
       </c>
     </row>
     <row r="181" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B181">
-        <v>2961</v>
+        <v>2962</v>
       </c>
       <c r="C181" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D181" t="s">
         <v>302</v>
@@ -9300,52 +9308,58 @@
     </row>
     <row r="182" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2962</v>
+        <v>2963</v>
       </c>
       <c r="C182" t="s">
-        <v>301</v>
+        <v>333</v>
       </c>
       <c r="D182" t="s">
         <v>302</v>
       </c>
+      <c r="L182" s="4">
+        <v>1</v>
+      </c>
+      <c r="N182">
+        <v>0.05</v>
+      </c>
     </row>
     <row r="183" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2963</v>
+        <v>2964</v>
       </c>
       <c r="C183" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="D183" t="s">
         <v>302</v>
       </c>
-      <c r="L183" s="4">
-        <v>1</v>
-      </c>
       <c r="N183">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="184" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2964</v>
+        <v>2965</v>
       </c>
       <c r="C184" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D184" t="s">
         <v>302</v>
       </c>
+      <c r="L184" s="4">
+        <v>1</v>
+      </c>
       <c r="N184">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="185" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B185">
-        <v>2965</v>
+        <v>2966</v>
       </c>
       <c r="C185" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="D185" t="s">
         <v>302</v>
@@ -9359,10 +9373,10 @@
     </row>
     <row r="186" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2966</v>
+        <v>2967</v>
       </c>
       <c r="C186" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="D186" t="s">
         <v>302</v>
@@ -9376,27 +9390,33 @@
     </row>
     <row r="187" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B187">
-        <v>2967</v>
+        <v>2971</v>
       </c>
       <c r="C187" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="D187" t="s">
-        <v>302</v>
+        <v>322</v>
+      </c>
+      <c r="E187">
+        <v>2</v>
       </c>
       <c r="L187" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N187">
-        <v>0.05</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q187">
+        <v>15</v>
       </c>
     </row>
     <row r="188" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2971</v>
+        <v>2972</v>
       </c>
       <c r="C188" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="D188" t="s">
         <v>322</v>
@@ -9405,21 +9425,18 @@
         <v>2</v>
       </c>
       <c r="L188" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N188">
-        <v>0.08</v>
-      </c>
-      <c r="Q188">
-        <v>15</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="189" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2972</v>
+        <v>2973</v>
       </c>
       <c r="C189" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D189" t="s">
         <v>322</v>
@@ -9428,18 +9445,15 @@
         <v>2</v>
       </c>
       <c r="L189" s="4">
-        <v>2</v>
-      </c>
-      <c r="N189">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2973</v>
+        <v>2974</v>
       </c>
       <c r="C190" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="D190" t="s">
         <v>322</v>
@@ -9447,81 +9461,84 @@
       <c r="E190">
         <v>2</v>
       </c>
-      <c r="L190" s="4">
-        <v>1</v>
+      <c r="N190">
+        <v>0.05</v>
       </c>
     </row>
     <row r="191" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2974</v>
+        <v>2975</v>
       </c>
       <c r="C191" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="D191" t="s">
         <v>322</v>
       </c>
-      <c r="E191">
-        <v>2</v>
-      </c>
-      <c r="N191">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="192" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2975</v>
+        <v>2976</v>
       </c>
       <c r="C192" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="D192" t="s">
         <v>322</v>
       </c>
+      <c r="L192" s="4">
+        <v>1</v>
+      </c>
+      <c r="N192">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="193" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2976</v>
+        <v>2977</v>
       </c>
       <c r="C193" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D193" t="s">
         <v>322</v>
       </c>
+      <c r="E193">
+        <v>2</v>
+      </c>
       <c r="L193" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N193">
-        <v>0.02</v>
+        <v>0.05</v>
+      </c>
+      <c r="Q193">
+        <v>5</v>
       </c>
     </row>
     <row r="194" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2977</v>
+        <v>2978</v>
       </c>
       <c r="C194" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="D194" t="s">
         <v>322</v>
       </c>
+      <c r="E194">
+        <v>3</v>
+      </c>
       <c r="L194" s="4">
-        <v>2</v>
-      </c>
-      <c r="N194">
-        <v>0.05</v>
-      </c>
-      <c r="Q194">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2978</v>
+        <v>2979</v>
       </c>
       <c r="C195" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D195" t="s">
         <v>322</v>
@@ -9535,10 +9552,10 @@
     </row>
     <row r="196" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2979</v>
+        <v>2980</v>
       </c>
       <c r="C196" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="D196" t="s">
         <v>322</v>
@@ -9547,83 +9564,66 @@
         <v>3</v>
       </c>
       <c r="L196" s="4">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="N196">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q196">
+        <v>20</v>
       </c>
     </row>
     <row r="197" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2980</v>
+        <v>2981</v>
       </c>
       <c r="C197" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="D197" t="s">
         <v>322</v>
       </c>
       <c r="E197">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L197" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N197">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q197">
-        <v>20</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="198" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2981</v>
+        <v>2982</v>
       </c>
       <c r="C198" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="D198" t="s">
         <v>322</v>
       </c>
       <c r="E198">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L198" s="4">
-        <v>2</v>
-      </c>
-      <c r="N198">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2982</v>
+        <v>2983</v>
       </c>
       <c r="C199" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D199" t="s">
         <v>322</v>
       </c>
-      <c r="E199">
-        <v>3</v>
-      </c>
       <c r="L199" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B200">
-        <v>2983</v>
-      </c>
-      <c r="C200" t="s">
-        <v>339</v>
-      </c>
-      <c r="D200" t="s">
-        <v>322</v>
-      </c>
-      <c r="L200" s="4">
-        <v>1</v>
-      </c>
-      <c r="N200">
+      <c r="N199">
         <v>0.02</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.6.3n: Began Item images
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8544B0B7-BF7B-43A3-A87D-9C7197D16D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FB563A-9889-421D-BA43-8A939938634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1425" uniqueCount="831">
   <si>
     <t>ID</t>
   </si>
@@ -2532,6 +2532,12 @@
   </si>
   <si>
     <t>Can launch game (tutorial gives 1 achievement token)</t>
+  </si>
+  <si>
+    <t>Can see allied vision</t>
+  </si>
+  <si>
+    <t>"14"</t>
   </si>
 </sst>
 </file>
@@ -3621,10 +3627,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4010,6 +4016,9 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
+      <c r="D31" t="s">
+        <v>830</v>
+      </c>
       <c r="E31">
         <v>1</v>
       </c>
@@ -4028,6 +4037,11 @@
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
         <v>826</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>829</v>
       </c>
     </row>
   </sheetData>
@@ -4148,7 +4162,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
@@ -5468,8 +5482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6413,13 +6427,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y199"/>
+  <dimension ref="A1:Y202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D165" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E187" sqref="E187"/>
+      <selection pane="bottomRight" activeCell="E199" sqref="E199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9242,7 +9256,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B177">
         <v>2946</v>
       </c>
@@ -9256,7 +9270,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B178">
         <v>2947</v>
       </c>
@@ -9270,7 +9284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B179">
         <v>2948</v>
       </c>
@@ -9284,7 +9298,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B180">
         <v>2961</v>
       </c>
@@ -9295,7 +9309,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B181">
         <v>2962</v>
       </c>
@@ -9306,7 +9320,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B182">
         <v>2963</v>
       </c>
@@ -9323,7 +9337,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B183">
         <v>2964</v>
       </c>
@@ -9337,7 +9351,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B184">
         <v>2965</v>
       </c>
@@ -9354,7 +9368,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B185">
         <v>2966</v>
       </c>
@@ -9371,7 +9385,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B186">
         <v>2967</v>
       </c>
@@ -9388,67 +9402,52 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B187">
         <v>2971</v>
       </c>
       <c r="C187" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D187" t="s">
         <v>322</v>
       </c>
-      <c r="E187">
-        <v>2</v>
-      </c>
-      <c r="L187" s="4">
-        <v>3</v>
-      </c>
-      <c r="N187">
-        <v>0.08</v>
-      </c>
-      <c r="Q187">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="188" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B188">
         <v>2972</v>
       </c>
       <c r="C188" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="D188" t="s">
         <v>322</v>
       </c>
-      <c r="E188">
-        <v>2</v>
-      </c>
       <c r="L188" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N188">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="189" spans="2:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B189">
         <v>2973</v>
       </c>
       <c r="C189" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="D189" t="s">
         <v>322</v>
       </c>
-      <c r="E189">
-        <v>2</v>
-      </c>
       <c r="L189" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="190" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N189">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="190" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B190">
         <v>2974</v>
       </c>
@@ -9465,32 +9464,41 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="191" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B191">
         <v>2975</v>
       </c>
       <c r="C191" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="D191" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E191">
+        <v>2</v>
+      </c>
+      <c r="L191" s="4">
+        <v>2</v>
+      </c>
+      <c r="N191">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B192">
         <v>2976</v>
       </c>
       <c r="C192" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D192" t="s">
         <v>322</v>
       </c>
+      <c r="E192">
+        <v>2</v>
+      </c>
       <c r="L192" s="4">
         <v>1</v>
-      </c>
-      <c r="N192">
-        <v>0.02</v>
       </c>
     </row>
     <row r="193" spans="2:17" x14ac:dyDescent="0.25">
@@ -9498,22 +9506,22 @@
         <v>2977</v>
       </c>
       <c r="C193" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D193" t="s">
         <v>322</v>
       </c>
       <c r="E193">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L193" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N193">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Q193">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="194" spans="2:17" x14ac:dyDescent="0.25">
@@ -9521,7 +9529,7 @@
         <v>2978</v>
       </c>
       <c r="C194" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="D194" t="s">
         <v>322</v>
@@ -9530,7 +9538,10 @@
         <v>3</v>
       </c>
       <c r="L194" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N194">
+        <v>0.1</v>
       </c>
     </row>
     <row r="195" spans="2:17" x14ac:dyDescent="0.25">
@@ -9538,7 +9549,7 @@
         <v>2979</v>
       </c>
       <c r="C195" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D195" t="s">
         <v>322</v>
@@ -9547,7 +9558,13 @@
         <v>3</v>
       </c>
       <c r="L195" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N195">
+        <v>0.05</v>
+      </c>
+      <c r="Q195">
+        <v>5</v>
       </c>
     </row>
     <row r="196" spans="2:17" x14ac:dyDescent="0.25">
@@ -9555,22 +9572,16 @@
         <v>2980</v>
       </c>
       <c r="C196" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="D196" t="s">
         <v>322</v>
       </c>
       <c r="E196">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L196" s="4">
-        <v>5</v>
-      </c>
-      <c r="N196">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q196">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197" spans="2:17" x14ac:dyDescent="0.25">
@@ -9578,19 +9589,16 @@
         <v>2981</v>
       </c>
       <c r="C197" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D197" t="s">
         <v>322</v>
       </c>
       <c r="E197">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L197" s="4">
-        <v>2</v>
-      </c>
-      <c r="N197">
-        <v>0.02</v>
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="2:17" x14ac:dyDescent="0.25">
@@ -9598,13 +9606,13 @@
         <v>2982</v>
       </c>
       <c r="C198" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D198" t="s">
         <v>322</v>
       </c>
       <c r="E198">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L198" s="4">
         <v>1</v>
@@ -9615,17 +9623,35 @@
         <v>2983</v>
       </c>
       <c r="C199" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D199" t="s">
         <v>322</v>
       </c>
+      <c r="E199">
+        <v>5</v>
+      </c>
       <c r="L199" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N199">
-        <v>0.02</v>
-      </c>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q199">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="200" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K200" s="4"/>
+      <c r="L200"/>
+    </row>
+    <row r="201" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K201" s="4"/>
+      <c r="L201"/>
+    </row>
+    <row r="202" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K202" s="4"/>
+      <c r="L202"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
v0.6.3s: Finished initial item images
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D952E5EE-7E2F-4F82-9C31-4DC11272AD63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0290B12B-A1B4-451F-BDCA-4212435BACA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -989,9 +989,6 @@
     <t>holds 30 thirst, can also throw</t>
   </si>
   <si>
-    <t>Glass</t>
-  </si>
-  <si>
     <t>Wire</t>
   </si>
   <si>
@@ -2538,6 +2535,9 @@
   </si>
   <si>
     <t>Recurve Bow</t>
+  </si>
+  <si>
+    <t>Broken Glass</t>
   </si>
 </sst>
 </file>
@@ -2953,7 +2953,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -2965,10 +2965,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2979,7 +2979,7 @@
         <v>211</v>
       </c>
       <c r="D4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -2990,7 +2990,7 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D6" t="s">
         <v>216</v>
@@ -3004,7 +3004,7 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3012,7 +3012,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
         <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3036,7 +3036,7 @@
         <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3044,7 +3044,7 @@
         <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3052,7 +3052,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3060,7 +3060,7 @@
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
         <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
         <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3092,7 +3092,7 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3100,7 +3100,7 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3116,7 +3116,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3124,7 +3124,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3132,7 +3132,7 @@
         <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3140,7 +3140,7 @@
         <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3148,7 +3148,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3164,7 +3164,7 @@
         <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3172,7 +3172,7 @@
         <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3180,7 +3180,7 @@
         <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3188,7 +3188,7 @@
         <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3196,7 +3196,7 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -3212,7 +3212,7 @@
         <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
         <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -3228,7 +3228,7 @@
         <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -3236,7 +3236,7 @@
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -3244,7 +3244,7 @@
         <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -3252,7 +3252,7 @@
         <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -3260,7 +3260,7 @@
         <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -3268,7 +3268,7 @@
         <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -3276,7 +3276,7 @@
         <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -3284,7 +3284,7 @@
         <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -3300,7 +3300,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -3308,7 +3308,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -3316,7 +3316,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -3324,7 +3324,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3332,7 +3332,7 @@
         <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D49" t="s">
         <v>219</v>
@@ -3346,7 +3346,7 @@
         <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -3354,7 +3354,7 @@
         <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -3362,7 +3362,7 @@
         <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -3370,7 +3370,7 @@
         <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -3378,7 +3378,7 @@
         <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -3394,7 +3394,7 @@
         <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
         <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -3410,7 +3410,7 @@
         <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -3421,13 +3421,13 @@
         <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="D60" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E60" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -3443,7 +3443,7 @@
         <v>303</v>
       </c>
       <c r="C62" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -3451,7 +3451,7 @@
         <v>304</v>
       </c>
       <c r="C63" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -3459,7 +3459,7 @@
         <v>305</v>
       </c>
       <c r="C64" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -3467,7 +3467,7 @@
         <v>306</v>
       </c>
       <c r="C65" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -3475,7 +3475,7 @@
         <v>307</v>
       </c>
       <c r="C66" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -3483,7 +3483,7 @@
         <v>308</v>
       </c>
       <c r="C67" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -3491,7 +3491,7 @@
         <v>309</v>
       </c>
       <c r="C68" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -3499,7 +3499,7 @@
         <v>310</v>
       </c>
       <c r="C69" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -3507,7 +3507,7 @@
         <v>311</v>
       </c>
       <c r="C70" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -3515,7 +3515,7 @@
         <v>312</v>
       </c>
       <c r="C71" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -3523,7 +3523,7 @@
         <v>313</v>
       </c>
       <c r="C72" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -3531,7 +3531,7 @@
         <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -3539,7 +3539,7 @@
         <v>315</v>
       </c>
       <c r="C74" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -3547,7 +3547,7 @@
         <v>316</v>
       </c>
       <c r="C75" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
@@ -3555,7 +3555,7 @@
         <v>317</v>
       </c>
       <c r="C76" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -3563,7 +3563,7 @@
         <v>318</v>
       </c>
       <c r="C77" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -3571,7 +3571,7 @@
         <v>319</v>
       </c>
       <c r="C78" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
@@ -3579,7 +3579,7 @@
         <v>320</v>
       </c>
       <c r="C79" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -3587,7 +3587,7 @@
         <v>321</v>
       </c>
       <c r="C80" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
         <v>322</v>
       </c>
       <c r="C81" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
@@ -3603,7 +3603,7 @@
         <v>323</v>
       </c>
       <c r="C82" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -3611,7 +3611,7 @@
         <v>324</v>
       </c>
       <c r="C83" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
@@ -3644,7 +3644,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3655,393 +3655,393 @@
         <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D4" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15"/>
       <c r="C5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15"/>
       <c r="C6" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15"/>
       <c r="C7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G7" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15"/>
       <c r="C8" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D8" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G8" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="15"/>
       <c r="C9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D9" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G9" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D10" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G10" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="15"/>
       <c r="C11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D11" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="15"/>
       <c r="C12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D12" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="G12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="15"/>
       <c r="C13" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D13" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G13" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C15" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D15" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="15"/>
       <c r="C16" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D16" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="15"/>
       <c r="C17" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D17" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G17" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="15"/>
       <c r="C18" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="15"/>
       <c r="C19" t="s">
+        <v>648</v>
+      </c>
+      <c r="D19" t="s">
         <v>649</v>
-      </c>
-      <c r="D19" t="s">
-        <v>650</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="15"/>
       <c r="C20" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="G20" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="15"/>
       <c r="C21" t="s">
+        <v>640</v>
+      </c>
+      <c r="D21" t="s">
         <v>641</v>
-      </c>
-      <c r="D21" t="s">
-        <v>642</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="G21" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="15"/>
       <c r="C22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="15"/>
       <c r="C23" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="15"/>
       <c r="C24" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D24" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="D31" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>821</v>
+      </c>
+      <c r="G32" t="s">
         <v>822</v>
-      </c>
-      <c r="G32" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
   </sheetData>
@@ -4178,7 +4178,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -4193,7 +4193,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>220</v>
@@ -4216,10 +4216,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="H4" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4230,13 +4230,13 @@
         <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4250,7 +4250,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4261,13 +4261,13 @@
         <v>214</v>
       </c>
       <c r="D8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4289,7 +4289,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>230</v>
@@ -4298,10 +4298,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H11" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4319,7 +4319,7 @@
         <v>239</v>
       </c>
       <c r="H12" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -4330,7 +4330,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -4338,16 +4338,16 @@
         <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H14" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -4355,7 +4355,7 @@
         <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -4363,7 +4363,7 @@
         <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -4371,7 +4371,7 @@
         <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -4379,10 +4379,10 @@
         <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -4396,10 +4396,10 @@
         <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H19" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -4407,7 +4407,7 @@
         <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -4415,7 +4415,7 @@
         <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -4423,7 +4423,7 @@
         <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -4431,16 +4431,16 @@
         <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H23" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -4448,7 +4448,7 @@
         <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -4459,7 +4459,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -4470,7 +4470,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -4484,10 +4484,10 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H27" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -4495,7 +4495,7 @@
         <v>132</v>
       </c>
       <c r="H28" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -4503,7 +4503,7 @@
         <v>133</v>
       </c>
       <c r="H29" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -4511,7 +4511,7 @@
         <v>134</v>
       </c>
       <c r="H30" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -4525,10 +4525,10 @@
         <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H31" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -4536,7 +4536,7 @@
         <v>142</v>
       </c>
       <c r="H32" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -4544,7 +4544,7 @@
         <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D33" t="s">
         <v>232</v>
@@ -4553,10 +4553,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="H33" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -4564,7 +4564,7 @@
         <v>152</v>
       </c>
       <c r="H34" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -4572,7 +4572,7 @@
         <v>153</v>
       </c>
       <c r="H35" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
         <v>154</v>
       </c>
       <c r="H36" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -4588,10 +4588,10 @@
         <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="H37" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -4599,7 +4599,7 @@
         <v>156</v>
       </c>
       <c r="H38" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -4607,7 +4607,7 @@
         <v>157</v>
       </c>
       <c r="H39" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -4615,7 +4615,7 @@
         <v>158</v>
       </c>
       <c r="H40" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -4696,7 +4696,7 @@
         <v>238</v>
       </c>
       <c r="D46" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -4716,10 +4716,10 @@
         <v>7</v>
       </c>
       <c r="G47" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H47" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -4733,7 +4733,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -4755,7 +4755,7 @@
         <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -4862,7 +4862,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -4870,16 +4870,16 @@
         <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H58" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -4887,7 +4887,7 @@
         <v>192</v>
       </c>
       <c r="H59" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -4895,10 +4895,10 @@
         <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H60" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -4906,7 +4906,7 @@
         <v>194</v>
       </c>
       <c r="H61" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -4917,13 +4917,13 @@
         <v>224</v>
       </c>
       <c r="D62" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E62">
         <v>100</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -4940,27 +4940,27 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C64" t="s">
         <v>250</v>
       </c>
       <c r="D64" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="G64" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="H64" t="s">
         <v>800</v>
-      </c>
-      <c r="H64" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C65" t="s">
         <v>249</v>
@@ -4969,10 +4969,10 @@
         <v>9</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H65" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -4983,16 +4983,16 @@
         <v>254</v>
       </c>
       <c r="D66" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H66" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -5001,12 +5001,12 @@
       </c>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C69" t="s">
         <v>218</v>
@@ -5018,10 +5018,10 @@
         <v>100</v>
       </c>
       <c r="G69" t="s">
+        <v>760</v>
+      </c>
+      <c r="H69" t="s">
         <v>761</v>
-      </c>
-      <c r="H69" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -5032,10 +5032,10 @@
         <v>223</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H70" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -5043,7 +5043,7 @@
         <v>312</v>
       </c>
       <c r="H71" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -5051,19 +5051,19 @@
         <v>321</v>
       </c>
       <c r="C72" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D72" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="H72" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -5074,10 +5074,10 @@
         <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H73" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -5085,10 +5085,10 @@
         <v>323</v>
       </c>
       <c r="G74" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="H74" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -5100,16 +5100,16 @@
         <v>222</v>
       </c>
       <c r="D75" t="s">
+        <v>780</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>767</v>
+      </c>
+      <c r="H75" t="s">
         <v>781</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75" t="s">
-        <v>768</v>
-      </c>
-      <c r="H75" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -5118,7 +5118,7 @@
         <v>332</v>
       </c>
       <c r="H76" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -5127,7 +5127,7 @@
         <v>333</v>
       </c>
       <c r="H77" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -5136,7 +5136,7 @@
         <v>334</v>
       </c>
       <c r="H78" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -5145,7 +5145,7 @@
         <v>335</v>
       </c>
       <c r="H79" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -5154,7 +5154,7 @@
         <v>336</v>
       </c>
       <c r="H80" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -5163,7 +5163,7 @@
         <v>337</v>
       </c>
       <c r="H81" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>338</v>
       </c>
       <c r="H82" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -5181,16 +5181,16 @@
         <v>339</v>
       </c>
       <c r="C83" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E83">
         <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="H83" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -5199,7 +5199,7 @@
         <v>340</v>
       </c>
       <c r="H84" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -5208,7 +5208,7 @@
         <v>341</v>
       </c>
       <c r="H85" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -5217,7 +5217,7 @@
         <v>342</v>
       </c>
       <c r="H86" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -5226,13 +5226,13 @@
         <v>343</v>
       </c>
       <c r="C87" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G87" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="H87" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -5241,7 +5241,7 @@
         <v>344</v>
       </c>
       <c r="H88" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -5250,7 +5250,7 @@
         <v>345</v>
       </c>
       <c r="H89" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -5259,7 +5259,7 @@
         <v>346</v>
       </c>
       <c r="H90" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -5284,7 +5284,7 @@
         <v>411</v>
       </c>
       <c r="C93" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -5293,7 +5293,7 @@
         <v>303</v>
       </c>
       <c r="H93" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -5304,7 +5304,7 @@
         <v>304</v>
       </c>
       <c r="H94" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -5312,13 +5312,13 @@
         <v>421</v>
       </c>
       <c r="C95" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E95">
         <v>20</v>
       </c>
       <c r="G95" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -5326,7 +5326,7 @@
         <v>422</v>
       </c>
       <c r="C96" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -5334,7 +5334,7 @@
         <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -5342,7 +5342,7 @@
         <v>424</v>
       </c>
       <c r="C98" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -5350,7 +5350,7 @@
         <v>425</v>
       </c>
       <c r="C99" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E99">
         <v>35</v>
@@ -5378,10 +5378,10 @@
         <v>5</v>
       </c>
       <c r="G101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H101" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
@@ -5389,7 +5389,7 @@
         <v>442</v>
       </c>
       <c r="H102" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -5397,7 +5397,7 @@
         <v>443</v>
       </c>
       <c r="H103" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
@@ -5483,7 +5483,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5542,13 +5542,13 @@
         <v>1001</v>
       </c>
       <c r="C3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D3" t="s">
         <v>414</v>
       </c>
-      <c r="D3" t="s">
-        <v>415</v>
-      </c>
       <c r="E3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -5557,7 +5557,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -5565,13 +5565,13 @@
         <v>1002</v>
       </c>
       <c r="C4" t="s">
+        <v>815</v>
+      </c>
+      <c r="D4" t="s">
         <v>816</v>
       </c>
-      <c r="D4" t="s">
-        <v>817</v>
-      </c>
       <c r="E4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -5585,7 +5585,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -5614,10 +5614,10 @@
         <v>1102</v>
       </c>
       <c r="C7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E7" t="s">
         <v>480</v>
-      </c>
-      <c r="E7" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -5625,10 +5625,10 @@
         <v>1103</v>
       </c>
       <c r="C8" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E8" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -5636,10 +5636,10 @@
         <v>1104</v>
       </c>
       <c r="C9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E9" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -5647,10 +5647,10 @@
         <v>1105</v>
       </c>
       <c r="C10" t="s">
+        <v>817</v>
+      </c>
+      <c r="E10" t="s">
         <v>818</v>
-      </c>
-      <c r="E10" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -5658,10 +5658,10 @@
         <v>1106</v>
       </c>
       <c r="C11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -5669,10 +5669,10 @@
         <v>1116</v>
       </c>
       <c r="C12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E12" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -5680,10 +5680,10 @@
         <v>1117</v>
       </c>
       <c r="C13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -5691,10 +5691,10 @@
         <v>1118</v>
       </c>
       <c r="C14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -5702,10 +5702,10 @@
         <v>1119</v>
       </c>
       <c r="C15" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -5713,10 +5713,10 @@
         <v>1120</v>
       </c>
       <c r="C16" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -6044,27 +6044,27 @@
     </row>
     <row r="3" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="4" spans="2:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
+        <v>448</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>525</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>449</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>526</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="E4" s="11" t="s">
         <v>450</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -6076,16 +6076,16 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -6093,27 +6093,27 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E8" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -6121,13 +6121,13 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -6135,159 +6135,159 @@
         <v>206</v>
       </c>
       <c r="C10" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D10" t="s">
         <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C12" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D13" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E13" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C15" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D15" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E15" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C16" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E16" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C17" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E17" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F17" s="13"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C18" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D18" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F18" s="13"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F19" s="13"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D20" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E20" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C21" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D21" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E21" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -6295,125 +6295,125 @@
         <v>205</v>
       </c>
       <c r="C22" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D22" t="s">
         <v>207</v>
       </c>
       <c r="E22" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C23" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D23" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E23" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C24" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D24" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E24" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C25" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D25" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E25" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C26" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C29" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C30" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C33" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E33" t="s">
+        <v>532</v>
+      </c>
+      <c r="F33" t="s">
         <v>533</v>
-      </c>
-      <c r="F33" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>557</v>
+      </c>
+      <c r="C34" t="s">
         <v>558</v>
-      </c>
-      <c r="C34" t="s">
-        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -6430,10 +6430,10 @@
   <dimension ref="A1:Y202"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D129" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomRight" activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6528,10 +6528,10 @@
         <v>7</v>
       </c>
       <c r="T2" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="U2" s="1" t="s">
         <v>345</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>346</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>9</v>
@@ -6601,7 +6601,7 @@
         <v>2105</v>
       </c>
       <c r="C8" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H8">
         <v>4</v>
@@ -7067,7 +7067,7 @@
         <v>30</v>
       </c>
       <c r="L42" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="N42">
         <v>3</v>
@@ -7076,7 +7076,7 @@
         <v>1</v>
       </c>
       <c r="W42" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
@@ -7084,13 +7084,13 @@
         <v>2311</v>
       </c>
       <c r="C43" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E43">
         <v>2</v>
       </c>
       <c r="L43" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="N43">
         <v>5</v>
@@ -7102,7 +7102,7 @@
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
@@ -7128,7 +7128,7 @@
         <v>8</v>
       </c>
       <c r="W44" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
@@ -7154,7 +7154,7 @@
         <v>6</v>
       </c>
       <c r="W45" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
@@ -7168,7 +7168,7 @@
         <v>3</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="N46">
         <v>7</v>
@@ -7180,7 +7180,7 @@
         <v>20</v>
       </c>
       <c r="W46" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
@@ -7194,7 +7194,7 @@
         <v>3</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="N47">
         <v>9</v>
@@ -7206,7 +7206,7 @@
         <v>30</v>
       </c>
       <c r="W47" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
@@ -7232,7 +7232,7 @@
         <v>6</v>
       </c>
       <c r="W48" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
@@ -7246,7 +7246,7 @@
         <v>4</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N49">
         <v>10</v>
@@ -7258,7 +7258,7 @@
         <v>20</v>
       </c>
       <c r="W49" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
@@ -7272,7 +7272,7 @@
         <v>4</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="N50">
         <v>7</v>
@@ -7284,7 +7284,7 @@
         <v>6</v>
       </c>
       <c r="W50" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
@@ -7313,7 +7313,7 @@
         <v>1</v>
       </c>
       <c r="W51" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
@@ -7339,7 +7339,7 @@
         <v>6</v>
       </c>
       <c r="W52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
@@ -7353,7 +7353,7 @@
         <v>5</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="N53">
         <v>8</v>
@@ -7365,7 +7365,7 @@
         <v>20</v>
       </c>
       <c r="W53" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
@@ -7379,7 +7379,7 @@
         <v>5</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="N54">
         <v>10</v>
@@ -7391,7 +7391,7 @@
         <v>30</v>
       </c>
       <c r="W54" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
@@ -7405,7 +7405,7 @@
         <v>5</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="N55">
         <v>4</v>
@@ -7417,7 +7417,7 @@
         <v>5</v>
       </c>
       <c r="W55" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
@@ -7431,7 +7431,7 @@
         <v>6</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="N56">
         <v>10</v>
@@ -7443,7 +7443,7 @@
         <v>35</v>
       </c>
       <c r="W56" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
@@ -7457,7 +7457,7 @@
         <v>6</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="N57">
         <v>11</v>
@@ -7469,7 +7469,7 @@
         <v>30</v>
       </c>
       <c r="W57" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
@@ -7501,7 +7501,7 @@
         <v>1</v>
       </c>
       <c r="W58" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
@@ -7515,7 +7515,7 @@
         <v>6</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="N59">
         <v>7</v>
@@ -7527,7 +7527,7 @@
         <v>12</v>
       </c>
       <c r="W59" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
@@ -7541,7 +7541,7 @@
         <v>6</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N60">
         <v>11</v>
@@ -7553,7 +7553,7 @@
         <v>30</v>
       </c>
       <c r="W60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
@@ -7567,7 +7567,7 @@
         <v>7</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="N61">
         <v>11</v>
@@ -7579,7 +7579,7 @@
         <v>100</v>
       </c>
       <c r="W61" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
@@ -7605,7 +7605,7 @@
         <v>8</v>
       </c>
       <c r="W62" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
@@ -7619,7 +7619,7 @@
         <v>7</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="N63">
         <v>16</v>
@@ -7634,7 +7634,7 @@
         <v>4</v>
       </c>
       <c r="W63" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
@@ -7648,7 +7648,7 @@
         <v>7</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N64">
         <v>5</v>
@@ -7660,7 +7660,7 @@
         <v>5</v>
       </c>
       <c r="W64" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
@@ -7674,7 +7674,7 @@
         <v>8</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="N65">
         <v>10</v>
@@ -7686,7 +7686,7 @@
         <v>125</v>
       </c>
       <c r="W65" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
@@ -7715,7 +7715,7 @@
         <v>20</v>
       </c>
       <c r="W66" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
@@ -7729,7 +7729,7 @@
         <v>8</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N67">
         <v>11</v>
@@ -7741,7 +7741,7 @@
         <v>35</v>
       </c>
       <c r="W67" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
@@ -7773,7 +7773,7 @@
         <v>1</v>
       </c>
       <c r="W68" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
@@ -7787,7 +7787,7 @@
         <v>8</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="N69">
         <v>12</v>
@@ -7799,7 +7799,7 @@
         <v>30</v>
       </c>
       <c r="W69" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
@@ -7813,7 +7813,7 @@
         <v>9</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="N70">
         <v>12</v>
@@ -7825,7 +7825,7 @@
         <v>125</v>
       </c>
       <c r="W70" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
@@ -7851,7 +7851,7 @@
         <v>8</v>
       </c>
       <c r="W71" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
@@ -7865,7 +7865,7 @@
         <v>10</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="N72">
         <v>11</v>
@@ -7877,7 +7877,7 @@
         <v>125</v>
       </c>
       <c r="W72" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
@@ -7906,7 +7906,7 @@
         <v>40</v>
       </c>
       <c r="W73" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
@@ -8171,7 +8171,7 @@
         <v>2513</v>
       </c>
       <c r="C95" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N95">
         <v>0.04</v>
@@ -8386,7 +8386,7 @@
         <v>2641</v>
       </c>
       <c r="C112" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E112">
         <v>5</v>
@@ -8517,7 +8517,7 @@
         <v>2705</v>
       </c>
       <c r="C123" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="O123">
         <v>2</v>
@@ -8562,7 +8562,7 @@
         <v>2713</v>
       </c>
       <c r="C126" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E126">
         <v>2</v>
@@ -8582,7 +8582,7 @@
         <v>2714</v>
       </c>
       <c r="C127" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E127">
         <v>2</v>
@@ -8722,7 +8722,7 @@
         <v>2802</v>
       </c>
       <c r="C138" t="s">
-        <v>314</v>
+        <v>830</v>
       </c>
     </row>
     <row r="139" spans="2:25" x14ac:dyDescent="0.25">
@@ -8730,7 +8730,7 @@
         <v>2803</v>
       </c>
       <c r="C139" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="140" spans="2:25" x14ac:dyDescent="0.25">
@@ -8749,7 +8749,7 @@
         <v>2812</v>
       </c>
       <c r="C141" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E141">
         <v>2</v>
@@ -8771,7 +8771,7 @@
         <v>2822</v>
       </c>
       <c r="C143" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E143">
         <v>3</v>
@@ -8986,7 +8986,7 @@
         <v>2917</v>
       </c>
       <c r="C161" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D161" t="s">
         <v>270</v>
@@ -9188,7 +9188,7 @@
         <v>2941</v>
       </c>
       <c r="C172" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D172" t="s">
         <v>293</v>
@@ -9199,7 +9199,7 @@
         <v>2942</v>
       </c>
       <c r="C173" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D173" t="s">
         <v>293</v>
@@ -9213,7 +9213,7 @@
         <v>2943</v>
       </c>
       <c r="C174" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D174" t="s">
         <v>293</v>
@@ -9227,7 +9227,7 @@
         <v>2944</v>
       </c>
       <c r="C175" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D175" t="s">
         <v>293</v>
@@ -9247,7 +9247,7 @@
         <v>2945</v>
       </c>
       <c r="C176" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D176" t="s">
         <v>293</v>
@@ -9261,7 +9261,7 @@
         <v>2946</v>
       </c>
       <c r="C177" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D177" t="s">
         <v>293</v>
@@ -9275,7 +9275,7 @@
         <v>2947</v>
       </c>
       <c r="C178" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D178" t="s">
         <v>293</v>
@@ -9289,7 +9289,7 @@
         <v>2948</v>
       </c>
       <c r="C179" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D179" t="s">
         <v>293</v>
@@ -9325,7 +9325,7 @@
         <v>2963</v>
       </c>
       <c r="C182" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D182" t="s">
         <v>301</v>
@@ -9342,7 +9342,7 @@
         <v>2964</v>
       </c>
       <c r="C183" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D183" t="s">
         <v>301</v>
@@ -9356,7 +9356,7 @@
         <v>2965</v>
       </c>
       <c r="C184" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D184" t="s">
         <v>301</v>
@@ -9373,7 +9373,7 @@
         <v>2966</v>
       </c>
       <c r="C185" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D185" t="s">
         <v>301</v>
@@ -9390,7 +9390,7 @@
         <v>2967</v>
       </c>
       <c r="C186" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D186" t="s">
         <v>301</v>
@@ -9407,10 +9407,10 @@
         <v>2971</v>
       </c>
       <c r="C187" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D187" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="188" spans="2:14" x14ac:dyDescent="0.25">
@@ -9418,10 +9418,10 @@
         <v>2972</v>
       </c>
       <c r="C188" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D188" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L188" s="4">
         <v>1</v>
@@ -9435,10 +9435,10 @@
         <v>2973</v>
       </c>
       <c r="C189" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D189" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="L189" s="4">
         <v>1</v>
@@ -9452,10 +9452,10 @@
         <v>2974</v>
       </c>
       <c r="C190" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D190" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E190">
         <v>2</v>
@@ -9469,10 +9469,10 @@
         <v>2975</v>
       </c>
       <c r="C191" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D191" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E191">
         <v>2</v>
@@ -9489,10 +9489,10 @@
         <v>2976</v>
       </c>
       <c r="C192" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D192" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E192">
         <v>2</v>
@@ -9506,10 +9506,10 @@
         <v>2977</v>
       </c>
       <c r="C193" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D193" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E193">
         <v>3</v>
@@ -9529,10 +9529,10 @@
         <v>2978</v>
       </c>
       <c r="C194" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D194" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E194">
         <v>3</v>
@@ -9549,10 +9549,10 @@
         <v>2979</v>
       </c>
       <c r="C195" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D195" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E195">
         <v>3</v>
@@ -9572,10 +9572,10 @@
         <v>2980</v>
       </c>
       <c r="C196" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D196" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E196">
         <v>4</v>
@@ -9589,10 +9589,10 @@
         <v>2981</v>
       </c>
       <c r="C197" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D197" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E197">
         <v>4</v>
@@ -9606,10 +9606,10 @@
         <v>2982</v>
       </c>
       <c r="C198" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D198" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E198">
         <v>4</v>
@@ -9623,10 +9623,10 @@
         <v>2983</v>
       </c>
       <c r="C199" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D199" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E199">
         <v>5</v>
@@ -9701,7 +9701,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
@@ -9727,7 +9727,7 @@
         <v>0.5</v>
       </c>
       <c r="J3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9755,7 +9755,7 @@
         <v>3103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D5" t="s">
         <v>292</v>
@@ -9815,7 +9815,7 @@
         <v>3108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D8" t="s">
         <v>292</v>
@@ -9832,10 +9832,10 @@
         <v>3111</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D9" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9">
@@ -9850,10 +9850,10 @@
         <v>3112</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10">
@@ -9871,7 +9871,7 @@
         <v>7.62</v>
       </c>
       <c r="D11" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11">
@@ -9889,7 +9889,7 @@
         <v>7.62</v>
       </c>
       <c r="D12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12">
@@ -9907,7 +9907,7 @@
         <v>7.62</v>
       </c>
       <c r="D13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13">
@@ -9922,7 +9922,7 @@
         <v>7.62</v>
       </c>
       <c r="D14" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14">
@@ -9934,10 +9934,10 @@
         <v>3117</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D15" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15">
@@ -9949,10 +9949,10 @@
         <v>3118</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16">
@@ -9964,10 +9964,10 @@
         <v>3119</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17">
@@ -9982,10 +9982,10 @@
         <v>3120</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18">
@@ -10003,7 +10003,7 @@
         <v>5.56</v>
       </c>
       <c r="D19" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19">
@@ -10018,7 +10018,7 @@
         <v>7.62</v>
       </c>
       <c r="D20" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20">
@@ -10030,10 +10030,10 @@
         <v>3123</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D21" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21">
@@ -10048,10 +10048,10 @@
         <v>3124</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D22" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22">
@@ -10069,7 +10069,7 @@
         <v>7.62</v>
       </c>
       <c r="D23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23">
@@ -10087,7 +10087,7 @@
         <v>7.62</v>
       </c>
       <c r="D24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24">
@@ -10102,10 +10102,10 @@
         <v>3127</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D25" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25">
@@ -10120,10 +10120,10 @@
         <v>3128</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D26" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26">
@@ -10135,10 +10135,10 @@
         <v>3129</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27">
@@ -10153,10 +10153,10 @@
         <v>3130</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28">
@@ -10171,10 +10171,10 @@
         <v>3131</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D29" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29">
@@ -10186,10 +10186,10 @@
         <v>3132</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D30" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30">
@@ -10201,13 +10201,13 @@
         <v>3133</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D31" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G31">
         <v>40</v>
@@ -10221,13 +10221,13 @@
         <v>3134</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D32" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G32">
         <v>60</v>
@@ -10244,7 +10244,7 @@
         <v>5.56</v>
       </c>
       <c r="D33" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33">
@@ -10262,7 +10262,7 @@
         <v>5.56</v>
       </c>
       <c r="D34" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34">
@@ -10277,10 +10277,10 @@
         <v>3137</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35">
@@ -10295,10 +10295,10 @@
         <v>3138</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D36" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36">
@@ -10316,7 +10316,7 @@
         <v>5.56</v>
       </c>
       <c r="D37" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37">
@@ -10331,7 +10331,7 @@
         <v>5.56</v>
       </c>
       <c r="D38" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G38">
         <v>100</v>
@@ -10345,13 +10345,13 @@
         <v>3201</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D40" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F40" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -10365,13 +10365,13 @@
         <v>3202</v>
       </c>
       <c r="C41" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D41" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F41" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -10422,7 +10422,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10433,13 +10433,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -10453,19 +10453,19 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>534</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="I4" t="s">
         <v>535</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="I4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -10474,16 +10474,16 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E5" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I5" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -10492,16 +10492,16 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -10510,16 +10510,16 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
+        <v>538</v>
+      </c>
+      <c r="E7" t="s">
+        <v>540</v>
+      </c>
+      <c r="F7" t="s">
+        <v>503</v>
+      </c>
+      <c r="I7" t="s">
         <v>539</v>
-      </c>
-      <c r="E7" t="s">
-        <v>541</v>
-      </c>
-      <c r="F7" t="s">
-        <v>504</v>
-      </c>
-      <c r="I7" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -10528,16 +10528,16 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
+        <v>542</v>
+      </c>
+      <c r="E8" t="s">
+        <v>537</v>
+      </c>
+      <c r="F8" t="s">
+        <v>504</v>
+      </c>
+      <c r="I8" t="s">
         <v>543</v>
-      </c>
-      <c r="E8" t="s">
-        <v>538</v>
-      </c>
-      <c r="F8" t="s">
-        <v>505</v>
-      </c>
-      <c r="I8" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -10546,19 +10546,19 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -10567,16 +10567,16 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E10" t="s">
+        <v>573</v>
+      </c>
+      <c r="F10" t="s">
+        <v>501</v>
+      </c>
+      <c r="I10" t="s">
         <v>574</v>
-      </c>
-      <c r="F10" t="s">
-        <v>502</v>
-      </c>
-      <c r="I10" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -10585,16 +10585,16 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="E11" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I11" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -10603,16 +10603,16 @@
         <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="E12" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F12" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I12" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -10621,39 +10621,39 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
+        <v>567</v>
+      </c>
+      <c r="E13" t="s">
         <v>568</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>504</v>
+      </c>
+      <c r="I13" t="s">
         <v>569</v>
-      </c>
-      <c r="F13" t="s">
-        <v>505</v>
-      </c>
-      <c r="I13" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C15">
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -10662,19 +10662,19 @@
         <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E16" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F16" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -10683,19 +10683,19 @@
         <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F17" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -10704,19 +10704,19 @@
         <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E18" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F18" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -10725,19 +10725,19 @@
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="E19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F19" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -10746,19 +10746,19 @@
         <v>116</v>
       </c>
       <c r="D20" t="s">
+        <v>589</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>505</v>
+      </c>
+      <c r="I20" t="s">
         <v>590</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>585</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="I20" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -10767,19 +10767,19 @@
         <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E21" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -10788,19 +10788,19 @@
         <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="E22" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F22" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G22">
         <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -10809,19 +10809,19 @@
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E23" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F23" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -10830,24 +10830,24 @@
         <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E24" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F24" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G24">
         <v>100</v>
       </c>
       <c r="I24" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C26">
         <v>121</v>
@@ -10879,7 +10879,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C32">
         <v>131</v>
@@ -10891,10 +10891,10 @@
         <v>132</v>
       </c>
       <c r="D33" t="s">
+        <v>551</v>
+      </c>
+      <c r="I33" t="s">
         <v>552</v>
-      </c>
-      <c r="I33" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -10912,10 +10912,10 @@
         <v>134</v>
       </c>
       <c r="D35" t="s">
+        <v>554</v>
+      </c>
+      <c r="I35" t="s">
         <v>555</v>
-      </c>
-      <c r="I35" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.4a: Can view levels
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54C25D3A-4973-4B3D-A568-9EA9A329301C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCDACB-62D0-4013-BDFA-1C58BCFBEA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="6" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -16250,7 +16250,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.4g: Can add linkers, fixed some feature images
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACCDACB-62D0-4013-BDFA-1C58BCFBEA9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C53545-765D-4B5D-A90E-0B8920A40AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="6" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1101" uniqueCount="837">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="838">
   <si>
     <t>ID</t>
   </si>
@@ -2557,6 +2557,9 @@
   </si>
   <si>
     <t>max frame</t>
+  </si>
+  <si>
+    <t>Tree, pine</t>
   </si>
 </sst>
 </file>
@@ -10018,10 +10021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G98" sqref="G98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11216,118 +11219,129 @@
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="4">
+        <v>426</v>
+      </c>
+      <c r="C100" t="s">
+        <v>837</v>
+      </c>
+      <c r="E100">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="4">
         <v>431</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C101" t="s">
         <v>251</v>
       </c>
-      <c r="E100">
+      <c r="E101">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="3">
+    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="3">
         <v>441</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C102" t="s">
         <v>252</v>
       </c>
-      <c r="E101">
+      <c r="E102">
         <v>5</v>
       </c>
-      <c r="G101" t="s">
+      <c r="G102" t="s">
         <v>341</v>
       </c>
-      <c r="H101" t="s">
+      <c r="H102" t="s">
         <v>808</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="4">
-        <v>442</v>
-      </c>
-      <c r="H102" t="s">
-        <v>809</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="4">
+        <v>442</v>
+      </c>
+      <c r="H103" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="4">
         <v>443</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H104" t="s">
         <v>810</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B105" s="4">
-        <v>501</v>
-      </c>
-      <c r="C105" t="s">
-        <v>256</v>
-      </c>
-      <c r="D105" t="s">
-        <v>255</v>
-      </c>
-      <c r="E105">
-        <v>5</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="4">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C106" t="s">
-        <v>257</v>
+        <v>256</v>
+      </c>
+      <c r="D106" t="s">
+        <v>255</v>
+      </c>
+      <c r="E106">
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="4">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C107" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="4">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C108" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="4">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C109" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="4">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C110" t="s">
-        <v>261</v>
-      </c>
-      <c r="E110">
-        <v>9</v>
+        <v>260</v>
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="4">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C111" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="E111">
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="4">
+        <v>512</v>
+      </c>
+      <c r="C112" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="4">
         <v>513</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C113" t="s">
         <v>263</v>
       </c>
     </row>
@@ -16249,7 +16263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64CBCF6E-AD46-4C01-9700-4E08CEE8B938}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v0.6.4q: Updated Item constructor, getImage()
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B99E38-8216-46B3-B860-1709BD4F3950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE497A5C-F8F2-43D8-848C-90EE269729B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -3156,13 +3156,13 @@
     <t>Corundum Chunk</t>
   </si>
   <si>
-    <t>Ruby</t>
-  </si>
-  <si>
     <t>Selenite Crystal</t>
   </si>
   <si>
     <t>Topaz Gem</t>
+  </si>
+  <si>
+    <t>Sapphire</t>
   </si>
 </sst>
 </file>
@@ -13081,7 +13081,7 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D147" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C171" sqref="C171"/>
+      <selection pane="bottomRight" activeCell="C174" sqref="C174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15457,7 +15457,7 @@
         <v>2814</v>
       </c>
       <c r="C150" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
@@ -15638,7 +15638,7 @@
         <v>2873</v>
       </c>
       <c r="C170" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
@@ -15665,7 +15665,7 @@
         <v>2883</v>
       </c>
       <c r="C173" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.5i: Untested shoot/projectile logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40685795-ECA7-4BED-BA5C-B0E7BC847F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF4A62-50CD-4823-B718-D1490258510C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="9" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="5" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -4288,8 +4288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A114E18-4580-4CF1-BE70-B14A03AAF800}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13099,10 +13099,10 @@
   <dimension ref="A1:Y227"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C90" sqref="C90"/>
+      <selection pane="bottomRight" activeCell="W38" sqref="W38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16517,8 +16517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAF6DD-D8FA-4653-B50E-0B687056C45B}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16680,7 +16680,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>3111</v>
+        <v>3312</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
v0.6.5m: Projectile decay, can drop items
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9380534-0BC6-42B6-BADD-AFC8CC2D5CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A37C8-CABC-4BF1-90C0-83A1CD9491BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="891">
   <si>
     <t>ID</t>
   </si>
@@ -3169,6 +3169,9 @@
   </si>
   <si>
     <t>(level)</t>
+  </si>
+  <si>
+    <t>dur=60, cd=300, rec=0, inac=0.1</t>
   </si>
 </sst>
 </file>
@@ -10818,8 +10821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G95" sqref="G95"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E90" sqref="E90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13098,11 +13101,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y227"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W38" sqref="W38"/>
+      <selection pane="bottomRight" activeCell="W196" sqref="W196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15996,6 +15999,9 @@
       <c r="N194">
         <v>2.5</v>
       </c>
+      <c r="W194" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B195">
@@ -16032,6 +16038,9 @@
       </c>
       <c r="N196">
         <v>2</v>
+      </c>
+      <c r="W196" t="s">
+        <v>890</v>
       </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
@@ -16518,7 +16527,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.5r: Ability class outline
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EB40FA-63C2-4849-9798-98813DB54C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A3702-DF2A-4B30-8E0B-7BAE5030898E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="5" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="8" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="890">
   <si>
     <t>ID</t>
   </si>
@@ -3166,6 +3166,9 @@
   </si>
   <si>
     <t>dur=300, cd=1500, rec=0, inac=0.12</t>
+  </si>
+  <si>
+    <t>100s</t>
   </si>
 </sst>
 </file>
@@ -16520,8 +16523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAF6DD-D8FA-4653-B50E-0B687056C45B}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17324,8 +17327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E132C5F-9A98-41A1-A3AA-2A3458C20EAF}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17397,6 +17400,9 @@
       <c r="F5" t="s">
         <v>488</v>
       </c>
+      <c r="G5">
+        <v>25</v>
+      </c>
       <c r="I5" t="s">
         <v>543</v>
       </c>
@@ -17415,6 +17421,9 @@
       <c r="F6" t="s">
         <v>489</v>
       </c>
+      <c r="G6" s="3">
+        <v>-8</v>
+      </c>
       <c r="I6" t="s">
         <v>562</v>
       </c>
@@ -17433,6 +17442,9 @@
       <c r="F7" t="s">
         <v>490</v>
       </c>
+      <c r="G7" s="3">
+        <v>-8</v>
+      </c>
       <c r="I7" t="s">
         <v>526</v>
       </c>
@@ -17451,6 +17463,9 @@
       <c r="F8" t="s">
         <v>491</v>
       </c>
+      <c r="G8" s="9">
+        <v>-40</v>
+      </c>
       <c r="I8" t="s">
         <v>530</v>
       </c>
@@ -17490,6 +17505,9 @@
       <c r="F10" t="s">
         <v>488</v>
       </c>
+      <c r="G10">
+        <v>25</v>
+      </c>
       <c r="I10" t="s">
         <v>561</v>
       </c>
@@ -17508,6 +17526,9 @@
       <c r="F11" t="s">
         <v>489</v>
       </c>
+      <c r="G11">
+        <v>-15</v>
+      </c>
       <c r="I11" t="s">
         <v>563</v>
       </c>
@@ -17526,6 +17547,9 @@
       <c r="F12" t="s">
         <v>490</v>
       </c>
+      <c r="G12">
+        <v>-15</v>
+      </c>
       <c r="I12" t="s">
         <v>557</v>
       </c>
@@ -17539,10 +17563,13 @@
         <v>554</v>
       </c>
       <c r="E13" t="s">
-        <v>555</v>
+        <v>889</v>
       </c>
       <c r="F13" t="s">
         <v>491</v>
+      </c>
+      <c r="G13">
+        <v>-60</v>
       </c>
       <c r="I13" t="s">
         <v>556</v>

</xml_diff>

<commit_message>
v0.6.5s: StatusEffect class outline
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721A3702-DF2A-4B30-8E0B-7BAE5030898E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BDDB97-4A99-477C-B0C4-12DAEB06BC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="8" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -12681,8 +12681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A228F-2BB3-44AC-82E9-D9BE084DFD89}">
   <dimension ref="B2:F34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17327,8 +17327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E132C5F-9A98-41A1-A3AA-2A3458C20EAF}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.5v: Finished base StatusEffect logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F82D6B7-2DA1-482D-8120-1CFFAD31E784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0985A86-FC05-4CDF-BF63-5F86AA271A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -1406,9 +1406,6 @@
   </si>
   <si>
     <t>timer=1600, number=0.02, damageLimit = 0.1</t>
-  </si>
-  <si>
-    <t>timer=1000, number=0.02</t>
   </si>
   <si>
     <t>maxHealth DoT, lethal vs blue, gives decay</t>
@@ -3166,6 +3163,9 @@
   </si>
   <si>
     <t>timer=10s</t>
+  </si>
+  <si>
+    <t>timer=1000, number=0.025</t>
   </si>
 </sst>
 </file>
@@ -3609,7 +3609,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -3621,10 +3621,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3635,7 +3635,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3646,7 +3646,7 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D6" t="s">
         <v>205</v>
@@ -3660,7 +3660,7 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3668,7 +3668,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3676,7 +3676,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
         <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,7 +3692,7 @@
         <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3700,7 +3700,7 @@
         <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3708,7 +3708,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3716,7 +3716,7 @@
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3740,7 +3740,7 @@
         <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3748,7 +3748,7 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3756,7 +3756,7 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3764,7 +3764,7 @@
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3772,7 +3772,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3780,7 +3780,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3788,7 +3788,7 @@
         <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3796,7 +3796,7 @@
         <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3804,7 +3804,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3812,7 +3812,7 @@
         <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3820,7 +3820,7 @@
         <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3828,7 +3828,7 @@
         <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3836,7 +3836,7 @@
         <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3844,7 +3844,7 @@
         <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3852,7 +3852,7 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3860,7 +3860,7 @@
         <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -3868,7 +3868,7 @@
         <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -3876,7 +3876,7 @@
         <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -3884,7 +3884,7 @@
         <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -3892,7 +3892,7 @@
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -3900,7 +3900,7 @@
         <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -3908,7 +3908,7 @@
         <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -3916,7 +3916,7 @@
         <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -3924,7 +3924,7 @@
         <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -3932,7 +3932,7 @@
         <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -3940,7 +3940,7 @@
         <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -3948,7 +3948,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -3964,7 +3964,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -3972,7 +3972,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -3980,7 +3980,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -3988,7 +3988,7 @@
         <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D49" t="s">
         <v>208</v>
@@ -4002,7 +4002,7 @@
         <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -4010,7 +4010,7 @@
         <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -4018,7 +4018,7 @@
         <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -4026,7 +4026,7 @@
         <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -4034,7 +4034,7 @@
         <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -4042,7 +4042,7 @@
         <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
         <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -4058,7 +4058,7 @@
         <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
         <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -4077,13 +4077,13 @@
         <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D60" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E60" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -4091,7 +4091,7 @@
         <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -4099,7 +4099,7 @@
         <v>303</v>
       </c>
       <c r="C62" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -4107,7 +4107,7 @@
         <v>304</v>
       </c>
       <c r="C63" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -4115,7 +4115,7 @@
         <v>305</v>
       </c>
       <c r="C64" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -4123,7 +4123,7 @@
         <v>306</v>
       </c>
       <c r="C65" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>307</v>
       </c>
       <c r="C66" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -4139,7 +4139,7 @@
         <v>308</v>
       </c>
       <c r="C67" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -4147,7 +4147,7 @@
         <v>309</v>
       </c>
       <c r="C68" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -4155,7 +4155,7 @@
         <v>310</v>
       </c>
       <c r="C69" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -4163,7 +4163,7 @@
         <v>311</v>
       </c>
       <c r="C70" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -4171,7 +4171,7 @@
         <v>312</v>
       </c>
       <c r="C71" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>313</v>
       </c>
       <c r="C72" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -4187,7 +4187,7 @@
         <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -4195,7 +4195,7 @@
         <v>315</v>
       </c>
       <c r="C74" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -4203,7 +4203,7 @@
         <v>316</v>
       </c>
       <c r="C75" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
@@ -4211,7 +4211,7 @@
         <v>317</v>
       </c>
       <c r="C76" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -4219,7 +4219,7 @@
         <v>318</v>
       </c>
       <c r="C77" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -4227,7 +4227,7 @@
         <v>319</v>
       </c>
       <c r="C78" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
@@ -4235,7 +4235,7 @@
         <v>320</v>
       </c>
       <c r="C79" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -4243,7 +4243,7 @@
         <v>321</v>
       </c>
       <c r="C80" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -4251,7 +4251,7 @@
         <v>322</v>
       </c>
       <c r="C81" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
@@ -4259,7 +4259,7 @@
         <v>323</v>
       </c>
       <c r="C82" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -4267,7 +4267,7 @@
         <v>324</v>
       </c>
       <c r="C83" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
@@ -4353,7 +4353,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I4" s="1">
         <v>1.4</v>
@@ -4420,7 +4420,7 @@
         <v>2.5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
@@ -10153,7 +10153,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10164,393 +10164,393 @@
         <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D4" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="14"/>
       <c r="C5" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="14"/>
       <c r="C6" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D6" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="14"/>
       <c r="C7" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D7" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="14"/>
       <c r="C8" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
       <c r="C9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="14"/>
       <c r="C10" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D10" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="14"/>
       <c r="C11" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D12" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="14"/>
       <c r="C13" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="G13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C15" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="14"/>
       <c r="C16" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D16" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="14"/>
       <c r="C17" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
       <c r="C18" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" t="s">
+        <v>629</v>
+      </c>
+      <c r="D19" t="s">
         <v>630</v>
-      </c>
-      <c r="D19" t="s">
-        <v>631</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
       <c r="C20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D20" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G20" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" t="s">
+        <v>621</v>
+      </c>
+      <c r="D21" t="s">
         <v>622</v>
-      </c>
-      <c r="D21" t="s">
-        <v>623</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G21" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D24" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="D31" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>802</v>
+      </c>
+      <c r="G32" t="s">
         <v>803</v>
-      </c>
-      <c r="G32" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
   </sheetData>
@@ -10688,10 +10688,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>210</v>
@@ -10702,13 +10702,13 @@
         <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D3" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E3" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10716,13 +10716,13 @@
         <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D4" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E4" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10730,13 +10730,13 @@
         <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10744,7 +10744,7 @@
         <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.35">
@@ -10752,7 +10752,7 @@
         <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E7" s="16"/>
     </row>
@@ -10761,7 +10761,7 @@
         <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10769,10 +10769,10 @@
         <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="E9" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.35">
@@ -10780,10 +10780,10 @@
         <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E10" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10791,10 +10791,10 @@
         <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E11" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -10802,7 +10802,7 @@
         <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
   </sheetData>
@@ -10831,7 +10831,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -10846,7 +10846,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>209</v>
@@ -10869,10 +10869,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H4" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -10883,13 +10883,13 @@
         <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -10903,7 +10903,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -10920,7 +10920,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -10942,7 +10942,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>219</v>
@@ -10951,10 +10951,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H11" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -10972,7 +10972,7 @@
         <v>228</v>
       </c>
       <c r="H12" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -10983,7 +10983,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -10991,16 +10991,16 @@
         <v>111</v>
       </c>
       <c r="C14" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H14" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -11008,7 +11008,7 @@
         <v>112</v>
       </c>
       <c r="H15" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -11016,7 +11016,7 @@
         <v>113</v>
       </c>
       <c r="H16" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -11024,7 +11024,7 @@
         <v>114</v>
       </c>
       <c r="H17" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -11032,7 +11032,7 @@
         <v>115</v>
       </c>
       <c r="C18" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G18" t="s">
         <v>329</v>
@@ -11052,7 +11052,7 @@
         <v>329</v>
       </c>
       <c r="H19" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -11060,7 +11060,7 @@
         <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -11068,7 +11068,7 @@
         <v>123</v>
       </c>
       <c r="H21" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -11076,7 +11076,7 @@
         <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -11084,16 +11084,16 @@
         <v>125</v>
       </c>
       <c r="C23" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="H23" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -11101,7 +11101,7 @@
         <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -11112,7 +11112,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -11123,7 +11123,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -11140,7 +11140,7 @@
         <v>329</v>
       </c>
       <c r="H27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -11148,7 +11148,7 @@
         <v>132</v>
       </c>
       <c r="H28" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -11156,7 +11156,7 @@
         <v>133</v>
       </c>
       <c r="H29" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -11164,7 +11164,7 @@
         <v>134</v>
       </c>
       <c r="H30" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -11181,7 +11181,7 @@
         <v>329</v>
       </c>
       <c r="H31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -11189,7 +11189,7 @@
         <v>142</v>
       </c>
       <c r="H32" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -11197,7 +11197,7 @@
         <v>151</v>
       </c>
       <c r="C33" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D33" t="s">
         <v>221</v>
@@ -11206,10 +11206,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="H33" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -11217,7 +11217,7 @@
         <v>152</v>
       </c>
       <c r="H34" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -11225,7 +11225,7 @@
         <v>153</v>
       </c>
       <c r="H35" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -11233,7 +11233,7 @@
         <v>154</v>
       </c>
       <c r="H36" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -11241,10 +11241,10 @@
         <v>155</v>
       </c>
       <c r="C37" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="H37" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -11252,7 +11252,7 @@
         <v>156</v>
       </c>
       <c r="H38" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -11260,7 +11260,7 @@
         <v>157</v>
       </c>
       <c r="H39" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -11268,7 +11268,7 @@
         <v>158</v>
       </c>
       <c r="H40" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -11349,7 +11349,7 @@
         <v>227</v>
       </c>
       <c r="D46" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -11372,7 +11372,7 @@
         <v>332</v>
       </c>
       <c r="H47" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -11386,7 +11386,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -11408,7 +11408,7 @@
         <v>175</v>
       </c>
       <c r="C50" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -11515,7 +11515,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -11523,16 +11523,16 @@
         <v>191</v>
       </c>
       <c r="C58" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H58" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -11540,7 +11540,7 @@
         <v>192</v>
       </c>
       <c r="H59" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -11548,10 +11548,10 @@
         <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H60" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -11559,7 +11559,7 @@
         <v>194</v>
       </c>
       <c r="H61" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -11570,13 +11570,13 @@
         <v>213</v>
       </c>
       <c r="D62" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="E62">
         <v>100</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -11593,27 +11593,27 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C64" t="s">
         <v>239</v>
       </c>
       <c r="D64" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="G64" s="9" t="s">
+        <v>780</v>
+      </c>
+      <c r="H64" t="s">
         <v>781</v>
-      </c>
-      <c r="H64" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C65" t="s">
         <v>238</v>
@@ -11622,10 +11622,10 @@
         <v>9</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H65" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -11636,16 +11636,16 @@
         <v>243</v>
       </c>
       <c r="D66" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H66" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -11654,12 +11654,12 @@
       </c>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C69" t="s">
         <v>207</v>
@@ -11671,10 +11671,10 @@
         <v>100</v>
       </c>
       <c r="G69" t="s">
+        <v>741</v>
+      </c>
+      <c r="H69" t="s">
         <v>742</v>
-      </c>
-      <c r="H69" t="s">
-        <v>743</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -11685,10 +11685,10 @@
         <v>212</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H70" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -11696,7 +11696,7 @@
         <v>312</v>
       </c>
       <c r="H71" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -11704,19 +11704,19 @@
         <v>321</v>
       </c>
       <c r="C72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="H72" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -11727,10 +11727,10 @@
         <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H73" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -11738,10 +11738,10 @@
         <v>323</v>
       </c>
       <c r="G74" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="H74" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -11753,16 +11753,16 @@
         <v>211</v>
       </c>
       <c r="D75" t="s">
+        <v>761</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>748</v>
+      </c>
+      <c r="H75" t="s">
         <v>762</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75" t="s">
-        <v>749</v>
-      </c>
-      <c r="H75" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -11771,7 +11771,7 @@
         <v>332</v>
       </c>
       <c r="H76" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -11780,7 +11780,7 @@
         <v>333</v>
       </c>
       <c r="H77" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -11789,7 +11789,7 @@
         <v>334</v>
       </c>
       <c r="H78" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -11798,7 +11798,7 @@
         <v>335</v>
       </c>
       <c r="H79" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -11807,7 +11807,7 @@
         <v>336</v>
       </c>
       <c r="H80" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -11816,7 +11816,7 @@
         <v>337</v>
       </c>
       <c r="H81" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -11825,7 +11825,7 @@
         <v>338</v>
       </c>
       <c r="H82" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -11834,16 +11834,16 @@
         <v>339</v>
       </c>
       <c r="C83" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="E83">
         <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="H83" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -11852,7 +11852,7 @@
         <v>340</v>
       </c>
       <c r="H84" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -11861,7 +11861,7 @@
         <v>341</v>
       </c>
       <c r="H85" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -11870,7 +11870,7 @@
         <v>342</v>
       </c>
       <c r="H86" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -11879,13 +11879,13 @@
         <v>343</v>
       </c>
       <c r="C87" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G87" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="H87" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -11894,7 +11894,7 @@
         <v>344</v>
       </c>
       <c r="H88" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -11903,7 +11903,7 @@
         <v>345</v>
       </c>
       <c r="H89" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -11912,7 +11912,7 @@
         <v>346</v>
       </c>
       <c r="H90" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -11937,7 +11937,7 @@
         <v>411</v>
       </c>
       <c r="C93" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -11946,7 +11946,7 @@
         <v>292</v>
       </c>
       <c r="H93" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -11957,7 +11957,7 @@
         <v>293</v>
       </c>
       <c r="H94" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -11965,7 +11965,7 @@
         <v>421</v>
       </c>
       <c r="C95" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="E95">
         <v>20</v>
@@ -11979,7 +11979,7 @@
         <v>422</v>
       </c>
       <c r="C96" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -11987,7 +11987,7 @@
         <v>423</v>
       </c>
       <c r="C97" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -11995,7 +11995,7 @@
         <v>424</v>
       </c>
       <c r="C98" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -12003,7 +12003,7 @@
         <v>425</v>
       </c>
       <c r="C99" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E99">
         <v>35</v>
@@ -12014,7 +12014,7 @@
         <v>426</v>
       </c>
       <c r="C100" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E100">
         <v>20</v>
@@ -12045,7 +12045,7 @@
         <v>331</v>
       </c>
       <c r="H102" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -12053,7 +12053,7 @@
         <v>442</v>
       </c>
       <c r="H103" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
@@ -12061,7 +12061,7 @@
         <v>443</v>
       </c>
       <c r="H104" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
@@ -12230,10 +12230,10 @@
         <v>1002</v>
       </c>
       <c r="C4" t="s">
+        <v>796</v>
+      </c>
+      <c r="D4" t="s">
         <v>797</v>
-      </c>
-      <c r="D4" t="s">
-        <v>798</v>
       </c>
       <c r="E4" t="s">
         <v>402</v>
@@ -12250,7 +12250,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -12279,10 +12279,10 @@
         <v>1102</v>
       </c>
       <c r="C7" t="s">
+        <v>460</v>
+      </c>
+      <c r="E7" t="s">
         <v>461</v>
-      </c>
-      <c r="E7" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -12290,10 +12290,10 @@
         <v>1103</v>
       </c>
       <c r="C8" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -12301,10 +12301,10 @@
         <v>1104</v>
       </c>
       <c r="C9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -12312,10 +12312,10 @@
         <v>1105</v>
       </c>
       <c r="C10" t="s">
+        <v>798</v>
+      </c>
+      <c r="E10" t="s">
         <v>799</v>
-      </c>
-      <c r="E10" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -12323,10 +12323,10 @@
         <v>1106</v>
       </c>
       <c r="C11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -12334,10 +12334,10 @@
         <v>1116</v>
       </c>
       <c r="C12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E12" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -12345,10 +12345,10 @@
         <v>1117</v>
       </c>
       <c r="C13" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E13" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -12356,10 +12356,10 @@
         <v>1118</v>
       </c>
       <c r="C14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -12367,10 +12367,10 @@
         <v>1119</v>
       </c>
       <c r="C15" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -12378,10 +12378,10 @@
         <v>1120</v>
       </c>
       <c r="C16" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E16" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -12679,7 +12679,7 @@
   <dimension ref="B2:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12713,7 +12713,7 @@
         <v>429</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>433</v>
@@ -12724,7 +12724,7 @@
         <v>430</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>431</v>
@@ -12748,7 +12748,7 @@
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E6" t="s">
         <v>404</v>
@@ -12759,7 +12759,7 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
@@ -12776,7 +12776,7 @@
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E8" t="s">
         <v>405</v>
@@ -12787,10 +12787,10 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E9" t="s">
         <v>411</v>
@@ -12801,10 +12801,10 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D10" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E10" t="s">
         <v>412</v>
@@ -12815,10 +12815,10 @@
         <v>418</v>
       </c>
       <c r="C12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D12" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E12" t="s">
         <v>407</v>
@@ -12829,7 +12829,7 @@
         <v>417</v>
       </c>
       <c r="C13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D13" t="s">
         <v>410</v>
@@ -12843,7 +12843,7 @@
         <v>419</v>
       </c>
       <c r="C14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D14" t="s">
         <v>441</v>
@@ -12857,7 +12857,7 @@
         <v>420</v>
       </c>
       <c r="C15" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D15" t="s">
         <v>442</v>
@@ -12871,7 +12871,7 @@
         <v>413</v>
       </c>
       <c r="C16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D16" t="s">
         <v>445</v>
@@ -12880,7 +12880,7 @@
         <v>443</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -12888,7 +12888,7 @@
         <v>414</v>
       </c>
       <c r="C17" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D17" t="s">
         <v>409</v>
@@ -12903,13 +12903,13 @@
         <v>421</v>
       </c>
       <c r="C18" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D18" t="s">
         <v>445</v>
       </c>
       <c r="E18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F18" s="12"/>
     </row>
@@ -12918,13 +12918,13 @@
         <v>422</v>
       </c>
       <c r="C19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D19" t="s">
         <v>446</v>
       </c>
       <c r="E19" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F19" s="12"/>
     </row>
@@ -12933,13 +12933,13 @@
         <v>423</v>
       </c>
       <c r="C20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D20" t="s">
         <v>447</v>
       </c>
       <c r="E20" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -12947,7 +12947,7 @@
         <v>424</v>
       </c>
       <c r="C21" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D21" t="s">
         <v>452</v>
@@ -12961,7 +12961,7 @@
         <v>194</v>
       </c>
       <c r="C22" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D22" t="s">
         <v>196</v>
@@ -12975,7 +12975,7 @@
         <v>425</v>
       </c>
       <c r="C23" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D23" t="s">
         <v>448</v>
@@ -12989,13 +12989,13 @@
         <v>426</v>
       </c>
       <c r="C24" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -13003,13 +13003,13 @@
         <v>427</v>
       </c>
       <c r="C25" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D25" t="s">
-        <v>453</v>
+        <v>888</v>
       </c>
       <c r="E25" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -13017,7 +13017,7 @@
         <v>428</v>
       </c>
       <c r="C26" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -13025,7 +13025,7 @@
         <v>434</v>
       </c>
       <c r="C27" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -13033,7 +13033,7 @@
         <v>435</v>
       </c>
       <c r="C28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -13041,7 +13041,7 @@
         <v>436</v>
       </c>
       <c r="C29" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -13049,7 +13049,7 @@
         <v>437</v>
       </c>
       <c r="C30" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -13057,29 +13057,29 @@
         <v>438</v>
       </c>
       <c r="C31" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E33" t="s">
+        <v>513</v>
+      </c>
+      <c r="F33" t="s">
         <v>514</v>
-      </c>
-      <c r="F33" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>538</v>
+      </c>
+      <c r="C34" t="s">
         <v>539</v>
-      </c>
-      <c r="C34" t="s">
-        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -13742,7 +13742,7 @@
         <v>1</v>
       </c>
       <c r="W42" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
@@ -13750,7 +13750,7 @@
         <v>2311</v>
       </c>
       <c r="C43" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -13768,7 +13768,7 @@
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
@@ -14753,7 +14753,7 @@
         <v>2501</v>
       </c>
       <c r="C89" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D89" t="s">
         <v>24</v>
@@ -14803,7 +14803,7 @@
         <v>2511</v>
       </c>
       <c r="C93" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E93">
         <v>2</v>
@@ -14848,7 +14848,7 @@
         <v>2521</v>
       </c>
       <c r="C96" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -14862,7 +14862,7 @@
         <v>2531</v>
       </c>
       <c r="C97" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E97">
         <v>4</v>
@@ -14876,7 +14876,7 @@
         <v>2541</v>
       </c>
       <c r="C98" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E98">
         <v>5</v>
@@ -14890,7 +14890,7 @@
         <v>2551</v>
       </c>
       <c r="C99" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E99">
         <v>6</v>
@@ -14904,7 +14904,7 @@
         <v>2561</v>
       </c>
       <c r="C100" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E100">
         <v>7</v>
@@ -14918,7 +14918,7 @@
         <v>2571</v>
       </c>
       <c r="C101" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="E101">
         <v>8</v>
@@ -14932,7 +14932,7 @@
         <v>2581</v>
       </c>
       <c r="C102" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E102">
         <v>9</v>
@@ -14946,7 +14946,7 @@
         <v>2591</v>
       </c>
       <c r="C103" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="E103">
         <v>10</v>
@@ -15052,7 +15052,7 @@
         <v>2641</v>
       </c>
       <c r="C112" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E112">
         <v>5</v>
@@ -15377,7 +15377,7 @@
         <v>2801</v>
       </c>
       <c r="C137" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D137" t="s">
         <v>27</v>
@@ -15388,7 +15388,7 @@
         <v>2802</v>
       </c>
       <c r="C138" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="139" spans="2:15" x14ac:dyDescent="0.25">
@@ -15396,7 +15396,7 @@
         <v>2803</v>
       </c>
       <c r="C139" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="140" spans="2:15" x14ac:dyDescent="0.25">
@@ -15404,7 +15404,7 @@
         <v>2804</v>
       </c>
       <c r="C140" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
     </row>
     <row r="141" spans="2:15" x14ac:dyDescent="0.25">
@@ -15412,7 +15412,7 @@
         <v>2805</v>
       </c>
       <c r="C141" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
@@ -15448,7 +15448,7 @@
         <v>2811</v>
       </c>
       <c r="C147" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="E147">
         <v>2</v>
@@ -15459,7 +15459,7 @@
         <v>2812</v>
       </c>
       <c r="C148" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="149" spans="2:25" x14ac:dyDescent="0.25">
@@ -15467,7 +15467,7 @@
         <v>2813</v>
       </c>
       <c r="C149" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="150" spans="2:25" x14ac:dyDescent="0.25">
@@ -15475,7 +15475,7 @@
         <v>2814</v>
       </c>
       <c r="C150" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
@@ -15491,7 +15491,7 @@
         <v>2821</v>
       </c>
       <c r="C152" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="E152">
         <v>3</v>
@@ -15502,7 +15502,7 @@
         <v>2822</v>
       </c>
       <c r="C153" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="154" spans="2:25" x14ac:dyDescent="0.25">
@@ -15510,7 +15510,7 @@
         <v>2823</v>
       </c>
       <c r="C154" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="155" spans="2:25" x14ac:dyDescent="0.25">
@@ -15518,7 +15518,7 @@
         <v>2834</v>
       </c>
       <c r="C155" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="156" spans="2:25" x14ac:dyDescent="0.25">
@@ -15526,7 +15526,7 @@
         <v>2825</v>
       </c>
       <c r="C156" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="Y156" t="s">
         <v>202</v>
@@ -15537,7 +15537,7 @@
         <v>2831</v>
       </c>
       <c r="C157" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="E157">
         <v>4</v>
@@ -15548,7 +15548,7 @@
         <v>2832</v>
       </c>
       <c r="C158" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="159" spans="2:25" x14ac:dyDescent="0.25">
@@ -15556,7 +15556,7 @@
         <v>2841</v>
       </c>
       <c r="C159" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E159">
         <v>5</v>
@@ -15567,7 +15567,7 @@
         <v>2842</v>
       </c>
       <c r="C160" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
@@ -15575,7 +15575,7 @@
         <v>2851</v>
       </c>
       <c r="C161" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E161">
         <v>6</v>
@@ -15586,7 +15586,7 @@
         <v>2852</v>
       </c>
       <c r="C162" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
@@ -15594,7 +15594,7 @@
         <v>2853</v>
       </c>
       <c r="C163" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
@@ -15602,7 +15602,7 @@
         <v>2861</v>
       </c>
       <c r="C164" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="E164">
         <v>7</v>
@@ -15613,7 +15613,7 @@
         <v>2862</v>
       </c>
       <c r="C165" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
@@ -15621,7 +15621,7 @@
         <v>2863</v>
       </c>
       <c r="C166" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
@@ -15637,7 +15637,7 @@
         <v>2871</v>
       </c>
       <c r="C168" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="E168">
         <v>8</v>
@@ -15648,7 +15648,7 @@
         <v>2872</v>
       </c>
       <c r="C169" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
@@ -15656,7 +15656,7 @@
         <v>2873</v>
       </c>
       <c r="C170" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
@@ -15664,7 +15664,7 @@
         <v>2881</v>
       </c>
       <c r="C171" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="E171">
         <v>9</v>
@@ -15675,7 +15675,7 @@
         <v>2882</v>
       </c>
       <c r="C172" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="173" spans="2:5" x14ac:dyDescent="0.25">
@@ -15683,7 +15683,7 @@
         <v>2883</v>
       </c>
       <c r="C173" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">
@@ -15691,7 +15691,7 @@
         <v>2891</v>
       </c>
       <c r="C174" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="E174">
         <v>10</v>
@@ -15834,7 +15834,7 @@
         <v>2917</v>
       </c>
       <c r="C186" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D186" t="s">
         <v>259</v>
@@ -15994,7 +15994,7 @@
         <v>2.5</v>
       </c>
       <c r="W194" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
@@ -16034,7 +16034,7 @@
         <v>2</v>
       </c>
       <c r="W196" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
@@ -16609,7 +16609,7 @@
         <v>3103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D5" t="s">
         <v>281</v>
@@ -17061,7 +17061,7 @@
         <v>382</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G31">
         <v>40</v>
@@ -17081,7 +17081,7 @@
         <v>382</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="G32">
         <v>60</v>
@@ -17199,13 +17199,13 @@
         <v>3201</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D40" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -17219,13 +17219,13 @@
         <v>3202</v>
       </c>
       <c r="C41" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F41" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -17258,7 +17258,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17269,13 +17269,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>814</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>815</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -17283,10 +17283,10 @@
         <v>4001</v>
       </c>
       <c r="C3" t="s">
+        <v>815</v>
+      </c>
+      <c r="E3" t="s">
         <v>816</v>
-      </c>
-      <c r="E3" t="s">
-        <v>817</v>
       </c>
       <c r="F3">
         <v>35</v>
@@ -17337,7 +17337,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17348,13 +17348,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -17368,19 +17368,19 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>515</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="I4" t="s">
         <v>516</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="I4" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -17389,19 +17389,19 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G5">
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -17410,19 +17410,19 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G6" s="3">
         <v>-8</v>
       </c>
       <c r="I6" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -17431,19 +17431,19 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E7" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G7" s="3">
         <v>-8</v>
       </c>
       <c r="I7" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -17452,19 +17452,19 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F8" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G8" s="9">
         <v>-40</v>
       </c>
       <c r="I8" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -17473,19 +17473,19 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -17494,19 +17494,19 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E10" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G10">
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -17515,19 +17515,19 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E11" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G11">
         <v>-15</v>
       </c>
       <c r="I11" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -17536,19 +17536,19 @@
         <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G12">
         <v>-15</v>
       </c>
       <c r="I12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -17557,42 +17557,42 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="E13" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G13">
         <v>-60</v>
       </c>
       <c r="I13" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C15">
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I15" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -17601,19 +17601,19 @@
         <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E16" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F16" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -17622,19 +17622,19 @@
         <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E17" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -17643,19 +17643,19 @@
         <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E18" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -17664,19 +17664,19 @@
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E19" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -17685,19 +17685,19 @@
         <v>116</v>
       </c>
       <c r="D20" t="s">
+        <v>570</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>565</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="I20" t="s">
         <v>571</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="I20" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -17706,19 +17706,19 @@
         <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="E21" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -17727,19 +17727,19 @@
         <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F22" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G22">
         <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -17748,19 +17748,19 @@
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="E23" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F23" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -17769,24 +17769,24 @@
         <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="E24" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F24" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G24">
         <v>100</v>
       </c>
       <c r="I24" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C26">
         <v>121</v>
@@ -17818,7 +17818,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C32">
         <v>131</v>
@@ -17830,10 +17830,10 @@
         <v>132</v>
       </c>
       <c r="D33" t="s">
+        <v>532</v>
+      </c>
+      <c r="I33" t="s">
         <v>533</v>
-      </c>
-      <c r="I33" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -17842,7 +17842,7 @@
         <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -17851,10 +17851,10 @@
         <v>134</v>
       </c>
       <c r="D35" t="s">
+        <v>535</v>
+      </c>
+      <c r="I35" t="s">
         <v>536</v>
-      </c>
-      <c r="I35" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.5x: StatusEffect icons, descriptions
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0985A86-FC05-4CDF-BF63-5F86AA271A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3DC1E0-980C-40B2-BCD4-7AC764DB9911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="911">
   <si>
     <t>ID</t>
   </si>
@@ -3166,6 +3166,72 @@
   </si>
   <si>
     <t>timer=1000, number=0.025</t>
+  </si>
+  <si>
+    <t>Visual effect</t>
+  </si>
+  <si>
+    <t>cyan tint</t>
+  </si>
+  <si>
+    <t>blue tint</t>
+  </si>
+  <si>
+    <t>burn gif</t>
+  </si>
+  <si>
+    <t>smoke gif, black tint</t>
+  </si>
+  <si>
+    <t>water gif</t>
+  </si>
+  <si>
+    <t>thick water gif</t>
+  </si>
+  <si>
+    <t>bleed icon</t>
+  </si>
+  <si>
+    <t>hemorrhage icon</t>
+  </si>
+  <si>
+    <t>wilt icon</t>
+  </si>
+  <si>
+    <t>wither icon</t>
+  </si>
+  <si>
+    <t>sick icon</t>
+  </si>
+  <si>
+    <t>diseased icon</t>
+  </si>
+  <si>
+    <t>rot icon</t>
+  </si>
+  <si>
+    <t>decayed icon</t>
+  </si>
+  <si>
+    <t>hungry icon</t>
+  </si>
+  <si>
+    <t>weak icon</t>
+  </si>
+  <si>
+    <t>thirsty icon</t>
+  </si>
+  <si>
+    <t>woozy icon</t>
+  </si>
+  <si>
+    <t>confused icon</t>
+  </si>
+  <si>
+    <t>invulnerable icon</t>
+  </si>
+  <si>
+    <t>unkillable icon</t>
   </si>
 </sst>
 </file>
@@ -4286,7 +4352,7 @@
   <dimension ref="A1:S110"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H20" sqref="H20:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12676,10 +12742,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A228F-2BB3-44AC-82E9-D9BE084DFD89}">
-  <dimension ref="B2:F34"/>
+  <dimension ref="B2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B20" sqref="B20:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12689,9 +12755,10 @@
     <col min="4" max="4" width="57.140625" customWidth="1"/>
     <col min="5" max="5" width="70.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" customWidth="1"/>
+    <col min="7" max="7" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
@@ -12707,8 +12774,11 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
         <v>429</v>
       </c>
@@ -12718,8 +12788,11 @@
       <c r="E3" s="10" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="10" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>430</v>
       </c>
@@ -12732,15 +12805,18 @@
       <c r="E4" s="10" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="10" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>415</v>
       </c>
@@ -12753,8 +12829,11 @@
       <c r="E6" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>67</v>
       </c>
@@ -12767,8 +12846,11 @@
       <c r="E7" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>416</v>
       </c>
@@ -12781,8 +12863,11 @@
       <c r="E8" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>68</v>
       </c>
@@ -12795,8 +12880,11 @@
       <c r="E9" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>195</v>
       </c>
@@ -12809,8 +12897,11 @@
       <c r="E10" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>418</v>
       </c>
@@ -12823,8 +12914,11 @@
       <c r="E12" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>417</v>
       </c>
@@ -12837,8 +12931,11 @@
       <c r="E13" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>419</v>
       </c>
@@ -12851,8 +12948,11 @@
       <c r="E14" s="11" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>420</v>
       </c>
@@ -12865,8 +12965,11 @@
       <c r="E15" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>413</v>
       </c>
@@ -12882,8 +12985,11 @@
       <c r="F16" s="12" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>414</v>
       </c>
@@ -12897,8 +13003,11 @@
         <v>444</v>
       </c>
       <c r="F17" s="12"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>421</v>
       </c>
@@ -12912,8 +13021,11 @@
         <v>454</v>
       </c>
       <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>422</v>
       </c>
@@ -12927,8 +13039,11 @@
         <v>455</v>
       </c>
       <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>423</v>
       </c>
@@ -12941,8 +13056,11 @@
       <c r="E20" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>424</v>
       </c>
@@ -12955,8 +13073,11 @@
       <c r="E21" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>194</v>
       </c>
@@ -12969,8 +13090,11 @@
       <c r="E22" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>425</v>
       </c>
@@ -12983,8 +13107,11 @@
       <c r="E23" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>426</v>
       </c>
@@ -12997,8 +13124,11 @@
       <c r="E24" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>427</v>
       </c>
@@ -13011,8 +13141,11 @@
       <c r="E25" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>428</v>
       </c>
@@ -13020,7 +13153,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>434</v>
       </c>
@@ -13028,7 +13161,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>435</v>
       </c>
@@ -13036,7 +13169,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>436</v>
       </c>
@@ -13044,7 +13177,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>437</v>
       </c>
@@ -13052,7 +13185,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>438</v>
       </c>

</xml_diff>

<commit_message>
v0.6.6b: Feature inventories, some other interaction outlines
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3DC1E0-980C-40B2-BCD4-7AC764DB9911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C909A43-F695-4E21-8D02-A06597574854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="3" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="911">
   <si>
     <t>ID</t>
   </si>
@@ -3279,12 +3279,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3300,7 +3312,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3342,6 +3354,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10881,14 +10898,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="22" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47.140625" bestFit="1" customWidth="1"/>
@@ -10900,12 +10917,13 @@
         <v>640</v>
       </c>
       <c r="B1" s="2"/>
+      <c r="C1" s="21"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -10925,7 +10943,7 @@
       <c r="B4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="22" t="s">
         <v>199</v>
       </c>
       <c r="D4" t="s">
@@ -10945,7 +10963,7 @@
       <c r="B6" s="4">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="19" t="s">
         <v>201</v>
       </c>
       <c r="D6" t="s">
@@ -10962,7 +10980,7 @@
       <c r="B7" s="4">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="19" t="s">
         <v>202</v>
       </c>
       <c r="E7">
@@ -10976,7 +10994,7 @@
       <c r="B8" s="4">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="19" t="s">
         <v>203</v>
       </c>
       <c r="D8" t="s">
@@ -10993,7 +11011,7 @@
       <c r="B9" s="4">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="19" t="s">
         <v>204</v>
       </c>
       <c r="E9">
@@ -11007,7 +11025,7 @@
       <c r="B11" s="4">
         <v>101</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="20" t="s">
         <v>712</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -11027,7 +11045,7 @@
       <c r="B12" s="4">
         <v>102</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="20" t="s">
         <v>234</v>
       </c>
       <c r="D12" s="4"/>
@@ -11045,7 +11063,7 @@
       <c r="B13" s="4">
         <v>103</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
@@ -11056,7 +11074,7 @@
       <c r="B14" s="4">
         <v>111</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="19" t="s">
         <v>729</v>
       </c>
       <c r="E14">
@@ -11073,6 +11091,7 @@
       <c r="B15" s="4">
         <v>112</v>
       </c>
+      <c r="C15" s="19"/>
       <c r="H15" t="s">
         <v>726</v>
       </c>
@@ -11081,6 +11100,7 @@
       <c r="B16" s="4">
         <v>113</v>
       </c>
+      <c r="C16" s="19"/>
       <c r="H16" t="s">
         <v>727</v>
       </c>
@@ -11089,6 +11109,7 @@
       <c r="B17" s="4">
         <v>114</v>
       </c>
+      <c r="C17" s="19"/>
       <c r="H17" t="s">
         <v>728</v>
       </c>
@@ -11097,7 +11118,7 @@
       <c r="B18" s="4">
         <v>115</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="19" t="s">
         <v>730</v>
       </c>
       <c r="G18" t="s">
@@ -11108,7 +11129,7 @@
       <c r="B19" s="4">
         <v>121</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="19" t="s">
         <v>217</v>
       </c>
       <c r="E19">
@@ -11125,6 +11146,7 @@
       <c r="B20" s="4">
         <v>122</v>
       </c>
+      <c r="C20" s="19"/>
       <c r="H20" t="s">
         <v>726</v>
       </c>
@@ -11133,6 +11155,7 @@
       <c r="B21" s="4">
         <v>123</v>
       </c>
+      <c r="C21" s="19"/>
       <c r="H21" t="s">
         <v>727</v>
       </c>
@@ -11141,6 +11164,7 @@
       <c r="B22" s="4">
         <v>124</v>
       </c>
+      <c r="C22" s="19"/>
       <c r="H22" t="s">
         <v>728</v>
       </c>
@@ -11149,7 +11173,7 @@
       <c r="B23" s="4">
         <v>125</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="19" t="s">
         <v>753</v>
       </c>
       <c r="E23">
@@ -11166,6 +11190,7 @@
       <c r="B24" s="4">
         <v>126</v>
       </c>
+      <c r="C24" s="19"/>
       <c r="H24" t="s">
         <v>758</v>
       </c>
@@ -11174,6 +11199,7 @@
       <c r="B25" s="4">
         <v>127</v>
       </c>
+      <c r="C25" s="19"/>
       <c r="E25">
         <v>3</v>
       </c>
@@ -11185,6 +11211,7 @@
       <c r="B26" s="4">
         <v>128</v>
       </c>
+      <c r="C26" s="19"/>
       <c r="E26">
         <v>3</v>
       </c>
@@ -11196,7 +11223,7 @@
       <c r="B27" s="4">
         <v>131</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="19" t="s">
         <v>218</v>
       </c>
       <c r="E27">
@@ -11213,6 +11240,7 @@
       <c r="B28" s="4">
         <v>132</v>
       </c>
+      <c r="C28" s="19"/>
       <c r="H28" t="s">
         <v>726</v>
       </c>
@@ -11221,6 +11249,7 @@
       <c r="B29" s="4">
         <v>133</v>
       </c>
+      <c r="C29" s="19"/>
       <c r="H29" t="s">
         <v>727</v>
       </c>
@@ -11229,6 +11258,7 @@
       <c r="B30" s="4">
         <v>134</v>
       </c>
+      <c r="C30" s="19"/>
       <c r="H30" t="s">
         <v>728</v>
       </c>
@@ -11237,7 +11267,7 @@
       <c r="B31" s="4">
         <v>141</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="19" t="s">
         <v>220</v>
       </c>
       <c r="E31">
@@ -11254,6 +11284,7 @@
       <c r="B32" s="4">
         <v>142</v>
       </c>
+      <c r="C32" s="19"/>
       <c r="H32" t="s">
         <v>727</v>
       </c>
@@ -11262,7 +11293,7 @@
       <c r="B33" s="4">
         <v>151</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="19" t="s">
         <v>736</v>
       </c>
       <c r="D33" t="s">
@@ -11282,6 +11313,7 @@
       <c r="B34" s="4">
         <v>152</v>
       </c>
+      <c r="C34" s="19"/>
       <c r="H34" t="s">
         <v>726</v>
       </c>
@@ -11290,6 +11322,7 @@
       <c r="B35" s="4">
         <v>153</v>
       </c>
+      <c r="C35" s="19"/>
       <c r="H35" t="s">
         <v>727</v>
       </c>
@@ -11298,6 +11331,7 @@
       <c r="B36" s="4">
         <v>154</v>
       </c>
+      <c r="C36" s="19"/>
       <c r="H36" t="s">
         <v>728</v>
       </c>
@@ -11306,7 +11340,7 @@
       <c r="B37" s="4">
         <v>155</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="19" t="s">
         <v>737</v>
       </c>
       <c r="H37" t="s">
@@ -11317,6 +11351,7 @@
       <c r="B38" s="4">
         <v>156</v>
       </c>
+      <c r="C38" s="19"/>
       <c r="H38" t="s">
         <v>726</v>
       </c>
@@ -11325,6 +11360,7 @@
       <c r="B39" s="4">
         <v>157</v>
       </c>
+      <c r="C39" s="19"/>
       <c r="H39" t="s">
         <v>727</v>
       </c>
@@ -11333,6 +11369,7 @@
       <c r="B40" s="4">
         <v>158</v>
       </c>
+      <c r="C40" s="19"/>
       <c r="H40" t="s">
         <v>728</v>
       </c>
@@ -11341,7 +11378,7 @@
       <c r="B41" s="4">
         <v>161</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="23" t="s">
         <v>216</v>
       </c>
       <c r="E41">
@@ -11355,7 +11392,7 @@
       <c r="B42" s="4">
         <v>162</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="23" t="s">
         <v>222</v>
       </c>
       <c r="E42">
@@ -11369,7 +11406,7 @@
       <c r="B43" s="4">
         <v>163</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="23" t="s">
         <v>223</v>
       </c>
       <c r="E43">
@@ -11383,7 +11420,7 @@
       <c r="B44" s="4">
         <v>164</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="23" t="s">
         <v>224</v>
       </c>
       <c r="E44">
@@ -11397,7 +11434,7 @@
       <c r="B45" s="4">
         <v>165</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="23" t="s">
         <v>226</v>
       </c>
       <c r="E45">
@@ -11411,7 +11448,7 @@
       <c r="B46" s="4">
         <v>171</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="19" t="s">
         <v>227</v>
       </c>
       <c r="D46" t="s">
@@ -11428,7 +11465,7 @@
       <c r="B47" s="4">
         <v>172</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="19" t="s">
         <v>229</v>
       </c>
       <c r="E47">
@@ -11445,7 +11482,7 @@
       <c r="B48" s="4">
         <v>173</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="19" t="s">
         <v>229</v>
       </c>
       <c r="E48">
@@ -11459,7 +11496,7 @@
       <c r="B49" s="4">
         <v>174</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="19" t="s">
         <v>235</v>
       </c>
       <c r="E49">
@@ -11473,7 +11510,7 @@
       <c r="B50" s="4">
         <v>175</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="19" t="s">
         <v>794</v>
       </c>
       <c r="E50">
@@ -11487,7 +11524,7 @@
       <c r="B51" s="4">
         <v>176</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="19" t="s">
         <v>236</v>
       </c>
       <c r="E51">
@@ -11501,7 +11538,7 @@
       <c r="B52" s="4">
         <v>177</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="19" t="s">
         <v>237</v>
       </c>
       <c r="E52">
@@ -11515,7 +11552,7 @@
       <c r="B53" s="4">
         <v>181</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="19" t="s">
         <v>230</v>
       </c>
       <c r="D53" t="s">
@@ -11532,7 +11569,7 @@
       <c r="B54" s="4">
         <v>182</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="19" t="s">
         <v>231</v>
       </c>
       <c r="E54">
@@ -11546,7 +11583,7 @@
       <c r="B55" s="4">
         <v>183</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="19" t="s">
         <v>232</v>
       </c>
       <c r="E55">
@@ -11560,7 +11597,7 @@
       <c r="B56" s="4">
         <v>184</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="19" t="s">
         <v>233</v>
       </c>
       <c r="E56">
@@ -11574,7 +11611,7 @@
       <c r="B57" s="4">
         <v>185</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="23" t="s">
         <v>215</v>
       </c>
       <c r="E57">
@@ -11588,7 +11625,7 @@
       <c r="B58" s="4">
         <v>191</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="19" t="s">
         <v>774</v>
       </c>
       <c r="E58">
@@ -11605,6 +11642,7 @@
       <c r="B59" s="4">
         <v>192</v>
       </c>
+      <c r="C59" s="19"/>
       <c r="H59" t="s">
         <v>727</v>
       </c>
@@ -11613,7 +11651,7 @@
       <c r="B60" s="4">
         <v>193</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="19" t="s">
         <v>775</v>
       </c>
       <c r="H60" t="s">
@@ -11624,6 +11662,7 @@
       <c r="B61" s="4">
         <v>194</v>
       </c>
+      <c r="C61" s="19"/>
       <c r="H61" t="s">
         <v>727</v>
       </c>
@@ -11632,7 +11671,7 @@
       <c r="B62" s="4">
         <v>201</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="19" t="s">
         <v>213</v>
       </c>
       <c r="D62" t="s">
@@ -11649,7 +11688,7 @@
       <c r="B63" s="4">
         <v>202</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="19" t="s">
         <v>242</v>
       </c>
       <c r="E63">
@@ -11661,7 +11700,7 @@
       <c r="B64" s="4" t="s">
         <v>777</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="19" t="s">
         <v>239</v>
       </c>
       <c r="D64" t="s">
@@ -11681,7 +11720,7 @@
       <c r="B65" s="4" t="s">
         <v>778</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="19" t="s">
         <v>238</v>
       </c>
       <c r="E65">
@@ -11698,7 +11737,7 @@
       <c r="B66" s="4">
         <v>251</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="19" t="s">
         <v>243</v>
       </c>
       <c r="D66" t="s">
@@ -11718,6 +11757,7 @@
       <c r="B67" s="4">
         <v>252</v>
       </c>
+      <c r="C67" s="19"/>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
         <v>727</v>
@@ -11727,7 +11767,7 @@
       <c r="B69" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="19" t="s">
         <v>207</v>
       </c>
       <c r="D69" t="s">
@@ -11747,7 +11787,7 @@
       <c r="B70" s="4">
         <v>311</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="19" t="s">
         <v>212</v>
       </c>
       <c r="G70" s="9" t="s">
@@ -11761,6 +11801,7 @@
       <c r="B71" s="4">
         <v>312</v>
       </c>
+      <c r="C71" s="19"/>
       <c r="H71" t="s">
         <v>752</v>
       </c>
@@ -11769,7 +11810,7 @@
       <c r="B72" s="4">
         <v>321</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="19" t="s">
         <v>743</v>
       </c>
       <c r="D72" t="s">
@@ -11789,6 +11830,7 @@
       <c r="B73" s="4">
         <v>322</v>
       </c>
+      <c r="C73" s="19"/>
       <c r="E73">
         <v>100</v>
       </c>
@@ -11803,6 +11845,7 @@
       <c r="B74" s="4">
         <v>323</v>
       </c>
+      <c r="C74" s="19"/>
       <c r="G74" t="s">
         <v>750</v>
       </c>
@@ -11815,7 +11858,7 @@
       <c r="B75" s="4">
         <v>331</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="19" t="s">
         <v>211</v>
       </c>
       <c r="D75" t="s">
@@ -11836,6 +11879,7 @@
       <c r="B76" s="4">
         <v>332</v>
       </c>
+      <c r="C76" s="19"/>
       <c r="H76" t="s">
         <v>763</v>
       </c>
@@ -11845,6 +11889,7 @@
       <c r="B77" s="4">
         <v>333</v>
       </c>
+      <c r="C77" s="19"/>
       <c r="H77" t="s">
         <v>764</v>
       </c>
@@ -11854,6 +11899,7 @@
       <c r="B78" s="4">
         <v>334</v>
       </c>
+      <c r="C78" s="19"/>
       <c r="H78" t="s">
         <v>765</v>
       </c>
@@ -11863,6 +11909,7 @@
       <c r="B79" s="4">
         <v>335</v>
       </c>
+      <c r="C79" s="19"/>
       <c r="H79" t="s">
         <v>766</v>
       </c>
@@ -11872,6 +11919,7 @@
       <c r="B80" s="4">
         <v>336</v>
       </c>
+      <c r="C80" s="19"/>
       <c r="H80" t="s">
         <v>767</v>
       </c>
@@ -11881,6 +11929,7 @@
       <c r="B81" s="4">
         <v>337</v>
       </c>
+      <c r="C81" s="19"/>
       <c r="H81" t="s">
         <v>768</v>
       </c>
@@ -11890,6 +11939,7 @@
       <c r="B82" s="4">
         <v>338</v>
       </c>
+      <c r="C82" s="19"/>
       <c r="H82" t="s">
         <v>769</v>
       </c>
@@ -11899,7 +11949,7 @@
       <c r="B83" s="4">
         <v>339</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="19" t="s">
         <v>770</v>
       </c>
       <c r="E83">
@@ -11917,6 +11967,7 @@
       <c r="B84" s="4">
         <v>340</v>
       </c>
+      <c r="C84" s="19"/>
       <c r="H84" t="s">
         <v>727</v>
       </c>
@@ -11926,6 +11977,7 @@
       <c r="B85" s="4">
         <v>341</v>
       </c>
+      <c r="C85" s="19"/>
       <c r="H85" t="s">
         <v>772</v>
       </c>
@@ -11935,6 +11987,7 @@
       <c r="B86" s="4">
         <v>342</v>
       </c>
+      <c r="C86" s="19"/>
       <c r="H86" t="s">
         <v>773</v>
       </c>
@@ -11944,7 +11997,7 @@
       <c r="B87" s="4">
         <v>343</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="19" t="s">
         <v>771</v>
       </c>
       <c r="G87" t="s">
@@ -11959,6 +12012,7 @@
       <c r="B88" s="4">
         <v>344</v>
       </c>
+      <c r="C88" s="19"/>
       <c r="H88" t="s">
         <v>727</v>
       </c>
@@ -11968,6 +12022,7 @@
       <c r="B89" s="4">
         <v>345</v>
       </c>
+      <c r="C89" s="19"/>
       <c r="H89" t="s">
         <v>772</v>
       </c>
@@ -11977,6 +12032,7 @@
       <c r="B90" s="4">
         <v>346</v>
       </c>
+      <c r="C90" s="19"/>
       <c r="H90" t="s">
         <v>773</v>
       </c>
@@ -11985,7 +12041,7 @@
       <c r="B92" s="4">
         <v>401</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C92" s="19" t="s">
         <v>288</v>
       </c>
       <c r="D92" t="s">
@@ -12002,7 +12058,7 @@
       <c r="B93" s="4">
         <v>411</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C93" s="19" t="s">
         <v>709</v>
       </c>
       <c r="E93">
@@ -12019,6 +12075,7 @@
       <c r="B94" s="4">
         <v>412</v>
       </c>
+      <c r="C94" s="19"/>
       <c r="G94" t="s">
         <v>293</v>
       </c>
@@ -12030,7 +12087,7 @@
       <c r="B95" s="4">
         <v>421</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C95" s="19" t="s">
         <v>784</v>
       </c>
       <c r="E95">
@@ -12044,7 +12101,7 @@
       <c r="B96" s="4">
         <v>422</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C96" s="19" t="s">
         <v>785</v>
       </c>
     </row>
@@ -12052,7 +12109,7 @@
       <c r="B97" s="4">
         <v>423</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C97" s="19" t="s">
         <v>786</v>
       </c>
     </row>
@@ -12060,7 +12117,7 @@
       <c r="B98" s="4">
         <v>424</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="19" t="s">
         <v>787</v>
       </c>
     </row>
@@ -12068,7 +12125,7 @@
       <c r="B99" s="4">
         <v>425</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C99" s="19" t="s">
         <v>788</v>
       </c>
       <c r="E99">
@@ -12079,7 +12136,7 @@
       <c r="B100" s="4">
         <v>426</v>
       </c>
-      <c r="C100" t="s">
+      <c r="C100" s="19" t="s">
         <v>818</v>
       </c>
       <c r="E100">
@@ -12090,7 +12147,7 @@
       <c r="B101" s="4">
         <v>431</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C101" s="19" t="s">
         <v>240</v>
       </c>
       <c r="E101">
@@ -12101,7 +12158,7 @@
       <c r="B102" s="3">
         <v>441</v>
       </c>
-      <c r="C102" t="s">
+      <c r="C102" s="19" t="s">
         <v>241</v>
       </c>
       <c r="E102">
@@ -12118,6 +12175,7 @@
       <c r="B103" s="4">
         <v>442</v>
       </c>
+      <c r="C103" s="19"/>
       <c r="H103" t="s">
         <v>790</v>
       </c>
@@ -12126,6 +12184,7 @@
       <c r="B104" s="4">
         <v>443</v>
       </c>
+      <c r="C104" s="19"/>
       <c r="H104" t="s">
         <v>791</v>
       </c>
@@ -12134,7 +12193,7 @@
       <c r="B106" s="4">
         <v>501</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="19" t="s">
         <v>245</v>
       </c>
       <c r="D106" t="s">
@@ -12148,7 +12207,7 @@
       <c r="B107" s="4">
         <v>502</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C107" s="19" t="s">
         <v>246</v>
       </c>
     </row>
@@ -12156,7 +12215,7 @@
       <c r="B108" s="4">
         <v>503</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C108" s="19" t="s">
         <v>247</v>
       </c>
     </row>
@@ -12164,7 +12223,7 @@
       <c r="B109" s="4">
         <v>504</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C109" s="19" t="s">
         <v>248</v>
       </c>
     </row>
@@ -12172,7 +12231,7 @@
       <c r="B110" s="4">
         <v>505</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C110" s="19" t="s">
         <v>249</v>
       </c>
     </row>
@@ -12180,7 +12239,7 @@
       <c r="B111" s="4">
         <v>511</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="19" t="s">
         <v>250</v>
       </c>
       <c r="E111">
@@ -12191,7 +12250,7 @@
       <c r="B112" s="4">
         <v>512</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C112" s="19" t="s">
         <v>251</v>
       </c>
     </row>
@@ -12199,7 +12258,7 @@
       <c r="B113" s="4">
         <v>513</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C113" s="19" t="s">
         <v>252</v>
       </c>
     </row>
@@ -12744,8 +12803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981A228F-2BB3-44AC-82E9-D9BE084DFD89}">
   <dimension ref="B2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B25"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13229,7 +13288,7 @@
   <dimension ref="A1:Y227"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="S42" sqref="S42"/>

</xml_diff>

<commit_message>
v0.6.6e: Interaction Logic III
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AB400B-0037-4146-971D-B8B99F21C88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6C7B95-9B21-48A0-AF31-9F52D46F3011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -10902,8 +10902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C18" activeCellId="1" sqref="C27:C32 C18:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11122,7 +11122,7 @@
       <c r="B18" s="4">
         <v>115</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="19" t="s">
         <v>726</v>
       </c>
       <c r="G18" t="s">
@@ -11133,7 +11133,7 @@
       <c r="B19" s="4">
         <v>121</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="19" t="s">
         <v>216</v>
       </c>
       <c r="E19">
@@ -11150,7 +11150,7 @@
       <c r="B20" s="4">
         <v>122</v>
       </c>
-      <c r="C20" s="15"/>
+      <c r="C20" s="19"/>
       <c r="H20" t="s">
         <v>722</v>
       </c>
@@ -11159,7 +11159,7 @@
       <c r="B21" s="4">
         <v>123</v>
       </c>
-      <c r="C21" s="15"/>
+      <c r="C21" s="19"/>
       <c r="H21" t="s">
         <v>723</v>
       </c>
@@ -11168,7 +11168,7 @@
       <c r="B22" s="4">
         <v>124</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="19"/>
       <c r="H22" t="s">
         <v>724</v>
       </c>
@@ -11227,7 +11227,7 @@
       <c r="B27" s="4">
         <v>131</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="19" t="s">
         <v>217</v>
       </c>
       <c r="E27">
@@ -11244,7 +11244,7 @@
       <c r="B28" s="4">
         <v>132</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="19"/>
       <c r="H28" t="s">
         <v>722</v>
       </c>
@@ -11253,7 +11253,7 @@
       <c r="B29" s="4">
         <v>133</v>
       </c>
-      <c r="C29" s="15"/>
+      <c r="C29" s="19"/>
       <c r="H29" t="s">
         <v>723</v>
       </c>
@@ -11262,7 +11262,7 @@
       <c r="B30" s="4">
         <v>134</v>
       </c>
-      <c r="C30" s="15"/>
+      <c r="C30" s="19"/>
       <c r="H30" t="s">
         <v>724</v>
       </c>
@@ -11271,7 +11271,7 @@
       <c r="B31" s="4">
         <v>141</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="19" t="s">
         <v>219</v>
       </c>
       <c r="E31">
@@ -11288,7 +11288,7 @@
       <c r="B32" s="4">
         <v>142</v>
       </c>
-      <c r="C32" s="15"/>
+      <c r="C32" s="19"/>
       <c r="H32" t="s">
         <v>723</v>
       </c>
@@ -13292,10 +13292,10 @@
   <dimension ref="A1:Y228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D200" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N213" sqref="N213"/>
+      <selection pane="bottomRight" activeCell="C194" activeCellId="25" sqref="C4:C8 C19 C21 C24 C25 C26 C27 C15 C16 C13 C10 C76 C90 C106 C107 C108 C120 C121 C180 C181 C182 C185 C186 C190 C196 C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.6g: Interaction Logic V
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6C7B95-9B21-48A0-AF31-9F52D46F3011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42077637-6FC6-4CF4-A602-56E38D255AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -10902,8 +10902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" activeCellId="1" sqref="C27:C32 C18:C22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11724,7 +11724,7 @@
       <c r="B65" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="19" t="s">
         <v>237</v>
       </c>
       <c r="E65">
@@ -13291,11 +13291,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y228"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C194" activeCellId="25" sqref="C4:C8 C19 C21 C24 C25 C26 C27 C15 C16 C13 C10 C76 C90 C106 C107 C108 C120 C121 C180 C181 C182 C185 C186 C190 C196 C194"/>
+      <selection pane="bottomRight" activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.6h: Interaction Logic VI
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42077637-6FC6-4CF4-A602-56E38D255AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011A34A8-1E67-4AB3-911A-24E1F3FE52D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -3315,7 +3315,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3346,7 +3346,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -4390,26 +4389,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="H1" s="24" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="H1" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
@@ -4418,13 +4417,13 @@
       <c r="H3" t="s">
         <v>55</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -10262,7 +10261,7 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>606</v>
       </c>
       <c r="C4" t="s">
@@ -10282,7 +10281,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
+      <c r="B5" s="22"/>
       <c r="C5" t="s">
         <v>576</v>
       </c>
@@ -10300,7 +10299,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
+      <c r="B6" s="22"/>
       <c r="C6" t="s">
         <v>577</v>
       </c>
@@ -10318,7 +10317,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
+      <c r="B7" s="22"/>
       <c r="C7" t="s">
         <v>578</v>
       </c>
@@ -10336,7 +10335,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+      <c r="B8" s="22"/>
       <c r="C8" t="s">
         <v>579</v>
       </c>
@@ -10354,7 +10353,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="B9" s="22"/>
       <c r="C9" t="s">
         <v>580</v>
       </c>
@@ -10372,7 +10371,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
+      <c r="B10" s="22"/>
       <c r="C10" t="s">
         <v>581</v>
       </c>
@@ -10390,7 +10389,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
+      <c r="B11" s="22"/>
       <c r="C11" t="s">
         <v>582</v>
       </c>
@@ -10408,7 +10407,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12" t="s">
         <v>583</v>
       </c>
@@ -10426,7 +10425,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
+      <c r="B13" s="22"/>
       <c r="C13" t="s">
         <v>584</v>
       </c>
@@ -10444,7 +10443,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>623</v>
       </c>
       <c r="C15" t="s">
@@ -10461,7 +10460,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
+      <c r="B16" s="22"/>
       <c r="C16" t="s">
         <v>615</v>
       </c>
@@ -10476,7 +10475,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
+      <c r="B17" s="22"/>
       <c r="C17" t="s">
         <v>631</v>
       </c>
@@ -10494,7 +10493,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
+      <c r="B18" s="22"/>
       <c r="C18" t="s">
         <v>632</v>
       </c>
@@ -10506,7 +10505,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19" t="s">
         <v>625</v>
       </c>
@@ -10521,7 +10520,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
+      <c r="B20" s="22"/>
       <c r="C20" t="s">
         <v>614</v>
       </c>
@@ -10539,7 +10538,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
+      <c r="B21" s="22"/>
       <c r="C21" t="s">
         <v>617</v>
       </c>
@@ -10557,7 +10556,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
+      <c r="B22" s="22"/>
       <c r="C22" t="s">
         <v>632</v>
       </c>
@@ -10569,7 +10568,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
+      <c r="B23" s="22"/>
       <c r="C23" t="s">
         <v>632</v>
       </c>
@@ -10581,7 +10580,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
+      <c r="B24" s="22"/>
       <c r="C24" t="s">
         <v>629</v>
       </c>
@@ -10903,13 +10902,13 @@
   <dimension ref="A1:H113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.85546875" style="4"/>
-    <col min="3" max="3" width="30.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="17" customWidth="1"/>
     <col min="4" max="5" width="13.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="47.140625" bestFit="1" customWidth="1"/>
@@ -10921,13 +10920,13 @@
         <v>636</v>
       </c>
       <c r="B1" s="2"/>
-      <c r="C1" s="17"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -10947,7 +10946,7 @@
       <c r="B4" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>199</v>
       </c>
       <c r="D4" t="s">
@@ -11029,7 +11028,7 @@
       <c r="B11" s="4">
         <v>101</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="19" t="s">
         <v>708</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -11049,7 +11048,7 @@
       <c r="B12" s="4">
         <v>102</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="19" t="s">
         <v>233</v>
       </c>
       <c r="D12" s="4"/>
@@ -11067,7 +11066,7 @@
       <c r="B13" s="4">
         <v>103</v>
       </c>
-      <c r="C13" s="20"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
@@ -11078,7 +11077,7 @@
       <c r="B14" s="4">
         <v>111</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="18" t="s">
         <v>725</v>
       </c>
       <c r="E14">
@@ -11095,7 +11094,7 @@
       <c r="B15" s="4">
         <v>112</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="18"/>
       <c r="H15" t="s">
         <v>722</v>
       </c>
@@ -11104,7 +11103,7 @@
       <c r="B16" s="4">
         <v>113</v>
       </c>
-      <c r="C16" s="15"/>
+      <c r="C16" s="18"/>
       <c r="H16" t="s">
         <v>723</v>
       </c>
@@ -11113,7 +11112,7 @@
       <c r="B17" s="4">
         <v>114</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="18"/>
       <c r="H17" t="s">
         <v>724</v>
       </c>
@@ -11122,7 +11121,7 @@
       <c r="B18" s="4">
         <v>115</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>726</v>
       </c>
       <c r="G18" t="s">
@@ -11133,7 +11132,7 @@
       <c r="B19" s="4">
         <v>121</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>216</v>
       </c>
       <c r="E19">
@@ -11150,7 +11149,7 @@
       <c r="B20" s="4">
         <v>122</v>
       </c>
-      <c r="C20" s="19"/>
+      <c r="C20" s="18"/>
       <c r="H20" t="s">
         <v>722</v>
       </c>
@@ -11159,7 +11158,7 @@
       <c r="B21" s="4">
         <v>123</v>
       </c>
-      <c r="C21" s="19"/>
+      <c r="C21" s="18"/>
       <c r="H21" t="s">
         <v>723</v>
       </c>
@@ -11168,7 +11167,7 @@
       <c r="B22" s="4">
         <v>124</v>
       </c>
-      <c r="C22" s="19"/>
+      <c r="C22" s="18"/>
       <c r="H22" t="s">
         <v>724</v>
       </c>
@@ -11177,7 +11176,7 @@
       <c r="B23" s="4">
         <v>125</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="18" t="s">
         <v>749</v>
       </c>
       <c r="E23">
@@ -11194,7 +11193,7 @@
       <c r="B24" s="4">
         <v>126</v>
       </c>
-      <c r="C24" s="15"/>
+      <c r="C24" s="18"/>
       <c r="H24" t="s">
         <v>754</v>
       </c>
@@ -11203,7 +11202,7 @@
       <c r="B25" s="4">
         <v>127</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="18"/>
       <c r="E25">
         <v>3</v>
       </c>
@@ -11215,7 +11214,7 @@
       <c r="B26" s="4">
         <v>128</v>
       </c>
-      <c r="C26" s="15"/>
+      <c r="C26" s="18"/>
       <c r="E26">
         <v>3</v>
       </c>
@@ -11227,7 +11226,7 @@
       <c r="B27" s="4">
         <v>131</v>
       </c>
-      <c r="C27" s="19" t="s">
+      <c r="C27" s="18" t="s">
         <v>217</v>
       </c>
       <c r="E27">
@@ -11244,7 +11243,7 @@
       <c r="B28" s="4">
         <v>132</v>
       </c>
-      <c r="C28" s="19"/>
+      <c r="C28" s="18"/>
       <c r="H28" t="s">
         <v>722</v>
       </c>
@@ -11253,7 +11252,7 @@
       <c r="B29" s="4">
         <v>133</v>
       </c>
-      <c r="C29" s="19"/>
+      <c r="C29" s="18"/>
       <c r="H29" t="s">
         <v>723</v>
       </c>
@@ -11262,7 +11261,7 @@
       <c r="B30" s="4">
         <v>134</v>
       </c>
-      <c r="C30" s="19"/>
+      <c r="C30" s="18"/>
       <c r="H30" t="s">
         <v>724</v>
       </c>
@@ -11271,7 +11270,7 @@
       <c r="B31" s="4">
         <v>141</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="18" t="s">
         <v>219</v>
       </c>
       <c r="E31">
@@ -11288,7 +11287,7 @@
       <c r="B32" s="4">
         <v>142</v>
       </c>
-      <c r="C32" s="19"/>
+      <c r="C32" s="18"/>
       <c r="H32" t="s">
         <v>723</v>
       </c>
@@ -11297,7 +11296,7 @@
       <c r="B33" s="4">
         <v>151</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="18" t="s">
         <v>732</v>
       </c>
       <c r="D33" t="s">
@@ -11317,7 +11316,7 @@
       <c r="B34" s="4">
         <v>152</v>
       </c>
-      <c r="C34" s="19"/>
+      <c r="C34" s="18"/>
       <c r="H34" t="s">
         <v>722</v>
       </c>
@@ -11326,7 +11325,7 @@
       <c r="B35" s="4">
         <v>153</v>
       </c>
-      <c r="C35" s="19"/>
+      <c r="C35" s="18"/>
       <c r="H35" t="s">
         <v>723</v>
       </c>
@@ -11335,7 +11334,7 @@
       <c r="B36" s="4">
         <v>154</v>
       </c>
-      <c r="C36" s="19"/>
+      <c r="C36" s="18"/>
       <c r="H36" t="s">
         <v>724</v>
       </c>
@@ -11344,7 +11343,7 @@
       <c r="B37" s="4">
         <v>155</v>
       </c>
-      <c r="C37" s="19" t="s">
+      <c r="C37" s="18" t="s">
         <v>733</v>
       </c>
       <c r="H37" t="s">
@@ -11355,7 +11354,7 @@
       <c r="B38" s="4">
         <v>156</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="18"/>
       <c r="H38" t="s">
         <v>722</v>
       </c>
@@ -11364,7 +11363,7 @@
       <c r="B39" s="4">
         <v>157</v>
       </c>
-      <c r="C39" s="19"/>
+      <c r="C39" s="18"/>
       <c r="H39" t="s">
         <v>723</v>
       </c>
@@ -11373,7 +11372,7 @@
       <c r="B40" s="4">
         <v>158</v>
       </c>
-      <c r="C40" s="19"/>
+      <c r="C40" s="18"/>
       <c r="H40" t="s">
         <v>724</v>
       </c>
@@ -11382,7 +11381,7 @@
       <c r="B41" s="4">
         <v>161</v>
       </c>
-      <c r="C41" s="19" t="s">
+      <c r="C41" s="18" t="s">
         <v>215</v>
       </c>
       <c r="E41">
@@ -11396,7 +11395,7 @@
       <c r="B42" s="4">
         <v>162</v>
       </c>
-      <c r="C42" s="19" t="s">
+      <c r="C42" s="18" t="s">
         <v>221</v>
       </c>
       <c r="E42">
@@ -11410,7 +11409,7 @@
       <c r="B43" s="4">
         <v>163</v>
       </c>
-      <c r="C43" s="19" t="s">
+      <c r="C43" s="18" t="s">
         <v>222</v>
       </c>
       <c r="E43">
@@ -11424,7 +11423,7 @@
       <c r="B44" s="4">
         <v>164</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C44" s="18" t="s">
         <v>223</v>
       </c>
       <c r="E44">
@@ -11438,7 +11437,7 @@
       <c r="B45" s="4">
         <v>165</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="18" t="s">
         <v>225</v>
       </c>
       <c r="E45">
@@ -11452,7 +11451,7 @@
       <c r="B46" s="4">
         <v>171</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" s="18" t="s">
         <v>226</v>
       </c>
       <c r="D46" t="s">
@@ -11500,7 +11499,7 @@
       <c r="B49" s="4">
         <v>174</v>
       </c>
-      <c r="C49" s="19" t="s">
+      <c r="C49" s="18" t="s">
         <v>234</v>
       </c>
       <c r="E49">
@@ -11514,7 +11513,7 @@
       <c r="B50" s="4">
         <v>175</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C50" s="18" t="s">
         <v>790</v>
       </c>
       <c r="E50">
@@ -11528,7 +11527,7 @@
       <c r="B51" s="4">
         <v>176</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" s="18" t="s">
         <v>235</v>
       </c>
       <c r="E51">
@@ -11542,7 +11541,7 @@
       <c r="B52" s="4">
         <v>177</v>
       </c>
-      <c r="C52" s="19" t="s">
+      <c r="C52" s="18" t="s">
         <v>236</v>
       </c>
       <c r="E52">
@@ -11556,7 +11555,7 @@
       <c r="B53" s="4">
         <v>181</v>
       </c>
-      <c r="C53" s="19" t="s">
+      <c r="C53" s="18" t="s">
         <v>229</v>
       </c>
       <c r="D53" t="s">
@@ -11573,7 +11572,7 @@
       <c r="B54" s="4">
         <v>182</v>
       </c>
-      <c r="C54" s="19" t="s">
+      <c r="C54" s="18" t="s">
         <v>230</v>
       </c>
       <c r="E54">
@@ -11587,7 +11586,7 @@
       <c r="B55" s="4">
         <v>183</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C55" s="18" t="s">
         <v>231</v>
       </c>
       <c r="E55">
@@ -11601,7 +11600,7 @@
       <c r="B56" s="4">
         <v>184</v>
       </c>
-      <c r="C56" s="19" t="s">
+      <c r="C56" s="18" t="s">
         <v>232</v>
       </c>
       <c r="E56">
@@ -11615,7 +11614,7 @@
       <c r="B57" s="4">
         <v>185</v>
       </c>
-      <c r="C57" s="19" t="s">
+      <c r="C57" s="18" t="s">
         <v>214</v>
       </c>
       <c r="E57">
@@ -11629,7 +11628,7 @@
       <c r="B58" s="4">
         <v>191</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="C58" s="18" t="s">
         <v>770</v>
       </c>
       <c r="E58">
@@ -11646,7 +11645,7 @@
       <c r="B59" s="4">
         <v>192</v>
       </c>
-      <c r="C59" s="19"/>
+      <c r="C59" s="18"/>
       <c r="H59" t="s">
         <v>723</v>
       </c>
@@ -11655,7 +11654,7 @@
       <c r="B60" s="4">
         <v>193</v>
       </c>
-      <c r="C60" s="19" t="s">
+      <c r="C60" s="18" t="s">
         <v>771</v>
       </c>
       <c r="H60" t="s">
@@ -11666,7 +11665,7 @@
       <c r="B61" s="4">
         <v>194</v>
       </c>
-      <c r="C61" s="19"/>
+      <c r="C61" s="18"/>
       <c r="H61" t="s">
         <v>723</v>
       </c>
@@ -11675,7 +11674,7 @@
       <c r="B62" s="4">
         <v>201</v>
       </c>
-      <c r="C62" s="19" t="s">
+      <c r="C62" s="18" t="s">
         <v>212</v>
       </c>
       <c r="D62" t="s">
@@ -11692,7 +11691,7 @@
       <c r="B63" s="4">
         <v>202</v>
       </c>
-      <c r="C63" s="19" t="s">
+      <c r="C63" s="18" t="s">
         <v>241</v>
       </c>
       <c r="E63">
@@ -11704,7 +11703,7 @@
       <c r="B64" s="4" t="s">
         <v>773</v>
       </c>
-      <c r="C64" s="19" t="s">
+      <c r="C64" s="18" t="s">
         <v>238</v>
       </c>
       <c r="D64" t="s">
@@ -11724,7 +11723,7 @@
       <c r="B65" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="C65" s="19" t="s">
+      <c r="C65" s="18" t="s">
         <v>237</v>
       </c>
       <c r="E65">
@@ -11741,7 +11740,7 @@
       <c r="B66" s="4">
         <v>251</v>
       </c>
-      <c r="C66" s="19" t="s">
+      <c r="C66" s="18" t="s">
         <v>242</v>
       </c>
       <c r="D66" t="s">
@@ -11761,7 +11760,7 @@
       <c r="B67" s="4">
         <v>252</v>
       </c>
-      <c r="C67" s="19"/>
+      <c r="C67" s="18"/>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
         <v>723</v>
@@ -11771,7 +11770,7 @@
       <c r="B69" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="C69" s="19" t="s">
+      <c r="C69" s="18" t="s">
         <v>207</v>
       </c>
       <c r="D69" t="s">
@@ -11791,7 +11790,7 @@
       <c r="B70" s="4">
         <v>311</v>
       </c>
-      <c r="C70" s="19" t="s">
+      <c r="C70" s="18" t="s">
         <v>211</v>
       </c>
       <c r="G70" s="9" t="s">
@@ -11805,7 +11804,7 @@
       <c r="B71" s="4">
         <v>312</v>
       </c>
-      <c r="C71" s="19"/>
+      <c r="C71" s="18"/>
       <c r="H71" t="s">
         <v>748</v>
       </c>
@@ -11814,7 +11813,7 @@
       <c r="B72" s="4">
         <v>321</v>
       </c>
-      <c r="C72" s="19" t="s">
+      <c r="C72" s="18" t="s">
         <v>739</v>
       </c>
       <c r="D72" t="s">
@@ -11834,7 +11833,7 @@
       <c r="B73" s="4">
         <v>322</v>
       </c>
-      <c r="C73" s="19"/>
+      <c r="C73" s="18"/>
       <c r="E73">
         <v>100</v>
       </c>
@@ -11849,7 +11848,7 @@
       <c r="B74" s="4">
         <v>323</v>
       </c>
-      <c r="C74" s="19"/>
+      <c r="C74" s="18"/>
       <c r="G74" t="s">
         <v>746</v>
       </c>
@@ -11862,7 +11861,7 @@
       <c r="B75" s="4">
         <v>331</v>
       </c>
-      <c r="C75" s="19" t="s">
+      <c r="C75" s="18" t="s">
         <v>907</v>
       </c>
       <c r="D75" t="s">
@@ -11883,7 +11882,7 @@
       <c r="B76" s="4">
         <v>332</v>
       </c>
-      <c r="C76" s="19"/>
+      <c r="C76" s="18"/>
       <c r="H76" t="s">
         <v>759</v>
       </c>
@@ -11893,7 +11892,7 @@
       <c r="B77" s="4">
         <v>333</v>
       </c>
-      <c r="C77" s="19"/>
+      <c r="C77" s="18"/>
       <c r="H77" t="s">
         <v>760</v>
       </c>
@@ -11903,7 +11902,7 @@
       <c r="B78" s="4">
         <v>334</v>
       </c>
-      <c r="C78" s="19"/>
+      <c r="C78" s="18"/>
       <c r="H78" t="s">
         <v>761</v>
       </c>
@@ -11913,7 +11912,7 @@
       <c r="B79" s="4">
         <v>335</v>
       </c>
-      <c r="C79" s="19"/>
+      <c r="C79" s="18"/>
       <c r="H79" t="s">
         <v>762</v>
       </c>
@@ -11923,7 +11922,7 @@
       <c r="B80" s="4">
         <v>336</v>
       </c>
-      <c r="C80" s="19"/>
+      <c r="C80" s="18"/>
       <c r="H80" t="s">
         <v>763</v>
       </c>
@@ -11933,7 +11932,7 @@
       <c r="B81" s="4">
         <v>337</v>
       </c>
-      <c r="C81" s="19"/>
+      <c r="C81" s="18"/>
       <c r="H81" t="s">
         <v>764</v>
       </c>
@@ -11943,7 +11942,7 @@
       <c r="B82" s="4">
         <v>338</v>
       </c>
-      <c r="C82" s="19"/>
+      <c r="C82" s="18"/>
       <c r="H82" t="s">
         <v>765</v>
       </c>
@@ -11953,7 +11952,7 @@
       <c r="B83" s="4">
         <v>339</v>
       </c>
-      <c r="C83" s="19" t="s">
+      <c r="C83" s="18" t="s">
         <v>766</v>
       </c>
       <c r="E83">
@@ -11971,7 +11970,7 @@
       <c r="B84" s="4">
         <v>340</v>
       </c>
-      <c r="C84" s="19"/>
+      <c r="C84" s="18"/>
       <c r="H84" t="s">
         <v>723</v>
       </c>
@@ -11981,7 +11980,7 @@
       <c r="B85" s="4">
         <v>341</v>
       </c>
-      <c r="C85" s="19"/>
+      <c r="C85" s="18"/>
       <c r="H85" t="s">
         <v>768</v>
       </c>
@@ -11991,7 +11990,7 @@
       <c r="B86" s="4">
         <v>342</v>
       </c>
-      <c r="C86" s="19"/>
+      <c r="C86" s="18"/>
       <c r="H86" t="s">
         <v>769</v>
       </c>
@@ -12001,7 +12000,7 @@
       <c r="B87" s="4">
         <v>343</v>
       </c>
-      <c r="C87" s="19" t="s">
+      <c r="C87" s="18" t="s">
         <v>767</v>
       </c>
       <c r="G87" t="s">
@@ -12016,7 +12015,7 @@
       <c r="B88" s="4">
         <v>344</v>
       </c>
-      <c r="C88" s="19"/>
+      <c r="C88" s="18"/>
       <c r="H88" t="s">
         <v>723</v>
       </c>
@@ -12026,7 +12025,7 @@
       <c r="B89" s="4">
         <v>345</v>
       </c>
-      <c r="C89" s="19"/>
+      <c r="C89" s="18"/>
       <c r="H89" t="s">
         <v>768</v>
       </c>
@@ -12036,7 +12035,7 @@
       <c r="B90" s="4">
         <v>346</v>
       </c>
-      <c r="C90" s="19"/>
+      <c r="C90" s="18"/>
       <c r="H90" t="s">
         <v>769</v>
       </c>
@@ -12045,7 +12044,7 @@
       <c r="B92" s="4">
         <v>401</v>
       </c>
-      <c r="C92" s="19" t="s">
+      <c r="C92" s="18" t="s">
         <v>287</v>
       </c>
       <c r="D92" t="s">
@@ -12062,7 +12061,7 @@
       <c r="B93" s="4">
         <v>411</v>
       </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="18" t="s">
         <v>705</v>
       </c>
       <c r="E93">
@@ -12079,7 +12078,7 @@
       <c r="B94" s="4">
         <v>412</v>
       </c>
-      <c r="C94" s="19"/>
+      <c r="C94" s="18"/>
       <c r="G94" t="s">
         <v>292</v>
       </c>
@@ -12091,7 +12090,7 @@
       <c r="B95" s="4">
         <v>421</v>
       </c>
-      <c r="C95" s="19" t="s">
+      <c r="C95" s="18" t="s">
         <v>780</v>
       </c>
       <c r="E95">
@@ -12105,7 +12104,7 @@
       <c r="B96" s="4">
         <v>422</v>
       </c>
-      <c r="C96" s="19" t="s">
+      <c r="C96" s="18" t="s">
         <v>781</v>
       </c>
     </row>
@@ -12113,7 +12112,7 @@
       <c r="B97" s="4">
         <v>423</v>
       </c>
-      <c r="C97" s="19" t="s">
+      <c r="C97" s="18" t="s">
         <v>782</v>
       </c>
     </row>
@@ -12121,7 +12120,7 @@
       <c r="B98" s="4">
         <v>424</v>
       </c>
-      <c r="C98" s="19" t="s">
+      <c r="C98" s="18" t="s">
         <v>783</v>
       </c>
     </row>
@@ -12129,7 +12128,7 @@
       <c r="B99" s="4">
         <v>425</v>
       </c>
-      <c r="C99" s="19" t="s">
+      <c r="C99" s="18" t="s">
         <v>784</v>
       </c>
       <c r="E99">
@@ -12140,7 +12139,7 @@
       <c r="B100" s="4">
         <v>426</v>
       </c>
-      <c r="C100" s="19" t="s">
+      <c r="C100" s="18" t="s">
         <v>814</v>
       </c>
       <c r="E100">
@@ -12151,7 +12150,7 @@
       <c r="B101" s="4">
         <v>431</v>
       </c>
-      <c r="C101" s="19" t="s">
+      <c r="C101" s="18" t="s">
         <v>239</v>
       </c>
       <c r="E101">
@@ -12162,7 +12161,7 @@
       <c r="B102" s="3">
         <v>441</v>
       </c>
-      <c r="C102" s="19" t="s">
+      <c r="C102" s="18" t="s">
         <v>240</v>
       </c>
       <c r="E102">
@@ -12179,7 +12178,7 @@
       <c r="B103" s="4">
         <v>442</v>
       </c>
-      <c r="C103" s="19"/>
+      <c r="C103" s="18"/>
       <c r="H103" t="s">
         <v>786</v>
       </c>
@@ -12188,7 +12187,7 @@
       <c r="B104" s="4">
         <v>443</v>
       </c>
-      <c r="C104" s="19"/>
+      <c r="C104" s="18"/>
       <c r="H104" t="s">
         <v>787</v>
       </c>
@@ -13045,7 +13044,7 @@
       <c r="E16" t="s">
         <v>439</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>454</v>
       </c>
       <c r="G16" t="s">
@@ -13065,7 +13064,7 @@
       <c r="E17" t="s">
         <v>440</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="20"/>
       <c r="G17" t="s">
         <v>891</v>
       </c>
@@ -13083,7 +13082,7 @@
       <c r="E18" t="s">
         <v>450</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" t="s">
         <v>888</v>
       </c>
@@ -13101,7 +13100,7 @@
       <c r="E19" t="s">
         <v>451</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="20"/>
       <c r="G19" t="s">
         <v>889</v>
       </c>
@@ -13292,10 +13291,10 @@
   <dimension ref="A1:Y228"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D189" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C201" sqref="C201"/>
+      <selection pane="bottomRight" activeCell="C222" sqref="C222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13317,23 +13316,23 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="K1" s="22" t="s">
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="K1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
     </row>
@@ -17574,7 +17573,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C4">
@@ -17597,7 +17596,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
+      <c r="B5" s="22"/>
       <c r="C5">
         <v>102</v>
       </c>
@@ -17618,7 +17617,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
+      <c r="B6" s="22"/>
       <c r="C6">
         <v>103</v>
       </c>
@@ -17639,7 +17638,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
+      <c r="B7" s="22"/>
       <c r="C7">
         <v>104</v>
       </c>
@@ -17660,7 +17659,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+      <c r="B8" s="22"/>
       <c r="C8">
         <v>105</v>
       </c>
@@ -17681,7 +17680,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="B9" s="22"/>
       <c r="C9">
         <v>106</v>
       </c>
@@ -17702,7 +17701,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
+      <c r="B10" s="22"/>
       <c r="C10">
         <v>107</v>
       </c>
@@ -17723,7 +17722,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
+      <c r="B11" s="22"/>
       <c r="C11">
         <v>108</v>
       </c>
@@ -17744,7 +17743,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
+      <c r="B12" s="22"/>
       <c r="C12">
         <v>109</v>
       </c>
@@ -17765,7 +17764,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
+      <c r="B13" s="22"/>
       <c r="C13">
         <v>110</v>
       </c>
@@ -17786,7 +17785,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="22" t="s">
         <v>456</v>
       </c>
       <c r="C15">
@@ -17809,7 +17808,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
+      <c r="B16" s="22"/>
       <c r="C16">
         <v>112</v>
       </c>
@@ -17830,7 +17829,7 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
+      <c r="B17" s="22"/>
       <c r="C17">
         <v>113</v>
       </c>
@@ -17851,7 +17850,7 @@
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="23"/>
+      <c r="B18" s="22"/>
       <c r="C18">
         <v>114</v>
       </c>
@@ -17872,7 +17871,7 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="23"/>
+      <c r="B19" s="22"/>
       <c r="C19">
         <v>115</v>
       </c>
@@ -17893,7 +17892,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="23"/>
+      <c r="B20" s="22"/>
       <c r="C20">
         <v>116</v>
       </c>
@@ -17914,7 +17913,7 @@
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="23"/>
+      <c r="B21" s="22"/>
       <c r="C21">
         <v>117</v>
       </c>
@@ -17935,7 +17934,7 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="23"/>
+      <c r="B22" s="22"/>
       <c r="C22">
         <v>118</v>
       </c>
@@ -17956,7 +17955,7 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="23"/>
+      <c r="B23" s="22"/>
       <c r="C23">
         <v>119</v>
       </c>
@@ -17977,7 +17976,7 @@
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
+      <c r="B24" s="22"/>
       <c r="C24">
         <v>120</v>
       </c>
@@ -17998,7 +17997,7 @@
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="22" t="s">
         <v>521</v>
       </c>
       <c r="C26">
@@ -18006,31 +18005,31 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
+      <c r="B27" s="22"/>
       <c r="C27">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="23"/>
+      <c r="B28" s="22"/>
       <c r="C28">
         <v>123</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="23"/>
+      <c r="B29" s="22"/>
       <c r="C29">
         <v>124</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="23"/>
+      <c r="B30" s="22"/>
       <c r="C30">
         <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="23" t="s">
+      <c r="B32" s="22" t="s">
         <v>522</v>
       </c>
       <c r="C32">
@@ -18038,7 +18037,7 @@
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="23"/>
+      <c r="B33" s="22"/>
       <c r="C33">
         <v>132</v>
       </c>
@@ -18050,7 +18049,7 @@
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="23"/>
+      <c r="B34" s="22"/>
       <c r="C34">
         <v>133</v>
       </c>
@@ -18059,7 +18058,7 @@
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="23"/>
+      <c r="B35" s="22"/>
       <c r="C35">
         <v>134</v>
       </c>
@@ -18071,7 +18070,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="23"/>
+      <c r="B36" s="22"/>
       <c r="C36">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
v0.6.6l: Misc, started VendingForm
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011A34A8-1E67-4AB3-911A-24E1F3FE52D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B70D3D-7EA4-4F24-BDA5-C7AD8830AA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -10901,8 +10901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11468,7 +11468,7 @@
       <c r="B47" s="4">
         <v>172</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="18" t="s">
         <v>228</v>
       </c>
       <c r="E47">
@@ -11485,7 +11485,7 @@
       <c r="B48" s="4">
         <v>173</v>
       </c>
-      <c r="C48" s="15" t="s">
+      <c r="C48" s="18" t="s">
         <v>228</v>
       </c>
       <c r="E48">

</xml_diff>

<commit_message>
v0.6.6m: VendingForm, water bottles
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B70D3D-7EA4-4F24-BDA5-C7AD8830AA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B573439-FDBD-44C2-9C11-994D6C0522A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="912">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="913">
   <si>
     <t>ID</t>
   </si>
@@ -3235,6 +3235,9 @@
   </si>
   <si>
     <t>Branch (pine)</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
   </si>
 </sst>
 </file>
@@ -10901,7 +10904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
@@ -13288,13 +13291,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y228"/>
+  <dimension ref="A1:Y229"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D189" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C222" sqref="C222"/>
+      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13590,55 +13593,55 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>2131</v>
+        <v>2115</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>912</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I18">
-        <v>12</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="C19" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I19">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H20">
         <v>6</v>
       </c>
       <c r="I20">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21">
-        <v>2134</v>
+        <v>2133</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H21">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I21">
         <v>20</v>
@@ -13646,543 +13649,528 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>2141</v>
+        <v>2134</v>
       </c>
       <c r="C22" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22">
-        <v>2</v>
-      </c>
-      <c r="F22">
-        <v>10</v>
+        <v>84</v>
+      </c>
+      <c r="H22">
+        <v>8</v>
       </c>
       <c r="I22">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>2142</v>
+        <v>2141</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F23">
-        <v>30</v>
-      </c>
-      <c r="H23">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="I23">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>2151</v>
+        <v>2142</v>
       </c>
       <c r="C24" t="s">
-        <v>89</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
+        <v>88</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>30</v>
+      </c>
+      <c r="H24">
+        <v>35</v>
+      </c>
+      <c r="I24">
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="C25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G25">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>2153</v>
+        <v>2152</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G26">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G27">
-        <v>50</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>2155</v>
+        <v>2154</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E28">
-        <v>2</v>
+        <v>92</v>
       </c>
       <c r="G28">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2156</v>
+        <v>2155</v>
       </c>
       <c r="C29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29">
         <v>2</v>
       </c>
       <c r="G29">
-        <v>500</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="G30">
-        <v>1000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>2158</v>
+        <v>2157</v>
       </c>
       <c r="C31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="G31">
-        <v>5000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32">
+        <v>2158</v>
+      </c>
+      <c r="C32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B33">
         <v>2159</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>96</v>
       </c>
-      <c r="E32">
+      <c r="E33">
         <v>3</v>
       </c>
-      <c r="G32">
+      <c r="G33">
         <v>10000</v>
-      </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34">
-        <v>2201</v>
-      </c>
-      <c r="C34" t="s">
-        <v>275</v>
-      </c>
-      <c r="D34" t="s">
-        <v>28</v>
-      </c>
-      <c r="L34" s="4">
-        <v>1</v>
-      </c>
-      <c r="N34">
-        <v>0.15</v>
       </c>
     </row>
     <row r="35" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>275</v>
+      </c>
+      <c r="D35" t="s">
+        <v>28</v>
       </c>
       <c r="L35" s="4">
         <v>1</v>
       </c>
       <c r="N35">
-        <v>0.02</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="36" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="C36" t="s">
-        <v>272</v>
+        <v>22</v>
       </c>
       <c r="L36" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N36">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="37" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="C37" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L37" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N37">
-        <v>0.08</v>
-      </c>
-      <c r="Q37">
-        <v>4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>2211</v>
+        <v>2204</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
+        <v>271</v>
       </c>
       <c r="L38" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N38">
-        <v>0.15</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q38">
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="C39" t="s">
-        <v>273</v>
+        <v>21</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="L39" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N39">
-        <v>0.05</v>
-      </c>
-      <c r="Q39">
-        <v>8</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="40" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="C40" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
       <c r="L40" s="4">
+        <v>4</v>
+      </c>
+      <c r="N40">
+        <v>0.05</v>
+      </c>
+      <c r="Q40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>2213</v>
+      </c>
+      <c r="C41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="L41" s="4">
         <v>5</v>
       </c>
-      <c r="N40">
+      <c r="N41">
         <v>0.3</v>
       </c>
-      <c r="Q40">
+      <c r="Q41">
         <v>18</v>
       </c>
-      <c r="S40">
+      <c r="S41">
         <v>-1</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>2301</v>
-      </c>
-      <c r="C42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D42" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="14">
-        <v>5</v>
-      </c>
-      <c r="N42">
-        <v>3</v>
-      </c>
-      <c r="U42">
-        <v>1</v>
-      </c>
-      <c r="W42" t="s">
-        <v>877</v>
       </c>
     </row>
     <row r="43" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="C43" t="s">
-        <v>806</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
+        <v>37</v>
+      </c>
+      <c r="D43" t="s">
+        <v>30</v>
       </c>
       <c r="L43" s="14">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N43">
-        <v>5</v>
-      </c>
-      <c r="Q43">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="U43">
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B44">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>806</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
-      <c r="L44" s="4">
-        <v>20</v>
+      <c r="L44" s="14">
+        <v>8</v>
       </c>
       <c r="N44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q44">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U44">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W44" t="s">
-        <v>355</v>
+        <v>878</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>2321</v>
+        <v>2312</v>
       </c>
       <c r="C45" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="E45">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L45" s="4">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="N45">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Q45">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U45">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W45" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
-      <c r="L46" s="4" t="s">
-        <v>343</v>
+      <c r="L46" s="4">
+        <v>200</v>
       </c>
       <c r="N46">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q46">
         <v>10</v>
       </c>
       <c r="U46">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W46" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="C47" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E47">
         <v>3</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="N47">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q47">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="U47">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W47" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>2331</v>
+        <v>2323</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E48">
-        <v>4</v>
-      </c>
-      <c r="L48" s="4">
-        <v>1000</v>
+        <v>3</v>
+      </c>
+      <c r="L48" s="4" t="s">
+        <v>345</v>
       </c>
       <c r="N48">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q48">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="U48">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="W48" t="s">
-        <v>350</v>
+        <v>373</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="E49">
         <v>4</v>
       </c>
-      <c r="L49" s="4" t="s">
-        <v>340</v>
+      <c r="L49" s="4">
+        <v>1000</v>
       </c>
       <c r="N49">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q49">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="U49">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W49" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="N50">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q50">
         <v>15</v>
       </c>
       <c r="U50">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W50" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>2341</v>
+        <v>2333</v>
       </c>
       <c r="C51" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="E51">
-        <v>5</v>
-      </c>
-      <c r="L51" s="4">
-        <v>600</v>
+        <v>4</v>
+      </c>
+      <c r="L51" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="N51">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q51">
+        <v>15</v>
+      </c>
+      <c r="U51">
         <v>6</v>
       </c>
-      <c r="S51">
-        <v>-1</v>
-      </c>
-      <c r="U51">
-        <v>1</v>
-      </c>
       <c r="W51" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="C52" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E52">
         <v>5</v>
@@ -14191,241 +14179,244 @@
         <v>600</v>
       </c>
       <c r="N52">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q52">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="S52">
+        <v>-1</v>
       </c>
       <c r="U52">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W52" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="C53" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E53">
         <v>5</v>
       </c>
-      <c r="L53" s="4" t="s">
-        <v>344</v>
+      <c r="L53" s="4">
+        <v>600</v>
       </c>
       <c r="N53">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q53">
         <v>15</v>
       </c>
       <c r="U53">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W53" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="C54" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E54">
         <v>5</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="N54">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q54">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U54">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W54" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E55">
         <v>5</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="N55">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q55">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="U55">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="W55" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2351</v>
+        <v>2345</v>
       </c>
       <c r="C56" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="E56">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="N56">
+        <v>4</v>
+      </c>
+      <c r="Q56">
         <v>10</v>
       </c>
-      <c r="Q56">
-        <v>16</v>
-      </c>
       <c r="U56">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="W56" t="s">
-        <v>358</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="C57" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E57">
         <v>6</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="N57">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q57">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U57">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W57" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E58">
         <v>6</v>
       </c>
-      <c r="L58" s="4">
-        <v>500</v>
+      <c r="L58" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="N58">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q58">
-        <v>25</v>
-      </c>
-      <c r="S58">
-        <v>1</v>
-      </c>
-      <c r="T58">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="U58">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="W58" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="C59" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="E59">
         <v>6</v>
       </c>
-      <c r="L59" s="4" t="s">
-        <v>332</v>
+      <c r="L59" s="4">
+        <v>500</v>
       </c>
       <c r="N59">
         <v>7</v>
       </c>
       <c r="Q59">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="T59">
+        <v>0.1</v>
       </c>
       <c r="U59">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="W59" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="C60" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E60">
         <v>6</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N60">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q60">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U60">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="W60" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2361</v>
+        <v>2355</v>
       </c>
       <c r="C61" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E61">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L61" s="4" t="s">
         <v>334</v>
@@ -14434,247 +14425,247 @@
         <v>11</v>
       </c>
       <c r="Q61">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U61">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="W61" t="s">
-        <v>352</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="E62">
         <v>7</v>
       </c>
-      <c r="L62" s="4">
-        <v>1200</v>
+      <c r="L62" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="N62">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q62">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="U62">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="W62" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="C63" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="E63">
         <v>7</v>
       </c>
-      <c r="L63" s="4" t="s">
-        <v>342</v>
+      <c r="L63" s="4">
+        <v>1200</v>
       </c>
       <c r="N63">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q63">
-        <v>30</v>
-      </c>
-      <c r="S63">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="U63">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="W63" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="N64">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q64">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="S64">
+        <v>-1</v>
       </c>
       <c r="U64">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W64" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2371</v>
+        <v>2364</v>
       </c>
       <c r="C65" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="E65">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>336</v>
+        <v>349</v>
       </c>
       <c r="N65">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q65">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="U65">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="W65" t="s">
-        <v>353</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="C66" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E66">
         <v>8</v>
       </c>
-      <c r="L66" s="4">
-        <v>500</v>
-      </c>
-      <c r="M66">
-        <v>500</v>
+      <c r="L66" s="4" t="s">
+        <v>336</v>
       </c>
       <c r="N66">
-        <v>9</v>
-      </c>
-      <c r="R66">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="Q66">
+        <v>20</v>
       </c>
       <c r="U66">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="W66" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E67">
         <v>8</v>
       </c>
-      <c r="L67" s="4" t="s">
-        <v>339</v>
+      <c r="L67" s="4">
+        <v>500</v>
+      </c>
+      <c r="M67">
+        <v>500</v>
       </c>
       <c r="N67">
-        <v>11</v>
-      </c>
-      <c r="Q67">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="R67">
+        <v>4</v>
       </c>
       <c r="U67">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="W67" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="C68" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="E68">
         <v>8</v>
       </c>
-      <c r="L68" s="4">
-        <v>1000</v>
+      <c r="L68" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="N68">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Q68">
+        <v>22</v>
+      </c>
+      <c r="U68">
         <v>35</v>
       </c>
-      <c r="S68">
-        <v>2</v>
-      </c>
-      <c r="T68">
-        <v>0.15</v>
-      </c>
-      <c r="U68">
-        <v>1</v>
-      </c>
       <c r="W68" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="C69" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E69">
         <v>8</v>
       </c>
-      <c r="L69" s="4" t="s">
-        <v>347</v>
+      <c r="L69" s="4">
+        <v>1000</v>
       </c>
       <c r="N69">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Q69">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="S69">
+        <v>2</v>
+      </c>
+      <c r="T69">
+        <v>0.15</v>
       </c>
       <c r="U69">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W69" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>2381</v>
+        <v>2375</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E70">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="N70">
         <v>12</v>
@@ -14683,705 +14674,717 @@
         <v>20</v>
       </c>
       <c r="U70">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="W70" t="s">
-        <v>351</v>
+        <v>376</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="C71" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="E71">
         <v>9</v>
       </c>
-      <c r="L71" s="4">
-        <v>1000</v>
+      <c r="L71" s="4" t="s">
+        <v>335</v>
       </c>
       <c r="N71">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q71">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="U71">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="W71" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>2391</v>
+        <v>2382</v>
       </c>
       <c r="C72" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="E72">
-        <v>10</v>
-      </c>
-      <c r="L72" s="4" t="s">
-        <v>337</v>
+        <v>9</v>
+      </c>
+      <c r="L72" s="4">
+        <v>1000</v>
       </c>
       <c r="N72">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Q72">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="U72">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="W72" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="C73" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E73">
         <v>10</v>
       </c>
-      <c r="L73" s="4">
+      <c r="L73" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="N73">
+        <v>11</v>
+      </c>
+      <c r="Q73">
+        <v>25</v>
+      </c>
+      <c r="U73">
+        <v>125</v>
+      </c>
+      <c r="W73" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="74" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B74">
+        <v>2392</v>
+      </c>
+      <c r="C74" t="s">
+        <v>142</v>
+      </c>
+      <c r="E74">
+        <v>10</v>
+      </c>
+      <c r="L74" s="4">
         <v>500</v>
       </c>
-      <c r="M73">
+      <c r="M74">
         <v>500</v>
       </c>
-      <c r="N73">
+      <c r="N74">
         <v>9</v>
       </c>
-      <c r="R73">
+      <c r="R74">
         <v>8</v>
       </c>
-      <c r="U73">
+      <c r="U74">
         <v>40</v>
       </c>
-      <c r="W73" t="s">
+      <c r="W74" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="75" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B75">
-        <v>2401</v>
-      </c>
-      <c r="C75" t="s">
-        <v>98</v>
-      </c>
-      <c r="D75" t="s">
-        <v>23</v>
-      </c>
-      <c r="O75">
-        <v>1</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="C76" t="s">
-        <v>167</v>
+        <v>98</v>
+      </c>
+      <c r="D76" t="s">
+        <v>23</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
-      </c>
-      <c r="O77">
-        <v>1</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="O78">
-        <v>2</v>
-      </c>
-      <c r="S78">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>2411</v>
+        <v>2404</v>
       </c>
       <c r="C79" t="s">
-        <v>99</v>
-      </c>
-      <c r="E79">
-        <v>2</v>
+        <v>168</v>
       </c>
       <c r="O79">
         <v>2</v>
       </c>
+      <c r="S79">
+        <v>-1</v>
+      </c>
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>2421</v>
+        <v>2411</v>
       </c>
       <c r="C80" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O80">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>2431</v>
+        <v>2421</v>
       </c>
       <c r="C81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O81">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>2441</v>
+        <v>2431</v>
       </c>
       <c r="C82" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O82">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83">
-        <v>2451</v>
+        <v>2441</v>
       </c>
       <c r="C83" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E83">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O83">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>2461</v>
+        <v>2451</v>
       </c>
       <c r="C84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E84">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O84">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85">
-        <v>2471</v>
+        <v>2461</v>
       </c>
       <c r="C85" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E85">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O85">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>2481</v>
+        <v>2471</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E86">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O86">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87">
+        <v>2481</v>
+      </c>
+      <c r="C87" t="s">
+        <v>106</v>
+      </c>
+      <c r="E87">
+        <v>9</v>
+      </c>
+      <c r="O87">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B88">
         <v>2491</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>107</v>
       </c>
-      <c r="E87">
+      <c r="E88">
         <v>10</v>
       </c>
-      <c r="O87">
+      <c r="O88">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B89">
-        <v>2501</v>
-      </c>
-      <c r="C89" t="s">
-        <v>864</v>
-      </c>
-      <c r="D89" t="s">
-        <v>24</v>
-      </c>
-      <c r="O89">
-        <v>1</v>
       </c>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="C90" t="s">
-        <v>170</v>
-      </c>
-      <c r="N90">
-        <v>0.04</v>
+        <v>864</v>
+      </c>
+      <c r="D90" t="s">
+        <v>24</v>
+      </c>
+      <c r="O90">
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="C91" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N91">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="C92" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N92">
-        <v>0.04</v>
-      </c>
-      <c r="O92">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2511</v>
+        <v>2504</v>
       </c>
       <c r="C93" t="s">
-        <v>865</v>
-      </c>
-      <c r="E93">
-        <v>2</v>
+        <v>172</v>
+      </c>
+      <c r="N93">
+        <v>0.04</v>
       </c>
       <c r="O93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="C94" t="s">
-        <v>180</v>
+        <v>865</v>
       </c>
       <c r="E94">
         <v>2</v>
       </c>
-      <c r="K94">
-        <v>3</v>
-      </c>
-      <c r="N94">
-        <v>0.06</v>
-      </c>
       <c r="O94">
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="C95" t="s">
-        <v>305</v>
+        <v>180</v>
+      </c>
+      <c r="E95">
+        <v>2</v>
+      </c>
+      <c r="K95">
+        <v>3</v>
       </c>
       <c r="N95">
-        <v>0.04</v>
+        <v>0.06</v>
+      </c>
+      <c r="O95">
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2521</v>
+        <v>2513</v>
       </c>
       <c r="C96" t="s">
-        <v>866</v>
-      </c>
-      <c r="E96">
-        <v>3</v>
-      </c>
-      <c r="O96">
-        <v>14</v>
+        <v>305</v>
+      </c>
+      <c r="N96">
+        <v>0.04</v>
       </c>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>2531</v>
+        <v>2521</v>
       </c>
       <c r="C97" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O97">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="C98" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="E98">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O98">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>2551</v>
+        <v>2541</v>
       </c>
       <c r="C99" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="E99">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O99">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2561</v>
+        <v>2551</v>
       </c>
       <c r="C100" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="E100">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O100">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2571</v>
+        <v>2561</v>
       </c>
       <c r="C101" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E101">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O101">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2581</v>
+        <v>2571</v>
       </c>
       <c r="C102" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="E102">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O102">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103">
+        <v>2581</v>
+      </c>
+      <c r="C103" t="s">
+        <v>873</v>
+      </c>
+      <c r="E103">
+        <v>9</v>
+      </c>
+      <c r="O103">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B104">
         <v>2591</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C104" t="s">
         <v>872</v>
       </c>
-      <c r="E103">
+      <c r="E104">
         <v>10</v>
       </c>
-      <c r="O103">
+      <c r="O104">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B105">
-        <v>2601</v>
-      </c>
-      <c r="C105" t="s">
-        <v>108</v>
-      </c>
-      <c r="D105" t="s">
-        <v>25</v>
-      </c>
-      <c r="O105">
-        <v>1</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="C106" t="s">
-        <v>173</v>
-      </c>
-      <c r="N106">
-        <v>0.02</v>
+        <v>108</v>
+      </c>
+      <c r="D106" t="s">
+        <v>25</v>
+      </c>
+      <c r="O106">
+        <v>1</v>
       </c>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="C107" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="N107">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C108" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="N108">
-        <v>0.08</v>
-      </c>
-      <c r="O108">
-        <v>1</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2611</v>
+        <v>2604</v>
       </c>
       <c r="C109" t="s">
-        <v>109</v>
-      </c>
-      <c r="E109">
-        <v>2</v>
+        <v>174</v>
+      </c>
+      <c r="N109">
+        <v>0.08</v>
       </c>
       <c r="O109">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2621</v>
+        <v>2611</v>
       </c>
       <c r="C110" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E110">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O110">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2631</v>
+        <v>2621</v>
       </c>
       <c r="C111" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E111">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O111">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>2641</v>
+        <v>2631</v>
       </c>
       <c r="C112" t="s">
-        <v>800</v>
+        <v>111</v>
       </c>
       <c r="E112">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O112">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="113" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B113">
-        <v>2651</v>
+        <v>2641</v>
       </c>
       <c r="C113" t="s">
-        <v>112</v>
+        <v>800</v>
       </c>
       <c r="E113">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O113">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="114" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2661</v>
+        <v>2651</v>
       </c>
       <c r="C114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E114">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O114">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="115" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>2671</v>
+        <v>2661</v>
       </c>
       <c r="C115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E115">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O115">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="116" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>2681</v>
+        <v>2671</v>
       </c>
       <c r="C116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E116">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O116">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117">
+        <v>2681</v>
+      </c>
+      <c r="C117" t="s">
+        <v>115</v>
+      </c>
+      <c r="E117">
+        <v>9</v>
+      </c>
+      <c r="O117">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B118">
         <v>2691</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C118" t="s">
         <v>116</v>
       </c>
-      <c r="E117">
+      <c r="E118">
         <v>10</v>
       </c>
-      <c r="O117">
+      <c r="O118">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B119">
-        <v>2701</v>
-      </c>
-      <c r="C119" t="s">
-        <v>117</v>
-      </c>
-      <c r="D119" t="s">
-        <v>26</v>
-      </c>
-      <c r="O119">
-        <v>1</v>
       </c>
     </row>
     <row r="120" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="C120" t="s">
-        <v>176</v>
+        <v>117</v>
+      </c>
+      <c r="D120" t="s">
+        <v>26</v>
+      </c>
+      <c r="O120">
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="C121" t="s">
-        <v>177</v>
-      </c>
-      <c r="S121">
-        <v>1</v>
+        <v>176</v>
       </c>
     </row>
     <row r="122" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="C122" t="s">
-        <v>178</v>
-      </c>
-      <c r="O122">
+        <v>177</v>
+      </c>
+      <c r="S122">
         <v>1</v>
-      </c>
-      <c r="S122">
-        <v>2</v>
       </c>
     </row>
     <row r="123" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="C123" t="s">
-        <v>306</v>
+        <v>178</v>
       </c>
       <c r="O123">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S123">
         <v>2</v>
@@ -15389,611 +15392,614 @@
     </row>
     <row r="124" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2711</v>
+        <v>2705</v>
       </c>
       <c r="C124" t="s">
-        <v>118</v>
-      </c>
-      <c r="E124">
-        <v>2</v>
+        <v>306</v>
       </c>
       <c r="O124">
         <v>2</v>
       </c>
+      <c r="S124">
+        <v>2</v>
+      </c>
     </row>
     <row r="125" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="C125" t="s">
-        <v>179</v>
+        <v>118</v>
       </c>
       <c r="E125">
         <v>2</v>
       </c>
       <c r="O125">
-        <v>1</v>
-      </c>
-      <c r="S125">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="C126" t="s">
-        <v>307</v>
+        <v>179</v>
       </c>
       <c r="E126">
         <v>2</v>
       </c>
-      <c r="L126" s="4">
+      <c r="O126">
         <v>1</v>
       </c>
-      <c r="O126">
+      <c r="S126">
         <v>3</v>
-      </c>
-      <c r="S126">
-        <v>2</v>
       </c>
     </row>
     <row r="127" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B127">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="C127" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E127">
         <v>2</v>
       </c>
+      <c r="L127" s="4">
+        <v>1</v>
+      </c>
       <c r="O127">
+        <v>3</v>
+      </c>
+      <c r="S127">
         <v>2</v>
-      </c>
-      <c r="S127">
-        <v>3</v>
       </c>
     </row>
     <row r="128" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2721</v>
+        <v>2714</v>
       </c>
       <c r="C128" t="s">
-        <v>119</v>
+        <v>308</v>
       </c>
       <c r="E128">
+        <v>2</v>
+      </c>
+      <c r="O128">
+        <v>2</v>
+      </c>
+      <c r="S128">
         <v>3</v>
-      </c>
-      <c r="O128">
-        <v>14</v>
       </c>
     </row>
     <row r="129" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>2731</v>
+        <v>2721</v>
       </c>
       <c r="C129" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E129">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O129">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2741</v>
+        <v>2731</v>
       </c>
       <c r="C130" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E130">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O130">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="131" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2751</v>
+        <v>2741</v>
       </c>
       <c r="C131" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E131">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O131">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="132" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2761</v>
+        <v>2751</v>
       </c>
       <c r="C132" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E132">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O132">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="133" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2771</v>
+        <v>2761</v>
       </c>
       <c r="C133" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E133">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O133">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="134" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2781</v>
+        <v>2771</v>
       </c>
       <c r="C134" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E134">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O134">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="135" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B135">
+        <v>2781</v>
+      </c>
+      <c r="C135" t="s">
+        <v>125</v>
+      </c>
+      <c r="E135">
+        <v>9</v>
+      </c>
+      <c r="O135">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="136" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B136">
         <v>2791</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C136" t="s">
         <v>126</v>
       </c>
-      <c r="E135">
+      <c r="E136">
         <v>10</v>
       </c>
-      <c r="O135">
+      <c r="O136">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="137" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B137">
-        <v>2801</v>
-      </c>
-      <c r="C137" t="s">
-        <v>833</v>
-      </c>
-      <c r="D137" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="138" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="C138" t="s">
-        <v>834</v>
+        <v>833</v>
+      </c>
+      <c r="D138" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="139" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="C139" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="140" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="C140" t="s">
-        <v>827</v>
+        <v>835</v>
       </c>
     </row>
     <row r="141" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="C141" t="s">
-        <v>807</v>
+        <v>827</v>
       </c>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="C142" t="s">
-        <v>303</v>
+        <v>807</v>
       </c>
     </row>
     <row r="143" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>2807</v>
+        <v>2806</v>
+      </c>
+      <c r="C143" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="144" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2808</v>
+        <v>2807</v>
       </c>
     </row>
     <row r="145" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>2809</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="146" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>2810</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="147" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B147">
-        <v>2811</v>
-      </c>
-      <c r="C147" t="s">
-        <v>836</v>
-      </c>
-      <c r="E147">
-        <v>2</v>
+        <v>2810</v>
       </c>
     </row>
     <row r="148" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="C148" t="s">
-        <v>837</v>
+        <v>836</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="C149" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="150" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="C150" t="s">
-        <v>861</v>
+        <v>838</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="C151" t="s">
-        <v>304</v>
+        <v>861</v>
       </c>
     </row>
     <row r="152" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>2821</v>
+        <v>2815</v>
       </c>
       <c r="C152" t="s">
-        <v>839</v>
-      </c>
-      <c r="E152">
-        <v>3</v>
+        <v>304</v>
       </c>
     </row>
     <row r="153" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="C153" t="s">
-        <v>840</v>
+        <v>839</v>
+      </c>
+      <c r="E153">
+        <v>3</v>
       </c>
     </row>
     <row r="154" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="C154" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="155" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>2834</v>
+        <v>2823</v>
       </c>
       <c r="C155" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
     </row>
     <row r="156" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>2825</v>
+        <v>2834</v>
       </c>
       <c r="C156" t="s">
-        <v>573</v>
-      </c>
-      <c r="Y156" t="s">
-        <v>202</v>
+        <v>841</v>
       </c>
     </row>
     <row r="157" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>2831</v>
+        <v>2825</v>
       </c>
       <c r="C157" t="s">
-        <v>843</v>
-      </c>
-      <c r="E157">
-        <v>4</v>
+        <v>573</v>
+      </c>
+      <c r="Y157" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="158" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="C158" t="s">
-        <v>844</v>
+        <v>843</v>
+      </c>
+      <c r="E158">
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2841</v>
+        <v>2832</v>
       </c>
       <c r="C159" t="s">
-        <v>846</v>
-      </c>
-      <c r="E159">
-        <v>5</v>
+        <v>844</v>
       </c>
     </row>
     <row r="160" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="C160" t="s">
-        <v>845</v>
+        <v>846</v>
+      </c>
+      <c r="E160">
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2851</v>
+        <v>2842</v>
       </c>
       <c r="C161" t="s">
-        <v>847</v>
-      </c>
-      <c r="E161">
-        <v>6</v>
+        <v>845</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="C162" t="s">
-        <v>853</v>
+        <v>847</v>
+      </c>
+      <c r="E162">
+        <v>6</v>
       </c>
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="C163" t="s">
-        <v>848</v>
+        <v>853</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2861</v>
+        <v>2853</v>
       </c>
       <c r="C164" t="s">
-        <v>849</v>
-      </c>
-      <c r="E164">
-        <v>7</v>
+        <v>848</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="C165" t="s">
-        <v>854</v>
+        <v>849</v>
+      </c>
+      <c r="E165">
+        <v>7</v>
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="C166" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="C167" t="s">
-        <v>302</v>
+        <v>855</v>
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2871</v>
+        <v>2864</v>
       </c>
       <c r="C168" t="s">
-        <v>850</v>
-      </c>
-      <c r="E168">
-        <v>8</v>
+        <v>302</v>
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C169" t="s">
-        <v>858</v>
+        <v>850</v>
+      </c>
+      <c r="E169">
+        <v>8</v>
       </c>
     </row>
     <row r="170" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="C170" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2881</v>
+        <v>2873</v>
       </c>
       <c r="C171" t="s">
-        <v>851</v>
-      </c>
-      <c r="E171">
-        <v>9</v>
+        <v>862</v>
       </c>
     </row>
     <row r="172" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="C172" t="s">
-        <v>860</v>
+        <v>851</v>
+      </c>
+      <c r="E172">
+        <v>9</v>
       </c>
     </row>
     <row r="173" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="C173" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2891</v>
+        <v>2883</v>
       </c>
       <c r="C174" t="s">
-        <v>852</v>
-      </c>
-      <c r="E174">
-        <v>10</v>
+        <v>863</v>
       </c>
     </row>
     <row r="175" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B175">
+        <v>2891</v>
+      </c>
+      <c r="C175" t="s">
+        <v>852</v>
+      </c>
+      <c r="E175">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B176">
         <v>2892</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C176" t="s">
         <v>136</v>
-      </c>
-    </row>
-    <row r="177" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B177">
-        <v>2901</v>
-      </c>
-      <c r="C177" t="s">
-        <v>252</v>
-      </c>
-      <c r="D177" t="s">
-        <v>252</v>
-      </c>
-      <c r="W177" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="178" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B178">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="C178" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D178" t="s">
         <v>252</v>
       </c>
-      <c r="E178">
-        <v>2</v>
-      </c>
       <c r="W178" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="179" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="C179" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D179" t="s">
         <v>252</v>
       </c>
       <c r="E179">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W179" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="180" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2911</v>
+        <v>2903</v>
       </c>
       <c r="C180" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D180" t="s">
-        <v>258</v>
-      </c>
-      <c r="H180" s="7"/>
-      <c r="L180" s="4">
-        <v>1</v>
+        <v>252</v>
+      </c>
+      <c r="E180">
+        <v>3</v>
+      </c>
+      <c r="W180" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="181" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B181">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="C181" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D181" t="s">
         <v>258</v>
       </c>
+      <c r="H181" s="7"/>
       <c r="L181" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="182" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="C182" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D182" t="s">
         <v>258</v>
       </c>
+      <c r="L182" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="183" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="C183" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D183" t="s">
         <v>258</v>
@@ -16001,35 +16007,35 @@
     </row>
     <row r="184" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="C184" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D184" t="s">
         <v>258</v>
       </c>
-      <c r="L184" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="185" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B185">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="C185" t="s">
-        <v>293</v>
+        <v>263</v>
       </c>
       <c r="D185" t="s">
         <v>258</v>
       </c>
+      <c r="L185" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="186" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="C186" t="s">
-        <v>797</v>
+        <v>293</v>
       </c>
       <c r="D186" t="s">
         <v>258</v>
@@ -16037,187 +16043,178 @@
     </row>
     <row r="187" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B187">
-        <v>2921</v>
+        <v>2917</v>
       </c>
       <c r="C187" t="s">
-        <v>265</v>
+        <v>797</v>
       </c>
       <c r="D187" t="s">
-        <v>264</v>
-      </c>
-      <c r="N187">
-        <v>0.04</v>
-      </c>
-      <c r="W187" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="C188" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D188" t="s">
         <v>264</v>
       </c>
-      <c r="E188">
-        <v>2</v>
-      </c>
       <c r="N188">
         <v>0.04</v>
       </c>
       <c r="W188" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="189" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="C189" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D189" t="s">
         <v>264</v>
       </c>
+      <c r="E189">
+        <v>2</v>
+      </c>
       <c r="N189">
         <v>0.04</v>
       </c>
       <c r="W189" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="190" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="C190" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="D190" t="s">
         <v>264</v>
       </c>
-      <c r="L190" s="4">
-        <v>1</v>
-      </c>
       <c r="N190">
-        <v>2.5</v>
-      </c>
-      <c r="Q190">
-        <v>6</v>
+        <v>0.04</v>
       </c>
       <c r="W190" t="s">
-        <v>301</v>
+        <v>268</v>
       </c>
     </row>
     <row r="191" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="C191" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D191" t="s">
         <v>264</v>
       </c>
+      <c r="L191" s="4">
+        <v>1</v>
+      </c>
+      <c r="N191">
+        <v>2.5</v>
+      </c>
+      <c r="Q191">
+        <v>6</v>
+      </c>
       <c r="W191" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="192" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="C192" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D192" t="s">
         <v>264</v>
       </c>
-      <c r="E192">
-        <v>2</v>
-      </c>
-      <c r="L192" s="4">
-        <v>1</v>
-      </c>
-      <c r="N192">
-        <v>0.02</v>
-      </c>
       <c r="W192" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="193" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="C193" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D193" t="s">
         <v>264</v>
       </c>
       <c r="E193">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L193" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N193">
         <v>0.02</v>
       </c>
       <c r="W193" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="194" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2931</v>
+        <v>2927</v>
       </c>
       <c r="C194" t="s">
-        <v>239</v>
+        <v>297</v>
       </c>
       <c r="D194" t="s">
-        <v>281</v>
+        <v>264</v>
+      </c>
+      <c r="E194">
+        <v>3</v>
       </c>
       <c r="L194" s="4">
         <v>2</v>
       </c>
       <c r="N194">
-        <v>2.5</v>
+        <v>0.02</v>
       </c>
       <c r="W194" t="s">
-        <v>876</v>
+        <v>300</v>
       </c>
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="C195" t="s">
-        <v>282</v>
+        <v>239</v>
       </c>
       <c r="D195" t="s">
         <v>281</v>
       </c>
       <c r="L195" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N195">
         <v>2.5</v>
       </c>
-      <c r="Q195">
-        <v>4</v>
+      <c r="W195" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="196" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="C196" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D196" t="s">
         <v>281</v>
@@ -16226,43 +16223,49 @@
         <v>1</v>
       </c>
       <c r="N196">
-        <v>2</v>
-      </c>
-      <c r="W196" t="s">
-        <v>876</v>
+        <v>2.5</v>
+      </c>
+      <c r="Q196">
+        <v>4</v>
       </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2941</v>
+        <v>2933</v>
       </c>
       <c r="C197" t="s">
-        <v>382</v>
+        <v>286</v>
       </c>
       <c r="D197" t="s">
         <v>281</v>
       </c>
+      <c r="L197" s="4">
+        <v>1</v>
+      </c>
+      <c r="N197">
+        <v>2</v>
+      </c>
+      <c r="W197" t="s">
+        <v>876</v>
+      </c>
     </row>
     <row r="198" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="C198" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D198" t="s">
         <v>281</v>
       </c>
-      <c r="E198">
-        <v>2</v>
-      </c>
     </row>
     <row r="199" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="C199" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D199" t="s">
         <v>281</v>
@@ -16273,10 +16276,10 @@
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="C200" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D200" t="s">
         <v>281</v>
@@ -16284,19 +16287,13 @@
       <c r="E200">
         <v>2</v>
       </c>
-      <c r="L200" s="4">
-        <v>3</v>
-      </c>
-      <c r="N200">
-        <v>3</v>
-      </c>
     </row>
     <row r="201" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="C201" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D201" t="s">
         <v>281</v>
@@ -16304,13 +16301,19 @@
       <c r="E201">
         <v>2</v>
       </c>
+      <c r="L201" s="4">
+        <v>3</v>
+      </c>
+      <c r="N201">
+        <v>3</v>
+      </c>
     </row>
     <row r="202" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="C202" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D202" t="s">
         <v>281</v>
@@ -16321,10 +16324,10 @@
     </row>
     <row r="203" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="C203" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D203" t="s">
         <v>281</v>
@@ -16335,10 +16338,10 @@
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="C204" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D204" t="s">
         <v>281</v>
@@ -16349,21 +16352,24 @@
     </row>
     <row r="205" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2961</v>
+        <v>2948</v>
       </c>
       <c r="C205" t="s">
-        <v>287</v>
+        <v>389</v>
       </c>
       <c r="D205" t="s">
-        <v>289</v>
+        <v>281</v>
+      </c>
+      <c r="E205">
+        <v>2</v>
       </c>
     </row>
     <row r="206" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="C206" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D206" t="s">
         <v>289</v>
@@ -16371,58 +16377,52 @@
     </row>
     <row r="207" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="C207" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="D207" t="s">
         <v>289</v>
       </c>
-      <c r="L207" s="4">
-        <v>1</v>
-      </c>
-      <c r="N207">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="208" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="C208" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="D208" t="s">
         <v>289</v>
       </c>
+      <c r="L208" s="4">
+        <v>1</v>
+      </c>
       <c r="N208">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="209" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="C209" t="s">
-        <v>908</v>
+        <v>324</v>
       </c>
       <c r="D209" t="s">
         <v>289</v>
       </c>
-      <c r="L209" s="4">
-        <v>1</v>
-      </c>
       <c r="N209">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="210" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B210">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="C210" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D210" t="s">
         <v>289</v>
@@ -16436,10 +16436,10 @@
     </row>
     <row r="211" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B211">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="C211" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D211" t="s">
         <v>289</v>
@@ -16453,10 +16453,10 @@
     </row>
     <row r="212" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="C212" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D212" t="s">
         <v>289</v>
@@ -16470,38 +16470,38 @@
     </row>
     <row r="213" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2971</v>
+        <v>2968</v>
       </c>
       <c r="C213" t="s">
-        <v>314</v>
+        <v>911</v>
       </c>
       <c r="D213" t="s">
-        <v>309</v>
+        <v>289</v>
+      </c>
+      <c r="L213" s="4">
+        <v>1</v>
+      </c>
+      <c r="N213">
+        <v>0.05</v>
       </c>
     </row>
     <row r="214" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="C214" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D214" t="s">
         <v>309</v>
       </c>
-      <c r="L214" s="4">
-        <v>1</v>
-      </c>
-      <c r="N214">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="215" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="C215" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="D215" t="s">
         <v>309</v>
@@ -16515,27 +16515,27 @@
     </row>
     <row r="216" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B216">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="C216" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="D216" t="s">
         <v>309</v>
       </c>
-      <c r="E216">
-        <v>2</v>
+      <c r="L216" s="4">
+        <v>1</v>
       </c>
       <c r="N216">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="217" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B217">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="C217" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D217" t="s">
         <v>309</v>
@@ -16543,19 +16543,16 @@
       <c r="E217">
         <v>2</v>
       </c>
-      <c r="L217" s="4">
-        <v>2</v>
-      </c>
       <c r="N217">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="218" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B218">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="C218" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="D218" t="s">
         <v>309</v>
@@ -16564,38 +16561,35 @@
         <v>2</v>
       </c>
       <c r="L218" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N218">
+        <v>0.02</v>
       </c>
     </row>
     <row r="219" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B219">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="C219" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D219" t="s">
         <v>309</v>
       </c>
       <c r="E219">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L219" s="4">
-        <v>3</v>
-      </c>
-      <c r="N219">
-        <v>0.08</v>
-      </c>
-      <c r="Q219">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="220" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B220">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="C220" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D220" t="s">
         <v>309</v>
@@ -16604,18 +16598,21 @@
         <v>3</v>
       </c>
       <c r="L220" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N220">
-        <v>0.1</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q220">
+        <v>15</v>
       </c>
     </row>
     <row r="221" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B221">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="C221" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D221" t="s">
         <v>309</v>
@@ -16627,35 +16624,38 @@
         <v>2</v>
       </c>
       <c r="N221">
-        <v>0.05</v>
-      </c>
-      <c r="Q221">
-        <v>5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="222" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="C222" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D222" t="s">
         <v>309</v>
       </c>
       <c r="E222">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L222" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N222">
+        <v>0.05</v>
+      </c>
+      <c r="Q222">
+        <v>5</v>
       </c>
     </row>
     <row r="223" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="C223" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="D223" t="s">
         <v>309</v>
@@ -16669,10 +16669,10 @@
     </row>
     <row r="224" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="C224" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D224" t="s">
         <v>309</v>
@@ -16686,30 +16686,43 @@
     </row>
     <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="C225" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D225" t="s">
         <v>309</v>
       </c>
       <c r="E225">
+        <v>4</v>
+      </c>
+      <c r="L225" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B226">
+        <v>2983</v>
+      </c>
+      <c r="C226" t="s">
+        <v>319</v>
+      </c>
+      <c r="D226" t="s">
+        <v>309</v>
+      </c>
+      <c r="E226">
         <v>5</v>
       </c>
-      <c r="L225" s="4">
+      <c r="L226" s="4">
         <v>5</v>
       </c>
-      <c r="N225">
+      <c r="N226">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="Q225">
+      <c r="Q226">
         <v>20</v>
       </c>
-    </row>
-    <row r="226" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K226" s="4"/>
-      <c r="L226"/>
     </row>
     <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K227" s="4"/>
@@ -16718,6 +16731,10 @@
     <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K228" s="4"/>
       <c r="L228"/>
+    </row>
+    <row r="229" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K229" s="4"/>
+      <c r="L229"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
v0.6.6: KhalilForm / QuizmoForm outlines
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B573439-FDBD-44C2-9C11-994D6C0522A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7A7035-00D7-4887-AC95-A459CFDC8A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -10904,8 +10904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10969,7 +10969,7 @@
       <c r="B6" s="4">
         <v>11</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="18" t="s">
         <v>201</v>
       </c>
       <c r="D6" t="s">
@@ -10986,7 +10986,7 @@
       <c r="B7" s="4">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="18" t="s">
         <v>202</v>
       </c>
       <c r="E7">
@@ -13293,11 +13293,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D156" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I19" sqref="I19"/>
+      <selection pane="bottomRight" activeCell="C191" sqref="C191:C194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.6s: Gun stat functions
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314518E7-A252-44EA-A782-D66EF9F1F179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32F32C-B81C-4F8A-9F98-11E8FC79704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -1097,9 +1097,6 @@
   </si>
   <si>
     <t>4200-540</t>
-  </si>
-  <si>
-    <t>dur=20, cd=200, rec=0.1, inac=0.08, 1200-75 splash damage</t>
   </si>
   <si>
     <t>dur=8, cd=80, rec=0.02, inac=0.08, automatic</t>
@@ -3238,6 +3235,9 @@
   </si>
   <si>
     <t>Peanuts</t>
+  </si>
+  <si>
+    <t>dur=20, cd=200, rec=0.08, inac=0.08, 1200-75 splash damage</t>
   </si>
 </sst>
 </file>
@@ -3698,7 +3698,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -3710,10 +3710,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E4">
         <v>100</v>
@@ -3735,7 +3735,7 @@
         <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D6" t="s">
         <v>205</v>
@@ -3749,7 +3749,7 @@
         <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3757,7 +3757,7 @@
         <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3765,7 +3765,7 @@
         <v>104</v>
       </c>
       <c r="C9" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3773,7 +3773,7 @@
         <v>111</v>
       </c>
       <c r="C10" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3781,7 +3781,7 @@
         <v>112</v>
       </c>
       <c r="C11" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3789,7 +3789,7 @@
         <v>113</v>
       </c>
       <c r="C12" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3797,7 +3797,7 @@
         <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3805,7 +3805,7 @@
         <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3813,7 +3813,7 @@
         <v>123</v>
       </c>
       <c r="C15" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3829,7 +3829,7 @@
         <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
@@ -3837,7 +3837,7 @@
         <v>133</v>
       </c>
       <c r="C18" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -3845,7 +3845,7 @@
         <v>134</v>
       </c>
       <c r="C19" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -3853,7 +3853,7 @@
         <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -3861,7 +3861,7 @@
         <v>142</v>
       </c>
       <c r="C21" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -3869,7 +3869,7 @@
         <v>143</v>
       </c>
       <c r="C22" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -3877,7 +3877,7 @@
         <v>144</v>
       </c>
       <c r="C23" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -3885,7 +3885,7 @@
         <v>145</v>
       </c>
       <c r="C24" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -3893,7 +3893,7 @@
         <v>151</v>
       </c>
       <c r="C25" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -3901,7 +3901,7 @@
         <v>152</v>
       </c>
       <c r="C26" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -3909,7 +3909,7 @@
         <v>153</v>
       </c>
       <c r="C27" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -3917,7 +3917,7 @@
         <v>154</v>
       </c>
       <c r="C28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -3925,7 +3925,7 @@
         <v>155</v>
       </c>
       <c r="C29" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -3933,7 +3933,7 @@
         <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -3941,7 +3941,7 @@
         <v>161</v>
       </c>
       <c r="C31" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -3949,7 +3949,7 @@
         <v>162</v>
       </c>
       <c r="C32" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -3957,7 +3957,7 @@
         <v>163</v>
       </c>
       <c r="C33" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
@@ -3965,7 +3965,7 @@
         <v>171</v>
       </c>
       <c r="C34" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
@@ -3973,7 +3973,7 @@
         <v>172</v>
       </c>
       <c r="C35" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
@@ -3981,7 +3981,7 @@
         <v>173</v>
       </c>
       <c r="C36" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
@@ -3989,7 +3989,7 @@
         <v>174</v>
       </c>
       <c r="C37" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
@@ -3997,7 +3997,7 @@
         <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
@@ -4013,7 +4013,7 @@
         <v>177</v>
       </c>
       <c r="C40" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
@@ -4021,7 +4021,7 @@
         <v>178</v>
       </c>
       <c r="C41" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
@@ -4029,7 +4029,7 @@
         <v>179</v>
       </c>
       <c r="C42" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
@@ -4037,7 +4037,7 @@
         <v>181</v>
       </c>
       <c r="C43" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
@@ -4045,7 +4045,7 @@
         <v>182</v>
       </c>
       <c r="C44" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
@@ -4053,7 +4053,7 @@
         <v>183</v>
       </c>
       <c r="C45" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
@@ -4061,7 +4061,7 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
@@ -4069,7 +4069,7 @@
         <v>185</v>
       </c>
       <c r="C47" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -4077,7 +4077,7 @@
         <v>201</v>
       </c>
       <c r="C49" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D49" t="s">
         <v>208</v>
@@ -4091,7 +4091,7 @@
         <v>202</v>
       </c>
       <c r="C50" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
@@ -4099,7 +4099,7 @@
         <v>203</v>
       </c>
       <c r="C51" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -4107,7 +4107,7 @@
         <v>204</v>
       </c>
       <c r="C52" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
@@ -4115,7 +4115,7 @@
         <v>205</v>
       </c>
       <c r="C53" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
@@ -4123,7 +4123,7 @@
         <v>206</v>
       </c>
       <c r="C54" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
@@ -4131,7 +4131,7 @@
         <v>207</v>
       </c>
       <c r="C55" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
@@ -4139,7 +4139,7 @@
         <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
@@ -4147,7 +4147,7 @@
         <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
@@ -4155,7 +4155,7 @@
         <v>213</v>
       </c>
       <c r="C58" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
@@ -4166,13 +4166,13 @@
         <v>301</v>
       </c>
       <c r="C60" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D60" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E60" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
@@ -4180,7 +4180,7 @@
         <v>302</v>
       </c>
       <c r="C61" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
@@ -4188,7 +4188,7 @@
         <v>303</v>
       </c>
       <c r="C62" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.25">
@@ -4196,7 +4196,7 @@
         <v>304</v>
       </c>
       <c r="C63" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.25">
@@ -4204,7 +4204,7 @@
         <v>305</v>
       </c>
       <c r="C64" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>306</v>
       </c>
       <c r="C65" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -4220,7 +4220,7 @@
         <v>307</v>
       </c>
       <c r="C66" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
@@ -4228,7 +4228,7 @@
         <v>308</v>
       </c>
       <c r="C67" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
@@ -4236,7 +4236,7 @@
         <v>309</v>
       </c>
       <c r="C68" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
@@ -4244,7 +4244,7 @@
         <v>310</v>
       </c>
       <c r="C69" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
@@ -4252,7 +4252,7 @@
         <v>311</v>
       </c>
       <c r="C70" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
@@ -4260,7 +4260,7 @@
         <v>312</v>
       </c>
       <c r="C71" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -4268,7 +4268,7 @@
         <v>313</v>
       </c>
       <c r="C72" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
@@ -4276,7 +4276,7 @@
         <v>314</v>
       </c>
       <c r="C73" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -4284,7 +4284,7 @@
         <v>315</v>
       </c>
       <c r="C74" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
@@ -4292,7 +4292,7 @@
         <v>316</v>
       </c>
       <c r="C75" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
@@ -4300,7 +4300,7 @@
         <v>317</v>
       </c>
       <c r="C76" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
@@ -4308,7 +4308,7 @@
         <v>318</v>
       </c>
       <c r="C77" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
@@ -4316,7 +4316,7 @@
         <v>319</v>
       </c>
       <c r="C78" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
@@ -4324,7 +4324,7 @@
         <v>320</v>
       </c>
       <c r="C79" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
@@ -4332,7 +4332,7 @@
         <v>321</v>
       </c>
       <c r="C80" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
@@ -4340,7 +4340,7 @@
         <v>322</v>
       </c>
       <c r="C81" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
@@ -4348,7 +4348,7 @@
         <v>323</v>
       </c>
       <c r="C82" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
@@ -4356,7 +4356,7 @@
         <v>324</v>
       </c>
       <c r="C83" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I4" s="1">
         <v>1.4</v>
@@ -4509,7 +4509,7 @@
         <v>2.5</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="I6" s="1">
         <v>3</v>
@@ -10242,7 +10242,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10253,393 +10253,393 @@
         <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="22"/>
       <c r="C5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G5" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="22"/>
       <c r="C6" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D6" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="22"/>
       <c r="C7" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D7" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G7" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D8" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="G8" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="C9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
       <c r="C10" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D10" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G10" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D11" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G11" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
       <c r="C12" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D12" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
       <c r="C13" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D13" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="G13" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C15" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D15" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="22"/>
       <c r="C16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="22"/>
       <c r="C17" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D17" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
       <c r="C18" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="22"/>
       <c r="C19" t="s">
+        <v>624</v>
+      </c>
+      <c r="D19" t="s">
         <v>625</v>
-      </c>
-      <c r="D19" t="s">
-        <v>626</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="22"/>
       <c r="C20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D20" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="22"/>
       <c r="C21" t="s">
+        <v>616</v>
+      </c>
+      <c r="D21" t="s">
         <v>617</v>
-      </c>
-      <c r="D21" t="s">
-        <v>618</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G21" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="22"/>
       <c r="C22" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" s="22"/>
       <c r="C23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="22"/>
       <c r="C24" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D24" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G26" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G27" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="D31" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>797</v>
+      </c>
+      <c r="G32" t="s">
         <v>798</v>
-      </c>
-      <c r="G32" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G33" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G34" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
   </sheetData>
@@ -10777,10 +10777,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>210</v>
@@ -10791,13 +10791,13 @@
         <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="E3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10805,13 +10805,13 @@
         <v>128</v>
       </c>
       <c r="C4" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D4" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="E4" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10819,13 +10819,13 @@
         <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="E5" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10833,7 +10833,7 @@
         <v>130</v>
       </c>
       <c r="D6" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="18.75" x14ac:dyDescent="0.35">
@@ -10841,7 +10841,7 @@
         <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="E7" s="12"/>
     </row>
@@ -10850,7 +10850,7 @@
         <v>132</v>
       </c>
       <c r="D8" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10858,10 +10858,10 @@
         <v>133</v>
       </c>
       <c r="D9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E9" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="18.75" x14ac:dyDescent="0.35">
@@ -10869,10 +10869,10 @@
         <v>134</v>
       </c>
       <c r="D10" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E10" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="18" x14ac:dyDescent="0.35">
@@ -10880,10 +10880,10 @@
         <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E11" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -10891,7 +10891,7 @@
         <v>136</v>
       </c>
       <c r="D12" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
   </sheetData>
@@ -10920,7 +10920,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="16"/>
@@ -10936,7 +10936,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>209</v>
@@ -10959,10 +10959,10 @@
         <v>0</v>
       </c>
       <c r="G4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -10973,13 +10973,13 @@
         <v>201</v>
       </c>
       <c r="D6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E6">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -10993,7 +10993,7 @@
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -11010,7 +11010,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -11032,7 +11032,7 @@
         <v>101</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>218</v>
@@ -11041,10 +11041,10 @@
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H11" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -11062,7 +11062,7 @@
         <v>227</v>
       </c>
       <c r="H12" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -11073,7 +11073,7 @@
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="H13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -11081,16 +11081,16 @@
         <v>111</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -11099,7 +11099,7 @@
       </c>
       <c r="C15" s="18"/>
       <c r="H15" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -11108,7 +11108,7 @@
       </c>
       <c r="C16" s="18"/>
       <c r="H16" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -11117,7 +11117,7 @@
       </c>
       <c r="C17" s="18"/>
       <c r="H17" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -11125,7 +11125,7 @@
         <v>115</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G18" t="s">
         <v>325</v>
@@ -11145,7 +11145,7 @@
         <v>325</v>
       </c>
       <c r="H19" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -11154,7 +11154,7 @@
       </c>
       <c r="C20" s="18"/>
       <c r="H20" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -11163,7 +11163,7 @@
       </c>
       <c r="C21" s="18"/>
       <c r="H21" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -11172,7 +11172,7 @@
       </c>
       <c r="C22" s="18"/>
       <c r="H22" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -11180,16 +11180,16 @@
         <v>125</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="H23" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -11198,7 +11198,7 @@
       </c>
       <c r="C24" s="18"/>
       <c r="H24" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -11210,7 +11210,7 @@
         <v>3</v>
       </c>
       <c r="H25" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -11222,7 +11222,7 @@
         <v>3</v>
       </c>
       <c r="H26" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -11239,7 +11239,7 @@
         <v>325</v>
       </c>
       <c r="H27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -11248,7 +11248,7 @@
       </c>
       <c r="C28" s="18"/>
       <c r="H28" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -11257,7 +11257,7 @@
       </c>
       <c r="C29" s="18"/>
       <c r="H29" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -11266,7 +11266,7 @@
       </c>
       <c r="C30" s="18"/>
       <c r="H30" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -11283,7 +11283,7 @@
         <v>325</v>
       </c>
       <c r="H31" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -11292,7 +11292,7 @@
       </c>
       <c r="C32" s="18"/>
       <c r="H32" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -11300,7 +11300,7 @@
         <v>151</v>
       </c>
       <c r="C33" s="18" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D33" t="s">
         <v>220</v>
@@ -11309,10 +11309,10 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="H33" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -11321,7 +11321,7 @@
       </c>
       <c r="C34" s="18"/>
       <c r="H34" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -11330,7 +11330,7 @@
       </c>
       <c r="C35" s="18"/>
       <c r="H35" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
@@ -11339,7 +11339,7 @@
       </c>
       <c r="C36" s="18"/>
       <c r="H36" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
@@ -11347,10 +11347,10 @@
         <v>155</v>
       </c>
       <c r="C37" s="18" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="H37" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
@@ -11359,7 +11359,7 @@
       </c>
       <c r="C38" s="18"/>
       <c r="H38" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -11368,7 +11368,7 @@
       </c>
       <c r="C39" s="18"/>
       <c r="H39" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -11377,7 +11377,7 @@
       </c>
       <c r="C40" s="18"/>
       <c r="H40" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
@@ -11458,7 +11458,7 @@
         <v>226</v>
       </c>
       <c r="D46" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E46">
         <v>4</v>
@@ -11481,7 +11481,7 @@
         <v>328</v>
       </c>
       <c r="H47" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -11495,7 +11495,7 @@
         <v>7</v>
       </c>
       <c r="H48" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -11517,7 +11517,7 @@
         <v>175</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E50">
         <v>7</v>
@@ -11624,7 +11624,7 @@
         <v>1</v>
       </c>
       <c r="G57" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -11632,16 +11632,16 @@
         <v>191</v>
       </c>
       <c r="C58" s="18" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="E58">
         <v>5</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H58" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
@@ -11650,7 +11650,7 @@
       </c>
       <c r="C59" s="18"/>
       <c r="H59" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -11658,10 +11658,10 @@
         <v>193</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="H60" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -11670,7 +11670,7 @@
       </c>
       <c r="C61" s="18"/>
       <c r="H61" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -11681,13 +11681,13 @@
         <v>212</v>
       </c>
       <c r="D62" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E62">
         <v>100</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -11704,27 +11704,27 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C64" s="18" t="s">
         <v>238</v>
       </c>
       <c r="D64" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="E64">
         <v>7</v>
       </c>
       <c r="G64" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="H64" t="s">
         <v>776</v>
-      </c>
-      <c r="H64" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C65" s="18" t="s">
         <v>237</v>
@@ -11733,10 +11733,10 @@
         <v>9</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H65" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -11747,16 +11747,16 @@
         <v>242</v>
       </c>
       <c r="D66" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="E66">
         <v>1</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H66" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -11766,12 +11766,12 @@
       <c r="C67" s="18"/>
       <c r="G67" s="9"/>
       <c r="H67" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B69" s="4" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C69" s="18" t="s">
         <v>207</v>
@@ -11783,10 +11783,10 @@
         <v>100</v>
       </c>
       <c r="G69" t="s">
+        <v>736</v>
+      </c>
+      <c r="H69" t="s">
         <v>737</v>
-      </c>
-      <c r="H69" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -11797,10 +11797,10 @@
         <v>211</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="H70" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -11809,7 +11809,7 @@
       </c>
       <c r="C71" s="18"/>
       <c r="H71" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -11817,19 +11817,19 @@
         <v>321</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D72" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
       <c r="G72" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="H72" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -11841,10 +11841,10 @@
         <v>100</v>
       </c>
       <c r="G73" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H73" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -11853,10 +11853,10 @@
       </c>
       <c r="C74" s="18"/>
       <c r="G74" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="H74" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
@@ -11865,19 +11865,19 @@
         <v>331</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D75" t="s">
+        <v>756</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="G75" t="s">
+        <v>743</v>
+      </c>
+      <c r="H75" t="s">
         <v>757</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="G75" t="s">
-        <v>744</v>
-      </c>
-      <c r="H75" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -11887,7 +11887,7 @@
       </c>
       <c r="C76" s="18"/>
       <c r="H76" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -11897,7 +11897,7 @@
       </c>
       <c r="C77" s="18"/>
       <c r="H77" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -11907,7 +11907,7 @@
       </c>
       <c r="C78" s="18"/>
       <c r="H78" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -11917,7 +11917,7 @@
       </c>
       <c r="C79" s="18"/>
       <c r="H79" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -11927,7 +11927,7 @@
       </c>
       <c r="C80" s="18"/>
       <c r="H80" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -11937,7 +11937,7 @@
       </c>
       <c r="C81" s="18"/>
       <c r="H81" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -11947,7 +11947,7 @@
       </c>
       <c r="C82" s="18"/>
       <c r="H82" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
@@ -11956,16 +11956,16 @@
         <v>339</v>
       </c>
       <c r="C83" s="18" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="E83">
         <v>100</v>
       </c>
       <c r="G83" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="H83" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
@@ -11975,7 +11975,7 @@
       </c>
       <c r="C84" s="18"/>
       <c r="H84" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -11985,7 +11985,7 @@
       </c>
       <c r="C85" s="18"/>
       <c r="H85" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -11995,7 +11995,7 @@
       </c>
       <c r="C86" s="18"/>
       <c r="H86" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -12004,13 +12004,13 @@
         <v>343</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G87" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H87" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -12020,7 +12020,7 @@
       </c>
       <c r="C88" s="18"/>
       <c r="H88" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -12030,7 +12030,7 @@
       </c>
       <c r="C89" s="18"/>
       <c r="H89" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -12040,7 +12040,7 @@
       </c>
       <c r="C90" s="18"/>
       <c r="H90" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -12065,7 +12065,7 @@
         <v>411</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -12074,7 +12074,7 @@
         <v>291</v>
       </c>
       <c r="H93" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -12086,7 +12086,7 @@
         <v>292</v>
       </c>
       <c r="H94" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
@@ -12094,7 +12094,7 @@
         <v>421</v>
       </c>
       <c r="C95" s="18" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E95">
         <v>20</v>
@@ -12108,7 +12108,7 @@
         <v>422</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
@@ -12116,7 +12116,7 @@
         <v>423</v>
       </c>
       <c r="C97" s="18" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
@@ -12124,7 +12124,7 @@
         <v>424</v>
       </c>
       <c r="C98" s="18" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
@@ -12132,7 +12132,7 @@
         <v>425</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="E99">
         <v>35</v>
@@ -12143,7 +12143,7 @@
         <v>426</v>
       </c>
       <c r="C100" s="18" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="E100">
         <v>20</v>
@@ -12174,7 +12174,7 @@
         <v>327</v>
       </c>
       <c r="H102" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -12183,7 +12183,7 @@
       </c>
       <c r="C103" s="18"/>
       <c r="H103" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
@@ -12192,7 +12192,7 @@
       </c>
       <c r="C104" s="18"/>
       <c r="H104" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
@@ -12338,13 +12338,13 @@
         <v>1001</v>
       </c>
       <c r="C3" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" t="s">
         <v>397</v>
       </c>
-      <c r="D3" t="s">
-        <v>398</v>
-      </c>
       <c r="E3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -12353,7 +12353,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -12361,13 +12361,13 @@
         <v>1002</v>
       </c>
       <c r="C4" t="s">
+        <v>791</v>
+      </c>
+      <c r="D4" t="s">
         <v>792</v>
       </c>
-      <c r="D4" t="s">
-        <v>793</v>
-      </c>
       <c r="E4" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -12381,7 +12381,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -12410,10 +12410,10 @@
         <v>1102</v>
       </c>
       <c r="C7" t="s">
+        <v>455</v>
+      </c>
+      <c r="E7" t="s">
         <v>456</v>
-      </c>
-      <c r="E7" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -12421,10 +12421,10 @@
         <v>1103</v>
       </c>
       <c r="C8" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -12432,10 +12432,10 @@
         <v>1104</v>
       </c>
       <c r="C9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -12443,10 +12443,10 @@
         <v>1105</v>
       </c>
       <c r="C10" t="s">
+        <v>793</v>
+      </c>
+      <c r="E10" t="s">
         <v>794</v>
-      </c>
-      <c r="E10" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -12454,10 +12454,10 @@
         <v>1106</v>
       </c>
       <c r="C11" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -12465,10 +12465,10 @@
         <v>1116</v>
       </c>
       <c r="C12" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -12476,10 +12476,10 @@
         <v>1117</v>
       </c>
       <c r="C13" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E13" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -12487,10 +12487,10 @@
         <v>1118</v>
       </c>
       <c r="C14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -12498,10 +12498,10 @@
         <v>1119</v>
       </c>
       <c r="C15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E15" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -12509,10 +12509,10 @@
         <v>1120</v>
       </c>
       <c r="C16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E16" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
@@ -12840,38 +12840,38 @@
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>426</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>502</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>428</v>
-      </c>
       <c r="G4" s="10" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
@@ -12883,19 +12883,19 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="E6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G6" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
@@ -12903,33 +12903,33 @@
         <v>67</v>
       </c>
       <c r="C7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D7" t="s">
         <v>70</v>
       </c>
       <c r="E7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G7" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C8" t="s">
         <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="E8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G8" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -12937,16 +12937,16 @@
         <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D9" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="G9" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -12954,192 +12954,192 @@
         <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D10" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="E10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G10" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C12" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D12" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G12" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D13" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G13" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G14" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C15" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="G15" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C16" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="G16" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C17" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D17" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E17" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C18" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D18" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E18" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C19" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D19" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E19" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D20" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E20" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="G20" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D21" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="G21" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -13147,137 +13147,137 @@
         <v>194</v>
       </c>
       <c r="C22" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D22" t="s">
         <v>196</v>
       </c>
       <c r="E22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G22" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D23" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E23" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="G23" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C24" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E24" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G24" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C25" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D25" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E25" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="G25" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C26" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C27" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C28" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C29" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C30" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C31" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C33" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E33" t="s">
+        <v>508</v>
+      </c>
+      <c r="F33" t="s">
         <v>509</v>
-      </c>
-      <c r="F33" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
+        <v>533</v>
+      </c>
+      <c r="C34" t="s">
         <v>534</v>
-      </c>
-      <c r="C34" t="s">
-        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -13294,10 +13294,10 @@
   <dimension ref="A1:Y229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D172" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="U41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N202" sqref="N202"/>
+      <selection pane="bottomRight" activeCell="W50" sqref="W50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13596,7 +13596,7 @@
         <v>2115</v>
       </c>
       <c r="C18" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="H18">
         <v>15</v>
@@ -13960,7 +13960,7 @@
         <v>1</v>
       </c>
       <c r="W43" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="44" spans="2:23" x14ac:dyDescent="0.25">
@@ -13968,7 +13968,7 @@
         <v>2311</v>
       </c>
       <c r="C44" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -13986,7 +13986,7 @@
         <v>1</v>
       </c>
       <c r="W44" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
     </row>
     <row r="45" spans="2:23" x14ac:dyDescent="0.25">
@@ -14012,7 +14012,7 @@
         <v>8</v>
       </c>
       <c r="W45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.25">
@@ -14038,7 +14038,7 @@
         <v>6</v>
       </c>
       <c r="W46" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.25">
@@ -14064,7 +14064,7 @@
         <v>20</v>
       </c>
       <c r="W47" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.25">
@@ -14090,7 +14090,7 @@
         <v>30</v>
       </c>
       <c r="W48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
@@ -14116,7 +14116,7 @@
         <v>6</v>
       </c>
       <c r="W49" t="s">
-        <v>350</v>
+        <v>912</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
@@ -14142,7 +14142,7 @@
         <v>20</v>
       </c>
       <c r="W50" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
@@ -14168,7 +14168,7 @@
         <v>6</v>
       </c>
       <c r="W51" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
@@ -14197,7 +14197,7 @@
         <v>1</v>
       </c>
       <c r="W52" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
@@ -14223,7 +14223,7 @@
         <v>6</v>
       </c>
       <c r="W53" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
@@ -14249,7 +14249,7 @@
         <v>20</v>
       </c>
       <c r="W54" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
@@ -14275,7 +14275,7 @@
         <v>30</v>
       </c>
       <c r="W55" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
@@ -14301,7 +14301,7 @@
         <v>5</v>
       </c>
       <c r="W56" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
@@ -14327,7 +14327,7 @@
         <v>35</v>
       </c>
       <c r="W57" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
@@ -14353,7 +14353,7 @@
         <v>30</v>
       </c>
       <c r="W58" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
@@ -14385,7 +14385,7 @@
         <v>1</v>
       </c>
       <c r="W59" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
@@ -14411,7 +14411,7 @@
         <v>12</v>
       </c>
       <c r="W60" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
@@ -14437,7 +14437,7 @@
         <v>30</v>
       </c>
       <c r="W61" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
@@ -14463,7 +14463,7 @@
         <v>100</v>
       </c>
       <c r="W62" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
@@ -14489,7 +14489,7 @@
         <v>8</v>
       </c>
       <c r="W63" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
@@ -14518,7 +14518,7 @@
         <v>4</v>
       </c>
       <c r="W64" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
@@ -14544,7 +14544,7 @@
         <v>5</v>
       </c>
       <c r="W65" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
@@ -14570,7 +14570,7 @@
         <v>125</v>
       </c>
       <c r="W66" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
@@ -14599,7 +14599,7 @@
         <v>20</v>
       </c>
       <c r="W67" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
@@ -14625,7 +14625,7 @@
         <v>35</v>
       </c>
       <c r="W68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
@@ -14657,7 +14657,7 @@
         <v>1</v>
       </c>
       <c r="W69" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
@@ -14683,7 +14683,7 @@
         <v>30</v>
       </c>
       <c r="W70" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
@@ -14709,7 +14709,7 @@
         <v>125</v>
       </c>
       <c r="W71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
@@ -14735,7 +14735,7 @@
         <v>8</v>
       </c>
       <c r="W72" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
@@ -14761,7 +14761,7 @@
         <v>125</v>
       </c>
       <c r="W73" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="74" spans="2:23" x14ac:dyDescent="0.25">
@@ -14790,7 +14790,7 @@
         <v>40</v>
       </c>
       <c r="W74" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
@@ -14971,7 +14971,7 @@
         <v>2501</v>
       </c>
       <c r="C90" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D90" t="s">
         <v>24</v>
@@ -15021,7 +15021,7 @@
         <v>2511</v>
       </c>
       <c r="C94" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E94">
         <v>2</v>
@@ -15066,7 +15066,7 @@
         <v>2521</v>
       </c>
       <c r="C97" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E97">
         <v>3</v>
@@ -15080,7 +15080,7 @@
         <v>2531</v>
       </c>
       <c r="C98" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E98">
         <v>4</v>
@@ -15094,7 +15094,7 @@
         <v>2541</v>
       </c>
       <c r="C99" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E99">
         <v>5</v>
@@ -15108,7 +15108,7 @@
         <v>2551</v>
       </c>
       <c r="C100" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E100">
         <v>6</v>
@@ -15122,7 +15122,7 @@
         <v>2561</v>
       </c>
       <c r="C101" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E101">
         <v>7</v>
@@ -15136,7 +15136,7 @@
         <v>2571</v>
       </c>
       <c r="C102" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E102">
         <v>8</v>
@@ -15150,7 +15150,7 @@
         <v>2581</v>
       </c>
       <c r="C103" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="E103">
         <v>9</v>
@@ -15164,7 +15164,7 @@
         <v>2591</v>
       </c>
       <c r="C104" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E104">
         <v>10</v>
@@ -15270,7 +15270,7 @@
         <v>2641</v>
       </c>
       <c r="C113" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="E113">
         <v>5</v>
@@ -15595,7 +15595,7 @@
         <v>2801</v>
       </c>
       <c r="C138" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D138" t="s">
         <v>27</v>
@@ -15606,7 +15606,7 @@
         <v>2802</v>
       </c>
       <c r="C139" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="140" spans="2:15" x14ac:dyDescent="0.25">
@@ -15614,7 +15614,7 @@
         <v>2803</v>
       </c>
       <c r="C140" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="141" spans="2:15" x14ac:dyDescent="0.25">
@@ -15622,7 +15622,7 @@
         <v>2804</v>
       </c>
       <c r="C141" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="142" spans="2:15" x14ac:dyDescent="0.25">
@@ -15630,7 +15630,7 @@
         <v>2805</v>
       </c>
       <c r="C142" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="143" spans="2:15" x14ac:dyDescent="0.25">
@@ -15666,7 +15666,7 @@
         <v>2811</v>
       </c>
       <c r="C148" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="E148">
         <v>2</v>
@@ -15677,7 +15677,7 @@
         <v>2812</v>
       </c>
       <c r="C149" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="150" spans="2:25" x14ac:dyDescent="0.25">
@@ -15685,7 +15685,7 @@
         <v>2813</v>
       </c>
       <c r="C150" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
@@ -15693,7 +15693,7 @@
         <v>2814</v>
       </c>
       <c r="C151" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="152" spans="2:25" x14ac:dyDescent="0.25">
@@ -15709,7 +15709,7 @@
         <v>2821</v>
       </c>
       <c r="C153" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="E153">
         <v>3</v>
@@ -15720,7 +15720,7 @@
         <v>2822</v>
       </c>
       <c r="C154" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="155" spans="2:25" x14ac:dyDescent="0.25">
@@ -15728,7 +15728,7 @@
         <v>2823</v>
       </c>
       <c r="C155" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="156" spans="2:25" x14ac:dyDescent="0.25">
@@ -15736,7 +15736,7 @@
         <v>2834</v>
       </c>
       <c r="C156" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="157" spans="2:25" x14ac:dyDescent="0.25">
@@ -15744,7 +15744,7 @@
         <v>2825</v>
       </c>
       <c r="C157" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Y157" t="s">
         <v>202</v>
@@ -15755,7 +15755,7 @@
         <v>2831</v>
       </c>
       <c r="C158" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E158">
         <v>4</v>
@@ -15766,7 +15766,7 @@
         <v>2832</v>
       </c>
       <c r="C159" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="160" spans="2:25" x14ac:dyDescent="0.25">
@@ -15774,7 +15774,7 @@
         <v>2841</v>
       </c>
       <c r="C160" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="E160">
         <v>5</v>
@@ -15785,7 +15785,7 @@
         <v>2842</v>
       </c>
       <c r="C161" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.25">
@@ -15793,7 +15793,7 @@
         <v>2851</v>
       </c>
       <c r="C162" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E162">
         <v>6</v>
@@ -15804,7 +15804,7 @@
         <v>2852</v>
       </c>
       <c r="C163" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.25">
@@ -15812,7 +15812,7 @@
         <v>2853</v>
       </c>
       <c r="C164" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="165" spans="2:5" x14ac:dyDescent="0.25">
@@ -15820,7 +15820,7 @@
         <v>2861</v>
       </c>
       <c r="C165" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="E165">
         <v>7</v>
@@ -15831,7 +15831,7 @@
         <v>2862</v>
       </c>
       <c r="C166" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="167" spans="2:5" x14ac:dyDescent="0.25">
@@ -15839,7 +15839,7 @@
         <v>2863</v>
       </c>
       <c r="C167" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="168" spans="2:5" x14ac:dyDescent="0.25">
@@ -15855,7 +15855,7 @@
         <v>2871</v>
       </c>
       <c r="C169" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="E169">
         <v>8</v>
@@ -15866,7 +15866,7 @@
         <v>2872</v>
       </c>
       <c r="C170" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.25">
@@ -15874,7 +15874,7 @@
         <v>2873</v>
       </c>
       <c r="C171" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
     </row>
     <row r="172" spans="2:5" x14ac:dyDescent="0.25">
@@ -15882,7 +15882,7 @@
         <v>2881</v>
       </c>
       <c r="C172" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="E172">
         <v>9</v>
@@ -15893,7 +15893,7 @@
         <v>2882</v>
       </c>
       <c r="C173" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.25">
@@ -15901,7 +15901,7 @@
         <v>2883</v>
       </c>
       <c r="C174" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="175" spans="2:5" x14ac:dyDescent="0.25">
@@ -15909,7 +15909,7 @@
         <v>2891</v>
       </c>
       <c r="C175" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="E175">
         <v>10</v>
@@ -16052,7 +16052,7 @@
         <v>2917</v>
       </c>
       <c r="C187" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="D187" t="s">
         <v>258</v>
@@ -16212,7 +16212,7 @@
         <v>2.5</v>
       </c>
       <c r="W195" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="196" spans="2:23" x14ac:dyDescent="0.25">
@@ -16252,7 +16252,7 @@
         <v>2</v>
       </c>
       <c r="W197" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
     </row>
     <row r="198" spans="2:23" x14ac:dyDescent="0.25">
@@ -16260,7 +16260,7 @@
         <v>2941</v>
       </c>
       <c r="C198" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D198" t="s">
         <v>281</v>
@@ -16271,7 +16271,7 @@
         <v>2942</v>
       </c>
       <c r="C199" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D199" t="s">
         <v>281</v>
@@ -16285,7 +16285,7 @@
         <v>2943</v>
       </c>
       <c r="C200" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D200" t="s">
         <v>281</v>
@@ -16299,7 +16299,7 @@
         <v>2944</v>
       </c>
       <c r="C201" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D201" t="s">
         <v>281</v>
@@ -16319,7 +16319,7 @@
         <v>2945</v>
       </c>
       <c r="C202" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D202" t="s">
         <v>281</v>
@@ -16333,7 +16333,7 @@
         <v>2946</v>
       </c>
       <c r="C203" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D203" t="s">
         <v>281</v>
@@ -16347,7 +16347,7 @@
         <v>2947</v>
       </c>
       <c r="C204" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D204" t="s">
         <v>281</v>
@@ -16361,7 +16361,7 @@
         <v>2948</v>
       </c>
       <c r="C205" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D205" t="s">
         <v>281</v>
@@ -16428,7 +16428,7 @@
         <v>2965</v>
       </c>
       <c r="C210" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D210" t="s">
         <v>289</v>
@@ -16445,7 +16445,7 @@
         <v>2966</v>
       </c>
       <c r="C211" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D211" t="s">
         <v>289</v>
@@ -16462,7 +16462,7 @@
         <v>2967</v>
       </c>
       <c r="C212" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D212" t="s">
         <v>289</v>
@@ -16479,7 +16479,7 @@
         <v>2968</v>
       </c>
       <c r="C213" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="D213" t="s">
         <v>289</v>
@@ -16759,7 +16759,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16793,7 +16793,7 @@
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>9</v>
@@ -16819,7 +16819,7 @@
         <v>0.5</v>
       </c>
       <c r="J3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -16847,7 +16847,7 @@
         <v>3103</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D5" t="s">
         <v>280</v>
@@ -16907,7 +16907,7 @@
         <v>3108</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D8" t="s">
         <v>280</v>
@@ -16924,10 +16924,10 @@
         <v>3312</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9">
@@ -16942,10 +16942,10 @@
         <v>3112</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10">
@@ -16963,7 +16963,7 @@
         <v>7.62</v>
       </c>
       <c r="D11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11">
@@ -16981,7 +16981,7 @@
         <v>7.62</v>
       </c>
       <c r="D12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12">
@@ -16999,7 +16999,7 @@
         <v>7.62</v>
       </c>
       <c r="D13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13">
@@ -17014,7 +17014,7 @@
         <v>7.62</v>
       </c>
       <c r="D14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14">
@@ -17026,10 +17026,10 @@
         <v>3117</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15">
@@ -17041,10 +17041,10 @@
         <v>3118</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16">
@@ -17056,10 +17056,10 @@
         <v>3119</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17">
@@ -17074,10 +17074,10 @@
         <v>3120</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18">
@@ -17095,7 +17095,7 @@
         <v>5.56</v>
       </c>
       <c r="D19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F19" s="9"/>
       <c r="G19">
@@ -17110,7 +17110,7 @@
         <v>7.62</v>
       </c>
       <c r="D20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F20" s="9"/>
       <c r="G20">
@@ -17122,10 +17122,10 @@
         <v>3123</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F21" s="9"/>
       <c r="G21">
@@ -17140,10 +17140,10 @@
         <v>3124</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22">
@@ -17161,7 +17161,7 @@
         <v>7.62</v>
       </c>
       <c r="D23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F23" s="9"/>
       <c r="G23">
@@ -17179,7 +17179,7 @@
         <v>7.62</v>
       </c>
       <c r="D24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24">
@@ -17194,10 +17194,10 @@
         <v>3127</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F25" s="9"/>
       <c r="G25">
@@ -17212,10 +17212,10 @@
         <v>3128</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26">
@@ -17227,10 +17227,10 @@
         <v>3129</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27">
@@ -17245,10 +17245,10 @@
         <v>3130</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28">
@@ -17263,10 +17263,10 @@
         <v>3131</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29">
@@ -17278,10 +17278,10 @@
         <v>3132</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30">
@@ -17293,13 +17293,13 @@
         <v>3133</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G31">
         <v>40</v>
@@ -17313,13 +17313,13 @@
         <v>3134</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="G32">
         <v>60</v>
@@ -17336,7 +17336,7 @@
         <v>5.56</v>
       </c>
       <c r="D33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F33" s="9"/>
       <c r="G33">
@@ -17354,7 +17354,7 @@
         <v>5.56</v>
       </c>
       <c r="D34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F34" s="9"/>
       <c r="G34">
@@ -17369,10 +17369,10 @@
         <v>3137</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F35" s="9"/>
       <c r="G35">
@@ -17387,10 +17387,10 @@
         <v>3138</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F36" s="9"/>
       <c r="G36">
@@ -17408,7 +17408,7 @@
         <v>5.56</v>
       </c>
       <c r="D37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F37" s="9"/>
       <c r="G37">
@@ -17423,7 +17423,7 @@
         <v>5.56</v>
       </c>
       <c r="D38" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G38">
         <v>100</v>
@@ -17437,13 +17437,13 @@
         <v>3201</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D40" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F40" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -17457,13 +17457,13 @@
         <v>3202</v>
       </c>
       <c r="C41" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D41" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F41" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G41">
         <v>12</v>
@@ -17496,7 +17496,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17507,13 +17507,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>809</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -17521,10 +17521,10 @@
         <v>4001</v>
       </c>
       <c r="C3" t="s">
+        <v>810</v>
+      </c>
+      <c r="E3" t="s">
         <v>811</v>
-      </c>
-      <c r="E3" t="s">
-        <v>812</v>
       </c>
       <c r="F3">
         <v>35</v>
@@ -17575,7 +17575,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -17586,13 +17586,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>13</v>
@@ -17606,19 +17606,19 @@
         <v>101</v>
       </c>
       <c r="D4" t="s">
+        <v>510</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="I4" t="s">
         <v>511</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="I4" t="s">
-        <v>512</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -17627,19 +17627,19 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F5" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G5">
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -17648,19 +17648,19 @@
         <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G6" s="3">
         <v>-8</v>
       </c>
       <c r="I6" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -17669,19 +17669,19 @@
         <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G7" s="3">
         <v>-8</v>
       </c>
       <c r="I7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -17690,19 +17690,19 @@
         <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="E8" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G8" s="9">
         <v>-40</v>
       </c>
       <c r="I8" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -17711,19 +17711,19 @@
         <v>106</v>
       </c>
       <c r="D9" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -17732,19 +17732,19 @@
         <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G10">
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -17753,19 +17753,19 @@
         <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="E11" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G11">
         <v>-15</v>
       </c>
       <c r="I11" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -17774,19 +17774,19 @@
         <v>109</v>
       </c>
       <c r="D12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="E12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F12" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G12">
         <v>-15</v>
       </c>
       <c r="I12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -17795,42 +17795,42 @@
         <v>110</v>
       </c>
       <c r="D13" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E13" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G13">
         <v>-60</v>
       </c>
       <c r="I13" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="22" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C15">
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I15" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -17839,19 +17839,19 @@
         <v>112</v>
       </c>
       <c r="D16" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E16" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G16">
         <v>5</v>
       </c>
       <c r="I16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
@@ -17860,19 +17860,19 @@
         <v>113</v>
       </c>
       <c r="D17" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F17" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G17">
         <v>10</v>
       </c>
       <c r="I17" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
@@ -17881,19 +17881,19 @@
         <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E18" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F18" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G18">
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -17902,19 +17902,19 @@
         <v>115</v>
       </c>
       <c r="D19" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="E19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F19" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G19">
         <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
@@ -17923,19 +17923,19 @@
         <v>116</v>
       </c>
       <c r="D20" t="s">
+        <v>565</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="I20" t="s">
         <v>566</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>482</v>
-      </c>
-      <c r="I20" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
@@ -17944,19 +17944,19 @@
         <v>117</v>
       </c>
       <c r="D21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E21" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F21" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
@@ -17965,19 +17965,19 @@
         <v>118</v>
       </c>
       <c r="D22" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E22" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F22" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G22">
         <v>35</v>
       </c>
       <c r="I22" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -17986,19 +17986,19 @@
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E23" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F23" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -18007,24 +18007,24 @@
         <v>120</v>
       </c>
       <c r="D24" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E24" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G24">
         <v>100</v>
       </c>
       <c r="I24" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C26">
         <v>121</v>
@@ -18056,7 +18056,7 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="22" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C32">
         <v>131</v>
@@ -18068,10 +18068,10 @@
         <v>132</v>
       </c>
       <c r="D33" t="s">
+        <v>527</v>
+      </c>
+      <c r="I33" t="s">
         <v>528</v>
-      </c>
-      <c r="I33" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
@@ -18080,7 +18080,7 @@
         <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
@@ -18089,10 +18089,10 @@
         <v>134</v>
       </c>
       <c r="D35" t="s">
+        <v>530</v>
+      </c>
+      <c r="I35" t="s">
         <v>531</v>
-      </c>
-      <c r="I35" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.6t: Can shoot all CoD guns
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD32F32C-B81C-4F8A-9F98-11E8FC79704A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702001BF-9D4C-47D9-A2C3-23D79164DD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="390" yWindow="345" windowWidth="9210" windowHeight="6135" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1198" uniqueCount="926">
   <si>
     <t>ID</t>
   </si>
@@ -3238,6 +3238,45 @@
   </si>
   <si>
     <t>dur=20, cd=200, rec=0.08, inac=0.08, 1200-75 splash damage</t>
+  </si>
+  <si>
+    <t>rpd</t>
+  </si>
+  <si>
+    <t>hamr</t>
+  </si>
+  <si>
+    <t>rpg</t>
+  </si>
+  <si>
+    <t>ray gun</t>
+  </si>
+  <si>
+    <t>galil</t>
+  </si>
+  <si>
+    <t>war machine</t>
+  </si>
+  <si>
+    <t>python</t>
+  </si>
+  <si>
+    <t>dsr</t>
+  </si>
+  <si>
+    <t>five seven</t>
+  </si>
+  <si>
+    <t>type25</t>
+  </si>
+  <si>
+    <t>executioner</t>
+  </si>
+  <si>
+    <t>mtar</t>
+  </si>
+  <si>
+    <t>m1911</t>
   </si>
 </sst>
 </file>
@@ -13294,10 +13333,10 @@
   <dimension ref="A1:Y229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="U41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="L41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W50" sqref="W50"/>
+      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16759,7 +16798,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16801,7 +16840,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>3101</v>
+        <v>3301</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>284</v>
@@ -16824,7 +16863,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>3102</v>
+        <v>3931</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>284</v>
@@ -16844,7 +16883,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>3103</v>
+        <v>3933</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>471</v>
@@ -16864,7 +16903,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>3106</v>
+        <v>3311</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>283</v>
@@ -16884,7 +16923,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>3107</v>
+        <v>3932</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>283</v>
@@ -16904,7 +16943,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>3108</v>
+        <v>3944</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>390</v>
@@ -16920,6 +16959,9 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>925</v>
+      </c>
       <c r="B9">
         <v>3312</v>
       </c>
@@ -16939,7 +16981,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>3112</v>
+        <v>3331</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>390</v>
@@ -16956,8 +16998,11 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>913</v>
+      </c>
       <c r="B11">
-        <v>3113</v>
+        <v>3361</v>
       </c>
       <c r="C11" s="4">
         <v>7.62</v>
@@ -16975,7 +17020,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>3114</v>
+        <v>3381</v>
       </c>
       <c r="C12" s="4">
         <v>7.62</v>
@@ -16992,8 +17037,11 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>914</v>
+      </c>
       <c r="B13">
-        <v>3115</v>
+        <v>3371</v>
       </c>
       <c r="C13" s="4">
         <v>7.62</v>
@@ -17008,7 +17056,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>3116</v>
+        <v>3391</v>
       </c>
       <c r="C14" s="4">
         <v>7.62</v>
@@ -17022,8 +17070,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>915</v>
+      </c>
       <c r="B15">
-        <v>3117</v>
+        <v>3341</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>390</v>
@@ -17038,7 +17089,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16">
-        <v>3118</v>
+        <v>3362</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>390</v>
@@ -17051,9 +17102,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>916</v>
+      </c>
       <c r="B17">
-        <v>3119</v>
+        <v>3372</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>391</v>
@@ -17069,9 +17123,9 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B18">
-        <v>3120</v>
+        <v>3392</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>391</v>
@@ -17087,9 +17141,12 @@
         <v>1.2161908339594292</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>917</v>
+      </c>
       <c r="B19">
-        <v>3121</v>
+        <v>3351</v>
       </c>
       <c r="C19" s="4">
         <v>5.56</v>
@@ -17102,9 +17159,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B20">
-        <v>3122</v>
+        <v>3373</v>
       </c>
       <c r="C20" s="4">
         <v>7.62</v>
@@ -17117,9 +17174,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>918</v>
+      </c>
       <c r="B21">
-        <v>3123</v>
+        <v>3321</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>390</v>
@@ -17135,9 +17195,9 @@
         <v>0.849609375</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B22">
-        <v>3124</v>
+        <v>3342</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>390</v>
@@ -17153,9 +17213,12 @@
         <v>0.99431818181818188</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>147</v>
+      </c>
       <c r="B23">
-        <v>3125</v>
+        <v>3332</v>
       </c>
       <c r="C23" s="4">
         <v>7.62</v>
@@ -17171,9 +17234,9 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>3126</v>
+        <v>3352</v>
       </c>
       <c r="C24" s="4">
         <v>7.62</v>
@@ -17189,9 +17252,12 @@
         <v>2.285714285714286</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>919</v>
+      </c>
       <c r="B25">
-        <v>3127</v>
+        <v>3333</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>392</v>
@@ -17207,9 +17273,9 @@
         <v>0.823974609375</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>3128</v>
+        <v>3354</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>392</v>
@@ -17221,10 +17287,17 @@
       <c r="G26">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f>(1-300/1000) * 0.25 * (1 + 300/1000) * 100 / 7</f>
+        <v>3.2499999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>920</v>
+      </c>
       <c r="B27">
-        <v>3129</v>
+        <v>3363</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>393</v>
@@ -17240,9 +17313,9 @@
         <v>2.197265625</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>3130</v>
+        <v>3382</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>393</v>
@@ -17258,9 +17331,12 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>921</v>
+      </c>
       <c r="B29">
-        <v>3131</v>
+        <v>3322</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>394</v>
@@ -17273,9 +17349,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>3132</v>
+        <v>3343</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>394</v>
@@ -17288,9 +17364,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>378</v>
+      </c>
       <c r="B31">
-        <v>3133</v>
+        <v>3353</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>378</v>
@@ -17308,9 +17387,9 @@
         <v>1.4876033057851239</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>3134</v>
+        <v>3374</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>378</v>
@@ -17328,9 +17407,12 @@
         <v>1.1865234375</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>922</v>
+      </c>
       <c r="B33">
-        <v>3135</v>
+        <v>3323</v>
       </c>
       <c r="C33" s="4">
         <v>5.56</v>
@@ -17346,9 +17428,9 @@
         <v>5.550110946745562</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>3136</v>
+        <v>3344</v>
       </c>
       <c r="C34" s="4">
         <v>5.56</v>
@@ -17364,9 +17446,12 @@
         <v>4.9173469387755109</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>923</v>
+      </c>
       <c r="B35">
-        <v>3137</v>
+        <v>3345</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>395</v>
@@ -17382,9 +17467,9 @@
         <v>1.0018552875695732</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>3138</v>
+        <v>3364</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>395</v>
@@ -17400,9 +17485,12 @@
         <v>1.0204081632653061</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>924</v>
+      </c>
       <c r="B37">
-        <v>3139</v>
+        <v>3355</v>
       </c>
       <c r="C37" s="4">
         <v>5.56</v>
@@ -17415,9 +17503,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>3140</v>
+        <v>3375</v>
       </c>
       <c r="C38" s="4">
         <v>5.56</v>
@@ -17429,10 +17517,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C39" s="4"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>3201</v>
       </c>
@@ -17452,7 +17540,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>3202</v>
       </c>

</xml_diff>

<commit_message>
v0.6.6u: Begin feature sound logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702001BF-9D4C-47D9-A2C3-23D79164DD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6E71B6-ECEA-4B47-9615-9B2735FE187C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="345" windowWidth="9210" windowHeight="6135" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -3324,7 +3324,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3343,6 +3343,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -3357,7 +3363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3404,6 +3410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -10943,8 +10950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11423,7 +11430,7 @@
       <c r="B41" s="4">
         <v>161</v>
       </c>
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="24" t="s">
         <v>215</v>
       </c>
       <c r="E41">
@@ -11437,7 +11444,7 @@
       <c r="B42" s="4">
         <v>162</v>
       </c>
-      <c r="C42" s="18" t="s">
+      <c r="C42" s="24" t="s">
         <v>221</v>
       </c>
       <c r="E42">
@@ -11451,7 +11458,7 @@
       <c r="B43" s="4">
         <v>163</v>
       </c>
-      <c r="C43" s="18" t="s">
+      <c r="C43" s="24" t="s">
         <v>222</v>
       </c>
       <c r="E43">
@@ -11465,7 +11472,7 @@
       <c r="B44" s="4">
         <v>164</v>
       </c>
-      <c r="C44" s="18" t="s">
+      <c r="C44" s="24" t="s">
         <v>223</v>
       </c>
       <c r="E44">
@@ -11479,7 +11486,7 @@
       <c r="B45" s="4">
         <v>165</v>
       </c>
-      <c r="C45" s="18" t="s">
+      <c r="C45" s="24" t="s">
         <v>225</v>
       </c>
       <c r="E45">
@@ -11493,7 +11500,7 @@
       <c r="B46" s="4">
         <v>171</v>
       </c>
-      <c r="C46" s="18" t="s">
+      <c r="C46" s="24" t="s">
         <v>226</v>
       </c>
       <c r="D46" t="s">
@@ -11510,7 +11517,7 @@
       <c r="B47" s="4">
         <v>172</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="C47" s="24" t="s">
         <v>228</v>
       </c>
       <c r="E47">
@@ -11527,7 +11534,7 @@
       <c r="B48" s="4">
         <v>173</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="24" t="s">
         <v>228</v>
       </c>
       <c r="E48">
@@ -11541,7 +11548,7 @@
       <c r="B49" s="4">
         <v>174</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="24" t="s">
         <v>234</v>
       </c>
       <c r="E49">
@@ -11555,7 +11562,7 @@
       <c r="B50" s="4">
         <v>175</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="24" t="s">
         <v>789</v>
       </c>
       <c r="E50">
@@ -11569,7 +11576,7 @@
       <c r="B51" s="4">
         <v>176</v>
       </c>
-      <c r="C51" s="18" t="s">
+      <c r="C51" s="24" t="s">
         <v>235</v>
       </c>
       <c r="E51">
@@ -11583,7 +11590,7 @@
       <c r="B52" s="4">
         <v>177</v>
       </c>
-      <c r="C52" s="18" t="s">
+      <c r="C52" s="24" t="s">
         <v>236</v>
       </c>
       <c r="E52">
@@ -13332,11 +13339,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="L41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L51" sqref="L51"/>
+      <selection pane="bottomRight" activeCell="C43" sqref="C43:C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16798,7 +16805,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.7j: HeroTree fully functional
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D075529-0F81-4702-B6AB-3CB5E388786D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B496B73B-7E02-4A23-9348-614A82087012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="11" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1297" uniqueCount="989">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1331" uniqueCount="1020">
   <si>
     <t>ID</t>
   </si>
@@ -3379,9 +3379,6 @@
     <t>Gear</t>
   </si>
   <si>
-    <t>Inventory +2 slots</t>
-  </si>
-  <si>
     <t>HealthIII</t>
   </si>
   <si>
@@ -3400,12 +3397,6 @@
     <t>Can use Belt II gear slot</t>
   </si>
   <si>
-    <t>Can use inventory bar</t>
-  </si>
-  <si>
-    <t>Can use items directly from inventory bar</t>
-  </si>
-  <si>
     <t>Inventory Bar II</t>
   </si>
   <si>
@@ -3467,6 +3458,108 @@
   </si>
   <si>
     <t>passive: heal 1% missing health every 1s, active: heal 7% missing health and gain 35% move speed for 4.5s</t>
+  </si>
+  <si>
+    <t>Can use half of inventory bar</t>
+  </si>
+  <si>
+    <t>Can use other half of inventory bar</t>
+  </si>
+  <si>
+    <t>Inventory +2 slots and unlock inventory</t>
+  </si>
+  <si>
+    <t>+2 base defense</t>
+  </si>
+  <si>
+    <t>+3 base attack</t>
+  </si>
+  <si>
+    <t>+5% base piercing</t>
+  </si>
+  <si>
+    <t>+0.3 base speed</t>
+  </si>
+  <si>
+    <t>+1 base agility</t>
+  </si>
+  <si>
+    <t>+5 base magic</t>
+  </si>
+  <si>
+    <t>+3 base resistance</t>
+  </si>
+  <si>
+    <t>+5% base resistance</t>
+  </si>
+  <si>
+    <t>+1.5 base sight</t>
+  </si>
+  <si>
+    <t>+25 base health</t>
+  </si>
+  <si>
+    <t>+10 base attack</t>
+  </si>
+  <si>
+    <t>+5 base defense</t>
+  </si>
+  <si>
+    <t>+7% base piercing</t>
+  </si>
+  <si>
+    <t>+0.5 base speed</t>
+  </si>
+  <si>
+    <t>+2 base sight</t>
+  </si>
+  <si>
+    <t>+20 base magic</t>
+  </si>
+  <si>
+    <t>+7 base resistance</t>
+  </si>
+  <si>
+    <t>+7% base penetration</t>
+  </si>
+  <si>
+    <t>+120 base health</t>
+  </si>
+  <si>
+    <t>Can use offhand gear slot</t>
+  </si>
+  <si>
+    <t>Unlocks follower</t>
+  </si>
+  <si>
+    <t>TenacityII</t>
+  </si>
+  <si>
+    <t>Tenacity II</t>
+  </si>
+  <si>
+    <t>TenacityI</t>
+  </si>
+  <si>
+    <t>+7% base tenacity</t>
+  </si>
+  <si>
+    <t>Tenacity I</t>
+  </si>
+  <si>
+    <t>+5% base tenacity</t>
+  </si>
+  <si>
+    <t>+4 base health</t>
+  </si>
+  <si>
+    <t>base health regen</t>
+  </si>
+  <si>
+    <t>hunger less quickly</t>
+  </si>
+  <si>
+    <t>thirst less quickly</t>
   </si>
 </sst>
 </file>
@@ -10484,10 +10577,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10525,8 +10618,8 @@
         <v>879</v>
       </c>
       <c r="C4">
-        <f>SUM(HeroTree!E8:E51)</f>
-        <v>1864</v>
+        <f>SUM(HeroTree!E8:E53)</f>
+        <v>1918</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -10536,7 +10629,7 @@
       </c>
       <c r="C5">
         <f>C3-C4</f>
-        <v>3186</v>
+        <v>3132</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -10564,16 +10657,16 @@
         <v>956</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="E8" s="9">
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>959</v>
+        <v>988</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -10608,7 +10701,7 @@
         <v>568</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F11" s="9" t="s">
         <v>955</v>
@@ -10628,7 +10721,7 @@
         <v>569</v>
       </c>
       <c r="E12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="9" t="s">
         <v>955</v>
@@ -10648,7 +10741,7 @@
         <v>570</v>
       </c>
       <c r="E13">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F13" s="9" t="s">
         <v>955</v>
@@ -10763,7 +10856,7 @@
         <v>576</v>
       </c>
       <c r="E19">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="F19" t="s">
         <v>590</v>
@@ -10788,6 +10881,9 @@
       </c>
       <c r="F21" s="9" t="s">
         <v>955</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>1016</v>
       </c>
       <c r="I21" s="21"/>
     </row>
@@ -10805,6 +10901,9 @@
       <c r="F22" t="s">
         <v>932</v>
       </c>
+      <c r="G22" s="8" t="s">
+        <v>990</v>
+      </c>
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
@@ -10821,6 +10920,9 @@
       <c r="F23" t="s">
         <v>932</v>
       </c>
+      <c r="G23" s="8" t="s">
+        <v>989</v>
+      </c>
       <c r="I23" s="21"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
@@ -10837,6 +10939,9 @@
       <c r="F24" t="s">
         <v>932</v>
       </c>
+      <c r="G24" s="8" t="s">
+        <v>991</v>
+      </c>
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
@@ -10853,6 +10958,9 @@
       <c r="F25" t="s">
         <v>932</v>
       </c>
+      <c r="G25" s="8" t="s">
+        <v>992</v>
+      </c>
       <c r="I25" s="21"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -10869,373 +10977,479 @@
       <c r="F26" t="s">
         <v>932</v>
       </c>
+      <c r="G26" s="8" t="s">
+        <v>997</v>
+      </c>
       <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="C27" t="s">
-        <v>938</v>
+        <v>1012</v>
       </c>
       <c r="D27" t="s">
-        <v>591</v>
+        <v>1014</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27" t="s">
         <v>932</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>1015</v>
       </c>
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="C28" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D28" t="s">
-        <v>882</v>
+        <v>591</v>
       </c>
       <c r="E28">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
         <v>932</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>993</v>
       </c>
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
       <c r="C29" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D29" t="s">
-        <v>887</v>
+        <v>882</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F29" t="s">
         <v>932</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>994</v>
       </c>
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="30"/>
       <c r="C30" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D30" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F30" t="s">
         <v>932</v>
       </c>
+      <c r="G30" s="8" t="s">
+        <v>995</v>
+      </c>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="C31" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D31" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E31">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F31" t="s">
         <v>932</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>996</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="30"/>
       <c r="C32" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D32" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E32">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F32" t="s">
-        <v>933</v>
+        <v>932</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>998</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="C33" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D33" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E33">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
-        <v>934</v>
+        <v>933</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>999</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="C34" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D34" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E34">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F34" t="s">
-        <v>935</v>
+        <v>934</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>1000</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
       <c r="C35" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D35" t="s">
-        <v>594</v>
+        <v>892</v>
       </c>
       <c r="E35">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F35" t="s">
-        <v>936</v>
+        <v>935</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>1001</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" s="30"/>
       <c r="C36" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D36" t="s">
-        <v>893</v>
+        <v>594</v>
       </c>
       <c r="E36">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
-        <v>937</v>
+        <v>936</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="C37" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D37" t="s">
-        <v>595</v>
+        <v>893</v>
       </c>
       <c r="E37">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F37" t="s">
-        <v>938</v>
+        <v>937</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>1003</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" t="s">
-        <v>949</v>
+        <v>1010</v>
       </c>
       <c r="D38" t="s">
-        <v>894</v>
+        <v>1011</v>
       </c>
       <c r="E38">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>939</v>
+        <v>1012</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>1013</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="30"/>
       <c r="C39" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="D39" t="s">
-        <v>895</v>
+        <v>595</v>
       </c>
       <c r="E39">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F39" t="s">
-        <v>940</v>
+        <v>938</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>993</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="30"/>
       <c r="C40" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="D40" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="E40">
         <v>35</v>
       </c>
       <c r="F40" t="s">
-        <v>941</v>
+        <v>939</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="C41" t="s">
+        <v>950</v>
+      </c>
+      <c r="D41" t="s">
+        <v>895</v>
+      </c>
+      <c r="E41">
+        <v>35</v>
+      </c>
+      <c r="F41" t="s">
+        <v>940</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="30"/>
+      <c r="C42" t="s">
+        <v>951</v>
+      </c>
+      <c r="D42" t="s">
+        <v>896</v>
+      </c>
+      <c r="E42">
+        <v>35</v>
+      </c>
+      <c r="F42" t="s">
+        <v>941</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="30"/>
+      <c r="C43" t="s">
+        <v>959</v>
+      </c>
+      <c r="D43" t="s">
         <v>960</v>
       </c>
-      <c r="D41" t="s">
-        <v>961</v>
-      </c>
-      <c r="E41">
-        <v>100</v>
-      </c>
-      <c r="F41" t="s">
+      <c r="E43">
+        <v>70</v>
+      </c>
+      <c r="F43" t="s">
         <v>942</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="30" t="s">
+      <c r="G43" s="8" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="30" t="s">
         <v>958</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C45" t="s">
         <v>899</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D45" t="s">
         <v>899</v>
-      </c>
-      <c r="E43">
-        <v>150</v>
-      </c>
-      <c r="F43" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="30"/>
-      <c r="C44" t="s">
-        <v>952</v>
-      </c>
-      <c r="D44" t="s">
-        <v>898</v>
-      </c>
-      <c r="E44">
-        <v>50</v>
-      </c>
-      <c r="F44" t="s">
-        <v>971</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="30"/>
-      <c r="C45" t="s">
-        <v>953</v>
-      </c>
-      <c r="D45" t="s">
-        <v>900</v>
       </c>
       <c r="E45">
         <v>150</v>
       </c>
       <c r="F45" t="s">
-        <v>952</v>
-      </c>
-      <c r="G45" s="9" t="s">
-        <v>965</v>
+        <v>968</v>
+      </c>
+      <c r="G45" t="s">
+        <v>1008</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="30"/>
       <c r="C46" t="s">
-        <v>971</v>
+        <v>952</v>
       </c>
       <c r="D46" t="s">
-        <v>973</v>
+        <v>898</v>
       </c>
       <c r="E46">
-        <v>10</v>
-      </c>
-      <c r="F46" s="9" t="s">
-        <v>970</v>
+        <v>50</v>
+      </c>
+      <c r="F46" t="s">
+        <v>968</v>
       </c>
       <c r="G46" s="9" t="s">
-        <v>974</v>
+        <v>963</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="30"/>
       <c r="C47" t="s">
-        <v>962</v>
+        <v>953</v>
       </c>
       <c r="D47" t="s">
-        <v>969</v>
+        <v>900</v>
       </c>
       <c r="E47">
-        <v>40</v>
+        <v>150</v>
       </c>
       <c r="F47" t="s">
-        <v>971</v>
-      </c>
-      <c r="G47" t="s">
-        <v>966</v>
+        <v>952</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>964</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="30"/>
       <c r="C48" t="s">
-        <v>963</v>
+        <v>968</v>
       </c>
       <c r="D48" t="s">
+        <v>970</v>
+      </c>
+      <c r="E48">
+        <v>12</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>967</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" t="s">
+        <v>961</v>
+      </c>
+      <c r="D49" t="s">
+        <v>966</v>
+      </c>
+      <c r="E49">
+        <v>40</v>
+      </c>
+      <c r="F49" t="s">
         <v>968</v>
       </c>
-      <c r="E48">
-        <v>60</v>
-      </c>
-      <c r="F48" s="9" t="s">
+      <c r="G49" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="30"/>
+      <c r="C50" t="s">
         <v>962</v>
       </c>
-      <c r="G48" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="30" t="s">
+      <c r="D50" t="s">
+        <v>965</v>
+      </c>
+      <c r="E50">
+        <v>75</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>961</v>
+      </c>
+      <c r="G50" t="s">
+        <v>987</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="30" t="s">
         <v>897</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>897</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>954</v>
       </c>
-      <c r="E50">
-        <v>300</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E52">
+        <v>250</v>
+      </c>
+      <c r="F52" t="s">
         <v>955</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="30"/>
-      <c r="D51" t="s">
+      <c r="G52" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="30"/>
+      <c r="D53" t="s">
         <v>597</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>1017</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B21:B41"/>
-    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B21:B43"/>
+    <mergeCell ref="B45:B50"/>
     <mergeCell ref="I10:I19"/>
-    <mergeCell ref="I21:I29"/>
+    <mergeCell ref="I21:I30"/>
     <mergeCell ref="B10:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11246,8 +11460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2897401-3DAA-433E-A456-D69455BC7F6F}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11442,26 +11656,26 @@
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="G30" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="G31" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="G32" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
     </row>
   </sheetData>
@@ -18991,7 +19205,7 @@
         <v>478</v>
       </c>
       <c r="I4" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -19012,7 +19226,7 @@
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -19033,7 +19247,7 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -19054,7 +19268,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -19075,7 +19289,7 @@
         <v>-40</v>
       </c>
       <c r="I8" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -19096,7 +19310,7 @@
         <v>478</v>
       </c>
       <c r="I9" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -19117,7 +19331,7 @@
         <v>25</v>
       </c>
       <c r="I10" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -19138,7 +19352,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -19159,7 +19373,7 @@
         <v>0</v>
       </c>
       <c r="I12" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -19180,7 +19394,7 @@
         <v>-60</v>
       </c>
       <c r="I13" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.6.7r: InventoryBar displays weapon
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D18140-ED16-4804-9D26-59C169BBA005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E61EBA-A948-4FDC-9902-1B389F41D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="8" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -3427,12 +3427,6 @@
     <t>passive: heal 1% missing health every 1s, active: heal 7% missing health and gain 35% move speed for 4.5s</t>
   </si>
   <si>
-    <t>Can use half of inventory bar</t>
-  </si>
-  <si>
-    <t>Can use other half of inventory bar</t>
-  </si>
-  <si>
     <t>Inventory +2 slots and unlock inventory</t>
   </si>
   <si>
@@ -3575,6 +3569,12 @@
   </si>
   <si>
     <t>Alkaloid Secretion II</t>
+  </si>
+  <si>
+    <t>Can use half of inventory bar, +3 slots</t>
+  </si>
+  <si>
+    <t>Can use other half of inventory bar, +3 slots</t>
   </si>
 </sst>
 </file>
@@ -10594,8 +10594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G57" sqref="G57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10681,7 +10681,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -10898,7 +10898,7 @@
         <v>944</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="I21" s="21"/>
     </row>
@@ -10917,7 +10917,7 @@
         <v>921</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="I22" s="21"/>
     </row>
@@ -10936,7 +10936,7 @@
         <v>921</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="I23" s="21"/>
     </row>
@@ -10955,7 +10955,7 @@
         <v>921</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="I24" s="21"/>
     </row>
@@ -10974,7 +10974,7 @@
         <v>921</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="I25" s="21"/>
     </row>
@@ -10993,17 +10993,17 @@
         <v>921</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="C27" t="s">
+        <v>999</v>
+      </c>
+      <c r="D27" t="s">
         <v>1001</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1003</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -11012,7 +11012,7 @@
         <v>921</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="I27" s="21"/>
     </row>
@@ -11031,7 +11031,7 @@
         <v>921</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="I28" s="21"/>
     </row>
@@ -11050,7 +11050,7 @@
         <v>921</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="I29" s="21"/>
     </row>
@@ -11069,7 +11069,7 @@
         <v>921</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="I30" s="21"/>
     </row>
@@ -11088,7 +11088,7 @@
         <v>921</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
@@ -11106,7 +11106,7 @@
         <v>921</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -11124,7 +11124,7 @@
         <v>922</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -11142,7 +11142,7 @@
         <v>923</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -11160,7 +11160,7 @@
         <v>924</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -11178,7 +11178,7 @@
         <v>925</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -11196,25 +11196,25 @@
         <v>926</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="C38" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D38" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="E38">
         <v>30</v>
       </c>
       <c r="F38" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -11232,7 +11232,7 @@
         <v>927</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -11250,7 +11250,7 @@
         <v>928</v>
       </c>
       <c r="G40" s="8" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -11268,7 +11268,7 @@
         <v>929</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -11286,7 +11286,7 @@
         <v>930</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -11304,7 +11304,7 @@
         <v>931</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -11324,7 +11324,7 @@
         <v>957</v>
       </c>
       <c r="G45" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
@@ -11396,7 +11396,7 @@
         <v>957</v>
       </c>
       <c r="G49" t="s">
-        <v>975</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
@@ -11414,7 +11414,7 @@
         <v>950</v>
       </c>
       <c r="G50" t="s">
-        <v>976</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
@@ -11434,7 +11434,7 @@
         <v>944</v>
       </c>
       <c r="G52" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
@@ -11445,17 +11445,17 @@
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G57" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G58" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
   </sheetData>
@@ -19164,7 +19164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E132C5F-9A98-41A1-A3AA-2A3458C20EAF}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
@@ -19288,7 +19288,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B8" s="21"/>
       <c r="C8">
@@ -19423,7 +19423,7 @@
         <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>542</v>
@@ -19435,7 +19435,7 @@
         <v>478</v>
       </c>
       <c r="I15" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -19456,7 +19456,7 @@
         <v>10</v>
       </c>
       <c r="I16" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -19477,19 +19477,19 @@
         <v>20</v>
       </c>
       <c r="I17" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18">
         <v>114</v>
       </c>
       <c r="D18" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="E18" t="s">
         <v>543</v>
@@ -19522,7 +19522,7 @@
         <v>60</v>
       </c>
       <c r="I19" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -19531,7 +19531,7 @@
         <v>116</v>
       </c>
       <c r="D20" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>543</v>
@@ -19543,7 +19543,7 @@
         <v>478</v>
       </c>
       <c r="I20" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -19564,7 +19564,7 @@
         <v>15</v>
       </c>
       <c r="I21" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -19576,7 +19576,7 @@
         <v>540</v>
       </c>
       <c r="E22" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="F22" t="s">
         <v>475</v>
@@ -19585,7 +19585,7 @@
         <v>30</v>
       </c>
       <c r="I22" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -19594,7 +19594,7 @@
         <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="E23" t="s">
         <v>545</v>
@@ -19627,7 +19627,7 @@
         <v>90</v>
       </c>
       <c r="I24" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -19684,7 +19684,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34">

</xml_diff>

<commit_message>
v0.6.7v: Base Achievement logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E61EBA-A948-4FDC-9902-1B389F41D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA20D0D-96D3-497F-BED0-D929C4B4FB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="11" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="1025">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="1026">
   <si>
     <t>ID</t>
   </si>
@@ -3575,6 +3575,9 @@
   </si>
   <si>
     <t>Can use other half of inventory bar, +3 slots</t>
+  </si>
+  <si>
+    <t>CAN_PLAY</t>
   </si>
 </sst>
 </file>
@@ -10594,7 +10597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
   <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
@@ -11475,8 +11478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2897401-3DAA-433E-A456-D69455BC7F6F}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11539,6 +11542,9 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>1025</v>
+      </c>
       <c r="D9">
         <v>14</v>
       </c>
@@ -14341,10 +14347,10 @@
   <dimension ref="A1:Y229"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="L174" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C181" sqref="C181"/>
+      <selection pane="bottomRight" activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.8r: CoD weapon sounds
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{983ABE29-D613-434D-9707-24EDFA53A523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF7E03-971C-4E5F-96D5-B70889A47413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -12024,7 +12024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -14508,16 +14508,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y233"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D66" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q231" sqref="Q231"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5703125" customWidth="1"/>
     <col min="6" max="9" width="9.7109375" customWidth="1"/>
@@ -15227,7 +15227,7 @@
       <c r="C47" t="s">
         <v>37</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="16" t="s">
         <v>30</v>
       </c>
       <c r="L47" s="13" t="s">
@@ -15250,6 +15250,7 @@
       <c r="C48" t="s">
         <v>749</v>
       </c>
+      <c r="D48" s="16"/>
       <c r="E48">
         <v>2</v>
       </c>
@@ -15276,6 +15277,7 @@
       <c r="C49" t="s">
         <v>163</v>
       </c>
+      <c r="D49" s="16"/>
       <c r="E49">
         <v>2</v>
       </c>
@@ -15302,6 +15304,7 @@
       <c r="C50" t="s">
         <v>145</v>
       </c>
+      <c r="D50" s="16"/>
       <c r="E50">
         <v>3</v>
       </c>
@@ -15328,6 +15331,7 @@
       <c r="C51" t="s">
         <v>153</v>
       </c>
+      <c r="D51" s="16"/>
       <c r="E51">
         <v>3</v>
       </c>
@@ -15354,6 +15358,7 @@
       <c r="C52" t="s">
         <v>157</v>
       </c>
+      <c r="D52" s="16"/>
       <c r="E52">
         <v>3</v>
       </c>
@@ -15380,6 +15385,7 @@
       <c r="C53" t="s">
         <v>164</v>
       </c>
+      <c r="D53" s="16"/>
       <c r="E53">
         <v>4</v>
       </c>
@@ -15406,6 +15412,7 @@
       <c r="C54" t="s">
         <v>147</v>
       </c>
+      <c r="D54" s="16"/>
       <c r="E54">
         <v>4</v>
       </c>
@@ -15432,6 +15439,7 @@
       <c r="C55" t="s">
         <v>149</v>
       </c>
+      <c r="D55" s="16"/>
       <c r="E55">
         <v>4</v>
       </c>
@@ -15458,6 +15466,7 @@
       <c r="C56" t="s">
         <v>139</v>
       </c>
+      <c r="D56" s="16"/>
       <c r="E56">
         <v>5</v>
       </c>
@@ -15487,6 +15496,7 @@
       <c r="C57" t="s">
         <v>146</v>
       </c>
+      <c r="D57" s="16"/>
       <c r="E57">
         <v>5</v>
       </c>
@@ -15513,6 +15523,7 @@
       <c r="C58" t="s">
         <v>154</v>
       </c>
+      <c r="D58" s="16"/>
       <c r="E58">
         <v>5</v>
       </c>
@@ -15539,6 +15550,7 @@
       <c r="C59" t="s">
         <v>158</v>
       </c>
+      <c r="D59" s="16"/>
       <c r="E59">
         <v>5</v>
       </c>
@@ -15565,6 +15577,7 @@
       <c r="C60" t="s">
         <v>159</v>
       </c>
+      <c r="D60" s="16"/>
       <c r="E60">
         <v>5</v>
       </c>
@@ -15591,6 +15604,7 @@
       <c r="C61" t="s">
         <v>143</v>
       </c>
+      <c r="D61" s="16"/>
       <c r="E61">
         <v>6</v>
       </c>
@@ -15617,6 +15631,7 @@
       <c r="C62" t="s">
         <v>148</v>
       </c>
+      <c r="D62" s="16"/>
       <c r="E62">
         <v>6</v>
       </c>
@@ -15643,6 +15658,7 @@
       <c r="C63" t="s">
         <v>155</v>
       </c>
+      <c r="D63" s="16"/>
       <c r="E63">
         <v>6</v>
       </c>
@@ -15675,6 +15691,7 @@
       <c r="C64" t="s">
         <v>150</v>
       </c>
+      <c r="D64" s="16"/>
       <c r="E64">
         <v>6</v>
       </c>
@@ -15701,6 +15718,7 @@
       <c r="C65" t="s">
         <v>161</v>
       </c>
+      <c r="D65" s="16"/>
       <c r="E65">
         <v>6</v>
       </c>
@@ -15727,6 +15745,7 @@
       <c r="C66" t="s">
         <v>165</v>
       </c>
+      <c r="D66" s="16"/>
       <c r="E66">
         <v>7</v>
       </c>
@@ -15753,6 +15772,7 @@
       <c r="C67" t="s">
         <v>140</v>
       </c>
+      <c r="D67" s="16"/>
       <c r="E67">
         <v>7</v>
       </c>
@@ -15779,6 +15799,7 @@
       <c r="C68" t="s">
         <v>151</v>
       </c>
+      <c r="D68" s="16"/>
       <c r="E68">
         <v>7</v>
       </c>
@@ -15808,6 +15829,7 @@
       <c r="C69" t="s">
         <v>160</v>
       </c>
+      <c r="D69" s="16"/>
       <c r="E69">
         <v>7</v>
       </c>
@@ -15834,6 +15856,7 @@
       <c r="C70" t="s">
         <v>137</v>
       </c>
+      <c r="D70" s="16"/>
       <c r="E70">
         <v>8</v>
       </c>
@@ -15860,6 +15883,7 @@
       <c r="C71" t="s">
         <v>141</v>
       </c>
+      <c r="D71" s="16"/>
       <c r="E71">
         <v>8</v>
       </c>
@@ -15889,6 +15913,7 @@
       <c r="C72" t="s">
         <v>144</v>
       </c>
+      <c r="D72" s="16"/>
       <c r="E72">
         <v>8</v>
       </c>
@@ -15915,6 +15940,7 @@
       <c r="C73" t="s">
         <v>156</v>
       </c>
+      <c r="D73" s="16"/>
       <c r="E73">
         <v>8</v>
       </c>
@@ -15947,6 +15973,7 @@
       <c r="C74" t="s">
         <v>162</v>
       </c>
+      <c r="D74" s="16"/>
       <c r="E74">
         <v>8</v>
       </c>
@@ -15973,6 +16000,7 @@
       <c r="C75" t="s">
         <v>166</v>
       </c>
+      <c r="D75" s="16"/>
       <c r="E75">
         <v>9</v>
       </c>
@@ -15999,6 +16027,7 @@
       <c r="C76" t="s">
         <v>152</v>
       </c>
+      <c r="D76" s="16"/>
       <c r="E76">
         <v>9</v>
       </c>
@@ -16025,6 +16054,7 @@
       <c r="C77" t="s">
         <v>138</v>
       </c>
+      <c r="D77" s="16"/>
       <c r="E77">
         <v>10</v>
       </c>
@@ -16051,6 +16081,7 @@
       <c r="C78" t="s">
         <v>142</v>
       </c>
+      <c r="D78" s="16"/>
       <c r="E78">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
v0.6.8s: Ranged weapon/use item sound effects
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BF7E03-971C-4E5F-96D5-B70889A47413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F8CCA9-A7C8-4C3D-B752-713B79CBF5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -14509,10 +14509,10 @@
   <dimension ref="A1:Y233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D192" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18085,13 +18085,13 @@
   <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="21"/>

</xml_diff>

<commit_message>
v0.6.8x: Unit walk sound effects
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648A246-89CB-48B1-BAC5-103B4521B8BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F07CF-1A86-4AAE-9E18-E181DB1AF388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -4134,8 +4134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.6.9k: Zombie AI logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Processing4\Programs\Games\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9F07CF-1A86-4AAE-9E18-E181DB1AF388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1708653-15DF-4F7B-9752-F928A8ADF776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -4134,7 +4134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
   <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -13435,8 +13435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13537,6 +13537,9 @@
       <c r="H4">
         <v>2.5</v>
       </c>
+      <c r="L4">
+        <v>1.4</v>
+      </c>
       <c r="N4" t="s">
         <v>1038</v>
       </c>
@@ -13557,6 +13560,9 @@
       <c r="H5">
         <v>1.5</v>
       </c>
+      <c r="L5">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -13587,7 +13593,7 @@
         <v>0</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N6" t="s">
         <v>1044</v>
@@ -13625,7 +13631,7 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -13767,7 +13773,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N20" t="s">
         <v>1036</v>
@@ -13799,7 +13805,7 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="N21" t="s">
         <v>1036</v>
@@ -13828,7 +13834,7 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N22" t="s">
         <v>1036</v>
@@ -13860,7 +13866,7 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N23" t="s">
         <v>1036</v>
@@ -13892,7 +13898,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24" t="s">
         <v>1036</v>
@@ -13912,7 +13918,7 @@
         <v>6</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I25">
         <v>3</v>
@@ -13924,7 +13930,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N25" t="s">
         <v>1036</v>
@@ -13953,7 +13959,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="N26" t="s">
         <v>1036</v>
@@ -13973,7 +13979,7 @@
         <v>8</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -13985,7 +13991,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="N27" t="s">
         <v>1036</v>
@@ -14005,7 +14011,7 @@
         <v>9</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I28">
         <v>3</v>
@@ -14017,7 +14023,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="N28" t="s">
         <v>1036</v>
@@ -14034,7 +14040,7 @@
         <v>10</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I29">
         <v>3</v>
@@ -14046,7 +14052,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="N29" t="s">
         <v>1037</v>

</xml_diff>

<commit_message>
v0.7.1r: Misc changes for outside francis hall
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72852124-B28C-4EF4-867A-47672FCB06EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111FCEC7-DD38-4A38-8988-303195079F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="1071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="1072">
   <si>
     <t>ID</t>
   </si>
@@ -3711,6 +3711,9 @@
   </si>
   <si>
     <t>Connor Giggles</t>
+  </si>
+  <si>
+    <t>Cigar</t>
   </si>
 </sst>
 </file>
@@ -13434,8 +13437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14637,13 +14640,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y233"/>
+  <dimension ref="A1:Y234"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D192" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C230" sqref="C230"/>
+      <selection pane="bottomRight" activeCell="C201" sqref="C201:C202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17642,50 +17645,41 @@
     </row>
     <row r="199" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2931</v>
+        <v>2928</v>
       </c>
       <c r="C199" t="s">
-        <v>238</v>
+        <v>1071</v>
       </c>
       <c r="D199" t="s">
-        <v>279</v>
-      </c>
-      <c r="L199" s="4">
-        <v>2</v>
-      </c>
-      <c r="N199">
-        <v>2.5</v>
-      </c>
-      <c r="W199" t="s">
-        <v>815</v>
+        <v>263</v>
       </c>
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="C200" t="s">
-        <v>280</v>
+        <v>238</v>
       </c>
       <c r="D200" t="s">
         <v>279</v>
       </c>
       <c r="L200" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N200">
-        <v>2</v>
-      </c>
-      <c r="Q200">
-        <v>4</v>
+        <v>2.5</v>
+      </c>
+      <c r="W200" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="201" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="C201" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="D201" t="s">
         <v>279</v>
@@ -17696,41 +17690,47 @@
       <c r="N201">
         <v>2</v>
       </c>
-      <c r="W201" t="s">
-        <v>815</v>
+      <c r="Q201">
+        <v>4</v>
       </c>
     </row>
     <row r="202" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2941</v>
+        <v>2933</v>
       </c>
       <c r="C202" t="s">
-        <v>375</v>
+        <v>283</v>
       </c>
       <c r="D202" t="s">
         <v>279</v>
       </c>
+      <c r="L202" s="4">
+        <v>1</v>
+      </c>
+      <c r="N202">
+        <v>2</v>
+      </c>
+      <c r="W202" t="s">
+        <v>815</v>
+      </c>
     </row>
     <row r="203" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="C203" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D203" t="s">
         <v>279</v>
       </c>
-      <c r="E203">
-        <v>2</v>
-      </c>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="C204" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D204" t="s">
         <v>279</v>
@@ -17741,10 +17741,10 @@
     </row>
     <row r="205" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="C205" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D205" t="s">
         <v>279</v>
@@ -17752,19 +17752,13 @@
       <c r="E205">
         <v>2</v>
       </c>
-      <c r="L205" s="4">
-        <v>3</v>
-      </c>
-      <c r="N205">
-        <v>3.5</v>
-      </c>
     </row>
     <row r="206" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="C206" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D206" t="s">
         <v>279</v>
@@ -17772,13 +17766,19 @@
       <c r="E206">
         <v>2</v>
       </c>
+      <c r="L206" s="4">
+        <v>3</v>
+      </c>
+      <c r="N206">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="207" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="C207" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D207" t="s">
         <v>279</v>
@@ -17789,10 +17789,10 @@
     </row>
     <row r="208" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="C208" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D208" t="s">
         <v>279</v>
@@ -17801,12 +17801,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="C209" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D209" t="s">
         <v>279</v>
@@ -17815,82 +17815,79 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B210">
+        <v>2948</v>
+      </c>
+      <c r="C210" t="s">
+        <v>382</v>
+      </c>
+      <c r="D210" t="s">
+        <v>279</v>
+      </c>
+      <c r="E210">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="211" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B211">
         <v>2961</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C211" t="s">
         <v>284</v>
-      </c>
-      <c r="D210" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="211" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B211">
-        <v>2962</v>
-      </c>
-      <c r="C211" t="s">
-        <v>285</v>
       </c>
       <c r="D211" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="212" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="C212" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="D212" t="s">
         <v>286</v>
       </c>
-      <c r="L212" s="4">
-        <v>1</v>
-      </c>
-      <c r="N212">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="213" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="C213" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D213" t="s">
         <v>286</v>
       </c>
+      <c r="L213" s="4">
+        <v>1</v>
+      </c>
       <c r="N213">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="214" spans="2:17" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="214" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="C214" t="s">
-        <v>847</v>
+        <v>321</v>
       </c>
       <c r="D214" t="s">
         <v>286</v>
       </c>
-      <c r="L214" s="4">
-        <v>1</v>
-      </c>
       <c r="N214">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="215" spans="2:17" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="215" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="C215" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="D215" t="s">
         <v>286</v>
@@ -17902,12 +17899,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="216" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B216">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="C216" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D216" t="s">
         <v>286</v>
@@ -17919,12 +17916,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="217" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B217">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="C217" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="D217" t="s">
         <v>286</v>
@@ -17936,40 +17933,40 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="218" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B218">
+        <v>2968</v>
+      </c>
+      <c r="C218" t="s">
+        <v>850</v>
+      </c>
+      <c r="D218" t="s">
+        <v>286</v>
+      </c>
+      <c r="L218" s="4">
+        <v>1</v>
+      </c>
+      <c r="N218">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="219" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B219">
         <v>2971</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C219" t="s">
         <v>311</v>
-      </c>
-      <c r="D218" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="219" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B219">
-        <v>2972</v>
-      </c>
-      <c r="C219" t="s">
-        <v>312</v>
       </c>
       <c r="D219" t="s">
         <v>306</v>
       </c>
-      <c r="L219" s="4">
-        <v>1</v>
-      </c>
-      <c r="N219">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="220" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B220">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="C220" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D220" t="s">
         <v>306</v>
@@ -17981,29 +17978,29 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="221" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B221">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="C221" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="D221" t="s">
         <v>306</v>
       </c>
-      <c r="E221">
-        <v>2</v>
+      <c r="L221" s="4">
+        <v>1</v>
       </c>
       <c r="N221">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="222" spans="2:17" x14ac:dyDescent="0.25">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="222" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="C222" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="D222" t="s">
         <v>306</v>
@@ -18011,19 +18008,16 @@
       <c r="E222">
         <v>2</v>
       </c>
-      <c r="L222" s="4">
-        <v>2</v>
-      </c>
       <c r="N222">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="223" spans="2:17" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="223" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="C223" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="D223" t="s">
         <v>306</v>
@@ -18032,38 +18026,35 @@
         <v>2</v>
       </c>
       <c r="L223" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="224" spans="2:17" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="N223">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="224" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="C224" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D224" t="s">
         <v>306</v>
       </c>
       <c r="E224">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L224" s="4">
-        <v>3</v>
-      </c>
-      <c r="N224">
-        <v>0.08</v>
-      </c>
-      <c r="Q224">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="C225" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D225" t="s">
         <v>306</v>
@@ -18072,18 +18063,21 @@
         <v>3</v>
       </c>
       <c r="L225" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N225">
-        <v>0.1</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q225">
+        <v>15</v>
       </c>
     </row>
     <row r="226" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="C226" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D226" t="s">
         <v>306</v>
@@ -18095,35 +18089,38 @@
         <v>2</v>
       </c>
       <c r="N226">
-        <v>0.05</v>
-      </c>
-      <c r="Q226">
-        <v>5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="C227" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="D227" t="s">
         <v>306</v>
       </c>
       <c r="E227">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L227" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N227">
+        <v>0.05</v>
+      </c>
+      <c r="Q227">
+        <v>5</v>
       </c>
     </row>
     <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="C228" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="D228" t="s">
         <v>306</v>
@@ -18134,16 +18131,13 @@
       <c r="L228" s="4">
         <v>1</v>
       </c>
-      <c r="Q228">
-        <v>5</v>
-      </c>
     </row>
     <row r="229" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="C229" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D229" t="s">
         <v>306</v>
@@ -18154,53 +18148,73 @@
       <c r="L229" s="4">
         <v>1</v>
       </c>
+      <c r="Q229">
+        <v>5</v>
+      </c>
     </row>
     <row r="230" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="C230" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D230" t="s">
         <v>306</v>
       </c>
       <c r="E230">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L230" s="4">
-        <v>5</v>
-      </c>
-      <c r="N230">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q230">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="231" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B231">
+        <v>2983</v>
+      </c>
+      <c r="C231" t="s">
+        <v>316</v>
+      </c>
+      <c r="D231" t="s">
+        <v>306</v>
+      </c>
+      <c r="E231">
+        <v>5</v>
+      </c>
+      <c r="L231" s="4">
+        <v>5</v>
+      </c>
+      <c r="N231">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q231">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="232" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B232">
         <v>2991</v>
       </c>
-      <c r="C231" t="s">
+      <c r="C232" t="s">
         <v>1042</v>
       </c>
-      <c r="D231" t="s">
+      <c r="D232" t="s">
         <v>1043</v>
       </c>
-      <c r="E231">
+      <c r="E232">
         <v>1</v>
       </c>
-      <c r="K231" s="4"/>
-      <c r="L231"/>
-    </row>
-    <row r="232" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K232" s="4"/>
       <c r="L232"/>
     </row>
     <row r="233" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K233" s="4"/>
       <c r="L233"/>
+    </row>
+    <row r="234" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K234" s="4"/>
+      <c r="L234"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
v0.7.2b: Profile starts with Ben, added background tracks
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F960DDF5-D556-43EB-99B4-797E688B2A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01949355-CF88-4B08-A442-F195574284BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -3698,9 +3698,6 @@
     <t>crows/attacks</t>
   </si>
   <si>
-    <t>70% feather, raw chicken</t>
-  </si>
-  <si>
     <t>Dan Gray</t>
   </si>
   <si>
@@ -3714,6 +3711,9 @@
   </si>
   <si>
     <t>Cigar</t>
+  </si>
+  <si>
+    <t>70% feather, raw chicken (25% extra feather)</t>
   </si>
 </sst>
 </file>
@@ -4162,7 +4162,7 @@
   <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11946,7 +11946,7 @@
   <dimension ref="B2:E12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13437,8 +13437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13650,7 +13650,7 @@
         <v>1.4</v>
       </c>
       <c r="Q7" t="s">
-        <v>1066</v>
+        <v>1071</v>
       </c>
       <c r="R7" t="s">
         <v>1065</v>
@@ -13729,7 +13729,7 @@
         <v>1102</v>
       </c>
       <c r="C11" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E11" t="s">
         <v>450</v>
@@ -13740,7 +13740,7 @@
         <v>1103</v>
       </c>
       <c r="C12" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E12" t="s">
         <v>455</v>
@@ -13784,7 +13784,7 @@
         <v>1116</v>
       </c>
       <c r="C16" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E16" t="s">
         <v>459</v>
@@ -13806,7 +13806,7 @@
         <v>1118</v>
       </c>
       <c r="C18" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="E18" t="s">
         <v>458</v>
@@ -14642,11 +14642,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y234"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H196" sqref="H196"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17648,7 +17648,7 @@
         <v>2928</v>
       </c>
       <c r="C199" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="D199" t="s">
         <v>263</v>

</xml_diff>

<commit_message>
v0.7.2c: Various bug fixes
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01949355-CF88-4B08-A442-F195574284BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD029813-AA18-46AF-BF8B-343DB2133BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="1073">
   <si>
     <t>ID</t>
   </si>
@@ -3714,6 +3714,9 @@
   </si>
   <si>
     <t>70% feather, raw chicken (25% extra feather)</t>
+  </si>
+  <si>
+    <t>Walkable Map Edge</t>
   </si>
 </sst>
 </file>
@@ -4159,10 +4162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
-  <dimension ref="A1:G87"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4212,660 +4215,671 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="19">
-        <v>101</v>
-      </c>
-      <c r="C6" t="s">
-        <v>583</v>
-      </c>
-      <c r="D6" t="s">
-        <v>204</v>
-      </c>
-      <c r="E6">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="19">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1072</v>
+      </c>
+      <c r="E5">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="19">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>583</v>
+      </c>
+      <c r="D7" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="19">
         <v>102</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>584</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
-        <v>103</v>
-      </c>
-      <c r="C8" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>634</v>
+        <v>585</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
+        <v>104</v>
+      </c>
+      <c r="C10" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
         <v>111</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="19">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="19">
         <v>112</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>587</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
-        <v>113</v>
-      </c>
-      <c r="C12" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C15" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C16" t="s">
-        <v>205</v>
+        <v>591</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" t="s">
-        <v>643</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C18" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C20" t="s">
-        <v>638</v>
+        <v>650</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C21" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C22" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C23" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
+        <v>145</v>
+      </c>
+      <c r="C25" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
         <v>151</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="19">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="19">
         <v>152</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="2">
-        <v>153</v>
-      </c>
-      <c r="C27" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C28" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C29" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
+        <v>155</v>
+      </c>
+      <c r="C30" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
         <v>156</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="19">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="19">
         <v>161</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>599</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="2">
-        <v>162</v>
-      </c>
-      <c r="C32" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
+        <v>163</v>
+      </c>
+      <c r="C34" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
         <v>171</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="20">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="20">
         <v>172</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C36" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="2">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
         <v>173</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="20">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="20">
         <v>174</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
         <v>175</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="20">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="20">
         <v>176</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>606</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="2">
-        <v>177</v>
-      </c>
-      <c r="C40" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
+        <v>177</v>
+      </c>
+      <c r="C41" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
         <v>178</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>608</v>
-      </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="19">
-        <v>179</v>
-      </c>
-      <c r="C42" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" s="19">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C43" t="s">
-        <v>645</v>
+        <v>609</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" s="19">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C44" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" s="19">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C45" t="s">
-        <v>647</v>
-      </c>
-      <c r="G45" t="s">
-        <v>1045</v>
+        <v>646</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" s="19">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C46" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="G46" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" s="19">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C47" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="G47" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" s="19">
+        <v>185</v>
+      </c>
+      <c r="C48" t="s">
+        <v>649</v>
+      </c>
+      <c r="G48" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="19">
         <v>191</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>1044</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G49" t="s">
         <v>1048</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="2">
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
         <v>201</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>610</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>207</v>
       </c>
-      <c r="E50">
+      <c r="E51">
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="19">
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="19">
         <v>202</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="2">
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
         <v>203</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="19">
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="19">
         <v>204</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="2">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
         <v>205</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="19">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="19">
         <v>206</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="2">
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
         <v>207</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="2">
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
         <v>211</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>695</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="2">
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
         <v>212</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="2">
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
         <v>213</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="19"/>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="2">
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="19"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
         <v>301</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>621</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>633</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E62" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="2">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
         <v>302</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="2">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
         <v>303</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>623</v>
-      </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="2">
-        <v>304</v>
-      </c>
-      <c r="C64" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C65" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C66" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C67" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C68" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C69" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C70" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C71" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C72" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C73" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="2">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C74" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C75" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C76" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C77" t="s">
-        <v>658</v>
+        <v>625</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C78" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C79" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C80" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C81" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C82" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="2">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C83" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="2">
+        <v>323</v>
+      </c>
+      <c r="C84" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="2">
         <v>324</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="19"/>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="19"/>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12089,8 +12103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H115"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13438,7 +13452,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14643,10 +14657,10 @@
   <dimension ref="A1:Y234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D159" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="F191" sqref="F191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17532,9 +17546,6 @@
       </c>
       <c r="D193" t="s">
         <v>263</v>
-      </c>
-      <c r="E193">
-        <v>2</v>
       </c>
       <c r="N193">
         <v>0.04</v>

</xml_diff>

<commit_message>
v0.7.2u: Fertilized chickens / eggs
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD029813-AA18-46AF-BF8B-343DB2133BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9408F319-EDE4-4F91-B448-03539B5C6C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -30,6 +30,7 @@
     <sheet name="Crafting" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1402" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="1074">
   <si>
     <t>ID</t>
   </si>
@@ -3587,9 +3588,6 @@
     <t>drops</t>
   </si>
   <si>
-    <t>25% chance to become sick for 5s, can also throw which gives it 20% to hatch</t>
-  </si>
-  <si>
     <t>Rotten Flesh</t>
   </si>
   <si>
@@ -3717,6 +3715,12 @@
   </si>
   <si>
     <t>Walkable Map Edge</t>
+  </si>
+  <si>
+    <t>lit when toggled</t>
+  </si>
+  <si>
+    <t>25% chance to become sick for 5s, can also throw which gives it 20% to hatch, fertilized when toggled</t>
   </si>
 </sst>
 </file>
@@ -4220,7 +4224,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -4552,7 +4556,7 @@
         <v>647</v>
       </c>
       <c r="G46" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
@@ -4563,7 +4567,7 @@
         <v>648</v>
       </c>
       <c r="G47" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -4574,7 +4578,7 @@
         <v>649</v>
       </c>
       <c r="G48" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -4582,10 +4586,10 @@
         <v>191</v>
       </c>
       <c r="C49" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G49" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
@@ -12420,7 +12424,7 @@
         <v>2</v>
       </c>
       <c r="H27" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -12428,7 +12432,7 @@
         <v>130</v>
       </c>
       <c r="H28" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -13568,7 +13572,7 @@
         <v>1.4</v>
       </c>
       <c r="Q4" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="R4" t="s">
         <v>1027</v>
@@ -13602,10 +13606,10 @@
         <v>1004</v>
       </c>
       <c r="C6" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D6" t="s">
         <v>1038</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1039</v>
       </c>
       <c r="E6" t="s">
         <v>391</v>
@@ -13629,10 +13633,10 @@
         <v>3</v>
       </c>
       <c r="Q6" t="s">
+        <v>1039</v>
+      </c>
+      <c r="R6" t="s">
         <v>1040</v>
-      </c>
-      <c r="R6" t="s">
-        <v>1041</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -13640,7 +13644,7 @@
         <v>1005</v>
       </c>
       <c r="C7" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D7" t="s">
         <v>738</v>
@@ -13664,10 +13668,10 @@
         <v>1.4</v>
       </c>
       <c r="Q7" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="R7" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -13675,10 +13679,10 @@
         <v>1006</v>
       </c>
       <c r="C8" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D8" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -13743,7 +13747,7 @@
         <v>1102</v>
       </c>
       <c r="C11" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E11" t="s">
         <v>450</v>
@@ -13754,7 +13758,7 @@
         <v>1103</v>
       </c>
       <c r="C12" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E12" t="s">
         <v>455</v>
@@ -13798,7 +13802,7 @@
         <v>1116</v>
       </c>
       <c r="C16" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="E16" t="s">
         <v>459</v>
@@ -13820,7 +13824,7 @@
         <v>1118</v>
       </c>
       <c r="C18" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="E18" t="s">
         <v>458</v>
@@ -13880,7 +13884,7 @@
         <v>0.5</v>
       </c>
       <c r="Q22" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R22" t="s">
         <v>188</v>
@@ -13912,7 +13916,7 @@
         <v>0.5</v>
       </c>
       <c r="Q23" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
@@ -13941,7 +13945,7 @@
         <v>0.7</v>
       </c>
       <c r="Q24" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R24" t="s">
         <v>188</v>
@@ -13973,7 +13977,7 @@
         <v>0.7</v>
       </c>
       <c r="Q25" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R25" t="s">
         <v>192</v>
@@ -14005,7 +14009,7 @@
         <v>1</v>
       </c>
       <c r="Q26" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R26" t="s">
         <v>192</v>
@@ -14037,7 +14041,7 @@
         <v>0.8</v>
       </c>
       <c r="Q27" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
@@ -14066,7 +14070,7 @@
         <v>1.2</v>
       </c>
       <c r="Q28" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R28" t="s">
         <v>189</v>
@@ -14098,7 +14102,7 @@
         <v>1.2</v>
       </c>
       <c r="Q29" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="R29" t="s">
         <v>189</v>
@@ -14130,7 +14134,7 @@
         <v>1.2</v>
       </c>
       <c r="Q30" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
@@ -14159,7 +14163,7 @@
         <v>1.2</v>
       </c>
       <c r="Q31" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
     </row>
   </sheetData>
@@ -14657,10 +14661,10 @@
   <dimension ref="A1:Y234"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D159" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F191" sqref="F191"/>
+      <selection pane="bottomRight" activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15013,7 +15017,7 @@
         <v>10</v>
       </c>
       <c r="W21" t="s">
-        <v>1029</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
@@ -15021,7 +15025,7 @@
         <v>2119</v>
       </c>
       <c r="C22" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H22">
         <v>10</v>
@@ -15030,7 +15034,7 @@
         <v>10</v>
       </c>
       <c r="W22" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
@@ -16021,7 +16025,7 @@
         <v>125</v>
       </c>
       <c r="W70" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
@@ -16219,7 +16223,7 @@
         <v>125</v>
       </c>
       <c r="W77" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
@@ -17659,10 +17663,13 @@
         <v>2928</v>
       </c>
       <c r="C199" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="D199" t="s">
         <v>263</v>
+      </c>
+      <c r="W199" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
@@ -18208,10 +18215,10 @@
         <v>2991</v>
       </c>
       <c r="C232" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D232" t="s">
         <v>1042</v>
-      </c>
-      <c r="D232" t="s">
-        <v>1043</v>
       </c>
       <c r="E232">
         <v>1</v>
@@ -18841,7 +18848,7 @@
         <v>154</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G20">
         <v>20</v>
@@ -19153,7 +19160,7 @@
         <v>155</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="G30">
         <v>30</v>
@@ -19625,16 +19632,16 @@
   <sheetData>
     <row r="2" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>1052</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>1053</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>1054</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -19642,13 +19649,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F3" t="s">
         <v>1056</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>1057</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -19656,7 +19663,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -19664,7 +19671,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -19677,7 +19684,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -19815,7 +19822,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -19823,7 +19830,7 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.3b: Desk rotations, small wooden table
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9408F319-EDE4-4F91-B448-03539B5C6C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA26BB5-91A4-4386-AA4E-B6E7F0C90C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409" uniqueCount="1075">
   <si>
     <t>ID</t>
   </si>
@@ -3721,6 +3721,9 @@
   </si>
   <si>
     <t>25% chance to become sick for 5s, can also throw which gives it 20% to hatch, fertilized when toggled</t>
+  </si>
+  <si>
+    <t>Wooden Table (small)</t>
   </si>
 </sst>
 </file>
@@ -12105,10 +12108,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H115"/>
+  <dimension ref="A1:H119"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12281,210 +12284,220 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>111</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="G14" t="s">
-        <v>672</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="H14" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>112</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="C15" s="23"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="H15" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>113</v>
+        <v>106</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>672</v>
       </c>
       <c r="H16" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>114</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="H17" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>671</v>
+        <v>670</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>322</v>
+        <v>672</v>
+      </c>
+      <c r="H18" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>121</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="G19" t="s">
-        <v>322</v>
+        <v>112</v>
       </c>
       <c r="H19" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="H20" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="H21" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>124</v>
-      </c>
-      <c r="H22" t="s">
-        <v>669</v>
+        <v>115</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>671</v>
+      </c>
+      <c r="G22" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>694</v>
+        <v>215</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="G23" t="s">
-        <v>672</v>
+        <v>322</v>
       </c>
       <c r="H23" t="s">
-        <v>698</v>
+        <v>666</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="H24" t="s">
-        <v>699</v>
+        <v>667</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>127</v>
-      </c>
-      <c r="E25">
-        <v>3</v>
+        <v>123</v>
       </c>
       <c r="H25" t="s">
-        <v>700</v>
+        <v>668</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="H26" t="s">
-        <v>701</v>
+        <v>669</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>694</v>
       </c>
       <c r="E27">
         <v>2</v>
       </c>
+      <c r="G27" t="s">
+        <v>672</v>
+      </c>
       <c r="H27" t="s">
-        <v>1048</v>
+        <v>698</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H28" t="s">
-        <v>1049</v>
+        <v>699</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>131</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>216</v>
+        <v>127</v>
       </c>
       <c r="E29">
         <v>3</v>
       </c>
-      <c r="G29" t="s">
-        <v>322</v>
-      </c>
       <c r="H29" t="s">
-        <v>666</v>
+        <v>700</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H30" t="s">
-        <v>667</v>
+        <v>701</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
-        <v>133</v>
+        <v>129</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>668</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H32" t="s">
-        <v>669</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E33">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G33" t="s">
         <v>322</v>
@@ -12495,62 +12508,68 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="H34" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
-        <v>151</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="D35" t="s">
-        <v>219</v>
-      </c>
-      <c r="E35">
-        <v>2</v>
-      </c>
-      <c r="G35" t="s">
-        <v>676</v>
+        <v>133</v>
       </c>
       <c r="H35" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
-        <v>152</v>
+        <v>134</v>
       </c>
       <c r="H36" t="s">
-        <v>667</v>
+        <v>669</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
-        <v>153</v>
+        <v>141</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>322</v>
       </c>
       <c r="H37" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="H38" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>678</v>
+        <v>677</v>
+      </c>
+      <c r="D39" t="s">
+        <v>219</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>676</v>
       </c>
       <c r="H39" t="s">
         <v>666</v>
@@ -12558,7 +12577,7 @@
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H40" t="s">
         <v>667</v>
@@ -12566,7 +12585,7 @@
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H41" t="s">
         <v>668</v>
@@ -12574,7 +12593,7 @@
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H42" t="s">
         <v>669</v>
@@ -12582,145 +12601,121 @@
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E43">
-        <v>4</v>
-      </c>
-      <c r="G43" t="s">
-        <v>212</v>
+        <v>678</v>
+      </c>
+      <c r="H43" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
-        <v>162</v>
-      </c>
-      <c r="C44" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="E44">
-        <v>4</v>
-      </c>
-      <c r="G44" t="s">
-        <v>212</v>
+        <v>156</v>
+      </c>
+      <c r="H44" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
-        <v>163</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="E45">
-        <v>-1</v>
-      </c>
-      <c r="G45" t="s">
-        <v>212</v>
+        <v>157</v>
+      </c>
+      <c r="H45" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
-        <v>164</v>
-      </c>
-      <c r="C46" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="E46">
-        <v>5</v>
-      </c>
-      <c r="G46" t="s">
-        <v>223</v>
+        <v>158</v>
+      </c>
+      <c r="H46" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D48" t="s">
-        <v>734</v>
+        <v>220</v>
       </c>
       <c r="E48">
         <v>4</v>
       </c>
       <c r="G48" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="E49">
-        <v>7</v>
+        <v>-1</v>
       </c>
       <c r="G49" t="s">
-        <v>325</v>
-      </c>
-      <c r="H49" t="s">
-        <v>679</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E50">
-        <v>7</v>
-      </c>
-      <c r="H50" t="s">
-        <v>680</v>
+        <v>5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E51">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G51" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>735</v>
+        <v>225</v>
+      </c>
+      <c r="D52" t="s">
+        <v>734</v>
       </c>
       <c r="E52">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G52" t="s">
         <v>226</v>
@@ -12728,44 +12723,44 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G53" t="s">
-        <v>226</v>
+        <v>325</v>
+      </c>
+      <c r="H53" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E54">
-        <v>4</v>
-      </c>
-      <c r="G54" t="s">
-        <v>226</v>
+        <v>7</v>
+      </c>
+      <c r="H54" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="D55" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="E55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
         <v>226</v>
@@ -12773,13 +12768,13 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>229</v>
+        <v>735</v>
       </c>
       <c r="E56">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G56" t="s">
         <v>226</v>
@@ -12787,13 +12782,13 @@
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E57">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G57" t="s">
         <v>226</v>
@@ -12801,13 +12796,13 @@
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="E58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G58" t="s">
         <v>226</v>
@@ -12815,383 +12810,400 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>213</v>
+        <v>228</v>
+      </c>
+      <c r="D59" t="s">
+        <v>217</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G59" t="s">
-        <v>681</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>715</v>
+        <v>229</v>
       </c>
       <c r="E60">
-        <v>5</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="H60" t="s">
-        <v>666</v>
+        <v>4</v>
+      </c>
+      <c r="G60" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
-        <v>192</v>
-      </c>
-      <c r="H61" t="s">
-        <v>668</v>
+        <v>183</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="G61" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>716</v>
-      </c>
-      <c r="H62" t="s">
-        <v>666</v>
+        <v>231</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="G62" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
-        <v>194</v>
-      </c>
-      <c r="H63" t="s">
-        <v>668</v>
+        <v>185</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D64" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="E64">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="G64" s="8" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H64" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
-        <v>202</v>
-      </c>
-      <c r="C65" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="E65">
-        <v>6</v>
-      </c>
-      <c r="G65" s="8"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B66" s="2" t="s">
-        <v>718</v>
+        <v>192</v>
+      </c>
+      <c r="H65" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
+        <v>193</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D66" t="s">
-        <v>720</v>
-      </c>
-      <c r="E66">
-        <v>7</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="H66" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B67" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="C67" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="E67">
-        <v>9</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>472</v>
+        <v>666</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="2">
+        <v>194</v>
       </c>
       <c r="H67" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D68" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="E68">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G68" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="H68" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
-        <v>252</v>
+        <v>202</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E69">
+        <v>6</v>
       </c>
       <c r="G69" s="8"/>
-      <c r="H69" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D70" t="s">
+        <v>720</v>
+      </c>
+      <c r="E70">
+        <v>7</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="H70" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>685</v>
+        <v>719</v>
       </c>
       <c r="C71" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D71" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="E71">
-        <v>100</v>
-      </c>
-      <c r="G71" t="s">
-        <v>682</v>
+        <v>9</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H71" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
-        <v>311</v>
+        <v>251</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>210</v>
+        <v>241</v>
+      </c>
+      <c r="D72" t="s">
+        <v>733</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>472</v>
       </c>
       <c r="H72" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
-        <v>312</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G73" s="8"/>
       <c r="H73" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="2">
-        <v>321</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="D74" t="s">
-        <v>684</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="G74" t="s">
-        <v>689</v>
-      </c>
-      <c r="H74" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="2">
-        <v>322</v>
+        <v>668</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D75" t="s">
+        <v>207</v>
       </c>
       <c r="E75">
         <v>100</v>
       </c>
       <c r="G75" t="s">
+        <v>682</v>
+      </c>
+      <c r="H75" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>311</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="H76" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>312</v>
+      </c>
+      <c r="H77" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>321</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="D78" t="s">
+        <v>684</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="G78" t="s">
+        <v>689</v>
+      </c>
+      <c r="H78" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="2">
+        <v>322</v>
+      </c>
+      <c r="E79">
+        <v>100</v>
+      </c>
+      <c r="G79" t="s">
         <v>690</v>
       </c>
-      <c r="H75" t="s">
+      <c r="H79" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="2">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
         <v>323</v>
       </c>
-      <c r="G76" t="s">
+      <c r="G80" t="s">
         <v>691</v>
       </c>
-      <c r="H76" t="s">
+      <c r="H80" t="s">
         <v>688</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="4"/>
-      <c r="B77" s="2">
-        <v>331</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>846</v>
-      </c>
-      <c r="D77" t="s">
-        <v>702</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="G77" t="s">
-        <v>689</v>
-      </c>
-      <c r="H77" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="2">
-        <v>332</v>
-      </c>
-      <c r="H78" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
-      <c r="B79" s="2">
-        <v>333</v>
-      </c>
-      <c r="H79" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-      <c r="B80" s="2">
-        <v>334</v>
-      </c>
-      <c r="H80" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="2">
-        <v>335</v>
+        <v>331</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>846</v>
+      </c>
+      <c r="D81" t="s">
+        <v>702</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="G81" t="s">
+        <v>689</v>
       </c>
       <c r="H81" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H82" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="2">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H83" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H84" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="2">
-        <v>339</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="E85">
-        <v>100</v>
-      </c>
-      <c r="G85" t="s">
-        <v>690</v>
+        <v>335</v>
       </c>
       <c r="H85" t="s">
-        <v>666</v>
+        <v>707</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H86" t="s">
-        <v>668</v>
+        <v>708</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H87" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H88" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C89" s="15" t="s">
-        <v>712</v>
+        <v>711</v>
+      </c>
+      <c r="E89">
+        <v>100</v>
       </c>
       <c r="G89" t="s">
-        <v>736</v>
+        <v>690</v>
       </c>
       <c r="H89" t="s">
         <v>666</v>
@@ -13200,7 +13212,7 @@
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H90" t="s">
         <v>668</v>
@@ -13209,7 +13221,7 @@
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="H91" t="s">
         <v>713</v>
@@ -13218,236 +13230,279 @@
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H92" t="s">
         <v>714</v>
       </c>
     </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="4"/>
+      <c r="B93" s="2">
+        <v>343</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="G93" t="s">
+        <v>736</v>
+      </c>
+      <c r="H93" t="s">
+        <v>666</v>
+      </c>
+    </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="4"/>
       <c r="B94" s="2">
-        <v>401</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D94" t="s">
-        <v>286</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="G94" t="s">
-        <v>287</v>
+        <v>344</v>
+      </c>
+      <c r="H94" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="4"/>
       <c r="B95" s="2">
-        <v>411</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="E95">
-        <v>0</v>
-      </c>
-      <c r="G95" t="s">
-        <v>288</v>
+        <v>345</v>
       </c>
       <c r="H95" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="4"/>
       <c r="B96" s="2">
-        <v>412</v>
-      </c>
-      <c r="G96" t="s">
-        <v>289</v>
+        <v>346</v>
       </c>
       <c r="H96" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="2">
-        <v>421</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="E97">
-        <v>20</v>
-      </c>
-      <c r="G97" t="s">
-        <v>323</v>
+        <v>714</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="C98" s="15" t="s">
-        <v>726</v>
+        <v>284</v>
+      </c>
+      <c r="D98" t="s">
+        <v>286</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="G98" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>727</v>
+        <v>650</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>288</v>
+      </c>
+      <c r="H99" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
-        <v>424</v>
-      </c>
-      <c r="C100" s="15" t="s">
-        <v>728</v>
+        <v>412</v>
+      </c>
+      <c r="G100" t="s">
+        <v>289</v>
+      </c>
+      <c r="H100" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C101" s="15" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="E101">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="G101" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>753</v>
-      </c>
-      <c r="E102">
-        <v>20</v>
+        <v>726</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C103" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E103">
-        <v>7</v>
+        <v>727</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B104" s="19">
-        <v>441</v>
+      <c r="B104" s="2">
+        <v>424</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="E104">
-        <v>5</v>
-      </c>
-      <c r="G104" t="s">
-        <v>324</v>
-      </c>
-      <c r="H104" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="2">
-        <v>442</v>
-      </c>
-      <c r="H105" t="s">
-        <v>731</v>
+        <v>425</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="E105">
+        <v>35</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="2">
-        <v>443</v>
-      </c>
-      <c r="H106" t="s">
-        <v>732</v>
+        <v>426</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E106">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B107" s="2">
+        <v>431</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E107">
+        <v>7</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="2">
-        <v>501</v>
+      <c r="B108" s="19">
+        <v>441</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D108" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E108">
         <v>5</v>
       </c>
+      <c r="G108" t="s">
+        <v>324</v>
+      </c>
+      <c r="H108" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="2">
-        <v>502</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>244</v>
+        <v>442</v>
+      </c>
+      <c r="H109" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="2">
-        <v>503</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="2">
-        <v>504</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>246</v>
+        <v>443</v>
+      </c>
+      <c r="H110" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="2">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>247</v>
+        <v>243</v>
+      </c>
+      <c r="D112" t="s">
+        <v>242</v>
+      </c>
+      <c r="E112">
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" s="2">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E113">
-        <v>9</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B114" s="2">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B115" s="2">
+        <v>504</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B116" s="2">
+        <v>505</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B117" s="2">
+        <v>511</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E117">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B118" s="2">
+        <v>512</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B119" s="2">
         <v>513</v>
       </c>
-      <c r="C115" s="15" t="s">
+      <c r="C119" s="15" t="s">
         <v>250</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14660,11 +14715,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y234"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W22" sqref="W22"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.7.3d: Added fruit, bread, scissors
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BAA0E4-A171-40B4-B75B-6275FA6C0250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8542E235-1922-4952-B39C-5803A3A74639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="1077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1082">
   <si>
     <t>ID</t>
   </si>
@@ -3730,6 +3730,21 @@
   </si>
   <si>
     <t>TV</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Pear</t>
+  </si>
+  <si>
+    <t>Scissors</t>
+  </si>
+  <si>
+    <t>Bread</t>
   </si>
 </sst>
 </file>
@@ -12116,7 +12131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G60" sqref="G60"/>
     </sheetView>
   </sheetViews>
@@ -14744,13 +14759,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y234"/>
+  <dimension ref="A1:Y239"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14932,10 +14947,10 @@
         <v>73</v>
       </c>
       <c r="H9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -15125,651 +15140,596 @@
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23">
-        <v>2131</v>
+        <v>2120</v>
       </c>
       <c r="C23" t="s">
-        <v>85</v>
+        <v>1077</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I23">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24">
-        <v>2132</v>
+        <v>2121</v>
       </c>
       <c r="C24" t="s">
-        <v>81</v>
+        <v>1078</v>
       </c>
       <c r="H24">
+        <v>16</v>
+      </c>
+      <c r="I24">
         <v>6</v>
-      </c>
-      <c r="I24">
-        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25">
-        <v>2133</v>
+        <v>2122</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>1079</v>
       </c>
       <c r="H25">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I25">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26">
-        <v>2134</v>
+        <v>2123</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
+        <v>1081</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="I26">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>2141</v>
+        <v>2131</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="F27">
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
       </c>
       <c r="I27">
-        <v>50</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>2142</v>
+        <v>2132</v>
       </c>
       <c r="C28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28">
-        <v>3</v>
-      </c>
-      <c r="F28">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="H28">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="I28">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2151</v>
+        <v>2133</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
+        <v>82</v>
+      </c>
+      <c r="H29">
+        <v>6</v>
+      </c>
+      <c r="I29">
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>2152</v>
+        <v>2134</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
-      </c>
-      <c r="G30">
-        <v>5</v>
+        <v>83</v>
+      </c>
+      <c r="H30">
+        <v>8</v>
+      </c>
+      <c r="I30">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>2153</v>
+        <v>2141</v>
       </c>
       <c r="C31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31">
+        <v>86</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
         <v>10</v>
+      </c>
+      <c r="I31">
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32">
+        <v>2142</v>
+      </c>
+      <c r="C32" t="s">
+        <v>87</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>35</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>2151</v>
+      </c>
+      <c r="C33" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>2152</v>
+      </c>
+      <c r="C34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>2153</v>
+      </c>
+      <c r="C35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36">
         <v>2154</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C36" t="s">
         <v>91</v>
       </c>
-      <c r="G32">
+      <c r="G36">
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B33">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37">
         <v>2155</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C37" t="s">
         <v>92</v>
       </c>
-      <c r="E33">
+      <c r="E37">
         <v>2</v>
       </c>
-      <c r="G33">
+      <c r="G37">
         <v>101</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B34">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38">
         <v>2156</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C38" t="s">
         <v>93</v>
       </c>
-      <c r="E34">
+      <c r="E38">
         <v>2</v>
       </c>
-      <c r="G34">
+      <c r="G38">
         <v>500</v>
       </c>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B35">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39">
         <v>2157</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C39" t="s">
         <v>96</v>
       </c>
-      <c r="E35">
+      <c r="E39">
         <v>2</v>
       </c>
-      <c r="G35">
+      <c r="G39">
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B36">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40">
         <v>2158</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" t="s">
         <v>94</v>
       </c>
-      <c r="E36">
+      <c r="E40">
         <v>2</v>
       </c>
-      <c r="G36">
+      <c r="G40">
         <v>5000</v>
       </c>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B37">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41">
         <v>2159</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C41" t="s">
         <v>95</v>
       </c>
-      <c r="E37">
+      <c r="E41">
         <v>3</v>
       </c>
-      <c r="G37">
+      <c r="G41">
         <v>10100</v>
       </c>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B39">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B43">
         <v>2201</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C43" t="s">
         <v>274</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D43" t="s">
         <v>27</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L43" s="4">
         <v>1</v>
-      </c>
-      <c r="N39">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B40">
-        <v>2202</v>
-      </c>
-      <c r="C40" t="s">
-        <v>21</v>
-      </c>
-      <c r="L40" s="4">
-        <v>1</v>
-      </c>
-      <c r="N40">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41">
-        <v>2203</v>
-      </c>
-      <c r="C41" t="s">
-        <v>271</v>
-      </c>
-      <c r="L41" s="4">
-        <v>2</v>
-      </c>
-      <c r="N41">
-        <v>0.01</v>
-      </c>
-      <c r="Q41">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42">
-        <v>2204</v>
-      </c>
-      <c r="C42" t="s">
-        <v>270</v>
-      </c>
-      <c r="L42" s="4">
-        <v>3</v>
-      </c>
-      <c r="N42">
-        <v>0.08</v>
-      </c>
-      <c r="Q42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B43">
-        <v>2211</v>
-      </c>
-      <c r="C43" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="L43" s="4">
-        <v>7</v>
       </c>
       <c r="N43">
         <v>0.15</v>
       </c>
-      <c r="Q43">
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>2202</v>
+      </c>
+      <c r="C44" t="s">
+        <v>21</v>
+      </c>
+      <c r="L44" s="4">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>2203</v>
+      </c>
+      <c r="C45" t="s">
+        <v>271</v>
+      </c>
+      <c r="L45" s="4">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>0.01</v>
+      </c>
+      <c r="Q45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B46">
+        <v>2204</v>
+      </c>
+      <c r="C46" t="s">
+        <v>270</v>
+      </c>
+      <c r="L46" s="4">
+        <v>3</v>
+      </c>
+      <c r="N46">
+        <v>0.08</v>
+      </c>
+      <c r="Q46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>2211</v>
+      </c>
+      <c r="C47" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="L47" s="4">
+        <v>7</v>
+      </c>
+      <c r="N47">
+        <v>0.15</v>
+      </c>
+      <c r="Q47">
         <v>8</v>
       </c>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B44">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B48">
         <v>2212</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C48" t="s">
         <v>272</v>
       </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="L44" s="4">
-        <v>4</v>
-      </c>
-      <c r="N44">
-        <v>0.05</v>
-      </c>
-      <c r="Q44">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B45">
-        <v>2213</v>
-      </c>
-      <c r="C45" t="s">
-        <v>273</v>
-      </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="L45" s="4">
-        <v>5</v>
-      </c>
-      <c r="N45">
-        <v>0.3</v>
-      </c>
-      <c r="Q45">
-        <v>18</v>
-      </c>
-      <c r="S45">
-        <v>-0.8</v>
-      </c>
-    </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>2301</v>
-      </c>
-      <c r="C47" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>855</v>
-      </c>
-      <c r="N47">
-        <v>3.5</v>
-      </c>
-      <c r="U47">
-        <v>1</v>
-      </c>
-      <c r="W47" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B48">
-        <v>2311</v>
-      </c>
-      <c r="C48" t="s">
-        <v>745</v>
-      </c>
-      <c r="D48" s="15"/>
       <c r="E48">
         <v>2</v>
       </c>
-      <c r="L48" s="13" t="s">
-        <v>856</v>
+      <c r="L48" s="4">
+        <v>4</v>
       </c>
       <c r="N48">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="Q48">
-        <v>15</v>
-      </c>
-      <c r="U48">
-        <v>1</v>
-      </c>
-      <c r="W48" t="s">
-        <v>817</v>
+        <v>8</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>2312</v>
+        <v>2213</v>
       </c>
       <c r="C49" t="s">
-        <v>162</v>
-      </c>
-      <c r="D49" s="15"/>
+        <v>273</v>
+      </c>
       <c r="E49">
         <v>2</v>
       </c>
       <c r="L49" s="4">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="N49">
-        <v>6</v>
+        <v>0.3</v>
       </c>
       <c r="Q49">
-        <v>12</v>
-      </c>
-      <c r="U49">
-        <v>8</v>
-      </c>
-      <c r="W49" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B50">
-        <v>2321</v>
-      </c>
-      <c r="C50" t="s">
-        <v>144</v>
-      </c>
-      <c r="D50" s="15"/>
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="L50" s="4">
-        <v>200</v>
-      </c>
-      <c r="N50">
-        <v>10</v>
-      </c>
-      <c r="Q50">
-        <v>10</v>
-      </c>
-      <c r="U50">
-        <v>6</v>
-      </c>
-      <c r="W50" t="s">
-        <v>356</v>
+        <v>18</v>
+      </c>
+      <c r="S49">
+        <v>-0.8</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>2322</v>
+        <v>2301</v>
       </c>
       <c r="C51" t="s">
-        <v>152</v>
-      </c>
-      <c r="D51" s="15"/>
-      <c r="E51">
-        <v>3</v>
-      </c>
-      <c r="L51" s="4" t="s">
-        <v>340</v>
+        <v>36</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L51" s="13" t="s">
+        <v>855</v>
       </c>
       <c r="N51">
-        <v>7</v>
-      </c>
-      <c r="Q51">
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="U51">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="W51" t="s">
-        <v>363</v>
+        <v>816</v>
       </c>
     </row>
     <row r="52" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B52">
-        <v>2323</v>
+        <v>2311</v>
       </c>
       <c r="C52" t="s">
-        <v>156</v>
+        <v>745</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52">
-        <v>3</v>
-      </c>
-      <c r="L52" s="4" t="s">
-        <v>342</v>
+        <v>2</v>
+      </c>
+      <c r="L52" s="13" t="s">
+        <v>856</v>
       </c>
       <c r="N52">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q52">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="U52">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W52" t="s">
-        <v>367</v>
+        <v>817</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>2331</v>
+        <v>2312</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L53" s="4">
-        <v>1000</v>
+        <v>20</v>
       </c>
       <c r="N53">
+        <v>6</v>
+      </c>
+      <c r="Q53">
         <v>12</v>
       </c>
-      <c r="Q53">
-        <v>5</v>
-      </c>
       <c r="U53">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W53" t="s">
-        <v>852</v>
+        <v>349</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>2332</v>
+        <v>2321</v>
       </c>
       <c r="C54" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54">
-        <v>4</v>
-      </c>
-      <c r="L54" s="4" t="s">
-        <v>337</v>
+        <v>3</v>
+      </c>
+      <c r="L54" s="4">
+        <v>200</v>
       </c>
       <c r="N54">
         <v>10</v>
       </c>
       <c r="Q54">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U54">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W54" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>2333</v>
+        <v>2322</v>
       </c>
       <c r="C55" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="N55">
         <v>7</v>
       </c>
       <c r="Q55">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U55">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W55" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2341</v>
+        <v>2323</v>
       </c>
       <c r="C56" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56">
-        <v>5</v>
-      </c>
-      <c r="L56" s="4">
-        <v>600</v>
+        <v>3</v>
+      </c>
+      <c r="L56" s="4" t="s">
+        <v>342</v>
       </c>
       <c r="N56">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q56">
-        <v>6</v>
-      </c>
-      <c r="S56">
-        <v>-1</v>
+        <v>18</v>
       </c>
       <c r="U56">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="W56" t="s">
-        <v>354</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>2342</v>
+        <v>2331</v>
       </c>
       <c r="C57" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L57" s="4">
-        <v>600</v>
+        <v>1000</v>
       </c>
       <c r="N57">
         <v>12</v>
       </c>
       <c r="Q57">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="U57">
         <v>6</v>
       </c>
       <c r="W57" t="s">
-        <v>357</v>
+        <v>852</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>2343</v>
+        <v>2332</v>
       </c>
       <c r="C58" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="N58">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q58">
         <v>15</v>
@@ -15778,1233 +15738,1279 @@
         <v>20</v>
       </c>
       <c r="W58" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>2344</v>
+        <v>2333</v>
       </c>
       <c r="C59" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="N59">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q59">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U59">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="W59" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>2345</v>
+        <v>2341</v>
       </c>
       <c r="C60" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60">
         <v>5</v>
       </c>
-      <c r="L60" s="4" t="s">
-        <v>345</v>
+      <c r="L60" s="4">
+        <v>600</v>
       </c>
       <c r="N60">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q60">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="S60">
+        <v>-1</v>
       </c>
       <c r="U60">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="W60" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2351</v>
+        <v>2342</v>
       </c>
       <c r="C61" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61">
+        <v>5</v>
+      </c>
+      <c r="L61" s="4">
+        <v>600</v>
+      </c>
+      <c r="N61">
+        <v>12</v>
+      </c>
+      <c r="Q61">
+        <v>15</v>
+      </c>
+      <c r="U61">
         <v>6</v>
       </c>
-      <c r="L61" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="N61">
-        <v>10</v>
-      </c>
-      <c r="Q61">
-        <v>16</v>
-      </c>
-      <c r="U61">
-        <v>35</v>
-      </c>
       <c r="W61" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2352</v>
+        <v>2343</v>
       </c>
       <c r="C62" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="N62">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q62">
+        <v>15</v>
+      </c>
+      <c r="U62">
         <v>20</v>
       </c>
-      <c r="U62">
-        <v>30</v>
-      </c>
       <c r="W62" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2353</v>
+        <v>2344</v>
       </c>
       <c r="C63" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63">
-        <v>6</v>
-      </c>
-      <c r="L63" s="4">
-        <v>500</v>
+        <v>5</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="N63">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q63">
-        <v>25</v>
-      </c>
-      <c r="S63">
-        <v>1</v>
-      </c>
-      <c r="T63">
-        <v>0.1</v>
+        <v>24</v>
       </c>
       <c r="U63">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="W63" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>2354</v>
+        <v>2345</v>
       </c>
       <c r="C64" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="N64">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q64">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U64">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="W64" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2355</v>
+        <v>2351</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
       <c r="D65" s="15"/>
       <c r="E65">
         <v>6</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="N65">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q65">
         <v>16</v>
       </c>
       <c r="U65">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W65" t="s">
-        <v>369</v>
+        <v>352</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>2361</v>
+        <v>2352</v>
       </c>
       <c r="C66" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D66" s="15"/>
       <c r="E66">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="N66">
         <v>11</v>
       </c>
       <c r="Q66">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U66">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="W66" t="s">
-        <v>348</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>2362</v>
+        <v>2353</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67">
+        <v>6</v>
+      </c>
+      <c r="L67" s="4">
+        <v>500</v>
+      </c>
+      <c r="N67">
         <v>7</v>
       </c>
-      <c r="L67" s="4">
-        <v>1200</v>
-      </c>
-      <c r="N67">
-        <v>12</v>
-      </c>
       <c r="Q67">
-        <v>8</v>
+        <v>25</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+      <c r="T67">
+        <v>0.1</v>
       </c>
       <c r="U67">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W67" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>2363</v>
+        <v>2354</v>
       </c>
       <c r="C68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68">
+        <v>6</v>
+      </c>
+      <c r="L68" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="N68">
         <v>7</v>
       </c>
-      <c r="L68" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="N68">
-        <v>16</v>
-      </c>
       <c r="Q68">
-        <v>30</v>
-      </c>
-      <c r="S68">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="U68">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="W68" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>2364</v>
+        <v>2355</v>
       </c>
       <c r="C69" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L69" s="4" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="N69">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="Q69">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="U69">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="W69" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>2371</v>
+        <v>2361</v>
       </c>
       <c r="C70" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N70">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q70">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="U70">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="W70" t="s">
-        <v>1035</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>2372</v>
+        <v>2362</v>
       </c>
       <c r="C71" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71">
+        <v>7</v>
+      </c>
+      <c r="L71" s="4">
+        <v>1200</v>
+      </c>
+      <c r="N71">
+        <v>12</v>
+      </c>
+      <c r="Q71">
         <v>8</v>
       </c>
-      <c r="L71" s="4">
-        <v>500</v>
-      </c>
-      <c r="M71">
-        <v>500</v>
-      </c>
-      <c r="N71">
-        <v>9</v>
-      </c>
-      <c r="R71">
+      <c r="U71">
         <v>8</v>
       </c>
-      <c r="U71">
-        <v>20</v>
-      </c>
       <c r="W71" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>2373</v>
+        <v>2363</v>
       </c>
       <c r="C72" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="N72">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="Q72">
-        <v>22</v>
+        <v>30</v>
+      </c>
+      <c r="S72">
+        <v>-1</v>
       </c>
       <c r="U72">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="W72" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>2374</v>
+        <v>2364</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73">
-        <v>8</v>
-      </c>
-      <c r="L73" s="4">
-        <v>1000</v>
+        <v>7</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="N73">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Q73">
-        <v>35</v>
-      </c>
-      <c r="S73">
-        <v>1.5</v>
-      </c>
-      <c r="T73">
-        <v>0.15</v>
+        <v>12</v>
       </c>
       <c r="U73">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W73" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="74" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>2375</v>
+        <v>2371</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>136</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74">
         <v>8</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="N74">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q74">
         <v>20</v>
       </c>
       <c r="U74">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="W74" t="s">
-        <v>370</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>2381</v>
+        <v>2372</v>
       </c>
       <c r="C75" t="s">
-        <v>165</v>
+        <v>140</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="L75" s="4">
+        <v>500</v>
+      </c>
+      <c r="M75">
+        <v>500</v>
+      </c>
+      <c r="N75">
         <v>9</v>
       </c>
-      <c r="L75" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="N75">
-        <v>12</v>
-      </c>
-      <c r="Q75">
+      <c r="R75">
+        <v>8</v>
+      </c>
+      <c r="U75">
         <v>20</v>
       </c>
-      <c r="U75">
-        <v>125</v>
-      </c>
       <c r="W75" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>2382</v>
+        <v>2373</v>
       </c>
       <c r="C76" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76">
-        <v>9</v>
-      </c>
-      <c r="L76" s="4">
-        <v>1000</v>
+        <v>8</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>336</v>
       </c>
       <c r="N76">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="Q76">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="U76">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="W76" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>2391</v>
+        <v>2374</v>
       </c>
       <c r="C77" t="s">
-        <v>137</v>
+        <v>155</v>
       </c>
       <c r="D77" s="15"/>
       <c r="E77">
-        <v>10</v>
-      </c>
-      <c r="L77" s="4" t="s">
-        <v>334</v>
+        <v>8</v>
+      </c>
+      <c r="L77" s="4">
+        <v>1000</v>
       </c>
       <c r="N77">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="Q77">
-        <v>25</v>
+        <v>35</v>
+      </c>
+      <c r="S77">
+        <v>1.5</v>
+      </c>
+      <c r="T77">
+        <v>0.15</v>
       </c>
       <c r="U77">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="W77" t="s">
-        <v>1036</v>
+        <v>366</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>2392</v>
+        <v>2375</v>
       </c>
       <c r="C78" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78">
-        <v>10</v>
-      </c>
-      <c r="L78" s="4">
-        <v>500</v>
-      </c>
-      <c r="M78">
-        <v>500</v>
+        <v>8</v>
+      </c>
+      <c r="L78" s="4" t="s">
+        <v>344</v>
       </c>
       <c r="N78">
+        <v>12</v>
+      </c>
+      <c r="Q78">
+        <v>20</v>
+      </c>
+      <c r="U78">
+        <v>30</v>
+      </c>
+      <c r="W78" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="79" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>2381</v>
+      </c>
+      <c r="C79" t="s">
+        <v>165</v>
+      </c>
+      <c r="D79" s="15"/>
+      <c r="E79">
         <v>9</v>
       </c>
-      <c r="R78">
+      <c r="L79" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="N79">
         <v>12</v>
       </c>
-      <c r="U78">
-        <v>40</v>
-      </c>
-      <c r="W78" t="s">
-        <v>351</v>
+      <c r="Q79">
+        <v>20</v>
+      </c>
+      <c r="U79">
+        <v>125</v>
+      </c>
+      <c r="W79" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80">
+        <v>2382</v>
+      </c>
+      <c r="C80" t="s">
+        <v>151</v>
+      </c>
+      <c r="D80" s="15"/>
+      <c r="E80">
+        <v>9</v>
+      </c>
+      <c r="L80" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N80">
+        <v>18</v>
+      </c>
+      <c r="Q80">
+        <v>45</v>
+      </c>
+      <c r="U80">
+        <v>8</v>
+      </c>
+      <c r="W80" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="81" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B81">
+        <v>2391</v>
+      </c>
+      <c r="C81" t="s">
+        <v>137</v>
+      </c>
+      <c r="D81" s="15"/>
+      <c r="E81">
+        <v>10</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="N81">
+        <v>11</v>
+      </c>
+      <c r="Q81">
+        <v>25</v>
+      </c>
+      <c r="U81">
+        <v>125</v>
+      </c>
+      <c r="W81" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="82" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B82">
+        <v>2392</v>
+      </c>
+      <c r="C82" t="s">
+        <v>141</v>
+      </c>
+      <c r="D82" s="15"/>
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="L82" s="4">
+        <v>500</v>
+      </c>
+      <c r="M82">
+        <v>500</v>
+      </c>
+      <c r="N82">
+        <v>9</v>
+      </c>
+      <c r="R82">
+        <v>12</v>
+      </c>
+      <c r="U82">
+        <v>40</v>
+      </c>
+      <c r="W82" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="84" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B84">
         <v>2401</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C84" t="s">
         <v>97</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D84" t="s">
         <v>22</v>
       </c>
-      <c r="O80">
+      <c r="O84">
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B81">
+    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B85">
         <v>2402</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C85" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B82">
+    <row r="86" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B86">
         <v>2403</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C86" t="s">
         <v>168</v>
       </c>
-      <c r="O82">
+      <c r="O86">
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B83">
+    <row r="87" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B87">
         <v>2404</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C87" t="s">
         <v>167</v>
       </c>
-      <c r="O83">
+      <c r="O87">
         <v>2</v>
       </c>
-      <c r="S83">
+      <c r="S87">
         <v>-0.5</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B84">
+    <row r="88" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B88">
         <v>2411</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C88" t="s">
         <v>98</v>
       </c>
-      <c r="E84">
+      <c r="E88">
         <v>2</v>
       </c>
-      <c r="O84">
+      <c r="O88">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B85">
+    <row r="89" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B89">
         <v>2421</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C89" t="s">
         <v>99</v>
       </c>
-      <c r="E85">
+      <c r="E89">
         <v>3</v>
       </c>
-      <c r="O85">
+      <c r="O89">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B86">
+    <row r="90" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B90">
         <v>2431</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C90" t="s">
         <v>100</v>
       </c>
-      <c r="E86">
+      <c r="E90">
         <v>4</v>
       </c>
-      <c r="O86">
+      <c r="O90">
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B87">
+    <row r="91" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B91">
         <v>2441</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C91" t="s">
         <v>101</v>
       </c>
-      <c r="E87">
+      <c r="E91">
         <v>5</v>
       </c>
-      <c r="O87">
+      <c r="O91">
         <v>48</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B88">
+    <row r="92" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B92">
         <v>2451</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C92" t="s">
         <v>102</v>
       </c>
-      <c r="E88">
+      <c r="E92">
         <v>6</v>
       </c>
-      <c r="O88">
+      <c r="O92">
         <v>72</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B89">
+    <row r="93" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B93">
         <v>2461</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C93" t="s">
         <v>103</v>
       </c>
-      <c r="E89">
+      <c r="E93">
         <v>7</v>
       </c>
-      <c r="O89">
+      <c r="O93">
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B90">
+    <row r="94" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B94">
         <v>2471</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C94" t="s">
         <v>104</v>
       </c>
-      <c r="E90">
+      <c r="E94">
         <v>8</v>
       </c>
-      <c r="O90">
+      <c r="O94">
         <v>200</v>
       </c>
     </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B91">
+    <row r="95" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B95">
         <v>2481</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C95" t="s">
         <v>105</v>
       </c>
-      <c r="E91">
+      <c r="E95">
         <v>9</v>
       </c>
-      <c r="O91">
+      <c r="O95">
         <v>400</v>
       </c>
     </row>
-    <row r="92" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B92">
+    <row r="96" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B96">
         <v>2491</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C96" t="s">
         <v>106</v>
       </c>
-      <c r="E92">
+      <c r="E96">
         <v>10</v>
       </c>
-      <c r="O92">
+      <c r="O96">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B94">
-        <v>2501</v>
-      </c>
-      <c r="C94" t="s">
-        <v>803</v>
-      </c>
-      <c r="D94" t="s">
-        <v>23</v>
-      </c>
-      <c r="O94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B95">
-        <v>2502</v>
-      </c>
-      <c r="C95" t="s">
-        <v>169</v>
-      </c>
-      <c r="N95">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B96">
-        <v>2503</v>
-      </c>
-      <c r="C96" t="s">
-        <v>170</v>
-      </c>
-      <c r="N96">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B97">
-        <v>2504</v>
-      </c>
-      <c r="C97" t="s">
-        <v>171</v>
-      </c>
-      <c r="N97">
-        <v>0.04</v>
-      </c>
-      <c r="O97">
-        <v>1</v>
       </c>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2511</v>
+        <v>2501</v>
       </c>
       <c r="C98" t="s">
-        <v>804</v>
-      </c>
-      <c r="E98">
-        <v>2</v>
+        <v>803</v>
+      </c>
+      <c r="D98" t="s">
+        <v>23</v>
       </c>
       <c r="O98">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>2512</v>
+        <v>2502</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
-      </c>
-      <c r="E99">
-        <v>2</v>
-      </c>
-      <c r="K99">
-        <v>3</v>
+        <v>169</v>
       </c>
       <c r="N99">
-        <v>0.05</v>
-      </c>
-      <c r="O99">
-        <v>2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2513</v>
+        <v>2503</v>
       </c>
       <c r="C100" t="s">
-        <v>302</v>
+        <v>170</v>
       </c>
       <c r="N100">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2521</v>
+        <v>2504</v>
       </c>
       <c r="C101" t="s">
-        <v>805</v>
-      </c>
-      <c r="E101">
-        <v>3</v>
+        <v>171</v>
+      </c>
+      <c r="N101">
+        <v>0.04</v>
       </c>
       <c r="O101">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2531</v>
+        <v>2511</v>
       </c>
       <c r="C102" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O102">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2541</v>
+        <v>2512</v>
       </c>
       <c r="C103" t="s">
-        <v>808</v>
+        <v>179</v>
       </c>
       <c r="E103">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="K103">
+        <v>3</v>
+      </c>
+      <c r="N103">
+        <v>0.05</v>
       </c>
       <c r="O103">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>2551</v>
+        <v>2513</v>
       </c>
       <c r="C104" t="s">
-        <v>807</v>
-      </c>
-      <c r="E104">
-        <v>6</v>
-      </c>
-      <c r="O104">
-        <v>72</v>
+        <v>302</v>
+      </c>
+      <c r="N104">
+        <v>0.04</v>
       </c>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>2561</v>
+        <v>2521</v>
       </c>
       <c r="C105" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="E105">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O105">
-        <v>100</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2571</v>
+        <v>2531</v>
       </c>
       <c r="C106" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="E106">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O106">
-        <v>200</v>
+        <v>21</v>
       </c>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2581</v>
+        <v>2541</v>
       </c>
       <c r="C107" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="E107">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O107">
-        <v>400</v>
+        <v>48</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2591</v>
+        <v>2551</v>
       </c>
       <c r="C108" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
       <c r="E108">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O108">
-        <v>1500</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B109">
+        <v>2561</v>
+      </c>
+      <c r="C109" t="s">
+        <v>809</v>
+      </c>
+      <c r="E109">
+        <v>7</v>
+      </c>
+      <c r="O109">
+        <v>100</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2601</v>
+        <v>2571</v>
       </c>
       <c r="C110" t="s">
-        <v>107</v>
-      </c>
-      <c r="D110" t="s">
-        <v>24</v>
+        <v>810</v>
+      </c>
+      <c r="E110">
+        <v>8</v>
       </c>
       <c r="O110">
-        <v>1</v>
+        <v>200</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2602</v>
+        <v>2581</v>
       </c>
       <c r="C111" t="s">
-        <v>172</v>
-      </c>
-      <c r="N111">
-        <v>0.02</v>
+        <v>812</v>
+      </c>
+      <c r="E111">
+        <v>9</v>
+      </c>
+      <c r="O111">
+        <v>400</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112">
+        <v>2591</v>
+      </c>
+      <c r="C112" t="s">
+        <v>811</v>
+      </c>
+      <c r="E112">
+        <v>10</v>
+      </c>
+      <c r="O112">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B114">
+        <v>2601</v>
+      </c>
+      <c r="C114" t="s">
+        <v>107</v>
+      </c>
+      <c r="D114" t="s">
+        <v>24</v>
+      </c>
+      <c r="O114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>2602</v>
+      </c>
+      <c r="C115" t="s">
+        <v>172</v>
+      </c>
+      <c r="N115">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B116">
         <v>2603</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C116" t="s">
         <v>174</v>
       </c>
-      <c r="N112">
+      <c r="N116">
         <v>0.06</v>
       </c>
     </row>
-    <row r="113" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B113">
+    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B117">
         <v>2604</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C117" t="s">
         <v>173</v>
       </c>
-      <c r="N113">
+      <c r="N117">
         <v>0.08</v>
       </c>
-      <c r="O113">
+      <c r="O117">
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B114">
+    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B118">
         <v>2611</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C118" t="s">
         <v>108</v>
       </c>
-      <c r="E114">
+      <c r="E118">
         <v>2</v>
       </c>
-      <c r="O114">
+      <c r="O118">
         <v>2</v>
       </c>
     </row>
-    <row r="115" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B115">
+    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B119">
         <v>2621</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C119" t="s">
         <v>109</v>
       </c>
-      <c r="E115">
+      <c r="E119">
         <v>3</v>
       </c>
-      <c r="O115">
+      <c r="O119">
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B116">
+    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B120">
         <v>2631</v>
       </c>
-      <c r="C116" t="s">
+      <c r="C120" t="s">
         <v>110</v>
       </c>
-      <c r="E116">
+      <c r="E120">
         <v>4</v>
       </c>
-      <c r="O116">
+      <c r="O120">
         <v>21</v>
       </c>
     </row>
-    <row r="117" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B117">
+    <row r="121" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B121">
         <v>2641</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C121" t="s">
         <v>743</v>
       </c>
-      <c r="E117">
+      <c r="E121">
         <v>5</v>
       </c>
-      <c r="O117">
+      <c r="O121">
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B118">
+    <row r="122" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B122">
         <v>2651</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C122" t="s">
         <v>111</v>
       </c>
-      <c r="E118">
+      <c r="E122">
         <v>6</v>
       </c>
-      <c r="O118">
+      <c r="O122">
         <v>72</v>
       </c>
     </row>
-    <row r="119" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B119">
+    <row r="123" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B123">
         <v>2661</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C123" t="s">
         <v>112</v>
       </c>
-      <c r="E119">
+      <c r="E123">
         <v>7</v>
       </c>
-      <c r="O119">
+      <c r="O123">
         <v>100</v>
       </c>
     </row>
-    <row r="120" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B120">
+    <row r="124" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B124">
         <v>2671</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C124" t="s">
         <v>113</v>
       </c>
-      <c r="E120">
+      <c r="E124">
         <v>8</v>
       </c>
-      <c r="O120">
+      <c r="O124">
         <v>200</v>
       </c>
     </row>
-    <row r="121" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B121">
+    <row r="125" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B125">
         <v>2681</v>
       </c>
-      <c r="C121" t="s">
+      <c r="C125" t="s">
         <v>114</v>
       </c>
-      <c r="E121">
+      <c r="E125">
         <v>9</v>
       </c>
-      <c r="O121">
+      <c r="O125">
         <v>400</v>
       </c>
     </row>
-    <row r="122" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B122">
+    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B126">
         <v>2691</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C126" t="s">
         <v>115</v>
       </c>
-      <c r="E122">
+      <c r="E126">
         <v>10</v>
       </c>
-      <c r="O122">
+      <c r="O126">
         <v>1500</v>
       </c>
     </row>
-    <row r="124" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B124">
+    <row r="128" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B128">
         <v>2701</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C128" t="s">
         <v>116</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D128" t="s">
         <v>25</v>
       </c>
-      <c r="O124">
+      <c r="O128">
         <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B125">
-        <v>2702</v>
-      </c>
-      <c r="C125" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="126" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B126">
-        <v>2703</v>
-      </c>
-      <c r="C126" t="s">
-        <v>176</v>
-      </c>
-      <c r="S126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>2704</v>
-      </c>
-      <c r="C127" t="s">
-        <v>177</v>
-      </c>
-      <c r="O127">
-        <v>1</v>
-      </c>
-      <c r="S127">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B128">
-        <v>2705</v>
-      </c>
-      <c r="C128" t="s">
-        <v>303</v>
-      </c>
-      <c r="O128">
-        <v>2</v>
-      </c>
-      <c r="S128">
-        <v>2</v>
       </c>
     </row>
     <row r="129" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>2711</v>
+        <v>2702</v>
       </c>
       <c r="C129" t="s">
-        <v>117</v>
-      </c>
-      <c r="E129">
-        <v>2</v>
-      </c>
-      <c r="O129">
-        <v>2</v>
+        <v>175</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2712</v>
+        <v>2703</v>
       </c>
       <c r="C130" t="s">
-        <v>178</v>
-      </c>
-      <c r="E130">
-        <v>2</v>
-      </c>
-      <c r="O130">
+        <v>176</v>
+      </c>
+      <c r="S130">
         <v>1</v>
-      </c>
-      <c r="S130">
-        <v>3</v>
       </c>
     </row>
     <row r="131" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2713</v>
+        <v>2704</v>
       </c>
       <c r="C131" t="s">
-        <v>304</v>
-      </c>
-      <c r="E131">
-        <v>2</v>
-      </c>
-      <c r="L131" s="4">
+        <v>177</v>
+      </c>
+      <c r="O131">
         <v>1</v>
-      </c>
-      <c r="O131">
-        <v>3</v>
       </c>
       <c r="S131">
         <v>2</v>
@@ -17012,599 +17018,617 @@
     </row>
     <row r="132" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2714</v>
+        <v>2705</v>
       </c>
       <c r="C132" t="s">
-        <v>305</v>
-      </c>
-      <c r="E132">
-        <v>2</v>
+        <v>303</v>
       </c>
       <c r="O132">
         <v>2</v>
       </c>
       <c r="S132">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2721</v>
+        <v>2711</v>
       </c>
       <c r="C133" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E133">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O133">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2731</v>
+        <v>2712</v>
       </c>
       <c r="C134" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="E134">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O134">
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="S134">
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2741</v>
+        <v>2713</v>
       </c>
       <c r="C135" t="s">
-        <v>120</v>
+        <v>304</v>
       </c>
       <c r="E135">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="L135" s="4">
+        <v>1</v>
       </c>
       <c r="O135">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="S135">
+        <v>2</v>
       </c>
     </row>
     <row r="136" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B136">
-        <v>2751</v>
+        <v>2714</v>
       </c>
       <c r="C136" t="s">
-        <v>121</v>
+        <v>305</v>
       </c>
       <c r="E136">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="O136">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="S136">
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>2761</v>
+        <v>2721</v>
       </c>
       <c r="C137" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E137">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O137">
-        <v>100</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2771</v>
+        <v>2731</v>
       </c>
       <c r="C138" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E138">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="O138">
-        <v>200</v>
+        <v>21</v>
       </c>
     </row>
     <row r="139" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2781</v>
+        <v>2741</v>
       </c>
       <c r="C139" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E139">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O139">
-        <v>400</v>
+        <v>48</v>
       </c>
     </row>
     <row r="140" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2791</v>
+        <v>2751</v>
       </c>
       <c r="C140" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E140">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="O140">
-        <v>1500</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="141" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B141">
+        <v>2761</v>
+      </c>
+      <c r="C141" t="s">
+        <v>122</v>
+      </c>
+      <c r="E141">
+        <v>7</v>
+      </c>
+      <c r="O141">
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2801</v>
+        <v>2771</v>
       </c>
       <c r="C142" t="s">
-        <v>772</v>
-      </c>
-      <c r="D142" t="s">
-        <v>26</v>
+        <v>123</v>
+      </c>
+      <c r="E142">
+        <v>8</v>
+      </c>
+      <c r="O142">
+        <v>200</v>
       </c>
     </row>
     <row r="143" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>2802</v>
+        <v>2781</v>
       </c>
       <c r="C143" t="s">
-        <v>773</v>
+        <v>124</v>
+      </c>
+      <c r="E143">
+        <v>9</v>
+      </c>
+      <c r="O143">
+        <v>400</v>
       </c>
     </row>
     <row r="144" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2803</v>
+        <v>2791</v>
       </c>
       <c r="C144" t="s">
-        <v>774</v>
-      </c>
-    </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145">
-        <v>2804</v>
-      </c>
-      <c r="C145" t="s">
-        <v>766</v>
+        <v>125</v>
+      </c>
+      <c r="E144">
+        <v>10</v>
+      </c>
+      <c r="O144">
+        <v>1500</v>
       </c>
     </row>
     <row r="146" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>2805</v>
+        <v>2801</v>
       </c>
       <c r="C146" t="s">
-        <v>746</v>
+        <v>772</v>
+      </c>
+      <c r="D146" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B147">
-        <v>2806</v>
+        <v>2802</v>
       </c>
       <c r="C147" t="s">
-        <v>300</v>
+        <v>773</v>
       </c>
     </row>
     <row r="148" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2807</v>
+        <v>2803</v>
       </c>
       <c r="C148" t="s">
-        <v>1019</v>
+        <v>774</v>
       </c>
     </row>
     <row r="149" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2808</v>
+        <v>2804</v>
+      </c>
+      <c r="C149" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="150" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2809</v>
+        <v>2805</v>
+      </c>
+      <c r="C150" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="151" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>2810</v>
+        <v>2806</v>
+      </c>
+      <c r="C151" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="152" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>2811</v>
+        <v>2807</v>
       </c>
       <c r="C152" t="s">
-        <v>775</v>
-      </c>
-      <c r="E152">
-        <v>2</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="153" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2812</v>
-      </c>
-      <c r="C153" t="s">
-        <v>776</v>
+        <v>2808</v>
       </c>
     </row>
     <row r="154" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2813</v>
-      </c>
-      <c r="C154" t="s">
-        <v>777</v>
+        <v>2809</v>
       </c>
     </row>
     <row r="155" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>2814</v>
-      </c>
-      <c r="C155" t="s">
-        <v>800</v>
+        <v>2810</v>
       </c>
     </row>
     <row r="156" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>2815</v>
+        <v>2811</v>
       </c>
       <c r="C156" t="s">
-        <v>301</v>
+        <v>775</v>
+      </c>
+      <c r="E156">
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>2821</v>
+        <v>2812</v>
       </c>
       <c r="C157" t="s">
-        <v>778</v>
-      </c>
-      <c r="E157">
-        <v>3</v>
+        <v>776</v>
       </c>
     </row>
     <row r="158" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2822</v>
+        <v>2813</v>
       </c>
       <c r="C158" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="159" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2823</v>
+        <v>2814</v>
       </c>
       <c r="C159" t="s">
-        <v>781</v>
+        <v>800</v>
       </c>
     </row>
     <row r="160" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>2834</v>
+        <v>2815</v>
       </c>
       <c r="C160" t="s">
-        <v>780</v>
+        <v>301</v>
       </c>
     </row>
     <row r="161" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2825</v>
+        <v>2821</v>
       </c>
       <c r="C161" t="s">
-        <v>541</v>
-      </c>
-      <c r="Y161" t="s">
-        <v>201</v>
+        <v>778</v>
+      </c>
+      <c r="E161">
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2831</v>
+        <v>2822</v>
       </c>
       <c r="C162" t="s">
-        <v>782</v>
-      </c>
-      <c r="E162">
-        <v>4</v>
+        <v>779</v>
       </c>
     </row>
     <row r="163" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2832</v>
+        <v>2823</v>
       </c>
       <c r="C163" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="164" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2841</v>
+        <v>2834</v>
       </c>
       <c r="C164" t="s">
-        <v>785</v>
-      </c>
-      <c r="E164">
-        <v>5</v>
+        <v>780</v>
       </c>
     </row>
     <row r="165" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2842</v>
+        <v>2825</v>
       </c>
       <c r="C165" t="s">
-        <v>784</v>
+        <v>541</v>
+      </c>
+      <c r="Y165" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2851</v>
+        <v>2831</v>
       </c>
       <c r="C166" t="s">
-        <v>786</v>
+        <v>782</v>
       </c>
       <c r="E166">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="167" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2852</v>
+        <v>2832</v>
       </c>
       <c r="C167" t="s">
-        <v>792</v>
+        <v>783</v>
       </c>
     </row>
     <row r="168" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2853</v>
+        <v>2841</v>
       </c>
       <c r="C168" t="s">
-        <v>787</v>
+        <v>785</v>
+      </c>
+      <c r="E168">
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2861</v>
+        <v>2842</v>
       </c>
       <c r="C169" t="s">
-        <v>788</v>
-      </c>
-      <c r="E169">
-        <v>7</v>
+        <v>784</v>
       </c>
     </row>
     <row r="170" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2862</v>
+        <v>2851</v>
       </c>
       <c r="C170" t="s">
-        <v>793</v>
+        <v>786</v>
+      </c>
+      <c r="E170">
+        <v>6</v>
       </c>
     </row>
     <row r="171" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2863</v>
+        <v>2852</v>
       </c>
       <c r="C171" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
     </row>
     <row r="172" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2864</v>
+        <v>2853</v>
       </c>
       <c r="C172" t="s">
-        <v>299</v>
+        <v>787</v>
       </c>
     </row>
     <row r="173" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2871</v>
+        <v>2861</v>
       </c>
       <c r="C173" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="E173">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="174" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2872</v>
+        <v>2862</v>
       </c>
       <c r="C174" t="s">
-        <v>797</v>
+        <v>793</v>
       </c>
     </row>
     <row r="175" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B175">
-        <v>2873</v>
+        <v>2863</v>
       </c>
       <c r="C175" t="s">
-        <v>801</v>
+        <v>794</v>
       </c>
     </row>
     <row r="176" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B176">
-        <v>2881</v>
+        <v>2864</v>
       </c>
       <c r="C176" t="s">
-        <v>790</v>
-      </c>
-      <c r="E176">
-        <v>9</v>
+        <v>299</v>
       </c>
     </row>
     <row r="177" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B177">
-        <v>2882</v>
+        <v>2871</v>
       </c>
       <c r="C177" t="s">
-        <v>799</v>
+        <v>789</v>
+      </c>
+      <c r="E177">
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B178">
-        <v>2883</v>
+        <v>2872</v>
       </c>
       <c r="C178" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
     </row>
     <row r="179" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2891</v>
+        <v>2873</v>
       </c>
       <c r="C179" t="s">
-        <v>791</v>
-      </c>
-      <c r="E179">
-        <v>10</v>
+        <v>801</v>
       </c>
     </row>
     <row r="180" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2892</v>
+        <v>2881</v>
       </c>
       <c r="C180" t="s">
-        <v>135</v>
+        <v>790</v>
+      </c>
+      <c r="E180">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="181" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B181">
+        <v>2882</v>
+      </c>
+      <c r="C181" t="s">
+        <v>799</v>
       </c>
     </row>
     <row r="182" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2901</v>
+        <v>2883</v>
       </c>
       <c r="C182" t="s">
-        <v>251</v>
-      </c>
-      <c r="D182" t="s">
-        <v>251</v>
-      </c>
-      <c r="W182" t="s">
-        <v>254</v>
+        <v>802</v>
       </c>
     </row>
     <row r="183" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2902</v>
+        <v>2891</v>
       </c>
       <c r="C183" t="s">
-        <v>253</v>
-      </c>
-      <c r="D183" t="s">
-        <v>251</v>
+        <v>791</v>
       </c>
       <c r="E183">
-        <v>2</v>
-      </c>
-      <c r="W183" t="s">
-        <v>255</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2903</v>
+        <v>2892</v>
       </c>
       <c r="C184" t="s">
-        <v>252</v>
-      </c>
-      <c r="D184" t="s">
-        <v>251</v>
-      </c>
-      <c r="E184">
-        <v>3</v>
-      </c>
-      <c r="W184" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="185" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B185">
-        <v>2911</v>
-      </c>
-      <c r="C185" t="s">
-        <v>258</v>
-      </c>
-      <c r="D185" t="s">
-        <v>257</v>
-      </c>
-      <c r="H185" s="6"/>
-      <c r="L185" s="4">
-        <v>1</v>
+        <v>135</v>
       </c>
     </row>
     <row r="186" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2912</v>
+        <v>2901</v>
       </c>
       <c r="C186" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D186" t="s">
-        <v>257</v>
-      </c>
-      <c r="L186" s="4">
-        <v>1</v>
+        <v>251</v>
+      </c>
+      <c r="W186" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="187" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B187">
-        <v>2913</v>
+        <v>2902</v>
       </c>
       <c r="C187" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D187" t="s">
-        <v>257</v>
+        <v>251</v>
+      </c>
+      <c r="E187">
+        <v>2</v>
+      </c>
+      <c r="W187" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2914</v>
+        <v>2903</v>
       </c>
       <c r="C188" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="D188" t="s">
-        <v>257</v>
+        <v>251</v>
+      </c>
+      <c r="E188">
+        <v>3</v>
+      </c>
+      <c r="W188" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="189" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2915</v>
+        <v>2911</v>
       </c>
       <c r="C189" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D189" t="s">
         <v>257</v>
       </c>
+      <c r="H189" s="6"/>
       <c r="L189" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="190" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2916</v>
+        <v>2912</v>
       </c>
       <c r="C190" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="D190" t="s">
         <v>257</v>
       </c>
+      <c r="L190" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="191" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2917</v>
+        <v>2913</v>
       </c>
       <c r="C191" t="s">
-        <v>742</v>
+        <v>260</v>
       </c>
       <c r="D191" t="s">
         <v>257</v>
@@ -17612,305 +17636,290 @@
     </row>
     <row r="192" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2921</v>
+        <v>2914</v>
       </c>
       <c r="C192" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D192" t="s">
-        <v>263</v>
-      </c>
-      <c r="N192">
-        <v>0.04</v>
-      </c>
-      <c r="W192" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="193" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2922</v>
+        <v>2915</v>
       </c>
       <c r="C193" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D193" t="s">
-        <v>263</v>
-      </c>
-      <c r="N193">
-        <v>0.04</v>
-      </c>
-      <c r="W193" t="s">
-        <v>269</v>
+        <v>257</v>
+      </c>
+      <c r="L193" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="194" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2923</v>
+        <v>2916</v>
       </c>
       <c r="C194" t="s">
-        <v>266</v>
+        <v>290</v>
       </c>
       <c r="D194" t="s">
-        <v>263</v>
-      </c>
-      <c r="N194">
-        <v>0.04</v>
-      </c>
-      <c r="W194" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C195" t="s">
-        <v>291</v>
+        <v>742</v>
       </c>
       <c r="D195" t="s">
-        <v>263</v>
-      </c>
-      <c r="L195" s="4">
-        <v>1</v>
-      </c>
-      <c r="N195">
-        <v>2.5</v>
-      </c>
-      <c r="Q195">
-        <v>6</v>
-      </c>
-      <c r="W195" t="s">
-        <v>298</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2925</v>
+        <v>2918</v>
       </c>
       <c r="C196" t="s">
-        <v>292</v>
+        <v>1080</v>
       </c>
       <c r="D196" t="s">
-        <v>263</v>
-      </c>
-      <c r="W196" t="s">
-        <v>295</v>
+        <v>257</v>
+      </c>
+      <c r="L196" s="4">
+        <v>1.5</v>
       </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2926</v>
+        <v>2921</v>
       </c>
       <c r="C197" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="D197" t="s">
         <v>263</v>
       </c>
-      <c r="E197">
-        <v>2</v>
-      </c>
-      <c r="L197" s="4">
-        <v>1</v>
-      </c>
       <c r="N197">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="W197" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
     </row>
     <row r="198" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2927</v>
+        <v>2922</v>
       </c>
       <c r="C198" t="s">
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="D198" t="s">
         <v>263</v>
       </c>
-      <c r="E198">
-        <v>3</v>
-      </c>
-      <c r="L198" s="4">
-        <v>2</v>
-      </c>
       <c r="N198">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="W198" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
     </row>
     <row r="199" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2928</v>
+        <v>2923</v>
       </c>
       <c r="C199" t="s">
-        <v>1069</v>
+        <v>266</v>
       </c>
       <c r="D199" t="s">
         <v>263</v>
       </c>
+      <c r="N199">
+        <v>0.04</v>
+      </c>
       <c r="W199" t="s">
-        <v>1072</v>
+        <v>267</v>
       </c>
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2931</v>
+        <v>2924</v>
       </c>
       <c r="C200" t="s">
-        <v>238</v>
+        <v>291</v>
       </c>
       <c r="D200" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="L200" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N200">
         <v>2.5</v>
       </c>
+      <c r="Q200">
+        <v>6</v>
+      </c>
       <c r="W200" t="s">
-        <v>815</v>
+        <v>298</v>
       </c>
     </row>
     <row r="201" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2932</v>
+        <v>2925</v>
       </c>
       <c r="C201" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="D201" t="s">
-        <v>279</v>
-      </c>
-      <c r="L201" s="4">
-        <v>1</v>
-      </c>
-      <c r="N201">
-        <v>2</v>
-      </c>
-      <c r="Q201">
-        <v>4</v>
+        <v>263</v>
+      </c>
+      <c r="W201" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="202" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2933</v>
+        <v>2926</v>
       </c>
       <c r="C202" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="D202" t="s">
-        <v>279</v>
+        <v>263</v>
+      </c>
+      <c r="E202">
+        <v>2</v>
       </c>
       <c r="L202" s="4">
         <v>1</v>
       </c>
       <c r="N202">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="W202" t="s">
-        <v>815</v>
+        <v>296</v>
       </c>
     </row>
     <row r="203" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2941</v>
+        <v>2927</v>
       </c>
       <c r="C203" t="s">
-        <v>375</v>
+        <v>294</v>
       </c>
       <c r="D203" t="s">
-        <v>279</v>
+        <v>263</v>
+      </c>
+      <c r="E203">
+        <v>3</v>
+      </c>
+      <c r="L203" s="4">
+        <v>2</v>
+      </c>
+      <c r="N203">
+        <v>0.02</v>
+      </c>
+      <c r="W203" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2942</v>
+        <v>2928</v>
       </c>
       <c r="C204" t="s">
-        <v>376</v>
+        <v>1069</v>
       </c>
       <c r="D204" t="s">
-        <v>279</v>
-      </c>
-      <c r="E204">
-        <v>2</v>
+        <v>263</v>
+      </c>
+      <c r="W204" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="205" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2943</v>
+        <v>2931</v>
       </c>
       <c r="C205" t="s">
-        <v>377</v>
+        <v>238</v>
       </c>
       <c r="D205" t="s">
         <v>279</v>
       </c>
-      <c r="E205">
+      <c r="L205" s="4">
         <v>2</v>
+      </c>
+      <c r="N205">
+        <v>2.5</v>
+      </c>
+      <c r="W205" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="206" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2944</v>
+        <v>2932</v>
       </c>
       <c r="C206" t="s">
-        <v>378</v>
+        <v>280</v>
       </c>
       <c r="D206" t="s">
         <v>279</v>
       </c>
-      <c r="E206">
+      <c r="L206" s="4">
+        <v>1</v>
+      </c>
+      <c r="N206">
         <v>2</v>
       </c>
-      <c r="L206" s="4">
-        <v>3</v>
-      </c>
-      <c r="N206">
-        <v>3.5</v>
+      <c r="Q206">
+        <v>4</v>
       </c>
     </row>
     <row r="207" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2945</v>
+        <v>2933</v>
       </c>
       <c r="C207" t="s">
-        <v>379</v>
+        <v>283</v>
       </c>
       <c r="D207" t="s">
         <v>279</v>
       </c>
-      <c r="E207">
+      <c r="L207" s="4">
+        <v>1</v>
+      </c>
+      <c r="N207">
         <v>2</v>
+      </c>
+      <c r="W207" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="208" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2946</v>
+        <v>2941</v>
       </c>
       <c r="C208" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D208" t="s">
         <v>279</v>
       </c>
-      <c r="E208">
-        <v>2</v>
-      </c>
     </row>
     <row r="209" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2947</v>
+        <v>2942</v>
       </c>
       <c r="C209" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D209" t="s">
         <v>279</v>
@@ -17921,10 +17930,10 @@
     </row>
     <row r="210" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B210">
-        <v>2948</v>
+        <v>2943</v>
       </c>
       <c r="C210" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="D210" t="s">
         <v>279</v>
@@ -17935,114 +17944,108 @@
     </row>
     <row r="211" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B211">
-        <v>2961</v>
+        <v>2944</v>
       </c>
       <c r="C211" t="s">
-        <v>284</v>
+        <v>378</v>
       </c>
       <c r="D211" t="s">
-        <v>286</v>
+        <v>279</v>
+      </c>
+      <c r="E211">
+        <v>2</v>
+      </c>
+      <c r="L211" s="4">
+        <v>3</v>
+      </c>
+      <c r="N211">
+        <v>3.5</v>
       </c>
     </row>
     <row r="212" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2962</v>
+        <v>2945</v>
       </c>
       <c r="C212" t="s">
-        <v>285</v>
+        <v>379</v>
       </c>
       <c r="D212" t="s">
-        <v>286</v>
+        <v>279</v>
+      </c>
+      <c r="E212">
+        <v>2</v>
       </c>
     </row>
     <row r="213" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2963</v>
+        <v>2946</v>
       </c>
       <c r="C213" t="s">
-        <v>317</v>
+        <v>380</v>
       </c>
       <c r="D213" t="s">
-        <v>286</v>
-      </c>
-      <c r="L213" s="4">
-        <v>1</v>
-      </c>
-      <c r="N213">
-        <v>0.05</v>
+        <v>279</v>
+      </c>
+      <c r="E213">
+        <v>2</v>
       </c>
     </row>
     <row r="214" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2964</v>
+        <v>2947</v>
       </c>
       <c r="C214" t="s">
-        <v>321</v>
+        <v>381</v>
       </c>
       <c r="D214" t="s">
-        <v>286</v>
-      </c>
-      <c r="N214">
-        <v>0.04</v>
+        <v>279</v>
+      </c>
+      <c r="E214">
+        <v>2</v>
       </c>
     </row>
     <row r="215" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2965</v>
+        <v>2948</v>
       </c>
       <c r="C215" t="s">
-        <v>847</v>
+        <v>382</v>
       </c>
       <c r="D215" t="s">
-        <v>286</v>
-      </c>
-      <c r="L215" s="4">
-        <v>1</v>
-      </c>
-      <c r="N215">
-        <v>0.05</v>
+        <v>279</v>
+      </c>
+      <c r="E215">
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B216">
-        <v>2966</v>
+        <v>2961</v>
       </c>
       <c r="C216" t="s">
-        <v>848</v>
+        <v>284</v>
       </c>
       <c r="D216" t="s">
         <v>286</v>
       </c>
-      <c r="L216" s="4">
-        <v>1</v>
-      </c>
-      <c r="N216">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="217" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B217">
-        <v>2967</v>
+        <v>2962</v>
       </c>
       <c r="C217" t="s">
-        <v>849</v>
+        <v>285</v>
       </c>
       <c r="D217" t="s">
         <v>286</v>
       </c>
-      <c r="L217" s="4">
-        <v>1</v>
-      </c>
-      <c r="N217">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="218" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B218">
-        <v>2968</v>
+        <v>2963</v>
       </c>
       <c r="C218" t="s">
-        <v>850</v>
+        <v>317</v>
       </c>
       <c r="D218" t="s">
         <v>286</v>
@@ -18056,61 +18059,64 @@
     </row>
     <row r="219" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B219">
-        <v>2971</v>
+        <v>2964</v>
       </c>
       <c r="C219" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="D219" t="s">
-        <v>306</v>
+        <v>286</v>
+      </c>
+      <c r="N219">
+        <v>0.04</v>
       </c>
     </row>
     <row r="220" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B220">
-        <v>2972</v>
+        <v>2965</v>
       </c>
       <c r="C220" t="s">
-        <v>312</v>
+        <v>847</v>
       </c>
       <c r="D220" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="L220" s="4">
         <v>1</v>
       </c>
       <c r="N220">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="221" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B221">
-        <v>2973</v>
+        <v>2966</v>
       </c>
       <c r="C221" t="s">
-        <v>320</v>
+        <v>848</v>
       </c>
       <c r="D221" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="L221" s="4">
         <v>1</v>
       </c>
       <c r="N221">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="222" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2974</v>
+        <v>2967</v>
       </c>
       <c r="C222" t="s">
-        <v>310</v>
+        <v>849</v>
       </c>
       <c r="D222" t="s">
-        <v>306</v>
-      </c>
-      <c r="E222">
-        <v>2</v>
+        <v>286</v>
+      </c>
+      <c r="L222" s="4">
+        <v>1</v>
       </c>
       <c r="N222">
         <v>0.05</v>
@@ -18118,207 +18124,286 @@
     </row>
     <row r="223" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2975</v>
+        <v>2968</v>
       </c>
       <c r="C223" t="s">
-        <v>318</v>
+        <v>850</v>
       </c>
       <c r="D223" t="s">
-        <v>306</v>
-      </c>
-      <c r="E223">
-        <v>2</v>
+        <v>286</v>
       </c>
       <c r="L223" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N223">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="224" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2976</v>
+        <v>2971</v>
       </c>
       <c r="C224" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D224" t="s">
         <v>306</v>
       </c>
-      <c r="E224">
-        <v>2</v>
-      </c>
-      <c r="L224" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2977</v>
+        <v>2972</v>
       </c>
       <c r="C225" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="D225" t="s">
         <v>306</v>
       </c>
-      <c r="E225">
-        <v>3</v>
-      </c>
       <c r="L225" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N225">
-        <v>0.08</v>
-      </c>
-      <c r="Q225">
-        <v>15</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="226" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2978</v>
+        <v>2973</v>
       </c>
       <c r="C226" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="D226" t="s">
         <v>306</v>
       </c>
-      <c r="E226">
-        <v>3</v>
-      </c>
       <c r="L226" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N226">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2979</v>
+        <v>2974</v>
       </c>
       <c r="C227" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D227" t="s">
         <v>306</v>
       </c>
       <c r="E227">
-        <v>3</v>
-      </c>
-      <c r="L227" s="4">
         <v>2</v>
       </c>
       <c r="N227">
         <v>0.05</v>
       </c>
-      <c r="Q227">
-        <v>5</v>
-      </c>
     </row>
     <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2980</v>
+        <v>2975</v>
       </c>
       <c r="C228" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D228" t="s">
         <v>306</v>
       </c>
       <c r="E228">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L228" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N228">
+        <v>0.02</v>
       </c>
     </row>
     <row r="229" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2981</v>
+        <v>2976</v>
       </c>
       <c r="C229" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D229" t="s">
         <v>306</v>
       </c>
       <c r="E229">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L229" s="4">
         <v>1</v>
       </c>
-      <c r="Q229">
-        <v>5</v>
-      </c>
     </row>
     <row r="230" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2982</v>
+        <v>2977</v>
       </c>
       <c r="C230" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="D230" t="s">
         <v>306</v>
       </c>
       <c r="E230">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L230" s="4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N230">
+        <v>0.08</v>
+      </c>
+      <c r="Q230">
+        <v>15</v>
       </c>
     </row>
     <row r="231" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2983</v>
+        <v>2978</v>
       </c>
       <c r="C231" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="D231" t="s">
         <v>306</v>
       </c>
       <c r="E231">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L231" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N231">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q231">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="232" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B232">
+        <v>2979</v>
+      </c>
+      <c r="C232" t="s">
+        <v>313</v>
+      </c>
+      <c r="D232" t="s">
+        <v>306</v>
+      </c>
+      <c r="E232">
+        <v>3</v>
+      </c>
+      <c r="L232" s="4">
+        <v>2</v>
+      </c>
+      <c r="N232">
+        <v>0.05</v>
+      </c>
+      <c r="Q232">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="233" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B233">
+        <v>2980</v>
+      </c>
+      <c r="C233" t="s">
+        <v>319</v>
+      </c>
+      <c r="D233" t="s">
+        <v>306</v>
+      </c>
+      <c r="E233">
+        <v>4</v>
+      </c>
+      <c r="L233" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B234">
+        <v>2981</v>
+      </c>
+      <c r="C234" t="s">
+        <v>314</v>
+      </c>
+      <c r="D234" t="s">
+        <v>306</v>
+      </c>
+      <c r="E234">
+        <v>4</v>
+      </c>
+      <c r="L234" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q234">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="235" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B235">
+        <v>2982</v>
+      </c>
+      <c r="C235" t="s">
+        <v>315</v>
+      </c>
+      <c r="D235" t="s">
+        <v>306</v>
+      </c>
+      <c r="E235">
+        <v>4</v>
+      </c>
+      <c r="L235" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B236">
+        <v>2983</v>
+      </c>
+      <c r="C236" t="s">
+        <v>316</v>
+      </c>
+      <c r="D236" t="s">
+        <v>306</v>
+      </c>
+      <c r="E236">
+        <v>5</v>
+      </c>
+      <c r="L236" s="4">
+        <v>5</v>
+      </c>
+      <c r="N236">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q236">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="237" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B237">
         <v>2991</v>
       </c>
-      <c r="C232" t="s">
+      <c r="C237" t="s">
         <v>1041</v>
       </c>
-      <c r="D232" t="s">
+      <c r="D237" t="s">
         <v>1042</v>
       </c>
-      <c r="E232">
+      <c r="E237">
         <v>1</v>
       </c>
-      <c r="K232" s="4"/>
-      <c r="L232"/>
-    </row>
-    <row r="233" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K233" s="4"/>
-      <c r="L233"/>
-    </row>
-    <row r="234" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K234" s="4"/>
-      <c r="L234"/>
+      <c r="K237" s="4"/>
+      <c r="L237"/>
+    </row>
+    <row r="238" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K238" s="4"/>
+      <c r="L238"/>
+    </row>
+    <row r="239" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K239" s="4"/>
+      <c r="L239"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
v0.7.3e: Added hot pockets
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8542E235-1922-4952-B39C-5803A3A74639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1579CEBF-82E5-46DC-9411-A35F20D969D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1418" uniqueCount="1082">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="1086">
   <si>
     <t>ID</t>
   </si>
@@ -3745,6 +3745,18 @@
   </si>
   <si>
     <t>Bread</t>
+  </si>
+  <si>
+    <t>Hot Pocket Box</t>
+  </si>
+  <si>
+    <t>Hot Pocket</t>
+  </si>
+  <si>
+    <t>Package</t>
+  </si>
+  <si>
+    <t>Gives stack of 5 hot pockets</t>
   </si>
 </sst>
 </file>
@@ -14759,13 +14771,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y239"/>
+  <dimension ref="A1:Y241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I26" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15196,624 +15208,598 @@
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27">
-        <v>2131</v>
+        <v>2124</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
-      </c>
-      <c r="H27">
-        <v>0</v>
-      </c>
-      <c r="I27">
-        <v>12</v>
+        <v>1082</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1084</v>
+      </c>
+      <c r="W27" t="s">
+        <v>1085</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28">
-        <v>2132</v>
+        <v>2125</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>1083</v>
+      </c>
+      <c r="D28" t="s">
+        <v>28</v>
       </c>
       <c r="H28">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="I28">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29">
-        <v>2133</v>
+        <v>2131</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I29">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30">
-        <v>2134</v>
+        <v>2132</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H30">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I30">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31">
-        <v>2141</v>
+        <v>2133</v>
       </c>
       <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
-      </c>
-      <c r="F31">
-        <v>10</v>
+        <v>82</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
       </c>
       <c r="I31">
-        <v>50</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32">
-        <v>2142</v>
+        <v>2134</v>
       </c>
       <c r="C32" t="s">
-        <v>87</v>
-      </c>
-      <c r="E32">
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <v>30</v>
+        <v>83</v>
       </c>
       <c r="H32">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="I32">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B33">
-        <v>2151</v>
+        <v>2141</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
-      </c>
-      <c r="G33">
-        <v>1</v>
+        <v>86</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B34">
-        <v>2152</v>
+        <v>2142</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34">
-        <v>5</v>
+        <v>87</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="F34">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <v>35</v>
+      </c>
+      <c r="I34">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B35">
-        <v>2153</v>
+        <v>2151</v>
       </c>
       <c r="C35" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G35">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B36">
-        <v>2154</v>
+        <v>2152</v>
       </c>
       <c r="C36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G36">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B37">
-        <v>2155</v>
+        <v>2153</v>
       </c>
       <c r="C37" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
+        <v>90</v>
       </c>
       <c r="G37">
-        <v>101</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B38">
-        <v>2156</v>
+        <v>2154</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="E38">
-        <v>2</v>
+        <v>91</v>
       </c>
       <c r="G38">
-        <v>500</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B39">
-        <v>2157</v>
+        <v>2155</v>
       </c>
       <c r="C39" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
       <c r="G39">
-        <v>1000</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B40">
-        <v>2158</v>
+        <v>2156</v>
       </c>
       <c r="C40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
       <c r="G40">
-        <v>5000</v>
+        <v>500</v>
       </c>
     </row>
     <row r="41" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B41">
-        <v>2159</v>
+        <v>2157</v>
       </c>
       <c r="C41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G41">
-        <v>10100</v>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>2158</v>
+      </c>
+      <c r="C42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>5000</v>
       </c>
     </row>
     <row r="43" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B43">
-        <v>2201</v>
+        <v>2159</v>
       </c>
       <c r="C43" t="s">
-        <v>274</v>
-      </c>
-      <c r="D43" t="s">
-        <v>27</v>
-      </c>
-      <c r="L43" s="4">
-        <v>1</v>
-      </c>
-      <c r="N43">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B44">
-        <v>2202</v>
-      </c>
-      <c r="C44" t="s">
-        <v>21</v>
-      </c>
-      <c r="L44" s="4">
-        <v>1</v>
-      </c>
-      <c r="N44">
-        <v>0.02</v>
+        <v>95</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="G43">
+        <v>10100</v>
       </c>
     </row>
     <row r="45" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>2203</v>
+        <v>2201</v>
       </c>
       <c r="C45" t="s">
-        <v>271</v>
+        <v>274</v>
+      </c>
+      <c r="D45" t="s">
+        <v>27</v>
       </c>
       <c r="L45" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N45">
-        <v>0.01</v>
-      </c>
-      <c r="Q45">
-        <v>4</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="46" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>2204</v>
+        <v>2202</v>
       </c>
       <c r="C46" t="s">
-        <v>270</v>
+        <v>21</v>
       </c>
       <c r="L46" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N46">
-        <v>0.08</v>
-      </c>
-      <c r="Q46">
-        <v>6</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="47" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>2211</v>
+        <v>2203</v>
       </c>
       <c r="C47" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47">
+        <v>271</v>
+      </c>
+      <c r="L47" s="4">
         <v>2</v>
       </c>
-      <c r="L47" s="4">
-        <v>7</v>
-      </c>
       <c r="N47">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="Q47">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>2212</v>
+        <v>2204</v>
       </c>
       <c r="C48" t="s">
-        <v>272</v>
-      </c>
-      <c r="E48">
-        <v>2</v>
+        <v>270</v>
       </c>
       <c r="L48" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N48">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Q48">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B49">
-        <v>2213</v>
+        <v>2211</v>
       </c>
       <c r="C49" t="s">
-        <v>273</v>
+        <v>20</v>
       </c>
       <c r="E49">
         <v>2</v>
       </c>
       <c r="L49" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N49">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="Q49">
-        <v>18</v>
-      </c>
-      <c r="S49">
-        <v>-0.8</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B50">
+        <v>2212</v>
+      </c>
+      <c r="C50" t="s">
+        <v>272</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="L50" s="4">
+        <v>4</v>
+      </c>
+      <c r="N50">
+        <v>0.05</v>
+      </c>
+      <c r="Q50">
+        <v>8</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>2301</v>
+        <v>2213</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L51" s="13" t="s">
-        <v>855</v>
+        <v>273</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="L51" s="4">
+        <v>5</v>
       </c>
       <c r="N51">
-        <v>3.5</v>
-      </c>
-      <c r="U51">
-        <v>1</v>
-      </c>
-      <c r="W51" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B52">
-        <v>2311</v>
-      </c>
-      <c r="C52" t="s">
-        <v>745</v>
-      </c>
-      <c r="D52" s="15"/>
-      <c r="E52">
-        <v>2</v>
-      </c>
-      <c r="L52" s="13" t="s">
-        <v>856</v>
-      </c>
-      <c r="N52">
-        <v>5</v>
-      </c>
-      <c r="Q52">
-        <v>15</v>
-      </c>
-      <c r="U52">
-        <v>1</v>
-      </c>
-      <c r="W52" t="s">
-        <v>817</v>
+        <v>0.3</v>
+      </c>
+      <c r="Q51">
+        <v>18</v>
+      </c>
+      <c r="S51">
+        <v>-0.8</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>2312</v>
+        <v>2301</v>
       </c>
       <c r="C53" t="s">
-        <v>162</v>
-      </c>
-      <c r="D53" s="15"/>
-      <c r="E53">
-        <v>2</v>
-      </c>
-      <c r="L53" s="4">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>855</v>
       </c>
       <c r="N53">
-        <v>6</v>
-      </c>
-      <c r="Q53">
-        <v>12</v>
+        <v>3.5</v>
       </c>
       <c r="U53">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W53" t="s">
-        <v>349</v>
+        <v>816</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>2321</v>
+        <v>2311</v>
       </c>
       <c r="C54" t="s">
-        <v>144</v>
+        <v>745</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54">
-        <v>3</v>
-      </c>
-      <c r="L54" s="4">
-        <v>200</v>
+        <v>2</v>
+      </c>
+      <c r="L54" s="13" t="s">
+        <v>856</v>
       </c>
       <c r="N54">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q54">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="U54">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W54" t="s">
-        <v>356</v>
+        <v>817</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>2322</v>
+        <v>2312</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D55" s="15"/>
       <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="L55" s="4" t="s">
-        <v>340</v>
+        <v>2</v>
+      </c>
+      <c r="L55" s="4">
+        <v>20</v>
       </c>
       <c r="N55">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q55">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U55">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="W55" t="s">
-        <v>363</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2323</v>
+        <v>2321</v>
       </c>
       <c r="C56" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56">
         <v>3</v>
       </c>
-      <c r="L56" s="4" t="s">
-        <v>342</v>
+      <c r="L56" s="4">
+        <v>200</v>
       </c>
       <c r="N56">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q56">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="U56">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="W56" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
     </row>
     <row r="57" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B57">
-        <v>2331</v>
+        <v>2322</v>
       </c>
       <c r="C57" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57">
-        <v>4</v>
-      </c>
-      <c r="L57" s="4">
-        <v>1000</v>
+        <v>3</v>
+      </c>
+      <c r="L57" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="N57">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q57">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U57">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W57" t="s">
-        <v>852</v>
+        <v>363</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>2332</v>
+        <v>2323</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L58" s="4" t="s">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="N58">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="Q58">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="U58">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="W58" t="s">
-        <v>353</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>2333</v>
+        <v>2331</v>
       </c>
       <c r="C59" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59">
         <v>4</v>
       </c>
-      <c r="L59" s="4" t="s">
-        <v>330</v>
+      <c r="L59" s="4">
+        <v>1000</v>
       </c>
       <c r="N59">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="Q59">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="U59">
         <v>6</v>
       </c>
       <c r="W59" t="s">
-        <v>359</v>
+        <v>852</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>2341</v>
+        <v>2332</v>
       </c>
       <c r="C60" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60">
-        <v>5</v>
-      </c>
-      <c r="L60" s="4">
-        <v>600</v>
+        <v>4</v>
+      </c>
+      <c r="L60" s="4" t="s">
+        <v>337</v>
       </c>
       <c r="N60">
         <v>10</v>
       </c>
       <c r="Q60">
-        <v>6</v>
-      </c>
-      <c r="S60">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="U60">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="W60" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2342</v>
+        <v>2333</v>
       </c>
       <c r="C61" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61">
-        <v>5</v>
-      </c>
-      <c r="L61" s="4">
-        <v>600</v>
+        <v>4</v>
+      </c>
+      <c r="L61" s="4" t="s">
+        <v>330</v>
       </c>
       <c r="N61">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="Q61">
         <v>15</v>
@@ -15822,625 +15808,663 @@
         <v>6</v>
       </c>
       <c r="W61" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2343</v>
+        <v>2341</v>
       </c>
       <c r="C62" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62">
         <v>5</v>
       </c>
-      <c r="L62" s="4" t="s">
-        <v>341</v>
+      <c r="L62" s="4">
+        <v>600</v>
       </c>
       <c r="N62">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q62">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="S62">
+        <v>-1</v>
       </c>
       <c r="U62">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="W62" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63">
         <v>5</v>
       </c>
-      <c r="L63" s="4" t="s">
-        <v>343</v>
+      <c r="L63" s="4">
+        <v>600</v>
       </c>
       <c r="N63">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q63">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U63">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="W63" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="C64" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64">
         <v>5</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="N64">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q64">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="U64">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="W64" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2351</v>
+        <v>2344</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="D65" s="15"/>
       <c r="E65">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="N65">
         <v>10</v>
       </c>
       <c r="Q65">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="U65">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="W65" t="s">
-        <v>352</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>2352</v>
+        <v>2345</v>
       </c>
       <c r="C66" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D66" s="15"/>
       <c r="E66">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="N66">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q66">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="U66">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="W66" t="s">
-        <v>358</v>
+        <v>368</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>2353</v>
+        <v>2351</v>
       </c>
       <c r="C67" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67">
         <v>6</v>
       </c>
-      <c r="L67" s="4">
-        <v>500</v>
+      <c r="L67" s="4" t="s">
+        <v>335</v>
       </c>
       <c r="N67">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q67">
-        <v>25</v>
-      </c>
-      <c r="S67">
-        <v>1</v>
-      </c>
-      <c r="T67">
-        <v>0.1</v>
+        <v>16</v>
       </c>
       <c r="U67">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="W67" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>2354</v>
+        <v>2352</v>
       </c>
       <c r="C68" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68">
         <v>6</v>
       </c>
       <c r="L68" s="4" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="N68">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q68">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="U68">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="W68" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>2355</v>
+        <v>2353</v>
       </c>
       <c r="C69" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69">
         <v>6</v>
       </c>
-      <c r="L69" s="4" t="s">
-        <v>331</v>
+      <c r="L69" s="4">
+        <v>500</v>
       </c>
       <c r="N69">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q69">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="S69">
+        <v>1</v>
+      </c>
+      <c r="T69">
+        <v>0.1</v>
       </c>
       <c r="U69">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W69" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>2361</v>
+        <v>2354</v>
       </c>
       <c r="C70" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70">
+        <v>6</v>
+      </c>
+      <c r="L70" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="N70">
         <v>7</v>
-      </c>
-      <c r="L70" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="N70">
-        <v>11</v>
       </c>
       <c r="Q70">
         <v>15</v>
       </c>
       <c r="U70">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="W70" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>2362</v>
+        <v>2355</v>
       </c>
       <c r="C71" t="s">
-        <v>139</v>
+        <v>160</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71">
-        <v>7</v>
-      </c>
-      <c r="L71" s="4">
-        <v>1200</v>
+        <v>6</v>
+      </c>
+      <c r="L71" s="4" t="s">
+        <v>331</v>
       </c>
       <c r="N71">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q71">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="U71">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="W71" t="s">
-        <v>355</v>
+        <v>369</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>2363</v>
+        <v>2361</v>
       </c>
       <c r="C72" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72">
         <v>7</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="N72">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Q72">
-        <v>30</v>
-      </c>
-      <c r="S72">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="U72">
-        <v>4</v>
+        <v>100</v>
       </c>
       <c r="W72" t="s">
-        <v>362</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>2364</v>
+        <v>2362</v>
       </c>
       <c r="C73" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73">
         <v>7</v>
       </c>
-      <c r="L73" s="4" t="s">
-        <v>346</v>
+      <c r="L73" s="4">
+        <v>1200</v>
       </c>
       <c r="N73">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q73">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="U73">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="W73" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
     </row>
     <row r="74" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>2371</v>
+        <v>2363</v>
       </c>
       <c r="C74" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="N74">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="Q74">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="S74">
+        <v>-1</v>
       </c>
       <c r="U74">
-        <v>125</v>
+        <v>4</v>
       </c>
       <c r="W74" t="s">
-        <v>1035</v>
+        <v>362</v>
       </c>
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>2372</v>
+        <v>2364</v>
       </c>
       <c r="C75" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75">
-        <v>8</v>
-      </c>
-      <c r="L75" s="4">
-        <v>500</v>
-      </c>
-      <c r="M75">
-        <v>500</v>
+        <v>7</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>346</v>
       </c>
       <c r="N75">
-        <v>9</v>
-      </c>
-      <c r="R75">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="Q75">
+        <v>12</v>
       </c>
       <c r="U75">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="W75" t="s">
-        <v>350</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>2373</v>
+        <v>2371</v>
       </c>
       <c r="C76" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76">
         <v>8</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N76">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q76">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="U76">
-        <v>35</v>
+        <v>125</v>
       </c>
       <c r="W76" t="s">
-        <v>352</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>2374</v>
+        <v>2372</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D77" s="15"/>
       <c r="E77">
         <v>8</v>
       </c>
       <c r="L77" s="4">
-        <v>1000</v>
+        <v>500</v>
+      </c>
+      <c r="M77">
+        <v>500</v>
       </c>
       <c r="N77">
+        <v>9</v>
+      </c>
+      <c r="R77">
         <v>8</v>
       </c>
-      <c r="Q77">
-        <v>35</v>
-      </c>
-      <c r="S77">
-        <v>1.5</v>
-      </c>
-      <c r="T77">
-        <v>0.15</v>
-      </c>
       <c r="U77">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="W77" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>2375</v>
+        <v>2373</v>
       </c>
       <c r="C78" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78">
         <v>8</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="N78">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q78">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="U78">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W78" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
     </row>
     <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>2381</v>
+        <v>2374</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D79" s="15"/>
       <c r="E79">
-        <v>9</v>
-      </c>
-      <c r="L79" s="4" t="s">
-        <v>332</v>
+        <v>8</v>
+      </c>
+      <c r="L79" s="4">
+        <v>1000</v>
       </c>
       <c r="N79">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Q79">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="S79">
+        <v>1.5</v>
+      </c>
+      <c r="T79">
+        <v>0.15</v>
       </c>
       <c r="U79">
-        <v>125</v>
+        <v>1</v>
       </c>
       <c r="W79" t="s">
-        <v>347</v>
+        <v>366</v>
       </c>
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>2382</v>
+        <v>2375</v>
       </c>
       <c r="C80" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="D80" s="15"/>
       <c r="E80">
-        <v>9</v>
-      </c>
-      <c r="L80" s="4">
-        <v>1000</v>
+        <v>8</v>
+      </c>
+      <c r="L80" s="4" t="s">
+        <v>344</v>
       </c>
       <c r="N80">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q80">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="U80">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="W80" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
     </row>
     <row r="81" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>2391</v>
+        <v>2381</v>
       </c>
       <c r="C81" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="D81" s="15"/>
       <c r="E81">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="N81">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q81">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="U81">
         <v>125</v>
       </c>
       <c r="W81" t="s">
-        <v>1036</v>
+        <v>347</v>
       </c>
     </row>
     <row r="82" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>2392</v>
+        <v>2382</v>
       </c>
       <c r="C82" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
       <c r="D82" s="15"/>
       <c r="E82">
+        <v>9</v>
+      </c>
+      <c r="L82" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N82">
+        <v>18</v>
+      </c>
+      <c r="Q82">
+        <v>45</v>
+      </c>
+      <c r="U82">
+        <v>8</v>
+      </c>
+      <c r="W82" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="83" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B83">
+        <v>2391</v>
+      </c>
+      <c r="C83" t="s">
+        <v>137</v>
+      </c>
+      <c r="D83" s="15"/>
+      <c r="E83">
         <v>10</v>
       </c>
-      <c r="L82" s="4">
-        <v>500</v>
-      </c>
-      <c r="M82">
-        <v>500</v>
-      </c>
-      <c r="N82">
-        <v>9</v>
-      </c>
-      <c r="R82">
-        <v>12</v>
-      </c>
-      <c r="U82">
-        <v>40</v>
-      </c>
-      <c r="W82" t="s">
-        <v>351</v>
+      <c r="L83" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="N83">
+        <v>11</v>
+      </c>
+      <c r="Q83">
+        <v>25</v>
+      </c>
+      <c r="U83">
+        <v>125</v>
+      </c>
+      <c r="W83" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="84" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>2401</v>
+        <v>2392</v>
       </c>
       <c r="C84" t="s">
-        <v>97</v>
-      </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="O84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B85">
-        <v>2402</v>
-      </c>
-      <c r="C85" t="s">
-        <v>166</v>
+        <v>141</v>
+      </c>
+      <c r="D84" s="15"/>
+      <c r="E84">
+        <v>10</v>
+      </c>
+      <c r="L84" s="4">
+        <v>500</v>
+      </c>
+      <c r="M84">
+        <v>500</v>
+      </c>
+      <c r="N84">
+        <v>9</v>
+      </c>
+      <c r="R84">
+        <v>12</v>
+      </c>
+      <c r="U84">
+        <v>40</v>
+      </c>
+      <c r="W84" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="86" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>2403</v>
+        <v>2401</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>97</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
       </c>
       <c r="O86">
         <v>1</v>
@@ -16448,651 +16472,633 @@
     </row>
     <row r="87" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>2404</v>
+        <v>2402</v>
       </c>
       <c r="C87" t="s">
-        <v>167</v>
-      </c>
-      <c r="O87">
-        <v>2</v>
-      </c>
-      <c r="S87">
-        <v>-0.5</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B88">
-        <v>2411</v>
+        <v>2403</v>
       </c>
       <c r="C88" t="s">
-        <v>98</v>
-      </c>
-      <c r="E88">
-        <v>2</v>
+        <v>168</v>
       </c>
       <c r="O88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>2421</v>
+        <v>2404</v>
       </c>
       <c r="C89" t="s">
-        <v>99</v>
-      </c>
-      <c r="E89">
-        <v>3</v>
+        <v>167</v>
       </c>
       <c r="O89">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="S89">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="90" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>2431</v>
+        <v>2411</v>
       </c>
       <c r="C90" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E90">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O90">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2441</v>
+        <v>2421</v>
       </c>
       <c r="C91" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E91">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O91">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2451</v>
+        <v>2431</v>
       </c>
       <c r="C92" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E92">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O92">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2461</v>
+        <v>2441</v>
       </c>
       <c r="C93" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E93">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O93">
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="94" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2471</v>
+        <v>2451</v>
       </c>
       <c r="C94" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E94">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O94">
-        <v>200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2481</v>
+        <v>2461</v>
       </c>
       <c r="C95" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E95">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O95">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2491</v>
+        <v>2471</v>
       </c>
       <c r="C96" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E96">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O96">
-        <v>1500</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>2481</v>
+      </c>
+      <c r="C97" t="s">
+        <v>105</v>
+      </c>
+      <c r="E97">
+        <v>9</v>
+      </c>
+      <c r="O97">
+        <v>400</v>
       </c>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2501</v>
+        <v>2491</v>
       </c>
       <c r="C98" t="s">
-        <v>803</v>
-      </c>
-      <c r="D98" t="s">
-        <v>23</v>
+        <v>106</v>
+      </c>
+      <c r="E98">
+        <v>10</v>
       </c>
       <c r="O98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B99">
-        <v>2502</v>
-      </c>
-      <c r="C99" t="s">
-        <v>169</v>
-      </c>
-      <c r="N99">
-        <v>0.04</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2503</v>
+        <v>2501</v>
       </c>
       <c r="C100" t="s">
-        <v>170</v>
-      </c>
-      <c r="N100">
-        <v>0.02</v>
+        <v>803</v>
+      </c>
+      <c r="D100" t="s">
+        <v>23</v>
+      </c>
+      <c r="O100">
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2504</v>
+        <v>2502</v>
       </c>
       <c r="C101" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N101">
         <v>0.04</v>
       </c>
-      <c r="O101">
-        <v>1</v>
-      </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2511</v>
+        <v>2503</v>
       </c>
       <c r="C102" t="s">
-        <v>804</v>
-      </c>
-      <c r="E102">
-        <v>2</v>
-      </c>
-      <c r="O102">
-        <v>2</v>
+        <v>170</v>
+      </c>
+      <c r="N102">
+        <v>0.02</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2512</v>
+        <v>2504</v>
       </c>
       <c r="C103" t="s">
-        <v>179</v>
-      </c>
-      <c r="E103">
-        <v>2</v>
-      </c>
-      <c r="K103">
-        <v>3</v>
+        <v>171</v>
       </c>
       <c r="N103">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="O103">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>2513</v>
+        <v>2511</v>
       </c>
       <c r="C104" t="s">
-        <v>302</v>
-      </c>
-      <c r="N104">
-        <v>0.04</v>
+        <v>804</v>
+      </c>
+      <c r="E104">
+        <v>2</v>
+      </c>
+      <c r="O104">
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>2521</v>
+        <v>2512</v>
       </c>
       <c r="C105" t="s">
-        <v>805</v>
+        <v>179</v>
       </c>
       <c r="E105">
+        <v>2</v>
+      </c>
+      <c r="K105">
         <v>3</v>
       </c>
+      <c r="N105">
+        <v>0.05</v>
+      </c>
       <c r="O105">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2531</v>
+        <v>2513</v>
       </c>
       <c r="C106" t="s">
-        <v>806</v>
-      </c>
-      <c r="E106">
-        <v>4</v>
-      </c>
-      <c r="O106">
-        <v>21</v>
+        <v>302</v>
+      </c>
+      <c r="N106">
+        <v>0.04</v>
       </c>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2541</v>
+        <v>2521</v>
       </c>
       <c r="C107" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="E107">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O107">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2551</v>
+        <v>2531</v>
       </c>
       <c r="C108" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E108">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O108">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2561</v>
+        <v>2541</v>
       </c>
       <c r="C109" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="E109">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O109">
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2571</v>
+        <v>2551</v>
       </c>
       <c r="C110" t="s">
-        <v>810</v>
+        <v>807</v>
       </c>
       <c r="E110">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O110">
-        <v>200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2581</v>
+        <v>2561</v>
       </c>
       <c r="C111" t="s">
-        <v>812</v>
+        <v>809</v>
       </c>
       <c r="E111">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O111">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>2591</v>
+        <v>2571</v>
       </c>
       <c r="C112" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E112">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O112">
-        <v>1500</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>2581</v>
+      </c>
+      <c r="C113" t="s">
+        <v>812</v>
+      </c>
+      <c r="E113">
+        <v>9</v>
+      </c>
+      <c r="O113">
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2601</v>
+        <v>2591</v>
       </c>
       <c r="C114" t="s">
-        <v>107</v>
-      </c>
-      <c r="D114" t="s">
-        <v>24</v>
+        <v>811</v>
+      </c>
+      <c r="E114">
+        <v>10</v>
       </c>
       <c r="O114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B115">
-        <v>2602</v>
-      </c>
-      <c r="C115" t="s">
-        <v>172</v>
-      </c>
-      <c r="N115">
-        <v>0.02</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>2603</v>
+        <v>2601</v>
       </c>
       <c r="C116" t="s">
-        <v>174</v>
-      </c>
-      <c r="N116">
-        <v>0.06</v>
+        <v>107</v>
+      </c>
+      <c r="D116" t="s">
+        <v>24</v>
+      </c>
+      <c r="O116">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>2604</v>
+        <v>2602</v>
       </c>
       <c r="C117" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N117">
-        <v>0.08</v>
-      </c>
-      <c r="O117">
-        <v>1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>2611</v>
+        <v>2603</v>
       </c>
       <c r="C118" t="s">
-        <v>108</v>
-      </c>
-      <c r="E118">
-        <v>2</v>
-      </c>
-      <c r="O118">
-        <v>2</v>
+        <v>174</v>
+      </c>
+      <c r="N118">
+        <v>0.06</v>
       </c>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>2621</v>
+        <v>2604</v>
       </c>
       <c r="C119" t="s">
-        <v>109</v>
-      </c>
-      <c r="E119">
-        <v>3</v>
+        <v>173</v>
+      </c>
+      <c r="N119">
+        <v>0.08</v>
       </c>
       <c r="O119">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>2631</v>
+        <v>2611</v>
       </c>
       <c r="C120" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E120">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O120">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2641</v>
+        <v>2621</v>
       </c>
       <c r="C121" t="s">
-        <v>743</v>
+        <v>109</v>
       </c>
       <c r="E121">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O121">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2651</v>
+        <v>2631</v>
       </c>
       <c r="C122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E122">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O122">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2661</v>
+        <v>2641</v>
       </c>
       <c r="C123" t="s">
-        <v>112</v>
+        <v>743</v>
       </c>
       <c r="E123">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O123">
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2671</v>
+        <v>2651</v>
       </c>
       <c r="C124" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E124">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O124">
-        <v>200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>2681</v>
+        <v>2661</v>
       </c>
       <c r="C125" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E125">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O125">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2691</v>
+        <v>2671</v>
       </c>
       <c r="C126" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E126">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="O126">
-        <v>1500</v>
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>2681</v>
+      </c>
+      <c r="C127" t="s">
+        <v>114</v>
+      </c>
+      <c r="E127">
+        <v>9</v>
+      </c>
+      <c r="O127">
+        <v>400</v>
       </c>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2701</v>
+        <v>2691</v>
       </c>
       <c r="C128" t="s">
-        <v>116</v>
-      </c>
-      <c r="D128" t="s">
-        <v>25</v>
+        <v>115</v>
+      </c>
+      <c r="E128">
+        <v>10</v>
       </c>
       <c r="O128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B129">
-        <v>2702</v>
-      </c>
-      <c r="C129" t="s">
-        <v>175</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2703</v>
+        <v>2701</v>
       </c>
       <c r="C130" t="s">
-        <v>176</v>
-      </c>
-      <c r="S130">
+        <v>116</v>
+      </c>
+      <c r="D130" t="s">
+        <v>25</v>
+      </c>
+      <c r="O130">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2704</v>
+        <v>2702</v>
       </c>
       <c r="C131" t="s">
-        <v>177</v>
-      </c>
-      <c r="O131">
-        <v>1</v>
-      </c>
-      <c r="S131">
-        <v>2</v>
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2705</v>
+        <v>2703</v>
       </c>
       <c r="C132" t="s">
-        <v>303</v>
-      </c>
-      <c r="O132">
-        <v>2</v>
+        <v>176</v>
       </c>
       <c r="S132">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2711</v>
+        <v>2704</v>
       </c>
       <c r="C133" t="s">
-        <v>117</v>
-      </c>
-      <c r="E133">
-        <v>2</v>
+        <v>177</v>
       </c>
       <c r="O133">
+        <v>1</v>
+      </c>
+      <c r="S133">
         <v>2</v>
       </c>
     </row>
     <row r="134" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2712</v>
+        <v>2705</v>
       </c>
       <c r="C134" t="s">
-        <v>178</v>
-      </c>
-      <c r="E134">
+        <v>303</v>
+      </c>
+      <c r="O134">
         <v>2</v>
       </c>
-      <c r="O134">
-        <v>1</v>
-      </c>
       <c r="S134">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="C135" t="s">
-        <v>304</v>
+        <v>117</v>
       </c>
       <c r="E135">
         <v>2</v>
       </c>
-      <c r="L135" s="4">
-        <v>1</v>
-      </c>
       <c r="O135">
-        <v>3</v>
-      </c>
-      <c r="S135">
         <v>2</v>
       </c>
     </row>
     <row r="136" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B136">
-        <v>2714</v>
+        <v>2712</v>
       </c>
       <c r="C136" t="s">
-        <v>305</v>
+        <v>178</v>
       </c>
       <c r="E136">
         <v>2</v>
       </c>
       <c r="O136">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S136">
         <v>3</v>
@@ -17100,571 +17106,583 @@
     </row>
     <row r="137" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>2721</v>
+        <v>2713</v>
       </c>
       <c r="C137" t="s">
-        <v>118</v>
+        <v>304</v>
       </c>
       <c r="E137">
+        <v>2</v>
+      </c>
+      <c r="L137" s="4">
+        <v>1</v>
+      </c>
+      <c r="O137">
         <v>3</v>
       </c>
-      <c r="O137">
-        <v>14</v>
+      <c r="S137">
+        <v>2</v>
       </c>
     </row>
     <row r="138" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2731</v>
+        <v>2714</v>
       </c>
       <c r="C138" t="s">
-        <v>119</v>
+        <v>305</v>
       </c>
       <c r="E138">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O138">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="S138">
+        <v>3</v>
       </c>
     </row>
     <row r="139" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2741</v>
+        <v>2721</v>
       </c>
       <c r="C139" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E139">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O139">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2751</v>
+        <v>2731</v>
       </c>
       <c r="C140" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E140">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O140">
-        <v>72</v>
+        <v>21</v>
       </c>
     </row>
     <row r="141" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>2761</v>
+        <v>2741</v>
       </c>
       <c r="C141" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E141">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="O141">
-        <v>100</v>
+        <v>48</v>
       </c>
     </row>
     <row r="142" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2771</v>
+        <v>2751</v>
       </c>
       <c r="C142" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E142">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O142">
-        <v>200</v>
+        <v>72</v>
       </c>
     </row>
     <row r="143" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>2781</v>
+        <v>2761</v>
       </c>
       <c r="C143" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E143">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O143">
-        <v>400</v>
+        <v>100</v>
       </c>
     </row>
     <row r="144" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B144">
+        <v>2771</v>
+      </c>
+      <c r="C144" t="s">
+        <v>123</v>
+      </c>
+      <c r="E144">
+        <v>8</v>
+      </c>
+      <c r="O144">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="145" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B145">
+        <v>2781</v>
+      </c>
+      <c r="C145" t="s">
+        <v>124</v>
+      </c>
+      <c r="E145">
+        <v>9</v>
+      </c>
+      <c r="O145">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="146" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B146">
         <v>2791</v>
       </c>
-      <c r="C144" t="s">
+      <c r="C146" t="s">
         <v>125</v>
       </c>
-      <c r="E144">
+      <c r="E146">
         <v>10</v>
       </c>
-      <c r="O144">
+      <c r="O146">
         <v>1500</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146">
+    <row r="148" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B148">
         <v>2801</v>
       </c>
-      <c r="C146" t="s">
+      <c r="C148" t="s">
         <v>772</v>
       </c>
-      <c r="D146" t="s">
+      <c r="D148" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147">
+    <row r="149" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B149">
         <v>2802</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C149" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148">
+    <row r="150" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B150">
         <v>2803</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C150" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="149" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B149">
+    <row r="151" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B151">
         <v>2804</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C151" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="150" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B150">
+    <row r="152" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B152">
         <v>2805</v>
       </c>
-      <c r="C150" t="s">
+      <c r="C152" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="151" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B151">
+    <row r="153" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B153">
         <v>2806</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C153" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="152" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B152">
+    <row r="154" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B154">
         <v>2807</v>
       </c>
-      <c r="C152" t="s">
+      <c r="C154" t="s">
         <v>1019</v>
       </c>
     </row>
-    <row r="153" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B153">
+    <row r="155" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B155">
         <v>2808</v>
       </c>
     </row>
-    <row r="154" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B154">
+    <row r="156" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B156">
         <v>2809</v>
       </c>
     </row>
-    <row r="155" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B155">
+    <row r="157" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B157">
         <v>2810</v>
       </c>
     </row>
-    <row r="156" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B156">
+    <row r="158" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B158">
         <v>2811</v>
       </c>
-      <c r="C156" t="s">
+      <c r="C158" t="s">
         <v>775</v>
       </c>
-      <c r="E156">
+      <c r="E158">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B157">
+    <row r="159" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B159">
         <v>2812</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C159" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="158" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B158">
+    <row r="160" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B160">
         <v>2813</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C160" t="s">
         <v>777</v>
-      </c>
-    </row>
-    <row r="159" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B159">
-        <v>2814</v>
-      </c>
-      <c r="C159" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="160" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B160">
-        <v>2815</v>
-      </c>
-      <c r="C160" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="161" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2821</v>
+        <v>2814</v>
       </c>
       <c r="C161" t="s">
-        <v>778</v>
-      </c>
-      <c r="E161">
-        <v>3</v>
+        <v>800</v>
       </c>
     </row>
     <row r="162" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2822</v>
+        <v>2815</v>
       </c>
       <c r="C162" t="s">
-        <v>779</v>
+        <v>301</v>
       </c>
     </row>
     <row r="163" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2823</v>
+        <v>2821</v>
       </c>
       <c r="C163" t="s">
-        <v>781</v>
+        <v>778</v>
+      </c>
+      <c r="E163">
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2834</v>
+        <v>2822</v>
       </c>
       <c r="C164" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="165" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2825</v>
+        <v>2823</v>
       </c>
       <c r="C165" t="s">
-        <v>541</v>
-      </c>
-      <c r="Y165" t="s">
-        <v>201</v>
+        <v>781</v>
       </c>
     </row>
     <row r="166" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2831</v>
+        <v>2834</v>
       </c>
       <c r="C166" t="s">
-        <v>782</v>
-      </c>
-      <c r="E166">
-        <v>4</v>
+        <v>780</v>
       </c>
     </row>
     <row r="167" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2832</v>
+        <v>2825</v>
       </c>
       <c r="C167" t="s">
-        <v>783</v>
+        <v>541</v>
+      </c>
+      <c r="Y167" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="168" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2841</v>
+        <v>2831</v>
       </c>
       <c r="C168" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="E168">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2842</v>
+        <v>2832</v>
       </c>
       <c r="C169" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="170" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2851</v>
+        <v>2841</v>
       </c>
       <c r="C170" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E170">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2852</v>
+        <v>2842</v>
       </c>
       <c r="C171" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
     </row>
     <row r="172" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2853</v>
+        <v>2851</v>
       </c>
       <c r="C172" t="s">
-        <v>787</v>
+        <v>786</v>
+      </c>
+      <c r="E172">
+        <v>6</v>
       </c>
     </row>
     <row r="173" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2861</v>
+        <v>2852</v>
       </c>
       <c r="C173" t="s">
-        <v>788</v>
-      </c>
-      <c r="E173">
-        <v>7</v>
+        <v>792</v>
       </c>
     </row>
     <row r="174" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2862</v>
+        <v>2853</v>
       </c>
       <c r="C174" t="s">
-        <v>793</v>
+        <v>787</v>
       </c>
     </row>
     <row r="175" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B175">
-        <v>2863</v>
+        <v>2861</v>
       </c>
       <c r="C175" t="s">
-        <v>794</v>
+        <v>788</v>
+      </c>
+      <c r="E175">
+        <v>7</v>
       </c>
     </row>
     <row r="176" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B176">
-        <v>2864</v>
+        <v>2862</v>
       </c>
       <c r="C176" t="s">
-        <v>299</v>
+        <v>793</v>
       </c>
     </row>
     <row r="177" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B177">
-        <v>2871</v>
+        <v>2863</v>
       </c>
       <c r="C177" t="s">
-        <v>789</v>
-      </c>
-      <c r="E177">
-        <v>8</v>
+        <v>794</v>
       </c>
     </row>
     <row r="178" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B178">
-        <v>2872</v>
+        <v>2864</v>
       </c>
       <c r="C178" t="s">
-        <v>797</v>
+        <v>299</v>
       </c>
     </row>
     <row r="179" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2873</v>
+        <v>2871</v>
       </c>
       <c r="C179" t="s">
-        <v>801</v>
+        <v>789</v>
+      </c>
+      <c r="E179">
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2881</v>
+        <v>2872</v>
       </c>
       <c r="C180" t="s">
-        <v>790</v>
-      </c>
-      <c r="E180">
-        <v>9</v>
+        <v>797</v>
       </c>
     </row>
     <row r="181" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B181">
-        <v>2882</v>
+        <v>2873</v>
       </c>
       <c r="C181" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
     </row>
     <row r="182" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2883</v>
+        <v>2881</v>
       </c>
       <c r="C182" t="s">
-        <v>802</v>
+        <v>790</v>
+      </c>
+      <c r="E182">
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2891</v>
+        <v>2882</v>
       </c>
       <c r="C183" t="s">
-        <v>791</v>
-      </c>
-      <c r="E183">
-        <v>10</v>
+        <v>799</v>
       </c>
     </row>
     <row r="184" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2892</v>
+        <v>2883</v>
       </c>
       <c r="C184" t="s">
-        <v>135</v>
+        <v>802</v>
+      </c>
+    </row>
+    <row r="185" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B185">
+        <v>2891</v>
+      </c>
+      <c r="C185" t="s">
+        <v>791</v>
+      </c>
+      <c r="E185">
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2901</v>
+        <v>2892</v>
       </c>
       <c r="C186" t="s">
-        <v>251</v>
-      </c>
-      <c r="D186" t="s">
-        <v>251</v>
-      </c>
-      <c r="W186" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="187" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B187">
-        <v>2902</v>
-      </c>
-      <c r="C187" t="s">
-        <v>253</v>
-      </c>
-      <c r="D187" t="s">
-        <v>251</v>
-      </c>
-      <c r="E187">
-        <v>2</v>
-      </c>
-      <c r="W187" t="s">
-        <v>255</v>
+        <v>135</v>
       </c>
     </row>
     <row r="188" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2903</v>
+        <v>2901</v>
       </c>
       <c r="C188" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D188" t="s">
         <v>251</v>
       </c>
-      <c r="E188">
-        <v>3</v>
-      </c>
       <c r="W188" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="189" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2911</v>
+        <v>2902</v>
       </c>
       <c r="C189" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D189" t="s">
-        <v>257</v>
-      </c>
-      <c r="H189" s="6"/>
-      <c r="L189" s="4">
-        <v>1</v>
+        <v>251</v>
+      </c>
+      <c r="E189">
+        <v>2</v>
+      </c>
+      <c r="W189" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="190" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2912</v>
+        <v>2903</v>
       </c>
       <c r="C190" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D190" t="s">
-        <v>257</v>
-      </c>
-      <c r="L190" s="4">
-        <v>1</v>
+        <v>251</v>
+      </c>
+      <c r="E190">
+        <v>3</v>
+      </c>
+      <c r="W190" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="191" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="C191" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D191" t="s">
         <v>257</v>
       </c>
+      <c r="H191" s="6"/>
+      <c r="L191" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="192" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="C192" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D192" t="s">
         <v>257</v>
       </c>
+      <c r="L192" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="193" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="C193" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D193" t="s">
         <v>257</v>
       </c>
-      <c r="L193" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="194" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2916</v>
+        <v>2914</v>
       </c>
       <c r="C194" t="s">
-        <v>290</v>
+        <v>261</v>
       </c>
       <c r="D194" t="s">
         <v>257</v>
@@ -17672,69 +17690,60 @@
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="C195" t="s">
-        <v>742</v>
+        <v>262</v>
       </c>
       <c r="D195" t="s">
         <v>257</v>
       </c>
+      <c r="L195" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="196" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2918</v>
+        <v>2916</v>
       </c>
       <c r="C196" t="s">
-        <v>1080</v>
+        <v>290</v>
       </c>
       <c r="D196" t="s">
         <v>257</v>
       </c>
-      <c r="L196" s="4">
-        <v>1.5</v>
-      </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2921</v>
+        <v>2917</v>
       </c>
       <c r="C197" t="s">
-        <v>264</v>
+        <v>742</v>
       </c>
       <c r="D197" t="s">
-        <v>263</v>
-      </c>
-      <c r="N197">
-        <v>0.04</v>
-      </c>
-      <c r="W197" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="198" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2922</v>
+        <v>2918</v>
       </c>
       <c r="C198" t="s">
-        <v>265</v>
+        <v>1080</v>
       </c>
       <c r="D198" t="s">
-        <v>263</v>
-      </c>
-      <c r="N198">
-        <v>0.04</v>
-      </c>
-      <c r="W198" t="s">
-        <v>269</v>
+        <v>257</v>
+      </c>
+      <c r="L198" s="4">
+        <v>1.5</v>
       </c>
     </row>
     <row r="199" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2923</v>
+        <v>2921</v>
       </c>
       <c r="C199" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D199" t="s">
         <v>263</v>
@@ -17743,161 +17752,155 @@
         <v>0.04</v>
       </c>
       <c r="W199" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2924</v>
+        <v>2922</v>
       </c>
       <c r="C200" t="s">
-        <v>291</v>
+        <v>265</v>
       </c>
       <c r="D200" t="s">
         <v>263</v>
       </c>
-      <c r="L200" s="4">
-        <v>1</v>
-      </c>
       <c r="N200">
-        <v>2.5</v>
-      </c>
-      <c r="Q200">
-        <v>6</v>
+        <v>0.04</v>
       </c>
       <c r="W200" t="s">
-        <v>298</v>
+        <v>269</v>
       </c>
     </row>
     <row r="201" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C201" t="s">
-        <v>292</v>
+        <v>266</v>
       </c>
       <c r="D201" t="s">
         <v>263</v>
       </c>
+      <c r="N201">
+        <v>0.04</v>
+      </c>
       <c r="W201" t="s">
-        <v>295</v>
+        <v>267</v>
       </c>
     </row>
     <row r="202" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2926</v>
+        <v>2924</v>
       </c>
       <c r="C202" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D202" t="s">
         <v>263</v>
       </c>
-      <c r="E202">
-        <v>2</v>
-      </c>
       <c r="L202" s="4">
         <v>1</v>
       </c>
       <c r="N202">
-        <v>0.02</v>
+        <v>2.5</v>
+      </c>
+      <c r="Q202">
+        <v>6</v>
       </c>
       <c r="W202" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="203" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="C203" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D203" t="s">
         <v>263</v>
       </c>
-      <c r="E203">
-        <v>3</v>
-      </c>
-      <c r="L203" s="4">
-        <v>2</v>
-      </c>
-      <c r="N203">
-        <v>0.02</v>
-      </c>
       <c r="W203" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2928</v>
+        <v>2926</v>
       </c>
       <c r="C204" t="s">
-        <v>1069</v>
+        <v>293</v>
       </c>
       <c r="D204" t="s">
         <v>263</v>
       </c>
+      <c r="E204">
+        <v>2</v>
+      </c>
+      <c r="L204" s="4">
+        <v>1</v>
+      </c>
+      <c r="N204">
+        <v>0.02</v>
+      </c>
       <c r="W204" t="s">
-        <v>1072</v>
+        <v>296</v>
       </c>
     </row>
     <row r="205" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2931</v>
+        <v>2927</v>
       </c>
       <c r="C205" t="s">
-        <v>238</v>
+        <v>294</v>
       </c>
       <c r="D205" t="s">
-        <v>279</v>
+        <v>263</v>
+      </c>
+      <c r="E205">
+        <v>3</v>
       </c>
       <c r="L205" s="4">
         <v>2</v>
       </c>
       <c r="N205">
-        <v>2.5</v>
+        <v>0.02</v>
       </c>
       <c r="W205" t="s">
-        <v>815</v>
+        <v>297</v>
       </c>
     </row>
     <row r="206" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2932</v>
+        <v>2928</v>
       </c>
       <c r="C206" t="s">
-        <v>280</v>
+        <v>1069</v>
       </c>
       <c r="D206" t="s">
-        <v>279</v>
-      </c>
-      <c r="L206" s="4">
-        <v>1</v>
-      </c>
-      <c r="N206">
-        <v>2</v>
-      </c>
-      <c r="Q206">
-        <v>4</v>
+        <v>263</v>
+      </c>
+      <c r="W206" t="s">
+        <v>1072</v>
       </c>
     </row>
     <row r="207" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="C207" t="s">
-        <v>283</v>
+        <v>238</v>
       </c>
       <c r="D207" t="s">
         <v>279</v>
       </c>
       <c r="L207" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N207">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W207" t="s">
         <v>815</v>
@@ -17905,49 +17908,61 @@
     </row>
     <row r="208" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2941</v>
+        <v>2932</v>
       </c>
       <c r="C208" t="s">
-        <v>375</v>
+        <v>280</v>
       </c>
       <c r="D208" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="209" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L208" s="4">
+        <v>1</v>
+      </c>
+      <c r="N208">
+        <v>2</v>
+      </c>
+      <c r="Q208">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="209" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2942</v>
+        <v>2933</v>
       </c>
       <c r="C209" t="s">
-        <v>376</v>
+        <v>283</v>
       </c>
       <c r="D209" t="s">
         <v>279</v>
       </c>
-      <c r="E209">
+      <c r="L209" s="4">
+        <v>1</v>
+      </c>
+      <c r="N209">
         <v>2</v>
       </c>
-    </row>
-    <row r="210" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="W209" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="210" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B210">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="C210" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D210" t="s">
         <v>279</v>
       </c>
-      <c r="E210">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="211" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="211" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B211">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="C211" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D211" t="s">
         <v>279</v>
@@ -17955,19 +17970,13 @@
       <c r="E211">
         <v>2</v>
       </c>
-      <c r="L211" s="4">
-        <v>3</v>
-      </c>
-      <c r="N211">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="212" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="212" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="C212" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D212" t="s">
         <v>279</v>
@@ -17976,12 +17985,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="213" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="C213" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D213" t="s">
         <v>279</v>
@@ -17989,13 +17998,19 @@
       <c r="E213">
         <v>2</v>
       </c>
-    </row>
-    <row r="214" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L213" s="4">
+        <v>3</v>
+      </c>
+      <c r="N213">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="214" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="C214" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D214" t="s">
         <v>279</v>
@@ -18004,12 +18019,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="C215" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D215" t="s">
         <v>279</v>
@@ -18018,65 +18033,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B216">
+        <v>2947</v>
+      </c>
+      <c r="C216" t="s">
+        <v>381</v>
+      </c>
+      <c r="D216" t="s">
+        <v>279</v>
+      </c>
+      <c r="E216">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="217" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B217">
+        <v>2948</v>
+      </c>
+      <c r="C217" t="s">
+        <v>382</v>
+      </c>
+      <c r="D217" t="s">
+        <v>279</v>
+      </c>
+      <c r="E217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B218">
         <v>2961</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C218" t="s">
         <v>284</v>
-      </c>
-      <c r="D216" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="217" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B217">
-        <v>2962</v>
-      </c>
-      <c r="C217" t="s">
-        <v>285</v>
-      </c>
-      <c r="D217" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="218" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B218">
-        <v>2963</v>
-      </c>
-      <c r="C218" t="s">
-        <v>317</v>
       </c>
       <c r="D218" t="s">
         <v>286</v>
       </c>
-      <c r="L218" s="4">
-        <v>1</v>
-      </c>
-      <c r="N218">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="219" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="219" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B219">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="C219" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="D219" t="s">
         <v>286</v>
       </c>
-      <c r="N219">
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="220" spans="2:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="220" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B220">
-        <v>2965</v>
+        <v>2963</v>
       </c>
       <c r="C220" t="s">
-        <v>847</v>
+        <v>317</v>
       </c>
       <c r="D220" t="s">
         <v>286</v>
@@ -18088,29 +18100,26 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="221" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B221">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="C221" t="s">
-        <v>848</v>
+        <v>321</v>
       </c>
       <c r="D221" t="s">
         <v>286</v>
       </c>
-      <c r="L221" s="4">
-        <v>1</v>
-      </c>
       <c r="N221">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="222" spans="2:14" x14ac:dyDescent="0.25">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="222" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="C222" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="D222" t="s">
         <v>286</v>
@@ -18122,12 +18131,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="223" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2968</v>
+        <v>2966</v>
       </c>
       <c r="C223" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="D223" t="s">
         <v>286</v>
@@ -18139,83 +18148,80 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="224" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2971</v>
+        <v>2967</v>
       </c>
       <c r="C224" t="s">
-        <v>311</v>
+        <v>849</v>
       </c>
       <c r="D224" t="s">
-        <v>306</v>
+        <v>286</v>
+      </c>
+      <c r="L224" s="4">
+        <v>1</v>
+      </c>
+      <c r="N224">
+        <v>0.05</v>
       </c>
     </row>
     <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2972</v>
+        <v>2968</v>
       </c>
       <c r="C225" t="s">
-        <v>312</v>
+        <v>850</v>
       </c>
       <c r="D225" t="s">
-        <v>306</v>
+        <v>286</v>
       </c>
       <c r="L225" s="4">
         <v>1</v>
       </c>
       <c r="N225">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="226" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2973</v>
+        <v>2971</v>
       </c>
       <c r="C226" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="D226" t="s">
         <v>306</v>
       </c>
-      <c r="L226" s="4">
-        <v>1</v>
-      </c>
-      <c r="N226">
-        <v>0.02</v>
-      </c>
     </row>
     <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="C227" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D227" t="s">
         <v>306</v>
       </c>
-      <c r="E227">
-        <v>2</v>
+      <c r="L227" s="4">
+        <v>1</v>
       </c>
       <c r="N227">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="C228" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D228" t="s">
         <v>306</v>
       </c>
-      <c r="E228">
-        <v>2</v>
-      </c>
       <c r="L228" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N228">
         <v>0.02</v>
@@ -18223,10 +18229,10 @@
     </row>
     <row r="229" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="C229" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D229" t="s">
         <v>306</v>
@@ -18234,59 +18240,53 @@
       <c r="E229">
         <v>2</v>
       </c>
-      <c r="L229" s="4">
-        <v>1</v>
+      <c r="N229">
+        <v>0.05</v>
       </c>
     </row>
     <row r="230" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="C230" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="D230" t="s">
         <v>306</v>
       </c>
       <c r="E230">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L230" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N230">
-        <v>0.08</v>
-      </c>
-      <c r="Q230">
-        <v>15</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="231" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="C231" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="D231" t="s">
         <v>306</v>
       </c>
       <c r="E231">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L231" s="4">
-        <v>2</v>
-      </c>
-      <c r="N231">
-        <v>0.1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B232">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="C232" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D232" t="s">
         <v>306</v>
@@ -18295,47 +18295,53 @@
         <v>3</v>
       </c>
       <c r="L232" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N232">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Q232">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="233" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B233">
-        <v>2980</v>
+        <v>2978</v>
       </c>
       <c r="C233" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="D233" t="s">
         <v>306</v>
       </c>
       <c r="E233">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L233" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N233">
+        <v>0.1</v>
       </c>
     </row>
     <row r="234" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B234">
-        <v>2981</v>
+        <v>2979</v>
       </c>
       <c r="C234" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D234" t="s">
         <v>306</v>
       </c>
       <c r="E234">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L234" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N234">
+        <v>0.05</v>
       </c>
       <c r="Q234">
         <v>5</v>
@@ -18343,10 +18349,10 @@
     </row>
     <row r="235" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B235">
-        <v>2982</v>
+        <v>2980</v>
       </c>
       <c r="C235" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="D235" t="s">
         <v>306</v>
@@ -18360,50 +18366,87 @@
     </row>
     <row r="236" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B236">
-        <v>2983</v>
+        <v>2981</v>
       </c>
       <c r="C236" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D236" t="s">
         <v>306</v>
       </c>
       <c r="E236">
+        <v>4</v>
+      </c>
+      <c r="L236" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q236">
         <v>5</v>
-      </c>
-      <c r="L236" s="4">
-        <v>5</v>
-      </c>
-      <c r="N236">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q236">
-        <v>20</v>
       </c>
     </row>
     <row r="237" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B237">
+        <v>2982</v>
+      </c>
+      <c r="C237" t="s">
+        <v>315</v>
+      </c>
+      <c r="D237" t="s">
+        <v>306</v>
+      </c>
+      <c r="E237">
+        <v>4</v>
+      </c>
+      <c r="L237" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B238">
+        <v>2983</v>
+      </c>
+      <c r="C238" t="s">
+        <v>316</v>
+      </c>
+      <c r="D238" t="s">
+        <v>306</v>
+      </c>
+      <c r="E238">
+        <v>5</v>
+      </c>
+      <c r="L238" s="4">
+        <v>5</v>
+      </c>
+      <c r="N238">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q238">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="239" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B239">
         <v>2991</v>
       </c>
-      <c r="C237" t="s">
+      <c r="C239" t="s">
         <v>1041</v>
       </c>
-      <c r="D237" t="s">
+      <c r="D239" t="s">
         <v>1042</v>
       </c>
-      <c r="E237">
+      <c r="E239">
         <v>1</v>
       </c>
-      <c r="K237" s="4"/>
-      <c r="L237"/>
-    </row>
-    <row r="238" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K238" s="4"/>
-      <c r="L238"/>
-    </row>
-    <row r="239" spans="2:17" x14ac:dyDescent="0.25">
       <c r="K239" s="4"/>
       <c r="L239"/>
+    </row>
+    <row r="240" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K240" s="4"/>
+      <c r="L240"/>
+    </row>
+    <row r="241" spans="11:12" x14ac:dyDescent="0.25">
+      <c r="K241" s="4"/>
+      <c r="L241"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
v0.7.3g: Added several items
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14FF79A-75BD-4D8C-83FD-5AAC08E3D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6D363-EBC4-491D-B929-999FAFCCFAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1446" uniqueCount="1089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="1104">
   <si>
     <t>ID</t>
   </si>
@@ -3663,24 +3663,12 @@
     <t>relevance</t>
   </si>
   <si>
-    <t>Tutorial-soldiers door</t>
-  </si>
-  <si>
-    <t>Tutorial-bens door</t>
-  </si>
-  <si>
-    <t>get after unlocking inventory</t>
-  </si>
-  <si>
     <t>needed to enter ben's room in tutorial</t>
   </si>
   <si>
     <t>Tutorial-RA door</t>
   </si>
   <si>
-    <t>Tutorial-stub wing</t>
-  </si>
-  <si>
     <t>Tutorial-2F custodial</t>
   </si>
   <si>
@@ -3766,6 +3754,63 @@
   </si>
   <si>
     <t>Steel Door (locked)</t>
+  </si>
+  <si>
+    <t>Tutorial-bens door, FrancisHall-bens door</t>
+  </si>
+  <si>
+    <t>Tutorial-soldiers door, FrancisHall-soldiers door</t>
+  </si>
+  <si>
+    <t>Tutorial-get after unlocking inventory, FrancisHall-on table</t>
+  </si>
+  <si>
+    <t>Woodglue</t>
+  </si>
+  <si>
+    <t>Nails</t>
+  </si>
+  <si>
+    <t>Screws</t>
+  </si>
+  <si>
+    <t>Flint and Steel</t>
+  </si>
+  <si>
+    <t>Ashes</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Wax</t>
+  </si>
+  <si>
+    <t>Broken Candlestick</t>
+  </si>
+  <si>
+    <t>Candlestick</t>
+  </si>
+  <si>
+    <t>Candle</t>
+  </si>
+  <si>
+    <t>Lord's Day Candle</t>
+  </si>
+  <si>
+    <t>Soldier's Covenant</t>
+  </si>
+  <si>
+    <t>Household Item</t>
+  </si>
+  <si>
+    <t>Lighter</t>
+  </si>
+  <si>
+    <t>Lord's Day Papers</t>
   </si>
 </sst>
 </file>
@@ -4269,7 +4314,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>1071</v>
+        <v>1067</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -12152,7 +12197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
@@ -12351,7 +12396,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>1074</v>
+        <v>1070</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
@@ -12855,7 +12900,7 @@
         <v>178</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>1075</v>
+        <v>1071</v>
       </c>
       <c r="E59">
         <v>1</v>
@@ -12869,7 +12914,7 @@
         <v>179</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>1076</v>
+        <v>1072</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -13335,7 +13380,7 @@
         <v>351</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="D99" t="s">
         <v>702</v>
@@ -13419,7 +13464,7 @@
         <v>359</v>
       </c>
       <c r="C107" s="15" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
       <c r="E107">
         <v>100</v>
@@ -13464,7 +13509,7 @@
         <v>363</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
       <c r="G111" t="s">
         <v>736</v>
@@ -13921,7 +13966,7 @@
         <v>1005</v>
       </c>
       <c r="C7" t="s">
-        <v>1062</v>
+        <v>1058</v>
       </c>
       <c r="D7" t="s">
         <v>738</v>
@@ -13945,10 +13990,10 @@
         <v>1.4</v>
       </c>
       <c r="Q7" t="s">
-        <v>1070</v>
+        <v>1066</v>
       </c>
       <c r="R7" t="s">
-        <v>1064</v>
+        <v>1060</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -13956,7 +14001,7 @@
         <v>1006</v>
       </c>
       <c r="C8" t="s">
-        <v>1063</v>
+        <v>1059</v>
       </c>
       <c r="D8" t="s">
         <v>1038</v>
@@ -14024,7 +14069,7 @@
         <v>1102</v>
       </c>
       <c r="C11" t="s">
-        <v>1065</v>
+        <v>1061</v>
       </c>
       <c r="E11" t="s">
         <v>450</v>
@@ -14035,7 +14080,7 @@
         <v>1103</v>
       </c>
       <c r="C12" t="s">
-        <v>1067</v>
+        <v>1063</v>
       </c>
       <c r="E12" t="s">
         <v>455</v>
@@ -14079,7 +14124,7 @@
         <v>1116</v>
       </c>
       <c r="C16" t="s">
-        <v>1066</v>
+        <v>1062</v>
       </c>
       <c r="E16" t="s">
         <v>459</v>
@@ -14101,7 +14146,7 @@
         <v>1118</v>
       </c>
       <c r="C18" t="s">
-        <v>1068</v>
+        <v>1064</v>
       </c>
       <c r="E18" t="s">
         <v>458</v>
@@ -14935,13 +14980,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y241"/>
+  <dimension ref="A1:Y252"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
+      <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15294,7 +15339,7 @@
         <v>10</v>
       </c>
       <c r="W21" t="s">
-        <v>1073</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
@@ -15319,7 +15364,7 @@
         <v>2120</v>
       </c>
       <c r="C23" t="s">
-        <v>1077</v>
+        <v>1073</v>
       </c>
       <c r="H23">
         <v>18</v>
@@ -15333,7 +15378,7 @@
         <v>2121</v>
       </c>
       <c r="C24" t="s">
-        <v>1078</v>
+        <v>1074</v>
       </c>
       <c r="H24">
         <v>16</v>
@@ -15347,7 +15392,7 @@
         <v>2122</v>
       </c>
       <c r="C25" t="s">
-        <v>1079</v>
+        <v>1075</v>
       </c>
       <c r="H25">
         <v>18</v>
@@ -15361,7 +15406,7 @@
         <v>2123</v>
       </c>
       <c r="C26" t="s">
-        <v>1081</v>
+        <v>1077</v>
       </c>
       <c r="H26">
         <v>25</v>
@@ -15375,13 +15420,13 @@
         <v>2124</v>
       </c>
       <c r="C27" t="s">
-        <v>1082</v>
+        <v>1078</v>
       </c>
       <c r="D27" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="W27" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
@@ -15389,7 +15434,7 @@
         <v>2125</v>
       </c>
       <c r="C28" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -15457,7 +15502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>2141</v>
       </c>
@@ -15474,7 +15519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>2142</v>
       </c>
@@ -15494,18 +15539,21 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>2151</v>
       </c>
       <c r="C35" t="s">
         <v>88</v>
       </c>
+      <c r="D35" t="s">
+        <v>1093</v>
+      </c>
       <c r="G35">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>2152</v>
       </c>
@@ -15516,7 +15564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>2153</v>
       </c>
@@ -15527,7 +15575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>2154</v>
       </c>
@@ -15538,7 +15586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>2155</v>
       </c>
@@ -15552,7 +15600,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>2156</v>
       </c>
@@ -15566,7 +15614,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41">
         <v>2157</v>
       </c>
@@ -15580,7 +15628,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2158</v>
       </c>
@@ -15594,7 +15642,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43">
         <v>2159</v>
       </c>
@@ -15608,923 +15656,828 @@
         <v>10100</v>
       </c>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>2161</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1096</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45">
-        <v>2201</v>
+        <v>2162</v>
       </c>
       <c r="C45" t="s">
-        <v>274</v>
-      </c>
-      <c r="D45" t="s">
-        <v>27</v>
-      </c>
-      <c r="L45" s="4">
-        <v>1</v>
-      </c>
-      <c r="N45">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46">
-        <v>2202</v>
+        <v>2163</v>
       </c>
       <c r="C46" t="s">
-        <v>21</v>
-      </c>
-      <c r="L46" s="4">
-        <v>1</v>
-      </c>
-      <c r="N46">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47">
-        <v>2203</v>
+        <v>2164</v>
       </c>
       <c r="C47" t="s">
-        <v>271</v>
-      </c>
-      <c r="L47" s="4">
+        <v>1099</v>
+      </c>
+      <c r="E47">
         <v>2</v>
       </c>
-      <c r="N47">
-        <v>0.01</v>
-      </c>
-      <c r="Q47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48">
-        <v>2204</v>
+        <v>2165</v>
       </c>
       <c r="C48" t="s">
-        <v>270</v>
-      </c>
-      <c r="L48" s="4">
-        <v>3</v>
-      </c>
-      <c r="N48">
-        <v>0.08</v>
-      </c>
-      <c r="Q48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B49">
-        <v>2211</v>
-      </c>
-      <c r="C49" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49">
+        <v>1103</v>
+      </c>
+      <c r="E48">
         <v>2</v>
-      </c>
-      <c r="L49" s="4">
-        <v>7</v>
-      </c>
-      <c r="N49">
-        <v>0.15</v>
-      </c>
-      <c r="Q49">
-        <v>8</v>
       </c>
     </row>
     <row r="50" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B50">
-        <v>2212</v>
+        <v>2201</v>
       </c>
       <c r="C50" t="s">
-        <v>272</v>
-      </c>
-      <c r="E50">
-        <v>2</v>
+        <v>274</v>
+      </c>
+      <c r="D50" t="s">
+        <v>27</v>
       </c>
       <c r="L50" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N50">
-        <v>0.05</v>
-      </c>
-      <c r="Q50">
-        <v>8</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="51" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B51">
-        <v>2213</v>
+        <v>2202</v>
       </c>
       <c r="C51" t="s">
-        <v>273</v>
-      </c>
-      <c r="E51">
+        <v>21</v>
+      </c>
+      <c r="L51" s="4">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>2203</v>
+      </c>
+      <c r="C52" t="s">
+        <v>271</v>
+      </c>
+      <c r="L52" s="4">
         <v>2</v>
       </c>
-      <c r="L51" s="4">
-        <v>5</v>
-      </c>
-      <c r="N51">
-        <v>0.3</v>
-      </c>
-      <c r="Q51">
-        <v>18</v>
-      </c>
-      <c r="S51">
-        <v>-0.8</v>
+      <c r="N52">
+        <v>0.01</v>
+      </c>
+      <c r="Q52">
+        <v>4</v>
       </c>
     </row>
     <row r="53" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B53">
-        <v>2301</v>
+        <v>2204</v>
       </c>
       <c r="C53" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L53" s="13" t="s">
-        <v>855</v>
+        <v>270</v>
+      </c>
+      <c r="L53" s="4">
+        <v>3</v>
       </c>
       <c r="N53">
-        <v>3.5</v>
-      </c>
-      <c r="U53">
-        <v>1</v>
-      </c>
-      <c r="W53" t="s">
-        <v>816</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q53">
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B54">
-        <v>2311</v>
+        <v>2211</v>
       </c>
       <c r="C54" t="s">
-        <v>745</v>
-      </c>
-      <c r="D54" s="15"/>
+        <v>20</v>
+      </c>
       <c r="E54">
         <v>2</v>
       </c>
-      <c r="L54" s="13" t="s">
-        <v>856</v>
+      <c r="L54" s="4">
+        <v>7</v>
       </c>
       <c r="N54">
-        <v>5</v>
+        <v>0.15</v>
       </c>
       <c r="Q54">
-        <v>15</v>
-      </c>
-      <c r="U54">
-        <v>1</v>
-      </c>
-      <c r="W54" t="s">
-        <v>817</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B55">
-        <v>2312</v>
+        <v>2212</v>
       </c>
       <c r="C55" t="s">
-        <v>162</v>
-      </c>
-      <c r="D55" s="15"/>
+        <v>272</v>
+      </c>
       <c r="E55">
         <v>2</v>
       </c>
       <c r="L55" s="4">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="N55">
-        <v>6</v>
+        <v>0.05</v>
       </c>
       <c r="Q55">
-        <v>12</v>
-      </c>
-      <c r="U55">
         <v>8</v>
-      </c>
-      <c r="W55" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="56" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B56">
-        <v>2321</v>
+        <v>2213</v>
       </c>
       <c r="C56" t="s">
-        <v>144</v>
-      </c>
-      <c r="D56" s="15"/>
+        <v>273</v>
+      </c>
       <c r="E56">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L56" s="4">
-        <v>200</v>
+        <v>5</v>
       </c>
       <c r="N56">
-        <v>10</v>
+        <v>0.3</v>
       </c>
       <c r="Q56">
-        <v>10</v>
-      </c>
-      <c r="U56">
-        <v>6</v>
-      </c>
-      <c r="W56" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B57">
-        <v>2322</v>
-      </c>
-      <c r="C57" t="s">
-        <v>152</v>
-      </c>
-      <c r="D57" s="15"/>
-      <c r="E57">
-        <v>3</v>
-      </c>
-      <c r="L57" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="N57">
-        <v>7</v>
-      </c>
-      <c r="Q57">
-        <v>10</v>
-      </c>
-      <c r="U57">
-        <v>20</v>
-      </c>
-      <c r="W57" t="s">
-        <v>363</v>
+        <v>18</v>
+      </c>
+      <c r="S56">
+        <v>-0.8</v>
       </c>
     </row>
     <row r="58" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B58">
-        <v>2323</v>
+        <v>2301</v>
       </c>
       <c r="C58" t="s">
-        <v>156</v>
-      </c>
-      <c r="D58" s="15"/>
-      <c r="E58">
-        <v>3</v>
-      </c>
-      <c r="L58" s="4" t="s">
-        <v>342</v>
+        <v>36</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L58" s="13" t="s">
+        <v>855</v>
       </c>
       <c r="N58">
-        <v>9</v>
-      </c>
-      <c r="Q58">
-        <v>18</v>
+        <v>3.5</v>
       </c>
       <c r="U58">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W58" t="s">
-        <v>367</v>
+        <v>816</v>
       </c>
     </row>
     <row r="59" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B59">
-        <v>2331</v>
+        <v>2311</v>
       </c>
       <c r="C59" t="s">
-        <v>163</v>
+        <v>745</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59">
-        <v>4</v>
-      </c>
-      <c r="L59" s="4">
-        <v>1000</v>
+        <v>2</v>
+      </c>
+      <c r="L59" s="13" t="s">
+        <v>856</v>
       </c>
       <c r="N59">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="Q59">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="U59">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W59" t="s">
-        <v>852</v>
+        <v>817</v>
       </c>
     </row>
     <row r="60" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B60">
-        <v>2332</v>
+        <v>2312</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60">
-        <v>4</v>
-      </c>
-      <c r="L60" s="4" t="s">
-        <v>337</v>
+        <v>2</v>
+      </c>
+      <c r="L60" s="4">
+        <v>20</v>
       </c>
       <c r="N60">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Q60">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="U60">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="W60" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B61">
-        <v>2333</v>
+        <v>2321</v>
       </c>
       <c r="C61" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61">
-        <v>4</v>
-      </c>
-      <c r="L61" s="4" t="s">
-        <v>330</v>
+        <v>3</v>
+      </c>
+      <c r="L61" s="4">
+        <v>200</v>
       </c>
       <c r="N61">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q61">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="U61">
         <v>6</v>
       </c>
       <c r="W61" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="62" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B62">
-        <v>2341</v>
+        <v>2322</v>
       </c>
       <c r="C62" t="s">
-        <v>138</v>
+        <v>152</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62">
-        <v>5</v>
-      </c>
-      <c r="L62" s="4">
-        <v>600</v>
+        <v>3</v>
+      </c>
+      <c r="L62" s="4" t="s">
+        <v>340</v>
       </c>
       <c r="N62">
+        <v>7</v>
+      </c>
+      <c r="Q62">
         <v>10</v>
       </c>
-      <c r="Q62">
-        <v>6</v>
-      </c>
-      <c r="S62">
-        <v>-1</v>
-      </c>
       <c r="U62">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="W62" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="63" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B63">
-        <v>2342</v>
+        <v>2323</v>
       </c>
       <c r="C63" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63">
-        <v>5</v>
-      </c>
-      <c r="L63" s="4">
-        <v>600</v>
+        <v>3</v>
+      </c>
+      <c r="L63" s="4" t="s">
+        <v>342</v>
       </c>
       <c r="N63">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="Q63">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="U63">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="W63" t="s">
-        <v>357</v>
+        <v>367</v>
       </c>
     </row>
     <row r="64" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B64">
-        <v>2343</v>
+        <v>2331</v>
       </c>
       <c r="C64" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="L64" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N64">
+        <v>12</v>
+      </c>
+      <c r="Q64">
         <v>5</v>
       </c>
-      <c r="L64" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="N64">
-        <v>8</v>
-      </c>
-      <c r="Q64">
-        <v>15</v>
-      </c>
       <c r="U64">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W64" t="s">
-        <v>364</v>
+        <v>852</v>
       </c>
     </row>
     <row r="65" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B65">
-        <v>2344</v>
+        <v>2332</v>
       </c>
       <c r="C65" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D65" s="15"/>
       <c r="E65">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="N65">
         <v>10</v>
       </c>
       <c r="Q65">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U65">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W65" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
     </row>
     <row r="66" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B66">
-        <v>2345</v>
+        <v>2333</v>
       </c>
       <c r="C66" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D66" s="15"/>
       <c r="E66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="N66">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Q66">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="U66">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W66" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="67" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B67">
-        <v>2351</v>
+        <v>2341</v>
       </c>
       <c r="C67" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67">
-        <v>6</v>
-      </c>
-      <c r="L67" s="4" t="s">
-        <v>335</v>
+        <v>5</v>
+      </c>
+      <c r="L67" s="4">
+        <v>600</v>
       </c>
       <c r="N67">
         <v>10</v>
       </c>
       <c r="Q67">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="S67">
+        <v>-1</v>
       </c>
       <c r="U67">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="W67" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="68" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B68">
-        <v>2352</v>
+        <v>2342</v>
       </c>
       <c r="C68" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68">
+        <v>5</v>
+      </c>
+      <c r="L68" s="4">
+        <v>600</v>
+      </c>
+      <c r="N68">
+        <v>12</v>
+      </c>
+      <c r="Q68">
+        <v>15</v>
+      </c>
+      <c r="U68">
         <v>6</v>
       </c>
-      <c r="L68" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="N68">
-        <v>11</v>
-      </c>
-      <c r="Q68">
-        <v>20</v>
-      </c>
-      <c r="U68">
-        <v>30</v>
-      </c>
       <c r="W68" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="69" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B69">
-        <v>2353</v>
+        <v>2343</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69">
-        <v>6</v>
-      </c>
-      <c r="L69" s="4">
-        <v>500</v>
+        <v>5</v>
+      </c>
+      <c r="L69" s="4" t="s">
+        <v>341</v>
       </c>
       <c r="N69">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q69">
-        <v>25</v>
-      </c>
-      <c r="S69">
-        <v>1</v>
-      </c>
-      <c r="T69">
-        <v>0.1</v>
+        <v>15</v>
       </c>
       <c r="U69">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="W69" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="70" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B70">
-        <v>2354</v>
+        <v>2344</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
       <c r="N70">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q70">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="U70">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="W70" t="s">
-        <v>360</v>
+        <v>371</v>
       </c>
     </row>
     <row r="71" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B71">
-        <v>2355</v>
+        <v>2345</v>
       </c>
       <c r="C71" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>331</v>
+        <v>345</v>
       </c>
       <c r="N71">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q71">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="U71">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="W71" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="72" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B72">
-        <v>2361</v>
+        <v>2351</v>
       </c>
       <c r="C72" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="N72">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q72">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U72">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="W72" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row r="73" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B73">
-        <v>2362</v>
+        <v>2352</v>
       </c>
       <c r="C73" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73">
-        <v>7</v>
-      </c>
-      <c r="L73" s="4">
-        <v>1200</v>
+        <v>6</v>
+      </c>
+      <c r="L73" s="4" t="s">
+        <v>338</v>
       </c>
       <c r="N73">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q73">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="U73">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="W73" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
     </row>
     <row r="74" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B74">
-        <v>2363</v>
+        <v>2353</v>
       </c>
       <c r="C74" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74">
+        <v>6</v>
+      </c>
+      <c r="L74" s="4">
+        <v>500</v>
+      </c>
+      <c r="N74">
         <v>7</v>
       </c>
-      <c r="L74" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="N74">
-        <v>16</v>
-      </c>
       <c r="Q74">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="S74">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="T74">
+        <v>0.1</v>
       </c>
       <c r="U74">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W74" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
     </row>
     <row r="75" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B75">
-        <v>2364</v>
+        <v>2354</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75">
+        <v>6</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="N75">
         <v>7</v>
       </c>
-      <c r="L75" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="N75">
-        <v>5</v>
-      </c>
       <c r="Q75">
+        <v>15</v>
+      </c>
+      <c r="U75">
         <v>12</v>
       </c>
-      <c r="U75">
-        <v>5</v>
-      </c>
       <c r="W75" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="76" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B76">
-        <v>2371</v>
+        <v>2355</v>
       </c>
       <c r="C76" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="N76">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q76">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U76">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="W76" t="s">
-        <v>1035</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B77">
-        <v>2372</v>
+        <v>2361</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>164</v>
       </c>
       <c r="D77" s="15"/>
       <c r="E77">
-        <v>8</v>
-      </c>
-      <c r="L77" s="4">
-        <v>500</v>
-      </c>
-      <c r="M77">
-        <v>500</v>
+        <v>7</v>
+      </c>
+      <c r="L77" s="4" t="s">
+        <v>331</v>
       </c>
       <c r="N77">
-        <v>9</v>
-      </c>
-      <c r="R77">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="Q77">
+        <v>15</v>
       </c>
       <c r="U77">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="W77" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="78" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B78">
-        <v>2373</v>
+        <v>2362</v>
       </c>
       <c r="C78" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D78" s="15"/>
       <c r="E78">
+        <v>7</v>
+      </c>
+      <c r="L78" s="4">
+        <v>1200</v>
+      </c>
+      <c r="N78">
+        <v>12</v>
+      </c>
+      <c r="Q78">
         <v>8</v>
       </c>
-      <c r="L78" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="N78">
-        <v>11</v>
-      </c>
-      <c r="Q78">
-        <v>22</v>
-      </c>
       <c r="U78">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="W78" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B79">
-        <v>2374</v>
+        <v>2363</v>
       </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D79" s="15"/>
       <c r="E79">
-        <v>8</v>
-      </c>
-      <c r="L79" s="4">
-        <v>1000</v>
+        <v>7</v>
+      </c>
+      <c r="L79" s="4" t="s">
+        <v>339</v>
       </c>
       <c r="N79">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Q79">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="S79">
-        <v>1.5</v>
-      </c>
-      <c r="T79">
-        <v>0.15</v>
+        <v>-1</v>
       </c>
       <c r="U79">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W79" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="80" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B80">
-        <v>2375</v>
+        <v>2364</v>
       </c>
       <c r="C80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D80" s="15"/>
       <c r="E80">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L80" s="4" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="N80">
+        <v>5</v>
+      </c>
+      <c r="Q80">
         <v>12</v>
       </c>
-      <c r="Q80">
-        <v>20</v>
-      </c>
       <c r="U80">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="W80" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="81" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>2381</v>
+        <v>2371</v>
       </c>
       <c r="C81" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="D81" s="15"/>
       <c r="E81">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L81" s="4" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="N81">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q81">
         <v>20</v>
@@ -16533,356 +16486,430 @@
         <v>125</v>
       </c>
       <c r="W81" t="s">
-        <v>347</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="82" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>2382</v>
+        <v>2372</v>
       </c>
       <c r="C82" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="D82" s="15"/>
       <c r="E82">
+        <v>8</v>
+      </c>
+      <c r="L82" s="4">
+        <v>500</v>
+      </c>
+      <c r="M82">
+        <v>500</v>
+      </c>
+      <c r="N82">
         <v>9</v>
       </c>
-      <c r="L82" s="4">
-        <v>1000</v>
-      </c>
-      <c r="N82">
-        <v>18</v>
-      </c>
-      <c r="Q82">
-        <v>45</v>
+      <c r="R82">
+        <v>8</v>
       </c>
       <c r="U82">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="W82" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="83" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B83">
-        <v>2391</v>
+        <v>2373</v>
       </c>
       <c r="C83" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="D83" s="15"/>
       <c r="E83">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="N83">
         <v>11</v>
       </c>
       <c r="Q83">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="U83">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="W83" t="s">
-        <v>1036</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>2392</v>
+        <v>2374</v>
       </c>
       <c r="C84" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="D84" s="15"/>
       <c r="E84">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L84" s="4">
-        <v>500</v>
-      </c>
-      <c r="M84">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N84">
-        <v>9</v>
-      </c>
-      <c r="R84">
+        <v>8</v>
+      </c>
+      <c r="Q84">
+        <v>35</v>
+      </c>
+      <c r="S84">
+        <v>1.5</v>
+      </c>
+      <c r="T84">
+        <v>0.15</v>
+      </c>
+      <c r="U84">
+        <v>1</v>
+      </c>
+      <c r="W84" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="85" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>2375</v>
+      </c>
+      <c r="C85" t="s">
+        <v>161</v>
+      </c>
+      <c r="D85" s="15"/>
+      <c r="E85">
+        <v>8</v>
+      </c>
+      <c r="L85" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="N85">
         <v>12</v>
       </c>
-      <c r="U84">
-        <v>40</v>
-      </c>
-      <c r="W84" t="s">
-        <v>351</v>
+      <c r="Q85">
+        <v>20</v>
+      </c>
+      <c r="U85">
+        <v>30</v>
+      </c>
+      <c r="W85" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="86" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>2401</v>
+        <v>2381</v>
       </c>
       <c r="C86" t="s">
-        <v>97</v>
-      </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="O86">
-        <v>1</v>
+        <v>165</v>
+      </c>
+      <c r="D86" s="15"/>
+      <c r="E86">
+        <v>9</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="N86">
+        <v>12</v>
+      </c>
+      <c r="Q86">
+        <v>20</v>
+      </c>
+      <c r="U86">
+        <v>125</v>
+      </c>
+      <c r="W86" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="87" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>2402</v>
+        <v>2382</v>
       </c>
       <c r="C87" t="s">
-        <v>166</v>
+        <v>151</v>
+      </c>
+      <c r="D87" s="15"/>
+      <c r="E87">
+        <v>9</v>
+      </c>
+      <c r="L87" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N87">
+        <v>18</v>
+      </c>
+      <c r="Q87">
+        <v>45</v>
+      </c>
+      <c r="U87">
+        <v>8</v>
+      </c>
+      <c r="W87" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="88" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B88">
-        <v>2403</v>
+        <v>2391</v>
       </c>
       <c r="C88" t="s">
-        <v>168</v>
-      </c>
-      <c r="O88">
-        <v>1</v>
+        <v>137</v>
+      </c>
+      <c r="D88" s="15"/>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="L88" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="N88">
+        <v>11</v>
+      </c>
+      <c r="Q88">
+        <v>25</v>
+      </c>
+      <c r="U88">
+        <v>125</v>
+      </c>
+      <c r="W88" t="s">
+        <v>1036</v>
       </c>
     </row>
     <row r="89" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>2404</v>
+        <v>2392</v>
       </c>
       <c r="C89" t="s">
-        <v>167</v>
-      </c>
-      <c r="O89">
-        <v>2</v>
-      </c>
-      <c r="S89">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="90" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B90">
-        <v>2411</v>
-      </c>
-      <c r="C90" t="s">
-        <v>98</v>
-      </c>
-      <c r="E90">
-        <v>2</v>
-      </c>
-      <c r="O90">
-        <v>2</v>
+        <v>141</v>
+      </c>
+      <c r="D89" s="15"/>
+      <c r="E89">
+        <v>10</v>
+      </c>
+      <c r="L89" s="4">
+        <v>500</v>
+      </c>
+      <c r="M89">
+        <v>500</v>
+      </c>
+      <c r="N89">
+        <v>9</v>
+      </c>
+      <c r="R89">
+        <v>12</v>
+      </c>
+      <c r="U89">
+        <v>40</v>
+      </c>
+      <c r="W89" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="91" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2421</v>
+        <v>2401</v>
       </c>
       <c r="C91" t="s">
-        <v>99</v>
-      </c>
-      <c r="E91">
-        <v>3</v>
+        <v>97</v>
+      </c>
+      <c r="D91" t="s">
+        <v>22</v>
       </c>
       <c r="O91">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2431</v>
+        <v>2402</v>
       </c>
       <c r="C92" t="s">
-        <v>100</v>
-      </c>
-      <c r="E92">
-        <v>4</v>
-      </c>
-      <c r="O92">
-        <v>21</v>
+        <v>166</v>
       </c>
     </row>
     <row r="93" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2441</v>
+        <v>2403</v>
       </c>
       <c r="C93" t="s">
-        <v>101</v>
-      </c>
-      <c r="E93">
-        <v>5</v>
+        <v>168</v>
       </c>
       <c r="O93">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2451</v>
+        <v>2404</v>
       </c>
       <c r="C94" t="s">
-        <v>102</v>
-      </c>
-      <c r="E94">
-        <v>6</v>
+        <v>167</v>
       </c>
       <c r="O94">
-        <v>72</v>
+        <v>2</v>
+      </c>
+      <c r="S94">
+        <v>-0.5</v>
       </c>
     </row>
     <row r="95" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2461</v>
+        <v>2411</v>
       </c>
       <c r="C95" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E95">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O95">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2471</v>
+        <v>2421</v>
       </c>
       <c r="C96" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E96">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O96">
-        <v>200</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>2481</v>
+        <v>2431</v>
       </c>
       <c r="C97" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E97">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O97">
-        <v>400</v>
+        <v>21</v>
       </c>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2491</v>
+        <v>2441</v>
       </c>
       <c r="C98" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E98">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O98">
-        <v>1500</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <v>2451</v>
+      </c>
+      <c r="C99" t="s">
+        <v>102</v>
+      </c>
+      <c r="E99">
+        <v>6</v>
+      </c>
+      <c r="O99">
+        <v>72</v>
       </c>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2501</v>
+        <v>2461</v>
       </c>
       <c r="C100" t="s">
-        <v>803</v>
-      </c>
-      <c r="D100" t="s">
-        <v>23</v>
+        <v>103</v>
+      </c>
+      <c r="E100">
+        <v>7</v>
       </c>
       <c r="O100">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2502</v>
+        <v>2471</v>
       </c>
       <c r="C101" t="s">
-        <v>169</v>
-      </c>
-      <c r="N101">
-        <v>0.04</v>
+        <v>104</v>
+      </c>
+      <c r="E101">
+        <v>8</v>
+      </c>
+      <c r="O101">
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2503</v>
+        <v>2481</v>
       </c>
       <c r="C102" t="s">
-        <v>170</v>
-      </c>
-      <c r="N102">
-        <v>0.02</v>
+        <v>105</v>
+      </c>
+      <c r="E102">
+        <v>9</v>
+      </c>
+      <c r="O102">
+        <v>400</v>
       </c>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2504</v>
+        <v>2491</v>
       </c>
       <c r="C103" t="s">
-        <v>171</v>
-      </c>
-      <c r="N103">
-        <v>0.04</v>
+        <v>106</v>
+      </c>
+      <c r="E103">
+        <v>10</v>
       </c>
       <c r="O103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B104">
-        <v>2511</v>
-      </c>
-      <c r="C104" t="s">
-        <v>804</v>
-      </c>
-      <c r="E104">
-        <v>2</v>
-      </c>
-      <c r="O104">
-        <v>2</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>2512</v>
+        <v>2501</v>
       </c>
       <c r="C105" t="s">
-        <v>179</v>
-      </c>
-      <c r="E105">
-        <v>2</v>
-      </c>
-      <c r="K105">
-        <v>3</v>
-      </c>
-      <c r="N105">
-        <v>0.05</v>
+        <v>803</v>
+      </c>
+      <c r="D105" t="s">
+        <v>23</v>
       </c>
       <c r="O105">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2513</v>
+        <v>2502</v>
       </c>
       <c r="C106" t="s">
-        <v>302</v>
+        <v>169</v>
       </c>
       <c r="N106">
         <v>0.04</v>
@@ -16890,1322 +16917,1265 @@
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2521</v>
+        <v>2503</v>
       </c>
       <c r="C107" t="s">
-        <v>805</v>
-      </c>
-      <c r="E107">
-        <v>3</v>
-      </c>
-      <c r="O107">
-        <v>14</v>
+        <v>170</v>
+      </c>
+      <c r="N107">
+        <v>0.02</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2531</v>
+        <v>2504</v>
       </c>
       <c r="C108" t="s">
-        <v>806</v>
-      </c>
-      <c r="E108">
-        <v>4</v>
+        <v>171</v>
+      </c>
+      <c r="N108">
+        <v>0.04</v>
       </c>
       <c r="O108">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2541</v>
+        <v>2511</v>
       </c>
       <c r="C109" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="E109">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O109">
-        <v>48</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2551</v>
+        <v>2512</v>
       </c>
       <c r="C110" t="s">
-        <v>807</v>
+        <v>179</v>
       </c>
       <c r="E110">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="K110">
+        <v>3</v>
+      </c>
+      <c r="N110">
+        <v>0.05</v>
       </c>
       <c r="O110">
-        <v>72</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2561</v>
+        <v>2513</v>
       </c>
       <c r="C111" t="s">
-        <v>809</v>
-      </c>
-      <c r="E111">
-        <v>7</v>
-      </c>
-      <c r="O111">
-        <v>100</v>
+        <v>302</v>
+      </c>
+      <c r="N111">
+        <v>0.04</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>2571</v>
+        <v>2521</v>
       </c>
       <c r="C112" t="s">
-        <v>810</v>
+        <v>805</v>
       </c>
       <c r="E112">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O112">
-        <v>200</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B113">
-        <v>2581</v>
+        <v>2531</v>
       </c>
       <c r="C113" t="s">
-        <v>812</v>
+        <v>806</v>
       </c>
       <c r="E113">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O113">
-        <v>400</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2591</v>
+        <v>2541</v>
       </c>
       <c r="C114" t="s">
-        <v>811</v>
+        <v>808</v>
       </c>
       <c r="E114">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O114">
-        <v>1500</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <v>2551</v>
+      </c>
+      <c r="C115" t="s">
+        <v>807</v>
+      </c>
+      <c r="E115">
+        <v>6</v>
+      </c>
+      <c r="O115">
+        <v>72</v>
       </c>
     </row>
     <row r="116" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>2601</v>
+        <v>2561</v>
       </c>
       <c r="C116" t="s">
-        <v>107</v>
-      </c>
-      <c r="D116" t="s">
-        <v>24</v>
+        <v>809</v>
+      </c>
+      <c r="E116">
+        <v>7</v>
       </c>
       <c r="O116">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>2602</v>
+        <v>2571</v>
       </c>
       <c r="C117" t="s">
-        <v>172</v>
-      </c>
-      <c r="N117">
-        <v>0.02</v>
+        <v>810</v>
+      </c>
+      <c r="E117">
+        <v>8</v>
+      </c>
+      <c r="O117">
+        <v>200</v>
       </c>
     </row>
     <row r="118" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>2603</v>
+        <v>2581</v>
       </c>
       <c r="C118" t="s">
-        <v>174</v>
-      </c>
-      <c r="N118">
-        <v>0.06</v>
+        <v>812</v>
+      </c>
+      <c r="E118">
+        <v>9</v>
+      </c>
+      <c r="O118">
+        <v>400</v>
       </c>
     </row>
     <row r="119" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>2604</v>
+        <v>2591</v>
       </c>
       <c r="C119" t="s">
-        <v>173</v>
-      </c>
-      <c r="N119">
-        <v>0.08</v>
+        <v>811</v>
+      </c>
+      <c r="E119">
+        <v>10</v>
       </c>
       <c r="O119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B120">
-        <v>2611</v>
-      </c>
-      <c r="C120" t="s">
-        <v>108</v>
-      </c>
-      <c r="E120">
-        <v>2</v>
-      </c>
-      <c r="O120">
-        <v>2</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="121" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2621</v>
+        <v>2601</v>
       </c>
       <c r="C121" t="s">
-        <v>109</v>
-      </c>
-      <c r="E121">
-        <v>3</v>
+        <v>107</v>
+      </c>
+      <c r="D121" t="s">
+        <v>24</v>
       </c>
       <c r="O121">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2631</v>
+        <v>2602</v>
       </c>
       <c r="C122" t="s">
-        <v>110</v>
-      </c>
-      <c r="E122">
-        <v>4</v>
-      </c>
-      <c r="O122">
-        <v>21</v>
+        <v>172</v>
+      </c>
+      <c r="N122">
+        <v>0.02</v>
       </c>
     </row>
     <row r="123" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2641</v>
+        <v>2603</v>
       </c>
       <c r="C123" t="s">
-        <v>743</v>
-      </c>
-      <c r="E123">
-        <v>5</v>
-      </c>
-      <c r="O123">
-        <v>48</v>
+        <v>174</v>
+      </c>
+      <c r="N123">
+        <v>0.06</v>
       </c>
     </row>
     <row r="124" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2651</v>
+        <v>2604</v>
       </c>
       <c r="C124" t="s">
-        <v>111</v>
-      </c>
-      <c r="E124">
-        <v>6</v>
+        <v>173</v>
+      </c>
+      <c r="N124">
+        <v>0.08</v>
       </c>
       <c r="O124">
-        <v>72</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>2661</v>
+        <v>2611</v>
       </c>
       <c r="C125" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E125">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O125">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2671</v>
+        <v>2621</v>
       </c>
       <c r="C126" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E126">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O126">
-        <v>200</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B127">
-        <v>2681</v>
+        <v>2631</v>
       </c>
       <c r="C127" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E127">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O127">
-        <v>400</v>
+        <v>21</v>
       </c>
     </row>
     <row r="128" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2691</v>
+        <v>2641</v>
       </c>
       <c r="C128" t="s">
-        <v>115</v>
+        <v>743</v>
       </c>
       <c r="E128">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O128">
-        <v>1500</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="129" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>2651</v>
+      </c>
+      <c r="C129" t="s">
+        <v>111</v>
+      </c>
+      <c r="E129">
+        <v>6</v>
+      </c>
+      <c r="O129">
+        <v>72</v>
       </c>
     </row>
     <row r="130" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2701</v>
+        <v>2661</v>
       </c>
       <c r="C130" t="s">
-        <v>116</v>
-      </c>
-      <c r="D130" t="s">
-        <v>25</v>
+        <v>112</v>
+      </c>
+      <c r="E130">
+        <v>7</v>
       </c>
       <c r="O130">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="131" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2702</v>
+        <v>2671</v>
       </c>
       <c r="C131" t="s">
-        <v>175</v>
+        <v>113</v>
+      </c>
+      <c r="E131">
+        <v>8</v>
+      </c>
+      <c r="O131">
+        <v>200</v>
       </c>
     </row>
     <row r="132" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2703</v>
+        <v>2681</v>
       </c>
       <c r="C132" t="s">
-        <v>176</v>
-      </c>
-      <c r="S132">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="E132">
+        <v>9</v>
+      </c>
+      <c r="O132">
+        <v>400</v>
       </c>
     </row>
     <row r="133" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2704</v>
+        <v>2691</v>
       </c>
       <c r="C133" t="s">
-        <v>177</v>
+        <v>115</v>
+      </c>
+      <c r="E133">
+        <v>10</v>
       </c>
       <c r="O133">
-        <v>1</v>
-      </c>
-      <c r="S133">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="134" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B134">
-        <v>2705</v>
-      </c>
-      <c r="C134" t="s">
-        <v>303</v>
-      </c>
-      <c r="O134">
-        <v>2</v>
-      </c>
-      <c r="S134">
-        <v>2</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="135" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2711</v>
+        <v>2701</v>
       </c>
       <c r="C135" t="s">
-        <v>117</v>
-      </c>
-      <c r="E135">
-        <v>2</v>
+        <v>116</v>
+      </c>
+      <c r="D135" t="s">
+        <v>25</v>
       </c>
       <c r="O135">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B136">
-        <v>2712</v>
+        <v>2702</v>
       </c>
       <c r="C136" t="s">
-        <v>178</v>
-      </c>
-      <c r="E136">
-        <v>2</v>
-      </c>
-      <c r="O136">
-        <v>1</v>
-      </c>
-      <c r="S136">
-        <v>3</v>
+        <v>175</v>
       </c>
     </row>
     <row r="137" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>2713</v>
+        <v>2703</v>
       </c>
       <c r="C137" t="s">
-        <v>304</v>
-      </c>
-      <c r="E137">
-        <v>2</v>
-      </c>
-      <c r="L137" s="4">
+        <v>176</v>
+      </c>
+      <c r="S137">
         <v>1</v>
-      </c>
-      <c r="O137">
-        <v>3</v>
-      </c>
-      <c r="S137">
-        <v>2</v>
       </c>
     </row>
     <row r="138" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2714</v>
+        <v>2704</v>
       </c>
       <c r="C138" t="s">
-        <v>305</v>
-      </c>
-      <c r="E138">
+        <v>177</v>
+      </c>
+      <c r="O138">
+        <v>1</v>
+      </c>
+      <c r="S138">
         <v>2</v>
-      </c>
-      <c r="O138">
-        <v>2</v>
-      </c>
-      <c r="S138">
-        <v>3</v>
       </c>
     </row>
     <row r="139" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2721</v>
+        <v>2705</v>
       </c>
       <c r="C139" t="s">
-        <v>118</v>
-      </c>
-      <c r="E139">
-        <v>3</v>
+        <v>303</v>
       </c>
       <c r="O139">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="S139">
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2731</v>
+        <v>2711</v>
       </c>
       <c r="C140" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E140">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O140">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="141" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>2741</v>
+        <v>2712</v>
       </c>
       <c r="C141" t="s">
-        <v>120</v>
+        <v>178</v>
       </c>
       <c r="E141">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O141">
-        <v>48</v>
+        <v>1</v>
+      </c>
+      <c r="S141">
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2751</v>
+        <v>2713</v>
       </c>
       <c r="C142" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="E142">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="L142" s="4">
+        <v>1</v>
       </c>
       <c r="O142">
-        <v>72</v>
+        <v>3</v>
+      </c>
+      <c r="S142">
+        <v>2</v>
       </c>
     </row>
     <row r="143" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B143">
-        <v>2761</v>
+        <v>2714</v>
       </c>
       <c r="C143" t="s">
-        <v>122</v>
+        <v>305</v>
       </c>
       <c r="E143">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O143">
-        <v>100</v>
+        <v>2</v>
+      </c>
+      <c r="S143">
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2771</v>
+        <v>2721</v>
       </c>
       <c r="C144" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E144">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="O144">
-        <v>200</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>2781</v>
+        <v>2731</v>
       </c>
       <c r="C145" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E145">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="O145">
-        <v>400</v>
+        <v>21</v>
       </c>
     </row>
     <row r="146" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>2791</v>
+        <v>2741</v>
       </c>
       <c r="C146" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E146">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="O146">
-        <v>1500</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="147" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B147">
+        <v>2751</v>
+      </c>
+      <c r="C147" t="s">
+        <v>121</v>
+      </c>
+      <c r="E147">
+        <v>6</v>
+      </c>
+      <c r="O147">
+        <v>72</v>
       </c>
     </row>
     <row r="148" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2801</v>
+        <v>2761</v>
       </c>
       <c r="C148" t="s">
-        <v>772</v>
-      </c>
-      <c r="D148" t="s">
-        <v>26</v>
+        <v>122</v>
+      </c>
+      <c r="E148">
+        <v>7</v>
+      </c>
+      <c r="O148">
+        <v>100</v>
       </c>
     </row>
     <row r="149" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2802</v>
+        <v>2771</v>
       </c>
       <c r="C149" t="s">
-        <v>773</v>
+        <v>123</v>
+      </c>
+      <c r="E149">
+        <v>8</v>
+      </c>
+      <c r="O149">
+        <v>200</v>
       </c>
     </row>
     <row r="150" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2803</v>
+        <v>2781</v>
       </c>
       <c r="C150" t="s">
-        <v>774</v>
+        <v>124</v>
+      </c>
+      <c r="E150">
+        <v>9</v>
+      </c>
+      <c r="O150">
+        <v>400</v>
       </c>
     </row>
     <row r="151" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>2804</v>
+        <v>2791</v>
       </c>
       <c r="C151" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="152" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B152">
-        <v>2805</v>
-      </c>
-      <c r="C152" t="s">
-        <v>746</v>
+        <v>125</v>
+      </c>
+      <c r="E151">
+        <v>10</v>
+      </c>
+      <c r="O151">
+        <v>1500</v>
       </c>
     </row>
     <row r="153" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2806</v>
+        <v>2801</v>
       </c>
       <c r="C153" t="s">
-        <v>300</v>
+        <v>772</v>
+      </c>
+      <c r="D153" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="154" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2807</v>
+        <v>2802</v>
       </c>
       <c r="C154" t="s">
-        <v>1019</v>
+        <v>773</v>
       </c>
     </row>
     <row r="155" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>2808</v>
+        <v>2803</v>
+      </c>
+      <c r="C155" t="s">
+        <v>774</v>
       </c>
     </row>
     <row r="156" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>2809</v>
+        <v>2804</v>
+      </c>
+      <c r="C156" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="157" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B157">
-        <v>2810</v>
+        <v>2805</v>
+      </c>
+      <c r="C157" t="s">
+        <v>746</v>
       </c>
     </row>
     <row r="158" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2811</v>
+        <v>2806</v>
       </c>
       <c r="C158" t="s">
-        <v>775</v>
-      </c>
-      <c r="E158">
-        <v>2</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2812</v>
+        <v>2807</v>
       </c>
       <c r="C159" t="s">
-        <v>776</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="160" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>2813</v>
+        <v>2808</v>
       </c>
       <c r="C160" t="s">
-        <v>777</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="161" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2814</v>
+        <v>2809</v>
       </c>
       <c r="C161" t="s">
-        <v>800</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="162" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2815</v>
+        <v>2810</v>
       </c>
       <c r="C162" t="s">
-        <v>301</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="163" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2821</v>
+        <v>2811</v>
       </c>
       <c r="C163" t="s">
-        <v>778</v>
+        <v>775</v>
       </c>
       <c r="E163">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2822</v>
+        <v>2812</v>
       </c>
       <c r="C164" t="s">
-        <v>779</v>
+        <v>776</v>
       </c>
     </row>
     <row r="165" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2823</v>
+        <v>2813</v>
       </c>
       <c r="C165" t="s">
-        <v>781</v>
+        <v>777</v>
       </c>
     </row>
     <row r="166" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2834</v>
+        <v>2814</v>
       </c>
       <c r="C166" t="s">
-        <v>780</v>
+        <v>800</v>
       </c>
     </row>
     <row r="167" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2825</v>
+        <v>2815</v>
       </c>
       <c r="C167" t="s">
-        <v>541</v>
-      </c>
-      <c r="Y167" t="s">
-        <v>201</v>
+        <v>301</v>
       </c>
     </row>
     <row r="168" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2831</v>
+        <v>2821</v>
       </c>
       <c r="C168" t="s">
-        <v>782</v>
+        <v>778</v>
       </c>
       <c r="E168">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2832</v>
+        <v>2822</v>
       </c>
       <c r="C169" t="s">
-        <v>783</v>
+        <v>779</v>
       </c>
     </row>
     <row r="170" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2841</v>
+        <v>2823</v>
       </c>
       <c r="C170" t="s">
-        <v>785</v>
-      </c>
-      <c r="E170">
-        <v>5</v>
+        <v>781</v>
       </c>
     </row>
     <row r="171" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2842</v>
+        <v>2834</v>
       </c>
       <c r="C171" t="s">
-        <v>784</v>
+        <v>780</v>
       </c>
     </row>
     <row r="172" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2851</v>
+        <v>2825</v>
       </c>
       <c r="C172" t="s">
-        <v>786</v>
-      </c>
-      <c r="E172">
-        <v>6</v>
+        <v>541</v>
+      </c>
+      <c r="Y172" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="173" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2852</v>
+        <v>2831</v>
       </c>
       <c r="C173" t="s">
-        <v>792</v>
+        <v>782</v>
+      </c>
+      <c r="E173">
+        <v>4</v>
       </c>
     </row>
     <row r="174" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2853</v>
+        <v>2832</v>
       </c>
       <c r="C174" t="s">
-        <v>787</v>
+        <v>783</v>
       </c>
     </row>
     <row r="175" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B175">
-        <v>2861</v>
+        <v>2841</v>
       </c>
       <c r="C175" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="E175">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B176">
+        <v>2842</v>
+      </c>
+      <c r="C176" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B177">
+        <v>2851</v>
+      </c>
+      <c r="C177" t="s">
+        <v>786</v>
+      </c>
+      <c r="E177">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B178">
+        <v>2852</v>
+      </c>
+      <c r="C178" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B179">
+        <v>2853</v>
+      </c>
+      <c r="C179" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B180">
+        <v>2861</v>
+      </c>
+      <c r="C180" t="s">
+        <v>788</v>
+      </c>
+      <c r="E180">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B181">
         <v>2862</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C181" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="177" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B177">
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B182">
         <v>2863</v>
       </c>
-      <c r="C177" t="s">
+      <c r="C182" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="178" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B178">
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B183">
         <v>2864</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C183" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="179" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B179">
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B184">
         <v>2871</v>
       </c>
-      <c r="C179" t="s">
+      <c r="C184" t="s">
         <v>789</v>
       </c>
-      <c r="E179">
+      <c r="E184">
         <v>8</v>
       </c>
     </row>
-    <row r="180" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B180">
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B185">
         <v>2872</v>
       </c>
-      <c r="C180" t="s">
+      <c r="C185" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="181" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B181">
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B186">
         <v>2873</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C186" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="182" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B182">
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B187">
         <v>2881</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C187" t="s">
         <v>790</v>
       </c>
-      <c r="E182">
+      <c r="E187">
         <v>9</v>
       </c>
     </row>
-    <row r="183" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B183">
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B188">
         <v>2882</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C188" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="184" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B184">
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B189">
         <v>2883</v>
       </c>
-      <c r="C184" t="s">
+      <c r="C189" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="185" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B185">
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B190">
         <v>2891</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C190" t="s">
         <v>791</v>
       </c>
-      <c r="E185">
+      <c r="E190">
         <v>10</v>
       </c>
     </row>
-    <row r="186" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B186">
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B191">
         <v>2892</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C191" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="188" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B188">
-        <v>2901</v>
-      </c>
-      <c r="C188" t="s">
-        <v>251</v>
-      </c>
-      <c r="D188" t="s">
-        <v>251</v>
-      </c>
-      <c r="W188" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="189" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B189">
-        <v>2902</v>
-      </c>
-      <c r="C189" t="s">
-        <v>253</v>
-      </c>
-      <c r="D189" t="s">
-        <v>251</v>
-      </c>
-      <c r="E189">
-        <v>2</v>
-      </c>
-      <c r="W189" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="190" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B190">
-        <v>2903</v>
-      </c>
-      <c r="C190" t="s">
-        <v>252</v>
-      </c>
-      <c r="D190" t="s">
-        <v>251</v>
-      </c>
-      <c r="E190">
-        <v>3</v>
-      </c>
-      <c r="W190" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="191" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B191">
-        <v>2911</v>
-      </c>
-      <c r="C191" t="s">
-        <v>258</v>
-      </c>
-      <c r="D191" t="s">
-        <v>257</v>
-      </c>
-      <c r="H191" s="6"/>
-      <c r="L191" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B192">
-        <v>2912</v>
-      </c>
-      <c r="C192" t="s">
-        <v>259</v>
-      </c>
-      <c r="D192" t="s">
-        <v>257</v>
-      </c>
-      <c r="L192" s="4">
-        <v>1</v>
       </c>
     </row>
     <row r="193" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2913</v>
+        <v>2901</v>
       </c>
       <c r="C193" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="D193" t="s">
-        <v>257</v>
+        <v>251</v>
+      </c>
+      <c r="W193" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="194" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2914</v>
+        <v>2902</v>
       </c>
       <c r="C194" t="s">
-        <v>261</v>
-      </c>
-      <c r="D194" t="s">
-        <v>257</v>
+        <v>253</v>
+      </c>
+      <c r="E194">
+        <v>2</v>
+      </c>
+      <c r="W194" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="195" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2915</v>
+        <v>2903</v>
       </c>
       <c r="C195" t="s">
-        <v>262</v>
-      </c>
-      <c r="D195" t="s">
-        <v>257</v>
-      </c>
-      <c r="L195" s="4">
-        <v>1</v>
+        <v>252</v>
+      </c>
+      <c r="E195">
+        <v>3</v>
+      </c>
+      <c r="W195" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="196" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2916</v>
+        <v>2911</v>
       </c>
       <c r="C196" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="D196" t="s">
         <v>257</v>
       </c>
+      <c r="H196" s="6"/>
+      <c r="L196" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="197" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2917</v>
+        <v>2912</v>
       </c>
       <c r="C197" t="s">
-        <v>742</v>
-      </c>
-      <c r="D197" t="s">
-        <v>257</v>
+        <v>259</v>
+      </c>
+      <c r="L197" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="198" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2918</v>
+        <v>2913</v>
       </c>
       <c r="C198" t="s">
-        <v>1080</v>
-      </c>
-      <c r="D198" t="s">
-        <v>257</v>
-      </c>
-      <c r="L198" s="4">
-        <v>1.5</v>
+        <v>260</v>
       </c>
     </row>
     <row r="199" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2921</v>
+        <v>2914</v>
       </c>
       <c r="C199" t="s">
-        <v>264</v>
-      </c>
-      <c r="D199" t="s">
-        <v>263</v>
-      </c>
-      <c r="N199">
-        <v>0.04</v>
-      </c>
-      <c r="W199" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="200" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2922</v>
+        <v>2915</v>
       </c>
       <c r="C200" t="s">
-        <v>265</v>
-      </c>
-      <c r="D200" t="s">
-        <v>263</v>
-      </c>
-      <c r="N200">
-        <v>0.04</v>
-      </c>
-      <c r="W200" t="s">
-        <v>269</v>
+        <v>262</v>
+      </c>
+      <c r="L200" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2923</v>
+        <v>2916</v>
       </c>
       <c r="C201" t="s">
-        <v>266</v>
-      </c>
-      <c r="D201" t="s">
-        <v>263</v>
-      </c>
-      <c r="N201">
-        <v>0.04</v>
-      </c>
-      <c r="W201" t="s">
-        <v>267</v>
+        <v>290</v>
       </c>
     </row>
     <row r="202" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2924</v>
+        <v>2917</v>
       </c>
       <c r="C202" t="s">
-        <v>291</v>
-      </c>
-      <c r="D202" t="s">
-        <v>263</v>
-      </c>
-      <c r="L202" s="4">
-        <v>1</v>
-      </c>
-      <c r="N202">
-        <v>2.5</v>
-      </c>
-      <c r="Q202">
-        <v>6</v>
-      </c>
-      <c r="W202" t="s">
-        <v>298</v>
+        <v>742</v>
       </c>
     </row>
     <row r="203" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2925</v>
+        <v>2918</v>
       </c>
       <c r="C203" t="s">
-        <v>292</v>
-      </c>
-      <c r="D203" t="s">
-        <v>263</v>
-      </c>
-      <c r="W203" t="s">
-        <v>295</v>
+        <v>1076</v>
+      </c>
+      <c r="L203" s="4">
+        <v>1.5</v>
       </c>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2926</v>
+        <v>2921</v>
       </c>
       <c r="C204" t="s">
-        <v>293</v>
+        <v>264</v>
       </c>
       <c r="D204" t="s">
         <v>263</v>
       </c>
-      <c r="E204">
-        <v>2</v>
-      </c>
-      <c r="L204" s="4">
-        <v>1</v>
-      </c>
       <c r="N204">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="W204" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
     </row>
     <row r="205" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2927</v>
+        <v>2922</v>
       </c>
       <c r="C205" t="s">
-        <v>294</v>
-      </c>
-      <c r="D205" t="s">
-        <v>263</v>
-      </c>
-      <c r="E205">
-        <v>3</v>
-      </c>
-      <c r="L205" s="4">
-        <v>2</v>
+        <v>265</v>
       </c>
       <c r="N205">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="W205" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
     </row>
     <row r="206" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2928</v>
+        <v>2923</v>
       </c>
       <c r="C206" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D206" t="s">
-        <v>263</v>
+        <v>266</v>
+      </c>
+      <c r="N206">
+        <v>0.04</v>
       </c>
       <c r="W206" t="s">
-        <v>1072</v>
+        <v>267</v>
       </c>
     </row>
     <row r="207" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2931</v>
+        <v>2924</v>
       </c>
       <c r="C207" t="s">
-        <v>238</v>
-      </c>
-      <c r="D207" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="L207" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N207">
         <v>2.5</v>
       </c>
+      <c r="Q207">
+        <v>6</v>
+      </c>
       <c r="W207" t="s">
-        <v>815</v>
+        <v>298</v>
       </c>
     </row>
     <row r="208" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2932</v>
+        <v>2925</v>
       </c>
       <c r="C208" t="s">
-        <v>280</v>
-      </c>
-      <c r="D208" t="s">
-        <v>279</v>
-      </c>
-      <c r="L208" s="4">
-        <v>1</v>
-      </c>
-      <c r="N208">
-        <v>2</v>
-      </c>
-      <c r="Q208">
-        <v>4</v>
+        <v>292</v>
+      </c>
+      <c r="W208" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="209" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2933</v>
+        <v>2926</v>
       </c>
       <c r="C209" t="s">
-        <v>283</v>
-      </c>
-      <c r="D209" t="s">
-        <v>279</v>
+        <v>293</v>
+      </c>
+      <c r="E209">
+        <v>2</v>
       </c>
       <c r="L209" s="4">
         <v>1</v>
       </c>
       <c r="N209">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="W209" t="s">
-        <v>815</v>
+        <v>296</v>
       </c>
     </row>
     <row r="210" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B210">
-        <v>2941</v>
+        <v>2927</v>
       </c>
       <c r="C210" t="s">
-        <v>375</v>
-      </c>
-      <c r="D210" t="s">
-        <v>279</v>
+        <v>294</v>
+      </c>
+      <c r="E210">
+        <v>3</v>
+      </c>
+      <c r="L210" s="4">
+        <v>2</v>
+      </c>
+      <c r="N210">
+        <v>0.02</v>
+      </c>
+      <c r="W210" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="211" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B211">
-        <v>2942</v>
+        <v>2928</v>
       </c>
       <c r="C211" t="s">
-        <v>376</v>
-      </c>
-      <c r="D211" t="s">
-        <v>279</v>
-      </c>
-      <c r="E211">
-        <v>2</v>
+        <v>1065</v>
+      </c>
+      <c r="W211" t="s">
+        <v>1068</v>
       </c>
     </row>
     <row r="212" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2943</v>
+        <v>2931</v>
       </c>
       <c r="C212" t="s">
-        <v>377</v>
+        <v>238</v>
       </c>
       <c r="D212" t="s">
         <v>279</v>
       </c>
-      <c r="E212">
+      <c r="L212" s="4">
         <v>2</v>
+      </c>
+      <c r="N212">
+        <v>2.5</v>
+      </c>
+      <c r="W212" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="213" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2944</v>
+        <v>2932</v>
       </c>
       <c r="C213" t="s">
-        <v>378</v>
-      </c>
-      <c r="D213" t="s">
-        <v>279</v>
-      </c>
-      <c r="E213">
+        <v>280</v>
+      </c>
+      <c r="L213" s="4">
+        <v>1</v>
+      </c>
+      <c r="N213">
         <v>2</v>
       </c>
-      <c r="L213" s="4">
-        <v>3</v>
-      </c>
-      <c r="N213">
-        <v>3.5</v>
+      <c r="Q213">
+        <v>4</v>
       </c>
     </row>
     <row r="214" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2945</v>
+        <v>2933</v>
       </c>
       <c r="C214" t="s">
-        <v>379</v>
-      </c>
-      <c r="D214" t="s">
-        <v>279</v>
-      </c>
-      <c r="E214">
+        <v>283</v>
+      </c>
+      <c r="L214" s="4">
+        <v>1</v>
+      </c>
+      <c r="N214">
         <v>2</v>
+      </c>
+      <c r="W214" t="s">
+        <v>815</v>
       </c>
     </row>
     <row r="215" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2946</v>
+        <v>2941</v>
       </c>
       <c r="C215" t="s">
-        <v>380</v>
-      </c>
-      <c r="D215" t="s">
-        <v>279</v>
-      </c>
-      <c r="E215">
-        <v>2</v>
+        <v>375</v>
       </c>
     </row>
     <row r="216" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B216">
-        <v>2947</v>
+        <v>2942</v>
       </c>
       <c r="C216" t="s">
-        <v>381</v>
-      </c>
-      <c r="D216" t="s">
-        <v>279</v>
+        <v>376</v>
       </c>
       <c r="E216">
         <v>2</v>
@@ -18213,13 +18183,10 @@
     </row>
     <row r="217" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B217">
-        <v>2948</v>
+        <v>2943</v>
       </c>
       <c r="C217" t="s">
-        <v>382</v>
-      </c>
-      <c r="D217" t="s">
-        <v>279</v>
+        <v>377</v>
       </c>
       <c r="E217">
         <v>2</v>
@@ -18227,117 +18194,90 @@
     </row>
     <row r="218" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B218">
-        <v>2961</v>
+        <v>2944</v>
       </c>
       <c r="C218" t="s">
-        <v>284</v>
-      </c>
-      <c r="D218" t="s">
-        <v>286</v>
+        <v>378</v>
+      </c>
+      <c r="E218">
+        <v>2</v>
+      </c>
+      <c r="L218" s="4">
+        <v>3</v>
+      </c>
+      <c r="N218">
+        <v>3.5</v>
       </c>
     </row>
     <row r="219" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B219">
-        <v>2962</v>
+        <v>2945</v>
       </c>
       <c r="C219" t="s">
-        <v>285</v>
-      </c>
-      <c r="D219" t="s">
-        <v>286</v>
+        <v>379</v>
+      </c>
+      <c r="E219">
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B220">
-        <v>2963</v>
+        <v>2946</v>
       </c>
       <c r="C220" t="s">
-        <v>317</v>
-      </c>
-      <c r="D220" t="s">
-        <v>286</v>
-      </c>
-      <c r="L220" s="4">
-        <v>1</v>
-      </c>
-      <c r="N220">
-        <v>0.05</v>
+        <v>380</v>
+      </c>
+      <c r="E220">
+        <v>2</v>
       </c>
     </row>
     <row r="221" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B221">
-        <v>2964</v>
+        <v>2947</v>
       </c>
       <c r="C221" t="s">
-        <v>321</v>
-      </c>
-      <c r="D221" t="s">
-        <v>286</v>
-      </c>
-      <c r="N221">
-        <v>0.04</v>
+        <v>381</v>
+      </c>
+      <c r="E221">
+        <v>2</v>
       </c>
     </row>
     <row r="222" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2965</v>
+        <v>2948</v>
       </c>
       <c r="C222" t="s">
-        <v>847</v>
-      </c>
-      <c r="D222" t="s">
-        <v>286</v>
-      </c>
-      <c r="L222" s="4">
-        <v>1</v>
-      </c>
-      <c r="N222">
-        <v>0.05</v>
+        <v>382</v>
+      </c>
+      <c r="E222">
+        <v>2</v>
       </c>
     </row>
     <row r="223" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2966</v>
+        <v>2961</v>
       </c>
       <c r="C223" t="s">
-        <v>848</v>
+        <v>284</v>
       </c>
       <c r="D223" t="s">
         <v>286</v>
       </c>
-      <c r="L223" s="4">
-        <v>1</v>
-      </c>
-      <c r="N223">
-        <v>0.05</v>
-      </c>
     </row>
     <row r="224" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2967</v>
+        <v>2962</v>
       </c>
       <c r="C224" t="s">
-        <v>849</v>
-      </c>
-      <c r="D224" t="s">
-        <v>286</v>
-      </c>
-      <c r="L224" s="4">
-        <v>1</v>
-      </c>
-      <c r="N224">
-        <v>0.05</v>
+        <v>285</v>
       </c>
     </row>
     <row r="225" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2968</v>
+        <v>2963</v>
       </c>
       <c r="C225" t="s">
-        <v>850</v>
-      </c>
-      <c r="D225" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="L225" s="4">
         <v>1</v>
@@ -18348,61 +18288,52 @@
     </row>
     <row r="226" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2971</v>
+        <v>2964</v>
       </c>
       <c r="C226" t="s">
-        <v>311</v>
-      </c>
-      <c r="D226" t="s">
-        <v>306</v>
+        <v>321</v>
+      </c>
+      <c r="N226">
+        <v>0.04</v>
       </c>
     </row>
     <row r="227" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2972</v>
+        <v>2965</v>
       </c>
       <c r="C227" t="s">
-        <v>312</v>
-      </c>
-      <c r="D227" t="s">
-        <v>306</v>
+        <v>847</v>
       </c>
       <c r="L227" s="4">
         <v>1</v>
       </c>
       <c r="N227">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="228" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2973</v>
+        <v>2966</v>
       </c>
       <c r="C228" t="s">
-        <v>320</v>
-      </c>
-      <c r="D228" t="s">
-        <v>306</v>
+        <v>848</v>
       </c>
       <c r="L228" s="4">
         <v>1</v>
       </c>
       <c r="N228">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="229" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2974</v>
+        <v>2967</v>
       </c>
       <c r="C229" t="s">
-        <v>310</v>
-      </c>
-      <c r="D229" t="s">
-        <v>306</v>
-      </c>
-      <c r="E229">
-        <v>2</v>
+        <v>849</v>
+      </c>
+      <c r="L229" s="4">
+        <v>1</v>
       </c>
       <c r="N229">
         <v>0.05</v>
@@ -18410,207 +18341,308 @@
     </row>
     <row r="230" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2975</v>
+        <v>2968</v>
       </c>
       <c r="C230" t="s">
-        <v>318</v>
-      </c>
-      <c r="D230" t="s">
-        <v>306</v>
-      </c>
-      <c r="E230">
-        <v>2</v>
+        <v>850</v>
       </c>
       <c r="L230" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N230">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="231" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2976</v>
+        <v>2971</v>
       </c>
       <c r="C231" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D231" t="s">
         <v>306</v>
       </c>
-      <c r="E231">
-        <v>2</v>
-      </c>
-      <c r="L231" s="4">
-        <v>1</v>
-      </c>
     </row>
     <row r="232" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B232">
-        <v>2977</v>
+        <v>2972</v>
       </c>
       <c r="C232" t="s">
-        <v>307</v>
-      </c>
-      <c r="D232" t="s">
-        <v>306</v>
-      </c>
-      <c r="E232">
-        <v>3</v>
+        <v>312</v>
       </c>
       <c r="L232" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N232">
-        <v>0.08</v>
-      </c>
-      <c r="Q232">
-        <v>15</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="233" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B233">
-        <v>2978</v>
+        <v>2973</v>
       </c>
       <c r="C233" t="s">
-        <v>308</v>
-      </c>
-      <c r="D233" t="s">
-        <v>306</v>
-      </c>
-      <c r="E233">
-        <v>3</v>
+        <v>320</v>
       </c>
       <c r="L233" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N233">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="234" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B234">
-        <v>2979</v>
+        <v>2974</v>
       </c>
       <c r="C234" t="s">
-        <v>313</v>
-      </c>
-      <c r="D234" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="E234">
-        <v>3</v>
-      </c>
-      <c r="L234" s="4">
         <v>2</v>
       </c>
       <c r="N234">
         <v>0.05</v>
       </c>
-      <c r="Q234">
-        <v>5</v>
-      </c>
     </row>
     <row r="235" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B235">
-        <v>2980</v>
+        <v>2975</v>
       </c>
       <c r="C235" t="s">
-        <v>319</v>
-      </c>
-      <c r="D235" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="E235">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L235" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N235">
+        <v>0.02</v>
       </c>
     </row>
     <row r="236" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B236">
-        <v>2981</v>
+        <v>2976</v>
       </c>
       <c r="C236" t="s">
-        <v>314</v>
-      </c>
-      <c r="D236" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="E236">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L236" s="4">
         <v>1</v>
       </c>
-      <c r="Q236">
-        <v>5</v>
-      </c>
     </row>
     <row r="237" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B237">
-        <v>2982</v>
+        <v>2977</v>
       </c>
       <c r="C237" t="s">
-        <v>315</v>
-      </c>
-      <c r="D237" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E237">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L237" s="4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N237">
+        <v>0.08</v>
+      </c>
+      <c r="Q237">
+        <v>15</v>
       </c>
     </row>
     <row r="238" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B238">
-        <v>2983</v>
+        <v>2978</v>
       </c>
       <c r="C238" t="s">
-        <v>316</v>
-      </c>
-      <c r="D238" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="E238">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L238" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N238">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q238">
-        <v>20</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="239" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B239">
+        <v>2979</v>
+      </c>
+      <c r="C239" t="s">
+        <v>313</v>
+      </c>
+      <c r="E239">
+        <v>3</v>
+      </c>
+      <c r="L239" s="4">
+        <v>2</v>
+      </c>
+      <c r="N239">
+        <v>0.05</v>
+      </c>
+      <c r="Q239">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="240" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B240">
+        <v>2980</v>
+      </c>
+      <c r="C240" t="s">
+        <v>319</v>
+      </c>
+      <c r="E240">
+        <v>4</v>
+      </c>
+      <c r="L240" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B241">
+        <v>2981</v>
+      </c>
+      <c r="C241" t="s">
+        <v>314</v>
+      </c>
+      <c r="E241">
+        <v>4</v>
+      </c>
+      <c r="L241" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q241">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="242" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B242">
+        <v>2982</v>
+      </c>
+      <c r="C242" t="s">
+        <v>315</v>
+      </c>
+      <c r="E242">
+        <v>4</v>
+      </c>
+      <c r="L242" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B243">
+        <v>2983</v>
+      </c>
+      <c r="C243" t="s">
+        <v>316</v>
+      </c>
+      <c r="E243">
+        <v>5</v>
+      </c>
+      <c r="L243" s="4">
+        <v>5</v>
+      </c>
+      <c r="N243">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q243">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="244" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B244">
+        <v>2984</v>
+      </c>
+      <c r="C244" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B245">
+        <v>2985</v>
+      </c>
+      <c r="C245" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="246" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B246">
+        <v>2986</v>
+      </c>
+      <c r="C246" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="247" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B247">
+        <v>2987</v>
+      </c>
+      <c r="C247" t="s">
+        <v>1091</v>
+      </c>
+      <c r="E247">
+        <v>3</v>
+      </c>
+      <c r="L247" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="248" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B248">
+        <v>2988</v>
+      </c>
+      <c r="C248" t="s">
+        <v>1102</v>
+      </c>
+      <c r="E248">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B250">
         <v>2991</v>
       </c>
-      <c r="C239" t="s">
+      <c r="C250" t="s">
         <v>1041</v>
       </c>
-      <c r="D239" t="s">
+      <c r="D250" t="s">
         <v>1042</v>
       </c>
-      <c r="E239">
+      <c r="E250">
         <v>1</v>
       </c>
-      <c r="K239" s="4"/>
-      <c r="L239"/>
-    </row>
-    <row r="240" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="K240" s="4"/>
-      <c r="L240"/>
-    </row>
-    <row r="241" spans="11:12" x14ac:dyDescent="0.25">
-      <c r="K241" s="4"/>
-      <c r="L241"/>
+      <c r="K250" s="4"/>
+      <c r="L250"/>
+    </row>
+    <row r="251" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B251">
+        <v>2992</v>
+      </c>
+      <c r="C251" t="s">
+        <v>1100</v>
+      </c>
+      <c r="E251">
+        <v>2</v>
+      </c>
+      <c r="K251" s="4"/>
+      <c r="L251"/>
+    </row>
+    <row r="252" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K252" s="4"/>
+      <c r="L252"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -19993,17 +20025,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H122"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="3.28515625" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="85.42578125" customWidth="1"/>
     <col min="5" max="5" width="4.140625" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3.140625" customWidth="1"/>
     <col min="8" max="8" width="96.140625" customWidth="1"/>
   </cols>
@@ -20027,13 +20059,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>1055</v>
+        <v>1085</v>
       </c>
       <c r="F3" t="s">
-        <v>1056</v>
+        <v>1087</v>
       </c>
       <c r="H3" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -20041,16 +20073,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1054</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>1059</v>
-      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -20062,7 +20091,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -20200,7 +20229,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>1060</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -20208,7 +20237,7 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>1061</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.3i: Continued francis hall maps
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB6D363-EBC4-491D-B929-999FAFCCFAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7229C30-320F-4C88-A0BE-544C82B4EB93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="1125">
   <si>
     <t>ID</t>
   </si>
@@ -3666,15 +3666,6 @@
     <t>needed to enter ben's room in tutorial</t>
   </si>
   <si>
-    <t>Tutorial-RA door</t>
-  </si>
-  <si>
-    <t>Tutorial-2F custodial</t>
-  </si>
-  <si>
-    <t>Tutorial-2F storage</t>
-  </si>
-  <si>
     <t>Rooster</t>
   </si>
   <si>
@@ -3811,6 +3802,78 @@
   </si>
   <si>
     <t>Lord's Day Papers</t>
+  </si>
+  <si>
+    <t>Tutorial-RA door, FrancisHall-RA doors 2nd floor</t>
+  </si>
+  <si>
+    <t>FrancisHall-RA doors 1st floor</t>
+  </si>
+  <si>
+    <t>FrancisHall-RA doors ground floor</t>
+  </si>
+  <si>
+    <t>Tutorial-2F custodial, FrancisHall-2F custodial</t>
+  </si>
+  <si>
+    <t>Tutorial-2F storage, FranciscHall-2F storage</t>
+  </si>
+  <si>
+    <t>FrancisHall-LOJ door1</t>
+  </si>
+  <si>
+    <t>FrancisHall-LOJ door2</t>
+  </si>
+  <si>
+    <t>FrancisHall-LOJ door3</t>
+  </si>
+  <si>
+    <t>FrancisHall-2F mechanical</t>
+  </si>
+  <si>
+    <t>FrancisHall-stubwing door1</t>
+  </si>
+  <si>
+    <t>FrancisHall-stubwing door2</t>
+  </si>
+  <si>
+    <t>FrancisHall-chapel</t>
+  </si>
+  <si>
+    <t>FrancisHall-chapelwing door2</t>
+  </si>
+  <si>
+    <t>FrancisHall-chapelwing door1</t>
+  </si>
+  <si>
+    <t>FrancisHall-1F custodial</t>
+  </si>
+  <si>
+    <t>FrancisHall-1F storage</t>
+  </si>
+  <si>
+    <t>FrancisHall-corpus door</t>
+  </si>
+  <si>
+    <t>FrancisHall-servants common room</t>
+  </si>
+  <si>
+    <t>FrancisHall-servants door1</t>
+  </si>
+  <si>
+    <t>FrancisHall-brothers door1</t>
+  </si>
+  <si>
+    <t>FrancisHall-RD room</t>
+  </si>
+  <si>
+    <t>FrancisHall-brothers door2</t>
+  </si>
+  <si>
+    <t>FrancisHall-brothers door3</t>
+  </si>
+  <si>
+    <t>Ping Pong Table</t>
   </si>
 </sst>
 </file>
@@ -4314,7 +4377,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -12195,10 +12258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H138"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12396,7 +12459,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4">
@@ -12422,325 +12485,329 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>111</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>670</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
+        <v>108</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>1124</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
+        <v>3</v>
       </c>
       <c r="G18" t="s">
         <v>672</v>
       </c>
       <c r="H18" t="s">
-        <v>666</v>
+        <v>654</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>670</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="G19" t="s">
+        <v>672</v>
       </c>
       <c r="H19" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H20" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H21" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
-        <v>115</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>671</v>
-      </c>
-      <c r="G22" t="s">
-        <v>322</v>
+        <v>114</v>
+      </c>
+      <c r="H22" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
+        <v>671</v>
       </c>
       <c r="G23" t="s">
         <v>322</v>
       </c>
-      <c r="H23" t="s">
-        <v>666</v>
-      </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
-        <v>122</v>
+        <v>121</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>322</v>
       </c>
       <c r="H24" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H25" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H26" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
-        <v>125</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>694</v>
-      </c>
-      <c r="E27">
-        <v>2</v>
-      </c>
-      <c r="G27" t="s">
-        <v>672</v>
+        <v>124</v>
       </c>
       <c r="H27" t="s">
-        <v>698</v>
+        <v>669</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>694</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>672</v>
       </c>
       <c r="H28" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
-        <v>127</v>
-      </c>
-      <c r="E29">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="H29" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
       </c>
       <c r="H30" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
-        <v>129</v>
-      </c>
-      <c r="E31">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="H31" t="s">
-        <v>1048</v>
+        <v>701</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
       </c>
       <c r="H32" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
-        <v>131</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="G33" t="s">
-        <v>322</v>
+        <v>130</v>
       </c>
       <c r="H33" t="s">
-        <v>666</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
-        <v>132</v>
+        <v>131</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
+      </c>
+      <c r="G34" t="s">
+        <v>322</v>
       </c>
       <c r="H34" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H35" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H36" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
-        <v>141</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="E37">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
-        <v>322</v>
+        <v>134</v>
       </c>
       <c r="H37" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
-        <v>142</v>
+        <v>141</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="E38">
+        <v>9</v>
+      </c>
+      <c r="G38" t="s">
+        <v>322</v>
       </c>
       <c r="H38" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
-        <v>151</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>677</v>
-      </c>
-      <c r="D39" t="s">
-        <v>219</v>
-      </c>
-      <c r="E39">
-        <v>2</v>
-      </c>
-      <c r="G39" t="s">
-        <v>676</v>
+        <v>142</v>
       </c>
       <c r="H39" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>677</v>
+      </c>
+      <c r="D40" t="s">
+        <v>219</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="G40" t="s">
+        <v>676</v>
       </c>
       <c r="H40" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H41" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H42" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
-        <v>155</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>678</v>
+        <v>154</v>
       </c>
       <c r="H43" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="2">
-        <v>156</v>
+        <v>155</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>678</v>
       </c>
       <c r="H44" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="2">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H45" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="2">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H46" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="2">
-        <v>161</v>
-      </c>
-      <c r="C47" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E47">
-        <v>4</v>
-      </c>
-      <c r="G47" t="s">
-        <v>212</v>
+        <v>158</v>
+      </c>
+      <c r="H47" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="2">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="E48">
         <v>4</v>
@@ -12751,13 +12818,13 @@
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="2">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E49">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="G49" t="s">
         <v>212</v>
@@ -12765,27 +12832,27 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="2">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C50" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E50">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="G50" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="2">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G51" t="s">
         <v>223</v>
@@ -12793,41 +12860,38 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="2">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>225</v>
-      </c>
-      <c r="D52" t="s">
-        <v>734</v>
+        <v>224</v>
       </c>
       <c r="E52">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G52" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="2">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+      <c r="D53" t="s">
+        <v>734</v>
       </c>
       <c r="E53">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G53" t="s">
-        <v>325</v>
-      </c>
-      <c r="H53" t="s">
-        <v>679</v>
+        <v>226</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="2">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>227</v>
@@ -12835,33 +12899,36 @@
       <c r="E54">
         <v>7</v>
       </c>
+      <c r="G54" t="s">
+        <v>325</v>
+      </c>
       <c r="H54" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="2">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="E55">
-        <v>3</v>
-      </c>
-      <c r="G55" t="s">
-        <v>226</v>
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="2">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>735</v>
+        <v>233</v>
       </c>
       <c r="E56">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G56" t="s">
         <v>226</v>
@@ -12869,13 +12936,13 @@
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="2">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>234</v>
+        <v>735</v>
       </c>
       <c r="E57">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G57" t="s">
         <v>226</v>
@@ -12883,10 +12950,10 @@
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="2">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E58">
         <v>4</v>
@@ -12897,13 +12964,13 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="2">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>1071</v>
+        <v>235</v>
       </c>
       <c r="E59">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G59" t="s">
         <v>226</v>
@@ -12911,38 +12978,38 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="2">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>1072</v>
+        <v>1068</v>
       </c>
       <c r="E60">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="2">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="D61" t="s">
-        <v>217</v>
+        <v>1069</v>
       </c>
       <c r="E61">
-        <v>4</v>
-      </c>
-      <c r="G61" t="s">
-        <v>226</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="2">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
+      </c>
+      <c r="D62" t="s">
+        <v>217</v>
       </c>
       <c r="E62">
         <v>4</v>
@@ -12953,13 +13020,13 @@
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="2">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G63" t="s">
         <v>226</v>
@@ -12967,10 +13034,10 @@
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="2">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E64">
         <v>2</v>
@@ -12981,789 +13048,803 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="2">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="E65">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G65" t="s">
-        <v>681</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="2">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>715</v>
+        <v>213</v>
       </c>
       <c r="E66">
-        <v>5</v>
-      </c>
-      <c r="G66" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="H66" t="s">
-        <v>666</v>
+        <v>1</v>
+      </c>
+      <c r="G66" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="2">
-        <v>192</v>
+        <v>191</v>
+      </c>
+      <c r="C67" s="15" t="s">
+        <v>715</v>
+      </c>
+      <c r="E67">
+        <v>5</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H67" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
-        <v>193</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>716</v>
+        <v>192</v>
       </c>
       <c r="H68" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>716</v>
       </c>
       <c r="H69" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
-        <v>201</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D70" t="s">
-        <v>717</v>
-      </c>
-      <c r="E70">
-        <v>100</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>472</v>
+        <v>194</v>
+      </c>
+      <c r="H70" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
+        <v>201</v>
+      </c>
+      <c r="C71" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D71" t="s">
+        <v>717</v>
+      </c>
+      <c r="E71">
+        <v>100</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
         <v>202</v>
       </c>
-      <c r="C71" s="15" t="s">
+      <c r="C72" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="E71">
+      <c r="E72">
         <v>6</v>
       </c>
-      <c r="G71" s="8"/>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D72" t="s">
-        <v>720</v>
-      </c>
-      <c r="E72">
-        <v>7</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>721</v>
-      </c>
-      <c r="H72" t="s">
-        <v>722</v>
-      </c>
+      <c r="G72" s="8"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
+      </c>
+      <c r="D73" t="s">
+        <v>720</v>
       </c>
       <c r="E73">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G73" s="8" t="s">
-        <v>472</v>
+        <v>721</v>
       </c>
       <c r="H73" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="2">
-        <v>251</v>
+      <c r="B74" s="2" t="s">
+        <v>719</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D74" t="s">
-        <v>733</v>
+        <v>236</v>
       </c>
       <c r="E74">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G74" s="8" t="s">
         <v>472</v>
       </c>
       <c r="H74" t="s">
-        <v>666</v>
+        <v>722</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="2">
+        <v>251</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D75" t="s">
+        <v>733</v>
+      </c>
+      <c r="E75">
+        <v>1</v>
+      </c>
+      <c r="G75" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="H75" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
         <v>252</v>
       </c>
-      <c r="G75" s="8"/>
-      <c r="H75" t="s">
+      <c r="G76" s="8"/>
+      <c r="H76" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="C77" s="15" t="s">
+      <c r="C78" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D78" t="s">
         <v>207</v>
       </c>
-      <c r="E77">
+      <c r="E78">
         <v>100</v>
       </c>
-      <c r="G77" t="s">
+      <c r="G78" t="s">
         <v>682</v>
       </c>
-      <c r="H77" t="s">
+      <c r="H78" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="2">
-        <v>311</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>472</v>
-      </c>
-      <c r="H78" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="2">
-        <v>312</v>
+        <v>311</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H79" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="2">
-        <v>321</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="D80" t="s">
-        <v>684</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="G80" t="s">
-        <v>689</v>
+        <v>312</v>
       </c>
       <c r="H80" t="s">
-        <v>686</v>
+        <v>693</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
-        <v>322</v>
+        <v>321</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="D81" t="s">
+        <v>684</v>
       </c>
       <c r="E81">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G81" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="H81" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
-        <v>323</v>
+        <v>322</v>
+      </c>
+      <c r="E82">
+        <v>100</v>
       </c>
       <c r="G82" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H82" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="2">
-        <v>331</v>
-      </c>
-      <c r="C83" s="15" t="s">
-        <v>846</v>
-      </c>
-      <c r="D83" t="s">
-        <v>702</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="G83" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="H83" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="2">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>846</v>
+      </c>
+      <c r="D84" t="s">
+        <v>702</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="G84" t="s">
+        <v>689</v>
       </c>
       <c r="H84" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H85" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H86" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H87" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H88" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H89" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H90" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
-        <v>339</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="E91">
-        <v>100</v>
-      </c>
-      <c r="G91" t="s">
-        <v>690</v>
+        <v>338</v>
       </c>
       <c r="H91" t="s">
-        <v>666</v>
+        <v>710</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>711</v>
+      </c>
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="G92" t="s">
+        <v>690</v>
       </c>
       <c r="H92" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H93" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H94" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
-        <v>343</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>712</v>
-      </c>
-      <c r="G95" t="s">
-        <v>736</v>
+        <v>342</v>
       </c>
       <c r="H95" t="s">
-        <v>666</v>
+        <v>714</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
-        <v>344</v>
+        <v>343</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="G96" t="s">
+        <v>736</v>
       </c>
       <c r="H96" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H97" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
+        <v>345</v>
+      </c>
+      <c r="H98" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B99" s="2">
         <v>346</v>
       </c>
-      <c r="H98" t="s">
+      <c r="H99" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="4"/>
-      <c r="B99" s="2">
-        <v>351</v>
-      </c>
-      <c r="C99" s="15" t="s">
-        <v>1082</v>
-      </c>
-      <c r="D99" t="s">
-        <v>702</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="G99" t="s">
-        <v>689</v>
-      </c>
-      <c r="H99" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="2">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>1079</v>
+      </c>
+      <c r="D100" t="s">
+        <v>702</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="G100" t="s">
+        <v>689</v>
       </c>
       <c r="H100" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H101" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H102" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H103" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H104" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H105" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H106" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="2">
-        <v>359</v>
-      </c>
-      <c r="C107" s="15" t="s">
-        <v>1083</v>
-      </c>
-      <c r="E107">
-        <v>100</v>
-      </c>
-      <c r="G107" t="s">
-        <v>690</v>
+        <v>358</v>
       </c>
       <c r="H107" t="s">
-        <v>666</v>
+        <v>710</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="2">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>1080</v>
+      </c>
+      <c r="E108">
+        <v>100</v>
+      </c>
+      <c r="G108" t="s">
+        <v>690</v>
       </c>
       <c r="H108" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H109" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H110" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="2">
-        <v>363</v>
-      </c>
-      <c r="C111" s="15" t="s">
-        <v>1084</v>
-      </c>
-      <c r="G111" t="s">
-        <v>736</v>
+        <v>362</v>
       </c>
       <c r="H111" t="s">
-        <v>666</v>
+        <v>714</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="2">
-        <v>364</v>
+        <v>363</v>
+      </c>
+      <c r="C112" s="15" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G112" t="s">
+        <v>736</v>
       </c>
       <c r="H112" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H113" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="2">
+        <v>365</v>
+      </c>
+      <c r="H114" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A115" s="4"/>
+      <c r="B115" s="2">
         <v>366</v>
       </c>
-      <c r="H114" t="s">
+      <c r="H115" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="2">
-        <v>401</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D116" t="s">
-        <v>286</v>
-      </c>
-      <c r="E116">
-        <v>0</v>
-      </c>
-      <c r="G116" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B117" s="2">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>650</v>
+        <v>284</v>
+      </c>
+      <c r="D117" t="s">
+        <v>286</v>
       </c>
       <c r="E117">
         <v>0</v>
       </c>
       <c r="G117" t="s">
-        <v>288</v>
-      </c>
-      <c r="H117" t="s">
-        <v>723</v>
+        <v>287</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B118" s="2">
-        <v>412</v>
+        <v>411</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>650</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
       </c>
       <c r="G118" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H118" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B119" s="2">
-        <v>421</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="E119">
-        <v>20</v>
+        <v>412</v>
       </c>
       <c r="G119" t="s">
-        <v>323</v>
+        <v>289</v>
+      </c>
+      <c r="H119" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B120" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>726</v>
+        <v>725</v>
+      </c>
+      <c r="E120">
+        <v>20</v>
+      </c>
+      <c r="G120" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B121" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B122" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B123" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>729</v>
-      </c>
-      <c r="E123">
-        <v>35</v>
+        <v>728</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>753</v>
+        <v>729</v>
       </c>
       <c r="E124">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="2">
+        <v>426</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E125">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="2">
         <v>431</v>
       </c>
-      <c r="C125" s="15" t="s">
+      <c r="C126" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="E125">
+      <c r="E126">
         <v>7</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="19">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="19">
         <v>441</v>
       </c>
-      <c r="C126" s="15" t="s">
+      <c r="C127" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="E126">
+      <c r="E127">
         <v>5</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G127" t="s">
         <v>324</v>
       </c>
-      <c r="H126" t="s">
+      <c r="H127" t="s">
         <v>730</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="2">
-        <v>442</v>
-      </c>
-      <c r="H127" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B128" s="2">
+        <v>442</v>
+      </c>
+      <c r="H128" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="2">
         <v>443</v>
       </c>
-      <c r="H128" t="s">
+      <c r="H129" t="s">
         <v>732</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B130" s="2">
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="2">
         <v>501</v>
       </c>
-      <c r="C130" s="15" t="s">
+      <c r="C131" s="15" t="s">
         <v>243</v>
       </c>
-      <c r="D130" t="s">
+      <c r="D131" t="s">
         <v>242</v>
       </c>
-      <c r="E130">
+      <c r="E131">
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="2">
+    <row r="132" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B132" s="2">
         <v>502</v>
       </c>
-      <c r="C131" s="15" t="s">
+      <c r="C132" s="15" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B132" s="2">
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="2">
         <v>503</v>
       </c>
-      <c r="C132" s="15" t="s">
+      <c r="C133" s="15" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="2">
+    <row r="134" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B134" s="2">
         <v>504</v>
       </c>
-      <c r="C133" s="15" t="s">
+      <c r="C134" s="15" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B134" s="2">
+    <row r="135" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B135" s="2">
         <v>505</v>
       </c>
-      <c r="C134" s="15" t="s">
+      <c r="C135" s="15" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B135" s="2">
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="2">
         <v>511</v>
       </c>
-      <c r="C135" s="15" t="s">
+      <c r="C136" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="E135">
+      <c r="E136">
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B136" s="2">
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="2">
         <v>512</v>
       </c>
-      <c r="C136" s="15" t="s">
+      <c r="C137" s="15" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B137" s="2">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="2">
         <v>513</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C138" s="15" t="s">
         <v>250</v>
       </c>
     </row>
@@ -13966,7 +14047,7 @@
         <v>1005</v>
       </c>
       <c r="C7" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="D7" t="s">
         <v>738</v>
@@ -13990,10 +14071,10 @@
         <v>1.4</v>
       </c>
       <c r="Q7" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="R7" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -14001,7 +14082,7 @@
         <v>1006</v>
       </c>
       <c r="C8" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="D8" t="s">
         <v>1038</v>
@@ -14069,7 +14150,7 @@
         <v>1102</v>
       </c>
       <c r="C11" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="E11" t="s">
         <v>450</v>
@@ -14080,7 +14161,7 @@
         <v>1103</v>
       </c>
       <c r="C12" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="E12" t="s">
         <v>455</v>
@@ -14124,7 +14205,7 @@
         <v>1116</v>
       </c>
       <c r="C16" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="E16" t="s">
         <v>459</v>
@@ -14146,7 +14227,7 @@
         <v>1118</v>
       </c>
       <c r="C18" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="E18" t="s">
         <v>458</v>
@@ -14982,8 +15063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y252"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D132" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C36" sqref="C36"/>
@@ -15339,7 +15420,7 @@
         <v>10</v>
       </c>
       <c r="W21" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
@@ -15364,7 +15445,7 @@
         <v>2120</v>
       </c>
       <c r="C23" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="H23">
         <v>18</v>
@@ -15378,7 +15459,7 @@
         <v>2121</v>
       </c>
       <c r="C24" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="H24">
         <v>16</v>
@@ -15392,7 +15473,7 @@
         <v>2122</v>
       </c>
       <c r="C25" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="H25">
         <v>18</v>
@@ -15406,7 +15487,7 @@
         <v>2123</v>
       </c>
       <c r="C26" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="H26">
         <v>25</v>
@@ -15420,13 +15501,13 @@
         <v>2124</v>
       </c>
       <c r="C27" t="s">
+        <v>1075</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1077</v>
+      </c>
+      <c r="W27" t="s">
         <v>1078</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1080</v>
-      </c>
-      <c r="W27" t="s">
-        <v>1081</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
@@ -15434,7 +15515,7 @@
         <v>2125</v>
       </c>
       <c r="C28" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="D28" t="s">
         <v>28</v>
@@ -15547,7 +15628,7 @@
         <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -15661,10 +15742,10 @@
         <v>2161</v>
       </c>
       <c r="C44" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
       <c r="D44" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -15672,7 +15753,7 @@
         <v>2162</v>
       </c>
       <c r="C45" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
@@ -15680,7 +15761,7 @@
         <v>2163</v>
       </c>
       <c r="C46" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
@@ -15688,7 +15769,7 @@
         <v>2164</v>
       </c>
       <c r="C47" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -15699,7 +15780,7 @@
         <v>2165</v>
       </c>
       <c r="C48" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -17578,7 +17659,7 @@
         <v>2808</v>
       </c>
       <c r="C160" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="161" spans="2:25" x14ac:dyDescent="0.25">
@@ -17586,7 +17667,7 @@
         <v>2809</v>
       </c>
       <c r="C161" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="162" spans="2:25" x14ac:dyDescent="0.25">
@@ -17594,7 +17675,7 @@
         <v>2810</v>
       </c>
       <c r="C162" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="163" spans="2:25" x14ac:dyDescent="0.25">
@@ -17975,7 +18056,7 @@
         <v>2918</v>
       </c>
       <c r="C203" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="L203" s="4">
         <v>1.5</v>
@@ -18102,10 +18183,10 @@
         <v>2928</v>
       </c>
       <c r="C211" t="s">
+        <v>1062</v>
+      </c>
+      <c r="W211" t="s">
         <v>1065</v>
-      </c>
-      <c r="W211" t="s">
-        <v>1068</v>
       </c>
     </row>
     <row r="212" spans="2:23" x14ac:dyDescent="0.25">
@@ -18564,7 +18645,7 @@
         <v>2984</v>
       </c>
       <c r="C244" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="E244">
         <v>2</v>
@@ -18575,7 +18656,7 @@
         <v>2985</v>
       </c>
       <c r="C245" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="246" spans="2:17" x14ac:dyDescent="0.25">
@@ -18583,7 +18664,7 @@
         <v>2986</v>
       </c>
       <c r="C246" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="247" spans="2:17" x14ac:dyDescent="0.25">
@@ -18591,7 +18672,7 @@
         <v>2987</v>
       </c>
       <c r="C247" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="E247">
         <v>3</v>
@@ -18605,7 +18686,7 @@
         <v>2988</v>
       </c>
       <c r="C248" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="E248">
         <v>3</v>
@@ -18632,7 +18713,7 @@
         <v>2992</v>
       </c>
       <c r="C251" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="E251">
         <v>2</v>
@@ -20025,8 +20106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H122"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20059,10 +20140,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="F3" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="H3" t="s">
         <v>1054</v>
@@ -20073,41 +20154,56 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>1106</v>
+      </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
+      <c r="D6" t="s">
+        <v>1107</v>
+      </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>1055</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>5</v>
       </c>
+      <c r="D8" t="s">
+        <v>1117</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>6</v>
       </c>
+      <c r="D9" t="s">
+        <v>1110</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>7</v>
       </c>
+      <c r="D10" t="s">
+        <v>1111</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
@@ -20118,105 +20214,141 @@
       <c r="B12" s="1">
         <v>9</v>
       </c>
+      <c r="D12" t="s">
+        <v>1101</v>
+      </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>10</v>
       </c>
+      <c r="D13" t="s">
+        <v>1112</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
         <v>11</v>
       </c>
+      <c r="D14" t="s">
+        <v>1114</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
         <v>12</v>
       </c>
+      <c r="D15" t="s">
+        <v>1113</v>
+      </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
         <v>29</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -20229,7 +20361,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>1056</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
@@ -20237,22 +20369,31 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>1057</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>33</v>
       </c>
+      <c r="D36" t="s">
+        <v>1109</v>
+      </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>34</v>
       </c>
+      <c r="D37" t="s">
+        <v>1115</v>
+      </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>35</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.3p: WorkbenchInventory, HeroTreeCodes for CraftingInventory
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4CF40A-D646-4195-9B0D-FC9ED84C4F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A1C15-3160-4412-93EE-D369D13CFE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1617" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1625" uniqueCount="1241">
   <si>
     <t>ID</t>
   </si>
@@ -4202,6 +4202,27 @@
   <si>
     <t>Wooden Piece</t>
   </si>
+  <si>
+    <t>CraftIII_row</t>
+  </si>
+  <si>
+    <t>CraftIII_col</t>
+  </si>
+  <si>
+    <t>Craft III row</t>
+  </si>
+  <si>
+    <t>Craft III column</t>
+  </si>
+  <si>
+    <t>Crafting</t>
+  </si>
+  <si>
+    <t>Unlock third row in self-crafting</t>
+  </si>
+  <si>
+    <t>Unlock third column in self-crafting</t>
+  </si>
 </sst>
 </file>
 
@@ -4273,7 +4294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -4330,6 +4351,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -11225,10 +11249,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
-  <dimension ref="A1:M62"/>
+  <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11266,8 +11290,8 @@
         <v>861</v>
       </c>
       <c r="C4">
-        <f>SUM(HeroTree!E8:E56)</f>
-        <v>2043</v>
+        <f>SUM(HeroTree!E8:E59)</f>
+        <v>2133</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -11277,7 +11301,7 @@
       </c>
       <c r="C5">
         <f>C3-C4</f>
-        <v>3007</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -12051,108 +12075,151 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="28"/>
-      <c r="C51" t="s">
+      <c r="B51" s="29"/>
+      <c r="F51" s="9"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="28" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C52" t="s">
         <v>1140</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>1143</v>
       </c>
-      <c r="E51">
-        <v>15</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>949</v>
-      </c>
-      <c r="G51" s="9" t="s">
+      <c r="E52">
+        <v>5</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>948</v>
+      </c>
+      <c r="G52" s="9" t="s">
         <v>1146</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="28"/>
-      <c r="C52" t="s">
-        <v>1141</v>
-      </c>
-      <c r="D52" t="s">
-        <v>1144</v>
-      </c>
-      <c r="E52">
-        <v>55</v>
-      </c>
-      <c r="F52" s="9" t="s">
-        <v>1140</v>
-      </c>
-      <c r="G52" s="9" t="s">
-        <v>1147</v>
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B53" s="28"/>
       <c r="C53" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="D53" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E53">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>1140</v>
       </c>
       <c r="G53" s="9" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="28"/>
+      <c r="C54" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G54" s="9" t="s">
         <v>1148</v>
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="28" t="s">
-        <v>879</v>
-      </c>
+      <c r="B55" s="28"/>
       <c r="C55" t="s">
-        <v>879</v>
+        <v>1234</v>
       </c>
       <c r="D55" t="s">
-        <v>936</v>
+        <v>1236</v>
       </c>
       <c r="E55">
-        <v>250</v>
+        <v>85</v>
       </c>
       <c r="F55" t="s">
-        <v>937</v>
-      </c>
-      <c r="G55" t="s">
-        <v>988</v>
+        <v>1141</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="28"/>
+      <c r="C56" t="s">
+        <v>1235</v>
+      </c>
       <c r="D56" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E56">
+        <v>85</v>
+      </c>
+      <c r="F56" t="s">
+        <v>1142</v>
+      </c>
+      <c r="G56" s="9" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="28" t="s">
+        <v>879</v>
+      </c>
+      <c r="C58" t="s">
+        <v>879</v>
+      </c>
+      <c r="D58" t="s">
+        <v>936</v>
+      </c>
+      <c r="E58">
+        <v>250</v>
+      </c>
+      <c r="F58" t="s">
+        <v>937</v>
+      </c>
+      <c r="G58" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="28"/>
+      <c r="D59" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G60" t="s">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
         <v>996</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G61" t="s">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
         <v>997</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="G62" t="s">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
         <v>998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B55:B56"/>
+  <mergeCells count="7">
+    <mergeCell ref="B58:B59"/>
     <mergeCell ref="B21:B43"/>
+    <mergeCell ref="B45:B50"/>
     <mergeCell ref="I10:I19"/>
     <mergeCell ref="I21:I30"/>
     <mergeCell ref="B10:B19"/>
-    <mergeCell ref="B45:B53"/>
+    <mergeCell ref="B52:B56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15444,11 +15511,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y261"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D146" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="S26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C175" sqref="C175"/>
+      <selection pane="bottomRight" activeCell="Y43" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16475,9 +16542,6 @@
       </c>
       <c r="Q60">
         <v>8</v>
-      </c>
-      <c r="Y60" t="s">
-        <v>1150</v>
       </c>
     </row>
     <row r="61" spans="2:25" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.3q: Need tools to craft certain items
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4A1C15-3160-4412-93EE-D369D13CFE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE0C89F-9D18-4FE4-8128-5440E63D65E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -11251,8 +11251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15512,7 +15512,7 @@
   <dimension ref="A1:Y261"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="S26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="R43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="Y43" sqref="Y43"/>

</xml_diff>

<commit_message>
v0.7.3t: Francis hall linkers
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE0C89F-9D18-4FE4-8128-5440E63D65E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614686DD-8B59-435B-BB9A-F8DF9F67EDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="10" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -11251,7 +11251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93F6F072-5AA1-4DF6-9E79-0C2773550AE1}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
@@ -14307,7 +14307,7 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15511,11 +15511,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y261"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="R43" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="R127" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y43" sqref="Y43"/>
+      <selection pane="bottomRight" activeCell="S149" sqref="S149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18064,7 +18064,7 @@
         <v>176</v>
       </c>
       <c r="S142">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="Y142" t="s">
         <v>1150</v>
@@ -18081,7 +18081,7 @@
         <v>1</v>
       </c>
       <c r="S143">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="144" spans="2:25" x14ac:dyDescent="0.25">
@@ -18095,7 +18095,7 @@
         <v>2</v>
       </c>
       <c r="S144">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="145" spans="2:19" x14ac:dyDescent="0.25">
@@ -18126,7 +18126,7 @@
         <v>1</v>
       </c>
       <c r="S146">
-        <v>3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="147" spans="2:19" x14ac:dyDescent="0.25">
@@ -18146,7 +18146,7 @@
         <v>3</v>
       </c>
       <c r="S147">
-        <v>2</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="148" spans="2:19" x14ac:dyDescent="0.25">
@@ -18163,7 +18163,7 @@
         <v>2</v>
       </c>
       <c r="S148">
-        <v>3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="149" spans="2:19" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.3x: Outside and Invisible light sources
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D719FE7-9403-4253-B2C0-42A2DA673E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D36230-921F-4D4E-AB32-946C51E55A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1627" uniqueCount="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="1250">
   <si>
     <t>ID</t>
   </si>
@@ -4228,6 +4228,27 @@
   </si>
   <si>
     <t>light source (9)</t>
+  </si>
+  <si>
+    <t>light source of outside light (for inside levels)</t>
+  </si>
+  <si>
+    <t>Invisible Light Source</t>
+  </si>
+  <si>
+    <t>Outside Light Source</t>
+  </si>
+  <si>
+    <t>1x1</t>
+  </si>
+  <si>
+    <t>2x1</t>
+  </si>
+  <si>
+    <t>1x2</t>
+  </si>
+  <si>
+    <t>simulates overhead light source, togglable</t>
   </si>
 </sst>
 </file>
@@ -12712,10 +12733,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H139"/>
+  <dimension ref="A1:H144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13544,775 +13565,842 @@
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>715</v>
+        <v>1245</v>
       </c>
       <c r="E68">
-        <v>5</v>
-      </c>
-      <c r="G68" s="8" t="s">
-        <v>472</v>
+        <v>0</v>
+      </c>
+      <c r="G68" t="s">
+        <v>1243</v>
       </c>
       <c r="H68" t="s">
-        <v>666</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="2">
-        <v>192</v>
+        <v>187</v>
+      </c>
+      <c r="C69" s="15" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="G69" t="s">
+        <v>1249</v>
       </c>
       <c r="H69" t="s">
-        <v>668</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="2">
-        <v>193</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>716</v>
+        <v>188</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>666</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="2">
-        <v>194</v>
+        <v>189</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>668</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="2">
-        <v>201</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>211</v>
-      </c>
-      <c r="D72" t="s">
-        <v>717</v>
+        <v>190</v>
       </c>
       <c r="E72">
-        <v>100</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>472</v>
+        <v>0</v>
+      </c>
+      <c r="H72" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="2">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>240</v>
+        <v>715</v>
       </c>
       <c r="E73">
-        <v>6</v>
-      </c>
-      <c r="G73" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>472</v>
+      </c>
+      <c r="H73" t="s">
+        <v>666</v>
+      </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D74" t="s">
-        <v>720</v>
-      </c>
-      <c r="E74">
-        <v>7</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>721</v>
+      <c r="B74" s="2">
+        <v>192</v>
       </c>
       <c r="H74" t="s">
-        <v>722</v>
+        <v>668</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="2" t="s">
-        <v>719</v>
+      <c r="B75" s="2">
+        <v>193</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="E75">
-        <v>9</v>
-      </c>
-      <c r="G75" s="8" t="s">
-        <v>472</v>
+        <v>716</v>
       </c>
       <c r="H75" t="s">
-        <v>722</v>
+        <v>666</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="2">
-        <v>251</v>
-      </c>
-      <c r="C76" s="15" t="s">
-        <v>241</v>
-      </c>
-      <c r="D76" t="s">
-        <v>733</v>
-      </c>
-      <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="G76" s="8" t="s">
-        <v>472</v>
+        <v>194</v>
       </c>
       <c r="H76" t="s">
-        <v>666</v>
+        <v>668</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
-        <v>252</v>
-      </c>
-      <c r="G77" s="8"/>
-      <c r="H77" t="s">
-        <v>668</v>
-      </c>
+        <v>201</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D77" t="s">
+        <v>717</v>
+      </c>
+      <c r="E77">
+        <v>100</v>
+      </c>
+      <c r="G77" s="8" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>202</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E78">
+        <v>6</v>
+      </c>
+      <c r="G78" s="8"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>685</v>
+        <v>718</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c r="D79" t="s">
-        <v>207</v>
+        <v>720</v>
       </c>
       <c r="E79">
-        <v>100</v>
-      </c>
-      <c r="G79" t="s">
-        <v>682</v>
+        <v>7</v>
+      </c>
+      <c r="G79" s="8" t="s">
+        <v>721</v>
       </c>
       <c r="H79" t="s">
-        <v>683</v>
+        <v>722</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="2">
-        <v>311</v>
+      <c r="B80" s="2" t="s">
+        <v>719</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>210</v>
+        <v>236</v>
+      </c>
+      <c r="E80">
+        <v>9</v>
       </c>
       <c r="G80" s="8" t="s">
         <v>472</v>
       </c>
       <c r="H80" t="s">
-        <v>692</v>
+        <v>722</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
-        <v>312</v>
+        <v>251</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" t="s">
+        <v>733</v>
+      </c>
+      <c r="E81">
+        <v>1</v>
+      </c>
+      <c r="G81" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H81" t="s">
-        <v>693</v>
+        <v>666</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
-        <v>321</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="D82" t="s">
-        <v>684</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="G82" t="s">
-        <v>689</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G82" s="8"/>
       <c r="H82" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="2">
-        <v>322</v>
-      </c>
-      <c r="E83">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B84" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C84" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D84" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84">
         <v>100</v>
       </c>
-      <c r="G83" t="s">
-        <v>690</v>
-      </c>
-      <c r="H83" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="2">
-        <v>323</v>
-      </c>
       <c r="G84" t="s">
-        <v>691</v>
+        <v>682</v>
       </c>
       <c r="H84" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>846</v>
-      </c>
-      <c r="D85" t="s">
-        <v>702</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="G85" t="s">
-        <v>689</v>
+        <v>210</v>
+      </c>
+      <c r="G85" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H85" t="s">
-        <v>703</v>
+        <v>692</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
-        <v>332</v>
+        <v>312</v>
       </c>
       <c r="H86" t="s">
-        <v>704</v>
+        <v>693</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="2">
-        <v>333</v>
+        <v>321</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="D87" t="s">
+        <v>684</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="G87" t="s">
+        <v>689</v>
       </c>
       <c r="H87" t="s">
-        <v>705</v>
+        <v>686</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="2">
-        <v>334</v>
+        <v>322</v>
+      </c>
+      <c r="E88">
+        <v>100</v>
+      </c>
+      <c r="G88" t="s">
+        <v>690</v>
       </c>
       <c r="H88" t="s">
-        <v>706</v>
+        <v>687</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="2">
-        <v>335</v>
+        <v>323</v>
+      </c>
+      <c r="G89" t="s">
+        <v>691</v>
       </c>
       <c r="H89" t="s">
-        <v>707</v>
+        <v>688</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>846</v>
+      </c>
+      <c r="D90" t="s">
+        <v>702</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="G90" t="s">
+        <v>689</v>
       </c>
       <c r="H90" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="H91" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H92" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
-        <v>339</v>
-      </c>
-      <c r="C93" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="E93">
-        <v>100</v>
-      </c>
-      <c r="G93" t="s">
-        <v>690</v>
+        <v>334</v>
       </c>
       <c r="H93" t="s">
-        <v>666</v>
+        <v>706</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H94" t="s">
-        <v>668</v>
+        <v>707</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="H95" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H96" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
-        <v>343</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>712</v>
-      </c>
-      <c r="G97" t="s">
-        <v>736</v>
+        <v>338</v>
       </c>
       <c r="H97" t="s">
-        <v>666</v>
+        <v>710</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
-        <v>344</v>
+        <v>339</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>711</v>
+      </c>
+      <c r="E98">
+        <v>100</v>
+      </c>
+      <c r="G98" t="s">
+        <v>690</v>
       </c>
       <c r="H98" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="H99" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
+        <v>341</v>
+      </c>
+      <c r="H100" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="2">
+        <v>342</v>
+      </c>
+      <c r="H101" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B102" s="2">
+        <v>343</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>712</v>
+      </c>
+      <c r="G102" t="s">
+        <v>736</v>
+      </c>
+      <c r="H102" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B103" s="2">
+        <v>344</v>
+      </c>
+      <c r="H103" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" s="2">
+        <v>345</v>
+      </c>
+      <c r="H104" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="2">
         <v>346</v>
       </c>
-      <c r="H100" t="s">
+      <c r="H105" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="4"/>
-      <c r="B101" s="2">
-        <v>351</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D101" t="s">
-        <v>702</v>
-      </c>
-      <c r="E101">
-        <v>0</v>
-      </c>
-      <c r="G101" t="s">
-        <v>689</v>
-      </c>
-      <c r="H101" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="4"/>
-      <c r="B102" s="2">
-        <v>352</v>
-      </c>
-      <c r="H102" t="s">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="4"/>
-      <c r="B103" s="2">
-        <v>353</v>
-      </c>
-      <c r="H103" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="4"/>
-      <c r="B104" s="2">
-        <v>354</v>
-      </c>
-      <c r="H104" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" s="4"/>
-      <c r="B105" s="2">
-        <v>355</v>
-      </c>
-      <c r="H105" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="2">
-        <v>356</v>
+        <v>351</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D106" t="s">
+        <v>702</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="G106" t="s">
+        <v>689</v>
       </c>
       <c r="H106" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="2">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="H107" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="2">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H108" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="2">
-        <v>359</v>
-      </c>
-      <c r="C109" s="15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E109">
-        <v>100</v>
-      </c>
-      <c r="G109" t="s">
-        <v>690</v>
+        <v>354</v>
       </c>
       <c r="H109" t="s">
-        <v>666</v>
+        <v>706</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="2">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H110" t="s">
-        <v>668</v>
+        <v>707</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="2">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="H111" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="2">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="H112" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="2">
-        <v>363</v>
-      </c>
-      <c r="C113" s="15" t="s">
-        <v>1079</v>
-      </c>
-      <c r="G113" t="s">
-        <v>736</v>
+        <v>358</v>
       </c>
       <c r="H113" t="s">
-        <v>666</v>
+        <v>710</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="2">
-        <v>364</v>
+        <v>359</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>1078</v>
+      </c>
+      <c r="E114">
+        <v>100</v>
+      </c>
+      <c r="G114" t="s">
+        <v>690</v>
       </c>
       <c r="H114" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H115" t="s">
-        <v>713</v>
+        <v>668</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="2">
+        <v>361</v>
+      </c>
+      <c r="H116" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A117" s="4"/>
+      <c r="B117" s="2">
+        <v>362</v>
+      </c>
+      <c r="H117" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A118" s="4"/>
+      <c r="B118" s="2">
+        <v>363</v>
+      </c>
+      <c r="C118" s="15" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G118" t="s">
+        <v>736</v>
+      </c>
+      <c r="H118" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A119" s="4"/>
+      <c r="B119" s="2">
+        <v>364</v>
+      </c>
+      <c r="H119" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A120" s="4"/>
+      <c r="B120" s="2">
+        <v>365</v>
+      </c>
+      <c r="H120" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A121" s="4"/>
+      <c r="B121" s="2">
         <v>366</v>
       </c>
-      <c r="H116" t="s">
+      <c r="H121" t="s">
         <v>714</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="2">
-        <v>401</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D118" t="s">
-        <v>286</v>
-      </c>
-      <c r="E118">
-        <v>0</v>
-      </c>
-      <c r="G118" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="2">
-        <v>411</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="E119">
-        <v>0</v>
-      </c>
-      <c r="G119" t="s">
-        <v>288</v>
-      </c>
-      <c r="H119" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="2">
-        <v>412</v>
-      </c>
-      <c r="G120" t="s">
-        <v>289</v>
-      </c>
-      <c r="H120" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="2">
-        <v>421</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="E121">
-        <v>20</v>
-      </c>
-      <c r="G121" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="2">
-        <v>422</v>
-      </c>
-      <c r="C122" s="15" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B123" s="2">
-        <v>423</v>
+        <v>401</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>727</v>
+        <v>284</v>
+      </c>
+      <c r="D123" t="s">
+        <v>286</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="G123" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B124" s="2">
-        <v>424</v>
+        <v>411</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>728</v>
+        <v>650</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="G124" t="s">
+        <v>288</v>
+      </c>
+      <c r="H124" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="2">
-        <v>425</v>
-      </c>
-      <c r="C125" s="15" t="s">
-        <v>729</v>
-      </c>
-      <c r="E125">
-        <v>35</v>
+        <v>412</v>
+      </c>
+      <c r="G125" t="s">
+        <v>289</v>
+      </c>
+      <c r="H125" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B126" s="2">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>753</v>
+        <v>725</v>
       </c>
       <c r="E126">
         <v>20</v>
       </c>
+      <c r="G126" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B127" s="2">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E127">
-        <v>7</v>
+        <v>726</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="19">
-        <v>441</v>
+      <c r="B128" s="2">
+        <v>423</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="E128">
-        <v>5</v>
-      </c>
-      <c r="G128" t="s">
-        <v>324</v>
-      </c>
-      <c r="H128" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="2">
-        <v>442</v>
-      </c>
-      <c r="H129" t="s">
-        <v>731</v>
+        <v>424</v>
+      </c>
+      <c r="C129" s="15" t="s">
+        <v>728</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="2">
-        <v>443</v>
-      </c>
-      <c r="H130" t="s">
-        <v>732</v>
+        <v>425</v>
+      </c>
+      <c r="C130" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="E130">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="2">
+        <v>426</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E131">
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="2">
-        <v>501</v>
+        <v>431</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D132" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E132">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B133" s="19">
+        <v>441</v>
+      </c>
+      <c r="C133" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="E133">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="2">
-        <v>502</v>
-      </c>
-      <c r="C133" s="15" t="s">
-        <v>244</v>
+      <c r="G133" t="s">
+        <v>324</v>
+      </c>
+      <c r="H133" t="s">
+        <v>730</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
-        <v>503</v>
-      </c>
-      <c r="C134" s="15" t="s">
-        <v>245</v>
+        <v>442</v>
+      </c>
+      <c r="H134" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
-        <v>504</v>
-      </c>
-      <c r="C135" s="15" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="2">
-        <v>505</v>
-      </c>
-      <c r="C136" s="15" t="s">
-        <v>247</v>
+        <v>443</v>
+      </c>
+      <c r="H135" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B137" s="2">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>248</v>
+        <v>243</v>
+      </c>
+      <c r="D137" t="s">
+        <v>242</v>
       </c>
       <c r="E137">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="2">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="C138" s="15" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="2">
+        <v>503</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="2">
+        <v>504</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B141" s="2">
+        <v>505</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B142" s="2">
+        <v>511</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E142">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="143" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B143" s="2">
+        <v>512</v>
+      </c>
+      <c r="C143" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="144" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B144" s="2">
         <v>513</v>
       </c>
-      <c r="C139" s="15" t="s">
+      <c r="C144" s="15" t="s">
         <v>250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.7.3y: GameMap::features is HashMap
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D36230-921F-4D4E-AB32-946C51E55A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60BE999-30E5-4859-80E5-81452A65ADDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" firstSheet="1" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1636" uniqueCount="1250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1644" uniqueCount="1252">
   <si>
     <t>ID</t>
   </si>
@@ -4249,6 +4249,12 @@
   </si>
   <si>
     <t>simulates overhead light source, togglable</t>
+  </si>
+  <si>
+    <t>Light Source</t>
+  </si>
+  <si>
+    <t>Light Switch</t>
   </si>
 </sst>
 </file>
@@ -4700,7 +4706,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12733,10 +12739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H144"/>
+  <dimension ref="A1:H148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13570,6 +13576,9 @@
       <c r="C68" s="15" t="s">
         <v>1245</v>
       </c>
+      <c r="D68" t="s">
+        <v>1250</v>
+      </c>
       <c r="E68">
         <v>0</v>
       </c>
@@ -13637,6 +13646,9 @@
       <c r="C73" s="15" t="s">
         <v>715</v>
       </c>
+      <c r="D73" t="s">
+        <v>217</v>
+      </c>
       <c r="E73">
         <v>5</v>
       </c>
@@ -13676,312 +13688,315 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="2">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>211</v>
+        <v>1251</v>
       </c>
       <c r="D77" t="s">
-        <v>717</v>
+        <v>734</v>
       </c>
       <c r="E77">
-        <v>100</v>
-      </c>
-      <c r="G77" s="8" t="s">
-        <v>472</v>
+        <v>0</v>
+      </c>
+      <c r="H77" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="2">
-        <v>202</v>
-      </c>
-      <c r="C78" s="15" t="s">
-        <v>240</v>
-      </c>
-      <c r="E78">
-        <v>6</v>
-      </c>
-      <c r="G78" s="8"/>
+        <v>196</v>
+      </c>
+      <c r="H78" t="s">
+        <v>667</v>
+      </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
-        <v>718</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>237</v>
-      </c>
-      <c r="D79" t="s">
-        <v>720</v>
-      </c>
-      <c r="E79">
-        <v>7</v>
-      </c>
-      <c r="G79" s="8" t="s">
-        <v>721</v>
+      <c r="B79" s="2">
+        <v>197</v>
       </c>
       <c r="H79" t="s">
-        <v>722</v>
+        <v>668</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="2" t="s">
-        <v>719</v>
-      </c>
-      <c r="C80" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="E80">
-        <v>9</v>
-      </c>
-      <c r="G80" s="8" t="s">
-        <v>472</v>
+      <c r="B80" s="2">
+        <v>198</v>
       </c>
       <c r="H80" t="s">
-        <v>722</v>
+        <v>669</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B81" s="2">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="D81" t="s">
-        <v>733</v>
+        <v>717</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G81" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="H81" t="s">
-        <v>666</v>
-      </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="2">
-        <v>252</v>
+        <v>202</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E82">
+        <v>6</v>
       </c>
       <c r="G82" s="8"/>
-      <c r="H82" t="s">
-        <v>668</v>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D83" t="s">
+        <v>720</v>
+      </c>
+      <c r="E83">
+        <v>7</v>
+      </c>
+      <c r="G83" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="H83" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>685</v>
+        <v>719</v>
       </c>
       <c r="C84" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="D84" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
       <c r="E84">
-        <v>100</v>
-      </c>
-      <c r="G84" t="s">
-        <v>682</v>
+        <v>9</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H84" t="s">
-        <v>683</v>
+        <v>722</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="2">
-        <v>311</v>
+        <v>251</v>
       </c>
       <c r="C85" s="15" t="s">
-        <v>210</v>
+        <v>241</v>
+      </c>
+      <c r="D85" t="s">
+        <v>733</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
       </c>
       <c r="G85" s="8" t="s">
         <v>472</v>
       </c>
       <c r="H85" t="s">
-        <v>692</v>
+        <v>666</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="2">
-        <v>312</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="G86" s="8"/>
       <c r="H86" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B87" s="2">
-        <v>321</v>
-      </c>
-      <c r="C87" s="15" t="s">
-        <v>684</v>
-      </c>
-      <c r="D87" t="s">
-        <v>684</v>
-      </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-      <c r="G87" t="s">
-        <v>689</v>
-      </c>
-      <c r="H87" t="s">
-        <v>686</v>
+        <v>668</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="2">
-        <v>322</v>
+      <c r="B88" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D88" t="s">
+        <v>207</v>
       </c>
       <c r="E88">
         <v>100</v>
       </c>
       <c r="G88" t="s">
-        <v>690</v>
+        <v>682</v>
       </c>
       <c r="H88" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="2">
-        <v>323</v>
-      </c>
-      <c r="G89" t="s">
-        <v>691</v>
+        <v>311</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G89" s="8" t="s">
+        <v>472</v>
       </c>
       <c r="H89" t="s">
-        <v>688</v>
+        <v>692</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
-        <v>331</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>846</v>
-      </c>
-      <c r="D90" t="s">
-        <v>702</v>
-      </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="G90" t="s">
-        <v>689</v>
+        <v>312</v>
       </c>
       <c r="H90" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
-        <v>332</v>
+        <v>321</v>
+      </c>
+      <c r="C91" s="15" t="s">
+        <v>684</v>
+      </c>
+      <c r="D91" t="s">
+        <v>684</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="G91" t="s">
+        <v>689</v>
       </c>
       <c r="H91" t="s">
-        <v>704</v>
+        <v>686</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
-        <v>333</v>
+        <v>322</v>
+      </c>
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="G92" t="s">
+        <v>690</v>
       </c>
       <c r="H92" t="s">
-        <v>705</v>
+        <v>687</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
-        <v>334</v>
+        <v>323</v>
+      </c>
+      <c r="G93" t="s">
+        <v>691</v>
       </c>
       <c r="H93" t="s">
-        <v>706</v>
+        <v>688</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
-        <v>335</v>
+        <v>331</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>846</v>
+      </c>
+      <c r="D94" t="s">
+        <v>702</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="G94" t="s">
+        <v>689</v>
       </c>
       <c r="H94" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="H95" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="H96" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="H97" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
-        <v>339</v>
-      </c>
-      <c r="C98" s="15" t="s">
-        <v>711</v>
-      </c>
-      <c r="E98">
-        <v>100</v>
-      </c>
-      <c r="G98" t="s">
-        <v>690</v>
+        <v>335</v>
       </c>
       <c r="H98" t="s">
-        <v>666</v>
+        <v>707</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="H99" t="s">
-        <v>668</v>
+        <v>708</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="H100" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="H101" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="C102" s="15" t="s">
-        <v>712</v>
+        <v>711</v>
+      </c>
+      <c r="E102">
+        <v>100</v>
       </c>
       <c r="G102" t="s">
-        <v>736</v>
+        <v>690</v>
       </c>
       <c r="H102" t="s">
         <v>666</v>
@@ -13989,7 +14004,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H103" t="s">
         <v>668</v>
@@ -13997,7 +14012,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="H104" t="s">
         <v>713</v>
@@ -14005,151 +14020,147 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="H105" t="s">
         <v>714</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A106" s="4"/>
       <c r="B106" s="2">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="C106" s="15" t="s">
-        <v>1077</v>
-      </c>
-      <c r="D106" t="s">
-        <v>702</v>
-      </c>
-      <c r="E106">
-        <v>0</v>
+        <v>712</v>
       </c>
       <c r="G106" t="s">
-        <v>689</v>
+        <v>736</v>
       </c>
       <c r="H106" t="s">
-        <v>703</v>
+        <v>666</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A107" s="4"/>
       <c r="B107" s="2">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="H107" t="s">
-        <v>704</v>
+        <v>668</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A108" s="4"/>
       <c r="B108" s="2">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="H108" t="s">
-        <v>705</v>
+        <v>713</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A109" s="4"/>
       <c r="B109" s="2">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="H109" t="s">
-        <v>706</v>
+        <v>714</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="2">
-        <v>355</v>
+        <v>351</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>1077</v>
+      </c>
+      <c r="D110" t="s">
+        <v>702</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="G110" t="s">
+        <v>689</v>
       </c>
       <c r="H110" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="2">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="H111" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="2">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="H112" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="2">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="H113" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="2">
-        <v>359</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>1078</v>
-      </c>
-      <c r="E114">
-        <v>100</v>
-      </c>
-      <c r="G114" t="s">
-        <v>690</v>
+        <v>355</v>
       </c>
       <c r="H114" t="s">
-        <v>666</v>
+        <v>707</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="2">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="H115" t="s">
-        <v>668</v>
+        <v>708</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="2">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="H116" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="2">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="H117" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="2">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>1079</v>
+        <v>1078</v>
+      </c>
+      <c r="E118">
+        <v>100</v>
       </c>
       <c r="G118" t="s">
-        <v>736</v>
+        <v>690</v>
       </c>
       <c r="H118" t="s">
         <v>666</v>
@@ -14158,7 +14169,7 @@
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="2">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="H119" t="s">
         <v>668</v>
@@ -14167,7 +14178,7 @@
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="2">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="H120" t="s">
         <v>713</v>
@@ -14176,231 +14187,273 @@
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="2">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="H121" t="s">
         <v>714</v>
       </c>
     </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A122" s="4"/>
+      <c r="B122" s="2">
+        <v>363</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G122" t="s">
+        <v>736</v>
+      </c>
+      <c r="H122" t="s">
+        <v>666</v>
+      </c>
+    </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A123" s="4"/>
       <c r="B123" s="2">
-        <v>401</v>
-      </c>
-      <c r="C123" s="15" t="s">
-        <v>284</v>
-      </c>
-      <c r="D123" t="s">
-        <v>286</v>
-      </c>
-      <c r="E123">
-        <v>0</v>
-      </c>
-      <c r="G123" t="s">
-        <v>287</v>
+        <v>364</v>
+      </c>
+      <c r="H123" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A124" s="4"/>
       <c r="B124" s="2">
-        <v>411</v>
-      </c>
-      <c r="C124" s="15" t="s">
-        <v>650</v>
-      </c>
-      <c r="E124">
-        <v>0</v>
-      </c>
-      <c r="G124" t="s">
-        <v>288</v>
+        <v>365</v>
       </c>
       <c r="H124" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A125" s="4"/>
       <c r="B125" s="2">
-        <v>412</v>
-      </c>
-      <c r="G125" t="s">
-        <v>289</v>
+        <v>366</v>
       </c>
       <c r="H125" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="2">
-        <v>421</v>
-      </c>
-      <c r="C126" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="E126">
-        <v>20</v>
-      </c>
-      <c r="G126" t="s">
-        <v>323</v>
+        <v>714</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B127" s="2">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>726</v>
+        <v>284</v>
+      </c>
+      <c r="D127" t="s">
+        <v>286</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="G127" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B128" s="2">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>727</v>
+        <v>650</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="G128" t="s">
+        <v>288</v>
+      </c>
+      <c r="H128" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="2">
-        <v>424</v>
-      </c>
-      <c r="C129" s="15" t="s">
-        <v>728</v>
+        <v>412</v>
+      </c>
+      <c r="G129" t="s">
+        <v>289</v>
+      </c>
+      <c r="H129" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="2">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="E130">
-        <v>35</v>
+        <v>20</v>
+      </c>
+      <c r="G130" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="2">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>753</v>
-      </c>
-      <c r="E131">
-        <v>20</v>
+        <v>726</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="2">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E132">
-        <v>7</v>
+        <v>727</v>
       </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="19">
-        <v>441</v>
+      <c r="B133" s="2">
+        <v>424</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="E133">
-        <v>5</v>
-      </c>
-      <c r="G133" t="s">
-        <v>324</v>
-      </c>
-      <c r="H133" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
-        <v>442</v>
-      </c>
-      <c r="H134" t="s">
-        <v>731</v>
+        <v>425</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>729</v>
+      </c>
+      <c r="E134">
+        <v>35</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
-        <v>443</v>
-      </c>
-      <c r="H135" t="s">
-        <v>732</v>
+        <v>426</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E135">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B136" s="2">
+        <v>431</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E136">
+        <v>7</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="2">
-        <v>501</v>
+      <c r="B137" s="19">
+        <v>441</v>
       </c>
       <c r="C137" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D137" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E137">
         <v>5</v>
       </c>
+      <c r="G137" t="s">
+        <v>324</v>
+      </c>
+      <c r="H137" t="s">
+        <v>730</v>
+      </c>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B138" s="2">
-        <v>502</v>
-      </c>
-      <c r="C138" s="15" t="s">
-        <v>244</v>
+        <v>442</v>
+      </c>
+      <c r="H138" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="2">
-        <v>503</v>
-      </c>
-      <c r="C139" s="15" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B140" s="2">
-        <v>504</v>
-      </c>
-      <c r="C140" s="15" t="s">
-        <v>246</v>
+        <v>443</v>
+      </c>
+      <c r="H139" t="s">
+        <v>732</v>
       </c>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="2">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>247</v>
+        <v>243</v>
+      </c>
+      <c r="D141" t="s">
+        <v>242</v>
+      </c>
+      <c r="E141">
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="2">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E142">
-        <v>9</v>
+        <v>244</v>
       </c>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" s="2">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" s="2">
+        <v>504</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B145" s="2">
+        <v>505</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B146" s="2">
+        <v>511</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="E146">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B147" s="2">
+        <v>512</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B148" s="2">
         <v>513</v>
       </c>
-      <c r="C144" s="15" t="s">
+      <c r="C148" s="15" t="s">
         <v>250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.7.4e: Fixed black line DImg bug
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A89690-0F6E-4C27-B306-ABE9564BF972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BCFF94-8F93-4874-A9D6-BD7E9685F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,6 @@
     <sheet name="Crafting" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="1271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="1276">
   <si>
     <t>ID</t>
   </si>
@@ -4313,6 +4312,21 @@
   <si>
     <t>Diamond Spear</t>
   </si>
+  <si>
+    <t>Named Zombie</t>
+  </si>
+  <si>
+    <t>Duggy</t>
+  </si>
+  <si>
+    <t>Jacob Sanchez</t>
+  </si>
+  <si>
+    <t>Mike Olenchuk</t>
+  </si>
+  <si>
+    <t>Grady Stuckman</t>
+  </si>
 </sst>
 </file>
 
@@ -4427,6 +4441,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4441,9 +4458,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5506,26 +5520,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="H1" s="27" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="H1" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
@@ -5534,13 +5548,13 @@
       <c r="H3" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="L3" s="27"/>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -11433,7 +11447,7 @@
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="29" t="s">
         <v>461</v>
       </c>
       <c r="C10" t="s">
@@ -11451,11 +11465,11 @@
       <c r="G10" t="s">
         <v>558</v>
       </c>
-      <c r="I10" s="26"/>
+      <c r="I10" s="27"/>
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+      <c r="B11" s="29"/>
       <c r="C11" t="s">
         <v>908</v>
       </c>
@@ -11471,11 +11485,11 @@
       <c r="G11" t="s">
         <v>559</v>
       </c>
-      <c r="I11" s="26"/>
+      <c r="I11" s="27"/>
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="28"/>
+      <c r="B12" s="29"/>
       <c r="C12" t="s">
         <v>909</v>
       </c>
@@ -11491,11 +11505,11 @@
       <c r="G12" t="s">
         <v>560</v>
       </c>
-      <c r="I12" s="26"/>
+      <c r="I12" s="27"/>
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="28"/>
+      <c r="B13" s="29"/>
       <c r="C13" t="s">
         <v>541</v>
       </c>
@@ -11511,11 +11525,11 @@
       <c r="G13" t="s">
         <v>561</v>
       </c>
-      <c r="I13" s="26"/>
+      <c r="I13" s="27"/>
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
+      <c r="B14" s="29"/>
       <c r="C14" t="s">
         <v>542</v>
       </c>
@@ -11531,10 +11545,10 @@
       <c r="G14" t="s">
         <v>562</v>
       </c>
-      <c r="I14" s="26"/>
+      <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="28"/>
+      <c r="B15" s="29"/>
       <c r="C15" t="s">
         <v>911</v>
       </c>
@@ -11550,10 +11564,10 @@
       <c r="G15" t="s">
         <v>563</v>
       </c>
-      <c r="I15" s="26"/>
+      <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="28"/>
+      <c r="B16" s="29"/>
       <c r="C16" t="s">
         <v>543</v>
       </c>
@@ -11569,10 +11583,10 @@
       <c r="G16" t="s">
         <v>564</v>
       </c>
-      <c r="I16" s="26"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="28"/>
+      <c r="B17" s="29"/>
       <c r="C17" t="s">
         <v>544</v>
       </c>
@@ -11588,10 +11602,10 @@
       <c r="G17" t="s">
         <v>565</v>
       </c>
-      <c r="I17" s="26"/>
+      <c r="I17" s="27"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
+      <c r="B18" s="29"/>
       <c r="C18" t="s">
         <v>545</v>
       </c>
@@ -11607,10 +11621,10 @@
       <c r="G18" t="s">
         <v>566</v>
       </c>
-      <c r="I18" s="26"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="28"/>
+      <c r="B19" s="29"/>
       <c r="C19" t="s">
         <v>546</v>
       </c>
@@ -11626,10 +11640,10 @@
       <c r="G19" t="s">
         <v>567</v>
       </c>
-      <c r="I19" s="26"/>
+      <c r="I19" s="27"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="29" t="s">
         <v>937</v>
       </c>
       <c r="C21" t="s">
@@ -11647,10 +11661,10 @@
       <c r="G21" s="8" t="s">
         <v>993</v>
       </c>
-      <c r="I21" s="26"/>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
+      <c r="B22" s="29"/>
       <c r="C22" t="s">
         <v>913</v>
       </c>
@@ -11666,10 +11680,10 @@
       <c r="G22" s="8" t="s">
         <v>967</v>
       </c>
-      <c r="I22" s="26"/>
+      <c r="I22" s="27"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="28"/>
+      <c r="B23" s="29"/>
       <c r="C23" t="s">
         <v>914</v>
       </c>
@@ -11685,10 +11699,10 @@
       <c r="G23" s="8" t="s">
         <v>966</v>
       </c>
-      <c r="I23" s="26"/>
+      <c r="I23" s="27"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="28"/>
+      <c r="B24" s="29"/>
       <c r="C24" t="s">
         <v>915</v>
       </c>
@@ -11704,10 +11718,10 @@
       <c r="G24" s="8" t="s">
         <v>968</v>
       </c>
-      <c r="I24" s="26"/>
+      <c r="I24" s="27"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="28"/>
+      <c r="B25" s="29"/>
       <c r="C25" t="s">
         <v>916</v>
       </c>
@@ -11723,10 +11737,10 @@
       <c r="G25" s="8" t="s">
         <v>969</v>
       </c>
-      <c r="I25" s="26"/>
+      <c r="I25" s="27"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="28"/>
+      <c r="B26" s="29"/>
       <c r="C26" t="s">
         <v>917</v>
       </c>
@@ -11742,10 +11756,10 @@
       <c r="G26" s="8" t="s">
         <v>974</v>
       </c>
-      <c r="I26" s="26"/>
+      <c r="I26" s="27"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="28"/>
+      <c r="B27" s="29"/>
       <c r="C27" t="s">
         <v>989</v>
       </c>
@@ -11761,10 +11775,10 @@
       <c r="G27" s="8" t="s">
         <v>992</v>
       </c>
-      <c r="I27" s="26"/>
+      <c r="I27" s="27"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="28"/>
+      <c r="B28" s="29"/>
       <c r="C28" t="s">
         <v>918</v>
       </c>
@@ -11780,10 +11794,10 @@
       <c r="G28" s="8" t="s">
         <v>970</v>
       </c>
-      <c r="I28" s="26"/>
+      <c r="I28" s="27"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="28"/>
+      <c r="B29" s="29"/>
       <c r="C29" t="s">
         <v>919</v>
       </c>
@@ -11799,10 +11813,10 @@
       <c r="G29" s="8" t="s">
         <v>971</v>
       </c>
-      <c r="I29" s="26"/>
+      <c r="I29" s="27"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="28"/>
+      <c r="B30" s="29"/>
       <c r="C30" t="s">
         <v>920</v>
       </c>
@@ -11818,10 +11832,10 @@
       <c r="G30" s="8" t="s">
         <v>972</v>
       </c>
-      <c r="I30" s="26"/>
+      <c r="I30" s="27"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="28"/>
+      <c r="B31" s="29"/>
       <c r="C31" t="s">
         <v>921</v>
       </c>
@@ -11839,7 +11853,7 @@
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="28"/>
+      <c r="B32" s="29"/>
       <c r="C32" t="s">
         <v>922</v>
       </c>
@@ -11857,7 +11871,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="28"/>
+      <c r="B33" s="29"/>
       <c r="C33" t="s">
         <v>923</v>
       </c>
@@ -11875,7 +11889,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B34" s="28"/>
+      <c r="B34" s="29"/>
       <c r="C34" t="s">
         <v>924</v>
       </c>
@@ -11893,7 +11907,7 @@
       </c>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="28"/>
+      <c r="B35" s="29"/>
       <c r="C35" t="s">
         <v>925</v>
       </c>
@@ -11911,7 +11925,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="28"/>
+      <c r="B36" s="29"/>
       <c r="C36" t="s">
         <v>926</v>
       </c>
@@ -11929,7 +11943,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" s="28"/>
+      <c r="B37" s="29"/>
       <c r="C37" t="s">
         <v>927</v>
       </c>
@@ -11947,7 +11961,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" s="28"/>
+      <c r="B38" s="29"/>
       <c r="C38" t="s">
         <v>987</v>
       </c>
@@ -11965,7 +11979,7 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" s="28"/>
+      <c r="B39" s="29"/>
       <c r="C39" t="s">
         <v>928</v>
       </c>
@@ -11983,7 +11997,7 @@
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="28"/>
+      <c r="B40" s="29"/>
       <c r="C40" t="s">
         <v>929</v>
       </c>
@@ -12001,7 +12015,7 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B41" s="28"/>
+      <c r="B41" s="29"/>
       <c r="C41" t="s">
         <v>930</v>
       </c>
@@ -12019,7 +12033,7 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B42" s="28"/>
+      <c r="B42" s="29"/>
       <c r="C42" t="s">
         <v>931</v>
       </c>
@@ -12037,7 +12051,7 @@
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B43" s="28"/>
+      <c r="B43" s="29"/>
       <c r="C43" t="s">
         <v>938</v>
       </c>
@@ -12055,7 +12069,7 @@
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>935</v>
       </c>
       <c r="C45" t="s">
@@ -12075,7 +12089,7 @@
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B46" s="28"/>
+      <c r="B46" s="29"/>
       <c r="C46" t="s">
         <v>932</v>
       </c>
@@ -12093,7 +12107,7 @@
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B47" s="28"/>
+      <c r="B47" s="29"/>
       <c r="C47" t="s">
         <v>933</v>
       </c>
@@ -12111,7 +12125,7 @@
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B48" s="28"/>
+      <c r="B48" s="29"/>
       <c r="C48" t="s">
         <v>947</v>
       </c>
@@ -12129,7 +12143,7 @@
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B49" s="28"/>
+      <c r="B49" s="29"/>
       <c r="C49" t="s">
         <v>940</v>
       </c>
@@ -12147,7 +12161,7 @@
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="28"/>
+      <c r="B50" s="29"/>
       <c r="C50" t="s">
         <v>941</v>
       </c>
@@ -12165,11 +12179,11 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B51" s="29"/>
+      <c r="B51" s="24"/>
       <c r="F51" s="9"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="29" t="s">
         <v>1236</v>
       </c>
       <c r="C52" t="s">
@@ -12189,7 +12203,7 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B53" s="28"/>
+      <c r="B53" s="29"/>
       <c r="C53" t="s">
         <v>1139</v>
       </c>
@@ -12207,7 +12221,7 @@
       </c>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B54" s="28"/>
+      <c r="B54" s="29"/>
       <c r="C54" t="s">
         <v>1140</v>
       </c>
@@ -12225,7 +12239,7 @@
       </c>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B55" s="28"/>
+      <c r="B55" s="29"/>
       <c r="C55" t="s">
         <v>1232</v>
       </c>
@@ -12243,7 +12257,7 @@
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B56" s="28"/>
+      <c r="B56" s="29"/>
       <c r="C56" t="s">
         <v>1233</v>
       </c>
@@ -12261,7 +12275,7 @@
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="29" t="s">
         <v>877</v>
       </c>
       <c r="C58" t="s">
@@ -12281,7 +12295,7 @@
       </c>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B59" s="28"/>
+      <c r="B59" s="29"/>
       <c r="D59" t="s">
         <v>577</v>
       </c>
@@ -14522,17 +14536,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
-  <dimension ref="A1:R31"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -15233,6 +15247,56 @@
       </c>
       <c r="Q31" t="s">
         <v>1029</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1301</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1272</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1271</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>1302</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1273</v>
+      </c>
+      <c r="F34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>1303</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>1304</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1275</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -15483,7 +15547,7 @@
       <c r="E16" t="s">
         <v>430</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="F16" s="25" t="s">
         <v>445</v>
       </c>
       <c r="G16" t="s">
@@ -15503,7 +15567,7 @@
       <c r="E17" t="s">
         <v>431</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="25"/>
       <c r="G17" t="s">
         <v>828</v>
       </c>
@@ -15521,7 +15585,7 @@
       <c r="E18" t="s">
         <v>441</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="25"/>
       <c r="G18" t="s">
         <v>825</v>
       </c>
@@ -15539,7 +15603,7 @@
       <c r="E19" t="s">
         <v>442</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="25"/>
       <c r="G19" t="s">
         <v>826</v>
       </c>
@@ -15729,11 +15793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y280"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L70" sqref="L70:L73"/>
+      <selection pane="bottomRight" activeCell="J67" sqref="J67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15755,23 +15819,23 @@
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="25" t="s">
+      <c r="F1" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="K1" s="25" t="s">
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="K1" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
       <c r="T1" s="7"/>
       <c r="U1" s="7"/>
     </row>
@@ -22533,7 +22597,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>38</v>
       </c>
       <c r="C4">
@@ -22556,7 +22620,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="26"/>
+      <c r="B5" s="27"/>
       <c r="C5">
         <v>102</v>
       </c>
@@ -22577,7 +22641,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="26"/>
+      <c r="B6" s="27"/>
       <c r="C6">
         <v>103</v>
       </c>
@@ -22598,7 +22662,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7">
         <v>104</v>
       </c>
@@ -22622,7 +22686,7 @@
       <c r="A8" t="s">
         <v>999</v>
       </c>
-      <c r="B8" s="26"/>
+      <c r="B8" s="27"/>
       <c r="C8">
         <v>105</v>
       </c>
@@ -22643,7 +22707,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
+      <c r="B9" s="27"/>
       <c r="C9">
         <v>106</v>
       </c>
@@ -22664,7 +22728,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10">
         <v>107</v>
       </c>
@@ -22685,7 +22749,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
+      <c r="B11" s="27"/>
       <c r="C11">
         <v>108</v>
       </c>
@@ -22706,7 +22770,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
+      <c r="B12" s="27"/>
       <c r="C12">
         <v>109</v>
       </c>
@@ -22727,7 +22791,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
+      <c r="B13" s="27"/>
       <c r="C13">
         <v>110</v>
       </c>
@@ -22748,7 +22812,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="27" t="s">
         <v>447</v>
       </c>
       <c r="C15">
@@ -22771,7 +22835,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
+      <c r="B16" s="27"/>
       <c r="C16">
         <v>112</v>
       </c>
@@ -22792,7 +22856,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
+      <c r="B17" s="27"/>
       <c r="C17">
         <v>113</v>
       </c>
@@ -22816,7 +22880,7 @@
       <c r="A18" t="s">
         <v>1000</v>
       </c>
-      <c r="B18" s="26"/>
+      <c r="B18" s="27"/>
       <c r="C18">
         <v>114</v>
       </c>
@@ -22837,7 +22901,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="26"/>
+      <c r="B19" s="27"/>
       <c r="C19">
         <v>115</v>
       </c>
@@ -22858,7 +22922,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="26"/>
+      <c r="B20" s="27"/>
       <c r="C20">
         <v>116</v>
       </c>
@@ -22879,7 +22943,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="26"/>
+      <c r="B21" s="27"/>
       <c r="C21">
         <v>117</v>
       </c>
@@ -22900,7 +22964,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="26"/>
+      <c r="B22" s="27"/>
       <c r="C22">
         <v>118</v>
       </c>
@@ -22921,7 +22985,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="26"/>
+      <c r="B23" s="27"/>
       <c r="C23">
         <v>119</v>
       </c>
@@ -22942,7 +23006,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="26"/>
+      <c r="B24" s="27"/>
       <c r="C24">
         <v>120</v>
       </c>
@@ -22963,7 +23027,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="27" t="s">
         <v>506</v>
       </c>
       <c r="C26">
@@ -22971,31 +23035,31 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="26"/>
+      <c r="B27" s="27"/>
       <c r="C27">
         <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
+      <c r="B28" s="27"/>
       <c r="C28">
         <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="26"/>
+      <c r="B29" s="27"/>
       <c r="C29">
         <v>124</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="26"/>
+      <c r="B30" s="27"/>
       <c r="C30">
         <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B32" s="26" t="s">
+      <c r="B32" s="27" t="s">
         <v>507</v>
       </c>
       <c r="C32">
@@ -23003,7 +23067,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="26"/>
+      <c r="B33" s="27"/>
       <c r="C33">
         <v>132</v>
       </c>
@@ -23018,7 +23082,7 @@
       <c r="A34" t="s">
         <v>1001</v>
       </c>
-      <c r="B34" s="26"/>
+      <c r="B34" s="27"/>
       <c r="C34">
         <v>133</v>
       </c>
@@ -23027,7 +23091,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="26"/>
+      <c r="B35" s="27"/>
       <c r="C35">
         <v>134</v>
       </c>
@@ -23039,7 +23103,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="26"/>
+      <c r="B36" s="27"/>
       <c r="C36">
         <v>135</v>
       </c>

</xml_diff>

<commit_message>
v0.7.4f: Added named zombies and swords
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BCFF94-8F93-4874-A9D6-BD7E9685F9F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62EA9BF-2CAB-4EDF-9381-3AF3D85BAFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1669" uniqueCount="1276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="1284">
   <si>
     <t>ID</t>
   </si>
@@ -4326,6 +4326,30 @@
   </si>
   <si>
     <t>Grady Stuckman</t>
+  </si>
+  <si>
+    <t>Ethan Pitney</t>
+  </si>
+  <si>
+    <t>Michael Schmiesing</t>
+  </si>
+  <si>
+    <t>Molly Schmiesing</t>
+  </si>
+  <si>
+    <t>James Sarlo</t>
+  </si>
+  <si>
+    <t>Matt Hair</t>
+  </si>
+  <si>
+    <t>Nicholas Belt</t>
+  </si>
+  <si>
+    <t>cigar, lighter</t>
+  </si>
+  <si>
+    <t>agility=2</t>
   </si>
 </sst>
 </file>
@@ -12812,7 +12836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
@@ -14536,10 +14560,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14550,7 +14574,7 @@
     <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14791,232 +14815,253 @@
       <c r="O8">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="Q8" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>1007</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1035</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>1101</v>
+        <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>1278</v>
       </c>
       <c r="D10" t="s">
-        <v>739</v>
+        <v>1035</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H10">
+        <v>9</v>
+      </c>
+      <c r="I10">
         <v>4</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
       <c r="L10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B11" s="1">
-        <v>1102</v>
-      </c>
-      <c r="C11" t="s">
-        <v>1054</v>
-      </c>
-      <c r="E11" t="s">
-        <v>448</v>
-      </c>
-    </row>
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="C12" t="s">
-        <v>1056</v>
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>739</v>
       </c>
       <c r="E12" t="s">
-        <v>453</v>
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>1054</v>
       </c>
       <c r="E13" t="s">
-        <v>454</v>
+        <v>448</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>3</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1283</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="C14" t="s">
-        <v>737</v>
+        <v>1056</v>
       </c>
       <c r="E14" t="s">
-        <v>738</v>
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="C15" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E15" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <v>1116</v>
+        <v>1105</v>
       </c>
       <c r="C16" t="s">
-        <v>1055</v>
+        <v>737</v>
       </c>
       <c r="E16" t="s">
-        <v>457</v>
+        <v>738</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <v>1117</v>
+        <v>1106</v>
       </c>
       <c r="C17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E17" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="C18" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="E18" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="C19" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="E19" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="C20" t="s">
-        <v>452</v>
+        <v>1057</v>
       </c>
       <c r="E20" t="s">
-        <v>455</v>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>1119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>459</v>
+      </c>
+      <c r="E21" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>1201</v>
+        <v>1120</v>
       </c>
       <c r="C22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
+        <v>452</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-      <c r="J22">
-        <v>0</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0.5</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>1028</v>
-      </c>
-      <c r="R22" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="1">
-        <v>1202</v>
-      </c>
-      <c r="C23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>2</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0.5</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>1028</v>
+        <v>455</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>1203</v>
+        <v>1201</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>11</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24">
         <v>0</v>
@@ -15025,7 +15070,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="Q24" t="s">
         <v>1028</v>
@@ -15036,19 +15081,19 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>1204</v>
+        <v>1202</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="F25">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>0</v>
@@ -15057,30 +15102,27 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="Q25" t="s">
         <v>1028</v>
       </c>
-      <c r="R25" t="s">
-        <v>192</v>
-      </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>1205</v>
+        <v>1203</v>
       </c>
       <c r="C26" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -15089,27 +15131,27 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="Q26" t="s">
         <v>1028</v>
       </c>
       <c r="R26" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C27" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I27">
         <v>3</v>
@@ -15121,24 +15163,27 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="Q27" t="s">
         <v>1028</v>
       </c>
+      <c r="R27" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <v>1207</v>
+        <v>1205</v>
       </c>
       <c r="C28" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H28">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I28">
         <v>3</v>
@@ -15150,27 +15195,27 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="Q28" t="s">
         <v>1028</v>
       </c>
       <c r="R28" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I29">
         <v>3</v>
@@ -15182,27 +15227,24 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="Q29" t="s">
         <v>1028</v>
       </c>
-      <c r="R29" t="s">
-        <v>189</v>
-      </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="C30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I30">
         <v>3</v>
@@ -15219,25 +15261,28 @@
       <c r="Q30" t="s">
         <v>1028</v>
       </c>
+      <c r="R30" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
-        <v>1210</v>
+        <v>1208</v>
       </c>
       <c r="C31" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H31">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I31">
         <v>3</v>
       </c>
       <c r="J31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -15246,57 +15291,162 @@
         <v>1.2</v>
       </c>
       <c r="Q31" t="s">
+        <v>1028</v>
+      </c>
+      <c r="R31" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>1209</v>
+      </c>
+      <c r="C32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32">
+        <v>9</v>
+      </c>
+      <c r="H32">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>1.2</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>1210</v>
+      </c>
+      <c r="C33" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>1.2</v>
+      </c>
+      <c r="Q33" t="s">
         <v>1029</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
         <v>1301</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>1272</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>1271</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
         <v>12</v>
       </c>
-      <c r="F33">
+      <c r="F35">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
         <v>1302</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>1273</v>
       </c>
-      <c r="F34">
+      <c r="F36">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="1">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
         <v>1303</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C37" t="s">
         <v>1274</v>
       </c>
-      <c r="F35">
+      <c r="F37">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="1">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
         <v>1304</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>1275</v>
       </c>
-      <c r="F36">
+      <c r="F38">
         <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>1305</v>
+      </c>
+      <c r="C39" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>1306</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1279</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>1307</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>1308</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.7.4h: Added keys/locks/base items in Francis hall
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE570CEA-811D-420C-A1BC-573BFBB64629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E002D8-26D6-41A9-9854-31E1AB597FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1682" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1322">
   <si>
     <t>ID</t>
   </si>
@@ -3959,48 +3959,24 @@
     <t>zombies</t>
   </si>
   <si>
-    <t>soldiers room</t>
-  </si>
-  <si>
     <t>needed to enter ben's room in tutorial/story</t>
   </si>
   <si>
     <t>wine in desk</t>
   </si>
   <si>
-    <t>on table in soldier RA room</t>
-  </si>
-  <si>
-    <t>Zombie holding it on soldier's wing</t>
-  </si>
-  <si>
     <t>FrancisHall-LOJ door3 (office)</t>
   </si>
   <si>
-    <t>rope in crate</t>
-  </si>
-  <si>
     <t>FrancisHall-LOJ door1 (middle)</t>
   </si>
   <si>
-    <t>boots</t>
-  </si>
-  <si>
     <t>FrancisHall-LOJ door2 (top)</t>
   </si>
   <si>
-    <t>hot pocket box in fridge</t>
-  </si>
-  <si>
-    <t>LOJ common room</t>
-  </si>
-  <si>
     <t>2nd floor TV room</t>
   </si>
   <si>
-    <t>zombie at corpus wing</t>
-  </si>
-  <si>
     <t>2nd floor lobby</t>
   </si>
   <si>
@@ -4013,162 +3989,42 @@
     <t>tutorial by killing rankin</t>
   </si>
   <si>
-    <t>LOJ office room in crate</t>
-  </si>
-  <si>
     <t>soldiers RA room</t>
   </si>
   <si>
-    <t>Unlocked stub wing room</t>
-  </si>
-  <si>
-    <t>Corpus stairway</t>
-  </si>
-  <si>
     <t>Corpus RA room</t>
   </si>
   <si>
-    <t>$50 on bed</t>
-  </si>
-  <si>
-    <t>Lighter and 2 cigars in desk</t>
-  </si>
-  <si>
-    <t>2nd floor garbage, stubwing right door</t>
-  </si>
-  <si>
-    <t>key (14) and key (31)</t>
-  </si>
-  <si>
-    <t>clamp in crate</t>
-  </si>
-  <si>
-    <t>wooden planks</t>
-  </si>
-  <si>
-    <t>candlestick, candle, holy water</t>
-  </si>
-  <si>
-    <t>corpus common room</t>
-  </si>
-  <si>
     <t>chapel</t>
   </si>
   <si>
-    <t>hammer, nails, screws in crate</t>
-  </si>
-  <si>
-    <t>slingshot in crate</t>
-  </si>
-  <si>
-    <t>sneakers</t>
-  </si>
-  <si>
-    <t>canteen, backpack in crates</t>
-  </si>
-  <si>
-    <t>boots, $30 in desk</t>
-  </si>
-  <si>
     <t>window breaker</t>
   </si>
   <si>
-    <t>$70 in servants RA room</t>
-  </si>
-  <si>
     <t>1st floor lobby</t>
   </si>
   <si>
-    <t>1st floor stairwell</t>
-  </si>
-  <si>
-    <t>Disciples common room</t>
-  </si>
-  <si>
     <t>RD room in desk</t>
   </si>
   <si>
-    <t>master key (1), 30 .45 ACP rounds, 6 28-gauge rounds</t>
-  </si>
-  <si>
-    <t>purse in desk, key (24) on table, corpus RA has master key (0) in desk</t>
-  </si>
-  <si>
-    <t>unlocked brothers room</t>
-  </si>
-  <si>
-    <t>1st floor brothers stairway</t>
-  </si>
-  <si>
-    <t>machete in desk, water bottle</t>
-  </si>
-  <si>
-    <t>ground floor lobby</t>
-  </si>
-  <si>
-    <t>ahim door3 (closest to stairway)</t>
-  </si>
-  <si>
-    <t>key (12), key (13), key (21)</t>
-  </si>
-  <si>
-    <t>scissors, $40 in desks</t>
-  </si>
-  <si>
     <t>francis hall kitchen</t>
   </si>
   <si>
     <t>chapel, outside RA office</t>
   </si>
   <si>
-    <t>chapelwing door 2</t>
-  </si>
-  <si>
-    <t>custodial 2nd floor</t>
-  </si>
-  <si>
-    <t>canteen, lighter</t>
-  </si>
-  <si>
     <t>lords day candle</t>
   </si>
   <si>
     <t>RA office</t>
   </si>
   <si>
-    <t>brothers door 3, RA office</t>
-  </si>
-  <si>
-    <t>wrench, bens coat</t>
-  </si>
-  <si>
-    <t>ground floor main stairway</t>
-  </si>
-  <si>
-    <t>ground floor guest bathroom</t>
-  </si>
-  <si>
-    <t>master key (2), keys (36, 32), window breaker, backpack</t>
-  </si>
-  <si>
     <t>2nd floor mechanical</t>
   </si>
   <si>
-    <t>zombie in 2nd floor lobby</t>
-  </si>
-  <si>
-    <t>zombie in 1st floor bathroom</t>
-  </si>
-  <si>
-    <t>unlocked soldiers room</t>
-  </si>
-  <si>
     <t>1st floor custodial</t>
   </si>
   <si>
-    <t>wrench in crate</t>
-  </si>
-  <si>
     <t>ben's backpack</t>
   </si>
   <si>
@@ -4353,6 +4209,261 @@
   </si>
   <si>
     <t>Board with Nails</t>
+  </si>
+  <si>
+    <t>chapel ra room</t>
+  </si>
+  <si>
+    <t>crate in common room</t>
+  </si>
+  <si>
+    <t>soldiers room, a couple other locked rooms</t>
+  </si>
+  <si>
+    <t>craftable</t>
+  </si>
+  <si>
+    <t>G floor storage</t>
+  </si>
+  <si>
+    <t>couple locked rooms</t>
+  </si>
+  <si>
+    <t>few in francis hall</t>
+  </si>
+  <si>
+    <t>several</t>
+  </si>
+  <si>
+    <t>couple in locked rooms</t>
+  </si>
+  <si>
+    <t>grady stuckman room</t>
+  </si>
+  <si>
+    <t>servants locked room</t>
+  </si>
+  <si>
+    <t>ahim locked room</t>
+  </si>
+  <si>
+    <t>burn things</t>
+  </si>
+  <si>
+    <t>few in random places</t>
+  </si>
+  <si>
+    <t>see key-lock</t>
+  </si>
+  <si>
+    <t>few in locked rooms</t>
+  </si>
+  <si>
+    <t>1 in G floor custodial</t>
+  </si>
+  <si>
+    <t>several in random places</t>
+  </si>
+  <si>
+    <t>RD room</t>
+  </si>
+  <si>
+    <t>several random places</t>
+  </si>
+  <si>
+    <t>zombie in g floor lobby</t>
+  </si>
+  <si>
+    <t>RD room, g floor mechanical</t>
+  </si>
+  <si>
+    <t>g floor mechanical</t>
+  </si>
+  <si>
+    <t>master key (2), keys (36, 32), backpack</t>
+  </si>
+  <si>
+    <t>bens coat, wooden handle, iron handle</t>
+  </si>
+  <si>
+    <t>ahim common room</t>
+  </si>
+  <si>
+    <t>1st floor storage</t>
+  </si>
+  <si>
+    <t>other half of ground floor</t>
+  </si>
+  <si>
+    <t>candlestick, holy water</t>
+  </si>
+  <si>
+    <t>M1911, ammo</t>
+  </si>
+  <si>
+    <t>sneakers, Grady</t>
+  </si>
+  <si>
+    <t>steel toed boots</t>
+  </si>
+  <si>
+    <t>cowboy boots, $40</t>
+  </si>
+  <si>
+    <t>2nd floor study room</t>
+  </si>
+  <si>
+    <t>golden apple</t>
+  </si>
+  <si>
+    <t>$50 bill, cheese</t>
+  </si>
+  <si>
+    <t>suit jacket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wooden horse, boots (chapel), </t>
+  </si>
+  <si>
+    <t>various, cut fence</t>
+  </si>
+  <si>
+    <t>stapler, scissors, document</t>
+  </si>
+  <si>
+    <t>woodglue</t>
+  </si>
+  <si>
+    <t>key (14), key (31)</t>
+  </si>
+  <si>
+    <t>key (34)</t>
+  </si>
+  <si>
+    <t>purse, rose (soldiers), master key 0 (corpus)</t>
+  </si>
+  <si>
+    <t>key (24)</t>
+  </si>
+  <si>
+    <t>chapelwing locked room</t>
+  </si>
+  <si>
+    <t>servants common room</t>
+  </si>
+  <si>
+    <t>wire clippers</t>
+  </si>
+  <si>
+    <t>brothers locked door</t>
+  </si>
+  <si>
+    <t>ahim locked door</t>
+  </si>
+  <si>
+    <t>key (38)</t>
+  </si>
+  <si>
+    <t>brothers locked room</t>
+  </si>
+  <si>
+    <t>key (6), key (18)</t>
+  </si>
+  <si>
+    <t>soldiers ra room</t>
+  </si>
+  <si>
+    <t>trees</t>
+  </si>
+  <si>
+    <t>soldiers covenant</t>
+  </si>
+  <si>
+    <t>wrench, screws, metal handle</t>
+  </si>
+  <si>
+    <t>hammer, nails</t>
+  </si>
+  <si>
+    <t>2nd floor custodial</t>
+  </si>
+  <si>
+    <t>suit jacket, ax</t>
+  </si>
+  <si>
+    <t>chapel lokced door</t>
+  </si>
+  <si>
+    <t>g floor custodial</t>
+  </si>
+  <si>
+    <t>chainsaw</t>
+  </si>
+  <si>
+    <t>g floor custodial storage</t>
+  </si>
+  <si>
+    <t>soldiers hallway</t>
+  </si>
+  <si>
+    <t>2nd floor bathroom</t>
+  </si>
+  <si>
+    <t>corpus stairway</t>
+  </si>
+  <si>
+    <t>2nd floor main stairway</t>
+  </si>
+  <si>
+    <t>1st floor bathroom</t>
+  </si>
+  <si>
+    <t>servants room</t>
+  </si>
+  <si>
+    <t>stub room</t>
+  </si>
+  <si>
+    <t>brothers room</t>
+  </si>
+  <si>
+    <t>1st floor laundry</t>
+  </si>
+  <si>
+    <t>disciples hallway</t>
+  </si>
+  <si>
+    <t>ahim room</t>
+  </si>
+  <si>
+    <t>g floor laundry</t>
+  </si>
+  <si>
+    <t>main foyer</t>
+  </si>
+  <si>
+    <t>g floor lobby</t>
+  </si>
+  <si>
+    <t>g floor behind stairwell</t>
+  </si>
+  <si>
+    <t>g floor bathroom</t>
+  </si>
+  <si>
+    <t>g floor guest bathroom</t>
+  </si>
+  <si>
+    <t>.45 ACP, 28 gauge, key (39)</t>
+  </si>
+  <si>
+    <t>Small Key Ring</t>
+  </si>
+  <si>
+    <t>Large Key Ring</t>
+  </si>
+  <si>
+    <t>Holds keys (in description)</t>
   </si>
 </sst>
 </file>
@@ -12211,7 +12322,7 @@
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B52" s="29" t="s">
-        <v>1236</v>
+        <v>1188</v>
       </c>
       <c r="C52" t="s">
         <v>1138</v>
@@ -12268,10 +12379,10 @@
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B55" s="29"/>
       <c r="C55" t="s">
-        <v>1232</v>
+        <v>1184</v>
       </c>
       <c r="D55" t="s">
-        <v>1234</v>
+        <v>1186</v>
       </c>
       <c r="E55">
         <v>85</v>
@@ -12280,16 +12391,16 @@
         <v>1139</v>
       </c>
       <c r="G55" s="9" t="s">
-        <v>1237</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B56" s="29"/>
       <c r="C56" t="s">
-        <v>1233</v>
+        <v>1185</v>
       </c>
       <c r="D56" t="s">
-        <v>1235</v>
+        <v>1187</v>
       </c>
       <c r="E56">
         <v>85</v>
@@ -12298,7 +12409,7 @@
         <v>1140</v>
       </c>
       <c r="G56" s="9" t="s">
-        <v>1238</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -13585,13 +13696,13 @@
         <v>180</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>1239</v>
+        <v>1191</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="G62" t="s">
-        <v>1240</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -13672,19 +13783,19 @@
         <v>186</v>
       </c>
       <c r="C68" s="15" t="s">
-        <v>1243</v>
+        <v>1195</v>
       </c>
       <c r="D68" t="s">
-        <v>1248</v>
+        <v>1200</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="G68" t="s">
-        <v>1241</v>
+        <v>1193</v>
       </c>
       <c r="H68" t="s">
-        <v>1244</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
@@ -13692,16 +13803,16 @@
         <v>187</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>1242</v>
+        <v>1194</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="G69" t="s">
-        <v>1247</v>
+        <v>1199</v>
       </c>
       <c r="H69" t="s">
-        <v>1244</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
@@ -13712,7 +13823,7 @@
         <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>1245</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
@@ -13723,7 +13834,7 @@
         <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>1246</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -13789,7 +13900,7 @@
         <v>195</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>1249</v>
+        <v>1201</v>
       </c>
       <c r="D77" t="s">
         <v>732</v>
@@ -14819,7 +14930,7 @@
         <v>0.05</v>
       </c>
       <c r="Q8" t="s">
-        <v>1282</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -14827,7 +14938,7 @@
         <v>1007</v>
       </c>
       <c r="C9" t="s">
-        <v>1277</v>
+        <v>1229</v>
       </c>
       <c r="D9" t="s">
         <v>1035</v>
@@ -14856,7 +14967,7 @@
         <v>1008</v>
       </c>
       <c r="C10" t="s">
-        <v>1278</v>
+        <v>1230</v>
       </c>
       <c r="D10" t="s">
         <v>1035</v>
@@ -14942,7 +15053,7 @@
         <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>1283</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -15363,10 +15474,10 @@
         <v>1301</v>
       </c>
       <c r="C35" t="s">
-        <v>1272</v>
+        <v>1224</v>
       </c>
       <c r="D35" t="s">
-        <v>1271</v>
+        <v>1223</v>
       </c>
       <c r="E35" t="s">
         <v>12</v>
@@ -15380,7 +15491,7 @@
         <v>1302</v>
       </c>
       <c r="C36" t="s">
-        <v>1273</v>
+        <v>1225</v>
       </c>
       <c r="F36">
         <v>2</v>
@@ -15391,7 +15502,7 @@
         <v>1303</v>
       </c>
       <c r="C37" t="s">
-        <v>1274</v>
+        <v>1226</v>
       </c>
       <c r="F37">
         <v>3</v>
@@ -15402,7 +15513,7 @@
         <v>1304</v>
       </c>
       <c r="C38" t="s">
-        <v>1275</v>
+        <v>1227</v>
       </c>
       <c r="F38">
         <v>4</v>
@@ -15413,7 +15524,7 @@
         <v>1305</v>
       </c>
       <c r="C39" t="s">
-        <v>1276</v>
+        <v>1228</v>
       </c>
       <c r="F39">
         <v>5</v>
@@ -15424,7 +15535,7 @@
         <v>1306</v>
       </c>
       <c r="C40" t="s">
-        <v>1279</v>
+        <v>1231</v>
       </c>
       <c r="F40">
         <v>6</v>
@@ -15435,7 +15546,7 @@
         <v>1307</v>
       </c>
       <c r="C41" t="s">
-        <v>1280</v>
+        <v>1232</v>
       </c>
       <c r="F41">
         <v>7</v>
@@ -15446,7 +15557,7 @@
         <v>1308</v>
       </c>
       <c r="C42" t="s">
-        <v>1281</v>
+        <v>1233</v>
       </c>
       <c r="F42">
         <v>8</v>
@@ -15944,13 +16055,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y281"/>
+  <dimension ref="A1:Y283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="R210" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P62" sqref="P62"/>
+      <selection pane="bottomRight" activeCell="W226" sqref="W226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16533,7 +16644,7 @@
         <v>20</v>
       </c>
       <c r="Y31" t="s">
-        <v>1153</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="32" spans="2:25" x14ac:dyDescent="0.25">
@@ -16570,7 +16681,7 @@
         <v>50</v>
       </c>
       <c r="Y33" t="s">
-        <v>1206</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="34" spans="2:25" x14ac:dyDescent="0.25">
@@ -16592,6 +16703,9 @@
       <c r="I34">
         <v>10</v>
       </c>
+      <c r="Y34" t="s">
+        <v>1270</v>
+      </c>
     </row>
     <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B35">
@@ -16649,7 +16763,7 @@
         <v>50</v>
       </c>
       <c r="Y38" t="s">
-        <v>1148</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="39" spans="2:25" x14ac:dyDescent="0.25">
@@ -16733,7 +16847,7 @@
         <v>1094</v>
       </c>
       <c r="Y44" t="s">
-        <v>1169</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="45" spans="2:25" x14ac:dyDescent="0.25">
@@ -16744,7 +16858,7 @@
         <v>1090</v>
       </c>
       <c r="Y45" t="s">
-        <v>1184</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="46" spans="2:25" x14ac:dyDescent="0.25">
@@ -16755,7 +16869,7 @@
         <v>1091</v>
       </c>
       <c r="Y46" t="s">
-        <v>1168</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="47" spans="2:25" x14ac:dyDescent="0.25">
@@ -16768,6 +16882,9 @@
       <c r="E47">
         <v>2</v>
       </c>
+      <c r="Y47" t="s">
+        <v>1262</v>
+      </c>
     </row>
     <row r="48" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B48">
@@ -16779,16 +16896,22 @@
       <c r="E48">
         <v>2</v>
       </c>
+      <c r="Y48" t="s">
+        <v>1238</v>
+      </c>
     </row>
     <row r="49" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>2166</v>
       </c>
       <c r="C49" t="s">
-        <v>1226</v>
+        <v>1178</v>
       </c>
       <c r="E49">
         <v>3</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>1237</v>
       </c>
     </row>
     <row r="51" spans="2:25" x14ac:dyDescent="0.25">
@@ -16825,7 +16948,7 @@
         <v>0.02</v>
       </c>
       <c r="Y52" t="s">
-        <v>1205</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="53" spans="2:25" x14ac:dyDescent="0.25">
@@ -16865,7 +16988,7 @@
         <v>6</v>
       </c>
       <c r="Y54" t="s">
-        <v>1218</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="55" spans="2:25" x14ac:dyDescent="0.25">
@@ -16873,7 +16996,7 @@
         <v>2205</v>
       </c>
       <c r="C55" t="s">
-        <v>1227</v>
+        <v>1179</v>
       </c>
       <c r="L55" s="4">
         <v>2.5</v>
@@ -16883,6 +17006,9 @@
       </c>
       <c r="Q55">
         <v>1</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="56" spans="2:25" x14ac:dyDescent="0.25">
@@ -16890,7 +17016,7 @@
         <v>2206</v>
       </c>
       <c r="C56" t="s">
-        <v>1228</v>
+        <v>1180</v>
       </c>
       <c r="L56" s="4">
         <v>2</v>
@@ -16900,6 +17026,9 @@
       </c>
       <c r="Q56">
         <v>0</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="57" spans="2:25" x14ac:dyDescent="0.25">
@@ -16907,7 +17036,7 @@
         <v>2207</v>
       </c>
       <c r="C57" t="s">
-        <v>1229</v>
+        <v>1181</v>
       </c>
       <c r="L57" s="4">
         <v>2</v>
@@ -16917,6 +17046,9 @@
       </c>
       <c r="Q57">
         <v>4</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="58" spans="2:25" x14ac:dyDescent="0.25">
@@ -16924,7 +17056,7 @@
         <v>2208</v>
       </c>
       <c r="C58" t="s">
-        <v>1230</v>
+        <v>1182</v>
       </c>
       <c r="L58" s="4">
         <v>1.7</v>
@@ -16934,6 +17066,9 @@
       </c>
       <c r="Q58">
         <v>3</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="59" spans="2:25" x14ac:dyDescent="0.25">
@@ -16956,7 +17091,7 @@
         <v>8</v>
       </c>
       <c r="Y59" t="s">
-        <v>1217</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="60" spans="2:25" x14ac:dyDescent="0.25">
@@ -16964,7 +17099,7 @@
         <v>2212</v>
       </c>
       <c r="C60" t="s">
-        <v>1250</v>
+        <v>1202</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -16984,7 +17119,7 @@
         <v>2213</v>
       </c>
       <c r="C61" t="s">
-        <v>1251</v>
+        <v>1203</v>
       </c>
       <c r="E61">
         <v>2</v>
@@ -17004,7 +17139,7 @@
         <v>2214</v>
       </c>
       <c r="C62" t="s">
-        <v>1284</v>
+        <v>1236</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -17027,7 +17162,7 @@
         <v>2221</v>
       </c>
       <c r="C63" t="s">
-        <v>1252</v>
+        <v>1204</v>
       </c>
       <c r="E63">
         <v>3</v>
@@ -17047,7 +17182,7 @@
         <v>2222</v>
       </c>
       <c r="C64" t="s">
-        <v>1253</v>
+        <v>1205</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -17067,7 +17202,7 @@
         <v>2231</v>
       </c>
       <c r="C65" t="s">
-        <v>1254</v>
+        <v>1206</v>
       </c>
       <c r="E65">
         <v>4</v>
@@ -17087,7 +17222,7 @@
         <v>2232</v>
       </c>
       <c r="C66" t="s">
-        <v>1255</v>
+        <v>1207</v>
       </c>
       <c r="E66">
         <v>4</v>
@@ -17107,7 +17242,7 @@
         <v>2241</v>
       </c>
       <c r="C67" t="s">
-        <v>1256</v>
+        <v>1208</v>
       </c>
       <c r="E67">
         <v>5</v>
@@ -17127,7 +17262,7 @@
         <v>2242</v>
       </c>
       <c r="C68" t="s">
-        <v>1257</v>
+        <v>1209</v>
       </c>
       <c r="E68">
         <v>5</v>
@@ -17147,7 +17282,7 @@
         <v>2251</v>
       </c>
       <c r="C69" t="s">
-        <v>1258</v>
+        <v>1210</v>
       </c>
       <c r="E69">
         <v>6</v>
@@ -17167,7 +17302,7 @@
         <v>2252</v>
       </c>
       <c r="C70" t="s">
-        <v>1259</v>
+        <v>1211</v>
       </c>
       <c r="E70">
         <v>6</v>
@@ -17187,7 +17322,7 @@
         <v>2261</v>
       </c>
       <c r="C71" t="s">
-        <v>1260</v>
+        <v>1212</v>
       </c>
       <c r="E71">
         <v>7</v>
@@ -17207,7 +17342,7 @@
         <v>2262</v>
       </c>
       <c r="C72" t="s">
-        <v>1261</v>
+        <v>1213</v>
       </c>
       <c r="E72">
         <v>7</v>
@@ -17227,7 +17362,7 @@
         <v>2271</v>
       </c>
       <c r="C73" t="s">
-        <v>1265</v>
+        <v>1217</v>
       </c>
       <c r="E73">
         <v>8</v>
@@ -17247,7 +17382,7 @@
         <v>2272</v>
       </c>
       <c r="C74" t="s">
-        <v>1266</v>
+        <v>1218</v>
       </c>
       <c r="E74">
         <v>8</v>
@@ -17267,7 +17402,7 @@
         <v>2281</v>
       </c>
       <c r="C75" t="s">
-        <v>1267</v>
+        <v>1219</v>
       </c>
       <c r="E75">
         <v>9</v>
@@ -17287,7 +17422,7 @@
         <v>2282</v>
       </c>
       <c r="C76" t="s">
-        <v>1268</v>
+        <v>1220</v>
       </c>
       <c r="E76">
         <v>9</v>
@@ -17307,7 +17442,7 @@
         <v>2291</v>
       </c>
       <c r="C77" t="s">
-        <v>1269</v>
+        <v>1221</v>
       </c>
       <c r="E77">
         <v>10</v>
@@ -17327,7 +17462,7 @@
         <v>2292</v>
       </c>
       <c r="C78" t="s">
-        <v>1270</v>
+        <v>1222</v>
       </c>
       <c r="E78">
         <v>10</v>
@@ -17368,7 +17503,7 @@
         <v>1148</v>
       </c>
     </row>
-    <row r="81" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B81">
         <v>2311</v>
       </c>
@@ -17395,7 +17530,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="82" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B82">
         <v>2312</v>
       </c>
@@ -17421,8 +17556,11 @@
       <c r="W82" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="83" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="Y82" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="83" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B83">
         <v>2321</v>
       </c>
@@ -17449,7 +17587,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="84" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B84">
         <v>2322</v>
       </c>
@@ -17476,7 +17614,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="85" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B85">
         <v>2323</v>
       </c>
@@ -17503,7 +17641,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="86" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B86">
         <v>2331</v>
       </c>
@@ -17527,11 +17665,11 @@
       <c r="V86">
         <v>6</v>
       </c>
-      <c r="X86" t="s">
+      <c r="W86" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="87" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B87">
         <v>2332</v>
       </c>
@@ -17558,7 +17696,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="88" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B88">
         <v>2333</v>
       </c>
@@ -17585,7 +17723,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="89" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B89">
         <v>2341</v>
       </c>
@@ -17615,7 +17753,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="90" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B90">
         <v>2342</v>
       </c>
@@ -17642,7 +17780,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="91" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B91">
         <v>2343</v>
       </c>
@@ -17669,7 +17807,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="92" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B92">
         <v>2344</v>
       </c>
@@ -17696,7 +17834,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="93" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B93">
         <v>2345</v>
       </c>
@@ -17723,7 +17861,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="94" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B94">
         <v>2351</v>
       </c>
@@ -17750,7 +17888,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="95" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B95">
         <v>2352</v>
       </c>
@@ -17777,7 +17915,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="96" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B96">
         <v>2353</v>
       </c>
@@ -18243,6 +18381,9 @@
       <c r="O113">
         <v>1</v>
       </c>
+      <c r="Y113" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="114" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B114">
@@ -18283,7 +18424,7 @@
         <v>-0.5</v>
       </c>
       <c r="Y116" t="s">
-        <v>1205</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="117" spans="2:25" x14ac:dyDescent="0.25">
@@ -18299,6 +18440,9 @@
       <c r="O117">
         <v>2</v>
       </c>
+      <c r="Y117" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="118" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B118">
@@ -18425,6 +18569,9 @@
       <c r="O127">
         <v>1</v>
       </c>
+      <c r="Y127" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="128" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B128">
@@ -18450,6 +18597,9 @@
       <c r="N129">
         <v>0.02</v>
       </c>
+      <c r="Y129" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="130" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B130">
@@ -18464,6 +18614,9 @@
       <c r="O130">
         <v>1</v>
       </c>
+      <c r="Y130" t="s">
+        <v>1243</v>
+      </c>
     </row>
     <row r="131" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B131">
@@ -18478,6 +18631,9 @@
       <c r="O131">
         <v>2</v>
       </c>
+      <c r="Y131" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="132" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B132">
@@ -18498,6 +18654,9 @@
       <c r="O132">
         <v>2</v>
       </c>
+      <c r="Y132" t="s">
+        <v>1241</v>
+      </c>
     </row>
     <row r="133" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B133">
@@ -18509,6 +18668,9 @@
       <c r="N133">
         <v>0.04</v>
       </c>
+      <c r="Y133" t="s">
+        <v>1242</v>
+      </c>
     </row>
     <row r="134" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B134">
@@ -18635,6 +18797,9 @@
       <c r="O143">
         <v>1</v>
       </c>
+      <c r="Y143" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="144" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B144">
@@ -18694,6 +18859,9 @@
       <c r="O147">
         <v>2</v>
       </c>
+      <c r="Y147" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="148" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B148">
@@ -18820,6 +18988,9 @@
       <c r="O157">
         <v>1</v>
       </c>
+      <c r="Y157" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="158" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B158">
@@ -18859,8 +19030,11 @@
       <c r="S160">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="161" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y160" t="s">
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="161" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B161">
         <v>2705</v>
       </c>
@@ -18873,8 +19047,11 @@
       <c r="S161">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="162" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y161" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="162" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B162">
         <v>2711</v>
       </c>
@@ -18887,8 +19064,11 @@
       <c r="O162">
         <v>2</v>
       </c>
-    </row>
-    <row r="163" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y162" t="s">
+        <v>1240</v>
+      </c>
+    </row>
+    <row r="163" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B163">
         <v>2712</v>
       </c>
@@ -18904,8 +19084,11 @@
       <c r="S163">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="164" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y163" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="164" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B164">
         <v>2713</v>
       </c>
@@ -18924,8 +19107,11 @@
       <c r="S164">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="165" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y164" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="165" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B165">
         <v>2714</v>
       </c>
@@ -18941,8 +19127,11 @@
       <c r="S165">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="166" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Y165" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="166" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B166">
         <v>2721</v>
       </c>
@@ -18956,7 +19145,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="167" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B167">
         <v>2731</v>
       </c>
@@ -18970,7 +19159,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="168" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B168">
         <v>2741</v>
       </c>
@@ -18984,7 +19173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="169" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B169">
         <v>2751</v>
       </c>
@@ -18998,7 +19187,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="170" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B170">
         <v>2761</v>
       </c>
@@ -19012,7 +19201,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="171" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B171">
         <v>2771</v>
       </c>
@@ -19026,7 +19215,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="172" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B172">
         <v>2781</v>
       </c>
@@ -19040,7 +19229,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="173" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B173">
         <v>2791</v>
       </c>
@@ -19054,7 +19243,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="175" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B175">
         <v>2801</v>
       </c>
@@ -19065,7 +19254,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="176" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B176">
         <v>2802</v>
       </c>
@@ -19107,6 +19296,9 @@
       <c r="C180" t="s">
         <v>298</v>
       </c>
+      <c r="Y180" t="s">
+        <v>1275</v>
+      </c>
     </row>
     <row r="181" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B181">
@@ -19115,6 +19307,9 @@
       <c r="C181" t="s">
         <v>1016</v>
       </c>
+      <c r="Y181" t="s">
+        <v>1151</v>
+      </c>
     </row>
     <row r="182" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B182">
@@ -19123,6 +19318,9 @@
       <c r="C182" t="s">
         <v>1085</v>
       </c>
+      <c r="Y182" t="s">
+        <v>1249</v>
+      </c>
     </row>
     <row r="183" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B183">
@@ -19131,6 +19329,9 @@
       <c r="C183" t="s">
         <v>1087</v>
       </c>
+      <c r="Y183" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="184" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B184">
@@ -19140,7 +19341,7 @@
         <v>1088</v>
       </c>
       <c r="Y184" t="s">
-        <v>1183</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="185" spans="2:25" x14ac:dyDescent="0.25">
@@ -19208,7 +19409,7 @@
         <v>2817</v>
       </c>
       <c r="C191" t="s">
-        <v>1225</v>
+        <v>1177</v>
       </c>
       <c r="L191" s="4">
         <v>2.8</v>
@@ -19222,7 +19423,7 @@
         <v>2818</v>
       </c>
       <c r="C192" t="s">
-        <v>1231</v>
+        <v>1183</v>
       </c>
       <c r="L192" s="4">
         <v>0.5</v>
@@ -19301,7 +19502,7 @@
         <v>2833</v>
       </c>
       <c r="C200" t="s">
-        <v>1262</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="201" spans="2:25" x14ac:dyDescent="0.25">
@@ -19309,7 +19510,7 @@
         <v>2834</v>
       </c>
       <c r="C201" t="s">
-        <v>1263</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="202" spans="2:25" x14ac:dyDescent="0.25">
@@ -19336,7 +19537,7 @@
         <v>2843</v>
       </c>
       <c r="C204" t="s">
-        <v>1264</v>
+        <v>1216</v>
       </c>
       <c r="L204" s="4">
         <v>12</v>
@@ -19494,7 +19695,7 @@
         <v>254</v>
       </c>
       <c r="Y221" t="s">
-        <v>1148</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="222" spans="2:25" x14ac:dyDescent="0.25">
@@ -19511,7 +19712,7 @@
         <v>255</v>
       </c>
       <c r="Y222" t="s">
-        <v>1148</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="223" spans="2:25" x14ac:dyDescent="0.25">
@@ -19528,47 +19729,50 @@
         <v>256</v>
       </c>
       <c r="Y223" t="s">
-        <v>1148</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="224" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2911</v>
+        <v>2904</v>
       </c>
       <c r="C224" t="s">
-        <v>258</v>
-      </c>
-      <c r="D224" t="s">
-        <v>257</v>
-      </c>
-      <c r="H224" s="6"/>
-      <c r="L224" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y224" t="s">
-        <v>1148</v>
+        <v>1319</v>
+      </c>
+      <c r="U224">
+        <v>8</v>
+      </c>
+      <c r="W224" t="s">
+        <v>1321</v>
       </c>
     </row>
     <row r="225" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2912</v>
+        <v>2905</v>
       </c>
       <c r="C225" t="s">
-        <v>259</v>
-      </c>
-      <c r="L225" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y225" t="s">
-        <v>1148</v>
+        <v>1320</v>
+      </c>
+      <c r="U225">
+        <v>24</v>
+      </c>
+      <c r="W225" t="s">
+        <v>1321</v>
       </c>
     </row>
     <row r="226" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2913</v>
+        <v>2911</v>
       </c>
       <c r="C226" t="s">
-        <v>260</v>
+        <v>258</v>
+      </c>
+      <c r="D226" t="s">
+        <v>257</v>
+      </c>
+      <c r="H226" s="6"/>
+      <c r="L226" s="4">
+        <v>1</v>
       </c>
       <c r="Y226" t="s">
         <v>1148</v>
@@ -19576,10 +19780,13 @@
     </row>
     <row r="227" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2914</v>
+        <v>2912</v>
       </c>
       <c r="C227" t="s">
-        <v>261</v>
+        <v>259</v>
+      </c>
+      <c r="L227" s="4">
+        <v>1</v>
       </c>
       <c r="Y227" t="s">
         <v>1148</v>
@@ -19587,13 +19794,10 @@
     </row>
     <row r="228" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2915</v>
+        <v>2913</v>
       </c>
       <c r="C228" t="s">
-        <v>262</v>
-      </c>
-      <c r="L228" s="4">
-        <v>1</v>
+        <v>260</v>
       </c>
       <c r="Y228" t="s">
         <v>1148</v>
@@ -19601,225 +19805,231 @@
     </row>
     <row r="229" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2916</v>
+        <v>2914</v>
       </c>
       <c r="C229" t="s">
-        <v>288</v>
+        <v>261</v>
       </c>
       <c r="Y229" t="s">
-        <v>1148</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="230" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2917</v>
+        <v>2915</v>
       </c>
       <c r="C230" t="s">
-        <v>740</v>
+        <v>262</v>
+      </c>
+      <c r="L230" s="4">
+        <v>1</v>
       </c>
       <c r="Y230" t="s">
-        <v>1148</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="231" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2918</v>
+        <v>2916</v>
       </c>
       <c r="C231" t="s">
-        <v>1069</v>
-      </c>
-      <c r="L231" s="4">
-        <v>1.5</v>
+        <v>288</v>
+      </c>
+      <c r="Y231" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="232" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B232">
-        <v>2921</v>
+        <v>2917</v>
       </c>
       <c r="C232" t="s">
-        <v>264</v>
-      </c>
-      <c r="D232" t="s">
-        <v>263</v>
-      </c>
-      <c r="N232">
-        <v>0.04</v>
-      </c>
-      <c r="W232" t="s">
-        <v>268</v>
+        <v>740</v>
+      </c>
+      <c r="Y232" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="233" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B233">
-        <v>2922</v>
+        <v>2918</v>
       </c>
       <c r="C233" t="s">
-        <v>265</v>
-      </c>
-      <c r="N233">
-        <v>0.04</v>
-      </c>
-      <c r="W233" t="s">
-        <v>269</v>
+        <v>1069</v>
+      </c>
+      <c r="L233" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="Y233" t="s">
+        <v>1252</v>
       </c>
     </row>
     <row r="234" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B234">
-        <v>2923</v>
+        <v>2921</v>
       </c>
       <c r="C234" t="s">
-        <v>266</v>
+        <v>264</v>
+      </c>
+      <c r="D234" t="s">
+        <v>263</v>
       </c>
       <c r="N234">
         <v>0.04</v>
       </c>
       <c r="W234" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Y234" t="s">
-        <v>1172</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="235" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B235">
-        <v>2924</v>
+        <v>2922</v>
       </c>
       <c r="C235" t="s">
-        <v>289</v>
-      </c>
-      <c r="L235" s="4">
-        <v>1</v>
+        <v>265</v>
       </c>
       <c r="N235">
-        <v>2.5</v>
-      </c>
-      <c r="Q235">
-        <v>6</v>
+        <v>0.04</v>
       </c>
       <c r="W235" t="s">
-        <v>296</v>
+        <v>269</v>
       </c>
       <c r="Y235" t="s">
-        <v>1148</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="236" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B236">
-        <v>2925</v>
+        <v>2923</v>
       </c>
       <c r="C236" t="s">
-        <v>290</v>
+        <v>266</v>
+      </c>
+      <c r="N236">
+        <v>0.04</v>
       </c>
       <c r="W236" t="s">
-        <v>293</v>
+        <v>267</v>
+      </c>
+      <c r="Y236" t="s">
+        <v>1163</v>
       </c>
     </row>
     <row r="237" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B237">
-        <v>2926</v>
+        <v>2924</v>
       </c>
       <c r="C237" t="s">
-        <v>291</v>
-      </c>
-      <c r="E237">
-        <v>2</v>
+        <v>289</v>
       </c>
       <c r="L237" s="4">
         <v>1</v>
       </c>
       <c r="N237">
-        <v>0.02</v>
+        <v>2.5</v>
+      </c>
+      <c r="Q237">
+        <v>6</v>
       </c>
       <c r="W237" t="s">
-        <v>294</v>
+        <v>296</v>
+      </c>
+      <c r="Y237" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="238" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B238">
-        <v>2927</v>
+        <v>2925</v>
       </c>
       <c r="C238" t="s">
-        <v>292</v>
-      </c>
-      <c r="E238">
-        <v>3</v>
-      </c>
-      <c r="L238" s="4">
-        <v>2</v>
-      </c>
-      <c r="N238">
-        <v>0.02</v>
+        <v>290</v>
       </c>
       <c r="W238" t="s">
-        <v>295</v>
+        <v>293</v>
+      </c>
+      <c r="Y238" t="s">
+        <v>1250</v>
       </c>
     </row>
     <row r="239" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B239">
-        <v>2928</v>
+        <v>2926</v>
       </c>
       <c r="C239" t="s">
-        <v>1058</v>
+        <v>291</v>
+      </c>
+      <c r="E239">
+        <v>2</v>
+      </c>
+      <c r="L239" s="4">
+        <v>1</v>
+      </c>
+      <c r="N239">
+        <v>0.02</v>
       </c>
       <c r="W239" t="s">
-        <v>1061</v>
+        <v>294</v>
       </c>
       <c r="Y239" t="s">
-        <v>1178</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="240" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B240">
-        <v>2931</v>
+        <v>2927</v>
       </c>
       <c r="C240" t="s">
-        <v>238</v>
-      </c>
-      <c r="D240" t="s">
-        <v>277</v>
+        <v>292</v>
+      </c>
+      <c r="E240">
+        <v>3</v>
       </c>
       <c r="L240" s="4">
         <v>2</v>
       </c>
       <c r="N240">
-        <v>2.5</v>
+        <v>0.02</v>
       </c>
       <c r="W240" t="s">
-        <v>813</v>
+        <v>295</v>
       </c>
       <c r="Y240" t="s">
-        <v>1148</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="241" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B241">
-        <v>2932</v>
+        <v>2928</v>
       </c>
       <c r="C241" t="s">
-        <v>278</v>
-      </c>
-      <c r="L241" s="4">
-        <v>1</v>
-      </c>
-      <c r="N241">
-        <v>2</v>
-      </c>
-      <c r="Q241">
-        <v>4</v>
+        <v>1058</v>
+      </c>
+      <c r="W241" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Y241" t="s">
+        <v>1254</v>
       </c>
     </row>
     <row r="242" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B242">
-        <v>2933</v>
+        <v>2931</v>
       </c>
       <c r="C242" t="s">
-        <v>281</v>
+        <v>238</v>
+      </c>
+      <c r="D242" t="s">
+        <v>277</v>
       </c>
       <c r="L242" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N242">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="W242" t="s">
         <v>813</v>
@@ -19830,57 +20040,69 @@
     </row>
     <row r="243" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B243">
-        <v>2941</v>
+        <v>2932</v>
       </c>
       <c r="C243" t="s">
-        <v>373</v>
+        <v>278</v>
+      </c>
+      <c r="L243" s="4">
+        <v>1</v>
+      </c>
+      <c r="N243">
+        <v>2</v>
+      </c>
+      <c r="Q243">
+        <v>4</v>
       </c>
     </row>
     <row r="244" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B244">
-        <v>2942</v>
+        <v>2933</v>
       </c>
       <c r="C244" t="s">
-        <v>374</v>
-      </c>
-      <c r="E244">
+        <v>281</v>
+      </c>
+      <c r="L244" s="4">
+        <v>1</v>
+      </c>
+      <c r="N244">
         <v>2</v>
+      </c>
+      <c r="W244" t="s">
+        <v>813</v>
+      </c>
+      <c r="Y244" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="245" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B245">
-        <v>2943</v>
+        <v>2941</v>
       </c>
       <c r="C245" t="s">
-        <v>375</v>
-      </c>
-      <c r="E245">
-        <v>2</v>
+        <v>373</v>
+      </c>
+      <c r="Y245" t="s">
+        <v>1258</v>
       </c>
     </row>
     <row r="246" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B246">
-        <v>2944</v>
+        <v>2942</v>
       </c>
       <c r="C246" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="E246">
         <v>2</v>
       </c>
-      <c r="L246" s="4">
-        <v>3</v>
-      </c>
-      <c r="N246">
-        <v>3.5</v>
-      </c>
     </row>
     <row r="247" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B247">
-        <v>2945</v>
+        <v>2943</v>
       </c>
       <c r="C247" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E247">
         <v>2</v>
@@ -19888,21 +20110,27 @@
     </row>
     <row r="248" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B248">
-        <v>2946</v>
+        <v>2944</v>
       </c>
       <c r="C248" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="E248">
         <v>2</v>
       </c>
+      <c r="L248" s="4">
+        <v>3</v>
+      </c>
+      <c r="N248">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="249" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B249">
-        <v>2947</v>
+        <v>2945</v>
       </c>
       <c r="C249" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="E249">
         <v>2</v>
@@ -19910,10 +20138,10 @@
     </row>
     <row r="250" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B250">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="C250" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="E250">
         <v>2</v>
@@ -19921,54 +20149,60 @@
     </row>
     <row r="251" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B251">
-        <v>2961</v>
+        <v>2947</v>
       </c>
       <c r="C251" t="s">
-        <v>282</v>
-      </c>
-      <c r="D251" t="s">
-        <v>284</v>
+        <v>379</v>
+      </c>
+      <c r="E251">
+        <v>2</v>
       </c>
     </row>
     <row r="252" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B252">
-        <v>2962</v>
+        <v>2948</v>
       </c>
       <c r="C252" t="s">
-        <v>283</v>
+        <v>380</v>
+      </c>
+      <c r="E252">
+        <v>2</v>
+      </c>
+      <c r="Y252" t="s">
+        <v>1255</v>
       </c>
     </row>
     <row r="253" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B253">
-        <v>2963</v>
+        <v>2961</v>
       </c>
       <c r="C253" t="s">
-        <v>315</v>
-      </c>
-      <c r="L253" s="4">
-        <v>1</v>
-      </c>
-      <c r="N253">
-        <v>0.05</v>
+        <v>282</v>
+      </c>
+      <c r="D253" t="s">
+        <v>284</v>
+      </c>
+      <c r="Y253" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="254" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B254">
-        <v>2964</v>
+        <v>2962</v>
       </c>
       <c r="C254" t="s">
-        <v>319</v>
-      </c>
-      <c r="N254">
-        <v>0.04</v>
+        <v>283</v>
+      </c>
+      <c r="Y254" t="s">
+        <v>1290</v>
       </c>
     </row>
     <row r="255" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B255">
-        <v>2965</v>
+        <v>2963</v>
       </c>
       <c r="C255" t="s">
-        <v>845</v>
+        <v>315</v>
       </c>
       <c r="L255" s="4">
         <v>1</v>
@@ -19976,27 +20210,30 @@
       <c r="N255">
         <v>0.05</v>
       </c>
+      <c r="Y255" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="256" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B256">
-        <v>2966</v>
+        <v>2964</v>
       </c>
       <c r="C256" t="s">
-        <v>846</v>
-      </c>
-      <c r="L256" s="4">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="N256">
-        <v>0.05</v>
+        <v>0.04</v>
+      </c>
+      <c r="Y256" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="257" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B257">
-        <v>2967</v>
+        <v>2965</v>
       </c>
       <c r="C257" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="L257" s="4">
         <v>1</v>
@@ -20004,13 +20241,16 @@
       <c r="N257">
         <v>0.05</v>
       </c>
+      <c r="Y257" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="258" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B258">
-        <v>2968</v>
+        <v>2966</v>
       </c>
       <c r="C258" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="L258" s="4">
         <v>1</v>
@@ -20018,217 +20258,238 @@
       <c r="N258">
         <v>0.05</v>
       </c>
+      <c r="Y258" t="s">
+        <v>1148</v>
+      </c>
     </row>
     <row r="259" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B259">
-        <v>2969</v>
+        <v>2967</v>
       </c>
       <c r="C259" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E259">
-        <v>2</v>
+        <v>847</v>
       </c>
       <c r="L259" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="S259">
-        <v>-1.4</v>
+        <v>1</v>
+      </c>
+      <c r="N259">
+        <v>0.05</v>
+      </c>
+      <c r="Y259" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="260" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B260">
-        <v>2971</v>
+        <v>2968</v>
       </c>
       <c r="C260" t="s">
-        <v>309</v>
-      </c>
-      <c r="D260" t="s">
-        <v>304</v>
+        <v>848</v>
+      </c>
+      <c r="L260" s="4">
+        <v>1</v>
+      </c>
+      <c r="N260">
+        <v>0.05</v>
+      </c>
+      <c r="Y260" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="261" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B261">
-        <v>2972</v>
+        <v>2969</v>
       </c>
       <c r="C261" t="s">
-        <v>310</v>
+        <v>1118</v>
+      </c>
+      <c r="E261">
+        <v>2</v>
       </c>
       <c r="L261" s="4">
-        <v>1</v>
-      </c>
-      <c r="N261">
-        <v>0.02</v>
+        <v>1.8</v>
+      </c>
+      <c r="S261">
+        <v>-1.4</v>
       </c>
       <c r="Y261" t="s">
-        <v>1208</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="262" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B262">
-        <v>2973</v>
+        <v>2971</v>
       </c>
       <c r="C262" t="s">
-        <v>318</v>
-      </c>
-      <c r="L262" s="4">
-        <v>1</v>
-      </c>
-      <c r="N262">
-        <v>0.02</v>
+        <v>309</v>
+      </c>
+      <c r="D262" t="s">
+        <v>304</v>
       </c>
       <c r="Y262" t="s">
-        <v>1221</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="263" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B263">
-        <v>2974</v>
+        <v>2972</v>
       </c>
       <c r="C263" t="s">
-        <v>308</v>
-      </c>
-      <c r="E263">
-        <v>2</v>
+        <v>310</v>
+      </c>
+      <c r="L263" s="4">
+        <v>1</v>
       </c>
       <c r="N263">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="Y263" t="s">
-        <v>1171</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="264" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B264">
-        <v>2975</v>
+        <v>2973</v>
       </c>
       <c r="C264" t="s">
-        <v>316</v>
-      </c>
-      <c r="E264">
-        <v>2</v>
+        <v>318</v>
       </c>
       <c r="L264" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N264">
         <v>0.02</v>
       </c>
       <c r="Y264" t="s">
-        <v>1207</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="265" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B265">
-        <v>2976</v>
+        <v>2974</v>
       </c>
       <c r="C265" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="E265">
         <v>2</v>
       </c>
-      <c r="L265" s="4">
-        <v>1</v>
+      <c r="N265">
+        <v>0.05</v>
       </c>
       <c r="Y265" t="s">
-        <v>1212</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="266" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B266">
-        <v>2977</v>
+        <v>2975</v>
       </c>
       <c r="C266" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="E266">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L266" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N266">
-        <v>0.08</v>
-      </c>
-      <c r="Q266">
-        <v>15</v>
+        <v>0.02</v>
+      </c>
+      <c r="Y266" t="s">
+        <v>1174</v>
       </c>
     </row>
     <row r="267" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B267">
-        <v>2978</v>
+        <v>2976</v>
       </c>
       <c r="C267" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E267">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L267" s="4">
-        <v>2</v>
-      </c>
-      <c r="N267">
-        <v>0.1</v>
+        <v>1</v>
+      </c>
+      <c r="Y267" t="s">
+        <v>1285</v>
       </c>
     </row>
     <row r="268" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B268">
-        <v>2979</v>
+        <v>2977</v>
       </c>
       <c r="C268" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="E268">
         <v>3</v>
       </c>
       <c r="L268" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N268">
-        <v>0.05</v>
+        <v>0.08</v>
       </c>
       <c r="Q268">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="Y268" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="269" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B269">
-        <v>2980</v>
+        <v>2978</v>
       </c>
       <c r="C269" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E269">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L269" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N269">
+        <v>0.1</v>
+      </c>
+      <c r="Y269" t="s">
+        <v>1286</v>
       </c>
     </row>
     <row r="270" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B270">
-        <v>2981</v>
+        <v>2979</v>
       </c>
       <c r="C270" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E270">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L270" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N270">
+        <v>0.05</v>
       </c>
       <c r="Q270">
         <v>5</v>
       </c>
+      <c r="Y270" t="s">
+        <v>1298</v>
+      </c>
     </row>
     <row r="271" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B271">
-        <v>2982</v>
+        <v>2980</v>
       </c>
       <c r="C271" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="E271">
         <v>4</v>
@@ -20236,132 +20497,181 @@
       <c r="L271" s="4">
         <v>1</v>
       </c>
+      <c r="Y271" t="s">
+        <v>1259</v>
+      </c>
     </row>
     <row r="272" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B272">
-        <v>2983</v>
+        <v>2981</v>
       </c>
       <c r="C272" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E272">
+        <v>4</v>
+      </c>
+      <c r="L272" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q272">
         <v>5</v>
       </c>
-      <c r="L272" s="4">
-        <v>5</v>
-      </c>
-      <c r="N272">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q272">
-        <v>20</v>
+      <c r="Y272" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="273" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B273">
-        <v>2984</v>
+        <v>2982</v>
       </c>
       <c r="C273" t="s">
-        <v>1081</v>
+        <v>313</v>
       </c>
       <c r="E273">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="L273" s="4">
+        <v>1</v>
+      </c>
+      <c r="Y273" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="274" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B274">
-        <v>2985</v>
+        <v>2983</v>
       </c>
       <c r="C274" t="s">
-        <v>1082</v>
+        <v>314</v>
+      </c>
+      <c r="E274">
+        <v>5</v>
+      </c>
+      <c r="L274" s="4">
+        <v>5</v>
+      </c>
+      <c r="N274">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q274">
+        <v>20</v>
       </c>
       <c r="Y274" t="s">
-        <v>1148</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="275" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B275">
-        <v>2986</v>
+        <v>2984</v>
       </c>
       <c r="C275" t="s">
-        <v>1083</v>
+        <v>1081</v>
+      </c>
+      <c r="E275">
+        <v>2</v>
       </c>
       <c r="Y275" t="s">
-        <v>1148</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="276" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B276">
-        <v>2987</v>
+        <v>2985</v>
       </c>
       <c r="C276" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E276">
-        <v>3</v>
-      </c>
-      <c r="L276" s="4">
-        <v>0.5</v>
+        <v>1082</v>
+      </c>
+      <c r="Y276" t="s">
+        <v>1245</v>
       </c>
     </row>
     <row r="277" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B277">
-        <v>2988</v>
+        <v>2986</v>
       </c>
       <c r="C277" t="s">
-        <v>1095</v>
-      </c>
-      <c r="E277">
+        <v>1083</v>
+      </c>
+      <c r="Y277" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="278" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B278">
+        <v>2987</v>
+      </c>
+      <c r="C278" t="s">
+        <v>1084</v>
+      </c>
+      <c r="E278">
         <v>3</v>
       </c>
-      <c r="Y277" t="s">
-        <v>1148</v>
+      <c r="L278" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="Y278" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="279" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B279">
-        <v>2991</v>
+        <v>2988</v>
       </c>
       <c r="C279" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D279" t="s">
-        <v>1039</v>
+        <v>1095</v>
       </c>
       <c r="E279">
-        <v>1</v>
-      </c>
-      <c r="K279" s="4"/>
-      <c r="L279"/>
+        <v>3</v>
+      </c>
       <c r="Y279" t="s">
-        <v>1170</v>
-      </c>
-    </row>
-    <row r="280" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B280">
-        <v>2992</v>
-      </c>
-      <c r="C280" t="s">
-        <v>1093</v>
-      </c>
-      <c r="E280">
-        <v>2</v>
-      </c>
-      <c r="K280" s="4"/>
-      <c r="L280"/>
+        <v>1256</v>
+      </c>
     </row>
     <row r="281" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B281">
-        <v>2993</v>
+        <v>2991</v>
       </c>
       <c r="C281" t="s">
-        <v>1224</v>
+        <v>1038</v>
+      </c>
+      <c r="D281" t="s">
+        <v>1039</v>
       </c>
       <c r="E281">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K281" s="4"/>
       <c r="L281"/>
+      <c r="Y281" t="s">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="282" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B282">
+        <v>2992</v>
+      </c>
+      <c r="C282" t="s">
+        <v>1093</v>
+      </c>
+      <c r="E282">
+        <v>2</v>
+      </c>
+      <c r="K282" s="4"/>
+      <c r="L282"/>
+    </row>
+    <row r="283" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B283">
+        <v>2993</v>
+      </c>
+      <c r="C283" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E283">
+        <v>3</v>
+      </c>
+      <c r="K283" s="4"/>
+      <c r="L283"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -21744,8 +22054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21782,7 +22092,7 @@
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9" t="s">
-        <v>1175</v>
+        <v>1164</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -21796,7 +22106,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>1195</v>
+        <v>1168</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
@@ -21810,7 +22120,7 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>1211</v>
+        <v>1172</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
@@ -21865,7 +22175,7 @@
         <v>1080</v>
       </c>
       <c r="H10" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -21876,10 +22186,10 @@
         <v>1079</v>
       </c>
       <c r="F11" t="s">
-        <v>1157</v>
+        <v>1301</v>
       </c>
       <c r="H11" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -21887,13 +22197,13 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="F12" t="s">
-        <v>1173</v>
+        <v>1308</v>
       </c>
       <c r="H12" t="s">
-        <v>1161</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -21901,13 +22211,13 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>1162</v>
+        <v>1157</v>
       </c>
       <c r="F13" t="s">
-        <v>1164</v>
+        <v>1302</v>
       </c>
       <c r="H13" t="s">
-        <v>1163</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -21915,13 +22225,13 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F14" t="s">
-        <v>1192</v>
+        <v>1305</v>
       </c>
       <c r="H14" t="s">
-        <v>1159</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -21932,10 +22242,10 @@
         <v>1110</v>
       </c>
       <c r="F15" t="s">
-        <v>1167</v>
+        <v>1311</v>
       </c>
       <c r="H15" t="s">
-        <v>1176</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -21946,10 +22256,10 @@
         <v>1103</v>
       </c>
       <c r="F16" t="s">
-        <v>1193</v>
+        <v>1167</v>
       </c>
       <c r="H16" t="s">
-        <v>1177</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -21960,10 +22270,10 @@
         <v>1104</v>
       </c>
       <c r="F17" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="H17" t="s">
-        <v>1179</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -21979,10 +22289,10 @@
         <v>1097</v>
       </c>
       <c r="F19" t="s">
-        <v>1194</v>
+        <v>1306</v>
       </c>
       <c r="H19" t="s">
-        <v>1197</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -21993,10 +22303,10 @@
         <v>1105</v>
       </c>
       <c r="F20" t="s">
-        <v>1201</v>
+        <v>1317</v>
       </c>
       <c r="H20" t="s">
-        <v>1182</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -22007,10 +22317,10 @@
         <v>1107</v>
       </c>
       <c r="F21" t="s">
-        <v>1201</v>
+        <v>1303</v>
       </c>
       <c r="H21" t="s">
-        <v>1200</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -22021,10 +22331,10 @@
         <v>1106</v>
       </c>
       <c r="F22" t="s">
-        <v>1202</v>
+        <v>1316</v>
       </c>
       <c r="H22" t="s">
-        <v>1185</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -22035,10 +22345,10 @@
         <v>1111</v>
       </c>
       <c r="F23" t="s">
-        <v>1202</v>
+        <v>1315</v>
       </c>
       <c r="H23" t="s">
-        <v>1186</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -22049,10 +22359,10 @@
         <v>1112</v>
       </c>
       <c r="F24" t="s">
-        <v>1165</v>
+        <v>1158</v>
       </c>
       <c r="H24" t="s">
-        <v>1187</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -22063,10 +22373,10 @@
         <v>1113</v>
       </c>
       <c r="F25" t="s">
-        <v>1214</v>
+        <v>1307</v>
       </c>
       <c r="H25" t="s">
-        <v>1188</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -22076,8 +22386,11 @@
       <c r="D26" t="s">
         <v>1114</v>
       </c>
+      <c r="F26" t="s">
+        <v>1314</v>
+      </c>
       <c r="H26" t="s">
-        <v>1196</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -22088,10 +22401,10 @@
         <v>1115</v>
       </c>
       <c r="F27" t="s">
-        <v>1215</v>
+        <v>1304</v>
       </c>
       <c r="H27" t="s">
-        <v>1189</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -22102,10 +22415,10 @@
         <v>1116</v>
       </c>
       <c r="F28" t="s">
+        <v>1310</v>
+      </c>
+      <c r="H28" t="s">
         <v>1166</v>
-      </c>
-      <c r="H28" t="s">
-        <v>1190</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -22116,10 +22429,10 @@
         <v>1098</v>
       </c>
       <c r="F29" t="s">
-        <v>1220</v>
+        <v>1314</v>
       </c>
       <c r="H29" t="s">
-        <v>1191</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -22130,10 +22443,10 @@
         <v>1119</v>
       </c>
       <c r="F30" t="s">
-        <v>1201</v>
+        <v>1306</v>
       </c>
       <c r="H30" t="s">
-        <v>1209</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -22144,10 +22457,10 @@
         <v>1120</v>
       </c>
       <c r="F31" t="s">
-        <v>1202</v>
+        <v>1312</v>
       </c>
       <c r="H31" t="s">
-        <v>1210</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
@@ -22158,10 +22471,10 @@
         <v>1121</v>
       </c>
       <c r="F32" t="s">
-        <v>1219</v>
+        <v>1302</v>
       </c>
       <c r="H32" t="s">
-        <v>1204</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -22172,10 +22485,10 @@
         <v>1124</v>
       </c>
       <c r="F33" t="s">
-        <v>1198</v>
+        <v>1313</v>
       </c>
       <c r="H33" t="s">
-        <v>1203</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -22186,10 +22499,10 @@
         <v>1122</v>
       </c>
       <c r="F34" t="s">
-        <v>1156</v>
+        <v>1283</v>
       </c>
       <c r="H34" t="s">
-        <v>1213</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
@@ -22220,7 +22533,7 @@
         <v>1099</v>
       </c>
       <c r="H39" t="s">
-        <v>1216</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
@@ -22236,10 +22549,10 @@
         <v>1100</v>
       </c>
       <c r="F41" t="s">
-        <v>1165</v>
+        <v>1158</v>
       </c>
       <c r="H41" t="s">
-        <v>1180</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -22250,10 +22563,10 @@
         <v>1101</v>
       </c>
       <c r="F42" t="s">
-        <v>1211</v>
+        <v>1172</v>
       </c>
       <c r="H42" t="s">
-        <v>1181</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -22274,8 +22587,11 @@
       <c r="D44" t="s">
         <v>1108</v>
       </c>
+      <c r="F44" t="s">
+        <v>1282</v>
+      </c>
       <c r="H44" t="s">
-        <v>1222</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -22285,8 +22601,11 @@
       <c r="D45" t="s">
         <v>1109</v>
       </c>
+      <c r="F45" t="s">
+        <v>1309</v>
+      </c>
       <c r="H45" t="s">
-        <v>1223</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -22297,7 +22616,10 @@
         <v>1123</v>
       </c>
       <c r="F46" t="s">
-        <v>1211</v>
+        <v>1172</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1264</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
@@ -22307,6 +22629,9 @@
       <c r="D47" t="s">
         <v>1125</v>
       </c>
+      <c r="H47" t="s">
+        <v>1299</v>
+      </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
@@ -22316,88 +22641,94 @@
         <v>1126</v>
       </c>
       <c r="F48" t="s">
-        <v>1199</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1288</v>
+      </c>
+      <c r="H48" t="s">
+        <v>1264</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
         <v>39</v>
       </c>
       <c r="D49" t="s">
         <v>1127</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="H49" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
         <v>41</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
         <v>54</v>
       </c>

</xml_diff>

<commit_message>
v0.7.4j: Finished basic features/items
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E002D8-26D6-41A9-9854-31E1AB597FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623C479-76D8-4822-8438-4D50DAEB272A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1750" uniqueCount="1322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1753" uniqueCount="1324">
   <si>
     <t>ID</t>
   </si>
@@ -4464,6 +4464,12 @@
   </si>
   <si>
     <t>Holds keys (in description)</t>
+  </si>
+  <si>
+    <t>matt hair keyring</t>
+  </si>
+  <si>
+    <t>Metal Pipe</t>
   </si>
 </sst>
 </file>
@@ -16055,13 +16061,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Y283"/>
+  <dimension ref="A1:Y284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="R210" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W226" sqref="W226"/>
+      <selection pane="bottomRight" activeCell="L65" sqref="L65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17197,568 +17203,555 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B65">
+        <v>2223</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1323</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="L65" s="4">
+        <v>13</v>
+      </c>
+      <c r="N65">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="66" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B66">
         <v>2231</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C66" t="s">
         <v>1206</v>
-      </c>
-      <c r="E65">
-        <v>4</v>
-      </c>
-      <c r="L65" s="4">
-        <v>120</v>
-      </c>
-      <c r="N65">
-        <v>0.15</v>
-      </c>
-      <c r="Q65">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B66">
-        <v>2232</v>
-      </c>
-      <c r="C66" t="s">
-        <v>1207</v>
       </c>
       <c r="E66">
         <v>4</v>
       </c>
       <c r="L66" s="4">
+        <v>120</v>
+      </c>
+      <c r="N66">
+        <v>0.15</v>
+      </c>
+      <c r="Q66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B67">
+        <v>2232</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1207</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="L67" s="4">
         <v>108</v>
       </c>
-      <c r="N66">
+      <c r="N67">
         <v>0.35</v>
       </c>
-      <c r="Q66">
+      <c r="Q67">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B67">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B68">
         <v>2241</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>1208</v>
-      </c>
-      <c r="E67">
-        <v>5</v>
-      </c>
-      <c r="L67" s="4">
-        <v>260</v>
-      </c>
-      <c r="N67">
-        <v>0.15</v>
-      </c>
-      <c r="Q67">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B68">
-        <v>2242</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1209</v>
       </c>
       <c r="E68">
         <v>5</v>
       </c>
       <c r="L68" s="4">
+        <v>260</v>
+      </c>
+      <c r="N68">
+        <v>0.15</v>
+      </c>
+      <c r="Q68">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B69">
+        <v>2242</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1209</v>
+      </c>
+      <c r="E69">
+        <v>5</v>
+      </c>
+      <c r="L69" s="4">
         <v>235</v>
       </c>
-      <c r="N68">
+      <c r="N69">
         <v>0.35</v>
       </c>
-      <c r="Q68">
+      <c r="Q69">
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B69">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B70">
         <v>2251</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>1210</v>
-      </c>
-      <c r="E69">
-        <v>6</v>
-      </c>
-      <c r="L69" s="4">
-        <v>350</v>
-      </c>
-      <c r="N69">
-        <v>0.15</v>
-      </c>
-      <c r="Q69">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B70">
-        <v>2252</v>
-      </c>
-      <c r="C70" t="s">
-        <v>1211</v>
       </c>
       <c r="E70">
         <v>6</v>
       </c>
       <c r="L70" s="4">
+        <v>350</v>
+      </c>
+      <c r="N70">
+        <v>0.15</v>
+      </c>
+      <c r="Q70">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B71">
+        <v>2252</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E71">
+        <v>6</v>
+      </c>
+      <c r="L71" s="4">
         <v>315</v>
       </c>
-      <c r="N70">
+      <c r="N71">
         <v>0.35</v>
       </c>
-      <c r="Q70">
+      <c r="Q71">
         <v>16</v>
       </c>
     </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B71">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B72">
         <v>2261</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>1212</v>
-      </c>
-      <c r="E71">
-        <v>7</v>
-      </c>
-      <c r="L71" s="4">
-        <v>460</v>
-      </c>
-      <c r="N71">
-        <v>0.15</v>
-      </c>
-      <c r="Q71">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B72">
-        <v>2262</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1213</v>
       </c>
       <c r="E72">
         <v>7</v>
       </c>
       <c r="L72" s="4">
+        <v>460</v>
+      </c>
+      <c r="N72">
+        <v>0.15</v>
+      </c>
+      <c r="Q72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B73">
+        <v>2262</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1213</v>
+      </c>
+      <c r="E73">
+        <v>7</v>
+      </c>
+      <c r="L73" s="4">
         <v>415</v>
       </c>
-      <c r="N72">
+      <c r="N73">
         <v>0.35</v>
       </c>
-      <c r="Q72">
+      <c r="Q73">
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B73">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B74">
         <v>2271</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C74" t="s">
         <v>1217</v>
-      </c>
-      <c r="E73">
-        <v>8</v>
-      </c>
-      <c r="L73" s="4">
-        <v>980</v>
-      </c>
-      <c r="N73">
-        <v>0.15</v>
-      </c>
-      <c r="Q73">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B74">
-        <v>2272</v>
-      </c>
-      <c r="C74" t="s">
-        <v>1218</v>
       </c>
       <c r="E74">
         <v>8</v>
       </c>
       <c r="L74" s="4">
+        <v>980</v>
+      </c>
+      <c r="N74">
+        <v>0.15</v>
+      </c>
+      <c r="Q74">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B75">
+        <v>2272</v>
+      </c>
+      <c r="C75" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E75">
+        <v>8</v>
+      </c>
+      <c r="L75" s="4">
         <v>890</v>
       </c>
-      <c r="N74">
+      <c r="N75">
         <v>0.35</v>
       </c>
-      <c r="Q74">
+      <c r="Q75">
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B75">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B76">
         <v>2281</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>1219</v>
-      </c>
-      <c r="E75">
-        <v>9</v>
-      </c>
-      <c r="L75" s="4">
-        <v>2000</v>
-      </c>
-      <c r="N75">
-        <v>0.15</v>
-      </c>
-      <c r="Q75">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B76">
-        <v>2282</v>
-      </c>
-      <c r="C76" t="s">
-        <v>1220</v>
       </c>
       <c r="E76">
         <v>9</v>
       </c>
       <c r="L76" s="4">
+        <v>2000</v>
+      </c>
+      <c r="N76">
+        <v>0.15</v>
+      </c>
+      <c r="Q76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B77">
+        <v>2282</v>
+      </c>
+      <c r="C77" t="s">
+        <v>1220</v>
+      </c>
+      <c r="E77">
+        <v>9</v>
+      </c>
+      <c r="L77" s="4">
         <v>1750</v>
       </c>
-      <c r="N76">
+      <c r="N77">
         <v>0.35</v>
       </c>
-      <c r="Q76">
+      <c r="Q77">
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B77">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B78">
         <v>2291</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>1221</v>
-      </c>
-      <c r="E77">
-        <v>10</v>
-      </c>
-      <c r="L77" s="4">
-        <v>9100</v>
-      </c>
-      <c r="N77">
-        <v>0.15</v>
-      </c>
-      <c r="Q77">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B78">
-        <v>2292</v>
-      </c>
-      <c r="C78" t="s">
-        <v>1222</v>
       </c>
       <c r="E78">
         <v>10</v>
       </c>
       <c r="L78" s="4">
+        <v>9100</v>
+      </c>
+      <c r="N78">
+        <v>0.15</v>
+      </c>
+      <c r="Q78">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B79">
+        <v>2292</v>
+      </c>
+      <c r="C79" t="s">
+        <v>1222</v>
+      </c>
+      <c r="E79">
+        <v>10</v>
+      </c>
+      <c r="L79" s="4">
         <v>7400</v>
       </c>
-      <c r="N78">
+      <c r="N79">
         <v>0.35</v>
       </c>
-      <c r="Q78">
+      <c r="Q79">
         <v>24</v>
-      </c>
-    </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B80">
-        <v>2301</v>
-      </c>
-      <c r="C80" t="s">
-        <v>36</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L80" s="13" t="s">
-        <v>853</v>
-      </c>
-      <c r="N80">
-        <v>3.5</v>
-      </c>
-      <c r="U80">
-        <v>1</v>
-      </c>
-      <c r="W80" t="s">
-        <v>814</v>
-      </c>
-      <c r="Y80" t="s">
-        <v>1148</v>
       </c>
     </row>
     <row r="81" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B81">
-        <v>2311</v>
+        <v>2301</v>
       </c>
       <c r="C81" t="s">
-        <v>743</v>
-      </c>
-      <c r="D81" s="15"/>
-      <c r="E81">
-        <v>2</v>
+        <v>36</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>29</v>
       </c>
       <c r="L81" s="13" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="N81">
-        <v>5</v>
-      </c>
-      <c r="Q81">
-        <v>15</v>
+        <v>3.5</v>
       </c>
       <c r="U81">
         <v>1</v>
       </c>
       <c r="W81" t="s">
-        <v>815</v>
+        <v>814</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="82" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B82">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="C82" t="s">
-        <v>162</v>
+        <v>743</v>
       </c>
       <c r="D82" s="15"/>
       <c r="E82">
         <v>2</v>
       </c>
-      <c r="L82" s="4">
-        <v>20</v>
+      <c r="L82" s="13" t="s">
+        <v>854</v>
       </c>
       <c r="N82">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q82">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U82">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="W82" t="s">
-        <v>347</v>
-      </c>
-      <c r="Y82" t="s">
-        <v>1259</v>
+        <v>815</v>
       </c>
     </row>
     <row r="83" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B83">
-        <v>2321</v>
+        <v>2312</v>
       </c>
       <c r="C83" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="D83" s="15"/>
       <c r="E83">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L83" s="4">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="N83">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="Q83">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="U83">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W83" t="s">
-        <v>354</v>
+        <v>347</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="84" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B84">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="C84" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D84" s="15"/>
       <c r="E84">
         <v>3</v>
       </c>
-      <c r="L84" s="4" t="s">
-        <v>338</v>
+      <c r="L84" s="4">
+        <v>200</v>
       </c>
       <c r="N84">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q84">
         <v>10</v>
       </c>
       <c r="U84">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W84" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="85" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B85">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="C85" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D85" s="15"/>
       <c r="E85">
         <v>3</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="N85">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q85">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="U85">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W85" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="86" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B86">
-        <v>2331</v>
+        <v>2323</v>
       </c>
       <c r="C86" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D86" s="15"/>
       <c r="E86">
-        <v>4</v>
-      </c>
-      <c r="L86"/>
-      <c r="M86" s="4">
-        <v>1000</v>
-      </c>
-      <c r="O86">
-        <v>12</v>
-      </c>
-      <c r="R86">
-        <v>5</v>
-      </c>
-      <c r="V86">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="N86">
+        <v>9</v>
+      </c>
+      <c r="Q86">
+        <v>18</v>
+      </c>
+      <c r="U86">
+        <v>30</v>
       </c>
       <c r="W86" t="s">
-        <v>850</v>
+        <v>365</v>
       </c>
     </row>
     <row r="87" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C87" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="D87" s="15"/>
       <c r="E87">
         <v>4</v>
       </c>
-      <c r="L87" s="4" t="s">
-        <v>335</v>
-      </c>
-      <c r="N87">
-        <v>10</v>
-      </c>
-      <c r="Q87">
-        <v>15</v>
-      </c>
-      <c r="U87">
-        <v>20</v>
+      <c r="L87"/>
+      <c r="M87" s="4">
+        <v>1000</v>
+      </c>
+      <c r="O87">
+        <v>12</v>
+      </c>
+      <c r="R87">
+        <v>5</v>
+      </c>
+      <c r="V87">
+        <v>6</v>
       </c>
       <c r="W87" t="s">
-        <v>351</v>
+        <v>850</v>
       </c>
     </row>
     <row r="88" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B88">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="C88" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D88" s="15"/>
       <c r="E88">
         <v>4</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="N88">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q88">
         <v>15</v>
       </c>
       <c r="U88">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="W88" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="89" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>2341</v>
+        <v>2333</v>
       </c>
       <c r="C89" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D89" s="15"/>
       <c r="E89">
-        <v>5</v>
-      </c>
-      <c r="L89" s="4">
-        <v>600</v>
+        <v>4</v>
+      </c>
+      <c r="L89" s="4" t="s">
+        <v>328</v>
       </c>
       <c r="N89">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q89">
+        <v>15</v>
+      </c>
+      <c r="U89">
         <v>6</v>
       </c>
-      <c r="S89">
-        <v>-1</v>
-      </c>
-      <c r="U89">
-        <v>1</v>
-      </c>
       <c r="W89" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="90" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="C90" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90">
@@ -17768,250 +17761,253 @@
         <v>600</v>
       </c>
       <c r="N90">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q90">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="S90">
+        <v>-1</v>
       </c>
       <c r="U90">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="W90" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="91" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="C91" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D91" s="15"/>
       <c r="E91">
         <v>5</v>
       </c>
-      <c r="L91" s="4" t="s">
-        <v>339</v>
+      <c r="L91" s="4">
+        <v>600</v>
       </c>
       <c r="N91">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="Q91">
         <v>15</v>
       </c>
       <c r="U91">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="W91" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="92" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="C92" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D92" s="15"/>
       <c r="E92">
         <v>5</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="N92">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q92">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U92">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="W92" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="93" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="C93" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D93" s="15"/>
       <c r="E93">
         <v>5</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="N93">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="Q93">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="U93">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="W93" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
     </row>
     <row r="94" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2351</v>
+        <v>2345</v>
       </c>
       <c r="C94" t="s">
-        <v>142</v>
+        <v>158</v>
       </c>
       <c r="D94" s="15"/>
       <c r="E94">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L94" s="4" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="N94">
+        <v>4</v>
+      </c>
+      <c r="Q94">
         <v>10</v>
       </c>
-      <c r="Q94">
-        <v>16</v>
-      </c>
       <c r="U94">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="W94" t="s">
-        <v>350</v>
+        <v>366</v>
       </c>
     </row>
     <row r="95" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="C95" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D95" s="15"/>
       <c r="E95">
         <v>6</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="N95">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Q95">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="U95">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="W95" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="96" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="C96" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D96" s="15"/>
       <c r="E96">
         <v>6</v>
       </c>
-      <c r="L96" s="4">
-        <v>500</v>
+      <c r="L96" s="4" t="s">
+        <v>336</v>
       </c>
       <c r="N96">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="Q96">
-        <v>25</v>
-      </c>
-      <c r="S96">
-        <v>1</v>
-      </c>
-      <c r="T96">
-        <v>0.1</v>
+        <v>20</v>
       </c>
       <c r="U96">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="W96" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="97" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="C97" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D97" s="15"/>
       <c r="E97">
         <v>6</v>
       </c>
-      <c r="L97" s="4" t="s">
-        <v>327</v>
+      <c r="L97" s="4">
+        <v>500</v>
       </c>
       <c r="N97">
         <v>7</v>
       </c>
       <c r="Q97">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="S97">
+        <v>1</v>
+      </c>
+      <c r="T97">
+        <v>0.1</v>
       </c>
       <c r="U97">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="W97" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="98" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="C98" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D98" s="15"/>
       <c r="E98">
         <v>6</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N98">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="Q98">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U98">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="W98" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="99" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>2361</v>
+        <v>2355</v>
       </c>
       <c r="C99" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D99" s="15"/>
       <c r="E99">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L99" s="4" t="s">
         <v>329</v>
@@ -18020,256 +18016,256 @@
         <v>11</v>
       </c>
       <c r="Q99">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U99">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="W99" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
     </row>
     <row r="100" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="C100" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="D100" s="15"/>
       <c r="E100">
         <v>7</v>
       </c>
-      <c r="L100" s="4">
-        <v>1200</v>
+      <c r="L100" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="N100">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q100">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="U100">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="W100" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="101" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="C101" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="D101" s="15"/>
       <c r="E101">
         <v>7</v>
       </c>
-      <c r="L101" s="4" t="s">
-        <v>337</v>
+      <c r="L101" s="4">
+        <v>1200</v>
       </c>
       <c r="N101">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="Q101">
-        <v>30</v>
-      </c>
-      <c r="S101">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="U101">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="W101" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="102" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="C102" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D102" s="15"/>
       <c r="E102">
         <v>7</v>
       </c>
       <c r="L102" s="4" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="N102">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="Q102">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="S102">
+        <v>-1</v>
       </c>
       <c r="U102">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W102" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="103" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2371</v>
+        <v>2364</v>
       </c>
       <c r="C103" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="D103" s="15"/>
       <c r="E103">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L103" s="4" t="s">
-        <v>331</v>
+        <v>344</v>
       </c>
       <c r="N103">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q103">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="U103">
-        <v>125</v>
+        <v>5</v>
       </c>
       <c r="W103" t="s">
-        <v>1032</v>
+        <v>366</v>
       </c>
     </row>
     <row r="104" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="C104" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D104" s="15"/>
       <c r="E104">
         <v>8</v>
       </c>
-      <c r="L104" s="4">
-        <v>500</v>
-      </c>
-      <c r="M104">
-        <v>500</v>
+      <c r="L104" s="4" t="s">
+        <v>331</v>
       </c>
       <c r="N104">
-        <v>9</v>
-      </c>
-      <c r="R104">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="Q104">
+        <v>20</v>
       </c>
       <c r="U104">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="W104" t="s">
-        <v>348</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="105" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D105" s="15"/>
       <c r="E105">
         <v>8</v>
       </c>
-      <c r="L105" s="4" t="s">
-        <v>334</v>
+      <c r="L105" s="4">
+        <v>500</v>
+      </c>
+      <c r="M105">
+        <v>500</v>
       </c>
       <c r="N105">
-        <v>11</v>
-      </c>
-      <c r="Q105">
-        <v>22</v>
+        <v>9</v>
+      </c>
+      <c r="R105">
+        <v>8</v>
       </c>
       <c r="U105">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="W105" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="106" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="D106" s="15"/>
       <c r="E106">
         <v>8</v>
       </c>
-      <c r="L106" s="4">
-        <v>1000</v>
+      <c r="L106" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="N106">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Q106">
+        <v>22</v>
+      </c>
+      <c r="U106">
         <v>35</v>
       </c>
-      <c r="S106">
-        <v>1.5</v>
-      </c>
-      <c r="T106">
-        <v>0.15</v>
-      </c>
-      <c r="U106">
-        <v>1</v>
-      </c>
       <c r="W106" t="s">
-        <v>364</v>
+        <v>350</v>
       </c>
     </row>
     <row r="107" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="C107" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D107" s="15"/>
       <c r="E107">
         <v>8</v>
       </c>
-      <c r="L107" s="4" t="s">
-        <v>342</v>
+      <c r="L107" s="4">
+        <v>1000</v>
       </c>
       <c r="N107">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="Q107">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="S107">
+        <v>1.5</v>
+      </c>
+      <c r="T107">
+        <v>0.15</v>
       </c>
       <c r="U107">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="W107" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="108" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2381</v>
+        <v>2375</v>
       </c>
       <c r="C108" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D108" s="15"/>
       <c r="E108">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L108" s="4" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="N108">
         <v>12</v>
@@ -18278,133 +18274,146 @@
         <v>20</v>
       </c>
       <c r="U108">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="W108" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
     </row>
     <row r="109" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="C109" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D109" s="15"/>
       <c r="E109">
         <v>9</v>
       </c>
-      <c r="L109" s="4">
-        <v>1000</v>
+      <c r="L109" s="4" t="s">
+        <v>330</v>
       </c>
       <c r="N109">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="Q109">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="U109">
-        <v>8</v>
+        <v>125</v>
       </c>
       <c r="W109" t="s">
-        <v>359</v>
+        <v>345</v>
       </c>
     </row>
     <row r="110" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2391</v>
+        <v>2382</v>
       </c>
       <c r="C110" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="D110" s="15"/>
       <c r="E110">
-        <v>10</v>
-      </c>
-      <c r="L110" s="4" t="s">
-        <v>332</v>
+        <v>9</v>
+      </c>
+      <c r="L110" s="4">
+        <v>1000</v>
       </c>
       <c r="N110">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Q110">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="U110">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="W110" t="s">
-        <v>1033</v>
+        <v>359</v>
       </c>
     </row>
     <row r="111" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="C111" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D111" s="15"/>
       <c r="E111">
         <v>10</v>
       </c>
-      <c r="L111" s="4">
+      <c r="L111" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="N111">
+        <v>11</v>
+      </c>
+      <c r="Q111">
+        <v>25</v>
+      </c>
+      <c r="U111">
+        <v>125</v>
+      </c>
+      <c r="W111" t="s">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="112" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B112">
+        <v>2392</v>
+      </c>
+      <c r="C112" t="s">
+        <v>141</v>
+      </c>
+      <c r="D112" s="15"/>
+      <c r="E112">
+        <v>10</v>
+      </c>
+      <c r="L112" s="4">
         <v>500</v>
       </c>
-      <c r="M111">
+      <c r="M112">
         <v>500</v>
       </c>
-      <c r="N111">
+      <c r="N112">
         <v>9</v>
       </c>
-      <c r="R111">
+      <c r="R112">
         <v>12</v>
       </c>
-      <c r="U111">
+      <c r="U112">
         <v>40</v>
       </c>
-      <c r="W111" t="s">
+      <c r="W112" t="s">
         <v>349</v>
-      </c>
-    </row>
-    <row r="113" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B113">
-        <v>2401</v>
-      </c>
-      <c r="C113" t="s">
-        <v>97</v>
-      </c>
-      <c r="D113" t="s">
-        <v>22</v>
-      </c>
-      <c r="O113">
-        <v>1</v>
-      </c>
-      <c r="Y113" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="114" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="C114" t="s">
-        <v>166</v>
+        <v>97</v>
+      </c>
+      <c r="D114" t="s">
+        <v>22</v>
+      </c>
+      <c r="O114">
+        <v>1</v>
       </c>
       <c r="Y114" t="s">
-        <v>1148</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="115" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="C115" t="s">
-        <v>168</v>
-      </c>
-      <c r="O115">
-        <v>1</v>
+        <v>166</v>
       </c>
       <c r="Y115" t="s">
         <v>1148</v>
@@ -18412,190 +18421,190 @@
     </row>
     <row r="116" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B116">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="C116" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O116">
-        <v>2</v>
-      </c>
-      <c r="S116">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="Y116" t="s">
-        <v>1169</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="117" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>2411</v>
+        <v>2404</v>
       </c>
       <c r="C117" t="s">
-        <v>98</v>
-      </c>
-      <c r="E117">
-        <v>2</v>
+        <v>167</v>
       </c>
       <c r="O117">
         <v>2</v>
       </c>
+      <c r="S117">
+        <v>-0.5</v>
+      </c>
       <c r="Y117" t="s">
-        <v>1240</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="118" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>2421</v>
+        <v>2411</v>
       </c>
       <c r="C118" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E118">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O118">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="Y118" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="119" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>2431</v>
+        <v>2421</v>
       </c>
       <c r="C119" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E119">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O119">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>2441</v>
+        <v>2431</v>
       </c>
       <c r="C120" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E120">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O120">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2451</v>
+        <v>2441</v>
       </c>
       <c r="C121" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E121">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O121">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="122" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2461</v>
+        <v>2451</v>
       </c>
       <c r="C122" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E122">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O122">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="123" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2471</v>
+        <v>2461</v>
       </c>
       <c r="C123" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E123">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O123">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2481</v>
+        <v>2471</v>
       </c>
       <c r="C124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E124">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O124">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="125" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B125">
+        <v>2481</v>
+      </c>
+      <c r="C125" t="s">
+        <v>105</v>
+      </c>
+      <c r="E125">
+        <v>9</v>
+      </c>
+      <c r="O125">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="126" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B126">
         <v>2491</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>106</v>
       </c>
-      <c r="E125">
+      <c r="E126">
         <v>10</v>
       </c>
-      <c r="O125">
+      <c r="O126">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="127" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>2501</v>
-      </c>
-      <c r="C127" t="s">
-        <v>801</v>
-      </c>
-      <c r="D127" t="s">
-        <v>23</v>
-      </c>
-      <c r="O127">
-        <v>1</v>
-      </c>
-      <c r="Y127" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="128" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="C128" t="s">
-        <v>169</v>
-      </c>
-      <c r="N128">
-        <v>0.04</v>
+        <v>801</v>
+      </c>
+      <c r="D128" t="s">
+        <v>23</v>
+      </c>
+      <c r="O128">
+        <v>1</v>
       </c>
       <c r="Y128" t="s">
-        <v>1148</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="129" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="C129" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N129">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="Y129" t="s">
         <v>1148</v>
@@ -18603,227 +18612,227 @@
     </row>
     <row r="130" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B130">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="C130" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N130">
-        <v>0.04</v>
-      </c>
-      <c r="O130">
-        <v>1</v>
+        <v>0.02</v>
       </c>
       <c r="Y130" t="s">
-        <v>1243</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="131" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2511</v>
+        <v>2504</v>
       </c>
       <c r="C131" t="s">
-        <v>802</v>
-      </c>
-      <c r="E131">
-        <v>2</v>
+        <v>171</v>
+      </c>
+      <c r="N131">
+        <v>0.04</v>
       </c>
       <c r="O131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y131" t="s">
-        <v>1240</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="132" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="C132" t="s">
-        <v>179</v>
+        <v>802</v>
       </c>
       <c r="E132">
         <v>2</v>
       </c>
-      <c r="K132">
-        <v>3</v>
-      </c>
-      <c r="N132">
-        <v>0.05</v>
-      </c>
       <c r="O132">
         <v>2</v>
       </c>
       <c r="Y132" t="s">
-        <v>1241</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="133" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="C133" t="s">
-        <v>300</v>
+        <v>179</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="K133">
+        <v>3</v>
       </c>
       <c r="N133">
-        <v>0.04</v>
+        <v>0.05</v>
+      </c>
+      <c r="O133">
+        <v>2</v>
       </c>
       <c r="Y133" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="134" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2521</v>
+        <v>2513</v>
       </c>
       <c r="C134" t="s">
-        <v>803</v>
-      </c>
-      <c r="E134">
-        <v>3</v>
-      </c>
-      <c r="O134">
-        <v>14</v>
+        <v>300</v>
+      </c>
+      <c r="N134">
+        <v>0.04</v>
+      </c>
+      <c r="Y134" t="s">
+        <v>1242</v>
       </c>
     </row>
     <row r="135" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2531</v>
+        <v>2521</v>
       </c>
       <c r="C135" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E135">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O135">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B136">
-        <v>2541</v>
+        <v>2531</v>
       </c>
       <c r="C136" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="E136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O136">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="137" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>2551</v>
+        <v>2541</v>
       </c>
       <c r="C137" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="E137">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O137">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="138" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2561</v>
+        <v>2551</v>
       </c>
       <c r="C138" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E138">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O138">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="139" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2571</v>
+        <v>2561</v>
       </c>
       <c r="C139" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E139">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O139">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="140" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2581</v>
+        <v>2571</v>
       </c>
       <c r="C140" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E140">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O140">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="141" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B141">
+        <v>2581</v>
+      </c>
+      <c r="C141" t="s">
+        <v>810</v>
+      </c>
+      <c r="E141">
+        <v>9</v>
+      </c>
+      <c r="O141">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="142" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B142">
         <v>2591</v>
       </c>
-      <c r="C141" t="s">
+      <c r="C142" t="s">
         <v>809</v>
       </c>
-      <c r="E141">
+      <c r="E142">
         <v>10</v>
       </c>
-      <c r="O141">
+      <c r="O142">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="143" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B143">
-        <v>2601</v>
-      </c>
-      <c r="C143" t="s">
-        <v>107</v>
-      </c>
-      <c r="D143" t="s">
-        <v>24</v>
-      </c>
-      <c r="O143">
-        <v>1</v>
-      </c>
-      <c r="Y143" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="144" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2602</v>
+        <v>2601</v>
       </c>
       <c r="C144" t="s">
-        <v>172</v>
-      </c>
-      <c r="N144">
-        <v>0.02</v>
+        <v>107</v>
+      </c>
+      <c r="D144" t="s">
+        <v>24</v>
+      </c>
+      <c r="O144">
+        <v>1</v>
       </c>
       <c r="Y144" t="s">
-        <v>1148</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="145" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="C145" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="N145">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="Y145" t="s">
         <v>1148</v>
@@ -18831,16 +18840,13 @@
     </row>
     <row r="146" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B146">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="C146" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="N146">
-        <v>0.08</v>
-      </c>
-      <c r="O146">
-        <v>1</v>
+        <v>0.06</v>
       </c>
       <c r="Y146" t="s">
         <v>1148</v>
@@ -18848,170 +18854,173 @@
     </row>
     <row r="147" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B147">
-        <v>2611</v>
+        <v>2604</v>
       </c>
       <c r="C147" t="s">
-        <v>108</v>
-      </c>
-      <c r="E147">
-        <v>2</v>
+        <v>173</v>
+      </c>
+      <c r="N147">
+        <v>0.08</v>
       </c>
       <c r="O147">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y147" t="s">
-        <v>1240</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="148" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2621</v>
+        <v>2611</v>
       </c>
       <c r="C148" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E148">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O148">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="Y148" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="149" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2631</v>
+        <v>2621</v>
       </c>
       <c r="C149" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E149">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O149">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2641</v>
+        <v>2631</v>
       </c>
       <c r="C150" t="s">
-        <v>741</v>
+        <v>110</v>
       </c>
       <c r="E150">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O150">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="151" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>2651</v>
+        <v>2641</v>
       </c>
       <c r="C151" t="s">
-        <v>111</v>
+        <v>741</v>
       </c>
       <c r="E151">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O151">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="152" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>2661</v>
+        <v>2651</v>
       </c>
       <c r="C152" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E152">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O152">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="153" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2671</v>
+        <v>2661</v>
       </c>
       <c r="C153" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E153">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O153">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="154" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2681</v>
+        <v>2671</v>
       </c>
       <c r="C154" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E154">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O154">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B155">
+        <v>2681</v>
+      </c>
+      <c r="C155" t="s">
+        <v>114</v>
+      </c>
+      <c r="E155">
+        <v>9</v>
+      </c>
+      <c r="O155">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="156" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B156">
         <v>2691</v>
       </c>
-      <c r="C155" t="s">
+      <c r="C156" t="s">
         <v>115</v>
       </c>
-      <c r="E155">
+      <c r="E156">
         <v>10</v>
       </c>
-      <c r="O155">
+      <c r="O156">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="157" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B157">
-        <v>2701</v>
-      </c>
-      <c r="C157" t="s">
-        <v>116</v>
-      </c>
-      <c r="D157" t="s">
-        <v>25</v>
-      </c>
-      <c r="O157">
-        <v>1</v>
-      </c>
-      <c r="Y157" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="158" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2702</v>
+        <v>2701</v>
       </c>
       <c r="C158" t="s">
-        <v>175</v>
+        <v>116</v>
+      </c>
+      <c r="D158" t="s">
+        <v>25</v>
+      </c>
+      <c r="O158">
+        <v>1</v>
       </c>
       <c r="Y158" t="s">
-        <v>1148</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="159" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2703</v>
+        <v>2702</v>
       </c>
       <c r="C159" t="s">
-        <v>176</v>
-      </c>
-      <c r="S159">
-        <v>0.2</v>
+        <v>175</v>
       </c>
       <c r="Y159" t="s">
         <v>1148</v>
@@ -19019,697 +19028,694 @@
     </row>
     <row r="160" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B160">
-        <v>2704</v>
+        <v>2703</v>
       </c>
       <c r="C160" t="s">
-        <v>177</v>
-      </c>
-      <c r="O160">
-        <v>1</v>
+        <v>176</v>
       </c>
       <c r="S160">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="Y160" t="s">
-        <v>1244</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="161" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2705</v>
+        <v>2704</v>
       </c>
       <c r="C161" t="s">
-        <v>301</v>
+        <v>177</v>
       </c>
       <c r="O161">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S161">
         <v>0.4</v>
       </c>
       <c r="Y161" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="162" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2711</v>
+        <v>2705</v>
       </c>
       <c r="C162" t="s">
-        <v>117</v>
-      </c>
-      <c r="E162">
-        <v>2</v>
+        <v>301</v>
       </c>
       <c r="O162">
         <v>2</v>
       </c>
+      <c r="S162">
+        <v>0.4</v>
+      </c>
       <c r="Y162" t="s">
-        <v>1240</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="163" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="C163" t="s">
-        <v>178</v>
+        <v>117</v>
       </c>
       <c r="E163">
         <v>2</v>
       </c>
       <c r="O163">
-        <v>1</v>
-      </c>
-      <c r="S163">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="Y163" t="s">
-        <v>1246</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="164" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2713</v>
+        <v>2712</v>
       </c>
       <c r="C164" t="s">
-        <v>302</v>
+        <v>178</v>
       </c>
       <c r="E164">
         <v>2</v>
       </c>
-      <c r="L164" s="4">
+      <c r="O164">
         <v>1</v>
       </c>
-      <c r="O164">
-        <v>3</v>
-      </c>
       <c r="S164">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="Y164" t="s">
-        <v>1248</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="165" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2714</v>
+        <v>2713</v>
       </c>
       <c r="C165" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E165">
         <v>2</v>
       </c>
+      <c r="L165" s="4">
+        <v>1</v>
+      </c>
       <c r="O165">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S165">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="Y165" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="166" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2721</v>
+        <v>2714</v>
       </c>
       <c r="C166" t="s">
-        <v>118</v>
+        <v>303</v>
       </c>
       <c r="E166">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O166">
-        <v>14</v>
+        <v>2</v>
+      </c>
+      <c r="S166">
+        <v>0.6</v>
+      </c>
+      <c r="Y166" t="s">
+        <v>1247</v>
       </c>
     </row>
     <row r="167" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2731</v>
+        <v>2721</v>
       </c>
       <c r="C167" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E167">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O167">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2741</v>
+        <v>2731</v>
       </c>
       <c r="C168" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E168">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O168">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="169" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2751</v>
+        <v>2741</v>
       </c>
       <c r="C169" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E169">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O169">
-        <v>72</v>
+        <v>48</v>
       </c>
     </row>
     <row r="170" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2761</v>
+        <v>2751</v>
       </c>
       <c r="C170" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E170">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O170">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="171" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2771</v>
+        <v>2761</v>
       </c>
       <c r="C171" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E171">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O171">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="172" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2781</v>
+        <v>2771</v>
       </c>
       <c r="C172" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E172">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O172">
-        <v>400</v>
+        <v>200</v>
       </c>
     </row>
     <row r="173" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B173">
+        <v>2781</v>
+      </c>
+      <c r="C173" t="s">
+        <v>124</v>
+      </c>
+      <c r="E173">
+        <v>9</v>
+      </c>
+      <c r="O173">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="174" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B174">
         <v>2791</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C174" t="s">
         <v>125</v>
       </c>
-      <c r="E173">
+      <c r="E174">
         <v>10</v>
       </c>
-      <c r="O173">
+      <c r="O174">
         <v>1500</v>
-      </c>
-    </row>
-    <row r="175" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B175">
-        <v>2801</v>
-      </c>
-      <c r="C175" t="s">
-        <v>770</v>
-      </c>
-      <c r="D175" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="176" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B176">
-        <v>2802</v>
+        <v>2801</v>
       </c>
       <c r="C176" t="s">
-        <v>771</v>
+        <v>770</v>
+      </c>
+      <c r="D176" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="177" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B177">
-        <v>2803</v>
+        <v>2802</v>
       </c>
       <c r="C177" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="178" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B178">
-        <v>2804</v>
+        <v>2803</v>
       </c>
       <c r="C178" t="s">
-        <v>764</v>
+        <v>772</v>
       </c>
     </row>
     <row r="179" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2805</v>
+        <v>2804</v>
       </c>
       <c r="C179" t="s">
-        <v>744</v>
-      </c>
-      <c r="Y179" t="s">
-        <v>1148</v>
+        <v>764</v>
       </c>
     </row>
     <row r="180" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2806</v>
+        <v>2805</v>
       </c>
       <c r="C180" t="s">
-        <v>298</v>
+        <v>744</v>
       </c>
       <c r="Y180" t="s">
-        <v>1275</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="181" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B181">
-        <v>2807</v>
+        <v>2806</v>
       </c>
       <c r="C181" t="s">
-        <v>1016</v>
+        <v>298</v>
       </c>
       <c r="Y181" t="s">
-        <v>1151</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="182" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2808</v>
+        <v>2807</v>
       </c>
       <c r="C182" t="s">
-        <v>1085</v>
+        <v>1016</v>
       </c>
       <c r="Y182" t="s">
-        <v>1249</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="183" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2809</v>
+        <v>2808</v>
       </c>
       <c r="C183" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="Y183" t="s">
-        <v>1148</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="184" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2810</v>
+        <v>2809</v>
       </c>
       <c r="C184" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="Y184" t="s">
-        <v>1250</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="185" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B185">
-        <v>2811</v>
+        <v>2810</v>
       </c>
       <c r="C185" t="s">
-        <v>773</v>
-      </c>
-      <c r="E185">
-        <v>2</v>
+        <v>1088</v>
+      </c>
+      <c r="Y185" t="s">
+        <v>1250</v>
       </c>
     </row>
     <row r="186" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2812</v>
+        <v>2811</v>
       </c>
       <c r="C186" t="s">
-        <v>774</v>
+        <v>773</v>
+      </c>
+      <c r="E186">
+        <v>2</v>
       </c>
     </row>
     <row r="187" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B187">
-        <v>2813</v>
+        <v>2812</v>
       </c>
       <c r="C187" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="188" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2814</v>
+        <v>2813</v>
       </c>
       <c r="C188" t="s">
-        <v>798</v>
+        <v>775</v>
       </c>
     </row>
     <row r="189" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2815</v>
+        <v>2814</v>
       </c>
       <c r="C189" t="s">
-        <v>299</v>
+        <v>798</v>
       </c>
     </row>
     <row r="190" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2816</v>
+        <v>2815</v>
       </c>
       <c r="C190" t="s">
-        <v>1147</v>
-      </c>
-      <c r="L190" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="N190">
-        <v>0.6</v>
-      </c>
-      <c r="S190">
-        <v>-0.8</v>
+        <v>299</v>
       </c>
     </row>
     <row r="191" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2817</v>
+        <v>2816</v>
       </c>
       <c r="C191" t="s">
-        <v>1177</v>
+        <v>1147</v>
       </c>
       <c r="L191" s="4">
-        <v>2.8</v>
+        <v>2.4</v>
       </c>
       <c r="N191">
-        <v>0.4</v>
+        <v>0.6</v>
+      </c>
+      <c r="S191">
+        <v>-0.8</v>
       </c>
     </row>
     <row r="192" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2818</v>
+        <v>2817</v>
       </c>
       <c r="C192" t="s">
-        <v>1183</v>
+        <v>1177</v>
       </c>
       <c r="L192" s="4">
-        <v>0.5</v>
+        <v>2.8</v>
       </c>
       <c r="N192">
-        <v>0.02</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="193" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2821</v>
+        <v>2818</v>
       </c>
       <c r="C193" t="s">
-        <v>776</v>
-      </c>
-      <c r="E193">
-        <v>3</v>
+        <v>1183</v>
+      </c>
+      <c r="L193" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N193">
+        <v>0.02</v>
       </c>
     </row>
     <row r="194" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2822</v>
+        <v>2821</v>
       </c>
       <c r="C194" t="s">
-        <v>777</v>
+        <v>776</v>
+      </c>
+      <c r="E194">
+        <v>3</v>
       </c>
     </row>
     <row r="195" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2823</v>
+        <v>2822</v>
       </c>
       <c r="C195" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="196" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2834</v>
+        <v>2823</v>
       </c>
       <c r="C196" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="197" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2825</v>
+        <v>2834</v>
       </c>
       <c r="C197" t="s">
-        <v>539</v>
-      </c>
-      <c r="Y197" t="s">
-        <v>201</v>
+        <v>778</v>
       </c>
     </row>
     <row r="198" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2831</v>
+        <v>2825</v>
       </c>
       <c r="C198" t="s">
-        <v>780</v>
-      </c>
-      <c r="E198">
-        <v>4</v>
+        <v>539</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="199" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2832</v>
+        <v>2831</v>
       </c>
       <c r="C199" t="s">
-        <v>781</v>
+        <v>780</v>
+      </c>
+      <c r="E199">
+        <v>4</v>
       </c>
     </row>
     <row r="200" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2833</v>
+        <v>2832</v>
       </c>
       <c r="C200" t="s">
-        <v>1214</v>
+        <v>781</v>
       </c>
     </row>
     <row r="201" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2834</v>
+        <v>2833</v>
       </c>
       <c r="C201" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="202" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2841</v>
+        <v>2834</v>
       </c>
       <c r="C202" t="s">
-        <v>783</v>
-      </c>
-      <c r="E202">
-        <v>5</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="203" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2842</v>
+        <v>2841</v>
       </c>
       <c r="C203" t="s">
-        <v>782</v>
+        <v>783</v>
+      </c>
+      <c r="E203">
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2843</v>
+        <v>2842</v>
       </c>
       <c r="C204" t="s">
-        <v>1216</v>
-      </c>
-      <c r="L204" s="4">
-        <v>12</v>
-      </c>
-      <c r="N204">
-        <v>0.4</v>
+        <v>782</v>
       </c>
     </row>
     <row r="205" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2851</v>
+        <v>2843</v>
       </c>
       <c r="C205" t="s">
-        <v>784</v>
-      </c>
-      <c r="E205">
-        <v>6</v>
+        <v>1216</v>
+      </c>
+      <c r="L205" s="4">
+        <v>12</v>
+      </c>
+      <c r="N205">
+        <v>0.4</v>
       </c>
     </row>
     <row r="206" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2852</v>
+        <v>2851</v>
       </c>
       <c r="C206" t="s">
-        <v>790</v>
+        <v>784</v>
+      </c>
+      <c r="E206">
+        <v>6</v>
       </c>
     </row>
     <row r="207" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2853</v>
+        <v>2852</v>
       </c>
       <c r="C207" t="s">
-        <v>785</v>
+        <v>790</v>
       </c>
     </row>
     <row r="208" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B208">
-        <v>2861</v>
+        <v>2853</v>
       </c>
       <c r="C208" t="s">
-        <v>786</v>
-      </c>
-      <c r="E208">
-        <v>7</v>
+        <v>785</v>
       </c>
     </row>
     <row r="209" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B209">
-        <v>2862</v>
+        <v>2861</v>
       </c>
       <c r="C209" t="s">
-        <v>791</v>
+        <v>786</v>
+      </c>
+      <c r="E209">
+        <v>7</v>
       </c>
     </row>
     <row r="210" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B210">
-        <v>2863</v>
+        <v>2862</v>
       </c>
       <c r="C210" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="211" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B211">
-        <v>2864</v>
+        <v>2863</v>
       </c>
       <c r="C211" t="s">
-        <v>297</v>
+        <v>792</v>
       </c>
     </row>
     <row r="212" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B212">
-        <v>2871</v>
+        <v>2864</v>
       </c>
       <c r="C212" t="s">
-        <v>787</v>
-      </c>
-      <c r="E212">
-        <v>8</v>
+        <v>297</v>
       </c>
     </row>
     <row r="213" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B213">
-        <v>2872</v>
+        <v>2871</v>
       </c>
       <c r="C213" t="s">
-        <v>795</v>
+        <v>787</v>
+      </c>
+      <c r="E213">
+        <v>8</v>
       </c>
     </row>
     <row r="214" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B214">
-        <v>2873</v>
+        <v>2872</v>
       </c>
       <c r="C214" t="s">
-        <v>799</v>
+        <v>795</v>
       </c>
     </row>
     <row r="215" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B215">
-        <v>2881</v>
+        <v>2873</v>
       </c>
       <c r="C215" t="s">
-        <v>788</v>
-      </c>
-      <c r="E215">
-        <v>9</v>
+        <v>799</v>
       </c>
     </row>
     <row r="216" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B216">
-        <v>2882</v>
+        <v>2881</v>
       </c>
       <c r="C216" t="s">
-        <v>797</v>
+        <v>788</v>
+      </c>
+      <c r="E216">
+        <v>9</v>
       </c>
     </row>
     <row r="217" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B217">
-        <v>2883</v>
+        <v>2882</v>
       </c>
       <c r="C217" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
     </row>
     <row r="218" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B218">
-        <v>2891</v>
+        <v>2883</v>
       </c>
       <c r="C218" t="s">
-        <v>789</v>
-      </c>
-      <c r="E218">
-        <v>10</v>
+        <v>800</v>
       </c>
     </row>
     <row r="219" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B219">
+        <v>2891</v>
+      </c>
+      <c r="C219" t="s">
+        <v>789</v>
+      </c>
+      <c r="E219">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="220" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B220">
         <v>2892</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C220" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="221" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B221">
-        <v>2901</v>
-      </c>
-      <c r="C221" t="s">
-        <v>251</v>
-      </c>
-      <c r="D221" t="s">
-        <v>251</v>
-      </c>
-      <c r="W221" t="s">
-        <v>254</v>
-      </c>
-      <c r="Y221" t="s">
-        <v>1251</v>
       </c>
     </row>
     <row r="222" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B222">
-        <v>2902</v>
+        <v>2901</v>
       </c>
       <c r="C222" t="s">
-        <v>253</v>
-      </c>
-      <c r="E222">
-        <v>2</v>
+        <v>251</v>
+      </c>
+      <c r="D222" t="s">
+        <v>251</v>
       </c>
       <c r="W222" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Y222" t="s">
         <v>1251</v>
@@ -19717,16 +19723,16 @@
     </row>
     <row r="223" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B223">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="C223" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E223">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="W223" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Y223" t="s">
         <v>1251</v>
@@ -19734,27 +19740,30 @@
     </row>
     <row r="224" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B224">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="C224" t="s">
-        <v>1319</v>
-      </c>
-      <c r="U224">
-        <v>8</v>
+        <v>252</v>
+      </c>
+      <c r="E224">
+        <v>3</v>
       </c>
       <c r="W224" t="s">
-        <v>1321</v>
+        <v>256</v>
+      </c>
+      <c r="Y224" t="s">
+        <v>1251</v>
       </c>
     </row>
     <row r="225" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2905</v>
+        <v>2904</v>
       </c>
       <c r="C225" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="U225">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="W225" t="s">
         <v>1321</v>
@@ -19762,29 +19771,29 @@
     </row>
     <row r="226" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2911</v>
+        <v>2905</v>
       </c>
       <c r="C226" t="s">
-        <v>258</v>
-      </c>
-      <c r="D226" t="s">
-        <v>257</v>
-      </c>
-      <c r="H226" s="6"/>
-      <c r="L226" s="4">
-        <v>1</v>
-      </c>
-      <c r="Y226" t="s">
-        <v>1148</v>
+        <v>1320</v>
+      </c>
+      <c r="U226">
+        <v>24</v>
+      </c>
+      <c r="W226" t="s">
+        <v>1321</v>
       </c>
     </row>
     <row r="227" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2912</v>
+        <v>2911</v>
       </c>
       <c r="C227" t="s">
-        <v>259</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="D227" t="s">
+        <v>257</v>
+      </c>
+      <c r="H227" s="6"/>
       <c r="L227" s="4">
         <v>1</v>
       </c>
@@ -19794,10 +19803,13 @@
     </row>
     <row r="228" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2913</v>
+        <v>2912</v>
       </c>
       <c r="C228" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="L228" s="4">
+        <v>1</v>
       </c>
       <c r="Y228" t="s">
         <v>1148</v>
@@ -19805,24 +19817,21 @@
     </row>
     <row r="229" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2914</v>
+        <v>2913</v>
       </c>
       <c r="C229" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Y229" t="s">
-        <v>1252</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="230" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2915</v>
+        <v>2914</v>
       </c>
       <c r="C230" t="s">
-        <v>262</v>
-      </c>
-      <c r="L230" s="4">
-        <v>1</v>
+        <v>261</v>
       </c>
       <c r="Y230" t="s">
         <v>1252</v>
@@ -19830,21 +19839,24 @@
     </row>
     <row r="231" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2916</v>
+        <v>2915</v>
       </c>
       <c r="C231" t="s">
-        <v>288</v>
+        <v>262</v>
+      </c>
+      <c r="L231" s="4">
+        <v>1</v>
       </c>
       <c r="Y231" t="s">
-        <v>1148</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="232" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B232">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="C232" t="s">
-        <v>740</v>
+        <v>288</v>
       </c>
       <c r="Y232" t="s">
         <v>1148</v>
@@ -19852,33 +19864,24 @@
     </row>
     <row r="233" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B233">
-        <v>2918</v>
+        <v>2917</v>
       </c>
       <c r="C233" t="s">
-        <v>1069</v>
-      </c>
-      <c r="L233" s="4">
-        <v>1.5</v>
+        <v>740</v>
       </c>
       <c r="Y233" t="s">
-        <v>1252</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="234" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B234">
-        <v>2921</v>
+        <v>2918</v>
       </c>
       <c r="C234" t="s">
-        <v>264</v>
-      </c>
-      <c r="D234" t="s">
-        <v>263</v>
-      </c>
-      <c r="N234">
-        <v>0.04</v>
-      </c>
-      <c r="W234" t="s">
-        <v>268</v>
+        <v>1069</v>
+      </c>
+      <c r="L234" s="4">
+        <v>1.5</v>
       </c>
       <c r="Y234" t="s">
         <v>1252</v>
@@ -19886,181 +19889,184 @@
     </row>
     <row r="235" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B235">
-        <v>2922</v>
+        <v>2921</v>
       </c>
       <c r="C235" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="D235" t="s">
+        <v>263</v>
       </c>
       <c r="N235">
         <v>0.04</v>
       </c>
       <c r="W235" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="Y235" t="s">
-        <v>1263</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="236" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B236">
-        <v>2923</v>
+        <v>2922</v>
       </c>
       <c r="C236" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N236">
         <v>0.04</v>
       </c>
       <c r="W236" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="Y236" t="s">
-        <v>1163</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="237" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B237">
-        <v>2924</v>
+        <v>2923</v>
       </c>
       <c r="C237" t="s">
-        <v>289</v>
-      </c>
-      <c r="L237" s="4">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="N237">
-        <v>2.5</v>
-      </c>
-      <c r="Q237">
-        <v>6</v>
+        <v>0.04</v>
       </c>
       <c r="W237" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="Y237" t="s">
-        <v>1148</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="238" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B238">
-        <v>2925</v>
+        <v>2924</v>
       </c>
       <c r="C238" t="s">
-        <v>290</v>
+        <v>289</v>
+      </c>
+      <c r="L238" s="4">
+        <v>1</v>
+      </c>
+      <c r="N238">
+        <v>2.5</v>
+      </c>
+      <c r="Q238">
+        <v>6</v>
       </c>
       <c r="W238" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="Y238" t="s">
-        <v>1250</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="239" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B239">
-        <v>2926</v>
+        <v>2925</v>
       </c>
       <c r="C239" t="s">
-        <v>291</v>
-      </c>
-      <c r="E239">
-        <v>2</v>
-      </c>
-      <c r="L239" s="4">
-        <v>1</v>
-      </c>
-      <c r="N239">
-        <v>0.02</v>
+        <v>290</v>
       </c>
       <c r="W239" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="Y239" t="s">
-        <v>1245</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="240" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B240">
-        <v>2927</v>
+        <v>2926</v>
       </c>
       <c r="C240" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E240">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L240" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N240">
         <v>0.02</v>
       </c>
       <c r="W240" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="Y240" t="s">
-        <v>1253</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="241" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B241">
-        <v>2928</v>
+        <v>2927</v>
       </c>
       <c r="C241" t="s">
-        <v>1058</v>
+        <v>292</v>
+      </c>
+      <c r="E241">
+        <v>3</v>
+      </c>
+      <c r="L241" s="4">
+        <v>2</v>
+      </c>
+      <c r="N241">
+        <v>0.02</v>
       </c>
       <c r="W241" t="s">
-        <v>1061</v>
+        <v>295</v>
       </c>
       <c r="Y241" t="s">
-        <v>1254</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="242" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B242">
-        <v>2931</v>
+        <v>2928</v>
       </c>
       <c r="C242" t="s">
-        <v>238</v>
-      </c>
-      <c r="D242" t="s">
-        <v>277</v>
-      </c>
-      <c r="L242" s="4">
-        <v>2</v>
-      </c>
-      <c r="N242">
-        <v>2.5</v>
+        <v>1058</v>
       </c>
       <c r="W242" t="s">
-        <v>813</v>
+        <v>1061</v>
       </c>
       <c r="Y242" t="s">
-        <v>1148</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="243" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B243">
-        <v>2932</v>
+        <v>2931</v>
       </c>
       <c r="C243" t="s">
-        <v>278</v>
+        <v>238</v>
+      </c>
+      <c r="D243" t="s">
+        <v>277</v>
       </c>
       <c r="L243" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N243">
-        <v>2</v>
-      </c>
-      <c r="Q243">
-        <v>4</v>
+        <v>2.5</v>
+      </c>
+      <c r="W243" t="s">
+        <v>813</v>
+      </c>
+      <c r="Y243" t="s">
+        <v>1148</v>
       </c>
     </row>
     <row r="244" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B244">
-        <v>2933</v>
+        <v>2932</v>
       </c>
       <c r="C244" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="L244" s="4">
         <v>1</v>
@@ -20068,41 +20074,47 @@
       <c r="N244">
         <v>2</v>
       </c>
-      <c r="W244" t="s">
-        <v>813</v>
-      </c>
-      <c r="Y244" t="s">
-        <v>1148</v>
+      <c r="Q244">
+        <v>4</v>
       </c>
     </row>
     <row r="245" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B245">
-        <v>2941</v>
+        <v>2933</v>
       </c>
       <c r="C245" t="s">
-        <v>373</v>
+        <v>281</v>
+      </c>
+      <c r="L245" s="4">
+        <v>1</v>
+      </c>
+      <c r="N245">
+        <v>2</v>
+      </c>
+      <c r="W245" t="s">
+        <v>813</v>
       </c>
       <c r="Y245" t="s">
-        <v>1258</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="246" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B246">
-        <v>2942</v>
+        <v>2941</v>
       </c>
       <c r="C246" t="s">
-        <v>374</v>
-      </c>
-      <c r="E246">
-        <v>2</v>
+        <v>373</v>
+      </c>
+      <c r="Y246" t="s">
+        <v>1258</v>
       </c>
     </row>
     <row r="247" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B247">
-        <v>2943</v>
+        <v>2942</v>
       </c>
       <c r="C247" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E247">
         <v>2</v>
@@ -20110,38 +20122,38 @@
     </row>
     <row r="248" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B248">
-        <v>2944</v>
+        <v>2943</v>
       </c>
       <c r="C248" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E248">
         <v>2</v>
       </c>
-      <c r="L248" s="4">
-        <v>3</v>
-      </c>
-      <c r="N248">
-        <v>3.5</v>
-      </c>
     </row>
     <row r="249" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B249">
-        <v>2945</v>
+        <v>2944</v>
       </c>
       <c r="C249" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E249">
         <v>2</v>
       </c>
+      <c r="L249" s="4">
+        <v>3</v>
+      </c>
+      <c r="N249">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="250" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B250">
-        <v>2946</v>
+        <v>2945</v>
       </c>
       <c r="C250" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E250">
         <v>2</v>
@@ -20149,10 +20161,10 @@
     </row>
     <row r="251" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B251">
-        <v>2947</v>
+        <v>2946</v>
       </c>
       <c r="C251" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E251">
         <v>2</v>
@@ -20160,69 +20172,66 @@
     </row>
     <row r="252" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B252">
-        <v>2948</v>
+        <v>2947</v>
       </c>
       <c r="C252" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E252">
         <v>2</v>
       </c>
-      <c r="Y252" t="s">
-        <v>1255</v>
-      </c>
     </row>
     <row r="253" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B253">
-        <v>2961</v>
+        <v>2948</v>
       </c>
       <c r="C253" t="s">
-        <v>282</v>
-      </c>
-      <c r="D253" t="s">
-        <v>284</v>
+        <v>380</v>
+      </c>
+      <c r="E253">
+        <v>2</v>
       </c>
       <c r="Y253" t="s">
-        <v>1148</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="254" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B254">
-        <v>2962</v>
+        <v>2961</v>
       </c>
       <c r="C254" t="s">
-        <v>283</v>
+        <v>282</v>
+      </c>
+      <c r="D254" t="s">
+        <v>284</v>
       </c>
       <c r="Y254" t="s">
-        <v>1290</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="255" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B255">
-        <v>2963</v>
+        <v>2962</v>
       </c>
       <c r="C255" t="s">
-        <v>315</v>
-      </c>
-      <c r="L255" s="4">
-        <v>1</v>
-      </c>
-      <c r="N255">
-        <v>0.05</v>
+        <v>283</v>
       </c>
       <c r="Y255" t="s">
-        <v>1148</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="256" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B256">
-        <v>2964</v>
+        <v>2963</v>
       </c>
       <c r="C256" t="s">
-        <v>319</v>
+        <v>315</v>
+      </c>
+      <c r="L256" s="4">
+        <v>1</v>
       </c>
       <c r="N256">
-        <v>0.04</v>
+        <v>0.05</v>
       </c>
       <c r="Y256" t="s">
         <v>1148</v>
@@ -20230,16 +20239,13 @@
     </row>
     <row r="257" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B257">
-        <v>2965</v>
+        <v>2964</v>
       </c>
       <c r="C257" t="s">
-        <v>845</v>
-      </c>
-      <c r="L257" s="4">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="N257">
-        <v>0.05</v>
+        <v>0.04</v>
       </c>
       <c r="Y257" t="s">
         <v>1148</v>
@@ -20247,10 +20253,10 @@
     </row>
     <row r="258" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B258">
-        <v>2966</v>
+        <v>2965</v>
       </c>
       <c r="C258" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="L258" s="4">
         <v>1</v>
@@ -20264,10 +20270,10 @@
     </row>
     <row r="259" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B259">
-        <v>2967</v>
+        <v>2966</v>
       </c>
       <c r="C259" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="L259" s="4">
         <v>1</v>
@@ -20281,10 +20287,10 @@
     </row>
     <row r="260" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B260">
-        <v>2968</v>
+        <v>2967</v>
       </c>
       <c r="C260" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="L260" s="4">
         <v>1</v>
@@ -20298,50 +20304,50 @@
     </row>
     <row r="261" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B261">
-        <v>2969</v>
+        <v>2968</v>
       </c>
       <c r="C261" t="s">
-        <v>1118</v>
-      </c>
-      <c r="E261">
-        <v>2</v>
+        <v>848</v>
       </c>
       <c r="L261" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="S261">
-        <v>-1.4</v>
+        <v>1</v>
+      </c>
+      <c r="N261">
+        <v>0.05</v>
       </c>
       <c r="Y261" t="s">
-        <v>1291</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="262" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B262">
-        <v>2971</v>
+        <v>2969</v>
       </c>
       <c r="C262" t="s">
-        <v>309</v>
-      </c>
-      <c r="D262" t="s">
-        <v>304</v>
+        <v>1118</v>
+      </c>
+      <c r="E262">
+        <v>2</v>
+      </c>
+      <c r="L262" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="S262">
+        <v>-1.4</v>
       </c>
       <c r="Y262" t="s">
-        <v>1298</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="263" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B263">
-        <v>2972</v>
+        <v>2971</v>
       </c>
       <c r="C263" t="s">
-        <v>310</v>
-      </c>
-      <c r="L263" s="4">
-        <v>1</v>
-      </c>
-      <c r="N263">
-        <v>0.02</v>
+        <v>309</v>
+      </c>
+      <c r="D263" t="s">
+        <v>304</v>
       </c>
       <c r="Y263" t="s">
         <v>1298</v>
@@ -20349,10 +20355,10 @@
     </row>
     <row r="264" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B264">
-        <v>2973</v>
+        <v>2972</v>
       </c>
       <c r="C264" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="L264" s="4">
         <v>1</v>
@@ -20361,112 +20367,109 @@
         <v>0.02</v>
       </c>
       <c r="Y264" t="s">
-        <v>1295</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="265" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B265">
-        <v>2974</v>
+        <v>2973</v>
       </c>
       <c r="C265" t="s">
-        <v>308</v>
-      </c>
-      <c r="E265">
-        <v>2</v>
+        <v>318</v>
+      </c>
+      <c r="L265" s="4">
+        <v>1</v>
       </c>
       <c r="N265">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="Y265" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="266" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B266">
-        <v>2975</v>
+        <v>2974</v>
       </c>
       <c r="C266" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="E266">
         <v>2</v>
       </c>
-      <c r="L266" s="4">
-        <v>2</v>
-      </c>
       <c r="N266">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="Y266" t="s">
-        <v>1174</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="267" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B267">
-        <v>2976</v>
+        <v>2975</v>
       </c>
       <c r="C267" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="E267">
         <v>2</v>
       </c>
       <c r="L267" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N267">
+        <v>0.02</v>
       </c>
       <c r="Y267" t="s">
-        <v>1285</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="268" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B268">
-        <v>2977</v>
+        <v>2976</v>
       </c>
       <c r="C268" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E268">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L268" s="4">
-        <v>3</v>
-      </c>
-      <c r="N268">
-        <v>0.08</v>
-      </c>
-      <c r="Q268">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="Y268" t="s">
-        <v>1297</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="269" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B269">
-        <v>2978</v>
+        <v>2977</v>
       </c>
       <c r="C269" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E269">
         <v>3</v>
       </c>
       <c r="L269" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N269">
-        <v>0.1</v>
+        <v>0.08</v>
+      </c>
+      <c r="Q269">
+        <v>15</v>
       </c>
       <c r="Y269" t="s">
-        <v>1286</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="270" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B270">
-        <v>2979</v>
+        <v>2978</v>
       </c>
       <c r="C270" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E270">
         <v>3</v>
@@ -20475,38 +20478,41 @@
         <v>2</v>
       </c>
       <c r="N270">
-        <v>0.05</v>
-      </c>
-      <c r="Q270">
-        <v>5</v>
+        <v>0.1</v>
       </c>
       <c r="Y270" t="s">
-        <v>1298</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="271" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B271">
-        <v>2980</v>
+        <v>2979</v>
       </c>
       <c r="C271" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E271">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L271" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N271">
+        <v>0.05</v>
+      </c>
+      <c r="Q271">
+        <v>5</v>
       </c>
       <c r="Y271" t="s">
-        <v>1259</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="272" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B272">
-        <v>2981</v>
+        <v>2980</v>
       </c>
       <c r="C272" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="E272">
         <v>4</v>
@@ -20514,19 +20520,16 @@
       <c r="L272" s="4">
         <v>1</v>
       </c>
-      <c r="Q272">
-        <v>5</v>
-      </c>
       <c r="Y272" t="s">
         <v>1259</v>
       </c>
     </row>
     <row r="273" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B273">
-        <v>2982</v>
+        <v>2981</v>
       </c>
       <c r="C273" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E273">
         <v>4</v>
@@ -20534,53 +20537,62 @@
       <c r="L273" s="4">
         <v>1</v>
       </c>
+      <c r="Q273">
+        <v>5</v>
+      </c>
       <c r="Y273" t="s">
         <v>1259</v>
       </c>
     </row>
     <row r="274" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B274">
-        <v>2983</v>
+        <v>2982</v>
       </c>
       <c r="C274" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E274">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L274" s="4">
-        <v>5</v>
-      </c>
-      <c r="N274">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q274">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="Y274" t="s">
-        <v>1300</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="275" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B275">
-        <v>2984</v>
+        <v>2983</v>
       </c>
       <c r="C275" t="s">
-        <v>1081</v>
+        <v>314</v>
       </c>
       <c r="E275">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="L275" s="4">
+        <v>5</v>
+      </c>
+      <c r="N275">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q275">
+        <v>20</v>
       </c>
       <c r="Y275" t="s">
-        <v>1245</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="276" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B276">
-        <v>2985</v>
+        <v>2984</v>
       </c>
       <c r="C276" t="s">
-        <v>1082</v>
+        <v>1081</v>
+      </c>
+      <c r="E276">
+        <v>2</v>
       </c>
       <c r="Y276" t="s">
         <v>1245</v>
@@ -20588,10 +20600,10 @@
     </row>
     <row r="277" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B277">
-        <v>2986</v>
+        <v>2985</v>
       </c>
       <c r="C277" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="Y277" t="s">
         <v>1245</v>
@@ -20599,79 +20611,90 @@
     </row>
     <row r="278" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B278">
-        <v>2987</v>
+        <v>2986</v>
       </c>
       <c r="C278" t="s">
-        <v>1084</v>
-      </c>
-      <c r="E278">
-        <v>3</v>
-      </c>
-      <c r="L278" s="4">
-        <v>0.5</v>
+        <v>1083</v>
       </c>
       <c r="Y278" t="s">
-        <v>1259</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="279" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B279">
-        <v>2988</v>
+        <v>2987</v>
       </c>
       <c r="C279" t="s">
-        <v>1095</v>
+        <v>1084</v>
       </c>
       <c r="E279">
         <v>3</v>
       </c>
+      <c r="L279" s="4">
+        <v>0.5</v>
+      </c>
       <c r="Y279" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="280" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B280">
+        <v>2988</v>
+      </c>
+      <c r="C280" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E280">
+        <v>3</v>
+      </c>
+      <c r="Y280" t="s">
         <v>1256</v>
-      </c>
-    </row>
-    <row r="281" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B281">
-        <v>2991</v>
-      </c>
-      <c r="C281" t="s">
-        <v>1038</v>
-      </c>
-      <c r="D281" t="s">
-        <v>1039</v>
-      </c>
-      <c r="E281">
-        <v>1</v>
-      </c>
-      <c r="K281" s="4"/>
-      <c r="L281"/>
-      <c r="Y281" t="s">
-        <v>1162</v>
       </c>
     </row>
     <row r="282" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B282">
-        <v>2992</v>
+        <v>2991</v>
       </c>
       <c r="C282" t="s">
-        <v>1093</v>
+        <v>1038</v>
+      </c>
+      <c r="D282" t="s">
+        <v>1039</v>
       </c>
       <c r="E282">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K282" s="4"/>
       <c r="L282"/>
+      <c r="Y282" t="s">
+        <v>1162</v>
+      </c>
     </row>
     <row r="283" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B283">
-        <v>2993</v>
+        <v>2992</v>
       </c>
       <c r="C283" t="s">
-        <v>1176</v>
+        <v>1093</v>
       </c>
       <c r="E283">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K283" s="4"/>
       <c r="L283"/>
+    </row>
+    <row r="284" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B284">
+        <v>2993</v>
+      </c>
+      <c r="C284" t="s">
+        <v>1176</v>
+      </c>
+      <c r="E284">
+        <v>3</v>
+      </c>
+      <c r="K284" s="4"/>
+      <c r="L284"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22054,8 +22077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F47" activeCellId="1" sqref="F39 F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22532,6 +22555,9 @@
       <c r="D39" t="s">
         <v>1099</v>
       </c>
+      <c r="F39" t="s">
+        <v>1322</v>
+      </c>
       <c r="H39" t="s">
         <v>1260</v>
       </c>
@@ -22628,6 +22654,9 @@
       </c>
       <c r="D47" t="s">
         <v>1125</v>
+      </c>
+      <c r="F47" t="s">
+        <v>1322</v>
       </c>
       <c r="H47" t="s">
         <v>1299</v>

</xml_diff>

<commit_message>
v0.7.4k: Added terrain_resolution, fog_update_time to optionsForm
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0623C479-76D8-4822-8438-4D50DAEB272A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9F22B4-0295-4959-8FE4-1284DC4A9504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="7" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -16063,7 +16063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Y284"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="3" ySplit="2" topLeftCell="D39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -22077,8 +22077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F47" activeCellId="1" sqref="F39 F47"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.7.4n: Victory triggers in francis hall
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D752CD2-AF95-407D-8138-5D2A879E04D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D593813-400E-4072-AE50-5F6296D09E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="1326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="1327">
   <si>
     <t>ID</t>
   </si>
@@ -4476,6 +4476,9 @@
   </si>
   <si>
     <t>durability</t>
+  </si>
+  <si>
+    <t>+20% attack range</t>
   </si>
 </sst>
 </file>
@@ -12965,8 +12968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E95" sqref="E95"/>
+    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14691,8 +14694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15036,7 +15039,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>1.7</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -15062,7 +15065,7 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="M13">
         <v>3</v>
@@ -15297,7 +15300,7 @@
         <v>3</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -15329,7 +15332,7 @@
         <v>3</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -15361,7 +15364,7 @@
         <v>3</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -15390,7 +15393,7 @@
         <v>3</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="K31">
         <v>0</v>
@@ -15422,7 +15425,7 @@
         <v>3</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="K32">
         <v>0</v>
@@ -15437,7 +15440,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
         <v>1209</v>
       </c>
@@ -15454,7 +15457,7 @@
         <v>3</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="K33">
         <v>0</v>
@@ -15466,7 +15469,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
         <v>1210</v>
       </c>
@@ -15477,10 +15480,10 @@
         <v>10</v>
       </c>
       <c r="H34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -15495,7 +15498,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
         <v>1301</v>
       </c>
@@ -15511,8 +15514,23 @@
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>6</v>
+      </c>
+      <c r="I36">
+        <v>2.5</v>
+      </c>
+      <c r="J36">
+        <v>0.2</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>1302</v>
       </c>
@@ -15522,8 +15540,23 @@
       <c r="F37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H37">
+        <v>5</v>
+      </c>
+      <c r="I37">
+        <v>4</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
         <v>1303</v>
       </c>
@@ -15533,8 +15566,23 @@
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <v>12</v>
+      </c>
+      <c r="I38">
+        <v>3.5</v>
+      </c>
+      <c r="J38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
         <v>1304</v>
       </c>
@@ -15544,8 +15592,23 @@
       <c r="F39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <v>10</v>
+      </c>
+      <c r="I39">
+        <v>5</v>
+      </c>
+      <c r="J39">
+        <v>0.4</v>
+      </c>
+      <c r="K39">
+        <v>0.05</v>
+      </c>
+      <c r="L39">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
         <v>1305</v>
       </c>
@@ -15555,8 +15618,23 @@
       <c r="F40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H40">
+        <v>9</v>
+      </c>
+      <c r="I40">
+        <v>7</v>
+      </c>
+      <c r="J40">
+        <v>0.4</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
         <v>1306</v>
       </c>
@@ -15566,8 +15644,23 @@
       <c r="F41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <v>15</v>
+      </c>
+      <c r="I41">
+        <v>8</v>
+      </c>
+      <c r="J41">
+        <v>0.4</v>
+      </c>
+      <c r="K41">
+        <v>0.12</v>
+      </c>
+      <c r="L41">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
         <v>1307</v>
       </c>
@@ -15577,8 +15670,23 @@
       <c r="F42">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="H42">
+        <v>25</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K42">
+        <v>0.03</v>
+      </c>
+      <c r="L42">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
         <v>1308</v>
       </c>
@@ -15587,6 +15695,24 @@
       </c>
       <c r="F43">
         <v>8</v>
+      </c>
+      <c r="H43">
+        <v>18</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <v>0.8</v>
+      </c>
+      <c r="K43">
+        <v>0.15</v>
+      </c>
+      <c r="L43">
+        <v>1.4</v>
+      </c>
+      <c r="R43" s="8" t="s">
+        <v>1326</v>
       </c>
     </row>
   </sheetData>
@@ -16084,10 +16210,10 @@
   <dimension ref="A1:Z284"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="G204" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U166" sqref="U166"/>
+      <selection pane="bottomRight" activeCell="U234" sqref="U234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19995,7 +20121,10 @@
       </c>
       <c r="H227" s="6"/>
       <c r="L227" s="4">
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+      <c r="U227">
+        <v>6</v>
       </c>
       <c r="Z227" t="s">
         <v>1147</v>
@@ -20009,7 +20138,10 @@
         <v>259</v>
       </c>
       <c r="L228" s="4">
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+      <c r="U228">
+        <v>6</v>
       </c>
       <c r="Z228" t="s">
         <v>1147</v>
@@ -20045,7 +20177,10 @@
         <v>262</v>
       </c>
       <c r="L231" s="4">
-        <v>1</v>
+        <v>0.6</v>
+      </c>
+      <c r="U231">
+        <v>15</v>
       </c>
       <c r="Z231" t="s">
         <v>1251</v>
@@ -20083,6 +20218,9 @@
       <c r="L234" s="4">
         <v>1.5</v>
       </c>
+      <c r="U234">
+        <v>12</v>
+      </c>
       <c r="Z234" t="s">
         <v>1251</v>
       </c>
@@ -20149,13 +20287,16 @@
         <v>289</v>
       </c>
       <c r="L238" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N238">
         <v>2.5</v>
       </c>
       <c r="Q238">
         <v>6</v>
+      </c>
+      <c r="U238">
+        <v>2</v>
       </c>
       <c r="X238" t="s">
         <v>296</v>
@@ -20433,6 +20574,9 @@
       <c r="N256">
         <v>0.05</v>
       </c>
+      <c r="U256">
+        <v>8</v>
+      </c>
       <c r="Z256" t="s">
         <v>1147</v>
       </c>
@@ -20464,6 +20608,9 @@
       <c r="N258">
         <v>0.05</v>
       </c>
+      <c r="U258">
+        <v>8</v>
+      </c>
       <c r="Z258" t="s">
         <v>1147</v>
       </c>
@@ -20481,6 +20628,9 @@
       <c r="N259">
         <v>0.05</v>
       </c>
+      <c r="U259">
+        <v>8</v>
+      </c>
       <c r="Z259" t="s">
         <v>1147</v>
       </c>
@@ -20498,6 +20648,9 @@
       <c r="N260">
         <v>0.05</v>
       </c>
+      <c r="U260">
+        <v>8</v>
+      </c>
       <c r="Z260" t="s">
         <v>1147</v>
       </c>
@@ -20515,6 +20668,9 @@
       <c r="N261">
         <v>0.05</v>
       </c>
+      <c r="U261">
+        <v>8</v>
+      </c>
       <c r="Z261" t="s">
         <v>1147</v>
       </c>
@@ -20535,6 +20691,9 @@
       <c r="S262">
         <v>-1.4</v>
       </c>
+      <c r="U262">
+        <v>18</v>
+      </c>
       <c r="Z262" t="s">
         <v>1290</v>
       </c>
@@ -20549,6 +20708,9 @@
       <c r="D263" t="s">
         <v>304</v>
       </c>
+      <c r="U263">
+        <v>100</v>
+      </c>
       <c r="Z263" t="s">
         <v>1297</v>
       </c>
@@ -20566,6 +20728,9 @@
       <c r="N264">
         <v>0.02</v>
       </c>
+      <c r="U264">
+        <v>100</v>
+      </c>
       <c r="Z264" t="s">
         <v>1297</v>
       </c>
@@ -20583,6 +20748,9 @@
       <c r="N265">
         <v>0.02</v>
       </c>
+      <c r="U265">
+        <v>100</v>
+      </c>
       <c r="Z265" t="s">
         <v>1294</v>
       </c>
@@ -20600,6 +20768,9 @@
       <c r="N266">
         <v>0.05</v>
       </c>
+      <c r="U266">
+        <v>100</v>
+      </c>
       <c r="Z266" t="s">
         <v>1297</v>
       </c>
@@ -20620,6 +20791,9 @@
       <c r="N267">
         <v>0.02</v>
       </c>
+      <c r="U267">
+        <v>100</v>
+      </c>
       <c r="Z267" t="s">
         <v>1173</v>
       </c>
@@ -20637,6 +20811,9 @@
       <c r="L268" s="4">
         <v>1</v>
       </c>
+      <c r="U268">
+        <v>100</v>
+      </c>
       <c r="Z268" t="s">
         <v>1284</v>
       </c>
@@ -20660,6 +20837,9 @@
       <c r="Q269">
         <v>15</v>
       </c>
+      <c r="U269">
+        <v>100</v>
+      </c>
       <c r="Z269" t="s">
         <v>1296</v>
       </c>
@@ -20680,6 +20860,9 @@
       <c r="N270">
         <v>0.1</v>
       </c>
+      <c r="U270">
+        <v>100</v>
+      </c>
       <c r="Z270" t="s">
         <v>1285</v>
       </c>
@@ -20703,6 +20886,9 @@
       <c r="Q271">
         <v>5</v>
       </c>
+      <c r="U271">
+        <v>100</v>
+      </c>
       <c r="Z271" t="s">
         <v>1297</v>
       </c>
@@ -20720,6 +20906,9 @@
       <c r="L272" s="4">
         <v>1</v>
       </c>
+      <c r="U272">
+        <v>100</v>
+      </c>
       <c r="Z272" t="s">
         <v>1258</v>
       </c>
@@ -20740,6 +20929,9 @@
       <c r="Q273">
         <v>5</v>
       </c>
+      <c r="U273">
+        <v>100</v>
+      </c>
       <c r="Z273" t="s">
         <v>1258</v>
       </c>
@@ -20757,6 +20949,9 @@
       <c r="L274" s="4">
         <v>1</v>
       </c>
+      <c r="U274">
+        <v>100</v>
+      </c>
       <c r="Z274" t="s">
         <v>1258</v>
       </c>
@@ -20780,6 +20975,9 @@
       <c r="Q275">
         <v>20</v>
       </c>
+      <c r="U275">
+        <v>100</v>
+      </c>
       <c r="Z275" t="s">
         <v>1299</v>
       </c>
@@ -20793,6 +20991,9 @@
       </c>
       <c r="E276">
         <v>2</v>
+      </c>
+      <c r="U276">
+        <v>100</v>
       </c>
       <c r="Z276" t="s">
         <v>1244</v>

</xml_diff>

<commit_message>
v0.7.4o: Fischer takes Ben's eyes
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D593813-400E-4072-AE50-5F6296D09E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684DBD04-396E-4E87-A8BC-048CDD0493E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="1327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1758" uniqueCount="1328">
   <si>
     <t>ID</t>
   </si>
@@ -4479,6 +4479,9 @@
   </si>
   <si>
     <t>+20% attack range</t>
+  </si>
+  <si>
+    <t>Ben's Eyes</t>
   </si>
 </sst>
 </file>
@@ -14694,8 +14697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R44" sqref="R44"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16207,13 +16210,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Z284"/>
+  <dimension ref="A1:Z291"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="G204" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D264" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U234" sqref="U234"/>
+      <selection pane="bottomRight" activeCell="G289" sqref="G289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20992,9 +20995,6 @@
       <c r="E276">
         <v>2</v>
       </c>
-      <c r="U276">
-        <v>100</v>
-      </c>
       <c r="Z276" t="s">
         <v>1244</v>
       </c>
@@ -21096,6 +21096,65 @@
       </c>
       <c r="K284" s="4"/>
       <c r="L284"/>
+    </row>
+    <row r="285" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B285">
+        <v>2994</v>
+      </c>
+      <c r="E285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B286">
+        <v>2995</v>
+      </c>
+      <c r="E286">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="287" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B287">
+        <v>2996</v>
+      </c>
+      <c r="E287">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="288" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B288">
+        <v>2997</v>
+      </c>
+      <c r="E288">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B289">
+        <v>2998</v>
+      </c>
+      <c r="E289">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="290" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B290">
+        <v>2999</v>
+      </c>
+      <c r="C290" t="s">
+        <v>1327</v>
+      </c>
+      <c r="E290">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B291">
+        <v>3000</v>
+      </c>
+      <c r="E291">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -22479,7 +22538,7 @@
   <dimension ref="B2:H129"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.7.4q: Francis Hall KhalilForm/Quizmo
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684DBD04-396E-4E87-A8BC-048CDD0493E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F1592D0-0592-4F7D-AB68-A079FAE883C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -4292,9 +4292,6 @@
     <t>other half of ground floor</t>
   </si>
   <si>
-    <t>candlestick, holy water</t>
-  </si>
-  <si>
     <t>M1911, ammo</t>
   </si>
   <si>
@@ -4482,6 +4479,9 @@
   </si>
   <si>
     <t>Ben's Eyes</t>
+  </si>
+  <si>
+    <t>candlestick, holy water, chuck quimo through window</t>
   </si>
 </sst>
 </file>
@@ -12971,7 +12971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H148"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
@@ -15181,7 +15181,7 @@
         <v>1131</v>
       </c>
       <c r="C23" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="E23" t="s">
         <v>455</v>
@@ -15715,7 +15715,7 @@
         <v>1.4</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
     </row>
   </sheetData>
@@ -16213,10 +16213,10 @@
   <dimension ref="A1:Z291"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D264" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D174" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G289" sqref="G289"/>
+      <selection pane="bottomRight" activeCell="C227" sqref="C227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16317,10 +16317,10 @@
         <v>325</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>9</v>
@@ -16865,7 +16865,7 @@
         <v>10</v>
       </c>
       <c r="Z34" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="35" spans="2:26" x14ac:dyDescent="0.25">
@@ -17363,7 +17363,7 @@
         <v>2223</v>
       </c>
       <c r="C65" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E65">
         <v>3</v>
@@ -19649,7 +19649,7 @@
         <v>298</v>
       </c>
       <c r="Z181" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="182" spans="2:26" x14ac:dyDescent="0.25">
@@ -20089,13 +20089,13 @@
         <v>2904</v>
       </c>
       <c r="C225" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="V225">
         <v>8</v>
       </c>
       <c r="X225" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="226" spans="2:26" x14ac:dyDescent="0.25">
@@ -20103,13 +20103,13 @@
         <v>2905</v>
       </c>
       <c r="C226" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="V226">
         <v>24</v>
       </c>
       <c r="X226" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="227" spans="2:26" x14ac:dyDescent="0.25">
@@ -20561,7 +20561,7 @@
         <v>283</v>
       </c>
       <c r="Z255" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="256" spans="2:26" x14ac:dyDescent="0.25">
@@ -20698,7 +20698,7 @@
         <v>18</v>
       </c>
       <c r="Z262" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="263" spans="2:26" x14ac:dyDescent="0.25">
@@ -20715,7 +20715,7 @@
         <v>100</v>
       </c>
       <c r="Z263" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="264" spans="2:26" x14ac:dyDescent="0.25">
@@ -20735,7 +20735,7 @@
         <v>100</v>
       </c>
       <c r="Z264" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="265" spans="2:26" x14ac:dyDescent="0.25">
@@ -20755,7 +20755,7 @@
         <v>100</v>
       </c>
       <c r="Z265" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="266" spans="2:26" x14ac:dyDescent="0.25">
@@ -20775,7 +20775,7 @@
         <v>100</v>
       </c>
       <c r="Z266" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="267" spans="2:26" x14ac:dyDescent="0.25">
@@ -20818,7 +20818,7 @@
         <v>100</v>
       </c>
       <c r="Z268" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="269" spans="2:26" x14ac:dyDescent="0.25">
@@ -20844,7 +20844,7 @@
         <v>100</v>
       </c>
       <c r="Z269" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="270" spans="2:26" x14ac:dyDescent="0.25">
@@ -20867,7 +20867,7 @@
         <v>100</v>
       </c>
       <c r="Z270" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="271" spans="2:26" x14ac:dyDescent="0.25">
@@ -20893,7 +20893,7 @@
         <v>100</v>
       </c>
       <c r="Z271" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="272" spans="2:26" x14ac:dyDescent="0.25">
@@ -20982,7 +20982,7 @@
         <v>100</v>
       </c>
       <c r="Z275" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="276" spans="2:26" x14ac:dyDescent="0.25">
@@ -21142,7 +21142,7 @@
         <v>2999</v>
       </c>
       <c r="C290" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="E290">
         <v>9</v>
@@ -22537,8 +22537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22669,7 +22669,7 @@
         <v>1078</v>
       </c>
       <c r="F11" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="H11" t="s">
         <v>1153</v>
@@ -22683,10 +22683,10 @@
         <v>1155</v>
       </c>
       <c r="F12" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="H12" t="s">
-        <v>1266</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -22697,10 +22697,10 @@
         <v>1156</v>
       </c>
       <c r="F13" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="H13" t="s">
-        <v>1271</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -22711,10 +22711,10 @@
         <v>1154</v>
       </c>
       <c r="F14" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="H14" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -22725,10 +22725,10 @@
         <v>1109</v>
       </c>
       <c r="F15" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="H15" t="s">
-        <v>1272</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -22742,7 +22742,7 @@
         <v>1166</v>
       </c>
       <c r="H16" t="s">
-        <v>1276</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -22756,7 +22756,7 @@
         <v>1158</v>
       </c>
       <c r="H17" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -22772,10 +22772,10 @@
         <v>1096</v>
       </c>
       <c r="F19" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H19" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -22786,10 +22786,10 @@
         <v>1104</v>
       </c>
       <c r="F20" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="H20" t="s">
-        <v>1264</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -22800,10 +22800,10 @@
         <v>1106</v>
       </c>
       <c r="F21" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="H21" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -22814,10 +22814,10 @@
         <v>1105</v>
       </c>
       <c r="F22" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="H22" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -22828,10 +22828,10 @@
         <v>1110</v>
       </c>
       <c r="F23" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H23" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -22845,7 +22845,7 @@
         <v>1157</v>
       </c>
       <c r="H24" t="s">
-        <v>1268</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -22856,10 +22856,10 @@
         <v>1112</v>
       </c>
       <c r="F25" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="H25" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -22870,10 +22870,10 @@
         <v>1113</v>
       </c>
       <c r="F26" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H26" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -22884,10 +22884,10 @@
         <v>1114</v>
       </c>
       <c r="F27" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="H27" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -22898,7 +22898,7 @@
         <v>1115</v>
       </c>
       <c r="F28" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="H28" t="s">
         <v>1165</v>
@@ -22912,10 +22912,10 @@
         <v>1097</v>
       </c>
       <c r="F29" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H29" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -22926,10 +22926,10 @@
         <v>1118</v>
       </c>
       <c r="F30" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="H30" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -22940,7 +22940,7 @@
         <v>1119</v>
       </c>
       <c r="F31" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="H31" t="s">
         <v>1170</v>
@@ -22954,10 +22954,10 @@
         <v>1120</v>
       </c>
       <c r="F32" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="H32" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -22968,10 +22968,10 @@
         <v>1123</v>
       </c>
       <c r="F33" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="H33" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
@@ -22982,7 +22982,7 @@
         <v>1121</v>
       </c>
       <c r="F34" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="H34" t="s">
         <v>1260</v>
@@ -23016,7 +23016,7 @@
         <v>1098</v>
       </c>
       <c r="F39" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H39" t="s">
         <v>1259</v>
@@ -23038,7 +23038,7 @@
         <v>1157</v>
       </c>
       <c r="H41" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -23052,7 +23052,7 @@
         <v>1171</v>
       </c>
       <c r="H42" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
@@ -23074,10 +23074,10 @@
         <v>1107</v>
       </c>
       <c r="F44" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="H44" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
@@ -23088,7 +23088,7 @@
         <v>1108</v>
       </c>
       <c r="F45" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="H45" t="s">
         <v>1174</v>
@@ -23116,10 +23116,10 @@
         <v>1124</v>
       </c>
       <c r="F47" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H47" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -23130,7 +23130,7 @@
         <v>1125</v>
       </c>
       <c r="F48" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="H48" t="s">
         <v>1263</v>
@@ -23144,7 +23144,7 @@
         <v>1126</v>
       </c>
       <c r="H49" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.4u: Finished all key placements
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8479F7A1-ABE7-4A4E-923C-BD7883877872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAC1D9E-8DE1-4BC2-9382-672C20F6463E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="9" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="7" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="1329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="1331">
   <si>
     <t>ID</t>
   </si>
@@ -4448,9 +4448,6 @@
     <t>g floor guest bathroom</t>
   </si>
   <si>
-    <t>.45 ACP, 28 gauge, key (39)</t>
-  </si>
-  <si>
     <t>Small Key Ring</t>
   </si>
   <si>
@@ -4485,6 +4482,15 @@
   </si>
   <si>
     <t>quizmo XP</t>
+  </si>
+  <si>
+    <t>.45 ACP, 28 gauge</t>
+  </si>
+  <si>
+    <t>powerful zombie on first floor lobby</t>
+  </si>
+  <si>
+    <t>g floor mechanical side room</t>
   </si>
 </sst>
 </file>
@@ -5664,7 +5670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A114E18-4580-4CF1-BE70-B14A03AAF800}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -5735,7 +5741,7 @@
         <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>811</v>
@@ -15234,7 +15240,7 @@
         <v>1131</v>
       </c>
       <c r="C23" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="E23" t="s">
         <v>455</v>
@@ -15768,7 +15774,7 @@
         <v>1.4</v>
       </c>
       <c r="R43" s="8" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
     </row>
   </sheetData>
@@ -16370,10 +16376,10 @@
         <v>325</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="X2" s="1" t="s">
         <v>9</v>
@@ -17416,7 +17422,7 @@
         <v>2223</v>
       </c>
       <c r="C65" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="E65">
         <v>3</v>
@@ -20142,13 +20148,13 @@
         <v>2904</v>
       </c>
       <c r="C225" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="V225">
         <v>8</v>
       </c>
       <c r="X225" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="226" spans="2:26" x14ac:dyDescent="0.25">
@@ -20156,13 +20162,13 @@
         <v>2905</v>
       </c>
       <c r="C226" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="V226">
         <v>24</v>
       </c>
       <c r="X226" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="227" spans="2:26" x14ac:dyDescent="0.25">
@@ -21195,7 +21201,7 @@
         <v>2999</v>
       </c>
       <c r="C290" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="E290">
         <v>9</v>
@@ -22590,8 +22596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22842,7 +22848,7 @@
         <v>1315</v>
       </c>
       <c r="H20" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -22926,7 +22932,7 @@
         <v>1312</v>
       </c>
       <c r="H26" t="s">
-        <v>1316</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -23069,7 +23075,7 @@
         <v>1098</v>
       </c>
       <c r="F39" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H39" t="s">
         <v>1259</v>
@@ -23115,6 +23121,9 @@
       <c r="D43" t="s">
         <v>1101</v>
       </c>
+      <c r="F43" t="s">
+        <v>1330</v>
+      </c>
       <c r="H43" t="s">
         <v>20</v>
       </c>
@@ -23169,7 +23178,7 @@
         <v>1124</v>
       </c>
       <c r="F47" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H47" t="s">
         <v>1297</v>
@@ -23195,6 +23204,9 @@
       </c>
       <c r="D49" t="s">
         <v>1126</v>
+      </c>
+      <c r="F49" t="s">
+        <v>1329</v>
       </c>
       <c r="H49" t="s">
         <v>1264</v>

</xml_diff>

<commit_message>
v0.7.4x: Item durability in crafting
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAC1D9E-8DE1-4BC2-9382-672C20F6463E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0550AC53-5691-4764-B1F5-EB9A2366A16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="7" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -16271,11 +16271,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Z291"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D204" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D249" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C222" sqref="C222"/>
+      <selection pane="bottomRight" activeCell="F278" sqref="F278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21075,6 +21075,9 @@
       </c>
       <c r="C278" t="s">
         <v>1082</v>
+      </c>
+      <c r="E278">
+        <v>2</v>
       </c>
       <c r="Z278" t="s">
         <v>1244</v>
@@ -22596,7 +22599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v0.7.4z: PlayerInventory drop single items
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0550AC53-5691-4764-B1F5-EB9A2366A16C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831DFCC9-3E53-40D0-A735-19A6B15A3A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="1334">
   <si>
     <t>ID</t>
   </si>
@@ -4491,6 +4491,15 @@
   </si>
   <si>
     <t>g floor mechanical side room</t>
+  </si>
+  <si>
+    <t>Longbow</t>
+  </si>
+  <si>
+    <t>Compound Bow</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
   </si>
 </sst>
 </file>
@@ -16269,13 +16278,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
-  <dimension ref="A1:Z291"/>
+  <dimension ref="A1:Z294"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D249" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D63" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F278" sqref="F278"/>
+      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17880,1627 +17889,1594 @@
     </row>
     <row r="87" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B87">
-        <v>2331</v>
+        <v>2324</v>
       </c>
       <c r="C87" t="s">
-        <v>163</v>
+        <v>1331</v>
       </c>
       <c r="D87" s="15"/>
       <c r="E87">
-        <v>4</v>
-      </c>
-      <c r="L87"/>
-      <c r="M87" s="4">
-        <v>1000</v>
-      </c>
-      <c r="O87">
-        <v>12</v>
-      </c>
-      <c r="R87">
-        <v>5</v>
-      </c>
-      <c r="W87">
-        <v>6</v>
-      </c>
-      <c r="X87" t="s">
-        <v>849</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B88">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="C88" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="D88" s="15"/>
       <c r="E88">
         <v>4</v>
       </c>
-      <c r="L88" s="4" t="s">
-        <v>334</v>
-      </c>
-      <c r="N88">
-        <v>10</v>
-      </c>
-      <c r="Q88">
-        <v>15</v>
-      </c>
-      <c r="V88">
-        <v>20</v>
+      <c r="L88"/>
+      <c r="M88" s="4">
+        <v>1000</v>
+      </c>
+      <c r="O88">
+        <v>12</v>
+      </c>
+      <c r="R88">
+        <v>5</v>
+      </c>
+      <c r="W88">
+        <v>6</v>
       </c>
       <c r="X88" t="s">
-        <v>350</v>
+        <v>849</v>
       </c>
     </row>
     <row r="89" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B89">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="C89" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D89" s="15"/>
       <c r="E89">
         <v>4</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="N89">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q89">
         <v>15</v>
       </c>
       <c r="V89">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="X89" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="90" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B90">
-        <v>2341</v>
+        <v>2333</v>
       </c>
       <c r="C90" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
       <c r="D90" s="15"/>
       <c r="E90">
-        <v>5</v>
-      </c>
-      <c r="L90" s="4">
-        <v>600</v>
+        <v>4</v>
+      </c>
+      <c r="L90" s="4" t="s">
+        <v>327</v>
       </c>
       <c r="N90">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="Q90">
+        <v>15</v>
+      </c>
+      <c r="V90">
         <v>6</v>
       </c>
-      <c r="S90">
-        <v>-1</v>
-      </c>
-      <c r="V90">
-        <v>1</v>
-      </c>
       <c r="X90" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="91" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B91">
-        <v>2342</v>
+        <v>2334</v>
       </c>
       <c r="C91" t="s">
-        <v>145</v>
+        <v>1332</v>
       </c>
       <c r="D91" s="15"/>
       <c r="E91">
-        <v>5</v>
-      </c>
-      <c r="L91" s="4">
-        <v>600</v>
-      </c>
-      <c r="N91">
-        <v>12</v>
-      </c>
-      <c r="Q91">
-        <v>15</v>
-      </c>
-      <c r="V91">
-        <v>6</v>
-      </c>
-      <c r="X91" t="s">
-        <v>354</v>
+        <v>4</v>
       </c>
     </row>
     <row r="92" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B92">
-        <v>2343</v>
+        <v>2341</v>
       </c>
       <c r="C92" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D92" s="15"/>
       <c r="E92">
         <v>5</v>
       </c>
-      <c r="L92" s="4" t="s">
-        <v>338</v>
+      <c r="L92" s="4">
+        <v>600</v>
       </c>
       <c r="N92">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q92">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="S92">
+        <v>-1</v>
       </c>
       <c r="V92">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="X92" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
     </row>
     <row r="93" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B93">
-        <v>2344</v>
+        <v>2342</v>
       </c>
       <c r="C93" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="D93" s="15"/>
       <c r="E93">
         <v>5</v>
       </c>
-      <c r="L93" s="4" t="s">
-        <v>340</v>
+      <c r="L93" s="4">
+        <v>600</v>
       </c>
       <c r="N93">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="Q93">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="V93">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="X93" t="s">
-        <v>368</v>
+        <v>354</v>
       </c>
     </row>
     <row r="94" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B94">
-        <v>2345</v>
+        <v>2343</v>
       </c>
       <c r="C94" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D94" s="15"/>
       <c r="E94">
         <v>5</v>
       </c>
       <c r="L94" s="4" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="N94">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q94">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="V94">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="X94" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="95" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B95">
-        <v>2351</v>
+        <v>2344</v>
       </c>
       <c r="C95" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="D95" s="15"/>
       <c r="E95">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="N95">
         <v>10</v>
       </c>
       <c r="Q95">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="V95">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="X95" t="s">
-        <v>349</v>
+        <v>368</v>
       </c>
     </row>
     <row r="96" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B96">
-        <v>2352</v>
+        <v>2345</v>
       </c>
       <c r="C96" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D96" s="15"/>
       <c r="E96">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L96" s="4" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="N96">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="Q96">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="V96">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="X96" t="s">
-        <v>355</v>
+        <v>365</v>
       </c>
     </row>
     <row r="97" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B97">
-        <v>2353</v>
+        <v>2346</v>
       </c>
       <c r="C97" t="s">
-        <v>154</v>
+        <v>1333</v>
       </c>
       <c r="D97" s="15"/>
       <c r="E97">
-        <v>6</v>
-      </c>
-      <c r="L97" s="4">
-        <v>500</v>
-      </c>
-      <c r="N97">
-        <v>7</v>
-      </c>
-      <c r="Q97">
-        <v>25</v>
-      </c>
-      <c r="S97">
-        <v>1</v>
-      </c>
-      <c r="T97">
-        <v>0.1</v>
-      </c>
-      <c r="V97">
-        <v>1</v>
-      </c>
-      <c r="X97" t="s">
-        <v>362</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B98">
-        <v>2354</v>
+        <v>2351</v>
       </c>
       <c r="C98" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D98" s="15"/>
       <c r="E98">
         <v>6</v>
       </c>
       <c r="L98" s="4" t="s">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="N98">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="Q98">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V98">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="X98" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="99" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B99">
-        <v>2355</v>
+        <v>2352</v>
       </c>
       <c r="C99" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="D99" s="15"/>
       <c r="E99">
         <v>6</v>
       </c>
       <c r="L99" s="4" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="N99">
         <v>11</v>
       </c>
       <c r="Q99">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="V99">
         <v>30</v>
       </c>
       <c r="X99" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="100" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B100">
-        <v>2361</v>
+        <v>2353</v>
       </c>
       <c r="C100" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="D100" s="15"/>
       <c r="E100">
+        <v>6</v>
+      </c>
+      <c r="L100" s="4">
+        <v>500</v>
+      </c>
+      <c r="N100">
         <v>7</v>
       </c>
-      <c r="L100" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="N100">
-        <v>11</v>
-      </c>
       <c r="Q100">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="S100">
+        <v>1</v>
+      </c>
+      <c r="T100">
+        <v>0.1</v>
       </c>
       <c r="V100">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="X100" t="s">
-        <v>345</v>
+        <v>362</v>
       </c>
     </row>
     <row r="101" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B101">
-        <v>2362</v>
+        <v>2354</v>
       </c>
       <c r="C101" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c r="D101" s="15"/>
       <c r="E101">
+        <v>6</v>
+      </c>
+      <c r="L101" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="N101">
         <v>7</v>
       </c>
-      <c r="L101" s="4">
-        <v>1200</v>
-      </c>
-      <c r="N101">
+      <c r="Q101">
+        <v>15</v>
+      </c>
+      <c r="V101">
         <v>12</v>
       </c>
-      <c r="Q101">
-        <v>8</v>
-      </c>
-      <c r="V101">
-        <v>8</v>
-      </c>
       <c r="X101" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="102" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B102">
-        <v>2363</v>
+        <v>2355</v>
       </c>
       <c r="C102" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D102" s="15"/>
       <c r="E102">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L102" s="4" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="N102">
+        <v>11</v>
+      </c>
+      <c r="Q102">
         <v>16</v>
       </c>
-      <c r="Q102">
+      <c r="V102">
         <v>30</v>
       </c>
-      <c r="S102">
-        <v>-1</v>
-      </c>
-      <c r="V102">
-        <v>4</v>
-      </c>
       <c r="X102" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
     </row>
     <row r="103" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B103">
-        <v>2364</v>
+        <v>2361</v>
       </c>
       <c r="C103" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D103" s="15"/>
       <c r="E103">
         <v>7</v>
       </c>
       <c r="L103" s="4" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="N103">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="Q103">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="V103">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="X103" t="s">
-        <v>365</v>
+        <v>345</v>
       </c>
     </row>
     <row r="104" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B104">
-        <v>2371</v>
+        <v>2362</v>
       </c>
       <c r="C104" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D104" s="15"/>
       <c r="E104">
+        <v>7</v>
+      </c>
+      <c r="L104" s="4">
+        <v>1200</v>
+      </c>
+      <c r="N104">
+        <v>12</v>
+      </c>
+      <c r="Q104">
         <v>8</v>
       </c>
-      <c r="L104" s="4" t="s">
-        <v>330</v>
-      </c>
-      <c r="N104">
-        <v>10</v>
-      </c>
-      <c r="Q104">
-        <v>20</v>
-      </c>
       <c r="V104">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="X104" t="s">
-        <v>1031</v>
+        <v>352</v>
       </c>
     </row>
     <row r="105" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B105">
-        <v>2372</v>
+        <v>2363</v>
       </c>
       <c r="C105" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="D105" s="15"/>
       <c r="E105">
-        <v>8</v>
-      </c>
-      <c r="L105" s="4">
-        <v>500</v>
-      </c>
-      <c r="M105">
-        <v>500</v>
+        <v>7</v>
+      </c>
+      <c r="L105" s="4" t="s">
+        <v>336</v>
       </c>
       <c r="N105">
-        <v>9</v>
-      </c>
-      <c r="R105">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="Q105">
+        <v>30</v>
+      </c>
+      <c r="S105">
+        <v>-1</v>
       </c>
       <c r="V105">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="X105" t="s">
-        <v>347</v>
+        <v>359</v>
       </c>
     </row>
     <row r="106" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B106">
-        <v>2373</v>
+        <v>2364</v>
       </c>
       <c r="C106" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D106" s="15"/>
       <c r="E106">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L106" s="4" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="N106">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="Q106">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="V106">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="X106" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
     </row>
     <row r="107" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B107">
-        <v>2374</v>
+        <v>2371</v>
       </c>
       <c r="C107" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="D107" s="15"/>
       <c r="E107">
         <v>8</v>
       </c>
-      <c r="L107" s="4">
-        <v>1000</v>
+      <c r="L107" s="4" t="s">
+        <v>330</v>
       </c>
       <c r="N107">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="Q107">
-        <v>35</v>
-      </c>
-      <c r="S107">
-        <v>1.5</v>
-      </c>
-      <c r="T107">
-        <v>0.15</v>
+        <v>20</v>
       </c>
       <c r="V107">
-        <v>1</v>
+        <v>125</v>
       </c>
       <c r="X107" t="s">
-        <v>363</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="108" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B108">
-        <v>2375</v>
+        <v>2372</v>
       </c>
       <c r="C108" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="D108" s="15"/>
       <c r="E108">
         <v>8</v>
       </c>
-      <c r="L108" s="4" t="s">
-        <v>341</v>
+      <c r="L108" s="4">
+        <v>500</v>
+      </c>
+      <c r="M108">
+        <v>500</v>
       </c>
       <c r="N108">
-        <v>12</v>
-      </c>
-      <c r="Q108">
+        <v>9</v>
+      </c>
+      <c r="R108">
+        <v>8</v>
+      </c>
+      <c r="V108">
         <v>20</v>
       </c>
-      <c r="V108">
-        <v>30</v>
-      </c>
       <c r="X108" t="s">
-        <v>367</v>
+        <v>347</v>
       </c>
     </row>
     <row r="109" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B109">
-        <v>2381</v>
+        <v>2373</v>
       </c>
       <c r="C109" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="D109" s="15"/>
       <c r="E109">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L109" s="4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="N109">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="Q109">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="V109">
-        <v>125</v>
+        <v>35</v>
       </c>
       <c r="X109" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
     </row>
     <row r="110" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B110">
-        <v>2382</v>
+        <v>2374</v>
       </c>
       <c r="C110" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="D110" s="15"/>
       <c r="E110">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L110" s="4">
         <v>1000</v>
       </c>
       <c r="N110">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="Q110">
-        <v>45</v>
+        <v>35</v>
+      </c>
+      <c r="S110">
+        <v>1.5</v>
+      </c>
+      <c r="T110">
+        <v>0.15</v>
       </c>
       <c r="V110">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="X110" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="111" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B111">
-        <v>2391</v>
+        <v>2375</v>
       </c>
       <c r="C111" t="s">
-        <v>137</v>
+        <v>161</v>
       </c>
       <c r="D111" s="15"/>
       <c r="E111">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L111" s="4" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="N111">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q111">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="V111">
-        <v>125</v>
+        <v>30</v>
       </c>
       <c r="X111" t="s">
-        <v>1032</v>
+        <v>367</v>
       </c>
     </row>
     <row r="112" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B112">
-        <v>2392</v>
+        <v>2381</v>
       </c>
       <c r="C112" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="D112" s="15"/>
       <c r="E112">
-        <v>10</v>
-      </c>
-      <c r="L112" s="4">
-        <v>500</v>
-      </c>
-      <c r="M112">
-        <v>500</v>
+        <v>9</v>
+      </c>
+      <c r="L112" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="N112">
+        <v>12</v>
+      </c>
+      <c r="Q112">
+        <v>20</v>
+      </c>
+      <c r="V112">
+        <v>125</v>
+      </c>
+      <c r="X112" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="113" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B113">
+        <v>2382</v>
+      </c>
+      <c r="C113" t="s">
+        <v>151</v>
+      </c>
+      <c r="D113" s="15"/>
+      <c r="E113">
         <v>9</v>
       </c>
-      <c r="R112">
-        <v>12</v>
-      </c>
-      <c r="V112">
-        <v>40</v>
-      </c>
-      <c r="X112" t="s">
-        <v>348</v>
+      <c r="L113" s="4">
+        <v>1000</v>
+      </c>
+      <c r="N113">
+        <v>18</v>
+      </c>
+      <c r="Q113">
+        <v>45</v>
+      </c>
+      <c r="V113">
+        <v>8</v>
+      </c>
+      <c r="X113" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="114" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B114">
-        <v>2401</v>
+        <v>2391</v>
       </c>
       <c r="C114" t="s">
-        <v>97</v>
-      </c>
-      <c r="D114" t="s">
-        <v>22</v>
-      </c>
-      <c r="O114">
-        <v>1</v>
-      </c>
-      <c r="U114">
+        <v>137</v>
+      </c>
+      <c r="D114" s="15"/>
+      <c r="E114">
         <v>10</v>
       </c>
-      <c r="Z114" t="s">
-        <v>1239</v>
+      <c r="L114" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="N114">
+        <v>11</v>
+      </c>
+      <c r="Q114">
+        <v>25</v>
+      </c>
+      <c r="V114">
+        <v>125</v>
+      </c>
+      <c r="X114" t="s">
+        <v>1032</v>
       </c>
     </row>
     <row r="115" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B115">
-        <v>2402</v>
+        <v>2392</v>
       </c>
       <c r="C115" t="s">
-        <v>166</v>
-      </c>
-      <c r="U115">
+        <v>141</v>
+      </c>
+      <c r="D115" s="15"/>
+      <c r="E115">
         <v>10</v>
       </c>
-      <c r="Z115" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="116" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B116">
-        <v>2403</v>
-      </c>
-      <c r="C116" t="s">
-        <v>168</v>
-      </c>
-      <c r="O116">
-        <v>1</v>
-      </c>
-      <c r="U116">
-        <v>25</v>
-      </c>
-      <c r="Z116" t="s">
-        <v>1147</v>
+      <c r="L115" s="4">
+        <v>500</v>
+      </c>
+      <c r="M115">
+        <v>500</v>
+      </c>
+      <c r="N115">
+        <v>9</v>
+      </c>
+      <c r="R115">
+        <v>12</v>
+      </c>
+      <c r="V115">
+        <v>40</v>
+      </c>
+      <c r="X115" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="117" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B117">
-        <v>2404</v>
+        <v>2401</v>
       </c>
       <c r="C117" t="s">
-        <v>167</v>
+        <v>97</v>
+      </c>
+      <c r="D117" t="s">
+        <v>22</v>
       </c>
       <c r="O117">
-        <v>2</v>
-      </c>
-      <c r="S117">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="U117">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="Z117" t="s">
-        <v>1168</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="118" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B118">
-        <v>2411</v>
+        <v>2402</v>
       </c>
       <c r="C118" t="s">
-        <v>98</v>
-      </c>
-      <c r="E118">
-        <v>2</v>
-      </c>
-      <c r="O118">
-        <v>2</v>
+        <v>166</v>
       </c>
       <c r="U118">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Z118" t="s">
-        <v>1239</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="119" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B119">
-        <v>2421</v>
+        <v>2403</v>
       </c>
       <c r="C119" t="s">
-        <v>99</v>
-      </c>
-      <c r="E119">
-        <v>3</v>
+        <v>168</v>
       </c>
       <c r="O119">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="U119">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="120" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B120">
-        <v>2431</v>
+        <v>2404</v>
       </c>
       <c r="C120" t="s">
-        <v>100</v>
-      </c>
-      <c r="E120">
-        <v>4</v>
+        <v>167</v>
       </c>
       <c r="O120">
-        <v>21</v>
+        <v>2</v>
+      </c>
+      <c r="S120">
+        <v>-0.5</v>
       </c>
       <c r="U120">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>1168</v>
       </c>
     </row>
     <row r="121" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B121">
-        <v>2441</v>
+        <v>2411</v>
       </c>
       <c r="C121" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E121">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O121">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="U121">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="Z121" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="122" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B122">
-        <v>2451</v>
+        <v>2421</v>
       </c>
       <c r="C122" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E122">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O122">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="U122">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B123">
-        <v>2461</v>
+        <v>2431</v>
       </c>
       <c r="C123" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E123">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O123">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="U123">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="124" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B124">
-        <v>2471</v>
+        <v>2441</v>
       </c>
       <c r="C124" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E124">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O124">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="U124">
-        <v>250</v>
+        <v>70</v>
       </c>
     </row>
     <row r="125" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B125">
-        <v>2481</v>
+        <v>2451</v>
       </c>
       <c r="C125" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E125">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O125">
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="U125">
-        <v>450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="126" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B126">
-        <v>2491</v>
+        <v>2461</v>
       </c>
       <c r="C126" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E126">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O126">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="U126">
-        <v>1000</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="127" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>2471</v>
+      </c>
+      <c r="C127" t="s">
+        <v>104</v>
+      </c>
+      <c r="E127">
+        <v>8</v>
+      </c>
+      <c r="O127">
+        <v>200</v>
+      </c>
+      <c r="U127">
+        <v>250</v>
       </c>
     </row>
     <row r="128" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B128">
-        <v>2501</v>
+        <v>2481</v>
       </c>
       <c r="C128" t="s">
-        <v>800</v>
-      </c>
-      <c r="D128" t="s">
-        <v>23</v>
+        <v>105</v>
+      </c>
+      <c r="E128">
+        <v>9</v>
       </c>
       <c r="O128">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="U128">
-        <v>10</v>
-      </c>
-      <c r="Z128" t="s">
-        <v>1239</v>
+        <v>450</v>
       </c>
     </row>
     <row r="129" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B129">
-        <v>2502</v>
+        <v>2491</v>
       </c>
       <c r="C129" t="s">
-        <v>169</v>
-      </c>
-      <c r="N129">
-        <v>0.04</v>
+        <v>106</v>
+      </c>
+      <c r="E129">
+        <v>10</v>
+      </c>
+      <c r="O129">
+        <v>1500</v>
       </c>
       <c r="U129">
-        <v>10</v>
-      </c>
-      <c r="Z129" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="130" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B130">
-        <v>2503</v>
-      </c>
-      <c r="C130" t="s">
-        <v>170</v>
-      </c>
-      <c r="N130">
-        <v>0.02</v>
-      </c>
-      <c r="U130">
-        <v>10</v>
-      </c>
-      <c r="Z130" t="s">
-        <v>1147</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="131" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B131">
-        <v>2504</v>
+        <v>2501</v>
       </c>
       <c r="C131" t="s">
-        <v>171</v>
-      </c>
-      <c r="N131">
-        <v>0.04</v>
+        <v>800</v>
+      </c>
+      <c r="D131" t="s">
+        <v>23</v>
       </c>
       <c r="O131">
         <v>1</v>
       </c>
       <c r="U131">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Z131" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="132" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B132">
-        <v>2511</v>
+        <v>2502</v>
       </c>
       <c r="C132" t="s">
-        <v>801</v>
-      </c>
-      <c r="E132">
-        <v>2</v>
-      </c>
-      <c r="O132">
-        <v>2</v>
+        <v>169</v>
+      </c>
+      <c r="N132">
+        <v>0.04</v>
       </c>
       <c r="U132">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Z132" t="s">
-        <v>1239</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="133" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B133">
-        <v>2512</v>
+        <v>2503</v>
       </c>
       <c r="C133" t="s">
-        <v>179</v>
-      </c>
-      <c r="E133">
-        <v>2</v>
-      </c>
-      <c r="K133">
-        <v>3</v>
+        <v>170</v>
       </c>
       <c r="N133">
-        <v>0.05</v>
-      </c>
-      <c r="O133">
-        <v>2</v>
+        <v>0.02</v>
       </c>
       <c r="U133">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="Z133" t="s">
-        <v>1240</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="134" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B134">
-        <v>2513</v>
+        <v>2504</v>
       </c>
       <c r="C134" t="s">
-        <v>300</v>
+        <v>171</v>
       </c>
       <c r="N134">
         <v>0.04</v>
       </c>
+      <c r="O134">
+        <v>1</v>
+      </c>
       <c r="U134">
         <v>15</v>
       </c>
       <c r="Z134" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="135" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B135">
-        <v>2521</v>
+        <v>2511</v>
       </c>
       <c r="C135" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E135">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O135">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="U135">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="Z135" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="136" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B136">
-        <v>2531</v>
+        <v>2512</v>
       </c>
       <c r="C136" t="s">
-        <v>803</v>
+        <v>179</v>
       </c>
       <c r="E136">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="K136">
+        <v>3</v>
+      </c>
+      <c r="N136">
+        <v>0.05</v>
       </c>
       <c r="O136">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="U136">
-        <v>50</v>
+        <v>35</v>
+      </c>
+      <c r="Z136" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="137" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B137">
-        <v>2541</v>
+        <v>2513</v>
       </c>
       <c r="C137" t="s">
-        <v>805</v>
-      </c>
-      <c r="E137">
-        <v>5</v>
-      </c>
-      <c r="O137">
-        <v>48</v>
+        <v>300</v>
+      </c>
+      <c r="N137">
+        <v>0.04</v>
       </c>
       <c r="U137">
-        <v>70</v>
+        <v>15</v>
+      </c>
+      <c r="Z137" t="s">
+        <v>1241</v>
       </c>
     </row>
     <row r="138" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B138">
-        <v>2551</v>
+        <v>2521</v>
       </c>
       <c r="C138" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="E138">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O138">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="U138">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="139" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B139">
-        <v>2561</v>
+        <v>2531</v>
       </c>
       <c r="C139" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="E139">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O139">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="U139">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="140" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B140">
-        <v>2571</v>
+        <v>2541</v>
       </c>
       <c r="C140" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="E140">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O140">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="U140">
-        <v>250</v>
+        <v>70</v>
       </c>
     </row>
     <row r="141" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B141">
-        <v>2581</v>
+        <v>2551</v>
       </c>
       <c r="C141" t="s">
-        <v>809</v>
+        <v>804</v>
       </c>
       <c r="E141">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O141">
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="U141">
-        <v>450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B142">
-        <v>2591</v>
+        <v>2561</v>
       </c>
       <c r="C142" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="E142">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O142">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="U142">
-        <v>1000</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B143">
+        <v>2571</v>
+      </c>
+      <c r="C143" t="s">
+        <v>807</v>
+      </c>
+      <c r="E143">
+        <v>8</v>
+      </c>
+      <c r="O143">
+        <v>200</v>
+      </c>
+      <c r="U143">
+        <v>250</v>
       </c>
     </row>
     <row r="144" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B144">
-        <v>2601</v>
+        <v>2581</v>
       </c>
       <c r="C144" t="s">
-        <v>107</v>
-      </c>
-      <c r="D144" t="s">
-        <v>24</v>
+        <v>809</v>
+      </c>
+      <c r="E144">
+        <v>9</v>
       </c>
       <c r="O144">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="U144">
-        <v>10</v>
-      </c>
-      <c r="Z144" t="s">
-        <v>1239</v>
+        <v>450</v>
       </c>
     </row>
     <row r="145" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B145">
-        <v>2602</v>
+        <v>2591</v>
       </c>
       <c r="C145" t="s">
-        <v>172</v>
-      </c>
-      <c r="N145">
-        <v>0.02</v>
+        <v>808</v>
+      </c>
+      <c r="E145">
+        <v>10</v>
+      </c>
+      <c r="O145">
+        <v>1500</v>
       </c>
       <c r="U145">
-        <v>10</v>
-      </c>
-      <c r="Z145" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="146" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B146">
-        <v>2603</v>
-      </c>
-      <c r="C146" t="s">
-        <v>174</v>
-      </c>
-      <c r="N146">
-        <v>0.06</v>
-      </c>
-      <c r="U146">
-        <v>8</v>
-      </c>
-      <c r="Z146" t="s">
-        <v>1147</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="147" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B147">
-        <v>2604</v>
+        <v>2601</v>
       </c>
       <c r="C147" t="s">
-        <v>173</v>
-      </c>
-      <c r="N147">
-        <v>0.08</v>
+        <v>107</v>
+      </c>
+      <c r="D147" t="s">
+        <v>24</v>
       </c>
       <c r="O147">
         <v>1</v>
       </c>
       <c r="U147">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="Z147" t="s">
-        <v>1147</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="148" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B148">
-        <v>2611</v>
+        <v>2602</v>
       </c>
       <c r="C148" t="s">
-        <v>108</v>
-      </c>
-      <c r="E148">
-        <v>2</v>
-      </c>
-      <c r="O148">
-        <v>2</v>
+        <v>172</v>
+      </c>
+      <c r="N148">
+        <v>0.02</v>
       </c>
       <c r="U148">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Z148" t="s">
-        <v>1239</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="149" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B149">
-        <v>2621</v>
+        <v>2603</v>
       </c>
       <c r="C149" t="s">
-        <v>109</v>
-      </c>
-      <c r="E149">
-        <v>3</v>
-      </c>
-      <c r="O149">
-        <v>14</v>
+        <v>174</v>
+      </c>
+      <c r="N149">
+        <v>0.06</v>
       </c>
       <c r="U149">
-        <v>30</v>
+        <v>8</v>
+      </c>
+      <c r="Z149" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="150" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B150">
-        <v>2631</v>
+        <v>2604</v>
       </c>
       <c r="C150" t="s">
-        <v>110</v>
-      </c>
-      <c r="E150">
-        <v>4</v>
+        <v>173</v>
+      </c>
+      <c r="N150">
+        <v>0.08</v>
       </c>
       <c r="O150">
-        <v>21</v>
+        <v>1</v>
       </c>
       <c r="U150">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="Z150" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="151" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B151">
-        <v>2641</v>
+        <v>2611</v>
       </c>
       <c r="C151" t="s">
-        <v>740</v>
+        <v>108</v>
       </c>
       <c r="E151">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O151">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="U151">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="Z151" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="152" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B152">
-        <v>2651</v>
+        <v>2621</v>
       </c>
       <c r="C152" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E152">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O152">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="U152">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="153" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B153">
-        <v>2661</v>
+        <v>2631</v>
       </c>
       <c r="C153" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E153">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O153">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="U153">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="154" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B154">
-        <v>2671</v>
+        <v>2641</v>
       </c>
       <c r="C154" t="s">
-        <v>113</v>
+        <v>740</v>
       </c>
       <c r="E154">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O154">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="U154">
-        <v>250</v>
+        <v>70</v>
       </c>
     </row>
     <row r="155" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B155">
-        <v>2681</v>
+        <v>2651</v>
       </c>
       <c r="C155" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E155">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O155">
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="U155">
-        <v>450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="156" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B156">
-        <v>2691</v>
+        <v>2661</v>
       </c>
       <c r="C156" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E156">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O156">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="U156">
-        <v>1000</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="157" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B157">
+        <v>2671</v>
+      </c>
+      <c r="C157" t="s">
+        <v>113</v>
+      </c>
+      <c r="E157">
+        <v>8</v>
+      </c>
+      <c r="O157">
+        <v>200</v>
+      </c>
+      <c r="U157">
+        <v>250</v>
       </c>
     </row>
     <row r="158" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B158">
-        <v>2701</v>
+        <v>2681</v>
       </c>
       <c r="C158" t="s">
-        <v>116</v>
-      </c>
-      <c r="D158" t="s">
-        <v>25</v>
+        <v>114</v>
+      </c>
+      <c r="E158">
+        <v>9</v>
       </c>
       <c r="O158">
-        <v>1</v>
+        <v>400</v>
       </c>
       <c r="U158">
-        <v>10</v>
-      </c>
-      <c r="Z158" t="s">
-        <v>1239</v>
+        <v>450</v>
       </c>
     </row>
     <row r="159" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B159">
-        <v>2702</v>
+        <v>2691</v>
       </c>
       <c r="C159" t="s">
-        <v>175</v>
+        <v>115</v>
+      </c>
+      <c r="E159">
+        <v>10</v>
+      </c>
+      <c r="O159">
+        <v>1500</v>
       </c>
       <c r="U159">
-        <v>8</v>
-      </c>
-      <c r="Z159" t="s">
-        <v>1147</v>
-      </c>
-    </row>
-    <row r="160" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B160">
-        <v>2703</v>
-      </c>
-      <c r="C160" t="s">
-        <v>176</v>
-      </c>
-      <c r="S160">
-        <v>0.2</v>
-      </c>
-      <c r="U160">
-        <v>12</v>
-      </c>
-      <c r="Z160" t="s">
-        <v>1147</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="161" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B161">
-        <v>2704</v>
+        <v>2701</v>
       </c>
       <c r="C161" t="s">
-        <v>177</v>
+        <v>116</v>
+      </c>
+      <c r="D161" t="s">
+        <v>25</v>
       </c>
       <c r="O161">
         <v>1</v>
       </c>
-      <c r="S161">
-        <v>0.4</v>
-      </c>
       <c r="U161">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="Z161" t="s">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="162" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B162">
-        <v>2705</v>
+        <v>2702</v>
       </c>
       <c r="C162" t="s">
-        <v>301</v>
-      </c>
-      <c r="O162">
-        <v>2</v>
-      </c>
-      <c r="S162">
-        <v>0.4</v>
+        <v>175</v>
       </c>
       <c r="U162">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="Z162" t="s">
-        <v>1244</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="163" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B163">
-        <v>2711</v>
+        <v>2703</v>
       </c>
       <c r="C163" t="s">
-        <v>117</v>
-      </c>
-      <c r="E163">
-        <v>2</v>
-      </c>
-      <c r="O163">
-        <v>2</v>
+        <v>176</v>
+      </c>
+      <c r="S163">
+        <v>0.2</v>
       </c>
       <c r="U163">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="Z163" t="s">
-        <v>1239</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="164" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B164">
-        <v>2712</v>
+        <v>2704</v>
       </c>
       <c r="C164" t="s">
-        <v>178</v>
-      </c>
-      <c r="E164">
-        <v>2</v>
+        <v>177</v>
       </c>
       <c r="O164">
         <v>1</v>
       </c>
       <c r="S164">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="U164">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="Z164" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="165" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B165">
-        <v>2713</v>
+        <v>2705</v>
       </c>
       <c r="C165" t="s">
-        <v>302</v>
-      </c>
-      <c r="E165">
+        <v>301</v>
+      </c>
+      <c r="O165">
         <v>2</v>
-      </c>
-      <c r="L165" s="4">
-        <v>1</v>
-      </c>
-      <c r="O165">
-        <v>3</v>
       </c>
       <c r="S165">
         <v>0.4</v>
       </c>
       <c r="U165">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="Z165" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="166" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B166">
-        <v>2714</v>
+        <v>2711</v>
       </c>
       <c r="C166" t="s">
-        <v>303</v>
+        <v>117</v>
       </c>
       <c r="E166">
         <v>2</v>
@@ -19508,752 +19484,782 @@
       <c r="O166">
         <v>2</v>
       </c>
-      <c r="S166">
-        <v>0.6</v>
-      </c>
       <c r="U166">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="Z166" t="s">
-        <v>1246</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="167" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B167">
-        <v>2721</v>
+        <v>2712</v>
       </c>
       <c r="C167" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="E167">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O167">
-        <v>14</v>
+        <v>1</v>
+      </c>
+      <c r="S167">
+        <v>0.6</v>
       </c>
       <c r="U167">
-        <v>30</v>
+        <v>40</v>
+      </c>
+      <c r="Z167" t="s">
+        <v>1245</v>
       </c>
     </row>
     <row r="168" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B168">
-        <v>2731</v>
+        <v>2713</v>
       </c>
       <c r="C168" t="s">
-        <v>119</v>
+        <v>302</v>
       </c>
       <c r="E168">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="L168" s="4">
+        <v>1</v>
       </c>
       <c r="O168">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="S168">
+        <v>0.4</v>
       </c>
       <c r="U168">
-        <v>50</v>
+        <v>60</v>
+      </c>
+      <c r="Z168" t="s">
+        <v>1247</v>
       </c>
     </row>
     <row r="169" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B169">
-        <v>2741</v>
+        <v>2714</v>
       </c>
       <c r="C169" t="s">
-        <v>120</v>
+        <v>303</v>
       </c>
       <c r="E169">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O169">
-        <v>48</v>
+        <v>2</v>
+      </c>
+      <c r="S169">
+        <v>0.6</v>
       </c>
       <c r="U169">
-        <v>70</v>
+        <v>60</v>
+      </c>
+      <c r="Z169" t="s">
+        <v>1246</v>
       </c>
     </row>
     <row r="170" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B170">
-        <v>2751</v>
+        <v>2721</v>
       </c>
       <c r="C170" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E170">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O170">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="U170">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="171" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B171">
-        <v>2761</v>
+        <v>2731</v>
       </c>
       <c r="C171" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E171">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="O171">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="U171">
-        <v>150</v>
+        <v>50</v>
       </c>
     </row>
     <row r="172" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B172">
-        <v>2771</v>
+        <v>2741</v>
       </c>
       <c r="C172" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E172">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O172">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="U172">
-        <v>250</v>
+        <v>70</v>
       </c>
     </row>
     <row r="173" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B173">
-        <v>2781</v>
+        <v>2751</v>
       </c>
       <c r="C173" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E173">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O173">
-        <v>400</v>
+        <v>72</v>
       </c>
       <c r="U173">
-        <v>450</v>
+        <v>100</v>
       </c>
     </row>
     <row r="174" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B174">
-        <v>2791</v>
+        <v>2761</v>
       </c>
       <c r="C174" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E174">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="O174">
-        <v>1500</v>
+        <v>100</v>
       </c>
       <c r="U174">
-        <v>1000</v>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="175" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B175">
+        <v>2771</v>
+      </c>
+      <c r="C175" t="s">
+        <v>123</v>
+      </c>
+      <c r="E175">
+        <v>8</v>
+      </c>
+      <c r="O175">
+        <v>200</v>
+      </c>
+      <c r="U175">
+        <v>250</v>
       </c>
     </row>
     <row r="176" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B176">
-        <v>2801</v>
+        <v>2781</v>
       </c>
       <c r="C176" t="s">
-        <v>769</v>
-      </c>
-      <c r="D176" t="s">
-        <v>26</v>
+        <v>124</v>
+      </c>
+      <c r="E176">
+        <v>9</v>
+      </c>
+      <c r="O176">
+        <v>400</v>
+      </c>
+      <c r="U176">
+        <v>450</v>
       </c>
     </row>
     <row r="177" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B177">
-        <v>2802</v>
+        <v>2791</v>
       </c>
       <c r="C177" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="178" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B178">
-        <v>2803</v>
-      </c>
-      <c r="C178" t="s">
-        <v>771</v>
+        <v>125</v>
+      </c>
+      <c r="E177">
+        <v>10</v>
+      </c>
+      <c r="O177">
+        <v>1500</v>
+      </c>
+      <c r="U177">
+        <v>1000</v>
       </c>
     </row>
     <row r="179" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B179">
-        <v>2804</v>
+        <v>2801</v>
       </c>
       <c r="C179" t="s">
-        <v>763</v>
+        <v>769</v>
+      </c>
+      <c r="D179" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="180" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B180">
-        <v>2805</v>
+        <v>2802</v>
       </c>
       <c r="C180" t="s">
-        <v>743</v>
-      </c>
-      <c r="Z180" t="s">
-        <v>1147</v>
+        <v>770</v>
       </c>
     </row>
     <row r="181" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B181">
-        <v>2806</v>
+        <v>2803</v>
       </c>
       <c r="C181" t="s">
-        <v>298</v>
-      </c>
-      <c r="Z181" t="s">
-        <v>1273</v>
+        <v>771</v>
       </c>
     </row>
     <row r="182" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B182">
-        <v>2807</v>
+        <v>2804</v>
       </c>
       <c r="C182" t="s">
-        <v>1015</v>
-      </c>
-      <c r="Z182" t="s">
-        <v>1150</v>
+        <v>763</v>
       </c>
     </row>
     <row r="183" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B183">
-        <v>2808</v>
+        <v>2805</v>
       </c>
       <c r="C183" t="s">
-        <v>1084</v>
+        <v>743</v>
       </c>
       <c r="Z183" t="s">
-        <v>1248</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="184" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B184">
-        <v>2809</v>
+        <v>2806</v>
       </c>
       <c r="C184" t="s">
-        <v>1086</v>
+        <v>298</v>
       </c>
       <c r="Z184" t="s">
-        <v>1147</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="185" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B185">
-        <v>2810</v>
+        <v>2807</v>
       </c>
       <c r="C185" t="s">
-        <v>1087</v>
+        <v>1015</v>
       </c>
       <c r="Z185" t="s">
-        <v>1249</v>
+        <v>1150</v>
       </c>
     </row>
     <row r="186" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B186">
-        <v>2811</v>
+        <v>2808</v>
       </c>
       <c r="C186" t="s">
-        <v>772</v>
-      </c>
-      <c r="E186">
-        <v>2</v>
+        <v>1084</v>
+      </c>
+      <c r="Z186" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="187" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B187">
-        <v>2812</v>
+        <v>2809</v>
       </c>
       <c r="C187" t="s">
-        <v>773</v>
+        <v>1086</v>
+      </c>
+      <c r="Z187" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="188" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B188">
-        <v>2813</v>
+        <v>2810</v>
       </c>
       <c r="C188" t="s">
-        <v>774</v>
+        <v>1087</v>
+      </c>
+      <c r="Z188" t="s">
+        <v>1249</v>
       </c>
     </row>
     <row r="189" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B189">
-        <v>2814</v>
+        <v>2811</v>
       </c>
       <c r="C189" t="s">
-        <v>797</v>
+        <v>772</v>
+      </c>
+      <c r="E189">
+        <v>2</v>
       </c>
     </row>
     <row r="190" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B190">
-        <v>2815</v>
+        <v>2812</v>
       </c>
       <c r="C190" t="s">
-        <v>299</v>
+        <v>773</v>
       </c>
     </row>
     <row r="191" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B191">
-        <v>2816</v>
+        <v>2813</v>
       </c>
       <c r="C191" t="s">
-        <v>1146</v>
-      </c>
-      <c r="L191" s="4">
-        <v>2.4</v>
-      </c>
-      <c r="N191">
-        <v>0.6</v>
-      </c>
-      <c r="S191">
-        <v>-0.8</v>
+        <v>774</v>
       </c>
     </row>
     <row r="192" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B192">
-        <v>2817</v>
+        <v>2814</v>
       </c>
       <c r="C192" t="s">
-        <v>1176</v>
-      </c>
-      <c r="L192" s="4">
-        <v>2.8</v>
-      </c>
-      <c r="N192">
-        <v>0.4</v>
+        <v>797</v>
       </c>
     </row>
     <row r="193" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B193">
-        <v>2818</v>
+        <v>2815</v>
       </c>
       <c r="C193" t="s">
-        <v>1182</v>
-      </c>
-      <c r="L193" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="N193">
-        <v>0.02</v>
+        <v>299</v>
       </c>
     </row>
     <row r="194" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B194">
-        <v>2821</v>
+        <v>2816</v>
       </c>
       <c r="C194" t="s">
-        <v>775</v>
-      </c>
-      <c r="E194">
-        <v>3</v>
+        <v>1146</v>
+      </c>
+      <c r="L194" s="4">
+        <v>2.4</v>
+      </c>
+      <c r="N194">
+        <v>0.6</v>
+      </c>
+      <c r="S194">
+        <v>-0.8</v>
       </c>
     </row>
     <row r="195" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B195">
-        <v>2822</v>
+        <v>2817</v>
       </c>
       <c r="C195" t="s">
-        <v>776</v>
+        <v>1176</v>
+      </c>
+      <c r="L195" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="N195">
+        <v>0.4</v>
       </c>
     </row>
     <row r="196" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B196">
-        <v>2823</v>
+        <v>2818</v>
       </c>
       <c r="C196" t="s">
-        <v>778</v>
+        <v>1182</v>
+      </c>
+      <c r="L196" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N196">
+        <v>0.02</v>
       </c>
     </row>
     <row r="197" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B197">
-        <v>2834</v>
+        <v>2821</v>
       </c>
       <c r="C197" t="s">
-        <v>777</v>
+        <v>775</v>
+      </c>
+      <c r="E197">
+        <v>3</v>
       </c>
     </row>
     <row r="198" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B198">
-        <v>2825</v>
+        <v>2822</v>
       </c>
       <c r="C198" t="s">
-        <v>538</v>
-      </c>
-      <c r="Z198" t="s">
-        <v>201</v>
+        <v>776</v>
       </c>
     </row>
     <row r="199" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B199">
-        <v>2831</v>
+        <v>2823</v>
       </c>
       <c r="C199" t="s">
-        <v>779</v>
-      </c>
-      <c r="E199">
-        <v>4</v>
+        <v>778</v>
       </c>
     </row>
     <row r="200" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B200">
-        <v>2832</v>
+        <v>2834</v>
       </c>
       <c r="C200" t="s">
-        <v>780</v>
+        <v>777</v>
       </c>
     </row>
     <row r="201" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B201">
-        <v>2833</v>
+        <v>2825</v>
       </c>
       <c r="C201" t="s">
-        <v>1213</v>
+        <v>538</v>
+      </c>
+      <c r="Z201" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="202" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B202">
-        <v>2834</v>
+        <v>2831</v>
       </c>
       <c r="C202" t="s">
-        <v>1214</v>
+        <v>779</v>
+      </c>
+      <c r="E202">
+        <v>4</v>
       </c>
     </row>
     <row r="203" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B203">
-        <v>2841</v>
+        <v>2832</v>
       </c>
       <c r="C203" t="s">
-        <v>782</v>
-      </c>
-      <c r="E203">
-        <v>5</v>
+        <v>780</v>
       </c>
     </row>
     <row r="204" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B204">
-        <v>2842</v>
+        <v>2833</v>
       </c>
       <c r="C204" t="s">
-        <v>781</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="205" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B205">
-        <v>2843</v>
+        <v>2834</v>
       </c>
       <c r="C205" t="s">
-        <v>1215</v>
-      </c>
-      <c r="L205" s="4">
-        <v>12</v>
-      </c>
-      <c r="N205">
-        <v>0.4</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="206" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B206">
-        <v>2851</v>
+        <v>2841</v>
       </c>
       <c r="C206" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="E206">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B207">
-        <v>2852</v>
+        <v>2842</v>
       </c>
       <c r="C207" t="s">
-        <v>789</v>
+        <v>781</v>
       </c>
     </row>
     <row r="208" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B208">
+        <v>2843</v>
+      </c>
+      <c r="C208" t="s">
+        <v>1215</v>
+      </c>
+      <c r="L208" s="4">
+        <v>12</v>
+      </c>
+      <c r="N208">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B209">
+        <v>2851</v>
+      </c>
+      <c r="C209" t="s">
+        <v>783</v>
+      </c>
+      <c r="E209">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B210">
+        <v>2852</v>
+      </c>
+      <c r="C210" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B211">
         <v>2853</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C211" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="209" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B209">
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B212">
         <v>2861</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C212" t="s">
         <v>785</v>
       </c>
-      <c r="E209">
+      <c r="E212">
         <v>7</v>
       </c>
     </row>
-    <row r="210" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B210">
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B213">
         <v>2862</v>
       </c>
-      <c r="C210" t="s">
+      <c r="C213" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="211" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B211">
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B214">
         <v>2863</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C214" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="212" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B212">
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B215">
         <v>2864</v>
       </c>
-      <c r="C212" t="s">
+      <c r="C215" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="213" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B213">
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B216">
         <v>2871</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C216" t="s">
         <v>786</v>
       </c>
-      <c r="E213">
+      <c r="E216">
         <v>8</v>
       </c>
     </row>
-    <row r="214" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B214">
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B217">
         <v>2872</v>
       </c>
-      <c r="C214" t="s">
+      <c r="C217" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="215" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B215">
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B218">
         <v>2873</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C218" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="216" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B216">
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B219">
         <v>2881</v>
       </c>
-      <c r="C216" t="s">
+      <c r="C219" t="s">
         <v>787</v>
       </c>
-      <c r="E216">
+      <c r="E219">
         <v>9</v>
       </c>
     </row>
-    <row r="217" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B217">
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B220">
         <v>2882</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C220" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="218" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B218">
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B221">
         <v>2883</v>
       </c>
-      <c r="C218" t="s">
+      <c r="C221" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="219" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B219">
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B222">
         <v>2891</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C222" t="s">
         <v>788</v>
       </c>
-      <c r="E219">
+      <c r="E222">
         <v>10</v>
       </c>
     </row>
-    <row r="220" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B220">
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B223">
         <v>2892</v>
       </c>
-      <c r="C220" t="s">
+      <c r="C223" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="222" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B222">
-        <v>2901</v>
-      </c>
-      <c r="C222" t="s">
-        <v>251</v>
-      </c>
-      <c r="D222" t="s">
-        <v>251</v>
-      </c>
-      <c r="X222" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z222" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="223" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B223">
-        <v>2902</v>
-      </c>
-      <c r="C223" t="s">
-        <v>253</v>
-      </c>
-      <c r="E223">
-        <v>2</v>
-      </c>
-      <c r="X223" t="s">
-        <v>255</v>
-      </c>
-      <c r="Z223" t="s">
-        <v>1250</v>
-      </c>
-    </row>
-    <row r="224" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B224">
-        <v>2903</v>
-      </c>
-      <c r="C224" t="s">
-        <v>252</v>
-      </c>
-      <c r="E224">
-        <v>3</v>
-      </c>
-      <c r="X224" t="s">
-        <v>256</v>
-      </c>
-      <c r="Z224" t="s">
-        <v>1250</v>
       </c>
     </row>
     <row r="225" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B225">
-        <v>2904</v>
+        <v>2901</v>
       </c>
       <c r="C225" t="s">
-        <v>1316</v>
-      </c>
-      <c r="V225">
-        <v>8</v>
+        <v>251</v>
+      </c>
+      <c r="D225" t="s">
+        <v>251</v>
       </c>
       <c r="X225" t="s">
-        <v>1318</v>
+        <v>254</v>
+      </c>
+      <c r="Z225" t="s">
+        <v>1250</v>
       </c>
     </row>
     <row r="226" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B226">
-        <v>2905</v>
+        <v>2902</v>
       </c>
       <c r="C226" t="s">
-        <v>1317</v>
-      </c>
-      <c r="V226">
-        <v>24</v>
+        <v>253</v>
+      </c>
+      <c r="E226">
+        <v>2</v>
       </c>
       <c r="X226" t="s">
-        <v>1318</v>
+        <v>255</v>
+      </c>
+      <c r="Z226" t="s">
+        <v>1250</v>
       </c>
     </row>
     <row r="227" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B227">
-        <v>2911</v>
+        <v>2903</v>
       </c>
       <c r="C227" t="s">
-        <v>258</v>
-      </c>
-      <c r="D227" t="s">
-        <v>257</v>
-      </c>
-      <c r="H227" s="6"/>
-      <c r="L227" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="U227">
-        <v>6</v>
+        <v>252</v>
+      </c>
+      <c r="E227">
+        <v>3</v>
+      </c>
+      <c r="X227" t="s">
+        <v>256</v>
       </c>
       <c r="Z227" t="s">
-        <v>1147</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="228" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B228">
-        <v>2912</v>
+        <v>2904</v>
       </c>
       <c r="C228" t="s">
-        <v>259</v>
-      </c>
-      <c r="L228" s="4">
-        <v>0.6</v>
-      </c>
-      <c r="U228">
-        <v>6</v>
-      </c>
-      <c r="Z228" t="s">
-        <v>1147</v>
+        <v>1316</v>
+      </c>
+      <c r="V228">
+        <v>8</v>
+      </c>
+      <c r="X228" t="s">
+        <v>1318</v>
       </c>
     </row>
     <row r="229" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B229">
-        <v>2913</v>
+        <v>2905</v>
       </c>
       <c r="C229" t="s">
-        <v>260</v>
-      </c>
-      <c r="Z229" t="s">
-        <v>1147</v>
+        <v>1317</v>
+      </c>
+      <c r="V229">
+        <v>24</v>
+      </c>
+      <c r="X229" t="s">
+        <v>1318</v>
       </c>
     </row>
     <row r="230" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B230">
-        <v>2914</v>
+        <v>2911</v>
       </c>
       <c r="C230" t="s">
-        <v>261</v>
+        <v>258</v>
+      </c>
+      <c r="D230" t="s">
+        <v>257</v>
+      </c>
+      <c r="H230" s="6"/>
+      <c r="L230" s="4">
+        <v>0.6</v>
+      </c>
+      <c r="U230">
+        <v>6</v>
       </c>
       <c r="Z230" t="s">
-        <v>1251</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="231" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B231">
-        <v>2915</v>
+        <v>2912</v>
       </c>
       <c r="C231" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="L231" s="4">
         <v>0.6</v>
       </c>
       <c r="U231">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="Z231" t="s">
-        <v>1251</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="232" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B232">
-        <v>2916</v>
+        <v>2913</v>
       </c>
       <c r="C232" t="s">
-        <v>288</v>
+        <v>260</v>
       </c>
       <c r="Z232" t="s">
         <v>1147</v>
@@ -20261,27 +20267,27 @@
     </row>
     <row r="233" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B233">
-        <v>2917</v>
+        <v>2914</v>
       </c>
       <c r="C233" t="s">
-        <v>739</v>
+        <v>261</v>
       </c>
       <c r="Z233" t="s">
-        <v>1147</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="234" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B234">
-        <v>2918</v>
+        <v>2915</v>
       </c>
       <c r="C234" t="s">
-        <v>1068</v>
+        <v>262</v>
       </c>
       <c r="L234" s="4">
-        <v>1.5</v>
+        <v>0.6</v>
       </c>
       <c r="U234">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Z234" t="s">
         <v>1251</v>
@@ -20289,274 +20295,274 @@
     </row>
     <row r="235" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B235">
-        <v>2921</v>
+        <v>2916</v>
       </c>
       <c r="C235" t="s">
-        <v>264</v>
-      </c>
-      <c r="D235" t="s">
-        <v>263</v>
-      </c>
-      <c r="N235">
-        <v>0.04</v>
-      </c>
-      <c r="X235" t="s">
-        <v>268</v>
+        <v>288</v>
       </c>
       <c r="Z235" t="s">
-        <v>1251</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="236" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B236">
-        <v>2922</v>
+        <v>2917</v>
       </c>
       <c r="C236" t="s">
-        <v>265</v>
-      </c>
-      <c r="N236">
-        <v>0.04</v>
-      </c>
-      <c r="X236" t="s">
-        <v>269</v>
+        <v>739</v>
       </c>
       <c r="Z236" t="s">
-        <v>1262</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="237" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B237">
-        <v>2923</v>
+        <v>2918</v>
       </c>
       <c r="C237" t="s">
-        <v>266</v>
-      </c>
-      <c r="N237">
-        <v>0.04</v>
-      </c>
-      <c r="X237" t="s">
-        <v>267</v>
+        <v>1068</v>
+      </c>
+      <c r="L237" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="U237">
+        <v>12</v>
       </c>
       <c r="Z237" t="s">
-        <v>1162</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="238" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B238">
-        <v>2924</v>
+        <v>2921</v>
       </c>
       <c r="C238" t="s">
-        <v>289</v>
-      </c>
-      <c r="L238" s="4">
-        <v>0.8</v>
+        <v>264</v>
+      </c>
+      <c r="D238" t="s">
+        <v>263</v>
       </c>
       <c r="N238">
-        <v>2.5</v>
-      </c>
-      <c r="Q238">
-        <v>6</v>
-      </c>
-      <c r="U238">
-        <v>2</v>
+        <v>0.04</v>
       </c>
       <c r="X238" t="s">
-        <v>296</v>
+        <v>268</v>
       </c>
       <c r="Z238" t="s">
-        <v>1147</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="239" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B239">
-        <v>2925</v>
+        <v>2922</v>
       </c>
       <c r="C239" t="s">
-        <v>290</v>
+        <v>265</v>
+      </c>
+      <c r="N239">
+        <v>0.04</v>
       </c>
       <c r="X239" t="s">
-        <v>293</v>
+        <v>269</v>
       </c>
       <c r="Z239" t="s">
-        <v>1249</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="240" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B240">
-        <v>2926</v>
+        <v>2923</v>
       </c>
       <c r="C240" t="s">
-        <v>291</v>
-      </c>
-      <c r="E240">
-        <v>2</v>
-      </c>
-      <c r="L240" s="4">
-        <v>1</v>
+        <v>266</v>
       </c>
       <c r="N240">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="X240" t="s">
-        <v>294</v>
+        <v>267</v>
       </c>
       <c r="Z240" t="s">
-        <v>1244</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="241" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B241">
-        <v>2927</v>
+        <v>2924</v>
       </c>
       <c r="C241" t="s">
-        <v>292</v>
-      </c>
-      <c r="E241">
-        <v>3</v>
+        <v>289</v>
       </c>
       <c r="L241" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="N241">
+        <v>2.5</v>
+      </c>
+      <c r="Q241">
+        <v>6</v>
+      </c>
+      <c r="U241">
         <v>2</v>
       </c>
-      <c r="N241">
-        <v>0.02</v>
-      </c>
       <c r="X241" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="Z241" t="s">
-        <v>1252</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="242" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B242">
-        <v>2928</v>
+        <v>2925</v>
       </c>
       <c r="C242" t="s">
-        <v>1057</v>
+        <v>290</v>
       </c>
       <c r="X242" t="s">
-        <v>1060</v>
+        <v>293</v>
       </c>
       <c r="Z242" t="s">
-        <v>1253</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="243" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B243">
-        <v>2931</v>
+        <v>2926</v>
       </c>
       <c r="C243" t="s">
-        <v>238</v>
-      </c>
-      <c r="D243" t="s">
-        <v>277</v>
+        <v>291</v>
+      </c>
+      <c r="E243">
+        <v>2</v>
       </c>
       <c r="L243" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N243">
-        <v>2.5</v>
+        <v>0.02</v>
       </c>
       <c r="X243" t="s">
-        <v>812</v>
+        <v>294</v>
       </c>
       <c r="Z243" t="s">
-        <v>1147</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="244" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B244">
-        <v>2932</v>
+        <v>2927</v>
       </c>
       <c r="C244" t="s">
-        <v>278</v>
+        <v>292</v>
+      </c>
+      <c r="E244">
+        <v>3</v>
       </c>
       <c r="L244" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N244">
-        <v>2</v>
-      </c>
-      <c r="Q244">
-        <v>4</v>
+        <v>0.02</v>
+      </c>
+      <c r="X244" t="s">
+        <v>295</v>
+      </c>
+      <c r="Z244" t="s">
+        <v>1252</v>
       </c>
     </row>
     <row r="245" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B245">
-        <v>2933</v>
+        <v>2928</v>
       </c>
       <c r="C245" t="s">
-        <v>281</v>
-      </c>
-      <c r="L245" s="4">
-        <v>1</v>
-      </c>
-      <c r="N245">
-        <v>2</v>
+        <v>1057</v>
       </c>
       <c r="X245" t="s">
-        <v>812</v>
+        <v>1060</v>
       </c>
       <c r="Z245" t="s">
-        <v>1147</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="246" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B246">
-        <v>2941</v>
+        <v>2931</v>
       </c>
       <c r="C246" t="s">
-        <v>372</v>
+        <v>238</v>
+      </c>
+      <c r="D246" t="s">
+        <v>277</v>
+      </c>
+      <c r="L246" s="4">
+        <v>2</v>
+      </c>
+      <c r="N246">
+        <v>2.5</v>
+      </c>
+      <c r="X246" t="s">
+        <v>812</v>
       </c>
       <c r="Z246" t="s">
-        <v>1257</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="247" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B247">
-        <v>2942</v>
+        <v>2932</v>
       </c>
       <c r="C247" t="s">
-        <v>373</v>
-      </c>
-      <c r="E247">
+        <v>278</v>
+      </c>
+      <c r="L247" s="4">
+        <v>1</v>
+      </c>
+      <c r="N247">
         <v>2</v>
+      </c>
+      <c r="Q247">
+        <v>4</v>
       </c>
     </row>
     <row r="248" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B248">
-        <v>2943</v>
+        <v>2933</v>
       </c>
       <c r="C248" t="s">
-        <v>374</v>
-      </c>
-      <c r="E248">
+        <v>281</v>
+      </c>
+      <c r="L248" s="4">
+        <v>1</v>
+      </c>
+      <c r="N248">
         <v>2</v>
+      </c>
+      <c r="X248" t="s">
+        <v>812</v>
+      </c>
+      <c r="Z248" t="s">
+        <v>1147</v>
       </c>
     </row>
     <row r="249" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B249">
-        <v>2944</v>
+        <v>2941</v>
       </c>
       <c r="C249" t="s">
-        <v>375</v>
-      </c>
-      <c r="E249">
-        <v>2</v>
-      </c>
-      <c r="L249" s="4">
-        <v>3</v>
-      </c>
-      <c r="N249">
-        <v>3.5</v>
+        <v>372</v>
+      </c>
+      <c r="Z249" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="250" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B250">
-        <v>2945</v>
+        <v>2942</v>
       </c>
       <c r="C250" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="E250">
         <v>2</v>
@@ -20564,10 +20570,10 @@
     </row>
     <row r="251" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B251">
-        <v>2946</v>
+        <v>2943</v>
       </c>
       <c r="C251" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="E251">
         <v>2</v>
@@ -20575,83 +20581,77 @@
     </row>
     <row r="252" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B252">
-        <v>2947</v>
+        <v>2944</v>
       </c>
       <c r="C252" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E252">
         <v>2</v>
       </c>
+      <c r="L252" s="4">
+        <v>3</v>
+      </c>
+      <c r="N252">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="253" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B253">
-        <v>2948</v>
+        <v>2945</v>
       </c>
       <c r="C253" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="E253">
         <v>2</v>
       </c>
-      <c r="Z253" t="s">
-        <v>1254</v>
-      </c>
     </row>
     <row r="254" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B254">
-        <v>2961</v>
+        <v>2946</v>
       </c>
       <c r="C254" t="s">
-        <v>282</v>
-      </c>
-      <c r="D254" t="s">
-        <v>284</v>
-      </c>
-      <c r="Z254" t="s">
-        <v>1147</v>
+        <v>377</v>
+      </c>
+      <c r="E254">
+        <v>2</v>
       </c>
     </row>
     <row r="255" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B255">
-        <v>2962</v>
+        <v>2947</v>
       </c>
       <c r="C255" t="s">
-        <v>283</v>
-      </c>
-      <c r="Z255" t="s">
-        <v>1288</v>
+        <v>378</v>
+      </c>
+      <c r="E255">
+        <v>2</v>
       </c>
     </row>
     <row r="256" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B256">
-        <v>2963</v>
+        <v>2948</v>
       </c>
       <c r="C256" t="s">
-        <v>315</v>
-      </c>
-      <c r="L256" s="4">
-        <v>1</v>
-      </c>
-      <c r="N256">
-        <v>0.05</v>
-      </c>
-      <c r="U256">
-        <v>8</v>
+        <v>379</v>
+      </c>
+      <c r="E256">
+        <v>2</v>
       </c>
       <c r="Z256" t="s">
-        <v>1147</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="257" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B257">
-        <v>2964</v>
+        <v>2961</v>
       </c>
       <c r="C257" t="s">
-        <v>319</v>
-      </c>
-      <c r="N257">
-        <v>0.04</v>
+        <v>282</v>
+      </c>
+      <c r="D257" t="s">
+        <v>284</v>
       </c>
       <c r="Z257" t="s">
         <v>1147</v>
@@ -20659,30 +20659,21 @@
     </row>
     <row r="258" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B258">
-        <v>2965</v>
+        <v>2962</v>
       </c>
       <c r="C258" t="s">
-        <v>844</v>
-      </c>
-      <c r="L258" s="4">
-        <v>1</v>
-      </c>
-      <c r="N258">
-        <v>0.05</v>
-      </c>
-      <c r="U258">
-        <v>8</v>
+        <v>283</v>
       </c>
       <c r="Z258" t="s">
-        <v>1147</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="259" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B259">
-        <v>2966</v>
+        <v>2963</v>
       </c>
       <c r="C259" t="s">
-        <v>845</v>
+        <v>315</v>
       </c>
       <c r="L259" s="4">
         <v>1</v>
@@ -20699,19 +20690,13 @@
     </row>
     <row r="260" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B260">
-        <v>2967</v>
+        <v>2964</v>
       </c>
       <c r="C260" t="s">
-        <v>846</v>
-      </c>
-      <c r="L260" s="4">
-        <v>1</v>
+        <v>319</v>
       </c>
       <c r="N260">
-        <v>0.05</v>
-      </c>
-      <c r="U260">
-        <v>8</v>
+        <v>0.04</v>
       </c>
       <c r="Z260" t="s">
         <v>1147</v>
@@ -20719,10 +20704,10 @@
     </row>
     <row r="261" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B261">
-        <v>2968</v>
+        <v>2965</v>
       </c>
       <c r="C261" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="L261" s="4">
         <v>1</v>
@@ -20739,96 +20724,96 @@
     </row>
     <row r="262" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B262">
-        <v>2969</v>
+        <v>2966</v>
       </c>
       <c r="C262" t="s">
-        <v>1117</v>
-      </c>
-      <c r="E262">
-        <v>2</v>
+        <v>845</v>
       </c>
       <c r="L262" s="4">
-        <v>1.8</v>
-      </c>
-      <c r="S262">
-        <v>-1.4</v>
+        <v>1</v>
+      </c>
+      <c r="N262">
+        <v>0.05</v>
       </c>
       <c r="U262">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="Z262" t="s">
-        <v>1289</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="263" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B263">
-        <v>2971</v>
+        <v>2967</v>
       </c>
       <c r="C263" t="s">
-        <v>309</v>
-      </c>
-      <c r="D263" t="s">
-        <v>304</v>
+        <v>846</v>
+      </c>
+      <c r="L263" s="4">
+        <v>1</v>
+      </c>
+      <c r="N263">
+        <v>0.05</v>
       </c>
       <c r="U263">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="Z263" t="s">
-        <v>1296</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="264" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B264">
-        <v>2972</v>
+        <v>2968</v>
       </c>
       <c r="C264" t="s">
-        <v>310</v>
+        <v>847</v>
       </c>
       <c r="L264" s="4">
         <v>1</v>
       </c>
       <c r="N264">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="U264">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="Z264" t="s">
-        <v>1296</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="265" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B265">
-        <v>2973</v>
+        <v>2969</v>
       </c>
       <c r="C265" t="s">
-        <v>318</v>
+        <v>1117</v>
+      </c>
+      <c r="E265">
+        <v>2</v>
       </c>
       <c r="L265" s="4">
-        <v>1</v>
-      </c>
-      <c r="N265">
-        <v>0.02</v>
+        <v>1.8</v>
+      </c>
+      <c r="S265">
+        <v>-1.4</v>
       </c>
       <c r="U265">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="Z265" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="266" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B266">
-        <v>2974</v>
+        <v>2971</v>
       </c>
       <c r="C266" t="s">
-        <v>308</v>
-      </c>
-      <c r="E266">
-        <v>2</v>
-      </c>
-      <c r="N266">
-        <v>0.05</v>
+        <v>309</v>
+      </c>
+      <c r="D266" t="s">
+        <v>304</v>
       </c>
       <c r="U266">
         <v>100</v>
@@ -20839,16 +20824,13 @@
     </row>
     <row r="267" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B267">
-        <v>2975</v>
+        <v>2972</v>
       </c>
       <c r="C267" t="s">
-        <v>316</v>
-      </c>
-      <c r="E267">
-        <v>2</v>
+        <v>310</v>
       </c>
       <c r="L267" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N267">
         <v>0.02</v>
@@ -20857,364 +20839,427 @@
         <v>100</v>
       </c>
       <c r="Z267" t="s">
-        <v>1173</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="268" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B268">
-        <v>2976</v>
+        <v>2973</v>
       </c>
       <c r="C268" t="s">
-        <v>307</v>
-      </c>
-      <c r="E268">
-        <v>2</v>
+        <v>318</v>
       </c>
       <c r="L268" s="4">
         <v>1</v>
       </c>
+      <c r="N268">
+        <v>0.02</v>
+      </c>
       <c r="U268">
         <v>100</v>
       </c>
       <c r="Z268" t="s">
-        <v>1283</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="269" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B269">
-        <v>2977</v>
+        <v>2974</v>
       </c>
       <c r="C269" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="E269">
-        <v>3</v>
-      </c>
-      <c r="L269" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N269">
-        <v>0.08</v>
-      </c>
-      <c r="Q269">
-        <v>15</v>
+        <v>0.05</v>
       </c>
       <c r="U269">
         <v>100</v>
       </c>
       <c r="Z269" t="s">
-        <v>1295</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="270" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B270">
-        <v>2978</v>
+        <v>2975</v>
       </c>
       <c r="C270" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="E270">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L270" s="4">
         <v>2</v>
       </c>
       <c r="N270">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="U270">
         <v>100</v>
       </c>
       <c r="Z270" t="s">
-        <v>1284</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="271" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B271">
-        <v>2979</v>
+        <v>2976</v>
       </c>
       <c r="C271" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E271">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L271" s="4">
-        <v>2</v>
-      </c>
-      <c r="N271">
-        <v>0.05</v>
-      </c>
-      <c r="Q271">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="U271">
         <v>100</v>
       </c>
       <c r="Z271" t="s">
-        <v>1296</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="272" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B272">
-        <v>2980</v>
+        <v>2977</v>
       </c>
       <c r="C272" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
       <c r="E272">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L272" s="4">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="N272">
+        <v>0.08</v>
+      </c>
+      <c r="Q272">
+        <v>15</v>
       </c>
       <c r="U272">
         <v>100</v>
       </c>
       <c r="Z272" t="s">
-        <v>1258</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="273" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B273">
-        <v>2981</v>
+        <v>2978</v>
       </c>
       <c r="C273" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E273">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L273" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q273">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="N273">
+        <v>0.1</v>
       </c>
       <c r="U273">
         <v>100</v>
       </c>
       <c r="Z273" t="s">
-        <v>1258</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="274" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B274">
-        <v>2982</v>
+        <v>2979</v>
       </c>
       <c r="C274" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E274">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L274" s="4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="N274">
+        <v>0.05</v>
+      </c>
+      <c r="Q274">
+        <v>5</v>
       </c>
       <c r="U274">
         <v>100</v>
       </c>
       <c r="Z274" t="s">
-        <v>1258</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="275" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B275">
-        <v>2983</v>
+        <v>2980</v>
       </c>
       <c r="C275" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="E275">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L275" s="4">
-        <v>5</v>
-      </c>
-      <c r="N275">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q275">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="U275">
         <v>100</v>
       </c>
       <c r="Z275" t="s">
-        <v>1298</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="276" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B276">
-        <v>2984</v>
+        <v>2981</v>
       </c>
       <c r="C276" t="s">
-        <v>1080</v>
+        <v>312</v>
       </c>
       <c r="E276">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="L276" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q276">
+        <v>5</v>
+      </c>
+      <c r="U276">
+        <v>100</v>
       </c>
       <c r="Z276" t="s">
-        <v>1244</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="277" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B277">
-        <v>2985</v>
+        <v>2982</v>
       </c>
       <c r="C277" t="s">
-        <v>1081</v>
+        <v>313</v>
+      </c>
+      <c r="E277">
+        <v>4</v>
+      </c>
+      <c r="L277" s="4">
+        <v>1</v>
+      </c>
+      <c r="U277">
+        <v>100</v>
       </c>
       <c r="Z277" t="s">
-        <v>1244</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="278" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B278">
-        <v>2986</v>
+        <v>2983</v>
       </c>
       <c r="C278" t="s">
-        <v>1082</v>
+        <v>314</v>
       </c>
       <c r="E278">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="L278" s="4">
+        <v>5</v>
+      </c>
+      <c r="N278">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q278">
+        <v>20</v>
+      </c>
+      <c r="U278">
+        <v>100</v>
       </c>
       <c r="Z278" t="s">
-        <v>1244</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="279" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B279">
-        <v>2987</v>
+        <v>2984</v>
       </c>
       <c r="C279" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="E279">
-        <v>3</v>
-      </c>
-      <c r="L279" s="4">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="Z279" t="s">
-        <v>1258</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="280" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B280">
-        <v>2988</v>
+        <v>2985</v>
       </c>
       <c r="C280" t="s">
-        <v>1094</v>
-      </c>
-      <c r="E280">
-        <v>3</v>
+        <v>1081</v>
       </c>
       <c r="Z280" t="s">
-        <v>1255</v>
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="281" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B281">
+        <v>2986</v>
+      </c>
+      <c r="C281" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E281">
+        <v>2</v>
+      </c>
+      <c r="Z281" t="s">
+        <v>1244</v>
       </c>
     </row>
     <row r="282" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B282">
-        <v>2991</v>
+        <v>2987</v>
       </c>
       <c r="C282" t="s">
-        <v>1037</v>
-      </c>
-      <c r="D282" t="s">
-        <v>1038</v>
+        <v>1083</v>
       </c>
       <c r="E282">
-        <v>1</v>
-      </c>
-      <c r="K282" s="4"/>
-      <c r="L282"/>
+        <v>3</v>
+      </c>
+      <c r="L282" s="4">
+        <v>0.5</v>
+      </c>
       <c r="Z282" t="s">
-        <v>1161</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="283" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B283">
-        <v>2992</v>
+        <v>2988</v>
       </c>
       <c r="C283" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="E283">
-        <v>2</v>
-      </c>
-      <c r="K283" s="4"/>
-      <c r="L283"/>
-    </row>
-    <row r="284" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B284">
-        <v>2993</v>
-      </c>
-      <c r="C284" t="s">
-        <v>1175</v>
-      </c>
-      <c r="E284">
         <v>3</v>
       </c>
-      <c r="K284" s="4"/>
-      <c r="L284"/>
+      <c r="Z283" t="s">
+        <v>1255</v>
+      </c>
     </row>
     <row r="285" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B285">
-        <v>2994</v>
+        <v>2991</v>
+      </c>
+      <c r="C285" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D285" t="s">
+        <v>1038</v>
       </c>
       <c r="E285">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="K285" s="4"/>
+      <c r="L285"/>
+      <c r="Z285" t="s">
+        <v>1161</v>
       </c>
     </row>
     <row r="286" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B286">
-        <v>2995</v>
+        <v>2992</v>
+      </c>
+      <c r="C286" t="s">
+        <v>1092</v>
       </c>
       <c r="E286">
-        <v>5</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="K286" s="4"/>
+      <c r="L286"/>
     </row>
     <row r="287" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B287">
-        <v>2996</v>
+        <v>2993</v>
+      </c>
+      <c r="C287" t="s">
+        <v>1175</v>
       </c>
       <c r="E287">
-        <v>6</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K287" s="4"/>
+      <c r="L287"/>
     </row>
     <row r="288" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B288">
-        <v>2997</v>
+        <v>2994</v>
       </c>
       <c r="E288">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="289" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B289">
-        <v>2998</v>
+        <v>2995</v>
       </c>
       <c r="E289">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B290">
-        <v>2999</v>
-      </c>
-      <c r="C290" t="s">
-        <v>1325</v>
+        <v>2996</v>
       </c>
       <c r="E290">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="291" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B291">
+        <v>2997</v>
+      </c>
+      <c r="E291">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="292" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B292">
+        <v>2998</v>
+      </c>
+      <c r="E292">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="293" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B293">
+        <v>2999</v>
+      </c>
+      <c r="C293" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E293">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="294" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B294">
         <v>3000</v>
       </c>
-      <c r="E291">
+      <c r="E294">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.7.5a: Initial Frontdoor map outlines
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831DFCC9-3E53-40D0-A735-19A6B15A3A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5652A12-71A9-48A3-865D-4CF6AFBE953C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1764" uniqueCount="1334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="1342">
   <si>
     <t>ID</t>
   </si>
@@ -4500,6 +4500,30 @@
   </si>
   <si>
     <t>Crossbow</t>
+  </si>
+  <si>
+    <t>4x4</t>
+  </si>
+  <si>
+    <t>3x3</t>
+  </si>
+  <si>
+    <t>Tree, maple, large</t>
+  </si>
+  <si>
+    <t>Tree, unknown, large</t>
+  </si>
+  <si>
+    <t>Tree, cedar, large</t>
+  </si>
+  <si>
+    <t>Tree, dead, large</t>
+  </si>
+  <si>
+    <t>Tree, large, large</t>
+  </si>
+  <si>
+    <t>Tree, pine, large</t>
   </si>
 </sst>
 </file>
@@ -13037,10 +13061,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H154"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H145" sqref="H145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14591,6 +14615,9 @@
       <c r="G130" t="s">
         <v>321</v>
       </c>
+      <c r="H130" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="2">
@@ -14599,6 +14626,9 @@
       <c r="C131" s="15" t="s">
         <v>723</v>
       </c>
+      <c r="H131" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="2">
@@ -14607,6 +14637,9 @@
       <c r="C132" s="15" t="s">
         <v>724</v>
       </c>
+      <c r="H132" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="2">
@@ -14615,6 +14648,9 @@
       <c r="C133" s="15" t="s">
         <v>725</v>
       </c>
+      <c r="H133" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
@@ -14626,6 +14662,9 @@
       <c r="E134">
         <v>35</v>
       </c>
+      <c r="H134" t="s">
+        <v>1335</v>
+      </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
@@ -14637,6 +14676,9 @@
       <c r="E135">
         <v>20</v>
       </c>
+      <c r="H135" t="s">
+        <v>651</v>
+      </c>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" s="2">
@@ -14682,76 +14724,163 @@
         <v>729</v>
       </c>
     </row>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B140" s="2">
+        <v>444</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>1336</v>
+      </c>
+      <c r="E140">
+        <v>35</v>
+      </c>
+      <c r="G140" t="s">
+        <v>321</v>
+      </c>
+      <c r="H140" t="s">
+        <v>1335</v>
+      </c>
+    </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="2">
-        <v>501</v>
+        <v>445</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D141" t="s">
-        <v>242</v>
+        <v>1337</v>
       </c>
       <c r="E141">
-        <v>5</v>
+        <v>35</v>
+      </c>
+      <c r="H141" t="s">
+        <v>1335</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="2">
-        <v>502</v>
+        <v>446</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>244</v>
+        <v>1338</v>
+      </c>
+      <c r="E142">
+        <v>35</v>
+      </c>
+      <c r="H142" t="s">
+        <v>1335</v>
       </c>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" s="2">
-        <v>503</v>
+        <v>447</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>245</v>
+        <v>1339</v>
+      </c>
+      <c r="E143">
+        <v>35</v>
+      </c>
+      <c r="H143" t="s">
+        <v>1335</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" s="2">
+        <v>448</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E144">
+        <v>50</v>
+      </c>
+      <c r="H144" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B145" s="2">
+        <v>449</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>1341</v>
+      </c>
+      <c r="E145">
+        <v>35</v>
+      </c>
+      <c r="H145" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B147" s="2">
+        <v>501</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D147" t="s">
+        <v>242</v>
+      </c>
+      <c r="E147">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B148" s="2">
+        <v>502</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B149" s="2">
+        <v>503</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B150" s="2">
         <v>504</v>
       </c>
-      <c r="C144" s="15" t="s">
+      <c r="C150" s="15" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="145" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B145" s="2">
+    <row r="151" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B151" s="2">
         <v>505</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="C151" s="15" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="146" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B146" s="2">
+    <row r="152" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B152" s="2">
         <v>511</v>
       </c>
-      <c r="C146" s="15" t="s">
+      <c r="C152" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="E146">
+      <c r="E152">
         <v>9</v>
       </c>
     </row>
-    <row r="147" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B147" s="2">
+    <row r="153" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B153" s="2">
         <v>512</v>
       </c>
-      <c r="C147" s="15" t="s">
+      <c r="C153" s="15" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="148" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B148" s="2">
+    <row r="154" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B154" s="2">
         <v>513</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="C154" s="15" t="s">
         <v>250</v>
       </c>
     </row>
@@ -16280,8 +16409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE22176D-CFFA-4A34-AB14-C1369F5F19BF}">
   <dimension ref="A1:Z294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D63" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D66" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="E91" sqref="E91"/>

</xml_diff>

<commit_message>
v0.7.5b: Initial Ahimdoor map outlines
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5652A12-71A9-48A3-865D-4CF6AFBE953C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A97E6B-AF2D-40AE-AF9A-38B3FDFD11D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1783" uniqueCount="1342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="1344">
   <si>
     <t>ID</t>
   </si>
@@ -4524,6 +4524,12 @@
   </si>
   <si>
     <t>Tree, pine, large</t>
+  </si>
+  <si>
+    <t>Gazebo</t>
+  </si>
+  <si>
+    <t>building</t>
   </si>
 </sst>
 </file>
@@ -13061,10 +13067,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
-  <dimension ref="A1:H154"/>
+  <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H145" sqref="H145"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14144,487 +14150,490 @@
         <v>665</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="2" t="s">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="2">
+        <v>253</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E87">
+        <v>7</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C89" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D89" t="s">
         <v>207</v>
       </c>
-      <c r="E88">
+      <c r="E89">
         <v>100</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G89" t="s">
         <v>679</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H89" t="s">
         <v>680</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="2">
-        <v>311</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>210</v>
-      </c>
-      <c r="G89" s="8" t="s">
-        <v>469</v>
-      </c>
-      <c r="H89" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="2">
-        <v>312</v>
+        <v>311</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>210</v>
+      </c>
+      <c r="G90" s="8" t="s">
+        <v>469</v>
       </c>
       <c r="H90" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="2">
-        <v>321</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>681</v>
-      </c>
-      <c r="D91" t="s">
-        <v>681</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="G91" t="s">
-        <v>686</v>
+        <v>312</v>
       </c>
       <c r="H91" t="s">
-        <v>683</v>
+        <v>690</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="2">
-        <v>322</v>
+        <v>321</v>
+      </c>
+      <c r="C92" s="15" t="s">
+        <v>681</v>
+      </c>
+      <c r="D92" t="s">
+        <v>681</v>
       </c>
       <c r="E92">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="G92" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H92" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="2">
-        <v>323</v>
+        <v>322</v>
+      </c>
+      <c r="E93">
+        <v>100</v>
       </c>
       <c r="G93" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="H93" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="2">
-        <v>331</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>843</v>
-      </c>
-      <c r="D94" t="s">
-        <v>699</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="G94" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="H94" t="s">
-        <v>700</v>
+        <v>685</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="2">
-        <v>332</v>
+        <v>331</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>843</v>
+      </c>
+      <c r="D95" t="s">
+        <v>699</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="G95" t="s">
+        <v>686</v>
       </c>
       <c r="H95" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="2">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H96" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B97" s="2">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H97" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B98" s="2">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H98" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B99" s="2">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H99" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" s="2">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H100" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B101" s="2">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H101" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B102" s="2">
-        <v>339</v>
-      </c>
-      <c r="C102" s="15" t="s">
-        <v>708</v>
-      </c>
-      <c r="E102">
-        <v>100</v>
-      </c>
-      <c r="G102" t="s">
-        <v>687</v>
+        <v>338</v>
       </c>
       <c r="H102" t="s">
-        <v>663</v>
+        <v>707</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B103" s="2">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>708</v>
+      </c>
+      <c r="E103">
+        <v>100</v>
+      </c>
+      <c r="G103" t="s">
+        <v>687</v>
       </c>
       <c r="H103" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" s="2">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H104" t="s">
-        <v>710</v>
+        <v>665</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" s="2">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H105" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B106" s="2">
-        <v>343</v>
-      </c>
-      <c r="C106" s="15" t="s">
-        <v>709</v>
-      </c>
-      <c r="G106" t="s">
-        <v>733</v>
+        <v>342</v>
       </c>
       <c r="H106" t="s">
-        <v>663</v>
+        <v>711</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B107" s="2">
-        <v>344</v>
+        <v>343</v>
+      </c>
+      <c r="C107" s="15" t="s">
+        <v>709</v>
+      </c>
+      <c r="G107" t="s">
+        <v>733</v>
       </c>
       <c r="H107" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" s="2">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H108" t="s">
-        <v>710</v>
+        <v>665</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" s="2">
+        <v>345</v>
+      </c>
+      <c r="H109" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B110" s="2">
         <v>346</v>
       </c>
-      <c r="H109" t="s">
+      <c r="H110" t="s">
         <v>711</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A110" s="4"/>
-      <c r="B110" s="2">
-        <v>351</v>
-      </c>
-      <c r="C110" s="15" t="s">
-        <v>1074</v>
-      </c>
-      <c r="D110" t="s">
-        <v>699</v>
-      </c>
-      <c r="E110">
-        <v>0</v>
-      </c>
-      <c r="G110" t="s">
-        <v>686</v>
-      </c>
-      <c r="H110" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="2">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D111" t="s">
+        <v>699</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="G111" t="s">
+        <v>686</v>
       </c>
       <c r="H111" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="2">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H112" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="2">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H113" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="2">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H114" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="2">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H115" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="2">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H116" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="2">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H117" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="2">
-        <v>359</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>1075</v>
-      </c>
-      <c r="E118">
-        <v>100</v>
-      </c>
-      <c r="G118" t="s">
-        <v>687</v>
+        <v>358</v>
       </c>
       <c r="H118" t="s">
-        <v>663</v>
+        <v>707</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="2">
-        <v>360</v>
+        <v>359</v>
+      </c>
+      <c r="C119" s="15" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E119">
+        <v>100</v>
+      </c>
+      <c r="G119" t="s">
+        <v>687</v>
       </c>
       <c r="H119" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="2">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H120" t="s">
-        <v>710</v>
+        <v>665</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="2">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H121" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="2">
-        <v>363</v>
-      </c>
-      <c r="C122" s="15" t="s">
-        <v>1076</v>
-      </c>
-      <c r="G122" t="s">
-        <v>733</v>
+        <v>362</v>
       </c>
       <c r="H122" t="s">
-        <v>663</v>
+        <v>711</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="2">
-        <v>364</v>
+        <v>363</v>
+      </c>
+      <c r="C123" s="15" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G123" t="s">
+        <v>733</v>
       </c>
       <c r="H123" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="2">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H124" t="s">
-        <v>710</v>
+        <v>665</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="2">
+        <v>365</v>
+      </c>
+      <c r="H125" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A126" s="4"/>
+      <c r="B126" s="2">
         <v>366</v>
       </c>
-      <c r="H125" t="s">
+      <c r="H126" t="s">
         <v>711</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="2">
-        <v>401</v>
-      </c>
-      <c r="C127" s="15" t="s">
-        <v>282</v>
-      </c>
-      <c r="D127" t="s">
-        <v>284</v>
-      </c>
-      <c r="E127">
-        <v>0</v>
-      </c>
-      <c r="G127" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B128" s="2">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>647</v>
+        <v>282</v>
+      </c>
+      <c r="D128" t="s">
+        <v>284</v>
       </c>
       <c r="E128">
         <v>0</v>
       </c>
       <c r="G128" t="s">
-        <v>286</v>
-      </c>
-      <c r="H128" t="s">
-        <v>720</v>
+        <v>285</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B129" s="2">
-        <v>412</v>
+        <v>411</v>
+      </c>
+      <c r="C129" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
       </c>
       <c r="G129" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H129" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" s="2">
-        <v>421</v>
-      </c>
-      <c r="C130" s="15" t="s">
-        <v>722</v>
-      </c>
-      <c r="E130">
-        <v>20</v>
+        <v>412</v>
       </c>
       <c r="G130" t="s">
-        <v>321</v>
+        <v>287</v>
       </c>
       <c r="H130" t="s">
-        <v>651</v>
+        <v>721</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B131" s="2">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>723</v>
+        <v>722</v>
+      </c>
+      <c r="E131">
+        <v>20</v>
+      </c>
+      <c r="G131" t="s">
+        <v>321</v>
       </c>
       <c r="H131" t="s">
         <v>651</v>
@@ -14632,10 +14641,10 @@
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B132" s="2">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C132" s="15" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="H132" t="s">
         <v>651</v>
@@ -14643,10 +14652,10 @@
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B133" s="2">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C133" s="15" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="H133" t="s">
         <v>651</v>
@@ -14654,102 +14663,99 @@
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" s="2">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C134" s="15" t="s">
-        <v>726</v>
-      </c>
-      <c r="E134">
-        <v>35</v>
+        <v>725</v>
       </c>
       <c r="H134" t="s">
-        <v>1335</v>
+        <v>651</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B135" s="2">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C135" s="15" t="s">
-        <v>750</v>
+        <v>726</v>
       </c>
       <c r="E135">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H135" t="s">
-        <v>651</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B136" s="2">
+        <v>426</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>750</v>
+      </c>
+      <c r="E136">
+        <v>20</v>
+      </c>
+      <c r="H136" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B137" s="2">
         <v>431</v>
       </c>
-      <c r="C136" s="15" t="s">
+      <c r="C137" s="15" t="s">
         <v>238</v>
       </c>
-      <c r="E136">
+      <c r="E137">
         <v>7</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="19">
+    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B138" s="19">
         <v>441</v>
       </c>
-      <c r="C137" s="15" t="s">
+      <c r="C138" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="E137">
+      <c r="E138">
         <v>5</v>
       </c>
-      <c r="G137" t="s">
+      <c r="G138" t="s">
         <v>322</v>
       </c>
-      <c r="H137" t="s">
+      <c r="H138" t="s">
         <v>727</v>
-      </c>
-    </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="2">
-        <v>442</v>
-      </c>
-      <c r="H138" t="s">
-        <v>728</v>
       </c>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B139" s="2">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H139" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B140" s="2">
-        <v>444</v>
-      </c>
-      <c r="C140" s="15" t="s">
-        <v>1336</v>
-      </c>
-      <c r="E140">
-        <v>35</v>
-      </c>
-      <c r="G140" t="s">
-        <v>321</v>
+        <v>443</v>
       </c>
       <c r="H140" t="s">
-        <v>1335</v>
+        <v>729</v>
       </c>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B141" s="2">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C141" s="15" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
       <c r="E141">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="G141" t="s">
+        <v>321</v>
       </c>
       <c r="H141" t="s">
         <v>1335</v>
@@ -14757,13 +14763,13 @@
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B142" s="2">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C142" s="15" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="E142">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H142" t="s">
         <v>1335</v>
@@ -14771,13 +14777,13 @@
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B143" s="2">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C143" s="15" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="E143">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H143" t="s">
         <v>1335</v>
@@ -14785,102 +14791,116 @@
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B144" s="2">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C144" s="15" t="s">
-        <v>1340</v>
+        <v>1339</v>
       </c>
       <c r="E144">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="H144" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B145" s="2">
+        <v>448</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>1340</v>
+      </c>
+      <c r="E145">
+        <v>40</v>
+      </c>
+      <c r="H145" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B146" s="2">
         <v>449</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="C146" s="15" t="s">
         <v>1341</v>
       </c>
-      <c r="E145">
-        <v>35</v>
-      </c>
-      <c r="H145" t="s">
+      <c r="E146">
+        <v>30</v>
+      </c>
+      <c r="H146" t="s">
         <v>1335</v>
-      </c>
-    </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="2">
-        <v>501</v>
-      </c>
-      <c r="C147" s="15" t="s">
-        <v>243</v>
-      </c>
-      <c r="D147" t="s">
-        <v>242</v>
-      </c>
-      <c r="E147">
-        <v>5</v>
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B148" s="2">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C148" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
+      </c>
+      <c r="D148" t="s">
+        <v>242</v>
+      </c>
+      <c r="E148">
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B149" s="2">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C149" s="15" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B150" s="2">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C150" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B151" s="2">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C151" s="15" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B152" s="2">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C152" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="E152">
-        <v>9</v>
+        <v>247</v>
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B153" s="2">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C153" s="15" t="s">
-        <v>249</v>
+        <v>248</v>
+      </c>
+      <c r="E153">
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B154" s="2">
+        <v>512</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B155" s="2">
         <v>513</v>
       </c>
-      <c r="C154" s="15" t="s">
+      <c r="C155" s="15" t="s">
         <v>250</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.7.5e: GameMap::mouseMove() thread, started GameMapArea
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A97E6B-AF2D-40AE-AF9A-38B3FDFD11D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5895E5D-62A5-426F-90AF-E39FE0195C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="1" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="7" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1785" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="1346">
   <si>
     <t>ID</t>
   </si>
@@ -4530,6 +4530,12 @@
   </si>
   <si>
     <t>building</t>
+  </si>
+  <si>
+    <t>Frontdoor-ahimdoor</t>
+  </si>
+  <si>
+    <t>Frontdoor-ahimOtherDoor</t>
   </si>
 </sst>
 </file>
@@ -13069,7 +13075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="H87" sqref="H87"/>
     </sheetView>
   </sheetViews>
@@ -22793,8 +22799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23418,10 +23424,16 @@
       <c r="B51" s="1">
         <v>41</v>
       </c>
+      <c r="D51" t="s">
+        <v>1344</v>
+      </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
         <v>42</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1345</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.5i: Initial Cathy Heck boss fight
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5895E5D-62A5-426F-90AF-E39FE0195C80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9F15D0-A787-4364-900F-25B2D626AA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="7" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1787" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1788" uniqueCount="1347">
   <si>
     <t>ID</t>
   </si>
@@ -4536,6 +4536,9 @@
   </si>
   <si>
     <t>Frontdoor-ahimOtherDoor</t>
+  </si>
+  <si>
+    <t>Cathy Heck</t>
   </si>
 </sst>
 </file>
@@ -13075,8 +13078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14918,10 +14921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
-  <dimension ref="A1:R43"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15939,6 +15942,17 @@
       </c>
       <c r="R43" s="8" t="s">
         <v>1324</v>
+      </c>
+    </row>
+    <row r="44" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>1311</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1346</v>
+      </c>
+      <c r="F44">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -16436,10 +16450,10 @@
   <dimension ref="A1:Z294"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D252" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E91" sqref="E91"/>
+      <selection pane="bottomRight" activeCell="K278" sqref="K278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17309,7 +17323,7 @@
         <v>27</v>
       </c>
       <c r="L51" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N51">
         <v>0.12</v>
@@ -17326,7 +17340,7 @@
         <v>21</v>
       </c>
       <c r="L52" s="4">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="N52">
         <v>0.02</v>
@@ -17343,7 +17357,7 @@
         <v>271</v>
       </c>
       <c r="L53" s="4">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="N53">
         <v>0.01</v>
@@ -17383,7 +17397,7 @@
         <v>1178</v>
       </c>
       <c r="L55" s="4">
-        <v>2.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N55">
         <v>0.15</v>
@@ -17423,7 +17437,7 @@
         <v>1180</v>
       </c>
       <c r="L57" s="4">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="N57">
         <v>0.35</v>
@@ -20831,7 +20845,7 @@
         <v>315</v>
       </c>
       <c r="L259" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="N259">
         <v>0.05</v>
@@ -20865,7 +20879,7 @@
         <v>844</v>
       </c>
       <c r="L261" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N261">
         <v>0.05</v>
@@ -20885,7 +20899,7 @@
         <v>845</v>
       </c>
       <c r="L262" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N262">
         <v>0.05</v>
@@ -20905,7 +20919,7 @@
         <v>846</v>
       </c>
       <c r="L263" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N263">
         <v>0.05</v>
@@ -20925,7 +20939,7 @@
         <v>847</v>
       </c>
       <c r="L264" s="4">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="N264">
         <v>0.05</v>
@@ -22799,7 +22813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
v0.7.5j: Upgraded pathfinding, fixed some ability bugs
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC9F15D0-A787-4364-900F-25B2D626AA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247F0FC2-D22B-44C9-8D6D-4CFF96220875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -4992,7 +4992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF2113E-D79E-4CB9-ADC9-BF3629B5384A}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -13078,7 +13078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE173168-AF21-4474-9878-DBD01A8D9EC7}">
   <dimension ref="A1:H155"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -14924,7 +14924,7 @@
   <dimension ref="A1:R44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15953,6 +15953,30 @@
       </c>
       <c r="F44">
         <v>11</v>
+      </c>
+      <c r="H44">
+        <v>40</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>1.8</v>
+      </c>
+      <c r="K44">
+        <v>0.1</v>
+      </c>
+      <c r="L44">
+        <v>0.6</v>
+      </c>
+      <c r="M44">
+        <v>10</v>
+      </c>
+      <c r="N44">
+        <v>1.2</v>
+      </c>
+      <c r="O44">
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.7.5k: Upgraded Cathy Heck boss fight
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247F0FC2-D22B-44C9-8D6D-4CFF96220875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062FC72D-3DA5-4EB7-9655-FDC19C684111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="5" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -4993,7 +4993,7 @@
   <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14923,8 +14923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15955,13 +15955,13 @@
         <v>11</v>
       </c>
       <c r="H44">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I44">
         <v>6</v>
       </c>
       <c r="J44">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="K44">
         <v>0.1</v>
@@ -21469,8 +21469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DAF6DD-D8FA-4653-B50E-0B687056C45B}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22578,7 +22578,7 @@
         <v>0.3</v>
       </c>
       <c r="I36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K36" s="4">
         <v>1</v>
@@ -22611,7 +22611,7 @@
         <v>0.3</v>
       </c>
       <c r="I37">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="K37">
         <v>2</v>
@@ -22644,7 +22644,7 @@
         <v>0.3</v>
       </c>
       <c r="I38">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="K38" s="4">
         <v>1</v>
@@ -22677,7 +22677,7 @@
         <v>0.3</v>
       </c>
       <c r="I39">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="K39" s="4">
         <v>1</v>
@@ -22707,7 +22707,7 @@
         <v>0.3</v>
       </c>
       <c r="I40">
-        <v>3.5</v>
+        <v>5.5</v>
       </c>
       <c r="K40" s="4">
         <v>3</v>

</xml_diff>

<commit_message>
v0.7.5m: Zombies auto-spawn at night
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19847321-1493-4CDA-AE2C-44190CC1B0F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3708EBB-F053-4CA2-9A56-275BF39C4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="9" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1786" uniqueCount="1346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1353">
   <si>
     <t>ID</t>
   </si>
@@ -4536,6 +4536,27 @@
   </si>
   <si>
     <t>stat,x(n) = c,0 + 0.5 * c,x * n * (n + 1)</t>
+  </si>
+  <si>
+    <t>Auto-spawned at night-time</t>
+  </si>
+  <si>
+    <t>0-100</t>
+  </si>
+  <si>
+    <t>frontdoor boss fight</t>
+  </si>
+  <si>
+    <t>3 (0.4)</t>
+  </si>
+  <si>
+    <t>1 (0.1)</t>
+  </si>
+  <si>
+    <t>0 (0)</t>
+  </si>
+  <si>
+    <t>0 (0.01)</t>
   </si>
 </sst>
 </file>
@@ -5729,8 +5750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A114E18-4580-4CF1-BE70-B14A03AAF800}">
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15732,10 +15753,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
-  <dimension ref="A1:R44"/>
+  <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16253,7 +16274,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="Q25" t="s">
         <v>1023</v>
@@ -16285,7 +16306,7 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="Q26" t="s">
         <v>1023</v>
@@ -16314,7 +16335,7 @@
         <v>0</v>
       </c>
       <c r="L27">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="Q27" t="s">
         <v>1023</v>
@@ -16346,7 +16367,7 @@
         <v>0</v>
       </c>
       <c r="L28">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="Q28" t="s">
         <v>1023</v>
@@ -16378,7 +16399,7 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="Q29" t="s">
         <v>1023</v>
@@ -16410,7 +16431,7 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="Q30" t="s">
         <v>1023</v>
@@ -16439,7 +16460,7 @@
         <v>0</v>
       </c>
       <c r="L31">
-        <v>1.2</v>
+        <v>0.9</v>
       </c>
       <c r="Q31" t="s">
         <v>1023</v>
@@ -16471,7 +16492,7 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="Q32" t="s">
         <v>1023</v>
@@ -16503,7 +16524,7 @@
         <v>0</v>
       </c>
       <c r="L33">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="Q33" t="s">
         <v>1023</v>
@@ -16538,256 +16559,314 @@
         <v>1024</v>
       </c>
     </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>1291</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1347</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1349</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1350</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1352</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1351</v>
+      </c>
+      <c r="L35">
+        <v>0.8</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>1023</v>
+      </c>
+      <c r="R35" t="s">
+        <v>1346</v>
+      </c>
+    </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <v>1301</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1219</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1218</v>
-      </c>
-      <c r="E36" t="s">
-        <v>12</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="H36">
-        <v>6</v>
-      </c>
-      <c r="I36">
-        <v>2.5</v>
-      </c>
-      <c r="J36">
-        <v>0.2</v>
-      </c>
-      <c r="K36">
-        <v>0</v>
-      </c>
-      <c r="L36">
-        <v>1</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <v>1302</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1220</v>
-      </c>
-      <c r="F37">
-        <v>2</v>
-      </c>
-      <c r="H37">
-        <v>5</v>
-      </c>
-      <c r="I37">
-        <v>4</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
-      <c r="L37">
-        <v>1.5</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <v>1303</v>
-      </c>
-      <c r="C38" t="s">
-        <v>1221</v>
-      </c>
-      <c r="F38">
-        <v>3</v>
-      </c>
-      <c r="H38">
-        <v>12</v>
-      </c>
-      <c r="I38">
-        <v>3.5</v>
-      </c>
-      <c r="J38">
-        <v>1</v>
-      </c>
-      <c r="K38">
-        <v>0</v>
-      </c>
-      <c r="L38">
-        <v>0.9</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <v>1304</v>
-      </c>
-      <c r="C39" t="s">
-        <v>1222</v>
-      </c>
-      <c r="F39">
-        <v>4</v>
-      </c>
-      <c r="H39">
-        <v>10</v>
-      </c>
-      <c r="I39">
-        <v>5</v>
-      </c>
-      <c r="J39">
-        <v>0.4</v>
-      </c>
-      <c r="K39">
-        <v>0.05</v>
-      </c>
-      <c r="L39">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B40" s="1">
-        <v>1305</v>
-      </c>
-      <c r="C40" t="s">
-        <v>1223</v>
-      </c>
-      <c r="F40">
-        <v>5</v>
-      </c>
-      <c r="H40">
-        <v>9</v>
-      </c>
-      <c r="I40">
-        <v>7</v>
-      </c>
-      <c r="J40">
-        <v>0.4</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>1.3</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <v>1306</v>
+        <v>1301</v>
       </c>
       <c r="C41" t="s">
-        <v>1226</v>
+        <v>1219</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1218</v>
+      </c>
+      <c r="E41" t="s">
+        <v>12</v>
       </c>
       <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="H41">
         <v>6</v>
       </c>
-      <c r="H41">
-        <v>15</v>
-      </c>
       <c r="I41">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="J41">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="K41">
-        <v>0.12</v>
+        <v>0</v>
       </c>
       <c r="L41">
-        <v>1.4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <v>1307</v>
+        <v>1302</v>
       </c>
       <c r="C42" t="s">
-        <v>1227</v>
+        <v>1220</v>
       </c>
       <c r="F42">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H42">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="I42">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J42">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="K42">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="L42">
-        <v>1.1000000000000001</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
-        <v>1308</v>
+        <v>1303</v>
       </c>
       <c r="C43" t="s">
-        <v>1228</v>
+        <v>1221</v>
       </c>
       <c r="F43">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H43">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="I43">
-        <v>10</v>
+        <v>3.5</v>
       </c>
       <c r="J43">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="K43">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="L43">
-        <v>1.4</v>
-      </c>
-      <c r="R43" s="8" t="s">
-        <v>1320</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
+        <v>1304</v>
+      </c>
+      <c r="C44" t="s">
+        <v>1222</v>
+      </c>
+      <c r="F44">
+        <v>4</v>
+      </c>
+      <c r="H44">
+        <v>10</v>
+      </c>
+      <c r="I44">
+        <v>5</v>
+      </c>
+      <c r="J44">
+        <v>0.4</v>
+      </c>
+      <c r="K44">
+        <v>0.05</v>
+      </c>
+      <c r="L44">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>1305</v>
+      </c>
+      <c r="C45" t="s">
+        <v>1223</v>
+      </c>
+      <c r="F45">
+        <v>5</v>
+      </c>
+      <c r="H45">
+        <v>9</v>
+      </c>
+      <c r="I45">
+        <v>7</v>
+      </c>
+      <c r="J45">
+        <v>0.4</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>1306</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1226</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+      <c r="H46">
+        <v>15</v>
+      </c>
+      <c r="I46">
+        <v>8</v>
+      </c>
+      <c r="J46">
+        <v>0.4</v>
+      </c>
+      <c r="K46">
+        <v>0.12</v>
+      </c>
+      <c r="L46">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>1307</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1227</v>
+      </c>
+      <c r="F47">
+        <v>7</v>
+      </c>
+      <c r="H47">
+        <v>25</v>
+      </c>
+      <c r="I47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K47">
+        <v>0.03</v>
+      </c>
+      <c r="L47">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>1308</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1228</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+      <c r="H48">
+        <v>18</v>
+      </c>
+      <c r="I48">
+        <v>10</v>
+      </c>
+      <c r="J48">
+        <v>0.8</v>
+      </c>
+      <c r="K48">
+        <v>0.15</v>
+      </c>
+      <c r="L48">
+        <v>1.4</v>
+      </c>
+      <c r="R48" s="8" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="49" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R49" s="8"/>
+    </row>
+    <row r="50" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
         <v>1311</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C50" t="s">
         <v>1342</v>
       </c>
-      <c r="F44">
+      <c r="F50">
         <v>11</v>
       </c>
-      <c r="H44">
+      <c r="H50">
         <v>35</v>
       </c>
-      <c r="I44">
+      <c r="I50">
         <v>6</v>
       </c>
-      <c r="J44">
+      <c r="J50">
         <v>1.6</v>
       </c>
-      <c r="K44">
+      <c r="K50">
         <v>0.1</v>
       </c>
-      <c r="L44">
+      <c r="L50">
         <v>0.6</v>
       </c>
-      <c r="M44">
+      <c r="M50">
         <v>10</v>
       </c>
-      <c r="N44">
+      <c r="N50">
         <v>1.2</v>
       </c>
-      <c r="O44">
+      <c r="O50">
         <v>0.05</v>
+      </c>
+      <c r="R50" t="s">
+        <v>1348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.7.5n: Added running zombie and armored zombie
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3708EBB-F053-4CA2-9A56-275BF39C4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C780390D-30EF-45F8-9792-27A8BD04C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="1358">
   <si>
     <t>ID</t>
   </si>
@@ -4556,7 +4556,22 @@
     <t>0 (0)</t>
   </si>
   <si>
-    <t>0 (0.01)</t>
+    <t>Running Zombie</t>
+  </si>
+  <si>
+    <t>0 (0.012)</t>
+  </si>
+  <si>
+    <t>2 (0.022)</t>
+  </si>
+  <si>
+    <t>20% rotten flesh, 10% sneakers</t>
+  </si>
+  <si>
+    <t>Armored Zombie</t>
+  </si>
+  <si>
+    <t>20% rotten flesh, 10% tier's ore (no corundum/diamond)</t>
   </si>
 </sst>
 </file>
@@ -15755,8 +15770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16576,7 +16591,7 @@
         <v>1350</v>
       </c>
       <c r="J35" t="s">
-        <v>1352</v>
+        <v>1353</v>
       </c>
       <c r="K35" t="s">
         <v>1351</v>
@@ -16595,10 +16610,28 @@
       <c r="B36" s="1">
         <v>1292</v>
       </c>
+      <c r="C36" t="s">
+        <v>1352</v>
+      </c>
+      <c r="L36">
+        <v>1.3</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>1355</v>
+      </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
         <v>1293</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1356</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1354</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>1357</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
v0.7.5o: Bug fixes, rebalancing
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C780390D-30EF-45F8-9792-27A8BD04C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B05D52-4683-4E9A-AB98-DA56865B6C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
@@ -15770,8 +15770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F803ACD-0C6B-4501-8A1D-9CD977C9D5BC}">
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I51" sqref="I51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16309,10 +16309,10 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>1.3</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -16338,7 +16338,7 @@
         <v>3</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="I27">
         <v>2</v>
@@ -16370,7 +16370,7 @@
         <v>4</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I28">
         <v>3</v>
@@ -16402,10 +16402,10 @@
         <v>5</v>
       </c>
       <c r="H29">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I29">
-        <v>3</v>
+        <v>3.2</v>
       </c>
       <c r="J29">
         <v>0.3</v>
@@ -16434,10 +16434,10 @@
         <v>6</v>
       </c>
       <c r="H30">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I30">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="J30">
         <v>0.3</v>
@@ -16463,10 +16463,10 @@
         <v>7</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="I31">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31">
         <v>0.6</v>
@@ -16495,10 +16495,10 @@
         <v>8</v>
       </c>
       <c r="H32">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I32">
-        <v>3</v>
+        <v>4.3</v>
       </c>
       <c r="J32">
         <v>0.6</v>
@@ -16527,10 +16527,10 @@
         <v>9</v>
       </c>
       <c r="H33">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="I33">
-        <v>3</v>
+        <v>4.7</v>
       </c>
       <c r="J33">
         <v>0.6</v>
@@ -16556,10 +16556,10 @@
         <v>10</v>
       </c>
       <c r="H34">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="I34">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -16687,10 +16687,10 @@
         <v>2</v>
       </c>
       <c r="H42">
+        <v>8</v>
+      </c>
+      <c r="I42">
         <v>5</v>
-      </c>
-      <c r="I42">
-        <v>4</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -16713,10 +16713,10 @@
         <v>3</v>
       </c>
       <c r="H43">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I43">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="J43">
         <v>1</v>
@@ -16739,10 +16739,10 @@
         <v>4</v>
       </c>
       <c r="H44">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I44">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="J44">
         <v>0.4</v>
@@ -16765,7 +16765,7 @@
         <v>5</v>
       </c>
       <c r="H45">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="I45">
         <v>7</v>
@@ -16791,7 +16791,7 @@
         <v>6</v>
       </c>
       <c r="H46">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I46">
         <v>8</v>
@@ -16820,7 +16820,7 @@
         <v>25</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="J47">
         <v>2.2000000000000002</v>
@@ -16843,7 +16843,7 @@
         <v>8</v>
       </c>
       <c r="H48">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="I48">
         <v>10</v>
@@ -16875,10 +16875,10 @@
         <v>11</v>
       </c>
       <c r="H50">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="I50">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="J50">
         <v>1.6</v>
@@ -23760,8 +23760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2E1DA2-B439-478A-B9E1-948DA404767C}">
   <dimension ref="B2:H129"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
v0.7.5p: Base car logic
</commit_message>
<xml_diff>
--- a/objects.xlsx
+++ b/objects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yodan\github\LNZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B05D52-4683-4E9A-AB98-DA56865B6C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B947BD-CB65-42EB-954E-B0FE4F872599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="2" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="657" activeTab="4" xr2:uid="{C87F634A-6B2D-4506-B485-5153AAAF3A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Terrains" sheetId="13" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <sheet name="Crafting" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="1358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1803" uniqueCount="1361">
   <si>
     <t>ID</t>
   </si>
@@ -4573,6 +4574,15 @@
   <si>
     <t>20% rotten flesh, 10% tier's ore (no corundum/diamond)</t>
   </si>
+  <si>
+    <t>Gas Can</t>
+  </si>
+  <si>
+    <t>holds 50 gas (5 gallons)</t>
+  </si>
+  <si>
+    <t>Car Key</t>
+  </si>
 </sst>
 </file>
 
@@ -4701,6 +4711,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -4713,14 +4726,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5783,26 +5793,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="H1" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
@@ -5814,19 +5824,19 @@
       <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="29" t="s">
+      <c r="K3" s="30" t="s">
         <v>1343</v>
       </c>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="32" t="s">
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="31" t="s">
         <v>1345</v>
       </c>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="32"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -12560,7 +12570,7 @@
     </row>
     <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="32" t="s">
         <v>456</v>
       </c>
       <c r="C10" t="s">
@@ -12578,11 +12588,11 @@
       <c r="G10" t="s">
         <v>553</v>
       </c>
-      <c r="I10" s="28"/>
+      <c r="I10" s="29"/>
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="30"/>
+      <c r="B11" s="32"/>
       <c r="C11" t="s">
         <v>903</v>
       </c>
@@ -12598,11 +12608,11 @@
       <c r="G11" t="s">
         <v>554</v>
       </c>
-      <c r="I11" s="28"/>
+      <c r="I11" s="29"/>
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
+      <c r="B12" s="32"/>
       <c r="C12" t="s">
         <v>904</v>
       </c>
@@ -12618,11 +12628,11 @@
       <c r="G12" t="s">
         <v>555</v>
       </c>
-      <c r="I12" s="28"/>
+      <c r="I12" s="29"/>
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="30"/>
+      <c r="B13" s="32"/>
       <c r="C13" t="s">
         <v>536</v>
       </c>
@@ -12638,11 +12648,11 @@
       <c r="G13" t="s">
         <v>556</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="29"/>
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="30"/>
+      <c r="B14" s="32"/>
       <c r="C14" t="s">
         <v>537</v>
       </c>
@@ -12658,10 +12668,10 @@
       <c r="G14" t="s">
         <v>557</v>
       </c>
-      <c r="I14" s="28"/>
+      <c r="I14" s="29"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="30"/>
+      <c r="B15" s="32"/>
       <c r="C15" t="s">
         <v>906</v>
       </c>
@@ -12677,10 +12687,10 @@
       <c r="G15" t="s">
         <v>558</v>
       </c>
-      <c r="I15" s="28"/>
+      <c r="I15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="30"/>
+      <c r="B16" s="32"/>
       <c r="C16" t="s">
         <v>538</v>
       </c>
@@ -12696,10 +12706,10 @@
       <c r="G16" t="s">
         <v>559</v>
       </c>
-      <c r="I16" s="28"/>
+      <c r="I16" s="29"/>
     </row>
     <row r="17" spans="2:9" 